<commit_message>
Data updated by GitHub Bot (2020-06-01 20) (#71)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1515" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1539" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -1699,10 +1699,10 @@
   <dimension ref="A1:S160"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B79" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B73" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H90" sqref="H90"/>
+      <selection pane="bottomRight" activeCell="J95" sqref="J95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6108,21 +6108,54 @@
       </c>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B90" s="28"/>
-      <c r="C90" s="28"/>
-      <c r="D90" s="28"/>
-      <c r="E90" s="28"/>
-      <c r="F90" s="28"/>
-      <c r="G90" s="28"/>
-      <c r="H90" s="28"/>
-      <c r="I90" s="28"/>
-      <c r="J90" s="28"/>
-      <c r="K90" s="28"/>
-      <c r="L90" s="28"/>
-      <c r="M90" s="28"/>
-      <c r="N90" s="28"/>
-      <c r="O90" s="28"/>
-      <c r="P90" s="28"/>
+      <c r="A90" s="5">
+        <v>43983</v>
+      </c>
+      <c r="B90" s="28">
+        <v>1061</v>
+      </c>
+      <c r="C90" s="28">
+        <v>325</v>
+      </c>
+      <c r="D90" s="28">
+        <v>260</v>
+      </c>
+      <c r="E90" s="28">
+        <v>836</v>
+      </c>
+      <c r="F90" s="28">
+        <v>931</v>
+      </c>
+      <c r="G90" s="28">
+        <v>1278</v>
+      </c>
+      <c r="H90" s="28">
+        <v>3949</v>
+      </c>
+      <c r="I90" s="28">
+        <v>338</v>
+      </c>
+      <c r="J90" s="28">
+        <v>1987</v>
+      </c>
+      <c r="K90" s="28">
+        <v>2714</v>
+      </c>
+      <c r="L90" s="28">
+        <v>8</v>
+      </c>
+      <c r="M90" s="28">
+        <v>54</v>
+      </c>
+      <c r="N90" s="28">
+        <v>1671</v>
+      </c>
+      <c r="O90" s="28">
+        <v>6</v>
+      </c>
+      <c r="P90" s="32">
+        <v>15418</v>
+      </c>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B91" s="28"/>
@@ -7322,11 +7355,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q78"/>
+  <dimension ref="A1:Q79"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A79" sqref="A79"/>
+      <pane ySplit="3" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H81" sqref="H81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11406,6 +11439,59 @@
         <v>27</v>
       </c>
     </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A79" s="30">
+        <v>43983</v>
+      </c>
+      <c r="B79" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C79" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D79" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E79" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F79" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G79" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H79" s="40">
+        <v>7</v>
+      </c>
+      <c r="I79" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J79" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K79" s="14">
+        <v>5</v>
+      </c>
+      <c r="L79" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M79" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N79" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O79" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P79" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q79" s="13">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -11414,13 +11500,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q70"/>
+  <dimension ref="A1:Q72"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B57" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="O73" sqref="O73"/>
+      <selection pane="bottomRight" activeCell="F72" sqref="F72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15076,6 +15162,75 @@
         <v>732</v>
       </c>
     </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A71" s="51">
+        <v>43983</v>
+      </c>
+      <c r="B71" s="11">
+        <v>13</v>
+      </c>
+      <c r="C71" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D71" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E71" s="14">
+        <v>63</v>
+      </c>
+      <c r="F71" s="14">
+        <v>9</v>
+      </c>
+      <c r="G71" s="14">
+        <v>69</v>
+      </c>
+      <c r="H71" s="14">
+        <v>338</v>
+      </c>
+      <c r="I71" s="14">
+        <v>9</v>
+      </c>
+      <c r="J71" s="14">
+        <v>68</v>
+      </c>
+      <c r="K71" s="14">
+        <v>156</v>
+      </c>
+      <c r="L71" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M71" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N71" s="14">
+        <v>10</v>
+      </c>
+      <c r="O71" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P71" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q71" s="13">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C72" s="14"/>
+      <c r="D72" s="14"/>
+      <c r="E72" s="14"/>
+      <c r="F72" s="14"/>
+      <c r="G72" s="14"/>
+      <c r="H72" s="14"/>
+      <c r="I72" s="14"/>
+      <c r="J72" s="14"/>
+      <c r="K72" s="14"/>
+      <c r="L72" s="14"/>
+      <c r="M72" s="14"/>
+      <c r="N72" s="14"/>
+      <c r="O72" s="14"/>
+      <c r="P72" s="14"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -15084,13 +15239,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q70"/>
+  <dimension ref="A1:Q71"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L88" sqref="L88"/>
+      <selection pane="bottomRight" activeCell="O77" sqref="O77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18744,6 +18899,59 @@
       </c>
       <c r="Q70" s="13">
         <v>341</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A71" s="30">
+        <v>43983</v>
+      </c>
+      <c r="B71" s="14">
+        <v>28</v>
+      </c>
+      <c r="C71" s="14">
+        <v>18</v>
+      </c>
+      <c r="D71" s="14">
+        <v>12</v>
+      </c>
+      <c r="E71" s="14">
+        <v>20</v>
+      </c>
+      <c r="F71" s="14">
+        <v>44</v>
+      </c>
+      <c r="G71" s="14">
+        <v>6</v>
+      </c>
+      <c r="H71" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I71" s="14">
+        <v>23</v>
+      </c>
+      <c r="J71" s="14">
+        <v>57</v>
+      </c>
+      <c r="K71" s="14">
+        <v>83</v>
+      </c>
+      <c r="L71" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M71" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N71" s="14">
+        <v>18</v>
+      </c>
+      <c r="O71" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P71" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q71" s="13">
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -18776,7 +18984,7 @@
       <value order="0"/>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-05-31T12:11:23Z</value>
+      <value order="0">2020-06-01T12:10:15Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -18791,13 +18999,13 @@
       <value order="0">Being Drafted</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41433326</value>
+      <value order="0">vA41452408</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">17.2</value>
+      <value order="0">17.4</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">137</value>
+      <value order="0">139</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-04 20:08)
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u201433\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA1432\A28088333\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u207826\Objective\Objects\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5985" windowHeight="6015" tabRatio="803" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5990" windowHeight="6020" tabRatio="803"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1584" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1605" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -389,7 +389,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -496,6 +496,9 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -526,8 +529,8 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -537,7 +540,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6886575" cy="11677650"/>
+          <a:ext cx="7204075" cy="12357100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -722,23 +725,6 @@
           </a:r>
         </a:p>
         <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
           <a:r>
             <a:rPr lang="en-GB" sz="1100">
               <a:effectLst/>
@@ -746,44 +732,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>4. No data has been received since 12</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" baseline="30000">
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>th</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100">
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> May for tests conducted at the NHS Western Isles lab. This lab sends some samples to other labs for testing and these have contained no positive cases.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100">
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100">
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>5. It should be noted that testing capacity tends to be lower at weekends, and on public holidays.</a:t>
+            <a:t>4. It should be noted that testing capacity tends to be lower at weekends, and on public holidays.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -805,7 +754,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>6. Where errors have been found in previous reported numbers, these have been corrected. </a:t>
+            <a:t>5. Where errors have been found in previous reported numbers, these have been corrected. </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -855,6 +804,34 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" i="0">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>On 4 June, also based on updated postcode information, one case has been reassigned from Highland to Forth Valley. This resulted in a decrease of one in the total number of cases in the Highlands.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
           <a:r>
             <a:rPr lang="en-GB" sz="1100">
               <a:effectLst/>
@@ -873,7 +850,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>7. The data in Table 2, 3a and 3b includes a snapshot of:</a:t>
+            <a:t>6. The data in Table 2, 3a and 3b includes a snapshot of:</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1040,7 +1017,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>8. NHS Boards provide Scottish Government with management information on the numbers of patients in ICU with confirmed or suspected COVID-19 at midnight – this is intended to provide information on patients receiving ICU level 3 care. A small number of NHS Boards have some combined ICU/HDU units and provide information on those units. For example NHS Tayside had included a standalone HDU in returns before 7</a:t>
+            <a:t>7. NHS Boards provide Scottish Government with management information on the numbers of patients in ICU with confirmed or suspected COVID-19 at midnight – this is intended to provide information on patients receiving ICU level 3 care. A small number of NHS Boards have some combined ICU/HDU units and provide information on those units. For example NHS Tayside had included a standalone HDU in returns before 7</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" baseline="30000">
@@ -1095,7 +1072,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>9. The number of patients in hospital or ICU reported each day refers to the number of patients overnight, at midnight on the preceding night.</a:t>
+            <a:t>8. The number of patients in hospital or ICU reported each day refers to the number of patients overnight, at midnight on the preceding night.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1117,7 +1094,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>10. Where Boards do not provide their overnight data in time for the daily publication, the previous day’s data will be used and highlighted on each occasion. The figure will be revised the subsequent day to include the correct data. Figures may also be revised if Boards discover an error and have to resubmit their data. </a:t>
+            <a:t>9. Where Boards do not provide their overnight data in time for the daily publication, the previous day’s data will be used and highlighted on each occasion. The figure will be revised the subsequent day to include the correct data. Figures may also be revised if Boards discover an error and have to resubmit their data. </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1234,7 +1211,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>11. Other minor variations in the daily returns from Boards (for tables 2 and 3a and 3b) include:</a:t>
+            <a:t>10. Other minor variations in the daily returns from Boards (for tables 2 and 3a and 3b) include:</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1339,7 +1316,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>12.</a:t>
+            <a:t>11.</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" baseline="0">
@@ -1349,6 +1326,59 @@
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t> For Table 1, the daily total of people found positive on 2/6/20 contains 40 historic samples from an NHS Fife laboratory.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB" sz="1100" baseline="0">
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>12. On 04/06/2020, the number of positive cases in Highland decreased by 1 due to an update to postcode of residence for one case.</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB">
             <a:effectLst/>
@@ -1645,23 +1675,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="90.42578125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.42578125" style="2"/>
+    <col min="2" max="2" width="29.453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="90.453125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B3" s="18" t="s">
         <v>20</v>
       </c>
@@ -1669,7 +1699,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="20" t="s">
         <v>22</v>
       </c>
@@ -1677,13 +1707,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="22" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="23"/>
     </row>
-    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="24" t="s">
         <v>26</v>
       </c>
@@ -1691,7 +1721,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="24" t="s">
         <v>27</v>
       </c>
@@ -1699,7 +1729,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="24" t="s">
         <v>36</v>
       </c>
@@ -1707,7 +1737,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="20" t="s">
         <v>37</v>
       </c>
@@ -1731,16 +1761,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K66" sqref="K66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="9.42578125" style="2"/>
+    <col min="1" max="16384" width="9.453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A44" s="43"/>
     </row>
   </sheetData>
@@ -1755,20 +1785,20 @@
   <dimension ref="A1:S160"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B67" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B75" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E91" sqref="E91"/>
+      <selection pane="bottomRight" activeCell="I94" sqref="I94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" style="2" customWidth="1"/>
-    <col min="2" max="16" width="11.42578125" style="11" customWidth="1"/>
-    <col min="17" max="16384" width="8.5703125" style="2"/>
+    <col min="2" max="16" width="11.453125" style="11" customWidth="1"/>
+    <col min="17" max="16384" width="8.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -1788,7 +1818,7 @@
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -1807,7 +1837,7 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -1857,7 +1887,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>43897</v>
       </c>
@@ -1907,7 +1937,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>43898</v>
       </c>
@@ -1957,7 +1987,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>43899</v>
       </c>
@@ -2007,7 +2037,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>43900</v>
       </c>
@@ -2057,7 +2087,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>43901</v>
       </c>
@@ -2107,7 +2137,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>43902</v>
       </c>
@@ -2157,7 +2187,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>43903</v>
       </c>
@@ -2207,7 +2237,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>43904</v>
       </c>
@@ -2257,7 +2287,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>43905</v>
       </c>
@@ -2307,7 +2337,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>43906</v>
       </c>
@@ -2357,7 +2387,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>43907</v>
       </c>
@@ -2407,7 +2437,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>43908</v>
       </c>
@@ -2457,7 +2487,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>43909</v>
       </c>
@@ -2507,7 +2537,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>43910</v>
       </c>
@@ -2557,7 +2587,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>43911</v>
       </c>
@@ -2607,7 +2637,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>43912</v>
       </c>
@@ -2657,7 +2687,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>43913</v>
       </c>
@@ -2707,7 +2737,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>43914</v>
       </c>
@@ -2757,7 +2787,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>43915</v>
       </c>
@@ -2807,7 +2837,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>43916</v>
       </c>
@@ -2857,7 +2887,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>43917</v>
       </c>
@@ -2907,7 +2937,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>43918</v>
       </c>
@@ -2957,7 +2987,7 @@
         <v>1264</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>43919</v>
       </c>
@@ -3007,7 +3037,7 @@
         <v>1417</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>43920</v>
       </c>
@@ -3057,7 +3087,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>43921</v>
       </c>
@@ -3107,7 +3137,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>43922</v>
       </c>
@@ -3157,7 +3187,7 @@
         <v>2310</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>43923</v>
       </c>
@@ -3207,7 +3237,7 @@
         <v>2602</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>43924</v>
       </c>
@@ -3257,7 +3287,7 @@
         <v>3001</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>43925</v>
       </c>
@@ -3307,7 +3337,7 @@
         <v>3345</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>43926</v>
       </c>
@@ -3357,7 +3387,7 @@
         <v>3706</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>43927</v>
       </c>
@@ -3407,7 +3437,7 @@
         <v>3961</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>43928</v>
       </c>
@@ -3457,7 +3487,7 @@
         <v>4229</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>43929</v>
       </c>
@@ -3507,7 +3537,7 @@
         <v>4565</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>43930</v>
       </c>
@@ -3557,7 +3587,7 @@
         <v>4957</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>43931</v>
       </c>
@@ -3607,7 +3637,7 @@
         <v>5275</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>43932</v>
       </c>
@@ -3657,7 +3687,7 @@
         <v>5590</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>43933</v>
       </c>
@@ -3707,7 +3737,7 @@
         <v>5912</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>43934</v>
       </c>
@@ -3757,7 +3787,7 @@
         <v>6067</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>43935</v>
       </c>
@@ -3807,7 +3837,7 @@
         <v>6358</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>43936</v>
       </c>
@@ -3857,7 +3887,7 @@
         <v>6748</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
         <v>43937</v>
       </c>
@@ -3907,7 +3937,7 @@
         <v>7102</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>43938</v>
       </c>
@@ -3957,7 +3987,7 @@
         <v>7409</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A46" s="5">
         <v>43939</v>
       </c>
@@ -4007,7 +4037,7 @@
         <v>7820</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A47" s="5">
         <v>43940</v>
       </c>
@@ -4057,7 +4087,7 @@
         <v>8187</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A48" s="5">
         <v>43941</v>
       </c>
@@ -4107,7 +4137,7 @@
         <v>8450</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A49" s="5">
         <v>43942</v>
       </c>
@@ -4157,7 +4187,7 @@
         <v>8672</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
         <v>43943</v>
       </c>
@@ -4207,7 +4237,7 @@
         <v>9038</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
         <v>43944</v>
       </c>
@@ -4257,7 +4287,7 @@
         <v>9409</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
         <v>43945</v>
       </c>
@@ -4307,7 +4337,7 @@
         <v>9697</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
         <v>43946</v>
       </c>
@@ -4357,7 +4387,7 @@
         <v>10051</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A54" s="5">
         <v>43947</v>
       </c>
@@ -4408,7 +4438,7 @@
       </c>
       <c r="R54" s="38"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
         <v>43948</v>
       </c>
@@ -4459,7 +4489,7 @@
       </c>
       <c r="R55" s="38"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A56" s="5">
         <v>43949</v>
       </c>
@@ -4510,7 +4540,7 @@
       </c>
       <c r="R56" s="39"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
         <v>43950</v>
       </c>
@@ -4560,7 +4590,7 @@
         <v>11034</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
         <v>43951</v>
       </c>
@@ -4611,7 +4641,7 @@
       </c>
       <c r="R58" s="38"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>43952</v>
       </c>
@@ -4663,7 +4693,7 @@
       <c r="R59" s="38"/>
       <c r="S59" s="38"/>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
         <v>43953</v>
       </c>
@@ -4713,7 +4743,7 @@
         <v>11927</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
         <v>43954</v>
       </c>
@@ -4763,7 +4793,7 @@
         <v>12097</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A62" s="5">
         <v>43955</v>
       </c>
@@ -4813,7 +4843,7 @@
         <v>12266</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A63" s="5">
         <v>43956</v>
       </c>
@@ -4863,7 +4893,7 @@
         <v>12437</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
         <v>43957</v>
       </c>
@@ -4913,7 +4943,7 @@
         <v>12709</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>43958</v>
       </c>
@@ -4963,7 +4993,7 @@
         <v>12924</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
         <v>43959</v>
       </c>
@@ -5013,7 +5043,7 @@
         <v>13149</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
         <v>43960</v>
       </c>
@@ -5063,7 +5093,7 @@
         <v>13305</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A68" s="5">
         <v>43961</v>
       </c>
@@ -5113,7 +5143,7 @@
         <v>13486</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A69" s="5">
         <v>43962</v>
       </c>
@@ -5163,7 +5193,7 @@
         <v>13627</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A70" s="5">
         <v>43963</v>
       </c>
@@ -5213,7 +5243,7 @@
         <v>13763</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A71" s="5">
         <v>43964</v>
       </c>
@@ -5263,7 +5293,7 @@
         <v>13929</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A72" s="5">
         <v>43965</v>
       </c>
@@ -5313,7 +5343,7 @@
         <v>14117</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A73" s="5">
         <v>43966</v>
       </c>
@@ -5363,7 +5393,7 @@
         <v>14260</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A74" s="5">
         <v>43967</v>
       </c>
@@ -5413,7 +5443,7 @@
         <v>14447</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A75" s="5">
         <v>43968</v>
       </c>
@@ -5463,7 +5493,7 @@
         <v>14537</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A76" s="5">
         <v>43969</v>
       </c>
@@ -5513,7 +5543,7 @@
         <v>14594</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A77" s="5">
         <v>43970</v>
       </c>
@@ -5563,7 +5593,7 @@
         <v>14655</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A78" s="5">
         <v>43971</v>
       </c>
@@ -5613,7 +5643,7 @@
         <v>14751</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A79" s="5">
         <v>43972</v>
       </c>
@@ -5663,7 +5693,7 @@
         <v>14856</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A80" s="5">
         <v>43973</v>
       </c>
@@ -5713,7 +5743,7 @@
         <v>14969</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A81" s="5">
         <v>43974</v>
       </c>
@@ -5763,7 +5793,7 @@
         <v>15041</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A82" s="5">
         <v>43975</v>
       </c>
@@ -5813,7 +5843,7 @@
         <v>15101</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A83" s="5">
         <v>43976</v>
       </c>
@@ -5863,7 +5893,7 @@
         <v>15156</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A84" s="5">
         <v>43977</v>
       </c>
@@ -5913,7 +5943,7 @@
         <v>15185</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A85" s="5">
         <v>43978</v>
       </c>
@@ -5963,7 +5993,7 @@
         <v>15240</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A86" s="5">
         <v>43979</v>
       </c>
@@ -6013,7 +6043,7 @@
         <v>15288</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A87" s="5">
         <v>43980</v>
       </c>
@@ -6063,7 +6093,7 @@
         <v>15327</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A88" s="5">
         <v>43981</v>
       </c>
@@ -6113,7 +6143,7 @@
         <v>15382</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A89" s="5">
         <v>43982</v>
       </c>
@@ -6163,7 +6193,7 @@
         <v>15400</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A90" s="5">
         <v>43983</v>
       </c>
@@ -6213,7 +6243,7 @@
         <v>15418</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A91" s="5">
         <v>43984</v>
       </c>
@@ -6263,7 +6293,7 @@
         <v>15471</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A92" s="5">
         <v>43985</v>
       </c>
@@ -6313,24 +6343,57 @@
         <v>15504</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B93" s="28"/>
-      <c r="C93" s="28"/>
-      <c r="D93" s="28"/>
-      <c r="E93" s="28"/>
-      <c r="F93" s="28"/>
-      <c r="G93" s="28"/>
-      <c r="H93" s="28"/>
-      <c r="I93" s="28"/>
-      <c r="J93" s="28"/>
-      <c r="K93" s="28"/>
-      <c r="L93" s="28"/>
-      <c r="M93" s="28"/>
-      <c r="N93" s="28"/>
-      <c r="O93" s="28"/>
-      <c r="P93" s="28"/>
-    </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A93" s="5">
+        <v>43986</v>
+      </c>
+      <c r="B93" s="28">
+        <v>1071</v>
+      </c>
+      <c r="C93" s="28">
+        <v>325</v>
+      </c>
+      <c r="D93" s="28">
+        <v>261</v>
+      </c>
+      <c r="E93" s="28">
+        <v>877</v>
+      </c>
+      <c r="F93" s="28">
+        <v>944</v>
+      </c>
+      <c r="G93" s="28">
+        <v>1283</v>
+      </c>
+      <c r="H93" s="28">
+        <v>3961</v>
+      </c>
+      <c r="I93" s="52">
+        <v>338</v>
+      </c>
+      <c r="J93" s="28">
+        <v>2002</v>
+      </c>
+      <c r="K93" s="28">
+        <v>2752</v>
+      </c>
+      <c r="L93" s="28">
+        <v>8</v>
+      </c>
+      <c r="M93" s="28">
+        <v>54</v>
+      </c>
+      <c r="N93" s="28">
+        <v>1671</v>
+      </c>
+      <c r="O93" s="28">
+        <v>6</v>
+      </c>
+      <c r="P93" s="32">
+        <v>15553</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B94" s="28"/>
       <c r="C94" s="28"/>
       <c r="D94" s="28"/>
@@ -6347,7 +6410,7 @@
       <c r="O94" s="28"/>
       <c r="P94" s="28"/>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B95" s="28"/>
       <c r="C95" s="28"/>
       <c r="D95" s="28"/>
@@ -6364,7 +6427,7 @@
       <c r="O95" s="28"/>
       <c r="P95" s="28"/>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B96" s="28"/>
       <c r="C96" s="28"/>
       <c r="D96" s="28"/>
@@ -6381,7 +6444,7 @@
       <c r="O96" s="28"/>
       <c r="P96" s="28"/>
     </row>
-    <row r="97" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B97" s="28"/>
       <c r="C97" s="28"/>
       <c r="D97" s="28"/>
@@ -6398,7 +6461,7 @@
       <c r="O97" s="28"/>
       <c r="P97" s="28"/>
     </row>
-    <row r="98" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B98" s="28"/>
       <c r="C98" s="28"/>
       <c r="D98" s="28"/>
@@ -6415,7 +6478,7 @@
       <c r="O98" s="28"/>
       <c r="P98" s="28"/>
     </row>
-    <row r="99" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B99" s="28"/>
       <c r="C99" s="28"/>
       <c r="D99" s="28"/>
@@ -6432,7 +6495,7 @@
       <c r="O99" s="28"/>
       <c r="P99" s="28"/>
     </row>
-    <row r="100" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B100" s="28"/>
       <c r="C100" s="28"/>
       <c r="D100" s="28"/>
@@ -6449,7 +6512,7 @@
       <c r="O100" s="28"/>
       <c r="P100" s="28"/>
     </row>
-    <row r="101" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B101" s="28"/>
       <c r="C101" s="28"/>
       <c r="D101" s="28"/>
@@ -6466,7 +6529,7 @@
       <c r="O101" s="28"/>
       <c r="P101" s="28"/>
     </row>
-    <row r="102" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B102" s="28"/>
       <c r="C102" s="28"/>
       <c r="D102" s="28"/>
@@ -6483,7 +6546,7 @@
       <c r="O102" s="28"/>
       <c r="P102" s="28"/>
     </row>
-    <row r="103" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B103" s="28"/>
       <c r="C103" s="28"/>
       <c r="D103" s="28"/>
@@ -6500,7 +6563,7 @@
       <c r="O103" s="28"/>
       <c r="P103" s="28"/>
     </row>
-    <row r="104" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B104" s="28"/>
       <c r="C104" s="28"/>
       <c r="D104" s="28"/>
@@ -6517,7 +6580,7 @@
       <c r="O104" s="28"/>
       <c r="P104" s="28"/>
     </row>
-    <row r="105" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B105" s="28"/>
       <c r="C105" s="28"/>
       <c r="D105" s="28"/>
@@ -6534,7 +6597,7 @@
       <c r="O105" s="28"/>
       <c r="P105" s="28"/>
     </row>
-    <row r="106" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B106" s="28"/>
       <c r="C106" s="28"/>
       <c r="D106" s="28"/>
@@ -6551,7 +6614,7 @@
       <c r="O106" s="28"/>
       <c r="P106" s="28"/>
     </row>
-    <row r="107" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B107" s="28"/>
       <c r="C107" s="28"/>
       <c r="D107" s="28"/>
@@ -6568,7 +6631,7 @@
       <c r="O107" s="28"/>
       <c r="P107" s="28"/>
     </row>
-    <row r="108" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B108" s="28"/>
       <c r="C108" s="28"/>
       <c r="D108" s="28"/>
@@ -6585,7 +6648,7 @@
       <c r="O108" s="28"/>
       <c r="P108" s="28"/>
     </row>
-    <row r="109" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B109" s="28"/>
       <c r="C109" s="28"/>
       <c r="D109" s="28"/>
@@ -6602,7 +6665,7 @@
       <c r="O109" s="28"/>
       <c r="P109" s="28"/>
     </row>
-    <row r="110" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B110" s="28"/>
       <c r="C110" s="28"/>
       <c r="D110" s="28"/>
@@ -6619,7 +6682,7 @@
       <c r="O110" s="28"/>
       <c r="P110" s="28"/>
     </row>
-    <row r="111" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B111" s="28"/>
       <c r="C111" s="28"/>
       <c r="D111" s="28"/>
@@ -6636,7 +6699,7 @@
       <c r="O111" s="28"/>
       <c r="P111" s="28"/>
     </row>
-    <row r="112" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B112" s="28"/>
       <c r="C112" s="28"/>
       <c r="D112" s="28"/>
@@ -6653,7 +6716,7 @@
       <c r="O112" s="28"/>
       <c r="P112" s="28"/>
     </row>
-    <row r="113" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B113" s="28"/>
       <c r="C113" s="28"/>
       <c r="D113" s="28"/>
@@ -6670,7 +6733,7 @@
       <c r="O113" s="28"/>
       <c r="P113" s="28"/>
     </row>
-    <row r="114" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B114" s="28"/>
       <c r="C114" s="28"/>
       <c r="D114" s="28"/>
@@ -6687,7 +6750,7 @@
       <c r="O114" s="28"/>
       <c r="P114" s="28"/>
     </row>
-    <row r="115" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B115" s="28"/>
       <c r="C115" s="28"/>
       <c r="D115" s="28"/>
@@ -6704,7 +6767,7 @@
       <c r="O115" s="28"/>
       <c r="P115" s="28"/>
     </row>
-    <row r="116" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B116" s="28"/>
       <c r="C116" s="28"/>
       <c r="D116" s="28"/>
@@ -6721,7 +6784,7 @@
       <c r="O116" s="28"/>
       <c r="P116" s="28"/>
     </row>
-    <row r="117" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B117" s="28"/>
       <c r="C117" s="28"/>
       <c r="D117" s="28"/>
@@ -6738,7 +6801,7 @@
       <c r="O117" s="28"/>
       <c r="P117" s="28"/>
     </row>
-    <row r="118" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B118" s="28"/>
       <c r="C118" s="28"/>
       <c r="D118" s="28"/>
@@ -6755,7 +6818,7 @@
       <c r="O118" s="28"/>
       <c r="P118" s="28"/>
     </row>
-    <row r="119" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B119" s="28"/>
       <c r="C119" s="28"/>
       <c r="D119" s="28"/>
@@ -6772,7 +6835,7 @@
       <c r="O119" s="28"/>
       <c r="P119" s="28"/>
     </row>
-    <row r="120" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B120" s="28"/>
       <c r="C120" s="28"/>
       <c r="D120" s="28"/>
@@ -6789,7 +6852,7 @@
       <c r="O120" s="28"/>
       <c r="P120" s="28"/>
     </row>
-    <row r="121" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B121" s="28"/>
       <c r="C121" s="28"/>
       <c r="D121" s="28"/>
@@ -6806,7 +6869,7 @@
       <c r="O121" s="28"/>
       <c r="P121" s="28"/>
     </row>
-    <row r="122" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B122" s="28"/>
       <c r="C122" s="28"/>
       <c r="D122" s="28"/>
@@ -6823,7 +6886,7 @@
       <c r="O122" s="28"/>
       <c r="P122" s="28"/>
     </row>
-    <row r="123" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B123" s="28"/>
       <c r="C123" s="28"/>
       <c r="D123" s="28"/>
@@ -6840,7 +6903,7 @@
       <c r="O123" s="28"/>
       <c r="P123" s="28"/>
     </row>
-    <row r="124" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B124" s="28"/>
       <c r="C124" s="28"/>
       <c r="D124" s="28"/>
@@ -6857,7 +6920,7 @@
       <c r="O124" s="28"/>
       <c r="P124" s="28"/>
     </row>
-    <row r="125" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B125" s="28"/>
       <c r="C125" s="28"/>
       <c r="D125" s="28"/>
@@ -6874,7 +6937,7 @@
       <c r="O125" s="28"/>
       <c r="P125" s="28"/>
     </row>
-    <row r="126" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B126" s="28"/>
       <c r="C126" s="28"/>
       <c r="D126" s="28"/>
@@ -6891,7 +6954,7 @@
       <c r="O126" s="28"/>
       <c r="P126" s="28"/>
     </row>
-    <row r="127" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B127" s="28"/>
       <c r="C127" s="28"/>
       <c r="D127" s="28"/>
@@ -6908,7 +6971,7 @@
       <c r="O127" s="28"/>
       <c r="P127" s="28"/>
     </row>
-    <row r="128" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B128" s="28"/>
       <c r="C128" s="28"/>
       <c r="D128" s="28"/>
@@ -6925,7 +6988,7 @@
       <c r="O128" s="28"/>
       <c r="P128" s="28"/>
     </row>
-    <row r="129" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B129" s="28"/>
       <c r="C129" s="28"/>
       <c r="D129" s="28"/>
@@ -6942,7 +7005,7 @@
       <c r="O129" s="28"/>
       <c r="P129" s="28"/>
     </row>
-    <row r="130" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B130" s="28"/>
       <c r="C130" s="28"/>
       <c r="D130" s="28"/>
@@ -6959,7 +7022,7 @@
       <c r="O130" s="28"/>
       <c r="P130" s="28"/>
     </row>
-    <row r="131" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B131" s="28"/>
       <c r="C131" s="28"/>
       <c r="D131" s="28"/>
@@ -6976,7 +7039,7 @@
       <c r="O131" s="28"/>
       <c r="P131" s="28"/>
     </row>
-    <row r="132" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B132" s="28"/>
       <c r="C132" s="28"/>
       <c r="D132" s="28"/>
@@ -6993,7 +7056,7 @@
       <c r="O132" s="28"/>
       <c r="P132" s="28"/>
     </row>
-    <row r="133" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B133" s="28"/>
       <c r="C133" s="28"/>
       <c r="D133" s="28"/>
@@ -7010,7 +7073,7 @@
       <c r="O133" s="28"/>
       <c r="P133" s="28"/>
     </row>
-    <row r="134" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B134" s="28"/>
       <c r="C134" s="28"/>
       <c r="D134" s="28"/>
@@ -7027,7 +7090,7 @@
       <c r="O134" s="28"/>
       <c r="P134" s="28"/>
     </row>
-    <row r="135" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B135" s="28"/>
       <c r="C135" s="28"/>
       <c r="D135" s="28"/>
@@ -7044,7 +7107,7 @@
       <c r="O135" s="28"/>
       <c r="P135" s="28"/>
     </row>
-    <row r="136" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B136" s="28"/>
       <c r="C136" s="28"/>
       <c r="D136" s="28"/>
@@ -7061,7 +7124,7 @@
       <c r="O136" s="28"/>
       <c r="P136" s="28"/>
     </row>
-    <row r="137" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B137" s="28"/>
       <c r="C137" s="28"/>
       <c r="D137" s="28"/>
@@ -7078,7 +7141,7 @@
       <c r="O137" s="28"/>
       <c r="P137" s="28"/>
     </row>
-    <row r="138" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B138" s="28"/>
       <c r="C138" s="28"/>
       <c r="D138" s="28"/>
@@ -7095,7 +7158,7 @@
       <c r="O138" s="28"/>
       <c r="P138" s="28"/>
     </row>
-    <row r="139" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B139" s="28"/>
       <c r="C139" s="28"/>
       <c r="D139" s="28"/>
@@ -7112,7 +7175,7 @@
       <c r="O139" s="28"/>
       <c r="P139" s="28"/>
     </row>
-    <row r="140" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B140" s="28"/>
       <c r="C140" s="28"/>
       <c r="D140" s="28"/>
@@ -7129,7 +7192,7 @@
       <c r="O140" s="28"/>
       <c r="P140" s="28"/>
     </row>
-    <row r="141" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B141" s="28"/>
       <c r="C141" s="28"/>
       <c r="D141" s="28"/>
@@ -7146,7 +7209,7 @@
       <c r="O141" s="28"/>
       <c r="P141" s="28"/>
     </row>
-    <row r="142" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B142" s="28"/>
       <c r="C142" s="28"/>
       <c r="D142" s="28"/>
@@ -7163,7 +7226,7 @@
       <c r="O142" s="28"/>
       <c r="P142" s="28"/>
     </row>
-    <row r="143" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B143" s="28"/>
       <c r="C143" s="28"/>
       <c r="D143" s="28"/>
@@ -7180,7 +7243,7 @@
       <c r="O143" s="28"/>
       <c r="P143" s="28"/>
     </row>
-    <row r="144" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B144" s="28"/>
       <c r="C144" s="28"/>
       <c r="D144" s="28"/>
@@ -7197,7 +7260,7 @@
       <c r="O144" s="28"/>
       <c r="P144" s="28"/>
     </row>
-    <row r="145" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B145" s="28"/>
       <c r="C145" s="28"/>
       <c r="D145" s="28"/>
@@ -7214,7 +7277,7 @@
       <c r="O145" s="28"/>
       <c r="P145" s="28"/>
     </row>
-    <row r="146" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B146" s="28"/>
       <c r="C146" s="28"/>
       <c r="D146" s="28"/>
@@ -7231,7 +7294,7 @@
       <c r="O146" s="28"/>
       <c r="P146" s="28"/>
     </row>
-    <row r="147" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B147" s="28"/>
       <c r="C147" s="28"/>
       <c r="D147" s="28"/>
@@ -7248,7 +7311,7 @@
       <c r="O147" s="28"/>
       <c r="P147" s="28"/>
     </row>
-    <row r="148" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B148" s="28"/>
       <c r="C148" s="28"/>
       <c r="D148" s="28"/>
@@ -7265,7 +7328,7 @@
       <c r="O148" s="28"/>
       <c r="P148" s="28"/>
     </row>
-    <row r="149" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B149" s="28"/>
       <c r="C149" s="28"/>
       <c r="D149" s="28"/>
@@ -7282,7 +7345,7 @@
       <c r="O149" s="28"/>
       <c r="P149" s="28"/>
     </row>
-    <row r="150" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B150" s="28"/>
       <c r="C150" s="28"/>
       <c r="D150" s="28"/>
@@ -7299,7 +7362,7 @@
       <c r="O150" s="28"/>
       <c r="P150" s="28"/>
     </row>
-    <row r="151" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B151" s="28"/>
       <c r="C151" s="28"/>
       <c r="D151" s="28"/>
@@ -7316,7 +7379,7 @@
       <c r="O151" s="28"/>
       <c r="P151" s="28"/>
     </row>
-    <row r="152" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B152" s="28"/>
       <c r="C152" s="28"/>
       <c r="D152" s="28"/>
@@ -7333,7 +7396,7 @@
       <c r="O152" s="28"/>
       <c r="P152" s="28"/>
     </row>
-    <row r="153" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B153" s="28"/>
       <c r="C153" s="28"/>
       <c r="D153" s="28"/>
@@ -7350,7 +7413,7 @@
       <c r="O153" s="28"/>
       <c r="P153" s="28"/>
     </row>
-    <row r="154" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B154" s="28"/>
       <c r="C154" s="28"/>
       <c r="D154" s="28"/>
@@ -7367,7 +7430,7 @@
       <c r="O154" s="28"/>
       <c r="P154" s="28"/>
     </row>
-    <row r="155" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B155" s="28"/>
       <c r="C155" s="28"/>
       <c r="D155" s="28"/>
@@ -7384,7 +7447,7 @@
       <c r="O155" s="28"/>
       <c r="P155" s="28"/>
     </row>
-    <row r="156" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B156" s="28"/>
       <c r="C156" s="28"/>
       <c r="D156" s="28"/>
@@ -7401,7 +7464,7 @@
       <c r="O156" s="28"/>
       <c r="P156" s="28"/>
     </row>
-    <row r="157" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B157" s="28"/>
       <c r="C157" s="28"/>
       <c r="D157" s="28"/>
@@ -7418,7 +7481,7 @@
       <c r="O157" s="28"/>
       <c r="P157" s="28"/>
     </row>
-    <row r="158" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B158" s="28"/>
       <c r="C158" s="28"/>
       <c r="D158" s="28"/>
@@ -7435,7 +7498,7 @@
       <c r="O158" s="28"/>
       <c r="P158" s="28"/>
     </row>
-    <row r="159" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B159" s="28"/>
       <c r="C159" s="28"/>
       <c r="D159" s="28"/>
@@ -7452,7 +7515,7 @@
       <c r="O159" s="28"/>
       <c r="P159" s="28"/>
     </row>
-    <row r="160" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B160" s="28"/>
       <c r="C160" s="28"/>
       <c r="D160" s="28"/>
@@ -7477,21 +7540,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q81"/>
+  <dimension ref="A1:Q82"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N80" sqref="N80"/>
+      <pane ySplit="3" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P85" sqref="P85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5703125" style="2"/>
+    <col min="1" max="1" width="12.453125" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.54296875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -7512,7 +7575,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -7533,7 +7596,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -7586,7 +7649,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="12">
         <v>43908</v>
       </c>
@@ -7639,7 +7702,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
         <v>43909</v>
       </c>
@@ -7692,7 +7755,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="12">
         <v>43910</v>
       </c>
@@ -7745,7 +7808,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
         <v>43911</v>
       </c>
@@ -7798,7 +7861,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="12">
         <v>43912</v>
       </c>
@@ -7851,7 +7914,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="12">
         <v>43913</v>
       </c>
@@ -7904,7 +7967,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="12">
         <v>43914</v>
       </c>
@@ -7957,7 +8020,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
         <v>43915</v>
       </c>
@@ -8010,7 +8073,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="12">
         <v>43916</v>
       </c>
@@ -8063,7 +8126,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <v>43917</v>
       </c>
@@ -8116,7 +8179,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>43918</v>
       </c>
@@ -8169,7 +8232,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="12">
         <v>43919</v>
       </c>
@@ -8222,7 +8285,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="12">
         <v>43920</v>
       </c>
@@ -8275,7 +8338,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="12">
         <v>43921</v>
       </c>
@@ -8328,7 +8391,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="12">
         <v>43922</v>
       </c>
@@ -8381,7 +8444,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="12">
         <v>43923</v>
       </c>
@@ -8434,7 +8497,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="12">
         <v>43924</v>
       </c>
@@ -8487,7 +8550,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="12">
         <v>43925</v>
       </c>
@@ -8540,7 +8603,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="12">
         <v>43926</v>
       </c>
@@ -8593,7 +8656,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="12">
         <v>43927</v>
       </c>
@@ -8646,7 +8709,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" s="12">
         <v>43928</v>
       </c>
@@ -8699,7 +8762,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" s="12">
         <v>43929</v>
       </c>
@@ -8752,7 +8815,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" s="12">
         <v>43930</v>
       </c>
@@ -8805,7 +8868,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" s="12">
         <v>43931</v>
       </c>
@@ -8858,7 +8921,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" s="12">
         <v>43932</v>
       </c>
@@ -8911,7 +8974,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" s="12">
         <v>43933</v>
       </c>
@@ -8964,7 +9027,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" s="12">
         <v>43934</v>
       </c>
@@ -9017,7 +9080,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="12">
         <v>43935</v>
       </c>
@@ -9070,7 +9133,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" s="12">
         <v>43936</v>
       </c>
@@ -9123,7 +9186,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" s="12">
         <v>43937</v>
       </c>
@@ -9176,7 +9239,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" s="12">
         <v>43938</v>
       </c>
@@ -9229,7 +9292,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" s="12">
         <v>43939</v>
       </c>
@@ -9282,7 +9345,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" s="30">
         <v>43940</v>
       </c>
@@ -9335,7 +9398,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" s="30">
         <v>43941</v>
       </c>
@@ -9388,7 +9451,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" s="30">
         <v>43942</v>
       </c>
@@ -9441,7 +9504,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" s="30">
         <v>43943</v>
       </c>
@@ -9494,7 +9557,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" s="30">
         <v>43944</v>
       </c>
@@ -9547,7 +9610,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" s="30">
         <v>43945</v>
       </c>
@@ -9600,7 +9663,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" s="30">
         <v>43946</v>
       </c>
@@ -9653,7 +9716,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" s="30">
         <v>43947</v>
       </c>
@@ -9706,7 +9769,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" s="30">
         <v>43948</v>
       </c>
@@ -9759,7 +9822,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" s="30">
         <v>43949</v>
       </c>
@@ -9812,7 +9875,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" s="30">
         <v>43950</v>
       </c>
@@ -9865,7 +9928,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" s="30">
         <v>43951</v>
       </c>
@@ -9918,7 +9981,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" s="30">
         <v>43952</v>
       </c>
@@ -9971,7 +10034,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" s="30">
         <v>43953</v>
       </c>
@@ -10024,7 +10087,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50" s="30">
         <v>43954</v>
       </c>
@@ -10077,7 +10140,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51" s="30">
         <v>43955</v>
       </c>
@@ -10130,7 +10193,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52" s="30">
         <v>43956</v>
       </c>
@@ -10183,7 +10246,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53" s="30">
         <v>43957</v>
       </c>
@@ -10236,7 +10299,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54" s="30">
         <v>43958</v>
       </c>
@@ -10289,7 +10352,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55" s="30">
         <v>43959</v>
       </c>
@@ -10342,7 +10405,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56" s="30">
         <v>43960</v>
       </c>
@@ -10395,7 +10458,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A57" s="30">
         <v>43961</v>
       </c>
@@ -10448,7 +10511,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A58" s="30">
         <v>43962</v>
       </c>
@@ -10501,7 +10564,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A59" s="30">
         <v>43963</v>
       </c>
@@ -10554,7 +10617,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A60" s="30">
         <v>43964</v>
       </c>
@@ -10607,7 +10670,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A61" s="30">
         <v>43965</v>
       </c>
@@ -10660,7 +10723,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A62" s="30">
         <v>43966</v>
       </c>
@@ -10713,7 +10776,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A63" s="30">
         <v>43967</v>
       </c>
@@ -10766,7 +10829,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A64" s="30">
         <v>43968</v>
       </c>
@@ -10819,7 +10882,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A65" s="30">
         <v>43969</v>
       </c>
@@ -10872,7 +10935,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A66" s="30">
         <v>43970</v>
       </c>
@@ -10925,7 +10988,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A67" s="30">
         <v>43971</v>
       </c>
@@ -10978,7 +11041,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A68" s="30">
         <v>43972</v>
       </c>
@@ -11031,7 +11094,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A69" s="30">
         <v>43973</v>
       </c>
@@ -11084,7 +11147,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A70" s="30">
         <v>43974</v>
       </c>
@@ -11137,7 +11200,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A71" s="30">
         <v>43975</v>
       </c>
@@ -11190,7 +11253,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A72" s="30">
         <v>43976</v>
       </c>
@@ -11243,7 +11306,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A73" s="30">
         <v>43977</v>
       </c>
@@ -11296,7 +11359,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A74" s="30">
         <v>43978</v>
       </c>
@@ -11349,7 +11412,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A75" s="30">
         <v>43979</v>
       </c>
@@ -11402,7 +11465,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A76" s="30">
         <v>43980</v>
       </c>
@@ -11455,7 +11518,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A77" s="30">
         <v>43981</v>
       </c>
@@ -11508,7 +11571,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A78" s="30">
         <v>43982</v>
       </c>
@@ -11561,7 +11624,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A79" s="30">
         <v>43983</v>
       </c>
@@ -11614,7 +11677,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A80" s="30">
         <v>43984</v>
       </c>
@@ -11667,7 +11730,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A81" s="30">
         <v>43985</v>
       </c>
@@ -11718,6 +11781,59 @@
       </c>
       <c r="Q81" s="13">
         <v>34</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A82" s="30">
+        <v>43986</v>
+      </c>
+      <c r="B82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H82" s="11">
+        <v>5</v>
+      </c>
+      <c r="I82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J82" s="11">
+        <v>6</v>
+      </c>
+      <c r="K82" s="11">
+        <v>5</v>
+      </c>
+      <c r="L82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P82" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q82" s="13">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -11728,23 +11844,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q73"/>
+  <dimension ref="A1:Q74"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B51" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="L61" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K74" sqref="K74"/>
+      <selection pane="bottomRight" activeCell="Q75" sqref="Q75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5703125" style="2"/>
+    <col min="1" max="1" width="15.1796875" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.54296875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -11765,7 +11881,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -11786,7 +11902,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -11839,7 +11955,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="12">
         <v>43916</v>
       </c>
@@ -11892,7 +12008,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
         <v>43917</v>
       </c>
@@ -11945,7 +12061,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="12">
         <v>43918</v>
       </c>
@@ -11998,7 +12114,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
         <v>43919</v>
       </c>
@@ -12051,7 +12167,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="12">
         <v>43920</v>
       </c>
@@ -12104,7 +12220,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="12">
         <v>43921</v>
       </c>
@@ -12157,7 +12273,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="12">
         <v>43922</v>
       </c>
@@ -12210,7 +12326,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
         <v>43923</v>
       </c>
@@ -12263,7 +12379,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="12">
         <v>43924</v>
       </c>
@@ -12316,7 +12432,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <v>43925</v>
       </c>
@@ -12369,7 +12485,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>43926</v>
       </c>
@@ -12422,7 +12538,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="12">
         <v>43927</v>
       </c>
@@ -12475,7 +12591,7 @@
         <v>1262</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="12">
         <v>43928</v>
       </c>
@@ -12528,7 +12644,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="12">
         <v>43929</v>
       </c>
@@ -12581,7 +12697,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="12">
         <v>43930</v>
       </c>
@@ -12634,7 +12750,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="12">
         <v>43931</v>
       </c>
@@ -12687,7 +12803,7 @@
         <v>1461</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="12">
         <v>43932</v>
       </c>
@@ -12740,7 +12856,7 @@
         <v>1467</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="12">
         <v>43933</v>
       </c>
@@ -12793,7 +12909,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="12">
         <v>43934</v>
       </c>
@@ -12846,7 +12962,7 @@
         <v>1482</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="12">
         <v>43935</v>
       </c>
@@ -12899,7 +13015,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" s="12">
         <v>43936</v>
       </c>
@@ -12952,7 +13068,7 @@
         <v>1486</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" s="12">
         <v>43937</v>
       </c>
@@ -13005,7 +13121,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" s="12">
         <v>43938</v>
       </c>
@@ -13058,7 +13174,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" s="12">
         <v>43939</v>
       </c>
@@ -13111,7 +13227,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" s="12">
         <v>43940</v>
       </c>
@@ -13164,7 +13280,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" s="12">
         <v>43941</v>
       </c>
@@ -13217,7 +13333,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" s="12">
         <v>43942</v>
       </c>
@@ -13270,7 +13386,7 @@
         <v>1472</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="12">
         <v>43943</v>
       </c>
@@ -13323,7 +13439,7 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" s="12">
         <v>43944</v>
       </c>
@@ -13376,7 +13492,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" s="12">
         <v>43945</v>
       </c>
@@ -13429,7 +13545,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" s="12">
         <v>43946</v>
       </c>
@@ -13482,7 +13598,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" s="12">
         <v>43947</v>
       </c>
@@ -13535,7 +13651,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" s="30">
         <v>43948</v>
       </c>
@@ -13588,7 +13704,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" s="30">
         <v>43949</v>
       </c>
@@ -13641,7 +13757,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" s="30">
         <v>43950</v>
       </c>
@@ -13694,7 +13810,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" s="30">
         <v>43951</v>
       </c>
@@ -13747,7 +13863,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" s="30">
         <v>43952</v>
       </c>
@@ -13800,7 +13916,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" s="30">
         <v>43953</v>
       </c>
@@ -13853,7 +13969,7 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" s="30">
         <v>43954</v>
       </c>
@@ -13906,7 +14022,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" s="30">
         <v>43955</v>
       </c>
@@ -13959,7 +14075,7 @@
         <v>1279</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" s="30">
         <v>43956</v>
       </c>
@@ -14012,7 +14128,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" s="30">
         <v>43957</v>
       </c>
@@ -14065,7 +14181,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" s="30">
         <v>43958</v>
       </c>
@@ -14118,7 +14234,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" s="30">
         <v>43959</v>
       </c>
@@ -14171,7 +14287,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" s="30">
         <v>43960</v>
       </c>
@@ -14224,7 +14340,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" s="30">
         <v>43961</v>
       </c>
@@ -14277,7 +14393,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50" s="30">
         <v>43962</v>
       </c>
@@ -14330,7 +14446,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51" s="30">
         <v>43963</v>
       </c>
@@ -14383,7 +14499,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52" s="30">
         <v>43964</v>
       </c>
@@ -14436,7 +14552,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53" s="30">
         <v>43965</v>
       </c>
@@ -14489,7 +14605,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54" s="30">
         <v>43966</v>
       </c>
@@ -14542,7 +14658,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55" s="30">
         <v>43967</v>
       </c>
@@ -14595,7 +14711,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56" s="30">
         <v>43968</v>
       </c>
@@ -14648,7 +14764,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A57" s="30">
         <v>43969</v>
       </c>
@@ -14701,7 +14817,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A58" s="30">
         <v>43970</v>
       </c>
@@ -14754,7 +14870,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A59" s="30">
         <v>43971</v>
       </c>
@@ -14807,7 +14923,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A60" s="30">
         <v>43972</v>
       </c>
@@ -14860,7 +14976,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A61" s="30">
         <v>43973</v>
       </c>
@@ -14913,7 +15029,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A62" s="30">
         <v>43974</v>
       </c>
@@ -14966,7 +15082,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A63" s="30">
         <v>43975</v>
       </c>
@@ -15019,7 +15135,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A64" s="30">
         <v>43976</v>
       </c>
@@ -15072,7 +15188,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A65" s="51">
         <v>43977</v>
       </c>
@@ -15125,7 +15241,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A66" s="51">
         <v>43978</v>
       </c>
@@ -15178,7 +15294,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A67" s="51">
         <v>43979</v>
       </c>
@@ -15231,7 +15347,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A68" s="51">
         <v>43980</v>
       </c>
@@ -15284,7 +15400,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A69" s="51">
         <v>43981</v>
       </c>
@@ -15337,7 +15453,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A70" s="51">
         <v>43982</v>
       </c>
@@ -15390,7 +15506,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A71" s="51">
         <v>43983</v>
       </c>
@@ -15443,7 +15559,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A72" s="51">
         <v>43984</v>
       </c>
@@ -15496,7 +15612,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A73" s="51">
         <v>43985</v>
       </c>
@@ -15547,6 +15663,59 @@
       </c>
       <c r="Q73" s="13">
         <v>706</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A74" s="51">
+        <v>43986</v>
+      </c>
+      <c r="B74" s="11">
+        <v>8</v>
+      </c>
+      <c r="C74" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D74" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E74" s="11">
+        <v>57</v>
+      </c>
+      <c r="F74" s="11">
+        <v>14</v>
+      </c>
+      <c r="G74" s="11">
+        <v>66</v>
+      </c>
+      <c r="H74" s="11">
+        <v>317</v>
+      </c>
+      <c r="I74" s="11">
+        <v>8</v>
+      </c>
+      <c r="J74" s="11">
+        <v>62</v>
+      </c>
+      <c r="K74" s="11">
+        <v>145</v>
+      </c>
+      <c r="L74" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M74" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N74" s="11">
+        <v>8</v>
+      </c>
+      <c r="O74" s="14">
+        <v>0</v>
+      </c>
+      <c r="P74" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q74" s="13">
+        <v>685</v>
       </c>
     </row>
   </sheetData>
@@ -15557,23 +15726,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q73"/>
+  <dimension ref="A1:Q74"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B62" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Q73" sqref="Q73"/>
+      <selection pane="bottomRight" activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5703125" style="2"/>
+    <col min="1" max="1" width="12.453125" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.54296875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -15594,7 +15763,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -15615,7 +15784,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -15668,7 +15837,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="12">
         <v>43916</v>
       </c>
@@ -15721,7 +15890,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
         <v>43917</v>
       </c>
@@ -15774,7 +15943,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="12">
         <v>43918</v>
       </c>
@@ -15827,7 +15996,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
         <v>43919</v>
       </c>
@@ -15880,7 +16049,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="12">
         <v>43920</v>
       </c>
@@ -15933,7 +16102,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="12">
         <v>43921</v>
       </c>
@@ -15986,7 +16155,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="12">
         <v>43922</v>
       </c>
@@ -16039,7 +16208,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
         <v>43923</v>
       </c>
@@ -16092,7 +16261,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="12">
         <v>43924</v>
       </c>
@@ -16145,7 +16314,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <v>43925</v>
       </c>
@@ -16198,7 +16367,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>43926</v>
       </c>
@@ -16251,7 +16420,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="12">
         <v>43927</v>
       </c>
@@ -16304,7 +16473,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="12">
         <v>43928</v>
       </c>
@@ -16357,7 +16526,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="12">
         <v>43929</v>
       </c>
@@ -16410,7 +16579,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="12">
         <v>43930</v>
       </c>
@@ -16463,7 +16632,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="12">
         <v>43931</v>
       </c>
@@ -16516,7 +16685,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="12">
         <v>43932</v>
       </c>
@@ -16569,7 +16738,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="12">
         <v>43933</v>
       </c>
@@ -16622,7 +16791,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="12">
         <v>43934</v>
       </c>
@@ -16675,7 +16844,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="12">
         <v>43935</v>
       </c>
@@ -16728,7 +16897,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" s="12">
         <v>43936</v>
       </c>
@@ -16781,7 +16950,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" s="12">
         <v>43937</v>
       </c>
@@ -16834,7 +17003,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" s="12">
         <v>43938</v>
       </c>
@@ -16887,7 +17056,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" s="12">
         <v>43939</v>
       </c>
@@ -16940,7 +17109,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" s="12">
         <v>43940</v>
       </c>
@@ -16993,7 +17162,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" s="12">
         <v>43941</v>
       </c>
@@ -17046,7 +17215,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" s="12">
         <v>43942</v>
       </c>
@@ -17099,7 +17268,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="12">
         <v>43943</v>
       </c>
@@ -17152,7 +17321,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" s="12">
         <v>43944</v>
       </c>
@@ -17205,7 +17374,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" s="12">
         <v>43945</v>
       </c>
@@ -17258,7 +17427,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" s="12">
         <v>43946</v>
       </c>
@@ -17311,7 +17480,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" s="12">
         <v>43947</v>
       </c>
@@ -17364,7 +17533,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" s="30">
         <v>43948</v>
       </c>
@@ -17417,7 +17586,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" s="30">
         <v>43949</v>
       </c>
@@ -17470,7 +17639,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" s="30">
         <v>43950</v>
       </c>
@@ -17523,7 +17692,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" s="30">
         <v>43951</v>
       </c>
@@ -17576,7 +17745,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" s="30">
         <v>43952</v>
       </c>
@@ -17629,7 +17798,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" s="30">
         <v>43953</v>
       </c>
@@ -17682,7 +17851,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" s="30">
         <v>43954</v>
       </c>
@@ -17735,7 +17904,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" s="30">
         <v>43955</v>
       </c>
@@ -17788,7 +17957,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" s="30">
         <v>43956</v>
       </c>
@@ -17841,7 +18010,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" s="30">
         <v>43957</v>
       </c>
@@ -17894,7 +18063,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" s="30">
         <v>43958</v>
       </c>
@@ -17947,7 +18116,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" s="30">
         <v>43959</v>
       </c>
@@ -18000,7 +18169,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" s="30">
         <v>43960</v>
       </c>
@@ -18053,7 +18222,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" s="30">
         <v>43961</v>
       </c>
@@ -18106,7 +18275,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50" s="30">
         <v>43962</v>
       </c>
@@ -18159,7 +18328,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51" s="30">
         <v>43963</v>
       </c>
@@ -18212,7 +18381,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52" s="30">
         <v>43964</v>
       </c>
@@ -18265,7 +18434,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53" s="30">
         <v>43965</v>
       </c>
@@ -18318,7 +18487,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54" s="30">
         <v>43966</v>
       </c>
@@ -18371,7 +18540,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55" s="30">
         <v>43967</v>
       </c>
@@ -18424,7 +18593,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56" s="30">
         <v>43968</v>
       </c>
@@ -18477,7 +18646,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A57" s="30">
         <v>43969</v>
       </c>
@@ -18530,7 +18699,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A58" s="30">
         <v>43970</v>
       </c>
@@ -18583,7 +18752,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A59" s="30">
         <v>43971</v>
       </c>
@@ -18636,7 +18805,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A60" s="30">
         <v>43972</v>
       </c>
@@ -18689,7 +18858,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A61" s="30">
         <v>43973</v>
       </c>
@@ -18742,7 +18911,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A62" s="30">
         <v>43974</v>
       </c>
@@ -18795,7 +18964,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A63" s="30">
         <v>43975</v>
       </c>
@@ -18848,7 +19017,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A64" s="30">
         <v>43976</v>
       </c>
@@ -18901,7 +19070,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A65" s="30">
         <v>43977</v>
       </c>
@@ -18954,7 +19123,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A66" s="30">
         <v>43978</v>
       </c>
@@ -19007,7 +19176,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A67" s="30">
         <v>43979</v>
       </c>
@@ -19060,7 +19229,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A68" s="30">
         <v>43980</v>
       </c>
@@ -19113,7 +19282,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A69" s="30">
         <v>43981</v>
       </c>
@@ -19166,7 +19335,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A70" s="30">
         <v>43982</v>
       </c>
@@ -19219,7 +19388,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A71" s="30">
         <v>43983</v>
       </c>
@@ -19272,7 +19441,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A72" s="30">
         <v>43984</v>
       </c>
@@ -19325,7 +19494,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A73" s="30">
         <v>43985</v>
       </c>
@@ -19376,6 +19545,59 @@
       </c>
       <c r="Q73" s="13">
         <v>411</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A74" s="30">
+        <v>43986</v>
+      </c>
+      <c r="B74" s="11">
+        <v>37</v>
+      </c>
+      <c r="C74" s="11">
+        <v>19</v>
+      </c>
+      <c r="D74" s="11">
+        <v>5</v>
+      </c>
+      <c r="E74" s="11">
+        <v>9</v>
+      </c>
+      <c r="F74" s="11">
+        <v>31</v>
+      </c>
+      <c r="G74" s="11">
+        <v>18</v>
+      </c>
+      <c r="H74" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I74" s="11">
+        <v>17</v>
+      </c>
+      <c r="J74" s="11">
+        <v>83</v>
+      </c>
+      <c r="K74" s="11">
+        <v>101</v>
+      </c>
+      <c r="L74" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M74" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N74" s="11">
+        <v>11</v>
+      </c>
+      <c r="O74" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P74" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q74" s="13">
+        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -19402,13 +19624,13 @@
       <value order="0">false</value>
     </field>
     <field name="Objective-IsPublished">
-      <value order="0">true</value>
+      <value order="0">false</value>
     </field>
     <field name="Objective-DatePublished">
-      <value order="0">2020-06-03T12:41:24Z</value>
+      <value order="0"/>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-03T12:41:24Z</value>
+      <value order="0">2020-06-04T12:39:07Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -19420,16 +19642,16 @@
       <value order="0">Analytical: COVID 19 Analysis: Restricted working papers: Research and analysis: Diseases: 2020-2025</value>
     </field>
     <field name="Objective-State">
-      <value order="0">Published</value>
+      <value order="0">Being Drafted</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41513351</value>
+      <value order="0">vA41545770</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">18.0</value>
+      <value order="0">19.1</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">144</value>
+      <value order="0">148</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-04 20:08) (#81)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u201433\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA1432\A28088333\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u207826\Objective\Objects\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5985" windowHeight="6015" tabRatio="803" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5990" windowHeight="6020" tabRatio="803"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1584" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1605" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -389,7 +389,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -496,6 +496,9 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -526,8 +529,8 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -537,7 +540,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6886575" cy="11677650"/>
+          <a:ext cx="7204075" cy="12357100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -722,23 +725,6 @@
           </a:r>
         </a:p>
         <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
           <a:r>
             <a:rPr lang="en-GB" sz="1100">
               <a:effectLst/>
@@ -746,44 +732,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>4. No data has been received since 12</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" baseline="30000">
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>th</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100">
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> May for tests conducted at the NHS Western Isles lab. This lab sends some samples to other labs for testing and these have contained no positive cases.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100">
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100">
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>5. It should be noted that testing capacity tends to be lower at weekends, and on public holidays.</a:t>
+            <a:t>4. It should be noted that testing capacity tends to be lower at weekends, and on public holidays.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -805,7 +754,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>6. Where errors have been found in previous reported numbers, these have been corrected. </a:t>
+            <a:t>5. Where errors have been found in previous reported numbers, these have been corrected. </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -855,6 +804,34 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" i="0">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>On 4 June, also based on updated postcode information, one case has been reassigned from Highland to Forth Valley. This resulted in a decrease of one in the total number of cases in the Highlands.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
           <a:r>
             <a:rPr lang="en-GB" sz="1100">
               <a:effectLst/>
@@ -873,7 +850,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>7. The data in Table 2, 3a and 3b includes a snapshot of:</a:t>
+            <a:t>6. The data in Table 2, 3a and 3b includes a snapshot of:</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1040,7 +1017,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>8. NHS Boards provide Scottish Government with management information on the numbers of patients in ICU with confirmed or suspected COVID-19 at midnight – this is intended to provide information on patients receiving ICU level 3 care. A small number of NHS Boards have some combined ICU/HDU units and provide information on those units. For example NHS Tayside had included a standalone HDU in returns before 7</a:t>
+            <a:t>7. NHS Boards provide Scottish Government with management information on the numbers of patients in ICU with confirmed or suspected COVID-19 at midnight – this is intended to provide information on patients receiving ICU level 3 care. A small number of NHS Boards have some combined ICU/HDU units and provide information on those units. For example NHS Tayside had included a standalone HDU in returns before 7</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" baseline="30000">
@@ -1095,7 +1072,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>9. The number of patients in hospital or ICU reported each day refers to the number of patients overnight, at midnight on the preceding night.</a:t>
+            <a:t>8. The number of patients in hospital or ICU reported each day refers to the number of patients overnight, at midnight on the preceding night.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1117,7 +1094,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>10. Where Boards do not provide their overnight data in time for the daily publication, the previous day’s data will be used and highlighted on each occasion. The figure will be revised the subsequent day to include the correct data. Figures may also be revised if Boards discover an error and have to resubmit their data. </a:t>
+            <a:t>9. Where Boards do not provide their overnight data in time for the daily publication, the previous day’s data will be used and highlighted on each occasion. The figure will be revised the subsequent day to include the correct data. Figures may also be revised if Boards discover an error and have to resubmit their data. </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1234,7 +1211,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>11. Other minor variations in the daily returns from Boards (for tables 2 and 3a and 3b) include:</a:t>
+            <a:t>10. Other minor variations in the daily returns from Boards (for tables 2 and 3a and 3b) include:</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1339,7 +1316,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>12.</a:t>
+            <a:t>11.</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" baseline="0">
@@ -1349,6 +1326,59 @@
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t> For Table 1, the daily total of people found positive on 2/6/20 contains 40 historic samples from an NHS Fife laboratory.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB" sz="1100" baseline="0">
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>12. On 04/06/2020, the number of positive cases in Highland decreased by 1 due to an update to postcode of residence for one case.</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB">
             <a:effectLst/>
@@ -1645,23 +1675,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="90.42578125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.42578125" style="2"/>
+    <col min="2" max="2" width="29.453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="90.453125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B3" s="18" t="s">
         <v>20</v>
       </c>
@@ -1669,7 +1699,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="20" t="s">
         <v>22</v>
       </c>
@@ -1677,13 +1707,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="22" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="23"/>
     </row>
-    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="24" t="s">
         <v>26</v>
       </c>
@@ -1691,7 +1721,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="24" t="s">
         <v>27</v>
       </c>
@@ -1699,7 +1729,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="24" t="s">
         <v>36</v>
       </c>
@@ -1707,7 +1737,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="20" t="s">
         <v>37</v>
       </c>
@@ -1731,16 +1761,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K66" sqref="K66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="9.42578125" style="2"/>
+    <col min="1" max="16384" width="9.453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A44" s="43"/>
     </row>
   </sheetData>
@@ -1755,20 +1785,20 @@
   <dimension ref="A1:S160"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B67" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B75" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E91" sqref="E91"/>
+      <selection pane="bottomRight" activeCell="I94" sqref="I94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" style="2" customWidth="1"/>
-    <col min="2" max="16" width="11.42578125" style="11" customWidth="1"/>
-    <col min="17" max="16384" width="8.5703125" style="2"/>
+    <col min="2" max="16" width="11.453125" style="11" customWidth="1"/>
+    <col min="17" max="16384" width="8.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -1788,7 +1818,7 @@
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -1807,7 +1837,7 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -1857,7 +1887,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>43897</v>
       </c>
@@ -1907,7 +1937,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>43898</v>
       </c>
@@ -1957,7 +1987,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>43899</v>
       </c>
@@ -2007,7 +2037,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>43900</v>
       </c>
@@ -2057,7 +2087,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>43901</v>
       </c>
@@ -2107,7 +2137,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>43902</v>
       </c>
@@ -2157,7 +2187,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>43903</v>
       </c>
@@ -2207,7 +2237,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>43904</v>
       </c>
@@ -2257,7 +2287,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>43905</v>
       </c>
@@ -2307,7 +2337,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>43906</v>
       </c>
@@ -2357,7 +2387,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>43907</v>
       </c>
@@ -2407,7 +2437,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>43908</v>
       </c>
@@ -2457,7 +2487,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>43909</v>
       </c>
@@ -2507,7 +2537,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>43910</v>
       </c>
@@ -2557,7 +2587,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>43911</v>
       </c>
@@ -2607,7 +2637,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>43912</v>
       </c>
@@ -2657,7 +2687,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>43913</v>
       </c>
@@ -2707,7 +2737,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>43914</v>
       </c>
@@ -2757,7 +2787,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>43915</v>
       </c>
@@ -2807,7 +2837,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>43916</v>
       </c>
@@ -2857,7 +2887,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>43917</v>
       </c>
@@ -2907,7 +2937,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>43918</v>
       </c>
@@ -2957,7 +2987,7 @@
         <v>1264</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>43919</v>
       </c>
@@ -3007,7 +3037,7 @@
         <v>1417</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>43920</v>
       </c>
@@ -3057,7 +3087,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>43921</v>
       </c>
@@ -3107,7 +3137,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>43922</v>
       </c>
@@ -3157,7 +3187,7 @@
         <v>2310</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>43923</v>
       </c>
@@ -3207,7 +3237,7 @@
         <v>2602</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>43924</v>
       </c>
@@ -3257,7 +3287,7 @@
         <v>3001</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>43925</v>
       </c>
@@ -3307,7 +3337,7 @@
         <v>3345</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>43926</v>
       </c>
@@ -3357,7 +3387,7 @@
         <v>3706</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>43927</v>
       </c>
@@ -3407,7 +3437,7 @@
         <v>3961</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>43928</v>
       </c>
@@ -3457,7 +3487,7 @@
         <v>4229</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>43929</v>
       </c>
@@ -3507,7 +3537,7 @@
         <v>4565</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>43930</v>
       </c>
@@ -3557,7 +3587,7 @@
         <v>4957</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>43931</v>
       </c>
@@ -3607,7 +3637,7 @@
         <v>5275</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>43932</v>
       </c>
@@ -3657,7 +3687,7 @@
         <v>5590</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>43933</v>
       </c>
@@ -3707,7 +3737,7 @@
         <v>5912</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>43934</v>
       </c>
@@ -3757,7 +3787,7 @@
         <v>6067</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>43935</v>
       </c>
@@ -3807,7 +3837,7 @@
         <v>6358</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>43936</v>
       </c>
@@ -3857,7 +3887,7 @@
         <v>6748</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
         <v>43937</v>
       </c>
@@ -3907,7 +3937,7 @@
         <v>7102</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>43938</v>
       </c>
@@ -3957,7 +3987,7 @@
         <v>7409</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A46" s="5">
         <v>43939</v>
       </c>
@@ -4007,7 +4037,7 @@
         <v>7820</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A47" s="5">
         <v>43940</v>
       </c>
@@ -4057,7 +4087,7 @@
         <v>8187</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A48" s="5">
         <v>43941</v>
       </c>
@@ -4107,7 +4137,7 @@
         <v>8450</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A49" s="5">
         <v>43942</v>
       </c>
@@ -4157,7 +4187,7 @@
         <v>8672</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
         <v>43943</v>
       </c>
@@ -4207,7 +4237,7 @@
         <v>9038</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
         <v>43944</v>
       </c>
@@ -4257,7 +4287,7 @@
         <v>9409</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
         <v>43945</v>
       </c>
@@ -4307,7 +4337,7 @@
         <v>9697</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
         <v>43946</v>
       </c>
@@ -4357,7 +4387,7 @@
         <v>10051</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A54" s="5">
         <v>43947</v>
       </c>
@@ -4408,7 +4438,7 @@
       </c>
       <c r="R54" s="38"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
         <v>43948</v>
       </c>
@@ -4459,7 +4489,7 @@
       </c>
       <c r="R55" s="38"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A56" s="5">
         <v>43949</v>
       </c>
@@ -4510,7 +4540,7 @@
       </c>
       <c r="R56" s="39"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
         <v>43950</v>
       </c>
@@ -4560,7 +4590,7 @@
         <v>11034</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
         <v>43951</v>
       </c>
@@ -4611,7 +4641,7 @@
       </c>
       <c r="R58" s="38"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>43952</v>
       </c>
@@ -4663,7 +4693,7 @@
       <c r="R59" s="38"/>
       <c r="S59" s="38"/>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
         <v>43953</v>
       </c>
@@ -4713,7 +4743,7 @@
         <v>11927</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
         <v>43954</v>
       </c>
@@ -4763,7 +4793,7 @@
         <v>12097</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A62" s="5">
         <v>43955</v>
       </c>
@@ -4813,7 +4843,7 @@
         <v>12266</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A63" s="5">
         <v>43956</v>
       </c>
@@ -4863,7 +4893,7 @@
         <v>12437</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
         <v>43957</v>
       </c>
@@ -4913,7 +4943,7 @@
         <v>12709</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>43958</v>
       </c>
@@ -4963,7 +4993,7 @@
         <v>12924</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
         <v>43959</v>
       </c>
@@ -5013,7 +5043,7 @@
         <v>13149</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
         <v>43960</v>
       </c>
@@ -5063,7 +5093,7 @@
         <v>13305</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A68" s="5">
         <v>43961</v>
       </c>
@@ -5113,7 +5143,7 @@
         <v>13486</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A69" s="5">
         <v>43962</v>
       </c>
@@ -5163,7 +5193,7 @@
         <v>13627</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A70" s="5">
         <v>43963</v>
       </c>
@@ -5213,7 +5243,7 @@
         <v>13763</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A71" s="5">
         <v>43964</v>
       </c>
@@ -5263,7 +5293,7 @@
         <v>13929</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A72" s="5">
         <v>43965</v>
       </c>
@@ -5313,7 +5343,7 @@
         <v>14117</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A73" s="5">
         <v>43966</v>
       </c>
@@ -5363,7 +5393,7 @@
         <v>14260</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A74" s="5">
         <v>43967</v>
       </c>
@@ -5413,7 +5443,7 @@
         <v>14447</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A75" s="5">
         <v>43968</v>
       </c>
@@ -5463,7 +5493,7 @@
         <v>14537</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A76" s="5">
         <v>43969</v>
       </c>
@@ -5513,7 +5543,7 @@
         <v>14594</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A77" s="5">
         <v>43970</v>
       </c>
@@ -5563,7 +5593,7 @@
         <v>14655</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A78" s="5">
         <v>43971</v>
       </c>
@@ -5613,7 +5643,7 @@
         <v>14751</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A79" s="5">
         <v>43972</v>
       </c>
@@ -5663,7 +5693,7 @@
         <v>14856</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A80" s="5">
         <v>43973</v>
       </c>
@@ -5713,7 +5743,7 @@
         <v>14969</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A81" s="5">
         <v>43974</v>
       </c>
@@ -5763,7 +5793,7 @@
         <v>15041</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A82" s="5">
         <v>43975</v>
       </c>
@@ -5813,7 +5843,7 @@
         <v>15101</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A83" s="5">
         <v>43976</v>
       </c>
@@ -5863,7 +5893,7 @@
         <v>15156</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A84" s="5">
         <v>43977</v>
       </c>
@@ -5913,7 +5943,7 @@
         <v>15185</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A85" s="5">
         <v>43978</v>
       </c>
@@ -5963,7 +5993,7 @@
         <v>15240</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A86" s="5">
         <v>43979</v>
       </c>
@@ -6013,7 +6043,7 @@
         <v>15288</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A87" s="5">
         <v>43980</v>
       </c>
@@ -6063,7 +6093,7 @@
         <v>15327</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A88" s="5">
         <v>43981</v>
       </c>
@@ -6113,7 +6143,7 @@
         <v>15382</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A89" s="5">
         <v>43982</v>
       </c>
@@ -6163,7 +6193,7 @@
         <v>15400</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A90" s="5">
         <v>43983</v>
       </c>
@@ -6213,7 +6243,7 @@
         <v>15418</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A91" s="5">
         <v>43984</v>
       </c>
@@ -6263,7 +6293,7 @@
         <v>15471</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A92" s="5">
         <v>43985</v>
       </c>
@@ -6313,24 +6343,57 @@
         <v>15504</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B93" s="28"/>
-      <c r="C93" s="28"/>
-      <c r="D93" s="28"/>
-      <c r="E93" s="28"/>
-      <c r="F93" s="28"/>
-      <c r="G93" s="28"/>
-      <c r="H93" s="28"/>
-      <c r="I93" s="28"/>
-      <c r="J93" s="28"/>
-      <c r="K93" s="28"/>
-      <c r="L93" s="28"/>
-      <c r="M93" s="28"/>
-      <c r="N93" s="28"/>
-      <c r="O93" s="28"/>
-      <c r="P93" s="28"/>
-    </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A93" s="5">
+        <v>43986</v>
+      </c>
+      <c r="B93" s="28">
+        <v>1071</v>
+      </c>
+      <c r="C93" s="28">
+        <v>325</v>
+      </c>
+      <c r="D93" s="28">
+        <v>261</v>
+      </c>
+      <c r="E93" s="28">
+        <v>877</v>
+      </c>
+      <c r="F93" s="28">
+        <v>944</v>
+      </c>
+      <c r="G93" s="28">
+        <v>1283</v>
+      </c>
+      <c r="H93" s="28">
+        <v>3961</v>
+      </c>
+      <c r="I93" s="52">
+        <v>338</v>
+      </c>
+      <c r="J93" s="28">
+        <v>2002</v>
+      </c>
+      <c r="K93" s="28">
+        <v>2752</v>
+      </c>
+      <c r="L93" s="28">
+        <v>8</v>
+      </c>
+      <c r="M93" s="28">
+        <v>54</v>
+      </c>
+      <c r="N93" s="28">
+        <v>1671</v>
+      </c>
+      <c r="O93" s="28">
+        <v>6</v>
+      </c>
+      <c r="P93" s="32">
+        <v>15553</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B94" s="28"/>
       <c r="C94" s="28"/>
       <c r="D94" s="28"/>
@@ -6347,7 +6410,7 @@
       <c r="O94" s="28"/>
       <c r="P94" s="28"/>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B95" s="28"/>
       <c r="C95" s="28"/>
       <c r="D95" s="28"/>
@@ -6364,7 +6427,7 @@
       <c r="O95" s="28"/>
       <c r="P95" s="28"/>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B96" s="28"/>
       <c r="C96" s="28"/>
       <c r="D96" s="28"/>
@@ -6381,7 +6444,7 @@
       <c r="O96" s="28"/>
       <c r="P96" s="28"/>
     </row>
-    <row r="97" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B97" s="28"/>
       <c r="C97" s="28"/>
       <c r="D97" s="28"/>
@@ -6398,7 +6461,7 @@
       <c r="O97" s="28"/>
       <c r="P97" s="28"/>
     </row>
-    <row r="98" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B98" s="28"/>
       <c r="C98" s="28"/>
       <c r="D98" s="28"/>
@@ -6415,7 +6478,7 @@
       <c r="O98" s="28"/>
       <c r="P98" s="28"/>
     </row>
-    <row r="99" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B99" s="28"/>
       <c r="C99" s="28"/>
       <c r="D99" s="28"/>
@@ -6432,7 +6495,7 @@
       <c r="O99" s="28"/>
       <c r="P99" s="28"/>
     </row>
-    <row r="100" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B100" s="28"/>
       <c r="C100" s="28"/>
       <c r="D100" s="28"/>
@@ -6449,7 +6512,7 @@
       <c r="O100" s="28"/>
       <c r="P100" s="28"/>
     </row>
-    <row r="101" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B101" s="28"/>
       <c r="C101" s="28"/>
       <c r="D101" s="28"/>
@@ -6466,7 +6529,7 @@
       <c r="O101" s="28"/>
       <c r="P101" s="28"/>
     </row>
-    <row r="102" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B102" s="28"/>
       <c r="C102" s="28"/>
       <c r="D102" s="28"/>
@@ -6483,7 +6546,7 @@
       <c r="O102" s="28"/>
       <c r="P102" s="28"/>
     </row>
-    <row r="103" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B103" s="28"/>
       <c r="C103" s="28"/>
       <c r="D103" s="28"/>
@@ -6500,7 +6563,7 @@
       <c r="O103" s="28"/>
       <c r="P103" s="28"/>
     </row>
-    <row r="104" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B104" s="28"/>
       <c r="C104" s="28"/>
       <c r="D104" s="28"/>
@@ -6517,7 +6580,7 @@
       <c r="O104" s="28"/>
       <c r="P104" s="28"/>
     </row>
-    <row r="105" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B105" s="28"/>
       <c r="C105" s="28"/>
       <c r="D105" s="28"/>
@@ -6534,7 +6597,7 @@
       <c r="O105" s="28"/>
       <c r="P105" s="28"/>
     </row>
-    <row r="106" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B106" s="28"/>
       <c r="C106" s="28"/>
       <c r="D106" s="28"/>
@@ -6551,7 +6614,7 @@
       <c r="O106" s="28"/>
       <c r="P106" s="28"/>
     </row>
-    <row r="107" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B107" s="28"/>
       <c r="C107" s="28"/>
       <c r="D107" s="28"/>
@@ -6568,7 +6631,7 @@
       <c r="O107" s="28"/>
       <c r="P107" s="28"/>
     </row>
-    <row r="108" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B108" s="28"/>
       <c r="C108" s="28"/>
       <c r="D108" s="28"/>
@@ -6585,7 +6648,7 @@
       <c r="O108" s="28"/>
       <c r="P108" s="28"/>
     </row>
-    <row r="109" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B109" s="28"/>
       <c r="C109" s="28"/>
       <c r="D109" s="28"/>
@@ -6602,7 +6665,7 @@
       <c r="O109" s="28"/>
       <c r="P109" s="28"/>
     </row>
-    <row r="110" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B110" s="28"/>
       <c r="C110" s="28"/>
       <c r="D110" s="28"/>
@@ -6619,7 +6682,7 @@
       <c r="O110" s="28"/>
       <c r="P110" s="28"/>
     </row>
-    <row r="111" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B111" s="28"/>
       <c r="C111" s="28"/>
       <c r="D111" s="28"/>
@@ -6636,7 +6699,7 @@
       <c r="O111" s="28"/>
       <c r="P111" s="28"/>
     </row>
-    <row r="112" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B112" s="28"/>
       <c r="C112" s="28"/>
       <c r="D112" s="28"/>
@@ -6653,7 +6716,7 @@
       <c r="O112" s="28"/>
       <c r="P112" s="28"/>
     </row>
-    <row r="113" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B113" s="28"/>
       <c r="C113" s="28"/>
       <c r="D113" s="28"/>
@@ -6670,7 +6733,7 @@
       <c r="O113" s="28"/>
       <c r="P113" s="28"/>
     </row>
-    <row r="114" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B114" s="28"/>
       <c r="C114" s="28"/>
       <c r="D114" s="28"/>
@@ -6687,7 +6750,7 @@
       <c r="O114" s="28"/>
       <c r="P114" s="28"/>
     </row>
-    <row r="115" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B115" s="28"/>
       <c r="C115" s="28"/>
       <c r="D115" s="28"/>
@@ -6704,7 +6767,7 @@
       <c r="O115" s="28"/>
       <c r="P115" s="28"/>
     </row>
-    <row r="116" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B116" s="28"/>
       <c r="C116" s="28"/>
       <c r="D116" s="28"/>
@@ -6721,7 +6784,7 @@
       <c r="O116" s="28"/>
       <c r="P116" s="28"/>
     </row>
-    <row r="117" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B117" s="28"/>
       <c r="C117" s="28"/>
       <c r="D117" s="28"/>
@@ -6738,7 +6801,7 @@
       <c r="O117" s="28"/>
       <c r="P117" s="28"/>
     </row>
-    <row r="118" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B118" s="28"/>
       <c r="C118" s="28"/>
       <c r="D118" s="28"/>
@@ -6755,7 +6818,7 @@
       <c r="O118" s="28"/>
       <c r="P118" s="28"/>
     </row>
-    <row r="119" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B119" s="28"/>
       <c r="C119" s="28"/>
       <c r="D119" s="28"/>
@@ -6772,7 +6835,7 @@
       <c r="O119" s="28"/>
       <c r="P119" s="28"/>
     </row>
-    <row r="120" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B120" s="28"/>
       <c r="C120" s="28"/>
       <c r="D120" s="28"/>
@@ -6789,7 +6852,7 @@
       <c r="O120" s="28"/>
       <c r="P120" s="28"/>
     </row>
-    <row r="121" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B121" s="28"/>
       <c r="C121" s="28"/>
       <c r="D121" s="28"/>
@@ -6806,7 +6869,7 @@
       <c r="O121" s="28"/>
       <c r="P121" s="28"/>
     </row>
-    <row r="122" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B122" s="28"/>
       <c r="C122" s="28"/>
       <c r="D122" s="28"/>
@@ -6823,7 +6886,7 @@
       <c r="O122" s="28"/>
       <c r="P122" s="28"/>
     </row>
-    <row r="123" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B123" s="28"/>
       <c r="C123" s="28"/>
       <c r="D123" s="28"/>
@@ -6840,7 +6903,7 @@
       <c r="O123" s="28"/>
       <c r="P123" s="28"/>
     </row>
-    <row r="124" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B124" s="28"/>
       <c r="C124" s="28"/>
       <c r="D124" s="28"/>
@@ -6857,7 +6920,7 @@
       <c r="O124" s="28"/>
       <c r="P124" s="28"/>
     </row>
-    <row r="125" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B125" s="28"/>
       <c r="C125" s="28"/>
       <c r="D125" s="28"/>
@@ -6874,7 +6937,7 @@
       <c r="O125" s="28"/>
       <c r="P125" s="28"/>
     </row>
-    <row r="126" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B126" s="28"/>
       <c r="C126" s="28"/>
       <c r="D126" s="28"/>
@@ -6891,7 +6954,7 @@
       <c r="O126" s="28"/>
       <c r="P126" s="28"/>
     </row>
-    <row r="127" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B127" s="28"/>
       <c r="C127" s="28"/>
       <c r="D127" s="28"/>
@@ -6908,7 +6971,7 @@
       <c r="O127" s="28"/>
       <c r="P127" s="28"/>
     </row>
-    <row r="128" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B128" s="28"/>
       <c r="C128" s="28"/>
       <c r="D128" s="28"/>
@@ -6925,7 +6988,7 @@
       <c r="O128" s="28"/>
       <c r="P128" s="28"/>
     </row>
-    <row r="129" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B129" s="28"/>
       <c r="C129" s="28"/>
       <c r="D129" s="28"/>
@@ -6942,7 +7005,7 @@
       <c r="O129" s="28"/>
       <c r="P129" s="28"/>
     </row>
-    <row r="130" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B130" s="28"/>
       <c r="C130" s="28"/>
       <c r="D130" s="28"/>
@@ -6959,7 +7022,7 @@
       <c r="O130" s="28"/>
       <c r="P130" s="28"/>
     </row>
-    <row r="131" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B131" s="28"/>
       <c r="C131" s="28"/>
       <c r="D131" s="28"/>
@@ -6976,7 +7039,7 @@
       <c r="O131" s="28"/>
       <c r="P131" s="28"/>
     </row>
-    <row r="132" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B132" s="28"/>
       <c r="C132" s="28"/>
       <c r="D132" s="28"/>
@@ -6993,7 +7056,7 @@
       <c r="O132" s="28"/>
       <c r="P132" s="28"/>
     </row>
-    <row r="133" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B133" s="28"/>
       <c r="C133" s="28"/>
       <c r="D133" s="28"/>
@@ -7010,7 +7073,7 @@
       <c r="O133" s="28"/>
       <c r="P133" s="28"/>
     </row>
-    <row r="134" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B134" s="28"/>
       <c r="C134" s="28"/>
       <c r="D134" s="28"/>
@@ -7027,7 +7090,7 @@
       <c r="O134" s="28"/>
       <c r="P134" s="28"/>
     </row>
-    <row r="135" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B135" s="28"/>
       <c r="C135" s="28"/>
       <c r="D135" s="28"/>
@@ -7044,7 +7107,7 @@
       <c r="O135" s="28"/>
       <c r="P135" s="28"/>
     </row>
-    <row r="136" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B136" s="28"/>
       <c r="C136" s="28"/>
       <c r="D136" s="28"/>
@@ -7061,7 +7124,7 @@
       <c r="O136" s="28"/>
       <c r="P136" s="28"/>
     </row>
-    <row r="137" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B137" s="28"/>
       <c r="C137" s="28"/>
       <c r="D137" s="28"/>
@@ -7078,7 +7141,7 @@
       <c r="O137" s="28"/>
       <c r="P137" s="28"/>
     </row>
-    <row r="138" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B138" s="28"/>
       <c r="C138" s="28"/>
       <c r="D138" s="28"/>
@@ -7095,7 +7158,7 @@
       <c r="O138" s="28"/>
       <c r="P138" s="28"/>
     </row>
-    <row r="139" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B139" s="28"/>
       <c r="C139" s="28"/>
       <c r="D139" s="28"/>
@@ -7112,7 +7175,7 @@
       <c r="O139" s="28"/>
       <c r="P139" s="28"/>
     </row>
-    <row r="140" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B140" s="28"/>
       <c r="C140" s="28"/>
       <c r="D140" s="28"/>
@@ -7129,7 +7192,7 @@
       <c r="O140" s="28"/>
       <c r="P140" s="28"/>
     </row>
-    <row r="141" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B141" s="28"/>
       <c r="C141" s="28"/>
       <c r="D141" s="28"/>
@@ -7146,7 +7209,7 @@
       <c r="O141" s="28"/>
       <c r="P141" s="28"/>
     </row>
-    <row r="142" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B142" s="28"/>
       <c r="C142" s="28"/>
       <c r="D142" s="28"/>
@@ -7163,7 +7226,7 @@
       <c r="O142" s="28"/>
       <c r="P142" s="28"/>
     </row>
-    <row r="143" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B143" s="28"/>
       <c r="C143" s="28"/>
       <c r="D143" s="28"/>
@@ -7180,7 +7243,7 @@
       <c r="O143" s="28"/>
       <c r="P143" s="28"/>
     </row>
-    <row r="144" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B144" s="28"/>
       <c r="C144" s="28"/>
       <c r="D144" s="28"/>
@@ -7197,7 +7260,7 @@
       <c r="O144" s="28"/>
       <c r="P144" s="28"/>
     </row>
-    <row r="145" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B145" s="28"/>
       <c r="C145" s="28"/>
       <c r="D145" s="28"/>
@@ -7214,7 +7277,7 @@
       <c r="O145" s="28"/>
       <c r="P145" s="28"/>
     </row>
-    <row r="146" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B146" s="28"/>
       <c r="C146" s="28"/>
       <c r="D146" s="28"/>
@@ -7231,7 +7294,7 @@
       <c r="O146" s="28"/>
       <c r="P146" s="28"/>
     </row>
-    <row r="147" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B147" s="28"/>
       <c r="C147" s="28"/>
       <c r="D147" s="28"/>
@@ -7248,7 +7311,7 @@
       <c r="O147" s="28"/>
       <c r="P147" s="28"/>
     </row>
-    <row r="148" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B148" s="28"/>
       <c r="C148" s="28"/>
       <c r="D148" s="28"/>
@@ -7265,7 +7328,7 @@
       <c r="O148" s="28"/>
       <c r="P148" s="28"/>
     </row>
-    <row r="149" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B149" s="28"/>
       <c r="C149" s="28"/>
       <c r="D149" s="28"/>
@@ -7282,7 +7345,7 @@
       <c r="O149" s="28"/>
       <c r="P149" s="28"/>
     </row>
-    <row r="150" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B150" s="28"/>
       <c r="C150" s="28"/>
       <c r="D150" s="28"/>
@@ -7299,7 +7362,7 @@
       <c r="O150" s="28"/>
       <c r="P150" s="28"/>
     </row>
-    <row r="151" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B151" s="28"/>
       <c r="C151" s="28"/>
       <c r="D151" s="28"/>
@@ -7316,7 +7379,7 @@
       <c r="O151" s="28"/>
       <c r="P151" s="28"/>
     </row>
-    <row r="152" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B152" s="28"/>
       <c r="C152" s="28"/>
       <c r="D152" s="28"/>
@@ -7333,7 +7396,7 @@
       <c r="O152" s="28"/>
       <c r="P152" s="28"/>
     </row>
-    <row r="153" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B153" s="28"/>
       <c r="C153" s="28"/>
       <c r="D153" s="28"/>
@@ -7350,7 +7413,7 @@
       <c r="O153" s="28"/>
       <c r="P153" s="28"/>
     </row>
-    <row r="154" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B154" s="28"/>
       <c r="C154" s="28"/>
       <c r="D154" s="28"/>
@@ -7367,7 +7430,7 @@
       <c r="O154" s="28"/>
       <c r="P154" s="28"/>
     </row>
-    <row r="155" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B155" s="28"/>
       <c r="C155" s="28"/>
       <c r="D155" s="28"/>
@@ -7384,7 +7447,7 @@
       <c r="O155" s="28"/>
       <c r="P155" s="28"/>
     </row>
-    <row r="156" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B156" s="28"/>
       <c r="C156" s="28"/>
       <c r="D156" s="28"/>
@@ -7401,7 +7464,7 @@
       <c r="O156" s="28"/>
       <c r="P156" s="28"/>
     </row>
-    <row r="157" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B157" s="28"/>
       <c r="C157" s="28"/>
       <c r="D157" s="28"/>
@@ -7418,7 +7481,7 @@
       <c r="O157" s="28"/>
       <c r="P157" s="28"/>
     </row>
-    <row r="158" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B158" s="28"/>
       <c r="C158" s="28"/>
       <c r="D158" s="28"/>
@@ -7435,7 +7498,7 @@
       <c r="O158" s="28"/>
       <c r="P158" s="28"/>
     </row>
-    <row r="159" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B159" s="28"/>
       <c r="C159" s="28"/>
       <c r="D159" s="28"/>
@@ -7452,7 +7515,7 @@
       <c r="O159" s="28"/>
       <c r="P159" s="28"/>
     </row>
-    <row r="160" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B160" s="28"/>
       <c r="C160" s="28"/>
       <c r="D160" s="28"/>
@@ -7477,21 +7540,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q81"/>
+  <dimension ref="A1:Q82"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N80" sqref="N80"/>
+      <pane ySplit="3" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P85" sqref="P85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5703125" style="2"/>
+    <col min="1" max="1" width="12.453125" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.54296875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -7512,7 +7575,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -7533,7 +7596,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -7586,7 +7649,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="12">
         <v>43908</v>
       </c>
@@ -7639,7 +7702,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
         <v>43909</v>
       </c>
@@ -7692,7 +7755,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="12">
         <v>43910</v>
       </c>
@@ -7745,7 +7808,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
         <v>43911</v>
       </c>
@@ -7798,7 +7861,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="12">
         <v>43912</v>
       </c>
@@ -7851,7 +7914,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="12">
         <v>43913</v>
       </c>
@@ -7904,7 +7967,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="12">
         <v>43914</v>
       </c>
@@ -7957,7 +8020,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
         <v>43915</v>
       </c>
@@ -8010,7 +8073,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="12">
         <v>43916</v>
       </c>
@@ -8063,7 +8126,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <v>43917</v>
       </c>
@@ -8116,7 +8179,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>43918</v>
       </c>
@@ -8169,7 +8232,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="12">
         <v>43919</v>
       </c>
@@ -8222,7 +8285,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="12">
         <v>43920</v>
       </c>
@@ -8275,7 +8338,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="12">
         <v>43921</v>
       </c>
@@ -8328,7 +8391,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="12">
         <v>43922</v>
       </c>
@@ -8381,7 +8444,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="12">
         <v>43923</v>
       </c>
@@ -8434,7 +8497,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="12">
         <v>43924</v>
       </c>
@@ -8487,7 +8550,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="12">
         <v>43925</v>
       </c>
@@ -8540,7 +8603,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="12">
         <v>43926</v>
       </c>
@@ -8593,7 +8656,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="12">
         <v>43927</v>
       </c>
@@ -8646,7 +8709,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" s="12">
         <v>43928</v>
       </c>
@@ -8699,7 +8762,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" s="12">
         <v>43929</v>
       </c>
@@ -8752,7 +8815,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" s="12">
         <v>43930</v>
       </c>
@@ -8805,7 +8868,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" s="12">
         <v>43931</v>
       </c>
@@ -8858,7 +8921,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" s="12">
         <v>43932</v>
       </c>
@@ -8911,7 +8974,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" s="12">
         <v>43933</v>
       </c>
@@ -8964,7 +9027,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" s="12">
         <v>43934</v>
       </c>
@@ -9017,7 +9080,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="12">
         <v>43935</v>
       </c>
@@ -9070,7 +9133,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" s="12">
         <v>43936</v>
       </c>
@@ -9123,7 +9186,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" s="12">
         <v>43937</v>
       </c>
@@ -9176,7 +9239,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" s="12">
         <v>43938</v>
       </c>
@@ -9229,7 +9292,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" s="12">
         <v>43939</v>
       </c>
@@ -9282,7 +9345,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" s="30">
         <v>43940</v>
       </c>
@@ -9335,7 +9398,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" s="30">
         <v>43941</v>
       </c>
@@ -9388,7 +9451,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" s="30">
         <v>43942</v>
       </c>
@@ -9441,7 +9504,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" s="30">
         <v>43943</v>
       </c>
@@ -9494,7 +9557,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" s="30">
         <v>43944</v>
       </c>
@@ -9547,7 +9610,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" s="30">
         <v>43945</v>
       </c>
@@ -9600,7 +9663,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" s="30">
         <v>43946</v>
       </c>
@@ -9653,7 +9716,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" s="30">
         <v>43947</v>
       </c>
@@ -9706,7 +9769,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" s="30">
         <v>43948</v>
       </c>
@@ -9759,7 +9822,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" s="30">
         <v>43949</v>
       </c>
@@ -9812,7 +9875,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" s="30">
         <v>43950</v>
       </c>
@@ -9865,7 +9928,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" s="30">
         <v>43951</v>
       </c>
@@ -9918,7 +9981,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" s="30">
         <v>43952</v>
       </c>
@@ -9971,7 +10034,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" s="30">
         <v>43953</v>
       </c>
@@ -10024,7 +10087,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50" s="30">
         <v>43954</v>
       </c>
@@ -10077,7 +10140,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51" s="30">
         <v>43955</v>
       </c>
@@ -10130,7 +10193,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52" s="30">
         <v>43956</v>
       </c>
@@ -10183,7 +10246,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53" s="30">
         <v>43957</v>
       </c>
@@ -10236,7 +10299,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54" s="30">
         <v>43958</v>
       </c>
@@ -10289,7 +10352,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55" s="30">
         <v>43959</v>
       </c>
@@ -10342,7 +10405,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56" s="30">
         <v>43960</v>
       </c>
@@ -10395,7 +10458,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A57" s="30">
         <v>43961</v>
       </c>
@@ -10448,7 +10511,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A58" s="30">
         <v>43962</v>
       </c>
@@ -10501,7 +10564,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A59" s="30">
         <v>43963</v>
       </c>
@@ -10554,7 +10617,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A60" s="30">
         <v>43964</v>
       </c>
@@ -10607,7 +10670,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A61" s="30">
         <v>43965</v>
       </c>
@@ -10660,7 +10723,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A62" s="30">
         <v>43966</v>
       </c>
@@ -10713,7 +10776,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A63" s="30">
         <v>43967</v>
       </c>
@@ -10766,7 +10829,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A64" s="30">
         <v>43968</v>
       </c>
@@ -10819,7 +10882,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A65" s="30">
         <v>43969</v>
       </c>
@@ -10872,7 +10935,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A66" s="30">
         <v>43970</v>
       </c>
@@ -10925,7 +10988,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A67" s="30">
         <v>43971</v>
       </c>
@@ -10978,7 +11041,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A68" s="30">
         <v>43972</v>
       </c>
@@ -11031,7 +11094,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A69" s="30">
         <v>43973</v>
       </c>
@@ -11084,7 +11147,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A70" s="30">
         <v>43974</v>
       </c>
@@ -11137,7 +11200,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A71" s="30">
         <v>43975</v>
       </c>
@@ -11190,7 +11253,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A72" s="30">
         <v>43976</v>
       </c>
@@ -11243,7 +11306,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A73" s="30">
         <v>43977</v>
       </c>
@@ -11296,7 +11359,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A74" s="30">
         <v>43978</v>
       </c>
@@ -11349,7 +11412,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A75" s="30">
         <v>43979</v>
       </c>
@@ -11402,7 +11465,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A76" s="30">
         <v>43980</v>
       </c>
@@ -11455,7 +11518,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A77" s="30">
         <v>43981</v>
       </c>
@@ -11508,7 +11571,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A78" s="30">
         <v>43982</v>
       </c>
@@ -11561,7 +11624,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A79" s="30">
         <v>43983</v>
       </c>
@@ -11614,7 +11677,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A80" s="30">
         <v>43984</v>
       </c>
@@ -11667,7 +11730,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A81" s="30">
         <v>43985</v>
       </c>
@@ -11718,6 +11781,59 @@
       </c>
       <c r="Q81" s="13">
         <v>34</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A82" s="30">
+        <v>43986</v>
+      </c>
+      <c r="B82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H82" s="11">
+        <v>5</v>
+      </c>
+      <c r="I82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J82" s="11">
+        <v>6</v>
+      </c>
+      <c r="K82" s="11">
+        <v>5</v>
+      </c>
+      <c r="L82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P82" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q82" s="13">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -11728,23 +11844,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q73"/>
+  <dimension ref="A1:Q74"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B51" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="L61" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K74" sqref="K74"/>
+      <selection pane="bottomRight" activeCell="Q75" sqref="Q75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5703125" style="2"/>
+    <col min="1" max="1" width="15.1796875" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.54296875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -11765,7 +11881,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -11786,7 +11902,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -11839,7 +11955,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="12">
         <v>43916</v>
       </c>
@@ -11892,7 +12008,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
         <v>43917</v>
       </c>
@@ -11945,7 +12061,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="12">
         <v>43918</v>
       </c>
@@ -11998,7 +12114,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
         <v>43919</v>
       </c>
@@ -12051,7 +12167,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="12">
         <v>43920</v>
       </c>
@@ -12104,7 +12220,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="12">
         <v>43921</v>
       </c>
@@ -12157,7 +12273,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="12">
         <v>43922</v>
       </c>
@@ -12210,7 +12326,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
         <v>43923</v>
       </c>
@@ -12263,7 +12379,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="12">
         <v>43924</v>
       </c>
@@ -12316,7 +12432,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <v>43925</v>
       </c>
@@ -12369,7 +12485,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>43926</v>
       </c>
@@ -12422,7 +12538,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="12">
         <v>43927</v>
       </c>
@@ -12475,7 +12591,7 @@
         <v>1262</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="12">
         <v>43928</v>
       </c>
@@ -12528,7 +12644,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="12">
         <v>43929</v>
       </c>
@@ -12581,7 +12697,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="12">
         <v>43930</v>
       </c>
@@ -12634,7 +12750,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="12">
         <v>43931</v>
       </c>
@@ -12687,7 +12803,7 @@
         <v>1461</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="12">
         <v>43932</v>
       </c>
@@ -12740,7 +12856,7 @@
         <v>1467</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="12">
         <v>43933</v>
       </c>
@@ -12793,7 +12909,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="12">
         <v>43934</v>
       </c>
@@ -12846,7 +12962,7 @@
         <v>1482</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="12">
         <v>43935</v>
       </c>
@@ -12899,7 +13015,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" s="12">
         <v>43936</v>
       </c>
@@ -12952,7 +13068,7 @@
         <v>1486</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" s="12">
         <v>43937</v>
       </c>
@@ -13005,7 +13121,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" s="12">
         <v>43938</v>
       </c>
@@ -13058,7 +13174,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" s="12">
         <v>43939</v>
       </c>
@@ -13111,7 +13227,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" s="12">
         <v>43940</v>
       </c>
@@ -13164,7 +13280,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" s="12">
         <v>43941</v>
       </c>
@@ -13217,7 +13333,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" s="12">
         <v>43942</v>
       </c>
@@ -13270,7 +13386,7 @@
         <v>1472</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="12">
         <v>43943</v>
       </c>
@@ -13323,7 +13439,7 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" s="12">
         <v>43944</v>
       </c>
@@ -13376,7 +13492,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" s="12">
         <v>43945</v>
       </c>
@@ -13429,7 +13545,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" s="12">
         <v>43946</v>
       </c>
@@ -13482,7 +13598,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" s="12">
         <v>43947</v>
       </c>
@@ -13535,7 +13651,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" s="30">
         <v>43948</v>
       </c>
@@ -13588,7 +13704,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" s="30">
         <v>43949</v>
       </c>
@@ -13641,7 +13757,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" s="30">
         <v>43950</v>
       </c>
@@ -13694,7 +13810,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" s="30">
         <v>43951</v>
       </c>
@@ -13747,7 +13863,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" s="30">
         <v>43952</v>
       </c>
@@ -13800,7 +13916,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" s="30">
         <v>43953</v>
       </c>
@@ -13853,7 +13969,7 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" s="30">
         <v>43954</v>
       </c>
@@ -13906,7 +14022,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" s="30">
         <v>43955</v>
       </c>
@@ -13959,7 +14075,7 @@
         <v>1279</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" s="30">
         <v>43956</v>
       </c>
@@ -14012,7 +14128,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" s="30">
         <v>43957</v>
       </c>
@@ -14065,7 +14181,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" s="30">
         <v>43958</v>
       </c>
@@ -14118,7 +14234,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" s="30">
         <v>43959</v>
       </c>
@@ -14171,7 +14287,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" s="30">
         <v>43960</v>
       </c>
@@ -14224,7 +14340,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" s="30">
         <v>43961</v>
       </c>
@@ -14277,7 +14393,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50" s="30">
         <v>43962</v>
       </c>
@@ -14330,7 +14446,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51" s="30">
         <v>43963</v>
       </c>
@@ -14383,7 +14499,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52" s="30">
         <v>43964</v>
       </c>
@@ -14436,7 +14552,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53" s="30">
         <v>43965</v>
       </c>
@@ -14489,7 +14605,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54" s="30">
         <v>43966</v>
       </c>
@@ -14542,7 +14658,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55" s="30">
         <v>43967</v>
       </c>
@@ -14595,7 +14711,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56" s="30">
         <v>43968</v>
       </c>
@@ -14648,7 +14764,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A57" s="30">
         <v>43969</v>
       </c>
@@ -14701,7 +14817,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A58" s="30">
         <v>43970</v>
       </c>
@@ -14754,7 +14870,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A59" s="30">
         <v>43971</v>
       </c>
@@ -14807,7 +14923,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A60" s="30">
         <v>43972</v>
       </c>
@@ -14860,7 +14976,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A61" s="30">
         <v>43973</v>
       </c>
@@ -14913,7 +15029,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A62" s="30">
         <v>43974</v>
       </c>
@@ -14966,7 +15082,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A63" s="30">
         <v>43975</v>
       </c>
@@ -15019,7 +15135,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A64" s="30">
         <v>43976</v>
       </c>
@@ -15072,7 +15188,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A65" s="51">
         <v>43977</v>
       </c>
@@ -15125,7 +15241,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A66" s="51">
         <v>43978</v>
       </c>
@@ -15178,7 +15294,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A67" s="51">
         <v>43979</v>
       </c>
@@ -15231,7 +15347,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A68" s="51">
         <v>43980</v>
       </c>
@@ -15284,7 +15400,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A69" s="51">
         <v>43981</v>
       </c>
@@ -15337,7 +15453,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A70" s="51">
         <v>43982</v>
       </c>
@@ -15390,7 +15506,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A71" s="51">
         <v>43983</v>
       </c>
@@ -15443,7 +15559,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A72" s="51">
         <v>43984</v>
       </c>
@@ -15496,7 +15612,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A73" s="51">
         <v>43985</v>
       </c>
@@ -15547,6 +15663,59 @@
       </c>
       <c r="Q73" s="13">
         <v>706</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A74" s="51">
+        <v>43986</v>
+      </c>
+      <c r="B74" s="11">
+        <v>8</v>
+      </c>
+      <c r="C74" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D74" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E74" s="11">
+        <v>57</v>
+      </c>
+      <c r="F74" s="11">
+        <v>14</v>
+      </c>
+      <c r="G74" s="11">
+        <v>66</v>
+      </c>
+      <c r="H74" s="11">
+        <v>317</v>
+      </c>
+      <c r="I74" s="11">
+        <v>8</v>
+      </c>
+      <c r="J74" s="11">
+        <v>62</v>
+      </c>
+      <c r="K74" s="11">
+        <v>145</v>
+      </c>
+      <c r="L74" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M74" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N74" s="11">
+        <v>8</v>
+      </c>
+      <c r="O74" s="14">
+        <v>0</v>
+      </c>
+      <c r="P74" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q74" s="13">
+        <v>685</v>
       </c>
     </row>
   </sheetData>
@@ -15557,23 +15726,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q73"/>
+  <dimension ref="A1:Q74"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B62" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Q73" sqref="Q73"/>
+      <selection pane="bottomRight" activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5703125" style="2"/>
+    <col min="1" max="1" width="12.453125" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.54296875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -15594,7 +15763,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -15615,7 +15784,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -15668,7 +15837,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="12">
         <v>43916</v>
       </c>
@@ -15721,7 +15890,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
         <v>43917</v>
       </c>
@@ -15774,7 +15943,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="12">
         <v>43918</v>
       </c>
@@ -15827,7 +15996,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
         <v>43919</v>
       </c>
@@ -15880,7 +16049,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="12">
         <v>43920</v>
       </c>
@@ -15933,7 +16102,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="12">
         <v>43921</v>
       </c>
@@ -15986,7 +16155,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="12">
         <v>43922</v>
       </c>
@@ -16039,7 +16208,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
         <v>43923</v>
       </c>
@@ -16092,7 +16261,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="12">
         <v>43924</v>
       </c>
@@ -16145,7 +16314,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <v>43925</v>
       </c>
@@ -16198,7 +16367,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>43926</v>
       </c>
@@ -16251,7 +16420,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="12">
         <v>43927</v>
       </c>
@@ -16304,7 +16473,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="12">
         <v>43928</v>
       </c>
@@ -16357,7 +16526,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="12">
         <v>43929</v>
       </c>
@@ -16410,7 +16579,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="12">
         <v>43930</v>
       </c>
@@ -16463,7 +16632,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="12">
         <v>43931</v>
       </c>
@@ -16516,7 +16685,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="12">
         <v>43932</v>
       </c>
@@ -16569,7 +16738,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="12">
         <v>43933</v>
       </c>
@@ -16622,7 +16791,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="12">
         <v>43934</v>
       </c>
@@ -16675,7 +16844,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="12">
         <v>43935</v>
       </c>
@@ -16728,7 +16897,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" s="12">
         <v>43936</v>
       </c>
@@ -16781,7 +16950,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" s="12">
         <v>43937</v>
       </c>
@@ -16834,7 +17003,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" s="12">
         <v>43938</v>
       </c>
@@ -16887,7 +17056,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" s="12">
         <v>43939</v>
       </c>
@@ -16940,7 +17109,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" s="12">
         <v>43940</v>
       </c>
@@ -16993,7 +17162,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" s="12">
         <v>43941</v>
       </c>
@@ -17046,7 +17215,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" s="12">
         <v>43942</v>
       </c>
@@ -17099,7 +17268,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="12">
         <v>43943</v>
       </c>
@@ -17152,7 +17321,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" s="12">
         <v>43944</v>
       </c>
@@ -17205,7 +17374,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" s="12">
         <v>43945</v>
       </c>
@@ -17258,7 +17427,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" s="12">
         <v>43946</v>
       </c>
@@ -17311,7 +17480,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" s="12">
         <v>43947</v>
       </c>
@@ -17364,7 +17533,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" s="30">
         <v>43948</v>
       </c>
@@ -17417,7 +17586,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" s="30">
         <v>43949</v>
       </c>
@@ -17470,7 +17639,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" s="30">
         <v>43950</v>
       </c>
@@ -17523,7 +17692,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" s="30">
         <v>43951</v>
       </c>
@@ -17576,7 +17745,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" s="30">
         <v>43952</v>
       </c>
@@ -17629,7 +17798,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" s="30">
         <v>43953</v>
       </c>
@@ -17682,7 +17851,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" s="30">
         <v>43954</v>
       </c>
@@ -17735,7 +17904,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" s="30">
         <v>43955</v>
       </c>
@@ -17788,7 +17957,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" s="30">
         <v>43956</v>
       </c>
@@ -17841,7 +18010,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" s="30">
         <v>43957</v>
       </c>
@@ -17894,7 +18063,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" s="30">
         <v>43958</v>
       </c>
@@ -17947,7 +18116,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" s="30">
         <v>43959</v>
       </c>
@@ -18000,7 +18169,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" s="30">
         <v>43960</v>
       </c>
@@ -18053,7 +18222,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" s="30">
         <v>43961</v>
       </c>
@@ -18106,7 +18275,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50" s="30">
         <v>43962</v>
       </c>
@@ -18159,7 +18328,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51" s="30">
         <v>43963</v>
       </c>
@@ -18212,7 +18381,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52" s="30">
         <v>43964</v>
       </c>
@@ -18265,7 +18434,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53" s="30">
         <v>43965</v>
       </c>
@@ -18318,7 +18487,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54" s="30">
         <v>43966</v>
       </c>
@@ -18371,7 +18540,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55" s="30">
         <v>43967</v>
       </c>
@@ -18424,7 +18593,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56" s="30">
         <v>43968</v>
       </c>
@@ -18477,7 +18646,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A57" s="30">
         <v>43969</v>
       </c>
@@ -18530,7 +18699,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A58" s="30">
         <v>43970</v>
       </c>
@@ -18583,7 +18752,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A59" s="30">
         <v>43971</v>
       </c>
@@ -18636,7 +18805,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A60" s="30">
         <v>43972</v>
       </c>
@@ -18689,7 +18858,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A61" s="30">
         <v>43973</v>
       </c>
@@ -18742,7 +18911,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A62" s="30">
         <v>43974</v>
       </c>
@@ -18795,7 +18964,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A63" s="30">
         <v>43975</v>
       </c>
@@ -18848,7 +19017,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A64" s="30">
         <v>43976</v>
       </c>
@@ -18901,7 +19070,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A65" s="30">
         <v>43977</v>
       </c>
@@ -18954,7 +19123,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A66" s="30">
         <v>43978</v>
       </c>
@@ -19007,7 +19176,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A67" s="30">
         <v>43979</v>
       </c>
@@ -19060,7 +19229,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A68" s="30">
         <v>43980</v>
       </c>
@@ -19113,7 +19282,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A69" s="30">
         <v>43981</v>
       </c>
@@ -19166,7 +19335,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A70" s="30">
         <v>43982</v>
       </c>
@@ -19219,7 +19388,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A71" s="30">
         <v>43983</v>
       </c>
@@ -19272,7 +19441,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A72" s="30">
         <v>43984</v>
       </c>
@@ -19325,7 +19494,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A73" s="30">
         <v>43985</v>
       </c>
@@ -19376,6 +19545,59 @@
       </c>
       <c r="Q73" s="13">
         <v>411</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A74" s="30">
+        <v>43986</v>
+      </c>
+      <c r="B74" s="11">
+        <v>37</v>
+      </c>
+      <c r="C74" s="11">
+        <v>19</v>
+      </c>
+      <c r="D74" s="11">
+        <v>5</v>
+      </c>
+      <c r="E74" s="11">
+        <v>9</v>
+      </c>
+      <c r="F74" s="11">
+        <v>31</v>
+      </c>
+      <c r="G74" s="11">
+        <v>18</v>
+      </c>
+      <c r="H74" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I74" s="11">
+        <v>17</v>
+      </c>
+      <c r="J74" s="11">
+        <v>83</v>
+      </c>
+      <c r="K74" s="11">
+        <v>101</v>
+      </c>
+      <c r="L74" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M74" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N74" s="11">
+        <v>11</v>
+      </c>
+      <c r="O74" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P74" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q74" s="13">
+        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -19402,13 +19624,13 @@
       <value order="0">false</value>
     </field>
     <field name="Objective-IsPublished">
-      <value order="0">true</value>
+      <value order="0">false</value>
     </field>
     <field name="Objective-DatePublished">
-      <value order="0">2020-06-03T12:41:24Z</value>
+      <value order="0"/>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-03T12:41:24Z</value>
+      <value order="0">2020-06-04T12:39:07Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -19420,16 +19642,16 @@
       <value order="0">Analytical: COVID 19 Analysis: Restricted working papers: Research and analysis: Diseases: 2020-2025</value>
     </field>
     <field name="Objective-State">
-      <value order="0">Published</value>
+      <value order="0">Being Drafted</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41513351</value>
+      <value order="0">vA41545770</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">18.0</value>
+      <value order="0">19.1</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">144</value>
+      <value order="0">148</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-05 20:08)
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1605" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1632" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -1675,7 +1675,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1785,10 +1787,10 @@
   <dimension ref="A1:S160"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B75" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B81" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I94" sqref="I94"/>
+      <selection pane="bottomRight" activeCell="F96" sqref="F96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6394,21 +6396,54 @@
       </c>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B94" s="28"/>
-      <c r="C94" s="28"/>
-      <c r="D94" s="28"/>
-      <c r="E94" s="28"/>
-      <c r="F94" s="28"/>
-      <c r="G94" s="28"/>
-      <c r="H94" s="28"/>
-      <c r="I94" s="28"/>
-      <c r="J94" s="28"/>
-      <c r="K94" s="28"/>
-      <c r="L94" s="28"/>
-      <c r="M94" s="28"/>
-      <c r="N94" s="28"/>
-      <c r="O94" s="28"/>
-      <c r="P94" s="28"/>
+      <c r="A94" s="5">
+        <v>43987</v>
+      </c>
+      <c r="B94" s="28">
+        <v>1076</v>
+      </c>
+      <c r="C94" s="28">
+        <v>326</v>
+      </c>
+      <c r="D94" s="28">
+        <v>261</v>
+      </c>
+      <c r="E94" s="28">
+        <v>877</v>
+      </c>
+      <c r="F94" s="28">
+        <v>946</v>
+      </c>
+      <c r="G94" s="28">
+        <v>1284</v>
+      </c>
+      <c r="H94" s="28">
+        <v>3968</v>
+      </c>
+      <c r="I94" s="52">
+        <v>338</v>
+      </c>
+      <c r="J94" s="28">
+        <v>2005</v>
+      </c>
+      <c r="K94" s="28">
+        <v>2760</v>
+      </c>
+      <c r="L94" s="28">
+        <v>8</v>
+      </c>
+      <c r="M94" s="28">
+        <v>54</v>
+      </c>
+      <c r="N94" s="28">
+        <v>1673</v>
+      </c>
+      <c r="O94" s="28">
+        <v>6</v>
+      </c>
+      <c r="P94" s="32">
+        <v>15582</v>
+      </c>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B95" s="28"/>
@@ -7540,11 +7575,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q82"/>
+  <dimension ref="A1:Q83"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P85" sqref="P85"/>
+      <pane ySplit="3" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11836,6 +11871,59 @@
         <v>28</v>
       </c>
     </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A83" s="30">
+        <v>43987</v>
+      </c>
+      <c r="B83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G83" s="11">
+        <v>5</v>
+      </c>
+      <c r="H83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="L83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q83" s="13">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -11844,13 +11932,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q74"/>
+  <dimension ref="A1:Q75"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="L61" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="F64" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Q75" sqref="Q75"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15708,14 +15796,67 @@
       <c r="N74" s="11">
         <v>8</v>
       </c>
-      <c r="O74" s="14">
-        <v>0</v>
-      </c>
-      <c r="P74" s="14">
-        <v>0</v>
+      <c r="O74" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P74" s="14" t="s">
+        <v>29</v>
       </c>
       <c r="Q74" s="13">
         <v>685</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A75" s="51">
+        <v>43987</v>
+      </c>
+      <c r="B75" s="11">
+        <v>8</v>
+      </c>
+      <c r="C75" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D75" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E75" s="11">
+        <v>59</v>
+      </c>
+      <c r="F75" s="11">
+        <v>13</v>
+      </c>
+      <c r="G75" s="11">
+        <v>63</v>
+      </c>
+      <c r="H75" s="11">
+        <v>311</v>
+      </c>
+      <c r="I75" s="11">
+        <v>6</v>
+      </c>
+      <c r="J75" s="11">
+        <v>65</v>
+      </c>
+      <c r="K75" s="11">
+        <v>143</v>
+      </c>
+      <c r="L75" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M75" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N75" s="11">
+        <v>8</v>
+      </c>
+      <c r="O75" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P75" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q75" s="13">
+        <v>676</v>
       </c>
     </row>
   </sheetData>
@@ -15726,13 +15867,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q74"/>
+  <dimension ref="A1:Q75"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B62" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B61" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B74" sqref="B74"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19598,6 +19739,59 @@
       </c>
       <c r="Q74" s="13">
         <v>336</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A75" s="30">
+        <v>43987</v>
+      </c>
+      <c r="B75" s="11">
+        <v>34</v>
+      </c>
+      <c r="C75" s="11">
+        <v>13</v>
+      </c>
+      <c r="D75" s="11">
+        <v>10</v>
+      </c>
+      <c r="E75" s="11">
+        <v>21</v>
+      </c>
+      <c r="F75" s="11">
+        <v>30</v>
+      </c>
+      <c r="G75" s="11">
+        <v>14</v>
+      </c>
+      <c r="H75" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I75" s="11">
+        <v>33</v>
+      </c>
+      <c r="J75" s="11">
+        <v>76</v>
+      </c>
+      <c r="K75" s="11">
+        <v>76</v>
+      </c>
+      <c r="L75" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M75" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N75" s="11">
+        <v>7</v>
+      </c>
+      <c r="O75" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P75" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q75" s="13">
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -19624,13 +19818,13 @@
       <value order="0">false</value>
     </field>
     <field name="Objective-IsPublished">
-      <value order="0">false</value>
+      <value order="0">true</value>
     </field>
     <field name="Objective-DatePublished">
-      <value order="0"/>
+      <value order="0">2020-06-05T12:12:14Z</value>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-04T12:39:07Z</value>
+      <value order="0">2020-06-05T12:12:14Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -19642,16 +19836,16 @@
       <value order="0">Analytical: COVID 19 Analysis: Restricted working papers: Research and analysis: Diseases: 2020-2025</value>
     </field>
     <field name="Objective-State">
-      <value order="0">Being Drafted</value>
+      <value order="0">Published</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41545770</value>
+      <value order="0">vA41574143</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">19.1</value>
+      <value order="0">20.0</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">148</value>
+      <value order="0">151</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-06 12:09)
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1605" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1632" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -1675,7 +1675,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1785,10 +1787,10 @@
   <dimension ref="A1:S160"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B75" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B81" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I94" sqref="I94"/>
+      <selection pane="bottomRight" activeCell="F96" sqref="F96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6394,21 +6396,54 @@
       </c>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B94" s="28"/>
-      <c r="C94" s="28"/>
-      <c r="D94" s="28"/>
-      <c r="E94" s="28"/>
-      <c r="F94" s="28"/>
-      <c r="G94" s="28"/>
-      <c r="H94" s="28"/>
-      <c r="I94" s="28"/>
-      <c r="J94" s="28"/>
-      <c r="K94" s="28"/>
-      <c r="L94" s="28"/>
-      <c r="M94" s="28"/>
-      <c r="N94" s="28"/>
-      <c r="O94" s="28"/>
-      <c r="P94" s="28"/>
+      <c r="A94" s="5">
+        <v>43987</v>
+      </c>
+      <c r="B94" s="28">
+        <v>1076</v>
+      </c>
+      <c r="C94" s="28">
+        <v>326</v>
+      </c>
+      <c r="D94" s="28">
+        <v>261</v>
+      </c>
+      <c r="E94" s="28">
+        <v>877</v>
+      </c>
+      <c r="F94" s="28">
+        <v>946</v>
+      </c>
+      <c r="G94" s="28">
+        <v>1284</v>
+      </c>
+      <c r="H94" s="28">
+        <v>3968</v>
+      </c>
+      <c r="I94" s="52">
+        <v>338</v>
+      </c>
+      <c r="J94" s="28">
+        <v>2005</v>
+      </c>
+      <c r="K94" s="28">
+        <v>2760</v>
+      </c>
+      <c r="L94" s="28">
+        <v>8</v>
+      </c>
+      <c r="M94" s="28">
+        <v>54</v>
+      </c>
+      <c r="N94" s="28">
+        <v>1673</v>
+      </c>
+      <c r="O94" s="28">
+        <v>6</v>
+      </c>
+      <c r="P94" s="32">
+        <v>15582</v>
+      </c>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B95" s="28"/>
@@ -7540,11 +7575,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q82"/>
+  <dimension ref="A1:Q83"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P85" sqref="P85"/>
+      <pane ySplit="3" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11836,6 +11871,59 @@
         <v>28</v>
       </c>
     </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A83" s="30">
+        <v>43987</v>
+      </c>
+      <c r="B83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G83" s="11">
+        <v>5</v>
+      </c>
+      <c r="H83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="L83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q83" s="13">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -11844,13 +11932,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q74"/>
+  <dimension ref="A1:Q75"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="L61" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="F64" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Q75" sqref="Q75"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15708,14 +15796,67 @@
       <c r="N74" s="11">
         <v>8</v>
       </c>
-      <c r="O74" s="14">
-        <v>0</v>
-      </c>
-      <c r="P74" s="14">
-        <v>0</v>
+      <c r="O74" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P74" s="14" t="s">
+        <v>29</v>
       </c>
       <c r="Q74" s="13">
         <v>685</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A75" s="51">
+        <v>43987</v>
+      </c>
+      <c r="B75" s="11">
+        <v>8</v>
+      </c>
+      <c r="C75" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D75" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E75" s="11">
+        <v>59</v>
+      </c>
+      <c r="F75" s="11">
+        <v>13</v>
+      </c>
+      <c r="G75" s="11">
+        <v>63</v>
+      </c>
+      <c r="H75" s="11">
+        <v>311</v>
+      </c>
+      <c r="I75" s="11">
+        <v>6</v>
+      </c>
+      <c r="J75" s="11">
+        <v>65</v>
+      </c>
+      <c r="K75" s="11">
+        <v>143</v>
+      </c>
+      <c r="L75" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M75" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N75" s="11">
+        <v>8</v>
+      </c>
+      <c r="O75" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P75" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q75" s="13">
+        <v>676</v>
       </c>
     </row>
   </sheetData>
@@ -15726,13 +15867,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q74"/>
+  <dimension ref="A1:Q75"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B62" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B61" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B74" sqref="B74"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19598,6 +19739,59 @@
       </c>
       <c r="Q74" s="13">
         <v>336</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A75" s="30">
+        <v>43987</v>
+      </c>
+      <c r="B75" s="11">
+        <v>34</v>
+      </c>
+      <c r="C75" s="11">
+        <v>13</v>
+      </c>
+      <c r="D75" s="11">
+        <v>10</v>
+      </c>
+      <c r="E75" s="11">
+        <v>21</v>
+      </c>
+      <c r="F75" s="11">
+        <v>30</v>
+      </c>
+      <c r="G75" s="11">
+        <v>14</v>
+      </c>
+      <c r="H75" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I75" s="11">
+        <v>33</v>
+      </c>
+      <c r="J75" s="11">
+        <v>76</v>
+      </c>
+      <c r="K75" s="11">
+        <v>76</v>
+      </c>
+      <c r="L75" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M75" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N75" s="11">
+        <v>7</v>
+      </c>
+      <c r="O75" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P75" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q75" s="13">
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -19624,13 +19818,13 @@
       <value order="0">false</value>
     </field>
     <field name="Objective-IsPublished">
-      <value order="0">false</value>
+      <value order="0">true</value>
     </field>
     <field name="Objective-DatePublished">
-      <value order="0"/>
+      <value order="0">2020-06-05T12:12:14Z</value>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-04T12:39:07Z</value>
+      <value order="0">2020-06-05T12:12:14Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -19642,16 +19836,16 @@
       <value order="0">Analytical: COVID 19 Analysis: Restricted working papers: Research and analysis: Diseases: 2020-2025</value>
     </field>
     <field name="Objective-State">
-      <value order="0">Being Drafted</value>
+      <value order="0">Published</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41545770</value>
+      <value order="0">vA41574143</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">19.1</value>
+      <value order="0">20.0</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">148</value>
+      <value order="0">151</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-06 12:09) (#90)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1605" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1632" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -1675,7 +1675,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1785,10 +1787,10 @@
   <dimension ref="A1:S160"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B75" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B81" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I94" sqref="I94"/>
+      <selection pane="bottomRight" activeCell="F96" sqref="F96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6394,21 +6396,54 @@
       </c>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B94" s="28"/>
-      <c r="C94" s="28"/>
-      <c r="D94" s="28"/>
-      <c r="E94" s="28"/>
-      <c r="F94" s="28"/>
-      <c r="G94" s="28"/>
-      <c r="H94" s="28"/>
-      <c r="I94" s="28"/>
-      <c r="J94" s="28"/>
-      <c r="K94" s="28"/>
-      <c r="L94" s="28"/>
-      <c r="M94" s="28"/>
-      <c r="N94" s="28"/>
-      <c r="O94" s="28"/>
-      <c r="P94" s="28"/>
+      <c r="A94" s="5">
+        <v>43987</v>
+      </c>
+      <c r="B94" s="28">
+        <v>1076</v>
+      </c>
+      <c r="C94" s="28">
+        <v>326</v>
+      </c>
+      <c r="D94" s="28">
+        <v>261</v>
+      </c>
+      <c r="E94" s="28">
+        <v>877</v>
+      </c>
+      <c r="F94" s="28">
+        <v>946</v>
+      </c>
+      <c r="G94" s="28">
+        <v>1284</v>
+      </c>
+      <c r="H94" s="28">
+        <v>3968</v>
+      </c>
+      <c r="I94" s="52">
+        <v>338</v>
+      </c>
+      <c r="J94" s="28">
+        <v>2005</v>
+      </c>
+      <c r="K94" s="28">
+        <v>2760</v>
+      </c>
+      <c r="L94" s="28">
+        <v>8</v>
+      </c>
+      <c r="M94" s="28">
+        <v>54</v>
+      </c>
+      <c r="N94" s="28">
+        <v>1673</v>
+      </c>
+      <c r="O94" s="28">
+        <v>6</v>
+      </c>
+      <c r="P94" s="32">
+        <v>15582</v>
+      </c>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B95" s="28"/>
@@ -7540,11 +7575,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q82"/>
+  <dimension ref="A1:Q83"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P85" sqref="P85"/>
+      <pane ySplit="3" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11836,6 +11871,59 @@
         <v>28</v>
       </c>
     </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A83" s="30">
+        <v>43987</v>
+      </c>
+      <c r="B83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G83" s="11">
+        <v>5</v>
+      </c>
+      <c r="H83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="L83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P83" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q83" s="13">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -11844,13 +11932,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q74"/>
+  <dimension ref="A1:Q75"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="L61" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="F64" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Q75" sqref="Q75"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15708,14 +15796,67 @@
       <c r="N74" s="11">
         <v>8</v>
       </c>
-      <c r="O74" s="14">
-        <v>0</v>
-      </c>
-      <c r="P74" s="14">
-        <v>0</v>
+      <c r="O74" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P74" s="14" t="s">
+        <v>29</v>
       </c>
       <c r="Q74" s="13">
         <v>685</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A75" s="51">
+        <v>43987</v>
+      </c>
+      <c r="B75" s="11">
+        <v>8</v>
+      </c>
+      <c r="C75" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D75" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E75" s="11">
+        <v>59</v>
+      </c>
+      <c r="F75" s="11">
+        <v>13</v>
+      </c>
+      <c r="G75" s="11">
+        <v>63</v>
+      </c>
+      <c r="H75" s="11">
+        <v>311</v>
+      </c>
+      <c r="I75" s="11">
+        <v>6</v>
+      </c>
+      <c r="J75" s="11">
+        <v>65</v>
+      </c>
+      <c r="K75" s="11">
+        <v>143</v>
+      </c>
+      <c r="L75" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M75" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N75" s="11">
+        <v>8</v>
+      </c>
+      <c r="O75" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P75" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q75" s="13">
+        <v>676</v>
       </c>
     </row>
   </sheetData>
@@ -15726,13 +15867,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q74"/>
+  <dimension ref="A1:Q75"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B62" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B61" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B74" sqref="B74"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19598,6 +19739,59 @@
       </c>
       <c r="Q74" s="13">
         <v>336</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A75" s="30">
+        <v>43987</v>
+      </c>
+      <c r="B75" s="11">
+        <v>34</v>
+      </c>
+      <c r="C75" s="11">
+        <v>13</v>
+      </c>
+      <c r="D75" s="11">
+        <v>10</v>
+      </c>
+      <c r="E75" s="11">
+        <v>21</v>
+      </c>
+      <c r="F75" s="11">
+        <v>30</v>
+      </c>
+      <c r="G75" s="11">
+        <v>14</v>
+      </c>
+      <c r="H75" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I75" s="11">
+        <v>33</v>
+      </c>
+      <c r="J75" s="11">
+        <v>76</v>
+      </c>
+      <c r="K75" s="11">
+        <v>76</v>
+      </c>
+      <c r="L75" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M75" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N75" s="11">
+        <v>7</v>
+      </c>
+      <c r="O75" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P75" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q75" s="13">
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -19624,13 +19818,13 @@
       <value order="0">false</value>
     </field>
     <field name="Objective-IsPublished">
-      <value order="0">false</value>
+      <value order="0">true</value>
     </field>
     <field name="Objective-DatePublished">
-      <value order="0"/>
+      <value order="0">2020-06-05T12:12:14Z</value>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-04T12:39:07Z</value>
+      <value order="0">2020-06-05T12:12:14Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -19642,16 +19836,16 @@
       <value order="0">Analytical: COVID 19 Analysis: Restricted working papers: Research and analysis: Diseases: 2020-2025</value>
     </field>
     <field name="Objective-State">
-      <value order="0">Being Drafted</value>
+      <value order="0">Published</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41545770</value>
+      <value order="0">vA41574143</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">19.1</value>
+      <value order="0">20.0</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">148</value>
+      <value order="0">151</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-06 20:08)
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u207826\Objective\Objects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\scotland.gov.uk\dc2\FS5_Home\u204186\Gov.scot content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5990" windowHeight="6020" tabRatio="803"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5985" windowHeight="6030" tabRatio="803"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1632" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1657" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -1676,24 +1676,24 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.453125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="90.453125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.453125" style="2"/>
+    <col min="2" max="2" width="29.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="90.42578125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>20</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
         <v>22</v>
       </c>
@@ -1709,13 +1709,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="22" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="23"/>
     </row>
-    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="24" t="s">
         <v>26</v>
       </c>
@@ -1723,7 +1723,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="24" t="s">
         <v>27</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="24" t="s">
         <v>36</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
         <v>37</v>
       </c>
@@ -1767,12 +1767,12 @@
       <selection activeCell="K66" sqref="K66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.453125" style="2"/>
+    <col min="1" max="16384" width="9.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="44" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="43"/>
     </row>
   </sheetData>
@@ -1790,17 +1790,17 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B81" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F96" sqref="F96"/>
+      <selection pane="bottomRight" activeCell="H98" sqref="H98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" style="2" customWidth="1"/>
-    <col min="2" max="16" width="11.453125" style="11" customWidth="1"/>
-    <col min="17" max="16384" width="8.54296875" style="2"/>
+    <col min="2" max="16" width="11.42578125" style="11" customWidth="1"/>
+    <col min="17" max="16384" width="8.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -1820,7 +1820,7 @@
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -1839,7 +1839,7 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>43897</v>
       </c>
@@ -1939,7 +1939,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>43898</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>43899</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>43900</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>43901</v>
       </c>
@@ -2139,7 +2139,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>43902</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>43903</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>43904</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>43905</v>
       </c>
@@ -2339,7 +2339,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>43906</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>43907</v>
       </c>
@@ -2439,7 +2439,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>43908</v>
       </c>
@@ -2489,7 +2489,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>43909</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>43910</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>43911</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>43912</v>
       </c>
@@ -2689,7 +2689,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>43913</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>43914</v>
       </c>
@@ -2789,7 +2789,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>43915</v>
       </c>
@@ -2839,7 +2839,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>43916</v>
       </c>
@@ -2889,7 +2889,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>43917</v>
       </c>
@@ -2939,7 +2939,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>43918</v>
       </c>
@@ -2989,7 +2989,7 @@
         <v>1264</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>43919</v>
       </c>
@@ -3039,7 +3039,7 @@
         <v>1417</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>43920</v>
       </c>
@@ -3089,7 +3089,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>43921</v>
       </c>
@@ -3139,7 +3139,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>43922</v>
       </c>
@@ -3189,7 +3189,7 @@
         <v>2310</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>43923</v>
       </c>
@@ -3239,7 +3239,7 @@
         <v>2602</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>43924</v>
       </c>
@@ -3289,7 +3289,7 @@
         <v>3001</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>43925</v>
       </c>
@@ -3339,7 +3339,7 @@
         <v>3345</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>43926</v>
       </c>
@@ -3389,7 +3389,7 @@
         <v>3706</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>43927</v>
       </c>
@@ -3439,7 +3439,7 @@
         <v>3961</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>43928</v>
       </c>
@@ -3489,7 +3489,7 @@
         <v>4229</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>43929</v>
       </c>
@@ -3539,7 +3539,7 @@
         <v>4565</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>43930</v>
       </c>
@@ -3589,7 +3589,7 @@
         <v>4957</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>43931</v>
       </c>
@@ -3639,7 +3639,7 @@
         <v>5275</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>43932</v>
       </c>
@@ -3689,7 +3689,7 @@
         <v>5590</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>43933</v>
       </c>
@@ -3739,7 +3739,7 @@
         <v>5912</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>43934</v>
       </c>
@@ -3789,7 +3789,7 @@
         <v>6067</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>43935</v>
       </c>
@@ -3839,7 +3839,7 @@
         <v>6358</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>43936</v>
       </c>
@@ -3889,7 +3889,7 @@
         <v>6748</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>43937</v>
       </c>
@@ -3939,7 +3939,7 @@
         <v>7102</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>43938</v>
       </c>
@@ -3989,7 +3989,7 @@
         <v>7409</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>43939</v>
       </c>
@@ -4039,7 +4039,7 @@
         <v>7820</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>43940</v>
       </c>
@@ -4089,7 +4089,7 @@
         <v>8187</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>43941</v>
       </c>
@@ -4139,7 +4139,7 @@
         <v>8450</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>43942</v>
       </c>
@@ -4189,7 +4189,7 @@
         <v>8672</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>43943</v>
       </c>
@@ -4239,7 +4239,7 @@
         <v>9038</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>43944</v>
       </c>
@@ -4289,7 +4289,7 @@
         <v>9409</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>43945</v>
       </c>
@@ -4339,7 +4339,7 @@
         <v>9697</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>43946</v>
       </c>
@@ -4389,7 +4389,7 @@
         <v>10051</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>43947</v>
       </c>
@@ -4440,7 +4440,7 @@
       </c>
       <c r="R54" s="38"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>43948</v>
       </c>
@@ -4491,7 +4491,7 @@
       </c>
       <c r="R55" s="38"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>43949</v>
       </c>
@@ -4542,7 +4542,7 @@
       </c>
       <c r="R56" s="39"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>43950</v>
       </c>
@@ -4592,7 +4592,7 @@
         <v>11034</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>43951</v>
       </c>
@@ -4643,7 +4643,7 @@
       </c>
       <c r="R58" s="38"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>43952</v>
       </c>
@@ -4695,7 +4695,7 @@
       <c r="R59" s="38"/>
       <c r="S59" s="38"/>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>43953</v>
       </c>
@@ -4745,7 +4745,7 @@
         <v>11927</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>43954</v>
       </c>
@@ -4795,7 +4795,7 @@
         <v>12097</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>43955</v>
       </c>
@@ -4845,7 +4845,7 @@
         <v>12266</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
         <v>43956</v>
       </c>
@@ -4895,7 +4895,7 @@
         <v>12437</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
         <v>43957</v>
       </c>
@@ -4945,7 +4945,7 @@
         <v>12709</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
         <v>43958</v>
       </c>
@@ -4995,7 +4995,7 @@
         <v>12924</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
         <v>43959</v>
       </c>
@@ -5045,7 +5045,7 @@
         <v>13149</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
         <v>43960</v>
       </c>
@@ -5095,7 +5095,7 @@
         <v>13305</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
         <v>43961</v>
       </c>
@@ -5145,7 +5145,7 @@
         <v>13486</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
         <v>43962</v>
       </c>
@@ -5195,7 +5195,7 @@
         <v>13627</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>43963</v>
       </c>
@@ -5245,7 +5245,7 @@
         <v>13763</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
         <v>43964</v>
       </c>
@@ -5295,7 +5295,7 @@
         <v>13929</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <v>43965</v>
       </c>
@@ -5345,7 +5345,7 @@
         <v>14117</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
         <v>43966</v>
       </c>
@@ -5395,7 +5395,7 @@
         <v>14260</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <v>43967</v>
       </c>
@@ -5445,7 +5445,7 @@
         <v>14447</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
         <v>43968</v>
       </c>
@@ -5495,7 +5495,7 @@
         <v>14537</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
         <v>43969</v>
       </c>
@@ -5545,7 +5545,7 @@
         <v>14594</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" s="5">
         <v>43970</v>
       </c>
@@ -5595,7 +5595,7 @@
         <v>14655</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
         <v>43971</v>
       </c>
@@ -5645,7 +5645,7 @@
         <v>14751</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" s="5">
         <v>43972</v>
       </c>
@@ -5695,7 +5695,7 @@
         <v>14856</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
         <v>43973</v>
       </c>
@@ -5745,7 +5745,7 @@
         <v>14969</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
         <v>43974</v>
       </c>
@@ -5795,7 +5795,7 @@
         <v>15041</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
         <v>43975</v>
       </c>
@@ -5845,7 +5845,7 @@
         <v>15101</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" s="5">
         <v>43976</v>
       </c>
@@ -5895,7 +5895,7 @@
         <v>15156</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" s="5">
         <v>43977</v>
       </c>
@@ -5945,7 +5945,7 @@
         <v>15185</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" s="5">
         <v>43978</v>
       </c>
@@ -5995,7 +5995,7 @@
         <v>15240</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" s="5">
         <v>43979</v>
       </c>
@@ -6045,7 +6045,7 @@
         <v>15288</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" s="5">
         <v>43980</v>
       </c>
@@ -6095,7 +6095,7 @@
         <v>15327</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" s="5">
         <v>43981</v>
       </c>
@@ -6145,7 +6145,7 @@
         <v>15382</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" s="5">
         <v>43982</v>
       </c>
@@ -6195,7 +6195,7 @@
         <v>15400</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" s="5">
         <v>43983</v>
       </c>
@@ -6245,7 +6245,7 @@
         <v>15418</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" s="5">
         <v>43984</v>
       </c>
@@ -6295,7 +6295,7 @@
         <v>15471</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
         <v>43985</v>
       </c>
@@ -6345,7 +6345,7 @@
         <v>15504</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" s="5">
         <v>43986</v>
       </c>
@@ -6395,7 +6395,7 @@
         <v>15553</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
         <v>43987</v>
       </c>
@@ -6445,24 +6445,57 @@
         <v>15582</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B95" s="28"/>
-      <c r="C95" s="28"/>
-      <c r="D95" s="28"/>
-      <c r="E95" s="28"/>
-      <c r="F95" s="28"/>
-      <c r="G95" s="28"/>
-      <c r="H95" s="28"/>
-      <c r="I95" s="28"/>
-      <c r="J95" s="28"/>
-      <c r="K95" s="28"/>
-      <c r="L95" s="28"/>
-      <c r="M95" s="28"/>
-      <c r="N95" s="28"/>
-      <c r="O95" s="28"/>
-      <c r="P95" s="28"/>
-    </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A95" s="5">
+        <v>43988</v>
+      </c>
+      <c r="B95" s="28">
+        <v>1077</v>
+      </c>
+      <c r="C95" s="28">
+        <v>326</v>
+      </c>
+      <c r="D95" s="28">
+        <v>261</v>
+      </c>
+      <c r="E95" s="28">
+        <v>879</v>
+      </c>
+      <c r="F95" s="28">
+        <v>946</v>
+      </c>
+      <c r="G95" s="28">
+        <v>1284</v>
+      </c>
+      <c r="H95" s="28">
+        <v>3971</v>
+      </c>
+      <c r="I95" s="28">
+        <v>339</v>
+      </c>
+      <c r="J95" s="28">
+        <v>2007</v>
+      </c>
+      <c r="K95" s="28">
+        <v>2769</v>
+      </c>
+      <c r="L95" s="28">
+        <v>8</v>
+      </c>
+      <c r="M95" s="28">
+        <v>54</v>
+      </c>
+      <c r="N95" s="28">
+        <v>1676</v>
+      </c>
+      <c r="O95" s="28">
+        <v>6</v>
+      </c>
+      <c r="P95" s="32">
+        <v>15603</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B96" s="28"/>
       <c r="C96" s="28"/>
       <c r="D96" s="28"/>
@@ -6479,7 +6512,7 @@
       <c r="O96" s="28"/>
       <c r="P96" s="28"/>
     </row>
-    <row r="97" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B97" s="28"/>
       <c r="C97" s="28"/>
       <c r="D97" s="28"/>
@@ -6496,7 +6529,7 @@
       <c r="O97" s="28"/>
       <c r="P97" s="28"/>
     </row>
-    <row r="98" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B98" s="28"/>
       <c r="C98" s="28"/>
       <c r="D98" s="28"/>
@@ -6513,7 +6546,7 @@
       <c r="O98" s="28"/>
       <c r="P98" s="28"/>
     </row>
-    <row r="99" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B99" s="28"/>
       <c r="C99" s="28"/>
       <c r="D99" s="28"/>
@@ -6530,7 +6563,7 @@
       <c r="O99" s="28"/>
       <c r="P99" s="28"/>
     </row>
-    <row r="100" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B100" s="28"/>
       <c r="C100" s="28"/>
       <c r="D100" s="28"/>
@@ -6547,7 +6580,7 @@
       <c r="O100" s="28"/>
       <c r="P100" s="28"/>
     </row>
-    <row r="101" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B101" s="28"/>
       <c r="C101" s="28"/>
       <c r="D101" s="28"/>
@@ -6564,7 +6597,7 @@
       <c r="O101" s="28"/>
       <c r="P101" s="28"/>
     </row>
-    <row r="102" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B102" s="28"/>
       <c r="C102" s="28"/>
       <c r="D102" s="28"/>
@@ -6581,7 +6614,7 @@
       <c r="O102" s="28"/>
       <c r="P102" s="28"/>
     </row>
-    <row r="103" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B103" s="28"/>
       <c r="C103" s="28"/>
       <c r="D103" s="28"/>
@@ -6598,7 +6631,7 @@
       <c r="O103" s="28"/>
       <c r="P103" s="28"/>
     </row>
-    <row r="104" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B104" s="28"/>
       <c r="C104" s="28"/>
       <c r="D104" s="28"/>
@@ -6615,7 +6648,7 @@
       <c r="O104" s="28"/>
       <c r="P104" s="28"/>
     </row>
-    <row r="105" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B105" s="28"/>
       <c r="C105" s="28"/>
       <c r="D105" s="28"/>
@@ -6632,7 +6665,7 @@
       <c r="O105" s="28"/>
       <c r="P105" s="28"/>
     </row>
-    <row r="106" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B106" s="28"/>
       <c r="C106" s="28"/>
       <c r="D106" s="28"/>
@@ -6649,7 +6682,7 @@
       <c r="O106" s="28"/>
       <c r="P106" s="28"/>
     </row>
-    <row r="107" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B107" s="28"/>
       <c r="C107" s="28"/>
       <c r="D107" s="28"/>
@@ -6666,7 +6699,7 @@
       <c r="O107" s="28"/>
       <c r="P107" s="28"/>
     </row>
-    <row r="108" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B108" s="28"/>
       <c r="C108" s="28"/>
       <c r="D108" s="28"/>
@@ -6683,7 +6716,7 @@
       <c r="O108" s="28"/>
       <c r="P108" s="28"/>
     </row>
-    <row r="109" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B109" s="28"/>
       <c r="C109" s="28"/>
       <c r="D109" s="28"/>
@@ -6700,7 +6733,7 @@
       <c r="O109" s="28"/>
       <c r="P109" s="28"/>
     </row>
-    <row r="110" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B110" s="28"/>
       <c r="C110" s="28"/>
       <c r="D110" s="28"/>
@@ -6717,7 +6750,7 @@
       <c r="O110" s="28"/>
       <c r="P110" s="28"/>
     </row>
-    <row r="111" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B111" s="28"/>
       <c r="C111" s="28"/>
       <c r="D111" s="28"/>
@@ -6734,7 +6767,7 @@
       <c r="O111" s="28"/>
       <c r="P111" s="28"/>
     </row>
-    <row r="112" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B112" s="28"/>
       <c r="C112" s="28"/>
       <c r="D112" s="28"/>
@@ -6751,7 +6784,7 @@
       <c r="O112" s="28"/>
       <c r="P112" s="28"/>
     </row>
-    <row r="113" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B113" s="28"/>
       <c r="C113" s="28"/>
       <c r="D113" s="28"/>
@@ -6768,7 +6801,7 @@
       <c r="O113" s="28"/>
       <c r="P113" s="28"/>
     </row>
-    <row r="114" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B114" s="28"/>
       <c r="C114" s="28"/>
       <c r="D114" s="28"/>
@@ -6785,7 +6818,7 @@
       <c r="O114" s="28"/>
       <c r="P114" s="28"/>
     </row>
-    <row r="115" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B115" s="28"/>
       <c r="C115" s="28"/>
       <c r="D115" s="28"/>
@@ -6802,7 +6835,7 @@
       <c r="O115" s="28"/>
       <c r="P115" s="28"/>
     </row>
-    <row r="116" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B116" s="28"/>
       <c r="C116" s="28"/>
       <c r="D116" s="28"/>
@@ -6819,7 +6852,7 @@
       <c r="O116" s="28"/>
       <c r="P116" s="28"/>
     </row>
-    <row r="117" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B117" s="28"/>
       <c r="C117" s="28"/>
       <c r="D117" s="28"/>
@@ -6836,7 +6869,7 @@
       <c r="O117" s="28"/>
       <c r="P117" s="28"/>
     </row>
-    <row r="118" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B118" s="28"/>
       <c r="C118" s="28"/>
       <c r="D118" s="28"/>
@@ -6853,7 +6886,7 @@
       <c r="O118" s="28"/>
       <c r="P118" s="28"/>
     </row>
-    <row r="119" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B119" s="28"/>
       <c r="C119" s="28"/>
       <c r="D119" s="28"/>
@@ -6870,7 +6903,7 @@
       <c r="O119" s="28"/>
       <c r="P119" s="28"/>
     </row>
-    <row r="120" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="120" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B120" s="28"/>
       <c r="C120" s="28"/>
       <c r="D120" s="28"/>
@@ -6887,7 +6920,7 @@
       <c r="O120" s="28"/>
       <c r="P120" s="28"/>
     </row>
-    <row r="121" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="121" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B121" s="28"/>
       <c r="C121" s="28"/>
       <c r="D121" s="28"/>
@@ -6904,7 +6937,7 @@
       <c r="O121" s="28"/>
       <c r="P121" s="28"/>
     </row>
-    <row r="122" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="122" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B122" s="28"/>
       <c r="C122" s="28"/>
       <c r="D122" s="28"/>
@@ -6921,7 +6954,7 @@
       <c r="O122" s="28"/>
       <c r="P122" s="28"/>
     </row>
-    <row r="123" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="123" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B123" s="28"/>
       <c r="C123" s="28"/>
       <c r="D123" s="28"/>
@@ -6938,7 +6971,7 @@
       <c r="O123" s="28"/>
       <c r="P123" s="28"/>
     </row>
-    <row r="124" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B124" s="28"/>
       <c r="C124" s="28"/>
       <c r="D124" s="28"/>
@@ -6955,7 +6988,7 @@
       <c r="O124" s="28"/>
       <c r="P124" s="28"/>
     </row>
-    <row r="125" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="125" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B125" s="28"/>
       <c r="C125" s="28"/>
       <c r="D125" s="28"/>
@@ -6972,7 +7005,7 @@
       <c r="O125" s="28"/>
       <c r="P125" s="28"/>
     </row>
-    <row r="126" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="126" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B126" s="28"/>
       <c r="C126" s="28"/>
       <c r="D126" s="28"/>
@@ -6989,7 +7022,7 @@
       <c r="O126" s="28"/>
       <c r="P126" s="28"/>
     </row>
-    <row r="127" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="127" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B127" s="28"/>
       <c r="C127" s="28"/>
       <c r="D127" s="28"/>
@@ -7006,7 +7039,7 @@
       <c r="O127" s="28"/>
       <c r="P127" s="28"/>
     </row>
-    <row r="128" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="128" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B128" s="28"/>
       <c r="C128" s="28"/>
       <c r="D128" s="28"/>
@@ -7023,7 +7056,7 @@
       <c r="O128" s="28"/>
       <c r="P128" s="28"/>
     </row>
-    <row r="129" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B129" s="28"/>
       <c r="C129" s="28"/>
       <c r="D129" s="28"/>
@@ -7040,7 +7073,7 @@
       <c r="O129" s="28"/>
       <c r="P129" s="28"/>
     </row>
-    <row r="130" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="130" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B130" s="28"/>
       <c r="C130" s="28"/>
       <c r="D130" s="28"/>
@@ -7057,7 +7090,7 @@
       <c r="O130" s="28"/>
       <c r="P130" s="28"/>
     </row>
-    <row r="131" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="131" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B131" s="28"/>
       <c r="C131" s="28"/>
       <c r="D131" s="28"/>
@@ -7074,7 +7107,7 @@
       <c r="O131" s="28"/>
       <c r="P131" s="28"/>
     </row>
-    <row r="132" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B132" s="28"/>
       <c r="C132" s="28"/>
       <c r="D132" s="28"/>
@@ -7091,7 +7124,7 @@
       <c r="O132" s="28"/>
       <c r="P132" s="28"/>
     </row>
-    <row r="133" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="133" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B133" s="28"/>
       <c r="C133" s="28"/>
       <c r="D133" s="28"/>
@@ -7108,7 +7141,7 @@
       <c r="O133" s="28"/>
       <c r="P133" s="28"/>
     </row>
-    <row r="134" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B134" s="28"/>
       <c r="C134" s="28"/>
       <c r="D134" s="28"/>
@@ -7125,7 +7158,7 @@
       <c r="O134" s="28"/>
       <c r="P134" s="28"/>
     </row>
-    <row r="135" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="135" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B135" s="28"/>
       <c r="C135" s="28"/>
       <c r="D135" s="28"/>
@@ -7142,7 +7175,7 @@
       <c r="O135" s="28"/>
       <c r="P135" s="28"/>
     </row>
-    <row r="136" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="136" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B136" s="28"/>
       <c r="C136" s="28"/>
       <c r="D136" s="28"/>
@@ -7159,7 +7192,7 @@
       <c r="O136" s="28"/>
       <c r="P136" s="28"/>
     </row>
-    <row r="137" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="137" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B137" s="28"/>
       <c r="C137" s="28"/>
       <c r="D137" s="28"/>
@@ -7176,7 +7209,7 @@
       <c r="O137" s="28"/>
       <c r="P137" s="28"/>
     </row>
-    <row r="138" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="138" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B138" s="28"/>
       <c r="C138" s="28"/>
       <c r="D138" s="28"/>
@@ -7193,7 +7226,7 @@
       <c r="O138" s="28"/>
       <c r="P138" s="28"/>
     </row>
-    <row r="139" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="139" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B139" s="28"/>
       <c r="C139" s="28"/>
       <c r="D139" s="28"/>
@@ -7210,7 +7243,7 @@
       <c r="O139" s="28"/>
       <c r="P139" s="28"/>
     </row>
-    <row r="140" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="140" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B140" s="28"/>
       <c r="C140" s="28"/>
       <c r="D140" s="28"/>
@@ -7227,7 +7260,7 @@
       <c r="O140" s="28"/>
       <c r="P140" s="28"/>
     </row>
-    <row r="141" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="141" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B141" s="28"/>
       <c r="C141" s="28"/>
       <c r="D141" s="28"/>
@@ -7244,7 +7277,7 @@
       <c r="O141" s="28"/>
       <c r="P141" s="28"/>
     </row>
-    <row r="142" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="142" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B142" s="28"/>
       <c r="C142" s="28"/>
       <c r="D142" s="28"/>
@@ -7261,7 +7294,7 @@
       <c r="O142" s="28"/>
       <c r="P142" s="28"/>
     </row>
-    <row r="143" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="143" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B143" s="28"/>
       <c r="C143" s="28"/>
       <c r="D143" s="28"/>
@@ -7278,7 +7311,7 @@
       <c r="O143" s="28"/>
       <c r="P143" s="28"/>
     </row>
-    <row r="144" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="144" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B144" s="28"/>
       <c r="C144" s="28"/>
       <c r="D144" s="28"/>
@@ -7295,7 +7328,7 @@
       <c r="O144" s="28"/>
       <c r="P144" s="28"/>
     </row>
-    <row r="145" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="145" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B145" s="28"/>
       <c r="C145" s="28"/>
       <c r="D145" s="28"/>
@@ -7312,7 +7345,7 @@
       <c r="O145" s="28"/>
       <c r="P145" s="28"/>
     </row>
-    <row r="146" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="146" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B146" s="28"/>
       <c r="C146" s="28"/>
       <c r="D146" s="28"/>
@@ -7329,7 +7362,7 @@
       <c r="O146" s="28"/>
       <c r="P146" s="28"/>
     </row>
-    <row r="147" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="147" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B147" s="28"/>
       <c r="C147" s="28"/>
       <c r="D147" s="28"/>
@@ -7346,7 +7379,7 @@
       <c r="O147" s="28"/>
       <c r="P147" s="28"/>
     </row>
-    <row r="148" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="148" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B148" s="28"/>
       <c r="C148" s="28"/>
       <c r="D148" s="28"/>
@@ -7363,7 +7396,7 @@
       <c r="O148" s="28"/>
       <c r="P148" s="28"/>
     </row>
-    <row r="149" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="149" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B149" s="28"/>
       <c r="C149" s="28"/>
       <c r="D149" s="28"/>
@@ -7380,7 +7413,7 @@
       <c r="O149" s="28"/>
       <c r="P149" s="28"/>
     </row>
-    <row r="150" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="150" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B150" s="28"/>
       <c r="C150" s="28"/>
       <c r="D150" s="28"/>
@@ -7397,7 +7430,7 @@
       <c r="O150" s="28"/>
       <c r="P150" s="28"/>
     </row>
-    <row r="151" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="151" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B151" s="28"/>
       <c r="C151" s="28"/>
       <c r="D151" s="28"/>
@@ -7414,7 +7447,7 @@
       <c r="O151" s="28"/>
       <c r="P151" s="28"/>
     </row>
-    <row r="152" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="152" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B152" s="28"/>
       <c r="C152" s="28"/>
       <c r="D152" s="28"/>
@@ -7431,7 +7464,7 @@
       <c r="O152" s="28"/>
       <c r="P152" s="28"/>
     </row>
-    <row r="153" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="153" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B153" s="28"/>
       <c r="C153" s="28"/>
       <c r="D153" s="28"/>
@@ -7448,7 +7481,7 @@
       <c r="O153" s="28"/>
       <c r="P153" s="28"/>
     </row>
-    <row r="154" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="154" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B154" s="28"/>
       <c r="C154" s="28"/>
       <c r="D154" s="28"/>
@@ -7465,7 +7498,7 @@
       <c r="O154" s="28"/>
       <c r="P154" s="28"/>
     </row>
-    <row r="155" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="155" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B155" s="28"/>
       <c r="C155" s="28"/>
       <c r="D155" s="28"/>
@@ -7482,7 +7515,7 @@
       <c r="O155" s="28"/>
       <c r="P155" s="28"/>
     </row>
-    <row r="156" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="156" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B156" s="28"/>
       <c r="C156" s="28"/>
       <c r="D156" s="28"/>
@@ -7499,7 +7532,7 @@
       <c r="O156" s="28"/>
       <c r="P156" s="28"/>
     </row>
-    <row r="157" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="157" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B157" s="28"/>
       <c r="C157" s="28"/>
       <c r="D157" s="28"/>
@@ -7516,7 +7549,7 @@
       <c r="O157" s="28"/>
       <c r="P157" s="28"/>
     </row>
-    <row r="158" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="158" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B158" s="28"/>
       <c r="C158" s="28"/>
       <c r="D158" s="28"/>
@@ -7533,7 +7566,7 @@
       <c r="O158" s="28"/>
       <c r="P158" s="28"/>
     </row>
-    <row r="159" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="159" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B159" s="28"/>
       <c r="C159" s="28"/>
       <c r="D159" s="28"/>
@@ -7550,7 +7583,7 @@
       <c r="O159" s="28"/>
       <c r="P159" s="28"/>
     </row>
-    <row r="160" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="160" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B160" s="28"/>
       <c r="C160" s="28"/>
       <c r="D160" s="28"/>
@@ -7575,21 +7608,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q83"/>
+  <dimension ref="A1:Q84"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="Q85" sqref="Q85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.453125" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.54296875" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.54296875" style="2"/>
+    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -7610,7 +7643,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -7631,7 +7664,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -7684,7 +7717,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>43908</v>
       </c>
@@ -7737,7 +7770,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>43909</v>
       </c>
@@ -7790,7 +7823,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>43910</v>
       </c>
@@ -7843,7 +7876,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>43911</v>
       </c>
@@ -7896,7 +7929,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>43912</v>
       </c>
@@ -7949,7 +7982,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>43913</v>
       </c>
@@ -8002,7 +8035,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>43914</v>
       </c>
@@ -8055,7 +8088,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>43915</v>
       </c>
@@ -8108,7 +8141,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>43916</v>
       </c>
@@ -8161,7 +8194,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>43917</v>
       </c>
@@ -8214,7 +8247,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>43918</v>
       </c>
@@ -8267,7 +8300,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>43919</v>
       </c>
@@ -8320,7 +8353,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>43920</v>
       </c>
@@ -8373,7 +8406,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>43921</v>
       </c>
@@ -8426,7 +8459,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>43922</v>
       </c>
@@ -8479,7 +8512,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>43923</v>
       </c>
@@ -8532,7 +8565,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>43924</v>
       </c>
@@ -8585,7 +8618,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>43925</v>
       </c>
@@ -8638,7 +8671,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>43926</v>
       </c>
@@ -8691,7 +8724,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>43927</v>
       </c>
@@ -8744,7 +8777,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>43928</v>
       </c>
@@ -8797,7 +8830,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>43929</v>
       </c>
@@ -8850,7 +8883,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>43930</v>
       </c>
@@ -8903,7 +8936,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>43931</v>
       </c>
@@ -8956,7 +8989,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <v>43932</v>
       </c>
@@ -9009,7 +9042,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <v>43933</v>
       </c>
@@ -9062,7 +9095,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <v>43934</v>
       </c>
@@ -9115,7 +9148,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <v>43935</v>
       </c>
@@ -9168,7 +9201,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>43936</v>
       </c>
@@ -9221,7 +9254,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <v>43937</v>
       </c>
@@ -9274,7 +9307,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <v>43938</v>
       </c>
@@ -9327,7 +9360,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <v>43939</v>
       </c>
@@ -9380,7 +9413,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="30">
         <v>43940</v>
       </c>
@@ -9433,7 +9466,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="30">
         <v>43941</v>
       </c>
@@ -9486,7 +9519,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="30">
         <v>43942</v>
       </c>
@@ -9539,7 +9572,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="30">
         <v>43943</v>
       </c>
@@ -9592,7 +9625,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="30">
         <v>43944</v>
       </c>
@@ -9645,7 +9678,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="30">
         <v>43945</v>
       </c>
@@ -9698,7 +9731,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="30">
         <v>43946</v>
       </c>
@@ -9751,7 +9784,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="30">
         <v>43947</v>
       </c>
@@ -9804,7 +9837,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="30">
         <v>43948</v>
       </c>
@@ -9857,7 +9890,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="30">
         <v>43949</v>
       </c>
@@ -9910,7 +9943,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="30">
         <v>43950</v>
       </c>
@@ -9963,7 +9996,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="30">
         <v>43951</v>
       </c>
@@ -10016,7 +10049,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="30">
         <v>43952</v>
       </c>
@@ -10069,7 +10102,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="30">
         <v>43953</v>
       </c>
@@ -10122,7 +10155,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="30">
         <v>43954</v>
       </c>
@@ -10175,7 +10208,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="30">
         <v>43955</v>
       </c>
@@ -10228,7 +10261,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="30">
         <v>43956</v>
       </c>
@@ -10281,7 +10314,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="30">
         <v>43957</v>
       </c>
@@ -10334,7 +10367,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="30">
         <v>43958</v>
       </c>
@@ -10387,7 +10420,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="30">
         <v>43959</v>
       </c>
@@ -10440,7 +10473,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="30">
         <v>43960</v>
       </c>
@@ -10493,7 +10526,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="30">
         <v>43961</v>
       </c>
@@ -10546,7 +10579,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="30">
         <v>43962</v>
       </c>
@@ -10599,7 +10632,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="30">
         <v>43963</v>
       </c>
@@ -10652,7 +10685,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="30">
         <v>43964</v>
       </c>
@@ -10705,7 +10738,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" s="30">
         <v>43965</v>
       </c>
@@ -10758,7 +10791,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="30">
         <v>43966</v>
       </c>
@@ -10811,7 +10844,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" s="30">
         <v>43967</v>
       </c>
@@ -10864,7 +10897,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" s="30">
         <v>43968</v>
       </c>
@@ -10917,7 +10950,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" s="30">
         <v>43969</v>
       </c>
@@ -10970,7 +11003,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" s="30">
         <v>43970</v>
       </c>
@@ -11023,7 +11056,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" s="30">
         <v>43971</v>
       </c>
@@ -11076,7 +11109,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" s="30">
         <v>43972</v>
       </c>
@@ -11129,7 +11162,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" s="30">
         <v>43973</v>
       </c>
@@ -11182,7 +11215,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" s="30">
         <v>43974</v>
       </c>
@@ -11235,7 +11268,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" s="30">
         <v>43975</v>
       </c>
@@ -11288,7 +11321,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" s="30">
         <v>43976</v>
       </c>
@@ -11341,7 +11374,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" s="30">
         <v>43977</v>
       </c>
@@ -11394,7 +11427,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" s="30">
         <v>43978</v>
       </c>
@@ -11447,7 +11480,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" s="30">
         <v>43979</v>
       </c>
@@ -11500,7 +11533,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" s="30">
         <v>43980</v>
       </c>
@@ -11553,7 +11586,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" s="30">
         <v>43981</v>
       </c>
@@ -11606,7 +11639,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" s="30">
         <v>43982</v>
       </c>
@@ -11659,7 +11692,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" s="30">
         <v>43983</v>
       </c>
@@ -11712,7 +11745,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" s="30">
         <v>43984</v>
       </c>
@@ -11765,7 +11798,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" s="30">
         <v>43985</v>
       </c>
@@ -11818,7 +11851,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" s="30">
         <v>43986</v>
       </c>
@@ -11871,7 +11904,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" s="30">
         <v>43987</v>
       </c>
@@ -11922,6 +11955,59 @@
       </c>
       <c r="Q83" s="13">
         <v>23</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A84" s="30">
+        <v>43988</v>
+      </c>
+      <c r="B84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K84" s="14">
+        <v>5</v>
+      </c>
+      <c r="L84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q84" s="13">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -11932,23 +12018,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q75"/>
+  <dimension ref="A1:Q76"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="F64" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B64" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="O80" sqref="O80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.1796875" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.54296875" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.54296875" style="2"/>
+    <col min="1" max="1" width="15.28515625" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -11969,7 +12055,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -11990,7 +12076,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -12043,7 +12129,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>43916</v>
       </c>
@@ -12096,7 +12182,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>43917</v>
       </c>
@@ -12149,7 +12235,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>43918</v>
       </c>
@@ -12202,7 +12288,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>43919</v>
       </c>
@@ -12255,7 +12341,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>43920</v>
       </c>
@@ -12308,7 +12394,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>43921</v>
       </c>
@@ -12361,7 +12447,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>43922</v>
       </c>
@@ -12414,7 +12500,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>43923</v>
       </c>
@@ -12467,7 +12553,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>43924</v>
       </c>
@@ -12520,7 +12606,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>43925</v>
       </c>
@@ -12573,7 +12659,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>43926</v>
       </c>
@@ -12626,7 +12712,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>43927</v>
       </c>
@@ -12679,7 +12765,7 @@
         <v>1262</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>43928</v>
       </c>
@@ -12732,7 +12818,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>43929</v>
       </c>
@@ -12785,7 +12871,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>43930</v>
       </c>
@@ -12838,7 +12924,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>43931</v>
       </c>
@@ -12891,7 +12977,7 @@
         <v>1461</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>43932</v>
       </c>
@@ -12944,7 +13030,7 @@
         <v>1467</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>43933</v>
       </c>
@@ -12997,7 +13083,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>43934</v>
       </c>
@@ -13050,7 +13136,7 @@
         <v>1482</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>43935</v>
       </c>
@@ -13103,7 +13189,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>43936</v>
       </c>
@@ -13156,7 +13242,7 @@
         <v>1486</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>43937</v>
       </c>
@@ -13209,7 +13295,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>43938</v>
       </c>
@@ -13262,7 +13348,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>43939</v>
       </c>
@@ -13315,7 +13401,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <v>43940</v>
       </c>
@@ -13368,7 +13454,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <v>43941</v>
       </c>
@@ -13421,7 +13507,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <v>43942</v>
       </c>
@@ -13474,7 +13560,7 @@
         <v>1472</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <v>43943</v>
       </c>
@@ -13527,7 +13613,7 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>43944</v>
       </c>
@@ -13580,7 +13666,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <v>43945</v>
       </c>
@@ -13633,7 +13719,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <v>43946</v>
       </c>
@@ -13686,7 +13772,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <v>43947</v>
       </c>
@@ -13739,7 +13825,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="30">
         <v>43948</v>
       </c>
@@ -13792,7 +13878,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="30">
         <v>43949</v>
       </c>
@@ -13845,7 +13931,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="30">
         <v>43950</v>
       </c>
@@ -13898,7 +13984,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="30">
         <v>43951</v>
       </c>
@@ -13951,7 +14037,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="30">
         <v>43952</v>
       </c>
@@ -14004,7 +14090,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="30">
         <v>43953</v>
       </c>
@@ -14057,7 +14143,7 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="30">
         <v>43954</v>
       </c>
@@ -14110,7 +14196,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="30">
         <v>43955</v>
       </c>
@@ -14163,7 +14249,7 @@
         <v>1279</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="30">
         <v>43956</v>
       </c>
@@ -14216,7 +14302,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="30">
         <v>43957</v>
       </c>
@@ -14269,7 +14355,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="30">
         <v>43958</v>
       </c>
@@ -14322,7 +14408,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="30">
         <v>43959</v>
       </c>
@@ -14375,7 +14461,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="30">
         <v>43960</v>
       </c>
@@ -14428,7 +14514,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="30">
         <v>43961</v>
       </c>
@@ -14481,7 +14567,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="30">
         <v>43962</v>
       </c>
@@ -14534,7 +14620,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="30">
         <v>43963</v>
       </c>
@@ -14587,7 +14673,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="30">
         <v>43964</v>
       </c>
@@ -14640,7 +14726,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="30">
         <v>43965</v>
       </c>
@@ -14693,7 +14779,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="30">
         <v>43966</v>
       </c>
@@ -14746,7 +14832,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="30">
         <v>43967</v>
       </c>
@@ -14799,7 +14885,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="30">
         <v>43968</v>
       </c>
@@ -14852,7 +14938,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="30">
         <v>43969</v>
       </c>
@@ -14905,7 +14991,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="30">
         <v>43970</v>
       </c>
@@ -14958,7 +15044,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="30">
         <v>43971</v>
       </c>
@@ -15011,7 +15097,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="30">
         <v>43972</v>
       </c>
@@ -15064,7 +15150,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" s="30">
         <v>43973</v>
       </c>
@@ -15117,7 +15203,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="30">
         <v>43974</v>
       </c>
@@ -15170,7 +15256,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" s="30">
         <v>43975</v>
       </c>
@@ -15223,7 +15309,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" s="30">
         <v>43976</v>
       </c>
@@ -15276,7 +15362,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" s="51">
         <v>43977</v>
       </c>
@@ -15329,7 +15415,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" s="51">
         <v>43978</v>
       </c>
@@ -15382,7 +15468,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" s="51">
         <v>43979</v>
       </c>
@@ -15435,7 +15521,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" s="51">
         <v>43980</v>
       </c>
@@ -15488,7 +15574,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" s="51">
         <v>43981</v>
       </c>
@@ -15541,7 +15627,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" s="51">
         <v>43982</v>
       </c>
@@ -15594,7 +15680,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" s="51">
         <v>43983</v>
       </c>
@@ -15647,7 +15733,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" s="51">
         <v>43984</v>
       </c>
@@ -15700,7 +15786,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" s="51">
         <v>43985</v>
       </c>
@@ -15753,7 +15839,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" s="51">
         <v>43986</v>
       </c>
@@ -15806,7 +15892,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" s="51">
         <v>43987</v>
       </c>
@@ -15857,6 +15943,59 @@
       </c>
       <c r="Q75" s="13">
         <v>676</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A76" s="51">
+        <v>43988</v>
+      </c>
+      <c r="B76" s="11">
+        <v>8</v>
+      </c>
+      <c r="C76" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D76" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E76" s="11">
+        <v>54</v>
+      </c>
+      <c r="F76" s="11">
+        <v>12</v>
+      </c>
+      <c r="G76" s="11">
+        <v>62</v>
+      </c>
+      <c r="H76" s="11">
+        <v>294</v>
+      </c>
+      <c r="I76" s="11">
+        <v>6</v>
+      </c>
+      <c r="J76" s="11">
+        <v>59</v>
+      </c>
+      <c r="K76" s="11">
+        <v>143</v>
+      </c>
+      <c r="L76" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M76" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N76" s="11">
+        <v>8</v>
+      </c>
+      <c r="O76" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P76" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q76" s="13">
+        <v>646</v>
       </c>
     </row>
   </sheetData>
@@ -15867,23 +16006,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q75"/>
+  <dimension ref="A1:Q76"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B61" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="M77" sqref="M77:M78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.453125" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.54296875" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.54296875" style="2"/>
+    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -15904,7 +16043,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -15925,7 +16064,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -15978,7 +16117,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>43916</v>
       </c>
@@ -16031,7 +16170,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>43917</v>
       </c>
@@ -16084,7 +16223,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>43918</v>
       </c>
@@ -16137,7 +16276,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>43919</v>
       </c>
@@ -16190,7 +16329,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>43920</v>
       </c>
@@ -16243,7 +16382,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>43921</v>
       </c>
@@ -16296,7 +16435,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>43922</v>
       </c>
@@ -16349,7 +16488,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>43923</v>
       </c>
@@ -16402,7 +16541,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>43924</v>
       </c>
@@ -16455,7 +16594,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>43925</v>
       </c>
@@ -16508,7 +16647,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>43926</v>
       </c>
@@ -16561,7 +16700,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>43927</v>
       </c>
@@ -16614,7 +16753,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>43928</v>
       </c>
@@ -16667,7 +16806,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>43929</v>
       </c>
@@ -16720,7 +16859,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>43930</v>
       </c>
@@ -16773,7 +16912,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>43931</v>
       </c>
@@ -16826,7 +16965,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>43932</v>
       </c>
@@ -16879,7 +17018,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>43933</v>
       </c>
@@ -16932,7 +17071,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>43934</v>
       </c>
@@ -16985,7 +17124,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>43935</v>
       </c>
@@ -17038,7 +17177,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>43936</v>
       </c>
@@ -17091,7 +17230,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>43937</v>
       </c>
@@ -17144,7 +17283,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>43938</v>
       </c>
@@ -17197,7 +17336,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>43939</v>
       </c>
@@ -17250,7 +17389,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <v>43940</v>
       </c>
@@ -17303,7 +17442,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <v>43941</v>
       </c>
@@ -17356,7 +17495,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <v>43942</v>
       </c>
@@ -17409,7 +17548,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <v>43943</v>
       </c>
@@ -17462,7 +17601,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>43944</v>
       </c>
@@ -17515,7 +17654,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <v>43945</v>
       </c>
@@ -17568,7 +17707,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <v>43946</v>
       </c>
@@ -17621,7 +17760,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <v>43947</v>
       </c>
@@ -17674,7 +17813,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="30">
         <v>43948</v>
       </c>
@@ -17727,7 +17866,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="30">
         <v>43949</v>
       </c>
@@ -17780,7 +17919,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="30">
         <v>43950</v>
       </c>
@@ -17833,7 +17972,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="30">
         <v>43951</v>
       </c>
@@ -17886,7 +18025,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="30">
         <v>43952</v>
       </c>
@@ -17939,7 +18078,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="30">
         <v>43953</v>
       </c>
@@ -17992,7 +18131,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="30">
         <v>43954</v>
       </c>
@@ -18045,7 +18184,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="30">
         <v>43955</v>
       </c>
@@ -18098,7 +18237,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="30">
         <v>43956</v>
       </c>
@@ -18151,7 +18290,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="30">
         <v>43957</v>
       </c>
@@ -18204,7 +18343,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="30">
         <v>43958</v>
       </c>
@@ -18257,7 +18396,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="30">
         <v>43959</v>
       </c>
@@ -18310,7 +18449,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="30">
         <v>43960</v>
       </c>
@@ -18363,7 +18502,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="30">
         <v>43961</v>
       </c>
@@ -18416,7 +18555,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="30">
         <v>43962</v>
       </c>
@@ -18469,7 +18608,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="30">
         <v>43963</v>
       </c>
@@ -18522,7 +18661,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="30">
         <v>43964</v>
       </c>
@@ -18575,7 +18714,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="30">
         <v>43965</v>
       </c>
@@ -18628,7 +18767,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="30">
         <v>43966</v>
       </c>
@@ -18681,7 +18820,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="30">
         <v>43967</v>
       </c>
@@ -18734,7 +18873,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="30">
         <v>43968</v>
       </c>
@@ -18787,7 +18926,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="30">
         <v>43969</v>
       </c>
@@ -18840,7 +18979,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="30">
         <v>43970</v>
       </c>
@@ -18893,7 +19032,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="30">
         <v>43971</v>
       </c>
@@ -18946,7 +19085,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="30">
         <v>43972</v>
       </c>
@@ -18999,7 +19138,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" s="30">
         <v>43973</v>
       </c>
@@ -19052,7 +19191,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="30">
         <v>43974</v>
       </c>
@@ -19105,7 +19244,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" s="30">
         <v>43975</v>
       </c>
@@ -19158,7 +19297,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" s="30">
         <v>43976</v>
       </c>
@@ -19211,7 +19350,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" s="30">
         <v>43977</v>
       </c>
@@ -19264,7 +19403,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" s="30">
         <v>43978</v>
       </c>
@@ -19317,7 +19456,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" s="30">
         <v>43979</v>
       </c>
@@ -19370,7 +19509,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" s="30">
         <v>43980</v>
       </c>
@@ -19423,7 +19562,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" s="30">
         <v>43981</v>
       </c>
@@ -19476,7 +19615,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" s="30">
         <v>43982</v>
       </c>
@@ -19529,7 +19668,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" s="30">
         <v>43983</v>
       </c>
@@ -19582,7 +19721,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" s="30">
         <v>43984</v>
       </c>
@@ -19635,7 +19774,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" s="30">
         <v>43985</v>
       </c>
@@ -19688,7 +19827,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" s="30">
         <v>43986</v>
       </c>
@@ -19741,7 +19880,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" s="30">
         <v>43987</v>
       </c>
@@ -19792,6 +19931,59 @@
       </c>
       <c r="Q75" s="13">
         <v>319</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A76" s="30">
+        <v>43988</v>
+      </c>
+      <c r="B76" s="11">
+        <v>35</v>
+      </c>
+      <c r="C76" s="11">
+        <v>20</v>
+      </c>
+      <c r="D76" s="11">
+        <v>14</v>
+      </c>
+      <c r="E76" s="11">
+        <v>27</v>
+      </c>
+      <c r="F76" s="11">
+        <v>39</v>
+      </c>
+      <c r="G76" s="11">
+        <v>15</v>
+      </c>
+      <c r="H76" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I76" s="11">
+        <v>9</v>
+      </c>
+      <c r="J76" s="11">
+        <v>60</v>
+      </c>
+      <c r="K76" s="11">
+        <v>142</v>
+      </c>
+      <c r="L76" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M76" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N76" s="11">
+        <v>11</v>
+      </c>
+      <c r="O76" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P76" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q76" s="13">
+        <v>373</v>
       </c>
     </row>
   </sheetData>
@@ -19799,7 +19991,7 @@
 </worksheet>
 </file>
 
-<file path=customXML/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA" version="1.0.0">
   <systemFields>
     <field name="Objective-Id">
@@ -19821,10 +20013,10 @@
       <value order="0">true</value>
     </field>
     <field name="Objective-DatePublished">
-      <value order="0">2020-06-05T12:12:14Z</value>
+      <value order="0">2020-06-06T11:52:20Z</value>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-05T12:12:14Z</value>
+      <value order="0">2020-06-06T11:52:20Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -19839,13 +20031,13 @@
       <value order="0">Published</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41574143</value>
+      <value order="0">vA41586174</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">20.0</value>
+      <value order="0">21.0</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">151</value>
+      <value order="0">154</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>
@@ -19882,7 +20074,7 @@
 </metadata>
 </file>
 
-<file path=customXML/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5745109E-2DDF-40CB-AC2B-FF9B10C90820}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-06 20:08) (#92)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u207826\Objective\Objects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\scotland.gov.uk\dc2\FS5_Home\u204186\Gov.scot content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5990" windowHeight="6020" tabRatio="803"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5985" windowHeight="6030" tabRatio="803"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1632" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1657" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -1676,24 +1676,24 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.453125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="90.453125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.453125" style="2"/>
+    <col min="2" max="2" width="29.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="90.42578125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>20</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
         <v>22</v>
       </c>
@@ -1709,13 +1709,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="22" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="23"/>
     </row>
-    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="24" t="s">
         <v>26</v>
       </c>
@@ -1723,7 +1723,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="24" t="s">
         <v>27</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="24" t="s">
         <v>36</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
         <v>37</v>
       </c>
@@ -1767,12 +1767,12 @@
       <selection activeCell="K66" sqref="K66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.453125" style="2"/>
+    <col min="1" max="16384" width="9.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="44" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="43"/>
     </row>
   </sheetData>
@@ -1790,17 +1790,17 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B81" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F96" sqref="F96"/>
+      <selection pane="bottomRight" activeCell="H98" sqref="H98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" style="2" customWidth="1"/>
-    <col min="2" max="16" width="11.453125" style="11" customWidth="1"/>
-    <col min="17" max="16384" width="8.54296875" style="2"/>
+    <col min="2" max="16" width="11.42578125" style="11" customWidth="1"/>
+    <col min="17" max="16384" width="8.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -1820,7 +1820,7 @@
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -1839,7 +1839,7 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>43897</v>
       </c>
@@ -1939,7 +1939,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>43898</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>43899</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>43900</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>43901</v>
       </c>
@@ -2139,7 +2139,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>43902</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>43903</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>43904</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>43905</v>
       </c>
@@ -2339,7 +2339,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>43906</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>43907</v>
       </c>
@@ -2439,7 +2439,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>43908</v>
       </c>
@@ -2489,7 +2489,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>43909</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>43910</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>43911</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>43912</v>
       </c>
@@ -2689,7 +2689,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>43913</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>43914</v>
       </c>
@@ -2789,7 +2789,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>43915</v>
       </c>
@@ -2839,7 +2839,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>43916</v>
       </c>
@@ -2889,7 +2889,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>43917</v>
       </c>
@@ -2939,7 +2939,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>43918</v>
       </c>
@@ -2989,7 +2989,7 @@
         <v>1264</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>43919</v>
       </c>
@@ -3039,7 +3039,7 @@
         <v>1417</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>43920</v>
       </c>
@@ -3089,7 +3089,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>43921</v>
       </c>
@@ -3139,7 +3139,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>43922</v>
       </c>
@@ -3189,7 +3189,7 @@
         <v>2310</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>43923</v>
       </c>
@@ -3239,7 +3239,7 @@
         <v>2602</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>43924</v>
       </c>
@@ -3289,7 +3289,7 @@
         <v>3001</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>43925</v>
       </c>
@@ -3339,7 +3339,7 @@
         <v>3345</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>43926</v>
       </c>
@@ -3389,7 +3389,7 @@
         <v>3706</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>43927</v>
       </c>
@@ -3439,7 +3439,7 @@
         <v>3961</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>43928</v>
       </c>
@@ -3489,7 +3489,7 @@
         <v>4229</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>43929</v>
       </c>
@@ -3539,7 +3539,7 @@
         <v>4565</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>43930</v>
       </c>
@@ -3589,7 +3589,7 @@
         <v>4957</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>43931</v>
       </c>
@@ -3639,7 +3639,7 @@
         <v>5275</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>43932</v>
       </c>
@@ -3689,7 +3689,7 @@
         <v>5590</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>43933</v>
       </c>
@@ -3739,7 +3739,7 @@
         <v>5912</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>43934</v>
       </c>
@@ -3789,7 +3789,7 @@
         <v>6067</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>43935</v>
       </c>
@@ -3839,7 +3839,7 @@
         <v>6358</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>43936</v>
       </c>
@@ -3889,7 +3889,7 @@
         <v>6748</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>43937</v>
       </c>
@@ -3939,7 +3939,7 @@
         <v>7102</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>43938</v>
       </c>
@@ -3989,7 +3989,7 @@
         <v>7409</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>43939</v>
       </c>
@@ -4039,7 +4039,7 @@
         <v>7820</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>43940</v>
       </c>
@@ -4089,7 +4089,7 @@
         <v>8187</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>43941</v>
       </c>
@@ -4139,7 +4139,7 @@
         <v>8450</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>43942</v>
       </c>
@@ -4189,7 +4189,7 @@
         <v>8672</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>43943</v>
       </c>
@@ -4239,7 +4239,7 @@
         <v>9038</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>43944</v>
       </c>
@@ -4289,7 +4289,7 @@
         <v>9409</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>43945</v>
       </c>
@@ -4339,7 +4339,7 @@
         <v>9697</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>43946</v>
       </c>
@@ -4389,7 +4389,7 @@
         <v>10051</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>43947</v>
       </c>
@@ -4440,7 +4440,7 @@
       </c>
       <c r="R54" s="38"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>43948</v>
       </c>
@@ -4491,7 +4491,7 @@
       </c>
       <c r="R55" s="38"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>43949</v>
       </c>
@@ -4542,7 +4542,7 @@
       </c>
       <c r="R56" s="39"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>43950</v>
       </c>
@@ -4592,7 +4592,7 @@
         <v>11034</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>43951</v>
       </c>
@@ -4643,7 +4643,7 @@
       </c>
       <c r="R58" s="38"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>43952</v>
       </c>
@@ -4695,7 +4695,7 @@
       <c r="R59" s="38"/>
       <c r="S59" s="38"/>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>43953</v>
       </c>
@@ -4745,7 +4745,7 @@
         <v>11927</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>43954</v>
       </c>
@@ -4795,7 +4795,7 @@
         <v>12097</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>43955</v>
       </c>
@@ -4845,7 +4845,7 @@
         <v>12266</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
         <v>43956</v>
       </c>
@@ -4895,7 +4895,7 @@
         <v>12437</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
         <v>43957</v>
       </c>
@@ -4945,7 +4945,7 @@
         <v>12709</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
         <v>43958</v>
       </c>
@@ -4995,7 +4995,7 @@
         <v>12924</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
         <v>43959</v>
       </c>
@@ -5045,7 +5045,7 @@
         <v>13149</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
         <v>43960</v>
       </c>
@@ -5095,7 +5095,7 @@
         <v>13305</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
         <v>43961</v>
       </c>
@@ -5145,7 +5145,7 @@
         <v>13486</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
         <v>43962</v>
       </c>
@@ -5195,7 +5195,7 @@
         <v>13627</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>43963</v>
       </c>
@@ -5245,7 +5245,7 @@
         <v>13763</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
         <v>43964</v>
       </c>
@@ -5295,7 +5295,7 @@
         <v>13929</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <v>43965</v>
       </c>
@@ -5345,7 +5345,7 @@
         <v>14117</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
         <v>43966</v>
       </c>
@@ -5395,7 +5395,7 @@
         <v>14260</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <v>43967</v>
       </c>
@@ -5445,7 +5445,7 @@
         <v>14447</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
         <v>43968</v>
       </c>
@@ -5495,7 +5495,7 @@
         <v>14537</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
         <v>43969</v>
       </c>
@@ -5545,7 +5545,7 @@
         <v>14594</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" s="5">
         <v>43970</v>
       </c>
@@ -5595,7 +5595,7 @@
         <v>14655</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
         <v>43971</v>
       </c>
@@ -5645,7 +5645,7 @@
         <v>14751</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" s="5">
         <v>43972</v>
       </c>
@@ -5695,7 +5695,7 @@
         <v>14856</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
         <v>43973</v>
       </c>
@@ -5745,7 +5745,7 @@
         <v>14969</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
         <v>43974</v>
       </c>
@@ -5795,7 +5795,7 @@
         <v>15041</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
         <v>43975</v>
       </c>
@@ -5845,7 +5845,7 @@
         <v>15101</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" s="5">
         <v>43976</v>
       </c>
@@ -5895,7 +5895,7 @@
         <v>15156</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" s="5">
         <v>43977</v>
       </c>
@@ -5945,7 +5945,7 @@
         <v>15185</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" s="5">
         <v>43978</v>
       </c>
@@ -5995,7 +5995,7 @@
         <v>15240</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" s="5">
         <v>43979</v>
       </c>
@@ -6045,7 +6045,7 @@
         <v>15288</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" s="5">
         <v>43980</v>
       </c>
@@ -6095,7 +6095,7 @@
         <v>15327</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" s="5">
         <v>43981</v>
       </c>
@@ -6145,7 +6145,7 @@
         <v>15382</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" s="5">
         <v>43982</v>
       </c>
@@ -6195,7 +6195,7 @@
         <v>15400</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" s="5">
         <v>43983</v>
       </c>
@@ -6245,7 +6245,7 @@
         <v>15418</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" s="5">
         <v>43984</v>
       </c>
@@ -6295,7 +6295,7 @@
         <v>15471</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
         <v>43985</v>
       </c>
@@ -6345,7 +6345,7 @@
         <v>15504</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" s="5">
         <v>43986</v>
       </c>
@@ -6395,7 +6395,7 @@
         <v>15553</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
         <v>43987</v>
       </c>
@@ -6445,24 +6445,57 @@
         <v>15582</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B95" s="28"/>
-      <c r="C95" s="28"/>
-      <c r="D95" s="28"/>
-      <c r="E95" s="28"/>
-      <c r="F95" s="28"/>
-      <c r="G95" s="28"/>
-      <c r="H95" s="28"/>
-      <c r="I95" s="28"/>
-      <c r="J95" s="28"/>
-      <c r="K95" s="28"/>
-      <c r="L95" s="28"/>
-      <c r="M95" s="28"/>
-      <c r="N95" s="28"/>
-      <c r="O95" s="28"/>
-      <c r="P95" s="28"/>
-    </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A95" s="5">
+        <v>43988</v>
+      </c>
+      <c r="B95" s="28">
+        <v>1077</v>
+      </c>
+      <c r="C95" s="28">
+        <v>326</v>
+      </c>
+      <c r="D95" s="28">
+        <v>261</v>
+      </c>
+      <c r="E95" s="28">
+        <v>879</v>
+      </c>
+      <c r="F95" s="28">
+        <v>946</v>
+      </c>
+      <c r="G95" s="28">
+        <v>1284</v>
+      </c>
+      <c r="H95" s="28">
+        <v>3971</v>
+      </c>
+      <c r="I95" s="28">
+        <v>339</v>
+      </c>
+      <c r="J95" s="28">
+        <v>2007</v>
+      </c>
+      <c r="K95" s="28">
+        <v>2769</v>
+      </c>
+      <c r="L95" s="28">
+        <v>8</v>
+      </c>
+      <c r="M95" s="28">
+        <v>54</v>
+      </c>
+      <c r="N95" s="28">
+        <v>1676</v>
+      </c>
+      <c r="O95" s="28">
+        <v>6</v>
+      </c>
+      <c r="P95" s="32">
+        <v>15603</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B96" s="28"/>
       <c r="C96" s="28"/>
       <c r="D96" s="28"/>
@@ -6479,7 +6512,7 @@
       <c r="O96" s="28"/>
       <c r="P96" s="28"/>
     </row>
-    <row r="97" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B97" s="28"/>
       <c r="C97" s="28"/>
       <c r="D97" s="28"/>
@@ -6496,7 +6529,7 @@
       <c r="O97" s="28"/>
       <c r="P97" s="28"/>
     </row>
-    <row r="98" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B98" s="28"/>
       <c r="C98" s="28"/>
       <c r="D98" s="28"/>
@@ -6513,7 +6546,7 @@
       <c r="O98" s="28"/>
       <c r="P98" s="28"/>
     </row>
-    <row r="99" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B99" s="28"/>
       <c r="C99" s="28"/>
       <c r="D99" s="28"/>
@@ -6530,7 +6563,7 @@
       <c r="O99" s="28"/>
       <c r="P99" s="28"/>
     </row>
-    <row r="100" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B100" s="28"/>
       <c r="C100" s="28"/>
       <c r="D100" s="28"/>
@@ -6547,7 +6580,7 @@
       <c r="O100" s="28"/>
       <c r="P100" s="28"/>
     </row>
-    <row r="101" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B101" s="28"/>
       <c r="C101" s="28"/>
       <c r="D101" s="28"/>
@@ -6564,7 +6597,7 @@
       <c r="O101" s="28"/>
       <c r="P101" s="28"/>
     </row>
-    <row r="102" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B102" s="28"/>
       <c r="C102" s="28"/>
       <c r="D102" s="28"/>
@@ -6581,7 +6614,7 @@
       <c r="O102" s="28"/>
       <c r="P102" s="28"/>
     </row>
-    <row r="103" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B103" s="28"/>
       <c r="C103" s="28"/>
       <c r="D103" s="28"/>
@@ -6598,7 +6631,7 @@
       <c r="O103" s="28"/>
       <c r="P103" s="28"/>
     </row>
-    <row r="104" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B104" s="28"/>
       <c r="C104" s="28"/>
       <c r="D104" s="28"/>
@@ -6615,7 +6648,7 @@
       <c r="O104" s="28"/>
       <c r="P104" s="28"/>
     </row>
-    <row r="105" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B105" s="28"/>
       <c r="C105" s="28"/>
       <c r="D105" s="28"/>
@@ -6632,7 +6665,7 @@
       <c r="O105" s="28"/>
       <c r="P105" s="28"/>
     </row>
-    <row r="106" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B106" s="28"/>
       <c r="C106" s="28"/>
       <c r="D106" s="28"/>
@@ -6649,7 +6682,7 @@
       <c r="O106" s="28"/>
       <c r="P106" s="28"/>
     </row>
-    <row r="107" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B107" s="28"/>
       <c r="C107" s="28"/>
       <c r="D107" s="28"/>
@@ -6666,7 +6699,7 @@
       <c r="O107" s="28"/>
       <c r="P107" s="28"/>
     </row>
-    <row r="108" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B108" s="28"/>
       <c r="C108" s="28"/>
       <c r="D108" s="28"/>
@@ -6683,7 +6716,7 @@
       <c r="O108" s="28"/>
       <c r="P108" s="28"/>
     </row>
-    <row r="109" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B109" s="28"/>
       <c r="C109" s="28"/>
       <c r="D109" s="28"/>
@@ -6700,7 +6733,7 @@
       <c r="O109" s="28"/>
       <c r="P109" s="28"/>
     </row>
-    <row r="110" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B110" s="28"/>
       <c r="C110" s="28"/>
       <c r="D110" s="28"/>
@@ -6717,7 +6750,7 @@
       <c r="O110" s="28"/>
       <c r="P110" s="28"/>
     </row>
-    <row r="111" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B111" s="28"/>
       <c r="C111" s="28"/>
       <c r="D111" s="28"/>
@@ -6734,7 +6767,7 @@
       <c r="O111" s="28"/>
       <c r="P111" s="28"/>
     </row>
-    <row r="112" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B112" s="28"/>
       <c r="C112" s="28"/>
       <c r="D112" s="28"/>
@@ -6751,7 +6784,7 @@
       <c r="O112" s="28"/>
       <c r="P112" s="28"/>
     </row>
-    <row r="113" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B113" s="28"/>
       <c r="C113" s="28"/>
       <c r="D113" s="28"/>
@@ -6768,7 +6801,7 @@
       <c r="O113" s="28"/>
       <c r="P113" s="28"/>
     </row>
-    <row r="114" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B114" s="28"/>
       <c r="C114" s="28"/>
       <c r="D114" s="28"/>
@@ -6785,7 +6818,7 @@
       <c r="O114" s="28"/>
       <c r="P114" s="28"/>
     </row>
-    <row r="115" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B115" s="28"/>
       <c r="C115" s="28"/>
       <c r="D115" s="28"/>
@@ -6802,7 +6835,7 @@
       <c r="O115" s="28"/>
       <c r="P115" s="28"/>
     </row>
-    <row r="116" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B116" s="28"/>
       <c r="C116" s="28"/>
       <c r="D116" s="28"/>
@@ -6819,7 +6852,7 @@
       <c r="O116" s="28"/>
       <c r="P116" s="28"/>
     </row>
-    <row r="117" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B117" s="28"/>
       <c r="C117" s="28"/>
       <c r="D117" s="28"/>
@@ -6836,7 +6869,7 @@
       <c r="O117" s="28"/>
       <c r="P117" s="28"/>
     </row>
-    <row r="118" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B118" s="28"/>
       <c r="C118" s="28"/>
       <c r="D118" s="28"/>
@@ -6853,7 +6886,7 @@
       <c r="O118" s="28"/>
       <c r="P118" s="28"/>
     </row>
-    <row r="119" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B119" s="28"/>
       <c r="C119" s="28"/>
       <c r="D119" s="28"/>
@@ -6870,7 +6903,7 @@
       <c r="O119" s="28"/>
       <c r="P119" s="28"/>
     </row>
-    <row r="120" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="120" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B120" s="28"/>
       <c r="C120" s="28"/>
       <c r="D120" s="28"/>
@@ -6887,7 +6920,7 @@
       <c r="O120" s="28"/>
       <c r="P120" s="28"/>
     </row>
-    <row r="121" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="121" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B121" s="28"/>
       <c r="C121" s="28"/>
       <c r="D121" s="28"/>
@@ -6904,7 +6937,7 @@
       <c r="O121" s="28"/>
       <c r="P121" s="28"/>
     </row>
-    <row r="122" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="122" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B122" s="28"/>
       <c r="C122" s="28"/>
       <c r="D122" s="28"/>
@@ -6921,7 +6954,7 @@
       <c r="O122" s="28"/>
       <c r="P122" s="28"/>
     </row>
-    <row r="123" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="123" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B123" s="28"/>
       <c r="C123" s="28"/>
       <c r="D123" s="28"/>
@@ -6938,7 +6971,7 @@
       <c r="O123" s="28"/>
       <c r="P123" s="28"/>
     </row>
-    <row r="124" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B124" s="28"/>
       <c r="C124" s="28"/>
       <c r="D124" s="28"/>
@@ -6955,7 +6988,7 @@
       <c r="O124" s="28"/>
       <c r="P124" s="28"/>
     </row>
-    <row r="125" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="125" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B125" s="28"/>
       <c r="C125" s="28"/>
       <c r="D125" s="28"/>
@@ -6972,7 +7005,7 @@
       <c r="O125" s="28"/>
       <c r="P125" s="28"/>
     </row>
-    <row r="126" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="126" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B126" s="28"/>
       <c r="C126" s="28"/>
       <c r="D126" s="28"/>
@@ -6989,7 +7022,7 @@
       <c r="O126" s="28"/>
       <c r="P126" s="28"/>
     </row>
-    <row r="127" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="127" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B127" s="28"/>
       <c r="C127" s="28"/>
       <c r="D127" s="28"/>
@@ -7006,7 +7039,7 @@
       <c r="O127" s="28"/>
       <c r="P127" s="28"/>
     </row>
-    <row r="128" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="128" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B128" s="28"/>
       <c r="C128" s="28"/>
       <c r="D128" s="28"/>
@@ -7023,7 +7056,7 @@
       <c r="O128" s="28"/>
       <c r="P128" s="28"/>
     </row>
-    <row r="129" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B129" s="28"/>
       <c r="C129" s="28"/>
       <c r="D129" s="28"/>
@@ -7040,7 +7073,7 @@
       <c r="O129" s="28"/>
       <c r="P129" s="28"/>
     </row>
-    <row r="130" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="130" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B130" s="28"/>
       <c r="C130" s="28"/>
       <c r="D130" s="28"/>
@@ -7057,7 +7090,7 @@
       <c r="O130" s="28"/>
       <c r="P130" s="28"/>
     </row>
-    <row r="131" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="131" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B131" s="28"/>
       <c r="C131" s="28"/>
       <c r="D131" s="28"/>
@@ -7074,7 +7107,7 @@
       <c r="O131" s="28"/>
       <c r="P131" s="28"/>
     </row>
-    <row r="132" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B132" s="28"/>
       <c r="C132" s="28"/>
       <c r="D132" s="28"/>
@@ -7091,7 +7124,7 @@
       <c r="O132" s="28"/>
       <c r="P132" s="28"/>
     </row>
-    <row r="133" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="133" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B133" s="28"/>
       <c r="C133" s="28"/>
       <c r="D133" s="28"/>
@@ -7108,7 +7141,7 @@
       <c r="O133" s="28"/>
       <c r="P133" s="28"/>
     </row>
-    <row r="134" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B134" s="28"/>
       <c r="C134" s="28"/>
       <c r="D134" s="28"/>
@@ -7125,7 +7158,7 @@
       <c r="O134" s="28"/>
       <c r="P134" s="28"/>
     </row>
-    <row r="135" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="135" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B135" s="28"/>
       <c r="C135" s="28"/>
       <c r="D135" s="28"/>
@@ -7142,7 +7175,7 @@
       <c r="O135" s="28"/>
       <c r="P135" s="28"/>
     </row>
-    <row r="136" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="136" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B136" s="28"/>
       <c r="C136" s="28"/>
       <c r="D136" s="28"/>
@@ -7159,7 +7192,7 @@
       <c r="O136" s="28"/>
       <c r="P136" s="28"/>
     </row>
-    <row r="137" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="137" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B137" s="28"/>
       <c r="C137" s="28"/>
       <c r="D137" s="28"/>
@@ -7176,7 +7209,7 @@
       <c r="O137" s="28"/>
       <c r="P137" s="28"/>
     </row>
-    <row r="138" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="138" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B138" s="28"/>
       <c r="C138" s="28"/>
       <c r="D138" s="28"/>
@@ -7193,7 +7226,7 @@
       <c r="O138" s="28"/>
       <c r="P138" s="28"/>
     </row>
-    <row r="139" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="139" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B139" s="28"/>
       <c r="C139" s="28"/>
       <c r="D139" s="28"/>
@@ -7210,7 +7243,7 @@
       <c r="O139" s="28"/>
       <c r="P139" s="28"/>
     </row>
-    <row r="140" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="140" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B140" s="28"/>
       <c r="C140" s="28"/>
       <c r="D140" s="28"/>
@@ -7227,7 +7260,7 @@
       <c r="O140" s="28"/>
       <c r="P140" s="28"/>
     </row>
-    <row r="141" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="141" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B141" s="28"/>
       <c r="C141" s="28"/>
       <c r="D141" s="28"/>
@@ -7244,7 +7277,7 @@
       <c r="O141" s="28"/>
       <c r="P141" s="28"/>
     </row>
-    <row r="142" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="142" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B142" s="28"/>
       <c r="C142" s="28"/>
       <c r="D142" s="28"/>
@@ -7261,7 +7294,7 @@
       <c r="O142" s="28"/>
       <c r="P142" s="28"/>
     </row>
-    <row r="143" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="143" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B143" s="28"/>
       <c r="C143" s="28"/>
       <c r="D143" s="28"/>
@@ -7278,7 +7311,7 @@
       <c r="O143" s="28"/>
       <c r="P143" s="28"/>
     </row>
-    <row r="144" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="144" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B144" s="28"/>
       <c r="C144" s="28"/>
       <c r="D144" s="28"/>
@@ -7295,7 +7328,7 @@
       <c r="O144" s="28"/>
       <c r="P144" s="28"/>
     </row>
-    <row r="145" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="145" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B145" s="28"/>
       <c r="C145" s="28"/>
       <c r="D145" s="28"/>
@@ -7312,7 +7345,7 @@
       <c r="O145" s="28"/>
       <c r="P145" s="28"/>
     </row>
-    <row r="146" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="146" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B146" s="28"/>
       <c r="C146" s="28"/>
       <c r="D146" s="28"/>
@@ -7329,7 +7362,7 @@
       <c r="O146" s="28"/>
       <c r="P146" s="28"/>
     </row>
-    <row r="147" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="147" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B147" s="28"/>
       <c r="C147" s="28"/>
       <c r="D147" s="28"/>
@@ -7346,7 +7379,7 @@
       <c r="O147" s="28"/>
       <c r="P147" s="28"/>
     </row>
-    <row r="148" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="148" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B148" s="28"/>
       <c r="C148" s="28"/>
       <c r="D148" s="28"/>
@@ -7363,7 +7396,7 @@
       <c r="O148" s="28"/>
       <c r="P148" s="28"/>
     </row>
-    <row r="149" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="149" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B149" s="28"/>
       <c r="C149" s="28"/>
       <c r="D149" s="28"/>
@@ -7380,7 +7413,7 @@
       <c r="O149" s="28"/>
       <c r="P149" s="28"/>
     </row>
-    <row r="150" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="150" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B150" s="28"/>
       <c r="C150" s="28"/>
       <c r="D150" s="28"/>
@@ -7397,7 +7430,7 @@
       <c r="O150" s="28"/>
       <c r="P150" s="28"/>
     </row>
-    <row r="151" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="151" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B151" s="28"/>
       <c r="C151" s="28"/>
       <c r="D151" s="28"/>
@@ -7414,7 +7447,7 @@
       <c r="O151" s="28"/>
       <c r="P151" s="28"/>
     </row>
-    <row r="152" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="152" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B152" s="28"/>
       <c r="C152" s="28"/>
       <c r="D152" s="28"/>
@@ -7431,7 +7464,7 @@
       <c r="O152" s="28"/>
       <c r="P152" s="28"/>
     </row>
-    <row r="153" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="153" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B153" s="28"/>
       <c r="C153" s="28"/>
       <c r="D153" s="28"/>
@@ -7448,7 +7481,7 @@
       <c r="O153" s="28"/>
       <c r="P153" s="28"/>
     </row>
-    <row r="154" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="154" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B154" s="28"/>
       <c r="C154" s="28"/>
       <c r="D154" s="28"/>
@@ -7465,7 +7498,7 @@
       <c r="O154" s="28"/>
       <c r="P154" s="28"/>
     </row>
-    <row r="155" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="155" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B155" s="28"/>
       <c r="C155" s="28"/>
       <c r="D155" s="28"/>
@@ -7482,7 +7515,7 @@
       <c r="O155" s="28"/>
       <c r="P155" s="28"/>
     </row>
-    <row r="156" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="156" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B156" s="28"/>
       <c r="C156" s="28"/>
       <c r="D156" s="28"/>
@@ -7499,7 +7532,7 @@
       <c r="O156" s="28"/>
       <c r="P156" s="28"/>
     </row>
-    <row r="157" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="157" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B157" s="28"/>
       <c r="C157" s="28"/>
       <c r="D157" s="28"/>
@@ -7516,7 +7549,7 @@
       <c r="O157" s="28"/>
       <c r="P157" s="28"/>
     </row>
-    <row r="158" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="158" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B158" s="28"/>
       <c r="C158" s="28"/>
       <c r="D158" s="28"/>
@@ -7533,7 +7566,7 @@
       <c r="O158" s="28"/>
       <c r="P158" s="28"/>
     </row>
-    <row r="159" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="159" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B159" s="28"/>
       <c r="C159" s="28"/>
       <c r="D159" s="28"/>
@@ -7550,7 +7583,7 @@
       <c r="O159" s="28"/>
       <c r="P159" s="28"/>
     </row>
-    <row r="160" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="160" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B160" s="28"/>
       <c r="C160" s="28"/>
       <c r="D160" s="28"/>
@@ -7575,21 +7608,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q83"/>
+  <dimension ref="A1:Q84"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="Q85" sqref="Q85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.453125" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.54296875" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.54296875" style="2"/>
+    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -7610,7 +7643,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -7631,7 +7664,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -7684,7 +7717,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>43908</v>
       </c>
@@ -7737,7 +7770,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>43909</v>
       </c>
@@ -7790,7 +7823,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>43910</v>
       </c>
@@ -7843,7 +7876,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>43911</v>
       </c>
@@ -7896,7 +7929,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>43912</v>
       </c>
@@ -7949,7 +7982,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>43913</v>
       </c>
@@ -8002,7 +8035,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>43914</v>
       </c>
@@ -8055,7 +8088,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>43915</v>
       </c>
@@ -8108,7 +8141,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>43916</v>
       </c>
@@ -8161,7 +8194,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>43917</v>
       </c>
@@ -8214,7 +8247,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>43918</v>
       </c>
@@ -8267,7 +8300,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>43919</v>
       </c>
@@ -8320,7 +8353,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>43920</v>
       </c>
@@ -8373,7 +8406,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>43921</v>
       </c>
@@ -8426,7 +8459,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>43922</v>
       </c>
@@ -8479,7 +8512,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>43923</v>
       </c>
@@ -8532,7 +8565,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>43924</v>
       </c>
@@ -8585,7 +8618,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>43925</v>
       </c>
@@ -8638,7 +8671,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>43926</v>
       </c>
@@ -8691,7 +8724,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>43927</v>
       </c>
@@ -8744,7 +8777,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>43928</v>
       </c>
@@ -8797,7 +8830,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>43929</v>
       </c>
@@ -8850,7 +8883,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>43930</v>
       </c>
@@ -8903,7 +8936,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>43931</v>
       </c>
@@ -8956,7 +8989,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <v>43932</v>
       </c>
@@ -9009,7 +9042,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <v>43933</v>
       </c>
@@ -9062,7 +9095,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <v>43934</v>
       </c>
@@ -9115,7 +9148,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <v>43935</v>
       </c>
@@ -9168,7 +9201,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>43936</v>
       </c>
@@ -9221,7 +9254,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <v>43937</v>
       </c>
@@ -9274,7 +9307,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <v>43938</v>
       </c>
@@ -9327,7 +9360,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <v>43939</v>
       </c>
@@ -9380,7 +9413,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="30">
         <v>43940</v>
       </c>
@@ -9433,7 +9466,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="30">
         <v>43941</v>
       </c>
@@ -9486,7 +9519,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="30">
         <v>43942</v>
       </c>
@@ -9539,7 +9572,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="30">
         <v>43943</v>
       </c>
@@ -9592,7 +9625,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="30">
         <v>43944</v>
       </c>
@@ -9645,7 +9678,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="30">
         <v>43945</v>
       </c>
@@ -9698,7 +9731,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="30">
         <v>43946</v>
       </c>
@@ -9751,7 +9784,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="30">
         <v>43947</v>
       </c>
@@ -9804,7 +9837,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="30">
         <v>43948</v>
       </c>
@@ -9857,7 +9890,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="30">
         <v>43949</v>
       </c>
@@ -9910,7 +9943,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="30">
         <v>43950</v>
       </c>
@@ -9963,7 +9996,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="30">
         <v>43951</v>
       </c>
@@ -10016,7 +10049,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="30">
         <v>43952</v>
       </c>
@@ -10069,7 +10102,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="30">
         <v>43953</v>
       </c>
@@ -10122,7 +10155,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="30">
         <v>43954</v>
       </c>
@@ -10175,7 +10208,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="30">
         <v>43955</v>
       </c>
@@ -10228,7 +10261,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="30">
         <v>43956</v>
       </c>
@@ -10281,7 +10314,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="30">
         <v>43957</v>
       </c>
@@ -10334,7 +10367,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="30">
         <v>43958</v>
       </c>
@@ -10387,7 +10420,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="30">
         <v>43959</v>
       </c>
@@ -10440,7 +10473,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="30">
         <v>43960</v>
       </c>
@@ -10493,7 +10526,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="30">
         <v>43961</v>
       </c>
@@ -10546,7 +10579,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="30">
         <v>43962</v>
       </c>
@@ -10599,7 +10632,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="30">
         <v>43963</v>
       </c>
@@ -10652,7 +10685,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="30">
         <v>43964</v>
       </c>
@@ -10705,7 +10738,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" s="30">
         <v>43965</v>
       </c>
@@ -10758,7 +10791,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="30">
         <v>43966</v>
       </c>
@@ -10811,7 +10844,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" s="30">
         <v>43967</v>
       </c>
@@ -10864,7 +10897,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" s="30">
         <v>43968</v>
       </c>
@@ -10917,7 +10950,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" s="30">
         <v>43969</v>
       </c>
@@ -10970,7 +11003,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" s="30">
         <v>43970</v>
       </c>
@@ -11023,7 +11056,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" s="30">
         <v>43971</v>
       </c>
@@ -11076,7 +11109,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" s="30">
         <v>43972</v>
       </c>
@@ -11129,7 +11162,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" s="30">
         <v>43973</v>
       </c>
@@ -11182,7 +11215,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" s="30">
         <v>43974</v>
       </c>
@@ -11235,7 +11268,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" s="30">
         <v>43975</v>
       </c>
@@ -11288,7 +11321,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" s="30">
         <v>43976</v>
       </c>
@@ -11341,7 +11374,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" s="30">
         <v>43977</v>
       </c>
@@ -11394,7 +11427,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" s="30">
         <v>43978</v>
       </c>
@@ -11447,7 +11480,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" s="30">
         <v>43979</v>
       </c>
@@ -11500,7 +11533,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" s="30">
         <v>43980</v>
       </c>
@@ -11553,7 +11586,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" s="30">
         <v>43981</v>
       </c>
@@ -11606,7 +11639,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" s="30">
         <v>43982</v>
       </c>
@@ -11659,7 +11692,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" s="30">
         <v>43983</v>
       </c>
@@ -11712,7 +11745,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" s="30">
         <v>43984</v>
       </c>
@@ -11765,7 +11798,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" s="30">
         <v>43985</v>
       </c>
@@ -11818,7 +11851,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" s="30">
         <v>43986</v>
       </c>
@@ -11871,7 +11904,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" s="30">
         <v>43987</v>
       </c>
@@ -11922,6 +11955,59 @@
       </c>
       <c r="Q83" s="13">
         <v>23</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A84" s="30">
+        <v>43988</v>
+      </c>
+      <c r="B84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K84" s="14">
+        <v>5</v>
+      </c>
+      <c r="L84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q84" s="13">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -11932,23 +12018,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q75"/>
+  <dimension ref="A1:Q76"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="F64" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B64" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="O80" sqref="O80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.1796875" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.54296875" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.54296875" style="2"/>
+    <col min="1" max="1" width="15.28515625" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -11969,7 +12055,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -11990,7 +12076,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -12043,7 +12129,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>43916</v>
       </c>
@@ -12096,7 +12182,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>43917</v>
       </c>
@@ -12149,7 +12235,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>43918</v>
       </c>
@@ -12202,7 +12288,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>43919</v>
       </c>
@@ -12255,7 +12341,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>43920</v>
       </c>
@@ -12308,7 +12394,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>43921</v>
       </c>
@@ -12361,7 +12447,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>43922</v>
       </c>
@@ -12414,7 +12500,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>43923</v>
       </c>
@@ -12467,7 +12553,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>43924</v>
       </c>
@@ -12520,7 +12606,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>43925</v>
       </c>
@@ -12573,7 +12659,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>43926</v>
       </c>
@@ -12626,7 +12712,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>43927</v>
       </c>
@@ -12679,7 +12765,7 @@
         <v>1262</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>43928</v>
       </c>
@@ -12732,7 +12818,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>43929</v>
       </c>
@@ -12785,7 +12871,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>43930</v>
       </c>
@@ -12838,7 +12924,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>43931</v>
       </c>
@@ -12891,7 +12977,7 @@
         <v>1461</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>43932</v>
       </c>
@@ -12944,7 +13030,7 @@
         <v>1467</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>43933</v>
       </c>
@@ -12997,7 +13083,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>43934</v>
       </c>
@@ -13050,7 +13136,7 @@
         <v>1482</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>43935</v>
       </c>
@@ -13103,7 +13189,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>43936</v>
       </c>
@@ -13156,7 +13242,7 @@
         <v>1486</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>43937</v>
       </c>
@@ -13209,7 +13295,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>43938</v>
       </c>
@@ -13262,7 +13348,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>43939</v>
       </c>
@@ -13315,7 +13401,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <v>43940</v>
       </c>
@@ -13368,7 +13454,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <v>43941</v>
       </c>
@@ -13421,7 +13507,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <v>43942</v>
       </c>
@@ -13474,7 +13560,7 @@
         <v>1472</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <v>43943</v>
       </c>
@@ -13527,7 +13613,7 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>43944</v>
       </c>
@@ -13580,7 +13666,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <v>43945</v>
       </c>
@@ -13633,7 +13719,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <v>43946</v>
       </c>
@@ -13686,7 +13772,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <v>43947</v>
       </c>
@@ -13739,7 +13825,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="30">
         <v>43948</v>
       </c>
@@ -13792,7 +13878,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="30">
         <v>43949</v>
       </c>
@@ -13845,7 +13931,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="30">
         <v>43950</v>
       </c>
@@ -13898,7 +13984,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="30">
         <v>43951</v>
       </c>
@@ -13951,7 +14037,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="30">
         <v>43952</v>
       </c>
@@ -14004,7 +14090,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="30">
         <v>43953</v>
       </c>
@@ -14057,7 +14143,7 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="30">
         <v>43954</v>
       </c>
@@ -14110,7 +14196,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="30">
         <v>43955</v>
       </c>
@@ -14163,7 +14249,7 @@
         <v>1279</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="30">
         <v>43956</v>
       </c>
@@ -14216,7 +14302,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="30">
         <v>43957</v>
       </c>
@@ -14269,7 +14355,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="30">
         <v>43958</v>
       </c>
@@ -14322,7 +14408,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="30">
         <v>43959</v>
       </c>
@@ -14375,7 +14461,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="30">
         <v>43960</v>
       </c>
@@ -14428,7 +14514,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="30">
         <v>43961</v>
       </c>
@@ -14481,7 +14567,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="30">
         <v>43962</v>
       </c>
@@ -14534,7 +14620,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="30">
         <v>43963</v>
       </c>
@@ -14587,7 +14673,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="30">
         <v>43964</v>
       </c>
@@ -14640,7 +14726,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="30">
         <v>43965</v>
       </c>
@@ -14693,7 +14779,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="30">
         <v>43966</v>
       </c>
@@ -14746,7 +14832,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="30">
         <v>43967</v>
       </c>
@@ -14799,7 +14885,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="30">
         <v>43968</v>
       </c>
@@ -14852,7 +14938,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="30">
         <v>43969</v>
       </c>
@@ -14905,7 +14991,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="30">
         <v>43970</v>
       </c>
@@ -14958,7 +15044,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="30">
         <v>43971</v>
       </c>
@@ -15011,7 +15097,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="30">
         <v>43972</v>
       </c>
@@ -15064,7 +15150,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" s="30">
         <v>43973</v>
       </c>
@@ -15117,7 +15203,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="30">
         <v>43974</v>
       </c>
@@ -15170,7 +15256,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" s="30">
         <v>43975</v>
       </c>
@@ -15223,7 +15309,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" s="30">
         <v>43976</v>
       </c>
@@ -15276,7 +15362,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" s="51">
         <v>43977</v>
       </c>
@@ -15329,7 +15415,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" s="51">
         <v>43978</v>
       </c>
@@ -15382,7 +15468,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" s="51">
         <v>43979</v>
       </c>
@@ -15435,7 +15521,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" s="51">
         <v>43980</v>
       </c>
@@ -15488,7 +15574,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" s="51">
         <v>43981</v>
       </c>
@@ -15541,7 +15627,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" s="51">
         <v>43982</v>
       </c>
@@ -15594,7 +15680,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" s="51">
         <v>43983</v>
       </c>
@@ -15647,7 +15733,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" s="51">
         <v>43984</v>
       </c>
@@ -15700,7 +15786,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" s="51">
         <v>43985</v>
       </c>
@@ -15753,7 +15839,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" s="51">
         <v>43986</v>
       </c>
@@ -15806,7 +15892,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" s="51">
         <v>43987</v>
       </c>
@@ -15857,6 +15943,59 @@
       </c>
       <c r="Q75" s="13">
         <v>676</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A76" s="51">
+        <v>43988</v>
+      </c>
+      <c r="B76" s="11">
+        <v>8</v>
+      </c>
+      <c r="C76" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D76" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E76" s="11">
+        <v>54</v>
+      </c>
+      <c r="F76" s="11">
+        <v>12</v>
+      </c>
+      <c r="G76" s="11">
+        <v>62</v>
+      </c>
+      <c r="H76" s="11">
+        <v>294</v>
+      </c>
+      <c r="I76" s="11">
+        <v>6</v>
+      </c>
+      <c r="J76" s="11">
+        <v>59</v>
+      </c>
+      <c r="K76" s="11">
+        <v>143</v>
+      </c>
+      <c r="L76" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M76" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N76" s="11">
+        <v>8</v>
+      </c>
+      <c r="O76" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P76" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q76" s="13">
+        <v>646</v>
       </c>
     </row>
   </sheetData>
@@ -15867,23 +16006,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q75"/>
+  <dimension ref="A1:Q76"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B61" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="M77" sqref="M77:M78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.453125" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.54296875" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.54296875" style="2"/>
+    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -15904,7 +16043,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -15925,7 +16064,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -15978,7 +16117,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>43916</v>
       </c>
@@ -16031,7 +16170,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>43917</v>
       </c>
@@ -16084,7 +16223,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>43918</v>
       </c>
@@ -16137,7 +16276,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>43919</v>
       </c>
@@ -16190,7 +16329,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>43920</v>
       </c>
@@ -16243,7 +16382,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>43921</v>
       </c>
@@ -16296,7 +16435,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>43922</v>
       </c>
@@ -16349,7 +16488,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>43923</v>
       </c>
@@ -16402,7 +16541,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>43924</v>
       </c>
@@ -16455,7 +16594,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>43925</v>
       </c>
@@ -16508,7 +16647,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>43926</v>
       </c>
@@ -16561,7 +16700,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>43927</v>
       </c>
@@ -16614,7 +16753,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>43928</v>
       </c>
@@ -16667,7 +16806,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>43929</v>
       </c>
@@ -16720,7 +16859,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>43930</v>
       </c>
@@ -16773,7 +16912,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>43931</v>
       </c>
@@ -16826,7 +16965,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>43932</v>
       </c>
@@ -16879,7 +17018,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>43933</v>
       </c>
@@ -16932,7 +17071,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>43934</v>
       </c>
@@ -16985,7 +17124,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>43935</v>
       </c>
@@ -17038,7 +17177,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>43936</v>
       </c>
@@ -17091,7 +17230,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>43937</v>
       </c>
@@ -17144,7 +17283,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>43938</v>
       </c>
@@ -17197,7 +17336,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>43939</v>
       </c>
@@ -17250,7 +17389,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <v>43940</v>
       </c>
@@ -17303,7 +17442,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <v>43941</v>
       </c>
@@ -17356,7 +17495,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <v>43942</v>
       </c>
@@ -17409,7 +17548,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <v>43943</v>
       </c>
@@ -17462,7 +17601,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>43944</v>
       </c>
@@ -17515,7 +17654,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <v>43945</v>
       </c>
@@ -17568,7 +17707,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <v>43946</v>
       </c>
@@ -17621,7 +17760,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <v>43947</v>
       </c>
@@ -17674,7 +17813,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="30">
         <v>43948</v>
       </c>
@@ -17727,7 +17866,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="30">
         <v>43949</v>
       </c>
@@ -17780,7 +17919,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="30">
         <v>43950</v>
       </c>
@@ -17833,7 +17972,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="30">
         <v>43951</v>
       </c>
@@ -17886,7 +18025,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="30">
         <v>43952</v>
       </c>
@@ -17939,7 +18078,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="30">
         <v>43953</v>
       </c>
@@ -17992,7 +18131,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="30">
         <v>43954</v>
       </c>
@@ -18045,7 +18184,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="30">
         <v>43955</v>
       </c>
@@ -18098,7 +18237,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="30">
         <v>43956</v>
       </c>
@@ -18151,7 +18290,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="30">
         <v>43957</v>
       </c>
@@ -18204,7 +18343,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="30">
         <v>43958</v>
       </c>
@@ -18257,7 +18396,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="30">
         <v>43959</v>
       </c>
@@ -18310,7 +18449,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="30">
         <v>43960</v>
       </c>
@@ -18363,7 +18502,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="30">
         <v>43961</v>
       </c>
@@ -18416,7 +18555,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="30">
         <v>43962</v>
       </c>
@@ -18469,7 +18608,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="30">
         <v>43963</v>
       </c>
@@ -18522,7 +18661,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="30">
         <v>43964</v>
       </c>
@@ -18575,7 +18714,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="30">
         <v>43965</v>
       </c>
@@ -18628,7 +18767,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="30">
         <v>43966</v>
       </c>
@@ -18681,7 +18820,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="30">
         <v>43967</v>
       </c>
@@ -18734,7 +18873,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="30">
         <v>43968</v>
       </c>
@@ -18787,7 +18926,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="30">
         <v>43969</v>
       </c>
@@ -18840,7 +18979,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="30">
         <v>43970</v>
       </c>
@@ -18893,7 +19032,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="30">
         <v>43971</v>
       </c>
@@ -18946,7 +19085,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="30">
         <v>43972</v>
       </c>
@@ -18999,7 +19138,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" s="30">
         <v>43973</v>
       </c>
@@ -19052,7 +19191,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="30">
         <v>43974</v>
       </c>
@@ -19105,7 +19244,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" s="30">
         <v>43975</v>
       </c>
@@ -19158,7 +19297,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" s="30">
         <v>43976</v>
       </c>
@@ -19211,7 +19350,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" s="30">
         <v>43977</v>
       </c>
@@ -19264,7 +19403,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" s="30">
         <v>43978</v>
       </c>
@@ -19317,7 +19456,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" s="30">
         <v>43979</v>
       </c>
@@ -19370,7 +19509,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" s="30">
         <v>43980</v>
       </c>
@@ -19423,7 +19562,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" s="30">
         <v>43981</v>
       </c>
@@ -19476,7 +19615,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" s="30">
         <v>43982</v>
       </c>
@@ -19529,7 +19668,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" s="30">
         <v>43983</v>
       </c>
@@ -19582,7 +19721,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" s="30">
         <v>43984</v>
       </c>
@@ -19635,7 +19774,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" s="30">
         <v>43985</v>
       </c>
@@ -19688,7 +19827,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" s="30">
         <v>43986</v>
       </c>
@@ -19741,7 +19880,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" s="30">
         <v>43987</v>
       </c>
@@ -19792,6 +19931,59 @@
       </c>
       <c r="Q75" s="13">
         <v>319</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A76" s="30">
+        <v>43988</v>
+      </c>
+      <c r="B76" s="11">
+        <v>35</v>
+      </c>
+      <c r="C76" s="11">
+        <v>20</v>
+      </c>
+      <c r="D76" s="11">
+        <v>14</v>
+      </c>
+      <c r="E76" s="11">
+        <v>27</v>
+      </c>
+      <c r="F76" s="11">
+        <v>39</v>
+      </c>
+      <c r="G76" s="11">
+        <v>15</v>
+      </c>
+      <c r="H76" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I76" s="11">
+        <v>9</v>
+      </c>
+      <c r="J76" s="11">
+        <v>60</v>
+      </c>
+      <c r="K76" s="11">
+        <v>142</v>
+      </c>
+      <c r="L76" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M76" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N76" s="11">
+        <v>11</v>
+      </c>
+      <c r="O76" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P76" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q76" s="13">
+        <v>373</v>
       </c>
     </row>
   </sheetData>
@@ -19799,7 +19991,7 @@
 </worksheet>
 </file>
 
-<file path=customXML/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA" version="1.0.0">
   <systemFields>
     <field name="Objective-Id">
@@ -19821,10 +20013,10 @@
       <value order="0">true</value>
     </field>
     <field name="Objective-DatePublished">
-      <value order="0">2020-06-05T12:12:14Z</value>
+      <value order="0">2020-06-06T11:52:20Z</value>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-05T12:12:14Z</value>
+      <value order="0">2020-06-06T11:52:20Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -19839,13 +20031,13 @@
       <value order="0">Published</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41574143</value>
+      <value order="0">vA41586174</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">20.0</value>
+      <value order="0">21.0</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">151</value>
+      <value order="0">154</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>
@@ -19882,7 +20074,7 @@
 </metadata>
 </file>
 
-<file path=customXML/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5745109E-2DDF-40CB-AC2B-FF9B10C90820}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-07 20:08)
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\scotland.gov.uk\dc2\FS5_Home\u204186\Gov.scot content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u201433\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA1432\A28088333\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1657" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1682" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -663,6 +663,23 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
           <a:r>
             <a:rPr lang="en-GB" sz="1100">
               <a:effectLst/>
@@ -688,8 +705,20 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>on the day preceding the notification date. These have been compiled into a cumulative figure for positive tests in Table 1.</a:t>
+            <a:t>on the day preceding the notification date. These have been compiled into a cumulative figure for positive tests in Table 1.  T</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>he daily total of people found positive on 2/6/20 contains 40 historic samples from an NHS Fife laboratory.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB">
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
@@ -703,6 +732,23 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
           <a:r>
             <a:rPr lang="en-GB" sz="1100">
               <a:effectLst/>
@@ -710,19 +756,33 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>3. Where labs do not provide their overnight data in time for the daily publication, the testing figures will then be added to the return for the subsequent day. Figures may also be revised if labs discover an error and have to resubmit their data. </a:t>
+            <a:t>3. Where labs do not provide their overnight data in time for the daily publication, the testing figures will then be added to the return for the subsequent day.   </a:t>
           </a:r>
         </a:p>
         <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100">
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB" sz="1100">
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
@@ -800,7 +860,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> on updated postcode information, one case has been reassigned from Dumfries and Galloway to Greater Glasgow and Clyde. This  resulted in a decrease of one in the total number of cases in Dumfries and Galloway.</a:t>
+            <a:t> on updated postcode information, one case has been reassigned from Dumfries and Galloway to Greater Glasgow and Clyde. This resulted in a decrease of one in the total number of cases in Dumfries and Galloway.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1292,107 +1352,6 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100">
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>11.</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" baseline="0">
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> For Table 1, the daily total of people found positive on 2/6/20 contains 40 historic samples from an NHS Fife laboratory.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:endParaRPr lang="en-GB" sz="1100" baseline="0">
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" baseline="0">
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>12. On 04/06/2020, the number of positive cases in Highland decreased by 1 due to an update to postcode of residence for one case.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-GB">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100">
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
           <a:r>
             <a:rPr lang="en-GB" sz="1100">
               <a:effectLst/>
@@ -1787,10 +1746,10 @@
   <dimension ref="A1:S160"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B81" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H98" sqref="H98"/>
+      <selection pane="bottomRight" activeCell="O96" sqref="B96:O96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6496,21 +6455,54 @@
       </c>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B96" s="28"/>
-      <c r="C96" s="28"/>
-      <c r="D96" s="28"/>
-      <c r="E96" s="28"/>
-      <c r="F96" s="28"/>
-      <c r="G96" s="28"/>
-      <c r="H96" s="28"/>
-      <c r="I96" s="28"/>
-      <c r="J96" s="28"/>
-      <c r="K96" s="28"/>
-      <c r="L96" s="28"/>
-      <c r="M96" s="28"/>
-      <c r="N96" s="28"/>
-      <c r="O96" s="28"/>
-      <c r="P96" s="28"/>
+      <c r="A96" s="5">
+        <v>43989</v>
+      </c>
+      <c r="B96" s="28">
+        <v>1079</v>
+      </c>
+      <c r="C96" s="28">
+        <v>326</v>
+      </c>
+      <c r="D96" s="28">
+        <v>261</v>
+      </c>
+      <c r="E96" s="28">
+        <v>879</v>
+      </c>
+      <c r="F96" s="28">
+        <v>946</v>
+      </c>
+      <c r="G96" s="28">
+        <v>1286</v>
+      </c>
+      <c r="H96" s="28">
+        <v>3981</v>
+      </c>
+      <c r="I96" s="28">
+        <v>339</v>
+      </c>
+      <c r="J96" s="28">
+        <v>2008</v>
+      </c>
+      <c r="K96" s="28">
+        <v>2772</v>
+      </c>
+      <c r="L96" s="28">
+        <v>8</v>
+      </c>
+      <c r="M96" s="28">
+        <v>54</v>
+      </c>
+      <c r="N96" s="28">
+        <v>1676</v>
+      </c>
+      <c r="O96" s="28">
+        <v>6</v>
+      </c>
+      <c r="P96" s="32">
+        <v>15621</v>
+      </c>
     </row>
     <row r="97" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B97" s="28"/>
@@ -7608,11 +7600,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q84"/>
+  <dimension ref="A1:Q85"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q85" sqref="Q85"/>
+      <pane ySplit="3" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12010,6 +12002,59 @@
         <v>20</v>
       </c>
     </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A85" s="30">
+        <v>43989</v>
+      </c>
+      <c r="B85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K85" s="11">
+        <v>7</v>
+      </c>
+      <c r="L85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P85" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q85" s="13">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -12018,13 +12063,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q76"/>
+  <dimension ref="A1:Q77"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B64" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="O80" sqref="O80"/>
+      <selection pane="bottomRight" activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15998,6 +16043,59 @@
         <v>646</v>
       </c>
     </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A77" s="51">
+        <v>43989</v>
+      </c>
+      <c r="B77" s="11">
+        <v>10</v>
+      </c>
+      <c r="C77" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D77" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E77" s="11">
+        <v>54</v>
+      </c>
+      <c r="F77" s="11">
+        <v>10</v>
+      </c>
+      <c r="G77" s="11">
+        <v>60</v>
+      </c>
+      <c r="H77" s="11">
+        <v>295</v>
+      </c>
+      <c r="I77" s="11">
+        <v>6</v>
+      </c>
+      <c r="J77" s="11">
+        <v>58</v>
+      </c>
+      <c r="K77" s="11">
+        <v>146</v>
+      </c>
+      <c r="L77" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M77" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N77" s="11">
+        <v>7</v>
+      </c>
+      <c r="O77" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P77" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q77" s="13">
+        <v>646</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -16006,13 +16104,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q76"/>
+  <dimension ref="A1:Q77"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B61" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B49" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M77" sqref="M77:M78"/>
+      <selection pane="bottomRight" activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19986,12 +20084,65 @@
         <v>373</v>
       </c>
     </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A77" s="30">
+        <v>43989</v>
+      </c>
+      <c r="B77" s="11">
+        <v>52</v>
+      </c>
+      <c r="C77" s="11">
+        <v>17</v>
+      </c>
+      <c r="D77" s="11">
+        <v>11</v>
+      </c>
+      <c r="E77" s="11">
+        <v>16</v>
+      </c>
+      <c r="F77" s="11">
+        <v>41</v>
+      </c>
+      <c r="G77" s="11">
+        <v>8</v>
+      </c>
+      <c r="H77" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I77" s="11">
+        <v>24</v>
+      </c>
+      <c r="J77" s="11">
+        <v>74</v>
+      </c>
+      <c r="K77" s="11">
+        <v>98</v>
+      </c>
+      <c r="L77" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M77" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N77" s="11">
+        <v>13</v>
+      </c>
+      <c r="O77" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P77" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q77" s="36">
+        <v>356</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXML/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA" version="1.0.0">
   <systemFields>
     <field name="Objective-Id">
@@ -20013,10 +20164,10 @@
       <value order="0">true</value>
     </field>
     <field name="Objective-DatePublished">
-      <value order="0">2020-06-06T11:52:20Z</value>
+      <value order="0">2020-06-07T11:47:42Z</value>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-06T11:52:20Z</value>
+      <value order="0">2020-06-07T11:47:42Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -20031,13 +20182,13 @@
       <value order="0">Published</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41586174</value>
+      <value order="0">vA41590260</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">21.0</value>
+      <value order="0">22.0</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">154</value>
+      <value order="0">157</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>
@@ -20074,7 +20225,7 @@
 </metadata>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXML/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5745109E-2DDF-40CB-AC2B-FF9B10C90820}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-08 12:09)
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\scotland.gov.uk\dc2\FS5_Home\u204186\Gov.scot content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u201433\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA1432\A28088333\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1657" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1682" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -663,6 +663,23 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
           <a:r>
             <a:rPr lang="en-GB" sz="1100">
               <a:effectLst/>
@@ -688,8 +705,20 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>on the day preceding the notification date. These have been compiled into a cumulative figure for positive tests in Table 1.</a:t>
+            <a:t>on the day preceding the notification date. These have been compiled into a cumulative figure for positive tests in Table 1.  T</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>he daily total of people found positive on 2/6/20 contains 40 historic samples from an NHS Fife laboratory.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB">
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
@@ -703,6 +732,23 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
           <a:r>
             <a:rPr lang="en-GB" sz="1100">
               <a:effectLst/>
@@ -710,19 +756,33 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>3. Where labs do not provide their overnight data in time for the daily publication, the testing figures will then be added to the return for the subsequent day. Figures may also be revised if labs discover an error and have to resubmit their data. </a:t>
+            <a:t>3. Where labs do not provide their overnight data in time for the daily publication, the testing figures will then be added to the return for the subsequent day.   </a:t>
           </a:r>
         </a:p>
         <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100">
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB" sz="1100">
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
@@ -800,7 +860,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> on updated postcode information, one case has been reassigned from Dumfries and Galloway to Greater Glasgow and Clyde. This  resulted in a decrease of one in the total number of cases in Dumfries and Galloway.</a:t>
+            <a:t> on updated postcode information, one case has been reassigned from Dumfries and Galloway to Greater Glasgow and Clyde. This resulted in a decrease of one in the total number of cases in Dumfries and Galloway.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1292,107 +1352,6 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100">
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>11.</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" baseline="0">
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> For Table 1, the daily total of people found positive on 2/6/20 contains 40 historic samples from an NHS Fife laboratory.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:endParaRPr lang="en-GB" sz="1100" baseline="0">
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" baseline="0">
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>12. On 04/06/2020, the number of positive cases in Highland decreased by 1 due to an update to postcode of residence for one case.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-GB">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100">
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
           <a:r>
             <a:rPr lang="en-GB" sz="1100">
               <a:effectLst/>
@@ -1787,10 +1746,10 @@
   <dimension ref="A1:S160"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B81" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H98" sqref="H98"/>
+      <selection pane="bottomRight" activeCell="O96" sqref="B96:O96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6496,21 +6455,54 @@
       </c>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B96" s="28"/>
-      <c r="C96" s="28"/>
-      <c r="D96" s="28"/>
-      <c r="E96" s="28"/>
-      <c r="F96" s="28"/>
-      <c r="G96" s="28"/>
-      <c r="H96" s="28"/>
-      <c r="I96" s="28"/>
-      <c r="J96" s="28"/>
-      <c r="K96" s="28"/>
-      <c r="L96" s="28"/>
-      <c r="M96" s="28"/>
-      <c r="N96" s="28"/>
-      <c r="O96" s="28"/>
-      <c r="P96" s="28"/>
+      <c r="A96" s="5">
+        <v>43989</v>
+      </c>
+      <c r="B96" s="28">
+        <v>1079</v>
+      </c>
+      <c r="C96" s="28">
+        <v>326</v>
+      </c>
+      <c r="D96" s="28">
+        <v>261</v>
+      </c>
+      <c r="E96" s="28">
+        <v>879</v>
+      </c>
+      <c r="F96" s="28">
+        <v>946</v>
+      </c>
+      <c r="G96" s="28">
+        <v>1286</v>
+      </c>
+      <c r="H96" s="28">
+        <v>3981</v>
+      </c>
+      <c r="I96" s="28">
+        <v>339</v>
+      </c>
+      <c r="J96" s="28">
+        <v>2008</v>
+      </c>
+      <c r="K96" s="28">
+        <v>2772</v>
+      </c>
+      <c r="L96" s="28">
+        <v>8</v>
+      </c>
+      <c r="M96" s="28">
+        <v>54</v>
+      </c>
+      <c r="N96" s="28">
+        <v>1676</v>
+      </c>
+      <c r="O96" s="28">
+        <v>6</v>
+      </c>
+      <c r="P96" s="32">
+        <v>15621</v>
+      </c>
     </row>
     <row r="97" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B97" s="28"/>
@@ -7608,11 +7600,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q84"/>
+  <dimension ref="A1:Q85"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q85" sqref="Q85"/>
+      <pane ySplit="3" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12010,6 +12002,59 @@
         <v>20</v>
       </c>
     </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A85" s="30">
+        <v>43989</v>
+      </c>
+      <c r="B85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K85" s="11">
+        <v>7</v>
+      </c>
+      <c r="L85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P85" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q85" s="13">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -12018,13 +12063,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q76"/>
+  <dimension ref="A1:Q77"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B64" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="O80" sqref="O80"/>
+      <selection pane="bottomRight" activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15998,6 +16043,59 @@
         <v>646</v>
       </c>
     </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A77" s="51">
+        <v>43989</v>
+      </c>
+      <c r="B77" s="11">
+        <v>10</v>
+      </c>
+      <c r="C77" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D77" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E77" s="11">
+        <v>54</v>
+      </c>
+      <c r="F77" s="11">
+        <v>10</v>
+      </c>
+      <c r="G77" s="11">
+        <v>60</v>
+      </c>
+      <c r="H77" s="11">
+        <v>295</v>
+      </c>
+      <c r="I77" s="11">
+        <v>6</v>
+      </c>
+      <c r="J77" s="11">
+        <v>58</v>
+      </c>
+      <c r="K77" s="11">
+        <v>146</v>
+      </c>
+      <c r="L77" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M77" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N77" s="11">
+        <v>7</v>
+      </c>
+      <c r="O77" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P77" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q77" s="13">
+        <v>646</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -16006,13 +16104,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q76"/>
+  <dimension ref="A1:Q77"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B61" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B49" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M77" sqref="M77:M78"/>
+      <selection pane="bottomRight" activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19986,12 +20084,65 @@
         <v>373</v>
       </c>
     </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A77" s="30">
+        <v>43989</v>
+      </c>
+      <c r="B77" s="11">
+        <v>52</v>
+      </c>
+      <c r="C77" s="11">
+        <v>17</v>
+      </c>
+      <c r="D77" s="11">
+        <v>11</v>
+      </c>
+      <c r="E77" s="11">
+        <v>16</v>
+      </c>
+      <c r="F77" s="11">
+        <v>41</v>
+      </c>
+      <c r="G77" s="11">
+        <v>8</v>
+      </c>
+      <c r="H77" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I77" s="11">
+        <v>24</v>
+      </c>
+      <c r="J77" s="11">
+        <v>74</v>
+      </c>
+      <c r="K77" s="11">
+        <v>98</v>
+      </c>
+      <c r="L77" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M77" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N77" s="11">
+        <v>13</v>
+      </c>
+      <c r="O77" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P77" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q77" s="36">
+        <v>356</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXML/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA" version="1.0.0">
   <systemFields>
     <field name="Objective-Id">
@@ -20013,10 +20164,10 @@
       <value order="0">true</value>
     </field>
     <field name="Objective-DatePublished">
-      <value order="0">2020-06-06T11:52:20Z</value>
+      <value order="0">2020-06-07T11:47:42Z</value>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-06T11:52:20Z</value>
+      <value order="0">2020-06-07T11:47:42Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -20031,13 +20182,13 @@
       <value order="0">Published</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41586174</value>
+      <value order="0">vA41590260</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">21.0</value>
+      <value order="0">22.0</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">154</value>
+      <value order="0">157</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>
@@ -20074,7 +20225,7 @@
 </metadata>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXML/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5745109E-2DDF-40CB-AC2B-FF9B10C90820}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-08 12:09) (#95)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\scotland.gov.uk\dc2\FS5_Home\u204186\Gov.scot content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u201433\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA1432\A28088333\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1657" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1682" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -663,6 +663,23 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
           <a:r>
             <a:rPr lang="en-GB" sz="1100">
               <a:effectLst/>
@@ -688,8 +705,20 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>on the day preceding the notification date. These have been compiled into a cumulative figure for positive tests in Table 1.</a:t>
+            <a:t>on the day preceding the notification date. These have been compiled into a cumulative figure for positive tests in Table 1.  T</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>he daily total of people found positive on 2/6/20 contains 40 historic samples from an NHS Fife laboratory.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB">
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
@@ -703,6 +732,23 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
           <a:r>
             <a:rPr lang="en-GB" sz="1100">
               <a:effectLst/>
@@ -710,19 +756,33 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>3. Where labs do not provide their overnight data in time for the daily publication, the testing figures will then be added to the return for the subsequent day. Figures may also be revised if labs discover an error and have to resubmit their data. </a:t>
+            <a:t>3. Where labs do not provide their overnight data in time for the daily publication, the testing figures will then be added to the return for the subsequent day.   </a:t>
           </a:r>
         </a:p>
         <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100">
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB" sz="1100">
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
@@ -800,7 +860,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> on updated postcode information, one case has been reassigned from Dumfries and Galloway to Greater Glasgow and Clyde. This  resulted in a decrease of one in the total number of cases in Dumfries and Galloway.</a:t>
+            <a:t> on updated postcode information, one case has been reassigned from Dumfries and Galloway to Greater Glasgow and Clyde. This resulted in a decrease of one in the total number of cases in Dumfries and Galloway.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1292,107 +1352,6 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100">
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>11.</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" baseline="0">
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> For Table 1, the daily total of people found positive on 2/6/20 contains 40 historic samples from an NHS Fife laboratory.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:endParaRPr lang="en-GB" sz="1100" baseline="0">
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" baseline="0">
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>12. On 04/06/2020, the number of positive cases in Highland decreased by 1 due to an update to postcode of residence for one case.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-GB">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100">
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
           <a:r>
             <a:rPr lang="en-GB" sz="1100">
               <a:effectLst/>
@@ -1787,10 +1746,10 @@
   <dimension ref="A1:S160"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B81" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H98" sqref="H98"/>
+      <selection pane="bottomRight" activeCell="O96" sqref="B96:O96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6496,21 +6455,54 @@
       </c>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B96" s="28"/>
-      <c r="C96" s="28"/>
-      <c r="D96" s="28"/>
-      <c r="E96" s="28"/>
-      <c r="F96" s="28"/>
-      <c r="G96" s="28"/>
-      <c r="H96" s="28"/>
-      <c r="I96" s="28"/>
-      <c r="J96" s="28"/>
-      <c r="K96" s="28"/>
-      <c r="L96" s="28"/>
-      <c r="M96" s="28"/>
-      <c r="N96" s="28"/>
-      <c r="O96" s="28"/>
-      <c r="P96" s="28"/>
+      <c r="A96" s="5">
+        <v>43989</v>
+      </c>
+      <c r="B96" s="28">
+        <v>1079</v>
+      </c>
+      <c r="C96" s="28">
+        <v>326</v>
+      </c>
+      <c r="D96" s="28">
+        <v>261</v>
+      </c>
+      <c r="E96" s="28">
+        <v>879</v>
+      </c>
+      <c r="F96" s="28">
+        <v>946</v>
+      </c>
+      <c r="G96" s="28">
+        <v>1286</v>
+      </c>
+      <c r="H96" s="28">
+        <v>3981</v>
+      </c>
+      <c r="I96" s="28">
+        <v>339</v>
+      </c>
+      <c r="J96" s="28">
+        <v>2008</v>
+      </c>
+      <c r="K96" s="28">
+        <v>2772</v>
+      </c>
+      <c r="L96" s="28">
+        <v>8</v>
+      </c>
+      <c r="M96" s="28">
+        <v>54</v>
+      </c>
+      <c r="N96" s="28">
+        <v>1676</v>
+      </c>
+      <c r="O96" s="28">
+        <v>6</v>
+      </c>
+      <c r="P96" s="32">
+        <v>15621</v>
+      </c>
     </row>
     <row r="97" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B97" s="28"/>
@@ -7608,11 +7600,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q84"/>
+  <dimension ref="A1:Q85"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q85" sqref="Q85"/>
+      <pane ySplit="3" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12010,6 +12002,59 @@
         <v>20</v>
       </c>
     </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A85" s="30">
+        <v>43989</v>
+      </c>
+      <c r="B85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K85" s="11">
+        <v>7</v>
+      </c>
+      <c r="L85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P85" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q85" s="13">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -12018,13 +12063,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q76"/>
+  <dimension ref="A1:Q77"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B64" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="O80" sqref="O80"/>
+      <selection pane="bottomRight" activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15998,6 +16043,59 @@
         <v>646</v>
       </c>
     </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A77" s="51">
+        <v>43989</v>
+      </c>
+      <c r="B77" s="11">
+        <v>10</v>
+      </c>
+      <c r="C77" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D77" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E77" s="11">
+        <v>54</v>
+      </c>
+      <c r="F77" s="11">
+        <v>10</v>
+      </c>
+      <c r="G77" s="11">
+        <v>60</v>
+      </c>
+      <c r="H77" s="11">
+        <v>295</v>
+      </c>
+      <c r="I77" s="11">
+        <v>6</v>
+      </c>
+      <c r="J77" s="11">
+        <v>58</v>
+      </c>
+      <c r="K77" s="11">
+        <v>146</v>
+      </c>
+      <c r="L77" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M77" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N77" s="11">
+        <v>7</v>
+      </c>
+      <c r="O77" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P77" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q77" s="13">
+        <v>646</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -16006,13 +16104,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q76"/>
+  <dimension ref="A1:Q77"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B61" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B49" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M77" sqref="M77:M78"/>
+      <selection pane="bottomRight" activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19986,12 +20084,65 @@
         <v>373</v>
       </c>
     </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A77" s="30">
+        <v>43989</v>
+      </c>
+      <c r="B77" s="11">
+        <v>52</v>
+      </c>
+      <c r="C77" s="11">
+        <v>17</v>
+      </c>
+      <c r="D77" s="11">
+        <v>11</v>
+      </c>
+      <c r="E77" s="11">
+        <v>16</v>
+      </c>
+      <c r="F77" s="11">
+        <v>41</v>
+      </c>
+      <c r="G77" s="11">
+        <v>8</v>
+      </c>
+      <c r="H77" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I77" s="11">
+        <v>24</v>
+      </c>
+      <c r="J77" s="11">
+        <v>74</v>
+      </c>
+      <c r="K77" s="11">
+        <v>98</v>
+      </c>
+      <c r="L77" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M77" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N77" s="11">
+        <v>13</v>
+      </c>
+      <c r="O77" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P77" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q77" s="36">
+        <v>356</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXML/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA" version="1.0.0">
   <systemFields>
     <field name="Objective-Id">
@@ -20013,10 +20164,10 @@
       <value order="0">true</value>
     </field>
     <field name="Objective-DatePublished">
-      <value order="0">2020-06-06T11:52:20Z</value>
+      <value order="0">2020-06-07T11:47:42Z</value>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-06T11:52:20Z</value>
+      <value order="0">2020-06-07T11:47:42Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -20031,13 +20182,13 @@
       <value order="0">Published</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41586174</value>
+      <value order="0">vA41590260</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">21.0</value>
+      <value order="0">22.0</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">154</value>
+      <value order="0">157</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>
@@ -20074,7 +20225,7 @@
 </metadata>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXML/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5745109E-2DDF-40CB-AC2B-FF9B10C90820}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-08 20:08)
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u201433\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA1432\A28088333\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Z616594\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA19704\A28088333\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1682" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1707" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -1634,9 +1634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1746,10 +1744,10 @@
   <dimension ref="A1:S160"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B72" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="O96" sqref="B96:O96"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6504,24 +6502,57 @@
         <v>15621</v>
       </c>
     </row>
-    <row r="97" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B97" s="28"/>
-      <c r="C97" s="28"/>
-      <c r="D97" s="28"/>
-      <c r="E97" s="28"/>
-      <c r="F97" s="28"/>
-      <c r="G97" s="28"/>
-      <c r="H97" s="28"/>
-      <c r="I97" s="28"/>
-      <c r="J97" s="28"/>
-      <c r="K97" s="28"/>
-      <c r="L97" s="28"/>
-      <c r="M97" s="28"/>
-      <c r="N97" s="28"/>
-      <c r="O97" s="28"/>
-      <c r="P97" s="28"/>
-    </row>
-    <row r="98" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A97" s="5">
+        <v>43990</v>
+      </c>
+      <c r="B97" s="28">
+        <v>1080</v>
+      </c>
+      <c r="C97" s="28">
+        <v>326</v>
+      </c>
+      <c r="D97" s="28">
+        <v>261</v>
+      </c>
+      <c r="E97" s="28">
+        <v>879</v>
+      </c>
+      <c r="F97" s="28">
+        <v>947</v>
+      </c>
+      <c r="G97" s="28">
+        <v>1286</v>
+      </c>
+      <c r="H97" s="28">
+        <v>3988</v>
+      </c>
+      <c r="I97" s="28">
+        <v>340</v>
+      </c>
+      <c r="J97" s="28">
+        <v>2013</v>
+      </c>
+      <c r="K97" s="28">
+        <v>2774</v>
+      </c>
+      <c r="L97" s="28">
+        <v>8</v>
+      </c>
+      <c r="M97" s="28">
+        <v>54</v>
+      </c>
+      <c r="N97" s="28">
+        <v>1677</v>
+      </c>
+      <c r="O97" s="41">
+        <v>6</v>
+      </c>
+      <c r="P97" s="32">
+        <v>15639</v>
+      </c>
+    </row>
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B98" s="28"/>
       <c r="C98" s="28"/>
       <c r="D98" s="28"/>
@@ -6538,7 +6569,7 @@
       <c r="O98" s="28"/>
       <c r="P98" s="28"/>
     </row>
-    <row r="99" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B99" s="28"/>
       <c r="C99" s="28"/>
       <c r="D99" s="28"/>
@@ -6555,7 +6586,7 @@
       <c r="O99" s="28"/>
       <c r="P99" s="28"/>
     </row>
-    <row r="100" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B100" s="28"/>
       <c r="C100" s="28"/>
       <c r="D100" s="28"/>
@@ -6572,7 +6603,7 @@
       <c r="O100" s="28"/>
       <c r="P100" s="28"/>
     </row>
-    <row r="101" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B101" s="28"/>
       <c r="C101" s="28"/>
       <c r="D101" s="28"/>
@@ -6589,7 +6620,7 @@
       <c r="O101" s="28"/>
       <c r="P101" s="28"/>
     </row>
-    <row r="102" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B102" s="28"/>
       <c r="C102" s="28"/>
       <c r="D102" s="28"/>
@@ -6606,7 +6637,7 @@
       <c r="O102" s="28"/>
       <c r="P102" s="28"/>
     </row>
-    <row r="103" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B103" s="28"/>
       <c r="C103" s="28"/>
       <c r="D103" s="28"/>
@@ -6623,7 +6654,7 @@
       <c r="O103" s="28"/>
       <c r="P103" s="28"/>
     </row>
-    <row r="104" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B104" s="28"/>
       <c r="C104" s="28"/>
       <c r="D104" s="28"/>
@@ -6640,7 +6671,7 @@
       <c r="O104" s="28"/>
       <c r="P104" s="28"/>
     </row>
-    <row r="105" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B105" s="28"/>
       <c r="C105" s="28"/>
       <c r="D105" s="28"/>
@@ -6657,7 +6688,7 @@
       <c r="O105" s="28"/>
       <c r="P105" s="28"/>
     </row>
-    <row r="106" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B106" s="28"/>
       <c r="C106" s="28"/>
       <c r="D106" s="28"/>
@@ -6674,7 +6705,7 @@
       <c r="O106" s="28"/>
       <c r="P106" s="28"/>
     </row>
-    <row r="107" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B107" s="28"/>
       <c r="C107" s="28"/>
       <c r="D107" s="28"/>
@@ -6691,7 +6722,7 @@
       <c r="O107" s="28"/>
       <c r="P107" s="28"/>
     </row>
-    <row r="108" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B108" s="28"/>
       <c r="C108" s="28"/>
       <c r="D108" s="28"/>
@@ -6708,7 +6739,7 @@
       <c r="O108" s="28"/>
       <c r="P108" s="28"/>
     </row>
-    <row r="109" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B109" s="28"/>
       <c r="C109" s="28"/>
       <c r="D109" s="28"/>
@@ -6725,7 +6756,7 @@
       <c r="O109" s="28"/>
       <c r="P109" s="28"/>
     </row>
-    <row r="110" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B110" s="28"/>
       <c r="C110" s="28"/>
       <c r="D110" s="28"/>
@@ -6742,7 +6773,7 @@
       <c r="O110" s="28"/>
       <c r="P110" s="28"/>
     </row>
-    <row r="111" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B111" s="28"/>
       <c r="C111" s="28"/>
       <c r="D111" s="28"/>
@@ -6759,7 +6790,7 @@
       <c r="O111" s="28"/>
       <c r="P111" s="28"/>
     </row>
-    <row r="112" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B112" s="28"/>
       <c r="C112" s="28"/>
       <c r="D112" s="28"/>
@@ -7600,11 +7631,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q85"/>
+  <dimension ref="A1:Q86"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A86" sqref="A86"/>
+      <pane ySplit="3" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12055,6 +12086,59 @@
         <v>25</v>
       </c>
     </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A86" s="30">
+        <v>43990</v>
+      </c>
+      <c r="B86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K86" s="11">
+        <v>6</v>
+      </c>
+      <c r="L86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P86" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q86" s="13">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -12063,13 +12147,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q77"/>
+  <dimension ref="A1:Q78"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A78" sqref="A78"/>
+      <selection pane="bottomRight" activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16096,6 +16180,59 @@
         <v>646</v>
       </c>
     </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A78" s="51">
+        <v>43990</v>
+      </c>
+      <c r="B78" s="11">
+        <v>10</v>
+      </c>
+      <c r="C78" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D78" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E78" s="11">
+        <v>56</v>
+      </c>
+      <c r="F78" s="11">
+        <v>12</v>
+      </c>
+      <c r="G78" s="11">
+        <v>60</v>
+      </c>
+      <c r="H78" s="11">
+        <v>301</v>
+      </c>
+      <c r="I78" s="11">
+        <v>7</v>
+      </c>
+      <c r="J78" s="11">
+        <v>57</v>
+      </c>
+      <c r="K78" s="11">
+        <v>145</v>
+      </c>
+      <c r="L78" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M78" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N78" s="11">
+        <v>7</v>
+      </c>
+      <c r="O78" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P78" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q78" s="13">
+        <v>655</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -16104,13 +16241,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q77"/>
+  <dimension ref="A1:Q78"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B49" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A78" sqref="A78"/>
+      <selection pane="bottomRight" activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20135,6 +20272,59 @@
       </c>
       <c r="Q77" s="36">
         <v>356</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A78" s="30">
+        <v>43990</v>
+      </c>
+      <c r="B78" s="11">
+        <v>39</v>
+      </c>
+      <c r="C78" s="11">
+        <v>20</v>
+      </c>
+      <c r="D78" s="11">
+        <v>8</v>
+      </c>
+      <c r="E78" s="11">
+        <v>11</v>
+      </c>
+      <c r="F78" s="11">
+        <v>29</v>
+      </c>
+      <c r="G78" s="11">
+        <v>10</v>
+      </c>
+      <c r="H78" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I78" s="11">
+        <v>23</v>
+      </c>
+      <c r="J78" s="11">
+        <v>78</v>
+      </c>
+      <c r="K78" s="11">
+        <v>153</v>
+      </c>
+      <c r="L78" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M78" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N78" s="11">
+        <v>13</v>
+      </c>
+      <c r="O78" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P78" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q78" s="13">
+        <v>387</v>
       </c>
     </row>
   </sheetData>
@@ -20161,13 +20351,13 @@
       <value order="0">false</value>
     </field>
     <field name="Objective-IsPublished">
-      <value order="0">true</value>
+      <value order="0">false</value>
     </field>
     <field name="Objective-DatePublished">
-      <value order="0">2020-06-07T11:47:42Z</value>
+      <value order="0"/>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-07T11:47:42Z</value>
+      <value order="0">2020-06-08T12:32:35Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -20179,16 +20369,16 @@
       <value order="0">Analytical: COVID 19 Analysis: Restricted working papers: Research and analysis: Diseases: 2020-2025</value>
     </field>
     <field name="Objective-State">
-      <value order="0">Published</value>
+      <value order="0">Being Drafted</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41590260</value>
+      <value order="0">vA41607398</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">22.0</value>
+      <value order="0">22.2</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">157</value>
+      <value order="0">159</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-08 20:08) (#97)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u201433\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA1432\A28088333\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Z616594\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA19704\A28088333\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1682" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1707" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -1634,9 +1634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1746,10 +1744,10 @@
   <dimension ref="A1:S160"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B72" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="O96" sqref="B96:O96"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6504,24 +6502,57 @@
         <v>15621</v>
       </c>
     </row>
-    <row r="97" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B97" s="28"/>
-      <c r="C97" s="28"/>
-      <c r="D97" s="28"/>
-      <c r="E97" s="28"/>
-      <c r="F97" s="28"/>
-      <c r="G97" s="28"/>
-      <c r="H97" s="28"/>
-      <c r="I97" s="28"/>
-      <c r="J97" s="28"/>
-      <c r="K97" s="28"/>
-      <c r="L97" s="28"/>
-      <c r="M97" s="28"/>
-      <c r="N97" s="28"/>
-      <c r="O97" s="28"/>
-      <c r="P97" s="28"/>
-    </row>
-    <row r="98" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A97" s="5">
+        <v>43990</v>
+      </c>
+      <c r="B97" s="28">
+        <v>1080</v>
+      </c>
+      <c r="C97" s="28">
+        <v>326</v>
+      </c>
+      <c r="D97" s="28">
+        <v>261</v>
+      </c>
+      <c r="E97" s="28">
+        <v>879</v>
+      </c>
+      <c r="F97" s="28">
+        <v>947</v>
+      </c>
+      <c r="G97" s="28">
+        <v>1286</v>
+      </c>
+      <c r="H97" s="28">
+        <v>3988</v>
+      </c>
+      <c r="I97" s="28">
+        <v>340</v>
+      </c>
+      <c r="J97" s="28">
+        <v>2013</v>
+      </c>
+      <c r="K97" s="28">
+        <v>2774</v>
+      </c>
+      <c r="L97" s="28">
+        <v>8</v>
+      </c>
+      <c r="M97" s="28">
+        <v>54</v>
+      </c>
+      <c r="N97" s="28">
+        <v>1677</v>
+      </c>
+      <c r="O97" s="41">
+        <v>6</v>
+      </c>
+      <c r="P97" s="32">
+        <v>15639</v>
+      </c>
+    </row>
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B98" s="28"/>
       <c r="C98" s="28"/>
       <c r="D98" s="28"/>
@@ -6538,7 +6569,7 @@
       <c r="O98" s="28"/>
       <c r="P98" s="28"/>
     </row>
-    <row r="99" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B99" s="28"/>
       <c r="C99" s="28"/>
       <c r="D99" s="28"/>
@@ -6555,7 +6586,7 @@
       <c r="O99" s="28"/>
       <c r="P99" s="28"/>
     </row>
-    <row r="100" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B100" s="28"/>
       <c r="C100" s="28"/>
       <c r="D100" s="28"/>
@@ -6572,7 +6603,7 @@
       <c r="O100" s="28"/>
       <c r="P100" s="28"/>
     </row>
-    <row r="101" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B101" s="28"/>
       <c r="C101" s="28"/>
       <c r="D101" s="28"/>
@@ -6589,7 +6620,7 @@
       <c r="O101" s="28"/>
       <c r="P101" s="28"/>
     </row>
-    <row r="102" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B102" s="28"/>
       <c r="C102" s="28"/>
       <c r="D102" s="28"/>
@@ -6606,7 +6637,7 @@
       <c r="O102" s="28"/>
       <c r="P102" s="28"/>
     </row>
-    <row r="103" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B103" s="28"/>
       <c r="C103" s="28"/>
       <c r="D103" s="28"/>
@@ -6623,7 +6654,7 @@
       <c r="O103" s="28"/>
       <c r="P103" s="28"/>
     </row>
-    <row r="104" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B104" s="28"/>
       <c r="C104" s="28"/>
       <c r="D104" s="28"/>
@@ -6640,7 +6671,7 @@
       <c r="O104" s="28"/>
       <c r="P104" s="28"/>
     </row>
-    <row r="105" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B105" s="28"/>
       <c r="C105" s="28"/>
       <c r="D105" s="28"/>
@@ -6657,7 +6688,7 @@
       <c r="O105" s="28"/>
       <c r="P105" s="28"/>
     </row>
-    <row r="106" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B106" s="28"/>
       <c r="C106" s="28"/>
       <c r="D106" s="28"/>
@@ -6674,7 +6705,7 @@
       <c r="O106" s="28"/>
       <c r="P106" s="28"/>
     </row>
-    <row r="107" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B107" s="28"/>
       <c r="C107" s="28"/>
       <c r="D107" s="28"/>
@@ -6691,7 +6722,7 @@
       <c r="O107" s="28"/>
       <c r="P107" s="28"/>
     </row>
-    <row r="108" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B108" s="28"/>
       <c r="C108" s="28"/>
       <c r="D108" s="28"/>
@@ -6708,7 +6739,7 @@
       <c r="O108" s="28"/>
       <c r="P108" s="28"/>
     </row>
-    <row r="109" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B109" s="28"/>
       <c r="C109" s="28"/>
       <c r="D109" s="28"/>
@@ -6725,7 +6756,7 @@
       <c r="O109" s="28"/>
       <c r="P109" s="28"/>
     </row>
-    <row r="110" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B110" s="28"/>
       <c r="C110" s="28"/>
       <c r="D110" s="28"/>
@@ -6742,7 +6773,7 @@
       <c r="O110" s="28"/>
       <c r="P110" s="28"/>
     </row>
-    <row r="111" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B111" s="28"/>
       <c r="C111" s="28"/>
       <c r="D111" s="28"/>
@@ -6759,7 +6790,7 @@
       <c r="O111" s="28"/>
       <c r="P111" s="28"/>
     </row>
-    <row r="112" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B112" s="28"/>
       <c r="C112" s="28"/>
       <c r="D112" s="28"/>
@@ -7600,11 +7631,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q85"/>
+  <dimension ref="A1:Q86"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A86" sqref="A86"/>
+      <pane ySplit="3" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12055,6 +12086,59 @@
         <v>25</v>
       </c>
     </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A86" s="30">
+        <v>43990</v>
+      </c>
+      <c r="B86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K86" s="11">
+        <v>6</v>
+      </c>
+      <c r="L86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P86" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q86" s="13">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -12063,13 +12147,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q77"/>
+  <dimension ref="A1:Q78"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A78" sqref="A78"/>
+      <selection pane="bottomRight" activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16096,6 +16180,59 @@
         <v>646</v>
       </c>
     </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A78" s="51">
+        <v>43990</v>
+      </c>
+      <c r="B78" s="11">
+        <v>10</v>
+      </c>
+      <c r="C78" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D78" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E78" s="11">
+        <v>56</v>
+      </c>
+      <c r="F78" s="11">
+        <v>12</v>
+      </c>
+      <c r="G78" s="11">
+        <v>60</v>
+      </c>
+      <c r="H78" s="11">
+        <v>301</v>
+      </c>
+      <c r="I78" s="11">
+        <v>7</v>
+      </c>
+      <c r="J78" s="11">
+        <v>57</v>
+      </c>
+      <c r="K78" s="11">
+        <v>145</v>
+      </c>
+      <c r="L78" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M78" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N78" s="11">
+        <v>7</v>
+      </c>
+      <c r="O78" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P78" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q78" s="13">
+        <v>655</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -16104,13 +16241,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q77"/>
+  <dimension ref="A1:Q78"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B49" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A78" sqref="A78"/>
+      <selection pane="bottomRight" activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20135,6 +20272,59 @@
       </c>
       <c r="Q77" s="36">
         <v>356</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A78" s="30">
+        <v>43990</v>
+      </c>
+      <c r="B78" s="11">
+        <v>39</v>
+      </c>
+      <c r="C78" s="11">
+        <v>20</v>
+      </c>
+      <c r="D78" s="11">
+        <v>8</v>
+      </c>
+      <c r="E78" s="11">
+        <v>11</v>
+      </c>
+      <c r="F78" s="11">
+        <v>29</v>
+      </c>
+      <c r="G78" s="11">
+        <v>10</v>
+      </c>
+      <c r="H78" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I78" s="11">
+        <v>23</v>
+      </c>
+      <c r="J78" s="11">
+        <v>78</v>
+      </c>
+      <c r="K78" s="11">
+        <v>153</v>
+      </c>
+      <c r="L78" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M78" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N78" s="11">
+        <v>13</v>
+      </c>
+      <c r="O78" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P78" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q78" s="13">
+        <v>387</v>
       </c>
     </row>
   </sheetData>
@@ -20161,13 +20351,13 @@
       <value order="0">false</value>
     </field>
     <field name="Objective-IsPublished">
-      <value order="0">true</value>
+      <value order="0">false</value>
     </field>
     <field name="Objective-DatePublished">
-      <value order="0">2020-06-07T11:47:42Z</value>
+      <value order="0"/>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-07T11:47:42Z</value>
+      <value order="0">2020-06-08T12:32:35Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -20179,16 +20369,16 @@
       <value order="0">Analytical: COVID 19 Analysis: Restricted working papers: Research and analysis: Diseases: 2020-2025</value>
     </field>
     <field name="Objective-State">
-      <value order="0">Published</value>
+      <value order="0">Being Drafted</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41590260</value>
+      <value order="0">vA41607398</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">22.0</value>
+      <value order="0">22.2</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">157</value>
+      <value order="0">159</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-09 20:09)
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Z616594\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA19704\A28088333\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U445783\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA18464\A28088333\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5985" windowHeight="6030" tabRatio="803"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5988" windowHeight="6036" tabRatio="803" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1707" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1732" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -1634,23 +1634,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="90.42578125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.42578125" style="2"/>
+    <col min="2" max="2" width="29.44140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="90.44140625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" s="18" t="s">
         <v>20</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20" t="s">
         <v>22</v>
       </c>
@@ -1666,13 +1666,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="22" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="23"/>
     </row>
-    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="24" t="s">
         <v>26</v>
       </c>
@@ -1680,7 +1680,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="24" t="s">
         <v>27</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="24" t="s">
         <v>36</v>
       </c>
@@ -1696,7 +1696,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="20" t="s">
         <v>37</v>
       </c>
@@ -1724,12 +1724,12 @@
       <selection activeCell="K66" sqref="K66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.42578125" style="2"/>
+    <col min="1" max="16384" width="9.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" ht="15" x14ac:dyDescent="0.3">
       <c r="A44" s="43"/>
     </row>
   </sheetData>
@@ -1743,21 +1743,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S160"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="64" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B88" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="R93" sqref="R93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" style="2" customWidth="1"/>
-    <col min="2" max="16" width="11.42578125" style="11" customWidth="1"/>
-    <col min="17" max="16384" width="8.5703125" style="2"/>
+    <col min="2" max="16" width="11.44140625" style="11" customWidth="1"/>
+    <col min="17" max="16384" width="8.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -1777,7 +1777,7 @@
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -1796,7 +1796,7 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>43897</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>43898</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>43899</v>
       </c>
@@ -1996,7 +1996,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>43900</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>43901</v>
       </c>
@@ -2096,7 +2096,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>43902</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>43903</v>
       </c>
@@ -2196,7 +2196,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>43904</v>
       </c>
@@ -2246,7 +2246,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>43905</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>43906</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>43907</v>
       </c>
@@ -2396,7 +2396,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>43908</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>43909</v>
       </c>
@@ -2496,7 +2496,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>43910</v>
       </c>
@@ -2546,7 +2546,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>43911</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>43912</v>
       </c>
@@ -2646,7 +2646,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>43913</v>
       </c>
@@ -2696,7 +2696,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>43914</v>
       </c>
@@ -2746,7 +2746,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>43915</v>
       </c>
@@ -2796,7 +2796,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>43916</v>
       </c>
@@ -2846,7 +2846,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>43917</v>
       </c>
@@ -2896,7 +2896,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>43918</v>
       </c>
@@ -2946,7 +2946,7 @@
         <v>1264</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>43919</v>
       </c>
@@ -2996,7 +2996,7 @@
         <v>1417</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>43920</v>
       </c>
@@ -3046,7 +3046,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>43921</v>
       </c>
@@ -3096,7 +3096,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>43922</v>
       </c>
@@ -3146,7 +3146,7 @@
         <v>2310</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>43923</v>
       </c>
@@ -3196,7 +3196,7 @@
         <v>2602</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <v>43924</v>
       </c>
@@ -3246,7 +3246,7 @@
         <v>3001</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>43925</v>
       </c>
@@ -3296,7 +3296,7 @@
         <v>3345</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
         <v>43926</v>
       </c>
@@ -3346,7 +3346,7 @@
         <v>3706</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
         <v>43927</v>
       </c>
@@ -3396,7 +3396,7 @@
         <v>3961</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
         <v>43928</v>
       </c>
@@ -3446,7 +3446,7 @@
         <v>4229</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>43929</v>
       </c>
@@ -3496,7 +3496,7 @@
         <v>4565</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
         <v>43930</v>
       </c>
@@ -3546,7 +3546,7 @@
         <v>4957</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
         <v>43931</v>
       </c>
@@ -3596,7 +3596,7 @@
         <v>5275</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>43932</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>5590</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
         <v>43933</v>
       </c>
@@ -3696,7 +3696,7 @@
         <v>5912</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
         <v>43934</v>
       </c>
@@ -3746,7 +3746,7 @@
         <v>6067</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>43935</v>
       </c>
@@ -3796,7 +3796,7 @@
         <v>6358</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
         <v>43936</v>
       </c>
@@ -3846,7 +3846,7 @@
         <v>6748</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" s="5">
         <v>43937</v>
       </c>
@@ -3896,7 +3896,7 @@
         <v>7102</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
         <v>43938</v>
       </c>
@@ -3946,7 +3946,7 @@
         <v>7409</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" s="5">
         <v>43939</v>
       </c>
@@ -3996,7 +3996,7 @@
         <v>7820</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" s="5">
         <v>43940</v>
       </c>
@@ -4046,7 +4046,7 @@
         <v>8187</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
         <v>43941</v>
       </c>
@@ -4096,7 +4096,7 @@
         <v>8450</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A49" s="5">
         <v>43942</v>
       </c>
@@ -4146,7 +4146,7 @@
         <v>8672</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
         <v>43943</v>
       </c>
@@ -4196,7 +4196,7 @@
         <v>9038</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A51" s="5">
         <v>43944</v>
       </c>
@@ -4246,7 +4246,7 @@
         <v>9409</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A52" s="5">
         <v>43945</v>
       </c>
@@ -4296,7 +4296,7 @@
         <v>9697</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A53" s="5">
         <v>43946</v>
       </c>
@@ -4346,7 +4346,7 @@
         <v>10051</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A54" s="5">
         <v>43947</v>
       </c>
@@ -4397,7 +4397,7 @@
       </c>
       <c r="R54" s="38"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A55" s="5">
         <v>43948</v>
       </c>
@@ -4448,7 +4448,7 @@
       </c>
       <c r="R55" s="38"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A56" s="5">
         <v>43949</v>
       </c>
@@ -4499,7 +4499,7 @@
       </c>
       <c r="R56" s="39"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A57" s="5">
         <v>43950</v>
       </c>
@@ -4549,7 +4549,7 @@
         <v>11034</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A58" s="5">
         <v>43951</v>
       </c>
@@ -4600,7 +4600,7 @@
       </c>
       <c r="R58" s="38"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A59" s="5">
         <v>43952</v>
       </c>
@@ -4652,7 +4652,7 @@
       <c r="R59" s="38"/>
       <c r="S59" s="38"/>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A60" s="5">
         <v>43953</v>
       </c>
@@ -4702,7 +4702,7 @@
         <v>11927</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A61" s="5">
         <v>43954</v>
       </c>
@@ -4752,7 +4752,7 @@
         <v>12097</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A62" s="5">
         <v>43955</v>
       </c>
@@ -4802,7 +4802,7 @@
         <v>12266</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A63" s="5">
         <v>43956</v>
       </c>
@@ -4852,7 +4852,7 @@
         <v>12437</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A64" s="5">
         <v>43957</v>
       </c>
@@ -4902,7 +4902,7 @@
         <v>12709</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65" s="5">
         <v>43958</v>
       </c>
@@ -4952,7 +4952,7 @@
         <v>12924</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66" s="5">
         <v>43959</v>
       </c>
@@ -5002,7 +5002,7 @@
         <v>13149</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A67" s="5">
         <v>43960</v>
       </c>
@@ -5052,7 +5052,7 @@
         <v>13305</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A68" s="5">
         <v>43961</v>
       </c>
@@ -5102,7 +5102,7 @@
         <v>13486</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A69" s="5">
         <v>43962</v>
       </c>
@@ -5152,7 +5152,7 @@
         <v>13627</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A70" s="5">
         <v>43963</v>
       </c>
@@ -5202,7 +5202,7 @@
         <v>13763</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A71" s="5">
         <v>43964</v>
       </c>
@@ -5252,7 +5252,7 @@
         <v>13929</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A72" s="5">
         <v>43965</v>
       </c>
@@ -5302,7 +5302,7 @@
         <v>14117</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A73" s="5">
         <v>43966</v>
       </c>
@@ -5352,7 +5352,7 @@
         <v>14260</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A74" s="5">
         <v>43967</v>
       </c>
@@ -5402,7 +5402,7 @@
         <v>14447</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A75" s="5">
         <v>43968</v>
       </c>
@@ -5452,7 +5452,7 @@
         <v>14537</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A76" s="5">
         <v>43969</v>
       </c>
@@ -5502,7 +5502,7 @@
         <v>14594</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A77" s="5">
         <v>43970</v>
       </c>
@@ -5552,7 +5552,7 @@
         <v>14655</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A78" s="5">
         <v>43971</v>
       </c>
@@ -5602,7 +5602,7 @@
         <v>14751</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A79" s="5">
         <v>43972</v>
       </c>
@@ -5652,7 +5652,7 @@
         <v>14856</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A80" s="5">
         <v>43973</v>
       </c>
@@ -5702,7 +5702,7 @@
         <v>14969</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A81" s="5">
         <v>43974</v>
       </c>
@@ -5752,7 +5752,7 @@
         <v>15041</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A82" s="5">
         <v>43975</v>
       </c>
@@ -5802,7 +5802,7 @@
         <v>15101</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A83" s="5">
         <v>43976</v>
       </c>
@@ -5852,7 +5852,7 @@
         <v>15156</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A84" s="5">
         <v>43977</v>
       </c>
@@ -5902,7 +5902,7 @@
         <v>15185</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A85" s="5">
         <v>43978</v>
       </c>
@@ -5952,7 +5952,7 @@
         <v>15240</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A86" s="5">
         <v>43979</v>
       </c>
@@ -6002,7 +6002,7 @@
         <v>15288</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A87" s="5">
         <v>43980</v>
       </c>
@@ -6052,7 +6052,7 @@
         <v>15327</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A88" s="5">
         <v>43981</v>
       </c>
@@ -6102,7 +6102,7 @@
         <v>15382</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A89" s="5">
         <v>43982</v>
       </c>
@@ -6152,7 +6152,7 @@
         <v>15400</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A90" s="5">
         <v>43983</v>
       </c>
@@ -6202,7 +6202,7 @@
         <v>15418</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A91" s="5">
         <v>43984</v>
       </c>
@@ -6252,7 +6252,7 @@
         <v>15471</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A92" s="5">
         <v>43985</v>
       </c>
@@ -6302,7 +6302,7 @@
         <v>15504</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A93" s="5">
         <v>43986</v>
       </c>
@@ -6352,7 +6352,7 @@
         <v>15553</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A94" s="5">
         <v>43987</v>
       </c>
@@ -6402,7 +6402,7 @@
         <v>15582</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A95" s="5">
         <v>43988</v>
       </c>
@@ -6452,7 +6452,7 @@
         <v>15603</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A96" s="5">
         <v>43989</v>
       </c>
@@ -6502,7 +6502,7 @@
         <v>15621</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A97" s="5">
         <v>43990</v>
       </c>
@@ -6552,25 +6552,57 @@
         <v>15639</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B98" s="28"/>
-      <c r="C98" s="28"/>
-      <c r="D98" s="28"/>
-      <c r="E98" s="28"/>
-      <c r="F98" s="28"/>
-      <c r="G98" s="28"/>
-      <c r="H98" s="28"/>
-      <c r="I98" s="28"/>
-      <c r="J98" s="28"/>
-      <c r="K98" s="28"/>
-      <c r="L98" s="28"/>
-      <c r="M98" s="28"/>
-      <c r="N98" s="28"/>
-      <c r="O98" s="28"/>
-      <c r="P98" s="28"/>
-    </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B99" s="28"/>
+    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A98" s="5">
+        <v>43991</v>
+      </c>
+      <c r="B98" s="28">
+        <v>1081</v>
+      </c>
+      <c r="C98" s="28">
+        <v>326</v>
+      </c>
+      <c r="D98" s="28">
+        <v>261</v>
+      </c>
+      <c r="E98" s="28">
+        <v>879</v>
+      </c>
+      <c r="F98" s="28">
+        <v>948</v>
+      </c>
+      <c r="G98" s="28">
+        <v>1287</v>
+      </c>
+      <c r="H98" s="28">
+        <v>3990</v>
+      </c>
+      <c r="I98" s="28">
+        <v>340</v>
+      </c>
+      <c r="J98" s="28">
+        <v>2018</v>
+      </c>
+      <c r="K98" s="28">
+        <v>2777</v>
+      </c>
+      <c r="L98" s="28">
+        <v>8</v>
+      </c>
+      <c r="M98" s="28">
+        <v>54</v>
+      </c>
+      <c r="N98" s="28">
+        <v>1678</v>
+      </c>
+      <c r="O98" s="28">
+        <v>6</v>
+      </c>
+      <c r="P98" s="32">
+        <v>15653</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C99" s="28"/>
       <c r="D99" s="28"/>
       <c r="E99" s="28"/>
@@ -6586,8 +6618,7 @@
       <c r="O99" s="28"/>
       <c r="P99" s="28"/>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B100" s="28"/>
+    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C100" s="28"/>
       <c r="D100" s="28"/>
       <c r="E100" s="28"/>
@@ -6603,8 +6634,7 @@
       <c r="O100" s="28"/>
       <c r="P100" s="28"/>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B101" s="28"/>
+    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C101" s="28"/>
       <c r="D101" s="28"/>
       <c r="E101" s="28"/>
@@ -6620,8 +6650,7 @@
       <c r="O101" s="28"/>
       <c r="P101" s="28"/>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B102" s="28"/>
+    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C102" s="28"/>
       <c r="D102" s="28"/>
       <c r="E102" s="28"/>
@@ -6637,8 +6666,7 @@
       <c r="O102" s="28"/>
       <c r="P102" s="28"/>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B103" s="28"/>
+    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C103" s="28"/>
       <c r="D103" s="28"/>
       <c r="E103" s="28"/>
@@ -6654,8 +6682,7 @@
       <c r="O103" s="28"/>
       <c r="P103" s="28"/>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B104" s="28"/>
+    <row r="104" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C104" s="28"/>
       <c r="D104" s="28"/>
       <c r="E104" s="28"/>
@@ -6671,8 +6698,7 @@
       <c r="O104" s="28"/>
       <c r="P104" s="28"/>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B105" s="28"/>
+    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C105" s="28"/>
       <c r="D105" s="28"/>
       <c r="E105" s="28"/>
@@ -6688,8 +6714,7 @@
       <c r="O105" s="28"/>
       <c r="P105" s="28"/>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B106" s="28"/>
+    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C106" s="28"/>
       <c r="D106" s="28"/>
       <c r="E106" s="28"/>
@@ -6705,8 +6730,7 @@
       <c r="O106" s="28"/>
       <c r="P106" s="28"/>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B107" s="28"/>
+    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C107" s="28"/>
       <c r="D107" s="28"/>
       <c r="E107" s="28"/>
@@ -6722,8 +6746,7 @@
       <c r="O107" s="28"/>
       <c r="P107" s="28"/>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B108" s="28"/>
+    <row r="108" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C108" s="28"/>
       <c r="D108" s="28"/>
       <c r="E108" s="28"/>
@@ -6739,8 +6762,7 @@
       <c r="O108" s="28"/>
       <c r="P108" s="28"/>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B109" s="28"/>
+    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C109" s="28"/>
       <c r="D109" s="28"/>
       <c r="E109" s="28"/>
@@ -6756,8 +6778,7 @@
       <c r="O109" s="28"/>
       <c r="P109" s="28"/>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B110" s="28"/>
+    <row r="110" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C110" s="28"/>
       <c r="D110" s="28"/>
       <c r="E110" s="28"/>
@@ -6773,8 +6794,7 @@
       <c r="O110" s="28"/>
       <c r="P110" s="28"/>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B111" s="28"/>
+    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C111" s="28"/>
       <c r="D111" s="28"/>
       <c r="E111" s="28"/>
@@ -6790,8 +6810,7 @@
       <c r="O111" s="28"/>
       <c r="P111" s="28"/>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B112" s="28"/>
+    <row r="112" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C112" s="28"/>
       <c r="D112" s="28"/>
       <c r="E112" s="28"/>
@@ -6807,8 +6826,7 @@
       <c r="O112" s="28"/>
       <c r="P112" s="28"/>
     </row>
-    <row r="113" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B113" s="28"/>
+    <row r="113" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C113" s="28"/>
       <c r="D113" s="28"/>
       <c r="E113" s="28"/>
@@ -6824,8 +6842,7 @@
       <c r="O113" s="28"/>
       <c r="P113" s="28"/>
     </row>
-    <row r="114" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B114" s="28"/>
+    <row r="114" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C114" s="28"/>
       <c r="D114" s="28"/>
       <c r="E114" s="28"/>
@@ -6841,7 +6858,7 @@
       <c r="O114" s="28"/>
       <c r="P114" s="28"/>
     </row>
-    <row r="115" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B115" s="28"/>
       <c r="C115" s="28"/>
       <c r="D115" s="28"/>
@@ -6858,7 +6875,7 @@
       <c r="O115" s="28"/>
       <c r="P115" s="28"/>
     </row>
-    <row r="116" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B116" s="28"/>
       <c r="C116" s="28"/>
       <c r="D116" s="28"/>
@@ -6875,7 +6892,7 @@
       <c r="O116" s="28"/>
       <c r="P116" s="28"/>
     </row>
-    <row r="117" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B117" s="28"/>
       <c r="C117" s="28"/>
       <c r="D117" s="28"/>
@@ -6892,7 +6909,7 @@
       <c r="O117" s="28"/>
       <c r="P117" s="28"/>
     </row>
-    <row r="118" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B118" s="28"/>
       <c r="C118" s="28"/>
       <c r="D118" s="28"/>
@@ -6909,7 +6926,7 @@
       <c r="O118" s="28"/>
       <c r="P118" s="28"/>
     </row>
-    <row r="119" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B119" s="28"/>
       <c r="C119" s="28"/>
       <c r="D119" s="28"/>
@@ -6926,7 +6943,7 @@
       <c r="O119" s="28"/>
       <c r="P119" s="28"/>
     </row>
-    <row r="120" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B120" s="28"/>
       <c r="C120" s="28"/>
       <c r="D120" s="28"/>
@@ -6943,7 +6960,7 @@
       <c r="O120" s="28"/>
       <c r="P120" s="28"/>
     </row>
-    <row r="121" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B121" s="28"/>
       <c r="C121" s="28"/>
       <c r="D121" s="28"/>
@@ -6960,7 +6977,7 @@
       <c r="O121" s="28"/>
       <c r="P121" s="28"/>
     </row>
-    <row r="122" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B122" s="28"/>
       <c r="C122" s="28"/>
       <c r="D122" s="28"/>
@@ -6977,7 +6994,7 @@
       <c r="O122" s="28"/>
       <c r="P122" s="28"/>
     </row>
-    <row r="123" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B123" s="28"/>
       <c r="C123" s="28"/>
       <c r="D123" s="28"/>
@@ -6994,7 +7011,7 @@
       <c r="O123" s="28"/>
       <c r="P123" s="28"/>
     </row>
-    <row r="124" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B124" s="28"/>
       <c r="C124" s="28"/>
       <c r="D124" s="28"/>
@@ -7011,7 +7028,7 @@
       <c r="O124" s="28"/>
       <c r="P124" s="28"/>
     </row>
-    <row r="125" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B125" s="28"/>
       <c r="C125" s="28"/>
       <c r="D125" s="28"/>
@@ -7028,7 +7045,7 @@
       <c r="O125" s="28"/>
       <c r="P125" s="28"/>
     </row>
-    <row r="126" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B126" s="28"/>
       <c r="C126" s="28"/>
       <c r="D126" s="28"/>
@@ -7045,7 +7062,7 @@
       <c r="O126" s="28"/>
       <c r="P126" s="28"/>
     </row>
-    <row r="127" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B127" s="28"/>
       <c r="C127" s="28"/>
       <c r="D127" s="28"/>
@@ -7062,7 +7079,7 @@
       <c r="O127" s="28"/>
       <c r="P127" s="28"/>
     </row>
-    <row r="128" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B128" s="28"/>
       <c r="C128" s="28"/>
       <c r="D128" s="28"/>
@@ -7079,7 +7096,7 @@
       <c r="O128" s="28"/>
       <c r="P128" s="28"/>
     </row>
-    <row r="129" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B129" s="28"/>
       <c r="C129" s="28"/>
       <c r="D129" s="28"/>
@@ -7096,7 +7113,7 @@
       <c r="O129" s="28"/>
       <c r="P129" s="28"/>
     </row>
-    <row r="130" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B130" s="28"/>
       <c r="C130" s="28"/>
       <c r="D130" s="28"/>
@@ -7113,7 +7130,7 @@
       <c r="O130" s="28"/>
       <c r="P130" s="28"/>
     </row>
-    <row r="131" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B131" s="28"/>
       <c r="C131" s="28"/>
       <c r="D131" s="28"/>
@@ -7130,7 +7147,7 @@
       <c r="O131" s="28"/>
       <c r="P131" s="28"/>
     </row>
-    <row r="132" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B132" s="28"/>
       <c r="C132" s="28"/>
       <c r="D132" s="28"/>
@@ -7147,7 +7164,7 @@
       <c r="O132" s="28"/>
       <c r="P132" s="28"/>
     </row>
-    <row r="133" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B133" s="28"/>
       <c r="C133" s="28"/>
       <c r="D133" s="28"/>
@@ -7164,7 +7181,7 @@
       <c r="O133" s="28"/>
       <c r="P133" s="28"/>
     </row>
-    <row r="134" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B134" s="28"/>
       <c r="C134" s="28"/>
       <c r="D134" s="28"/>
@@ -7181,7 +7198,7 @@
       <c r="O134" s="28"/>
       <c r="P134" s="28"/>
     </row>
-    <row r="135" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B135" s="28"/>
       <c r="C135" s="28"/>
       <c r="D135" s="28"/>
@@ -7198,7 +7215,7 @@
       <c r="O135" s="28"/>
       <c r="P135" s="28"/>
     </row>
-    <row r="136" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B136" s="28"/>
       <c r="C136" s="28"/>
       <c r="D136" s="28"/>
@@ -7215,7 +7232,7 @@
       <c r="O136" s="28"/>
       <c r="P136" s="28"/>
     </row>
-    <row r="137" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B137" s="28"/>
       <c r="C137" s="28"/>
       <c r="D137" s="28"/>
@@ -7232,7 +7249,7 @@
       <c r="O137" s="28"/>
       <c r="P137" s="28"/>
     </row>
-    <row r="138" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B138" s="28"/>
       <c r="C138" s="28"/>
       <c r="D138" s="28"/>
@@ -7249,7 +7266,7 @@
       <c r="O138" s="28"/>
       <c r="P138" s="28"/>
     </row>
-    <row r="139" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B139" s="28"/>
       <c r="C139" s="28"/>
       <c r="D139" s="28"/>
@@ -7266,7 +7283,7 @@
       <c r="O139" s="28"/>
       <c r="P139" s="28"/>
     </row>
-    <row r="140" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B140" s="28"/>
       <c r="C140" s="28"/>
       <c r="D140" s="28"/>
@@ -7283,7 +7300,7 @@
       <c r="O140" s="28"/>
       <c r="P140" s="28"/>
     </row>
-    <row r="141" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B141" s="28"/>
       <c r="C141" s="28"/>
       <c r="D141" s="28"/>
@@ -7300,7 +7317,7 @@
       <c r="O141" s="28"/>
       <c r="P141" s="28"/>
     </row>
-    <row r="142" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B142" s="28"/>
       <c r="C142" s="28"/>
       <c r="D142" s="28"/>
@@ -7317,7 +7334,7 @@
       <c r="O142" s="28"/>
       <c r="P142" s="28"/>
     </row>
-    <row r="143" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B143" s="28"/>
       <c r="C143" s="28"/>
       <c r="D143" s="28"/>
@@ -7334,7 +7351,7 @@
       <c r="O143" s="28"/>
       <c r="P143" s="28"/>
     </row>
-    <row r="144" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B144" s="28"/>
       <c r="C144" s="28"/>
       <c r="D144" s="28"/>
@@ -7351,7 +7368,7 @@
       <c r="O144" s="28"/>
       <c r="P144" s="28"/>
     </row>
-    <row r="145" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B145" s="28"/>
       <c r="C145" s="28"/>
       <c r="D145" s="28"/>
@@ -7368,7 +7385,7 @@
       <c r="O145" s="28"/>
       <c r="P145" s="28"/>
     </row>
-    <row r="146" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B146" s="28"/>
       <c r="C146" s="28"/>
       <c r="D146" s="28"/>
@@ -7385,7 +7402,7 @@
       <c r="O146" s="28"/>
       <c r="P146" s="28"/>
     </row>
-    <row r="147" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B147" s="28"/>
       <c r="C147" s="28"/>
       <c r="D147" s="28"/>
@@ -7402,7 +7419,7 @@
       <c r="O147" s="28"/>
       <c r="P147" s="28"/>
     </row>
-    <row r="148" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B148" s="28"/>
       <c r="C148" s="28"/>
       <c r="D148" s="28"/>
@@ -7419,7 +7436,7 @@
       <c r="O148" s="28"/>
       <c r="P148" s="28"/>
     </row>
-    <row r="149" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B149" s="28"/>
       <c r="C149" s="28"/>
       <c r="D149" s="28"/>
@@ -7436,7 +7453,7 @@
       <c r="O149" s="28"/>
       <c r="P149" s="28"/>
     </row>
-    <row r="150" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B150" s="28"/>
       <c r="C150" s="28"/>
       <c r="D150" s="28"/>
@@ -7453,7 +7470,7 @@
       <c r="O150" s="28"/>
       <c r="P150" s="28"/>
     </row>
-    <row r="151" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B151" s="28"/>
       <c r="C151" s="28"/>
       <c r="D151" s="28"/>
@@ -7470,7 +7487,7 @@
       <c r="O151" s="28"/>
       <c r="P151" s="28"/>
     </row>
-    <row r="152" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B152" s="28"/>
       <c r="C152" s="28"/>
       <c r="D152" s="28"/>
@@ -7487,7 +7504,7 @@
       <c r="O152" s="28"/>
       <c r="P152" s="28"/>
     </row>
-    <row r="153" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B153" s="28"/>
       <c r="C153" s="28"/>
       <c r="D153" s="28"/>
@@ -7504,7 +7521,7 @@
       <c r="O153" s="28"/>
       <c r="P153" s="28"/>
     </row>
-    <row r="154" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B154" s="28"/>
       <c r="C154" s="28"/>
       <c r="D154" s="28"/>
@@ -7521,7 +7538,7 @@
       <c r="O154" s="28"/>
       <c r="P154" s="28"/>
     </row>
-    <row r="155" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B155" s="28"/>
       <c r="C155" s="28"/>
       <c r="D155" s="28"/>
@@ -7538,7 +7555,7 @@
       <c r="O155" s="28"/>
       <c r="P155" s="28"/>
     </row>
-    <row r="156" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B156" s="28"/>
       <c r="C156" s="28"/>
       <c r="D156" s="28"/>
@@ -7555,7 +7572,7 @@
       <c r="O156" s="28"/>
       <c r="P156" s="28"/>
     </row>
-    <row r="157" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B157" s="28"/>
       <c r="C157" s="28"/>
       <c r="D157" s="28"/>
@@ -7572,7 +7589,7 @@
       <c r="O157" s="28"/>
       <c r="P157" s="28"/>
     </row>
-    <row r="158" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B158" s="28"/>
       <c r="C158" s="28"/>
       <c r="D158" s="28"/>
@@ -7589,7 +7606,7 @@
       <c r="O158" s="28"/>
       <c r="P158" s="28"/>
     </row>
-    <row r="159" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B159" s="28"/>
       <c r="C159" s="28"/>
       <c r="D159" s="28"/>
@@ -7606,7 +7623,7 @@
       <c r="O159" s="28"/>
       <c r="P159" s="28"/>
     </row>
-    <row r="160" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B160" s="28"/>
       <c r="C160" s="28"/>
       <c r="D160" s="28"/>
@@ -7631,21 +7648,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q86"/>
+  <dimension ref="A1:Q87"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5703125" style="2"/>
+    <col min="1" max="1" width="12.44140625" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.5546875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -7666,7 +7683,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -7687,7 +7704,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -7740,7 +7757,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>43908</v>
       </c>
@@ -7793,7 +7810,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>43909</v>
       </c>
@@ -7846,7 +7863,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>43910</v>
       </c>
@@ -7899,7 +7916,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>43911</v>
       </c>
@@ -7952,7 +7969,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>43912</v>
       </c>
@@ -8005,7 +8022,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>43913</v>
       </c>
@@ -8058,7 +8075,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>43914</v>
       </c>
@@ -8111,7 +8128,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>43915</v>
       </c>
@@ -8164,7 +8181,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
         <v>43916</v>
       </c>
@@ -8217,7 +8234,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>43917</v>
       </c>
@@ -8270,7 +8287,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>43918</v>
       </c>
@@ -8323,7 +8340,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>43919</v>
       </c>
@@ -8376,7 +8393,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>43920</v>
       </c>
@@ -8429,7 +8446,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>43921</v>
       </c>
@@ -8482,7 +8499,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>43922</v>
       </c>
@@ -8535,7 +8552,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>43923</v>
       </c>
@@ -8588,7 +8605,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>43924</v>
       </c>
@@ -8641,7 +8658,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>43925</v>
       </c>
@@ -8694,7 +8711,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="12">
         <v>43926</v>
       </c>
@@ -8747,7 +8764,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="12">
         <v>43927</v>
       </c>
@@ -8800,7 +8817,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="12">
         <v>43928</v>
       </c>
@@ -8853,7 +8870,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="12">
         <v>43929</v>
       </c>
@@ -8906,7 +8923,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="12">
         <v>43930</v>
       </c>
@@ -8959,7 +8976,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="12">
         <v>43931</v>
       </c>
@@ -9012,7 +9029,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="12">
         <v>43932</v>
       </c>
@@ -9065,7 +9082,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="12">
         <v>43933</v>
       </c>
@@ -9118,7 +9135,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <v>43934</v>
       </c>
@@ -9171,7 +9188,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="12">
         <v>43935</v>
       </c>
@@ -9224,7 +9241,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="12">
         <v>43936</v>
       </c>
@@ -9277,7 +9294,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="12">
         <v>43937</v>
       </c>
@@ -9330,7 +9347,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="12">
         <v>43938</v>
       </c>
@@ -9383,7 +9400,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="12">
         <v>43939</v>
       </c>
@@ -9436,7 +9453,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="30">
         <v>43940</v>
       </c>
@@ -9489,7 +9506,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="30">
         <v>43941</v>
       </c>
@@ -9542,7 +9559,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="30">
         <v>43942</v>
       </c>
@@ -9595,7 +9612,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="30">
         <v>43943</v>
       </c>
@@ -9648,7 +9665,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="30">
         <v>43944</v>
       </c>
@@ -9701,7 +9718,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="30">
         <v>43945</v>
       </c>
@@ -9754,7 +9771,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="30">
         <v>43946</v>
       </c>
@@ -9807,7 +9824,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="30">
         <v>43947</v>
       </c>
@@ -9860,7 +9877,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="30">
         <v>43948</v>
       </c>
@@ -9913,7 +9930,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="30">
         <v>43949</v>
       </c>
@@ -9966,7 +9983,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="30">
         <v>43950</v>
       </c>
@@ -10019,7 +10036,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="30">
         <v>43951</v>
       </c>
@@ -10072,7 +10089,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" s="30">
         <v>43952</v>
       </c>
@@ -10125,7 +10142,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="30">
         <v>43953</v>
       </c>
@@ -10178,7 +10195,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" s="30">
         <v>43954</v>
       </c>
@@ -10231,7 +10248,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="30">
         <v>43955</v>
       </c>
@@ -10284,7 +10301,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" s="30">
         <v>43956</v>
       </c>
@@ -10337,7 +10354,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" s="30">
         <v>43957</v>
       </c>
@@ -10390,7 +10407,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" s="30">
         <v>43958</v>
       </c>
@@ -10443,7 +10460,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" s="30">
         <v>43959</v>
       </c>
@@ -10496,7 +10513,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" s="30">
         <v>43960</v>
       </c>
@@ -10549,7 +10566,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" s="30">
         <v>43961</v>
       </c>
@@ -10602,7 +10619,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" s="30">
         <v>43962</v>
       </c>
@@ -10655,7 +10672,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" s="30">
         <v>43963</v>
       </c>
@@ -10708,7 +10725,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" s="30">
         <v>43964</v>
       </c>
@@ -10761,7 +10778,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" s="30">
         <v>43965</v>
       </c>
@@ -10814,7 +10831,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" s="30">
         <v>43966</v>
       </c>
@@ -10867,7 +10884,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" s="30">
         <v>43967</v>
       </c>
@@ -10920,7 +10937,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" s="30">
         <v>43968</v>
       </c>
@@ -10973,7 +10990,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" s="30">
         <v>43969</v>
       </c>
@@ -11026,7 +11043,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" s="30">
         <v>43970</v>
       </c>
@@ -11079,7 +11096,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" s="30">
         <v>43971</v>
       </c>
@@ -11132,7 +11149,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" s="30">
         <v>43972</v>
       </c>
@@ -11185,7 +11202,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" s="30">
         <v>43973</v>
       </c>
@@ -11238,7 +11255,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" s="30">
         <v>43974</v>
       </c>
@@ -11291,7 +11308,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" s="30">
         <v>43975</v>
       </c>
@@ -11344,7 +11361,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" s="30">
         <v>43976</v>
       </c>
@@ -11397,7 +11414,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" s="30">
         <v>43977</v>
       </c>
@@ -11450,7 +11467,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" s="30">
         <v>43978</v>
       </c>
@@ -11503,7 +11520,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75" s="30">
         <v>43979</v>
       </c>
@@ -11556,7 +11573,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76" s="30">
         <v>43980</v>
       </c>
@@ -11609,7 +11626,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77" s="30">
         <v>43981</v>
       </c>
@@ -11662,7 +11679,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78" s="30">
         <v>43982</v>
       </c>
@@ -11715,7 +11732,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79" s="30">
         <v>43983</v>
       </c>
@@ -11768,7 +11785,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A80" s="30">
         <v>43984</v>
       </c>
@@ -11821,7 +11838,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A81" s="30">
         <v>43985</v>
       </c>
@@ -11874,7 +11891,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A82" s="30">
         <v>43986</v>
       </c>
@@ -11927,7 +11944,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A83" s="30">
         <v>43987</v>
       </c>
@@ -11980,7 +11997,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A84" s="30">
         <v>43988</v>
       </c>
@@ -12033,7 +12050,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A85" s="30">
         <v>43989</v>
       </c>
@@ -12086,7 +12103,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A86" s="30">
         <v>43990</v>
       </c>
@@ -12137,6 +12154,59 @@
       </c>
       <c r="Q86" s="13">
         <v>24</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A87" s="30">
+        <v>43991</v>
+      </c>
+      <c r="B87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K87" s="11">
+        <v>6</v>
+      </c>
+      <c r="L87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P87" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q87" s="13">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -12147,23 +12217,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q78"/>
+  <dimension ref="A1:Q79"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B46" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B67" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5703125" style="2"/>
+    <col min="1" max="1" width="15.33203125" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.5546875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -12184,7 +12254,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -12205,7 +12275,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -12258,7 +12328,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>43916</v>
       </c>
@@ -12311,7 +12381,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>43917</v>
       </c>
@@ -12364,7 +12434,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>43918</v>
       </c>
@@ -12417,7 +12487,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>43919</v>
       </c>
@@ -12470,7 +12540,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>43920</v>
       </c>
@@ -12523,7 +12593,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>43921</v>
       </c>
@@ -12576,7 +12646,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>43922</v>
       </c>
@@ -12629,7 +12699,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>43923</v>
       </c>
@@ -12682,7 +12752,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
         <v>43924</v>
       </c>
@@ -12735,7 +12805,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>43925</v>
       </c>
@@ -12788,7 +12858,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>43926</v>
       </c>
@@ -12841,7 +12911,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>43927</v>
       </c>
@@ -12894,7 +12964,7 @@
         <v>1262</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>43928</v>
       </c>
@@ -12947,7 +13017,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>43929</v>
       </c>
@@ -13000,7 +13070,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>43930</v>
       </c>
@@ -13053,7 +13123,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>43931</v>
       </c>
@@ -13106,7 +13176,7 @@
         <v>1461</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>43932</v>
       </c>
@@ -13159,7 +13229,7 @@
         <v>1467</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>43933</v>
       </c>
@@ -13212,7 +13282,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="12">
         <v>43934</v>
       </c>
@@ -13265,7 +13335,7 @@
         <v>1482</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="12">
         <v>43935</v>
       </c>
@@ -13318,7 +13388,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="12">
         <v>43936</v>
       </c>
@@ -13371,7 +13441,7 @@
         <v>1486</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="12">
         <v>43937</v>
       </c>
@@ -13424,7 +13494,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="12">
         <v>43938</v>
       </c>
@@ -13477,7 +13547,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="12">
         <v>43939</v>
       </c>
@@ -13530,7 +13600,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="12">
         <v>43940</v>
       </c>
@@ -13583,7 +13653,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="12">
         <v>43941</v>
       </c>
@@ -13636,7 +13706,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <v>43942</v>
       </c>
@@ -13689,7 +13759,7 @@
         <v>1472</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="12">
         <v>43943</v>
       </c>
@@ -13742,7 +13812,7 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="12">
         <v>43944</v>
       </c>
@@ -13795,7 +13865,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="12">
         <v>43945</v>
       </c>
@@ -13848,7 +13918,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="12">
         <v>43946</v>
       </c>
@@ -13901,7 +13971,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="12">
         <v>43947</v>
       </c>
@@ -13954,7 +14024,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="30">
         <v>43948</v>
       </c>
@@ -14007,7 +14077,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="30">
         <v>43949</v>
       </c>
@@ -14060,7 +14130,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="30">
         <v>43950</v>
       </c>
@@ -14113,7 +14183,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="30">
         <v>43951</v>
       </c>
@@ -14166,7 +14236,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="30">
         <v>43952</v>
       </c>
@@ -14219,7 +14289,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="30">
         <v>43953</v>
       </c>
@@ -14272,7 +14342,7 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="30">
         <v>43954</v>
       </c>
@@ -14325,7 +14395,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="30">
         <v>43955</v>
       </c>
@@ -14378,7 +14448,7 @@
         <v>1279</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="30">
         <v>43956</v>
       </c>
@@ -14431,7 +14501,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="30">
         <v>43957</v>
       </c>
@@ -14484,7 +14554,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="30">
         <v>43958</v>
       </c>
@@ -14537,7 +14607,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="30">
         <v>43959</v>
       </c>
@@ -14590,7 +14660,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" s="30">
         <v>43960</v>
       </c>
@@ -14643,7 +14713,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="30">
         <v>43961</v>
       </c>
@@ -14696,7 +14766,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" s="30">
         <v>43962</v>
       </c>
@@ -14749,7 +14819,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="30">
         <v>43963</v>
       </c>
@@ -14802,7 +14872,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" s="30">
         <v>43964</v>
       </c>
@@ -14855,7 +14925,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" s="30">
         <v>43965</v>
       </c>
@@ -14908,7 +14978,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" s="30">
         <v>43966</v>
       </c>
@@ -14961,7 +15031,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" s="30">
         <v>43967</v>
       </c>
@@ -15014,7 +15084,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" s="30">
         <v>43968</v>
       </c>
@@ -15067,7 +15137,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" s="30">
         <v>43969</v>
       </c>
@@ -15120,7 +15190,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" s="30">
         <v>43970</v>
       </c>
@@ -15173,7 +15243,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" s="30">
         <v>43971</v>
       </c>
@@ -15226,7 +15296,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" s="30">
         <v>43972</v>
       </c>
@@ -15279,7 +15349,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" s="30">
         <v>43973</v>
       </c>
@@ -15332,7 +15402,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" s="30">
         <v>43974</v>
       </c>
@@ -15385,7 +15455,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" s="30">
         <v>43975</v>
       </c>
@@ -15438,7 +15508,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" s="30">
         <v>43976</v>
       </c>
@@ -15491,7 +15561,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" s="51">
         <v>43977</v>
       </c>
@@ -15544,7 +15614,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" s="51">
         <v>43978</v>
       </c>
@@ -15597,7 +15667,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" s="51">
         <v>43979</v>
       </c>
@@ -15650,7 +15720,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" s="51">
         <v>43980</v>
       </c>
@@ -15703,7 +15773,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" s="51">
         <v>43981</v>
       </c>
@@ -15756,7 +15826,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" s="51">
         <v>43982</v>
       </c>
@@ -15809,7 +15879,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" s="51">
         <v>43983</v>
       </c>
@@ -15862,7 +15932,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" s="51">
         <v>43984</v>
       </c>
@@ -15915,7 +15985,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" s="51">
         <v>43985</v>
       </c>
@@ -15968,7 +16038,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" s="51">
         <v>43986</v>
       </c>
@@ -16021,7 +16091,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75" s="51">
         <v>43987</v>
       </c>
@@ -16074,7 +16144,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76" s="51">
         <v>43988</v>
       </c>
@@ -16127,7 +16197,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77" s="51">
         <v>43989</v>
       </c>
@@ -16180,7 +16250,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78" s="51">
         <v>43990</v>
       </c>
@@ -16231,6 +16301,59 @@
       </c>
       <c r="Q78" s="13">
         <v>655</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A79" s="51">
+        <v>43991</v>
+      </c>
+      <c r="B79" s="11">
+        <v>11</v>
+      </c>
+      <c r="C79" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D79" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E79" s="11">
+        <v>52</v>
+      </c>
+      <c r="F79" s="11">
+        <v>10</v>
+      </c>
+      <c r="G79" s="11">
+        <v>62</v>
+      </c>
+      <c r="H79" s="11">
+        <v>289</v>
+      </c>
+      <c r="I79" s="11">
+        <v>8</v>
+      </c>
+      <c r="J79" s="11">
+        <v>56</v>
+      </c>
+      <c r="K79" s="11">
+        <v>145</v>
+      </c>
+      <c r="L79" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M79" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N79" s="11">
+        <v>8</v>
+      </c>
+      <c r="O79" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P79" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q79" s="13">
+        <v>641</v>
       </c>
     </row>
   </sheetData>
@@ -16241,23 +16364,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q78"/>
+  <dimension ref="A1:Q79"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B49" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B58" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5703125" style="2"/>
+    <col min="1" max="1" width="12.44140625" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.5546875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -16278,7 +16401,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -16299,7 +16422,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -16352,7 +16475,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>43916</v>
       </c>
@@ -16405,7 +16528,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>43917</v>
       </c>
@@ -16458,7 +16581,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>43918</v>
       </c>
@@ -16511,7 +16634,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>43919</v>
       </c>
@@ -16564,7 +16687,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>43920</v>
       </c>
@@ -16617,7 +16740,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>43921</v>
       </c>
@@ -16670,7 +16793,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>43922</v>
       </c>
@@ -16723,7 +16846,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>43923</v>
       </c>
@@ -16776,7 +16899,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
         <v>43924</v>
       </c>
@@ -16829,7 +16952,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>43925</v>
       </c>
@@ -16882,7 +17005,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>43926</v>
       </c>
@@ -16935,7 +17058,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>43927</v>
       </c>
@@ -16988,7 +17111,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>43928</v>
       </c>
@@ -17041,7 +17164,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>43929</v>
       </c>
@@ -17094,7 +17217,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>43930</v>
       </c>
@@ -17147,7 +17270,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>43931</v>
       </c>
@@ -17200,7 +17323,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>43932</v>
       </c>
@@ -17253,7 +17376,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>43933</v>
       </c>
@@ -17306,7 +17429,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="12">
         <v>43934</v>
       </c>
@@ -17359,7 +17482,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="12">
         <v>43935</v>
       </c>
@@ -17412,7 +17535,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="12">
         <v>43936</v>
       </c>
@@ -17465,7 +17588,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="12">
         <v>43937</v>
       </c>
@@ -17518,7 +17641,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="12">
         <v>43938</v>
       </c>
@@ -17571,7 +17694,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="12">
         <v>43939</v>
       </c>
@@ -17624,7 +17747,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="12">
         <v>43940</v>
       </c>
@@ -17677,7 +17800,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="12">
         <v>43941</v>
       </c>
@@ -17730,7 +17853,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <v>43942</v>
       </c>
@@ -17783,7 +17906,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="12">
         <v>43943</v>
       </c>
@@ -17836,7 +17959,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="12">
         <v>43944</v>
       </c>
@@ -17889,7 +18012,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="12">
         <v>43945</v>
       </c>
@@ -17942,7 +18065,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="12">
         <v>43946</v>
       </c>
@@ -17995,7 +18118,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="12">
         <v>43947</v>
       </c>
@@ -18048,7 +18171,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="30">
         <v>43948</v>
       </c>
@@ -18101,7 +18224,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="30">
         <v>43949</v>
       </c>
@@ -18154,7 +18277,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="30">
         <v>43950</v>
       </c>
@@ -18207,7 +18330,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="30">
         <v>43951</v>
       </c>
@@ -18260,7 +18383,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="30">
         <v>43952</v>
       </c>
@@ -18313,7 +18436,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="30">
         <v>43953</v>
       </c>
@@ -18366,7 +18489,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="30">
         <v>43954</v>
       </c>
@@ -18419,7 +18542,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="30">
         <v>43955</v>
       </c>
@@ -18472,7 +18595,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="30">
         <v>43956</v>
       </c>
@@ -18525,7 +18648,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="30">
         <v>43957</v>
       </c>
@@ -18578,7 +18701,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="30">
         <v>43958</v>
       </c>
@@ -18631,7 +18754,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="30">
         <v>43959</v>
       </c>
@@ -18684,7 +18807,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" s="30">
         <v>43960</v>
       </c>
@@ -18737,7 +18860,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="30">
         <v>43961</v>
       </c>
@@ -18790,7 +18913,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" s="30">
         <v>43962</v>
       </c>
@@ -18843,7 +18966,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="30">
         <v>43963</v>
       </c>
@@ -18896,7 +19019,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" s="30">
         <v>43964</v>
       </c>
@@ -18949,7 +19072,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" s="30">
         <v>43965</v>
       </c>
@@ -19002,7 +19125,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" s="30">
         <v>43966</v>
       </c>
@@ -19055,7 +19178,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" s="30">
         <v>43967</v>
       </c>
@@ -19108,7 +19231,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" s="30">
         <v>43968</v>
       </c>
@@ -19161,7 +19284,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" s="30">
         <v>43969</v>
       </c>
@@ -19214,7 +19337,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" s="30">
         <v>43970</v>
       </c>
@@ -19267,7 +19390,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" s="30">
         <v>43971</v>
       </c>
@@ -19320,7 +19443,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" s="30">
         <v>43972</v>
       </c>
@@ -19373,7 +19496,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" s="30">
         <v>43973</v>
       </c>
@@ -19426,7 +19549,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" s="30">
         <v>43974</v>
       </c>
@@ -19479,7 +19602,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" s="30">
         <v>43975</v>
       </c>
@@ -19532,7 +19655,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" s="30">
         <v>43976</v>
       </c>
@@ -19585,7 +19708,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" s="30">
         <v>43977</v>
       </c>
@@ -19638,7 +19761,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" s="30">
         <v>43978</v>
       </c>
@@ -19691,7 +19814,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" s="30">
         <v>43979</v>
       </c>
@@ -19744,7 +19867,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" s="30">
         <v>43980</v>
       </c>
@@ -19797,7 +19920,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" s="30">
         <v>43981</v>
       </c>
@@ -19850,7 +19973,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" s="30">
         <v>43982</v>
       </c>
@@ -19903,7 +20026,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" s="30">
         <v>43983</v>
       </c>
@@ -19956,7 +20079,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" s="30">
         <v>43984</v>
       </c>
@@ -20009,7 +20132,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" s="30">
         <v>43985</v>
       </c>
@@ -20062,7 +20185,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" s="30">
         <v>43986</v>
       </c>
@@ -20115,7 +20238,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75" s="30">
         <v>43987</v>
       </c>
@@ -20168,7 +20291,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76" s="30">
         <v>43988</v>
       </c>
@@ -20221,7 +20344,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77" s="30">
         <v>43989</v>
       </c>
@@ -20274,7 +20397,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78" s="30">
         <v>43990</v>
       </c>
@@ -20325,6 +20448,59 @@
       </c>
       <c r="Q78" s="13">
         <v>387</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A79" s="30">
+        <v>43991</v>
+      </c>
+      <c r="B79" s="11">
+        <v>19</v>
+      </c>
+      <c r="C79" s="11">
+        <v>18</v>
+      </c>
+      <c r="D79" s="11">
+        <v>18</v>
+      </c>
+      <c r="E79" s="11">
+        <v>17</v>
+      </c>
+      <c r="F79" s="11">
+        <v>24</v>
+      </c>
+      <c r="G79" s="11">
+        <v>9</v>
+      </c>
+      <c r="H79" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I79" s="11">
+        <v>11</v>
+      </c>
+      <c r="J79" s="11">
+        <v>58</v>
+      </c>
+      <c r="K79" s="11">
+        <v>181</v>
+      </c>
+      <c r="L79" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M79" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N79" s="11">
+        <v>13</v>
+      </c>
+      <c r="O79" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P79" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q79" s="13">
+        <v>370</v>
       </c>
     </row>
   </sheetData>
@@ -20357,7 +20533,7 @@
       <value order="0"/>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-08T12:32:35Z</value>
+      <value order="0">2020-06-09T12:29:11Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -20372,13 +20548,13 @@
       <value order="0">Being Drafted</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41607398</value>
+      <value order="0">vA41637421</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">22.2</value>
+      <value order="0">22.4</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">159</value>
+      <value order="0">161</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-09 20:09) (#102)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Z616594\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA19704\A28088333\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U445783\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA18464\A28088333\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5985" windowHeight="6030" tabRatio="803"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5988" windowHeight="6036" tabRatio="803" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1707" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1732" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -1634,23 +1634,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="90.42578125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.42578125" style="2"/>
+    <col min="2" max="2" width="29.44140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="90.44140625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" s="18" t="s">
         <v>20</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20" t="s">
         <v>22</v>
       </c>
@@ -1666,13 +1666,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="22" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="23"/>
     </row>
-    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="24" t="s">
         <v>26</v>
       </c>
@@ -1680,7 +1680,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="24" t="s">
         <v>27</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="24" t="s">
         <v>36</v>
       </c>
@@ -1696,7 +1696,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="20" t="s">
         <v>37</v>
       </c>
@@ -1724,12 +1724,12 @@
       <selection activeCell="K66" sqref="K66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.42578125" style="2"/>
+    <col min="1" max="16384" width="9.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" ht="15" x14ac:dyDescent="0.3">
       <c r="A44" s="43"/>
     </row>
   </sheetData>
@@ -1743,21 +1743,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S160"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="64" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B88" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="R93" sqref="R93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" style="2" customWidth="1"/>
-    <col min="2" max="16" width="11.42578125" style="11" customWidth="1"/>
-    <col min="17" max="16384" width="8.5703125" style="2"/>
+    <col min="2" max="16" width="11.44140625" style="11" customWidth="1"/>
+    <col min="17" max="16384" width="8.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -1777,7 +1777,7 @@
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -1796,7 +1796,7 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>43897</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>43898</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>43899</v>
       </c>
@@ -1996,7 +1996,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>43900</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>43901</v>
       </c>
@@ -2096,7 +2096,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>43902</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>43903</v>
       </c>
@@ -2196,7 +2196,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>43904</v>
       </c>
@@ -2246,7 +2246,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>43905</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>43906</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>43907</v>
       </c>
@@ -2396,7 +2396,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>43908</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>43909</v>
       </c>
@@ -2496,7 +2496,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>43910</v>
       </c>
@@ -2546,7 +2546,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>43911</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>43912</v>
       </c>
@@ -2646,7 +2646,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>43913</v>
       </c>
@@ -2696,7 +2696,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>43914</v>
       </c>
@@ -2746,7 +2746,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>43915</v>
       </c>
@@ -2796,7 +2796,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>43916</v>
       </c>
@@ -2846,7 +2846,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>43917</v>
       </c>
@@ -2896,7 +2896,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>43918</v>
       </c>
@@ -2946,7 +2946,7 @@
         <v>1264</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>43919</v>
       </c>
@@ -2996,7 +2996,7 @@
         <v>1417</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>43920</v>
       </c>
@@ -3046,7 +3046,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>43921</v>
       </c>
@@ -3096,7 +3096,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>43922</v>
       </c>
@@ -3146,7 +3146,7 @@
         <v>2310</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>43923</v>
       </c>
@@ -3196,7 +3196,7 @@
         <v>2602</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <v>43924</v>
       </c>
@@ -3246,7 +3246,7 @@
         <v>3001</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>43925</v>
       </c>
@@ -3296,7 +3296,7 @@
         <v>3345</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
         <v>43926</v>
       </c>
@@ -3346,7 +3346,7 @@
         <v>3706</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
         <v>43927</v>
       </c>
@@ -3396,7 +3396,7 @@
         <v>3961</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
         <v>43928</v>
       </c>
@@ -3446,7 +3446,7 @@
         <v>4229</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>43929</v>
       </c>
@@ -3496,7 +3496,7 @@
         <v>4565</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
         <v>43930</v>
       </c>
@@ -3546,7 +3546,7 @@
         <v>4957</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
         <v>43931</v>
       </c>
@@ -3596,7 +3596,7 @@
         <v>5275</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>43932</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>5590</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
         <v>43933</v>
       </c>
@@ -3696,7 +3696,7 @@
         <v>5912</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
         <v>43934</v>
       </c>
@@ -3746,7 +3746,7 @@
         <v>6067</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>43935</v>
       </c>
@@ -3796,7 +3796,7 @@
         <v>6358</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
         <v>43936</v>
       </c>
@@ -3846,7 +3846,7 @@
         <v>6748</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" s="5">
         <v>43937</v>
       </c>
@@ -3896,7 +3896,7 @@
         <v>7102</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
         <v>43938</v>
       </c>
@@ -3946,7 +3946,7 @@
         <v>7409</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" s="5">
         <v>43939</v>
       </c>
@@ -3996,7 +3996,7 @@
         <v>7820</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" s="5">
         <v>43940</v>
       </c>
@@ -4046,7 +4046,7 @@
         <v>8187</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
         <v>43941</v>
       </c>
@@ -4096,7 +4096,7 @@
         <v>8450</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A49" s="5">
         <v>43942</v>
       </c>
@@ -4146,7 +4146,7 @@
         <v>8672</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
         <v>43943</v>
       </c>
@@ -4196,7 +4196,7 @@
         <v>9038</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A51" s="5">
         <v>43944</v>
       </c>
@@ -4246,7 +4246,7 @@
         <v>9409</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A52" s="5">
         <v>43945</v>
       </c>
@@ -4296,7 +4296,7 @@
         <v>9697</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A53" s="5">
         <v>43946</v>
       </c>
@@ -4346,7 +4346,7 @@
         <v>10051</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A54" s="5">
         <v>43947</v>
       </c>
@@ -4397,7 +4397,7 @@
       </c>
       <c r="R54" s="38"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A55" s="5">
         <v>43948</v>
       </c>
@@ -4448,7 +4448,7 @@
       </c>
       <c r="R55" s="38"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A56" s="5">
         <v>43949</v>
       </c>
@@ -4499,7 +4499,7 @@
       </c>
       <c r="R56" s="39"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A57" s="5">
         <v>43950</v>
       </c>
@@ -4549,7 +4549,7 @@
         <v>11034</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A58" s="5">
         <v>43951</v>
       </c>
@@ -4600,7 +4600,7 @@
       </c>
       <c r="R58" s="38"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A59" s="5">
         <v>43952</v>
       </c>
@@ -4652,7 +4652,7 @@
       <c r="R59" s="38"/>
       <c r="S59" s="38"/>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A60" s="5">
         <v>43953</v>
       </c>
@@ -4702,7 +4702,7 @@
         <v>11927</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A61" s="5">
         <v>43954</v>
       </c>
@@ -4752,7 +4752,7 @@
         <v>12097</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A62" s="5">
         <v>43955</v>
       </c>
@@ -4802,7 +4802,7 @@
         <v>12266</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A63" s="5">
         <v>43956</v>
       </c>
@@ -4852,7 +4852,7 @@
         <v>12437</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A64" s="5">
         <v>43957</v>
       </c>
@@ -4902,7 +4902,7 @@
         <v>12709</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65" s="5">
         <v>43958</v>
       </c>
@@ -4952,7 +4952,7 @@
         <v>12924</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66" s="5">
         <v>43959</v>
       </c>
@@ -5002,7 +5002,7 @@
         <v>13149</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A67" s="5">
         <v>43960</v>
       </c>
@@ -5052,7 +5052,7 @@
         <v>13305</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A68" s="5">
         <v>43961</v>
       </c>
@@ -5102,7 +5102,7 @@
         <v>13486</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A69" s="5">
         <v>43962</v>
       </c>
@@ -5152,7 +5152,7 @@
         <v>13627</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A70" s="5">
         <v>43963</v>
       </c>
@@ -5202,7 +5202,7 @@
         <v>13763</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A71" s="5">
         <v>43964</v>
       </c>
@@ -5252,7 +5252,7 @@
         <v>13929</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A72" s="5">
         <v>43965</v>
       </c>
@@ -5302,7 +5302,7 @@
         <v>14117</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A73" s="5">
         <v>43966</v>
       </c>
@@ -5352,7 +5352,7 @@
         <v>14260</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A74" s="5">
         <v>43967</v>
       </c>
@@ -5402,7 +5402,7 @@
         <v>14447</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A75" s="5">
         <v>43968</v>
       </c>
@@ -5452,7 +5452,7 @@
         <v>14537</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A76" s="5">
         <v>43969</v>
       </c>
@@ -5502,7 +5502,7 @@
         <v>14594</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A77" s="5">
         <v>43970</v>
       </c>
@@ -5552,7 +5552,7 @@
         <v>14655</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A78" s="5">
         <v>43971</v>
       </c>
@@ -5602,7 +5602,7 @@
         <v>14751</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A79" s="5">
         <v>43972</v>
       </c>
@@ -5652,7 +5652,7 @@
         <v>14856</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A80" s="5">
         <v>43973</v>
       </c>
@@ -5702,7 +5702,7 @@
         <v>14969</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A81" s="5">
         <v>43974</v>
       </c>
@@ -5752,7 +5752,7 @@
         <v>15041</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A82" s="5">
         <v>43975</v>
       </c>
@@ -5802,7 +5802,7 @@
         <v>15101</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A83" s="5">
         <v>43976</v>
       </c>
@@ -5852,7 +5852,7 @@
         <v>15156</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A84" s="5">
         <v>43977</v>
       </c>
@@ -5902,7 +5902,7 @@
         <v>15185</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A85" s="5">
         <v>43978</v>
       </c>
@@ -5952,7 +5952,7 @@
         <v>15240</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A86" s="5">
         <v>43979</v>
       </c>
@@ -6002,7 +6002,7 @@
         <v>15288</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A87" s="5">
         <v>43980</v>
       </c>
@@ -6052,7 +6052,7 @@
         <v>15327</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A88" s="5">
         <v>43981</v>
       </c>
@@ -6102,7 +6102,7 @@
         <v>15382</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A89" s="5">
         <v>43982</v>
       </c>
@@ -6152,7 +6152,7 @@
         <v>15400</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A90" s="5">
         <v>43983</v>
       </c>
@@ -6202,7 +6202,7 @@
         <v>15418</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A91" s="5">
         <v>43984</v>
       </c>
@@ -6252,7 +6252,7 @@
         <v>15471</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A92" s="5">
         <v>43985</v>
       </c>
@@ -6302,7 +6302,7 @@
         <v>15504</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A93" s="5">
         <v>43986</v>
       </c>
@@ -6352,7 +6352,7 @@
         <v>15553</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A94" s="5">
         <v>43987</v>
       </c>
@@ -6402,7 +6402,7 @@
         <v>15582</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A95" s="5">
         <v>43988</v>
       </c>
@@ -6452,7 +6452,7 @@
         <v>15603</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A96" s="5">
         <v>43989</v>
       </c>
@@ -6502,7 +6502,7 @@
         <v>15621</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A97" s="5">
         <v>43990</v>
       </c>
@@ -6552,25 +6552,57 @@
         <v>15639</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B98" s="28"/>
-      <c r="C98" s="28"/>
-      <c r="D98" s="28"/>
-      <c r="E98" s="28"/>
-      <c r="F98" s="28"/>
-      <c r="G98" s="28"/>
-      <c r="H98" s="28"/>
-      <c r="I98" s="28"/>
-      <c r="J98" s="28"/>
-      <c r="K98" s="28"/>
-      <c r="L98" s="28"/>
-      <c r="M98" s="28"/>
-      <c r="N98" s="28"/>
-      <c r="O98" s="28"/>
-      <c r="P98" s="28"/>
-    </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B99" s="28"/>
+    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A98" s="5">
+        <v>43991</v>
+      </c>
+      <c r="B98" s="28">
+        <v>1081</v>
+      </c>
+      <c r="C98" s="28">
+        <v>326</v>
+      </c>
+      <c r="D98" s="28">
+        <v>261</v>
+      </c>
+      <c r="E98" s="28">
+        <v>879</v>
+      </c>
+      <c r="F98" s="28">
+        <v>948</v>
+      </c>
+      <c r="G98" s="28">
+        <v>1287</v>
+      </c>
+      <c r="H98" s="28">
+        <v>3990</v>
+      </c>
+      <c r="I98" s="28">
+        <v>340</v>
+      </c>
+      <c r="J98" s="28">
+        <v>2018</v>
+      </c>
+      <c r="K98" s="28">
+        <v>2777</v>
+      </c>
+      <c r="L98" s="28">
+        <v>8</v>
+      </c>
+      <c r="M98" s="28">
+        <v>54</v>
+      </c>
+      <c r="N98" s="28">
+        <v>1678</v>
+      </c>
+      <c r="O98" s="28">
+        <v>6</v>
+      </c>
+      <c r="P98" s="32">
+        <v>15653</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C99" s="28"/>
       <c r="D99" s="28"/>
       <c r="E99" s="28"/>
@@ -6586,8 +6618,7 @@
       <c r="O99" s="28"/>
       <c r="P99" s="28"/>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B100" s="28"/>
+    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C100" s="28"/>
       <c r="D100" s="28"/>
       <c r="E100" s="28"/>
@@ -6603,8 +6634,7 @@
       <c r="O100" s="28"/>
       <c r="P100" s="28"/>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B101" s="28"/>
+    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C101" s="28"/>
       <c r="D101" s="28"/>
       <c r="E101" s="28"/>
@@ -6620,8 +6650,7 @@
       <c r="O101" s="28"/>
       <c r="P101" s="28"/>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B102" s="28"/>
+    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C102" s="28"/>
       <c r="D102" s="28"/>
       <c r="E102" s="28"/>
@@ -6637,8 +6666,7 @@
       <c r="O102" s="28"/>
       <c r="P102" s="28"/>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B103" s="28"/>
+    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C103" s="28"/>
       <c r="D103" s="28"/>
       <c r="E103" s="28"/>
@@ -6654,8 +6682,7 @@
       <c r="O103" s="28"/>
       <c r="P103" s="28"/>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B104" s="28"/>
+    <row r="104" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C104" s="28"/>
       <c r="D104" s="28"/>
       <c r="E104" s="28"/>
@@ -6671,8 +6698,7 @@
       <c r="O104" s="28"/>
       <c r="P104" s="28"/>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B105" s="28"/>
+    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C105" s="28"/>
       <c r="D105" s="28"/>
       <c r="E105" s="28"/>
@@ -6688,8 +6714,7 @@
       <c r="O105" s="28"/>
       <c r="P105" s="28"/>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B106" s="28"/>
+    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C106" s="28"/>
       <c r="D106" s="28"/>
       <c r="E106" s="28"/>
@@ -6705,8 +6730,7 @@
       <c r="O106" s="28"/>
       <c r="P106" s="28"/>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B107" s="28"/>
+    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C107" s="28"/>
       <c r="D107" s="28"/>
       <c r="E107" s="28"/>
@@ -6722,8 +6746,7 @@
       <c r="O107" s="28"/>
       <c r="P107" s="28"/>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B108" s="28"/>
+    <row r="108" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C108" s="28"/>
       <c r="D108" s="28"/>
       <c r="E108" s="28"/>
@@ -6739,8 +6762,7 @@
       <c r="O108" s="28"/>
       <c r="P108" s="28"/>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B109" s="28"/>
+    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C109" s="28"/>
       <c r="D109" s="28"/>
       <c r="E109" s="28"/>
@@ -6756,8 +6778,7 @@
       <c r="O109" s="28"/>
       <c r="P109" s="28"/>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B110" s="28"/>
+    <row r="110" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C110" s="28"/>
       <c r="D110" s="28"/>
       <c r="E110" s="28"/>
@@ -6773,8 +6794,7 @@
       <c r="O110" s="28"/>
       <c r="P110" s="28"/>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B111" s="28"/>
+    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C111" s="28"/>
       <c r="D111" s="28"/>
       <c r="E111" s="28"/>
@@ -6790,8 +6810,7 @@
       <c r="O111" s="28"/>
       <c r="P111" s="28"/>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B112" s="28"/>
+    <row r="112" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C112" s="28"/>
       <c r="D112" s="28"/>
       <c r="E112" s="28"/>
@@ -6807,8 +6826,7 @@
       <c r="O112" s="28"/>
       <c r="P112" s="28"/>
     </row>
-    <row r="113" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B113" s="28"/>
+    <row r="113" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C113" s="28"/>
       <c r="D113" s="28"/>
       <c r="E113" s="28"/>
@@ -6824,8 +6842,7 @@
       <c r="O113" s="28"/>
       <c r="P113" s="28"/>
     </row>
-    <row r="114" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B114" s="28"/>
+    <row r="114" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C114" s="28"/>
       <c r="D114" s="28"/>
       <c r="E114" s="28"/>
@@ -6841,7 +6858,7 @@
       <c r="O114" s="28"/>
       <c r="P114" s="28"/>
     </row>
-    <row r="115" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B115" s="28"/>
       <c r="C115" s="28"/>
       <c r="D115" s="28"/>
@@ -6858,7 +6875,7 @@
       <c r="O115" s="28"/>
       <c r="P115" s="28"/>
     </row>
-    <row r="116" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B116" s="28"/>
       <c r="C116" s="28"/>
       <c r="D116" s="28"/>
@@ -6875,7 +6892,7 @@
       <c r="O116" s="28"/>
       <c r="P116" s="28"/>
     </row>
-    <row r="117" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B117" s="28"/>
       <c r="C117" s="28"/>
       <c r="D117" s="28"/>
@@ -6892,7 +6909,7 @@
       <c r="O117" s="28"/>
       <c r="P117" s="28"/>
     </row>
-    <row r="118" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B118" s="28"/>
       <c r="C118" s="28"/>
       <c r="D118" s="28"/>
@@ -6909,7 +6926,7 @@
       <c r="O118" s="28"/>
       <c r="P118" s="28"/>
     </row>
-    <row r="119" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B119" s="28"/>
       <c r="C119" s="28"/>
       <c r="D119" s="28"/>
@@ -6926,7 +6943,7 @@
       <c r="O119" s="28"/>
       <c r="P119" s="28"/>
     </row>
-    <row r="120" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B120" s="28"/>
       <c r="C120" s="28"/>
       <c r="D120" s="28"/>
@@ -6943,7 +6960,7 @@
       <c r="O120" s="28"/>
       <c r="P120" s="28"/>
     </row>
-    <row r="121" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B121" s="28"/>
       <c r="C121" s="28"/>
       <c r="D121" s="28"/>
@@ -6960,7 +6977,7 @@
       <c r="O121" s="28"/>
       <c r="P121" s="28"/>
     </row>
-    <row r="122" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B122" s="28"/>
       <c r="C122" s="28"/>
       <c r="D122" s="28"/>
@@ -6977,7 +6994,7 @@
       <c r="O122" s="28"/>
       <c r="P122" s="28"/>
     </row>
-    <row r="123" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B123" s="28"/>
       <c r="C123" s="28"/>
       <c r="D123" s="28"/>
@@ -6994,7 +7011,7 @@
       <c r="O123" s="28"/>
       <c r="P123" s="28"/>
     </row>
-    <row r="124" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B124" s="28"/>
       <c r="C124" s="28"/>
       <c r="D124" s="28"/>
@@ -7011,7 +7028,7 @@
       <c r="O124" s="28"/>
       <c r="P124" s="28"/>
     </row>
-    <row r="125" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B125" s="28"/>
       <c r="C125" s="28"/>
       <c r="D125" s="28"/>
@@ -7028,7 +7045,7 @@
       <c r="O125" s="28"/>
       <c r="P125" s="28"/>
     </row>
-    <row r="126" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B126" s="28"/>
       <c r="C126" s="28"/>
       <c r="D126" s="28"/>
@@ -7045,7 +7062,7 @@
       <c r="O126" s="28"/>
       <c r="P126" s="28"/>
     </row>
-    <row r="127" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B127" s="28"/>
       <c r="C127" s="28"/>
       <c r="D127" s="28"/>
@@ -7062,7 +7079,7 @@
       <c r="O127" s="28"/>
       <c r="P127" s="28"/>
     </row>
-    <row r="128" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B128" s="28"/>
       <c r="C128" s="28"/>
       <c r="D128" s="28"/>
@@ -7079,7 +7096,7 @@
       <c r="O128" s="28"/>
       <c r="P128" s="28"/>
     </row>
-    <row r="129" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B129" s="28"/>
       <c r="C129" s="28"/>
       <c r="D129" s="28"/>
@@ -7096,7 +7113,7 @@
       <c r="O129" s="28"/>
       <c r="P129" s="28"/>
     </row>
-    <row r="130" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B130" s="28"/>
       <c r="C130" s="28"/>
       <c r="D130" s="28"/>
@@ -7113,7 +7130,7 @@
       <c r="O130" s="28"/>
       <c r="P130" s="28"/>
     </row>
-    <row r="131" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B131" s="28"/>
       <c r="C131" s="28"/>
       <c r="D131" s="28"/>
@@ -7130,7 +7147,7 @@
       <c r="O131" s="28"/>
       <c r="P131" s="28"/>
     </row>
-    <row r="132" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B132" s="28"/>
       <c r="C132" s="28"/>
       <c r="D132" s="28"/>
@@ -7147,7 +7164,7 @@
       <c r="O132" s="28"/>
       <c r="P132" s="28"/>
     </row>
-    <row r="133" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B133" s="28"/>
       <c r="C133" s="28"/>
       <c r="D133" s="28"/>
@@ -7164,7 +7181,7 @@
       <c r="O133" s="28"/>
       <c r="P133" s="28"/>
     </row>
-    <row r="134" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B134" s="28"/>
       <c r="C134" s="28"/>
       <c r="D134" s="28"/>
@@ -7181,7 +7198,7 @@
       <c r="O134" s="28"/>
       <c r="P134" s="28"/>
     </row>
-    <row r="135" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B135" s="28"/>
       <c r="C135" s="28"/>
       <c r="D135" s="28"/>
@@ -7198,7 +7215,7 @@
       <c r="O135" s="28"/>
       <c r="P135" s="28"/>
     </row>
-    <row r="136" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B136" s="28"/>
       <c r="C136" s="28"/>
       <c r="D136" s="28"/>
@@ -7215,7 +7232,7 @@
       <c r="O136" s="28"/>
       <c r="P136" s="28"/>
     </row>
-    <row r="137" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B137" s="28"/>
       <c r="C137" s="28"/>
       <c r="D137" s="28"/>
@@ -7232,7 +7249,7 @@
       <c r="O137" s="28"/>
       <c r="P137" s="28"/>
     </row>
-    <row r="138" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B138" s="28"/>
       <c r="C138" s="28"/>
       <c r="D138" s="28"/>
@@ -7249,7 +7266,7 @@
       <c r="O138" s="28"/>
       <c r="P138" s="28"/>
     </row>
-    <row r="139" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B139" s="28"/>
       <c r="C139" s="28"/>
       <c r="D139" s="28"/>
@@ -7266,7 +7283,7 @@
       <c r="O139" s="28"/>
       <c r="P139" s="28"/>
     </row>
-    <row r="140" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B140" s="28"/>
       <c r="C140" s="28"/>
       <c r="D140" s="28"/>
@@ -7283,7 +7300,7 @@
       <c r="O140" s="28"/>
       <c r="P140" s="28"/>
     </row>
-    <row r="141" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B141" s="28"/>
       <c r="C141" s="28"/>
       <c r="D141" s="28"/>
@@ -7300,7 +7317,7 @@
       <c r="O141" s="28"/>
       <c r="P141" s="28"/>
     </row>
-    <row r="142" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B142" s="28"/>
       <c r="C142" s="28"/>
       <c r="D142" s="28"/>
@@ -7317,7 +7334,7 @@
       <c r="O142" s="28"/>
       <c r="P142" s="28"/>
     </row>
-    <row r="143" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B143" s="28"/>
       <c r="C143" s="28"/>
       <c r="D143" s="28"/>
@@ -7334,7 +7351,7 @@
       <c r="O143" s="28"/>
       <c r="P143" s="28"/>
     </row>
-    <row r="144" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B144" s="28"/>
       <c r="C144" s="28"/>
       <c r="D144" s="28"/>
@@ -7351,7 +7368,7 @@
       <c r="O144" s="28"/>
       <c r="P144" s="28"/>
     </row>
-    <row r="145" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B145" s="28"/>
       <c r="C145" s="28"/>
       <c r="D145" s="28"/>
@@ -7368,7 +7385,7 @@
       <c r="O145" s="28"/>
       <c r="P145" s="28"/>
     </row>
-    <row r="146" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B146" s="28"/>
       <c r="C146" s="28"/>
       <c r="D146" s="28"/>
@@ -7385,7 +7402,7 @@
       <c r="O146" s="28"/>
       <c r="P146" s="28"/>
     </row>
-    <row r="147" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B147" s="28"/>
       <c r="C147" s="28"/>
       <c r="D147" s="28"/>
@@ -7402,7 +7419,7 @@
       <c r="O147" s="28"/>
       <c r="P147" s="28"/>
     </row>
-    <row r="148" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B148" s="28"/>
       <c r="C148" s="28"/>
       <c r="D148" s="28"/>
@@ -7419,7 +7436,7 @@
       <c r="O148" s="28"/>
       <c r="P148" s="28"/>
     </row>
-    <row r="149" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B149" s="28"/>
       <c r="C149" s="28"/>
       <c r="D149" s="28"/>
@@ -7436,7 +7453,7 @@
       <c r="O149" s="28"/>
       <c r="P149" s="28"/>
     </row>
-    <row r="150" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B150" s="28"/>
       <c r="C150" s="28"/>
       <c r="D150" s="28"/>
@@ -7453,7 +7470,7 @@
       <c r="O150" s="28"/>
       <c r="P150" s="28"/>
     </row>
-    <row r="151" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B151" s="28"/>
       <c r="C151" s="28"/>
       <c r="D151" s="28"/>
@@ -7470,7 +7487,7 @@
       <c r="O151" s="28"/>
       <c r="P151" s="28"/>
     </row>
-    <row r="152" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B152" s="28"/>
       <c r="C152" s="28"/>
       <c r="D152" s="28"/>
@@ -7487,7 +7504,7 @@
       <c r="O152" s="28"/>
       <c r="P152" s="28"/>
     </row>
-    <row r="153" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B153" s="28"/>
       <c r="C153" s="28"/>
       <c r="D153" s="28"/>
@@ -7504,7 +7521,7 @@
       <c r="O153" s="28"/>
       <c r="P153" s="28"/>
     </row>
-    <row r="154" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B154" s="28"/>
       <c r="C154" s="28"/>
       <c r="D154" s="28"/>
@@ -7521,7 +7538,7 @@
       <c r="O154" s="28"/>
       <c r="P154" s="28"/>
     </row>
-    <row r="155" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B155" s="28"/>
       <c r="C155" s="28"/>
       <c r="D155" s="28"/>
@@ -7538,7 +7555,7 @@
       <c r="O155" s="28"/>
       <c r="P155" s="28"/>
     </row>
-    <row r="156" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B156" s="28"/>
       <c r="C156" s="28"/>
       <c r="D156" s="28"/>
@@ -7555,7 +7572,7 @@
       <c r="O156" s="28"/>
       <c r="P156" s="28"/>
     </row>
-    <row r="157" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B157" s="28"/>
       <c r="C157" s="28"/>
       <c r="D157" s="28"/>
@@ -7572,7 +7589,7 @@
       <c r="O157" s="28"/>
       <c r="P157" s="28"/>
     </row>
-    <row r="158" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B158" s="28"/>
       <c r="C158" s="28"/>
       <c r="D158" s="28"/>
@@ -7589,7 +7606,7 @@
       <c r="O158" s="28"/>
       <c r="P158" s="28"/>
     </row>
-    <row r="159" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B159" s="28"/>
       <c r="C159" s="28"/>
       <c r="D159" s="28"/>
@@ -7606,7 +7623,7 @@
       <c r="O159" s="28"/>
       <c r="P159" s="28"/>
     </row>
-    <row r="160" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B160" s="28"/>
       <c r="C160" s="28"/>
       <c r="D160" s="28"/>
@@ -7631,21 +7648,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q86"/>
+  <dimension ref="A1:Q87"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5703125" style="2"/>
+    <col min="1" max="1" width="12.44140625" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.5546875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -7666,7 +7683,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -7687,7 +7704,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -7740,7 +7757,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>43908</v>
       </c>
@@ -7793,7 +7810,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>43909</v>
       </c>
@@ -7846,7 +7863,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>43910</v>
       </c>
@@ -7899,7 +7916,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>43911</v>
       </c>
@@ -7952,7 +7969,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>43912</v>
       </c>
@@ -8005,7 +8022,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>43913</v>
       </c>
@@ -8058,7 +8075,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>43914</v>
       </c>
@@ -8111,7 +8128,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>43915</v>
       </c>
@@ -8164,7 +8181,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
         <v>43916</v>
       </c>
@@ -8217,7 +8234,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>43917</v>
       </c>
@@ -8270,7 +8287,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>43918</v>
       </c>
@@ -8323,7 +8340,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>43919</v>
       </c>
@@ -8376,7 +8393,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>43920</v>
       </c>
@@ -8429,7 +8446,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>43921</v>
       </c>
@@ -8482,7 +8499,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>43922</v>
       </c>
@@ -8535,7 +8552,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>43923</v>
       </c>
@@ -8588,7 +8605,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>43924</v>
       </c>
@@ -8641,7 +8658,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>43925</v>
       </c>
@@ -8694,7 +8711,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="12">
         <v>43926</v>
       </c>
@@ -8747,7 +8764,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="12">
         <v>43927</v>
       </c>
@@ -8800,7 +8817,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="12">
         <v>43928</v>
       </c>
@@ -8853,7 +8870,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="12">
         <v>43929</v>
       </c>
@@ -8906,7 +8923,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="12">
         <v>43930</v>
       </c>
@@ -8959,7 +8976,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="12">
         <v>43931</v>
       </c>
@@ -9012,7 +9029,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="12">
         <v>43932</v>
       </c>
@@ -9065,7 +9082,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="12">
         <v>43933</v>
       </c>
@@ -9118,7 +9135,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <v>43934</v>
       </c>
@@ -9171,7 +9188,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="12">
         <v>43935</v>
       </c>
@@ -9224,7 +9241,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="12">
         <v>43936</v>
       </c>
@@ -9277,7 +9294,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="12">
         <v>43937</v>
       </c>
@@ -9330,7 +9347,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="12">
         <v>43938</v>
       </c>
@@ -9383,7 +9400,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="12">
         <v>43939</v>
       </c>
@@ -9436,7 +9453,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="30">
         <v>43940</v>
       </c>
@@ -9489,7 +9506,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="30">
         <v>43941</v>
       </c>
@@ -9542,7 +9559,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="30">
         <v>43942</v>
       </c>
@@ -9595,7 +9612,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="30">
         <v>43943</v>
       </c>
@@ -9648,7 +9665,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="30">
         <v>43944</v>
       </c>
@@ -9701,7 +9718,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="30">
         <v>43945</v>
       </c>
@@ -9754,7 +9771,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="30">
         <v>43946</v>
       </c>
@@ -9807,7 +9824,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="30">
         <v>43947</v>
       </c>
@@ -9860,7 +9877,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="30">
         <v>43948</v>
       </c>
@@ -9913,7 +9930,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="30">
         <v>43949</v>
       </c>
@@ -9966,7 +9983,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="30">
         <v>43950</v>
       </c>
@@ -10019,7 +10036,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="30">
         <v>43951</v>
       </c>
@@ -10072,7 +10089,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" s="30">
         <v>43952</v>
       </c>
@@ -10125,7 +10142,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="30">
         <v>43953</v>
       </c>
@@ -10178,7 +10195,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" s="30">
         <v>43954</v>
       </c>
@@ -10231,7 +10248,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="30">
         <v>43955</v>
       </c>
@@ -10284,7 +10301,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" s="30">
         <v>43956</v>
       </c>
@@ -10337,7 +10354,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" s="30">
         <v>43957</v>
       </c>
@@ -10390,7 +10407,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" s="30">
         <v>43958</v>
       </c>
@@ -10443,7 +10460,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" s="30">
         <v>43959</v>
       </c>
@@ -10496,7 +10513,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" s="30">
         <v>43960</v>
       </c>
@@ -10549,7 +10566,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" s="30">
         <v>43961</v>
       </c>
@@ -10602,7 +10619,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" s="30">
         <v>43962</v>
       </c>
@@ -10655,7 +10672,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" s="30">
         <v>43963</v>
       </c>
@@ -10708,7 +10725,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" s="30">
         <v>43964</v>
       </c>
@@ -10761,7 +10778,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" s="30">
         <v>43965</v>
       </c>
@@ -10814,7 +10831,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" s="30">
         <v>43966</v>
       </c>
@@ -10867,7 +10884,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" s="30">
         <v>43967</v>
       </c>
@@ -10920,7 +10937,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" s="30">
         <v>43968</v>
       </c>
@@ -10973,7 +10990,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" s="30">
         <v>43969</v>
       </c>
@@ -11026,7 +11043,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" s="30">
         <v>43970</v>
       </c>
@@ -11079,7 +11096,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" s="30">
         <v>43971</v>
       </c>
@@ -11132,7 +11149,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" s="30">
         <v>43972</v>
       </c>
@@ -11185,7 +11202,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" s="30">
         <v>43973</v>
       </c>
@@ -11238,7 +11255,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" s="30">
         <v>43974</v>
       </c>
@@ -11291,7 +11308,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" s="30">
         <v>43975</v>
       </c>
@@ -11344,7 +11361,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" s="30">
         <v>43976</v>
       </c>
@@ -11397,7 +11414,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" s="30">
         <v>43977</v>
       </c>
@@ -11450,7 +11467,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" s="30">
         <v>43978</v>
       </c>
@@ -11503,7 +11520,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75" s="30">
         <v>43979</v>
       </c>
@@ -11556,7 +11573,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76" s="30">
         <v>43980</v>
       </c>
@@ -11609,7 +11626,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77" s="30">
         <v>43981</v>
       </c>
@@ -11662,7 +11679,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78" s="30">
         <v>43982</v>
       </c>
@@ -11715,7 +11732,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79" s="30">
         <v>43983</v>
       </c>
@@ -11768,7 +11785,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A80" s="30">
         <v>43984</v>
       </c>
@@ -11821,7 +11838,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A81" s="30">
         <v>43985</v>
       </c>
@@ -11874,7 +11891,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A82" s="30">
         <v>43986</v>
       </c>
@@ -11927,7 +11944,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A83" s="30">
         <v>43987</v>
       </c>
@@ -11980,7 +11997,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A84" s="30">
         <v>43988</v>
       </c>
@@ -12033,7 +12050,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A85" s="30">
         <v>43989</v>
       </c>
@@ -12086,7 +12103,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A86" s="30">
         <v>43990</v>
       </c>
@@ -12137,6 +12154,59 @@
       </c>
       <c r="Q86" s="13">
         <v>24</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A87" s="30">
+        <v>43991</v>
+      </c>
+      <c r="B87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K87" s="11">
+        <v>6</v>
+      </c>
+      <c r="L87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P87" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q87" s="13">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -12147,23 +12217,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q78"/>
+  <dimension ref="A1:Q79"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B46" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B67" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5703125" style="2"/>
+    <col min="1" max="1" width="15.33203125" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.5546875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -12184,7 +12254,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -12205,7 +12275,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -12258,7 +12328,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>43916</v>
       </c>
@@ -12311,7 +12381,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>43917</v>
       </c>
@@ -12364,7 +12434,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>43918</v>
       </c>
@@ -12417,7 +12487,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>43919</v>
       </c>
@@ -12470,7 +12540,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>43920</v>
       </c>
@@ -12523,7 +12593,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>43921</v>
       </c>
@@ -12576,7 +12646,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>43922</v>
       </c>
@@ -12629,7 +12699,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>43923</v>
       </c>
@@ -12682,7 +12752,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
         <v>43924</v>
       </c>
@@ -12735,7 +12805,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>43925</v>
       </c>
@@ -12788,7 +12858,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>43926</v>
       </c>
@@ -12841,7 +12911,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>43927</v>
       </c>
@@ -12894,7 +12964,7 @@
         <v>1262</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>43928</v>
       </c>
@@ -12947,7 +13017,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>43929</v>
       </c>
@@ -13000,7 +13070,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>43930</v>
       </c>
@@ -13053,7 +13123,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>43931</v>
       </c>
@@ -13106,7 +13176,7 @@
         <v>1461</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>43932</v>
       </c>
@@ -13159,7 +13229,7 @@
         <v>1467</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>43933</v>
       </c>
@@ -13212,7 +13282,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="12">
         <v>43934</v>
       </c>
@@ -13265,7 +13335,7 @@
         <v>1482</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="12">
         <v>43935</v>
       </c>
@@ -13318,7 +13388,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="12">
         <v>43936</v>
       </c>
@@ -13371,7 +13441,7 @@
         <v>1486</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="12">
         <v>43937</v>
       </c>
@@ -13424,7 +13494,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="12">
         <v>43938</v>
       </c>
@@ -13477,7 +13547,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="12">
         <v>43939</v>
       </c>
@@ -13530,7 +13600,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="12">
         <v>43940</v>
       </c>
@@ -13583,7 +13653,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="12">
         <v>43941</v>
       </c>
@@ -13636,7 +13706,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <v>43942</v>
       </c>
@@ -13689,7 +13759,7 @@
         <v>1472</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="12">
         <v>43943</v>
       </c>
@@ -13742,7 +13812,7 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="12">
         <v>43944</v>
       </c>
@@ -13795,7 +13865,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="12">
         <v>43945</v>
       </c>
@@ -13848,7 +13918,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="12">
         <v>43946</v>
       </c>
@@ -13901,7 +13971,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="12">
         <v>43947</v>
       </c>
@@ -13954,7 +14024,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="30">
         <v>43948</v>
       </c>
@@ -14007,7 +14077,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="30">
         <v>43949</v>
       </c>
@@ -14060,7 +14130,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="30">
         <v>43950</v>
       </c>
@@ -14113,7 +14183,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="30">
         <v>43951</v>
       </c>
@@ -14166,7 +14236,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="30">
         <v>43952</v>
       </c>
@@ -14219,7 +14289,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="30">
         <v>43953</v>
       </c>
@@ -14272,7 +14342,7 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="30">
         <v>43954</v>
       </c>
@@ -14325,7 +14395,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="30">
         <v>43955</v>
       </c>
@@ -14378,7 +14448,7 @@
         <v>1279</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="30">
         <v>43956</v>
       </c>
@@ -14431,7 +14501,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="30">
         <v>43957</v>
       </c>
@@ -14484,7 +14554,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="30">
         <v>43958</v>
       </c>
@@ -14537,7 +14607,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="30">
         <v>43959</v>
       </c>
@@ -14590,7 +14660,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" s="30">
         <v>43960</v>
       </c>
@@ -14643,7 +14713,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="30">
         <v>43961</v>
       </c>
@@ -14696,7 +14766,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" s="30">
         <v>43962</v>
       </c>
@@ -14749,7 +14819,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="30">
         <v>43963</v>
       </c>
@@ -14802,7 +14872,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" s="30">
         <v>43964</v>
       </c>
@@ -14855,7 +14925,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" s="30">
         <v>43965</v>
       </c>
@@ -14908,7 +14978,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" s="30">
         <v>43966</v>
       </c>
@@ -14961,7 +15031,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" s="30">
         <v>43967</v>
       </c>
@@ -15014,7 +15084,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" s="30">
         <v>43968</v>
       </c>
@@ -15067,7 +15137,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" s="30">
         <v>43969</v>
       </c>
@@ -15120,7 +15190,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" s="30">
         <v>43970</v>
       </c>
@@ -15173,7 +15243,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" s="30">
         <v>43971</v>
       </c>
@@ -15226,7 +15296,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" s="30">
         <v>43972</v>
       </c>
@@ -15279,7 +15349,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" s="30">
         <v>43973</v>
       </c>
@@ -15332,7 +15402,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" s="30">
         <v>43974</v>
       </c>
@@ -15385,7 +15455,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" s="30">
         <v>43975</v>
       </c>
@@ -15438,7 +15508,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" s="30">
         <v>43976</v>
       </c>
@@ -15491,7 +15561,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" s="51">
         <v>43977</v>
       </c>
@@ -15544,7 +15614,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" s="51">
         <v>43978</v>
       </c>
@@ -15597,7 +15667,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" s="51">
         <v>43979</v>
       </c>
@@ -15650,7 +15720,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" s="51">
         <v>43980</v>
       </c>
@@ -15703,7 +15773,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" s="51">
         <v>43981</v>
       </c>
@@ -15756,7 +15826,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" s="51">
         <v>43982</v>
       </c>
@@ -15809,7 +15879,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" s="51">
         <v>43983</v>
       </c>
@@ -15862,7 +15932,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" s="51">
         <v>43984</v>
       </c>
@@ -15915,7 +15985,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" s="51">
         <v>43985</v>
       </c>
@@ -15968,7 +16038,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" s="51">
         <v>43986</v>
       </c>
@@ -16021,7 +16091,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75" s="51">
         <v>43987</v>
       </c>
@@ -16074,7 +16144,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76" s="51">
         <v>43988</v>
       </c>
@@ -16127,7 +16197,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77" s="51">
         <v>43989</v>
       </c>
@@ -16180,7 +16250,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78" s="51">
         <v>43990</v>
       </c>
@@ -16231,6 +16301,59 @@
       </c>
       <c r="Q78" s="13">
         <v>655</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A79" s="51">
+        <v>43991</v>
+      </c>
+      <c r="B79" s="11">
+        <v>11</v>
+      </c>
+      <c r="C79" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D79" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E79" s="11">
+        <v>52</v>
+      </c>
+      <c r="F79" s="11">
+        <v>10</v>
+      </c>
+      <c r="G79" s="11">
+        <v>62</v>
+      </c>
+      <c r="H79" s="11">
+        <v>289</v>
+      </c>
+      <c r="I79" s="11">
+        <v>8</v>
+      </c>
+      <c r="J79" s="11">
+        <v>56</v>
+      </c>
+      <c r="K79" s="11">
+        <v>145</v>
+      </c>
+      <c r="L79" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M79" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N79" s="11">
+        <v>8</v>
+      </c>
+      <c r="O79" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P79" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q79" s="13">
+        <v>641</v>
       </c>
     </row>
   </sheetData>
@@ -16241,23 +16364,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q78"/>
+  <dimension ref="A1:Q79"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B49" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B58" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5703125" style="2"/>
+    <col min="1" max="1" width="12.44140625" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.5546875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -16278,7 +16401,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -16299,7 +16422,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -16352,7 +16475,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>43916</v>
       </c>
@@ -16405,7 +16528,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>43917</v>
       </c>
@@ -16458,7 +16581,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>43918</v>
       </c>
@@ -16511,7 +16634,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>43919</v>
       </c>
@@ -16564,7 +16687,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>43920</v>
       </c>
@@ -16617,7 +16740,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>43921</v>
       </c>
@@ -16670,7 +16793,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>43922</v>
       </c>
@@ -16723,7 +16846,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>43923</v>
       </c>
@@ -16776,7 +16899,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
         <v>43924</v>
       </c>
@@ -16829,7 +16952,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>43925</v>
       </c>
@@ -16882,7 +17005,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>43926</v>
       </c>
@@ -16935,7 +17058,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>43927</v>
       </c>
@@ -16988,7 +17111,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>43928</v>
       </c>
@@ -17041,7 +17164,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>43929</v>
       </c>
@@ -17094,7 +17217,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>43930</v>
       </c>
@@ -17147,7 +17270,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>43931</v>
       </c>
@@ -17200,7 +17323,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>43932</v>
       </c>
@@ -17253,7 +17376,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>43933</v>
       </c>
@@ -17306,7 +17429,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="12">
         <v>43934</v>
       </c>
@@ -17359,7 +17482,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="12">
         <v>43935</v>
       </c>
@@ -17412,7 +17535,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="12">
         <v>43936</v>
       </c>
@@ -17465,7 +17588,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="12">
         <v>43937</v>
       </c>
@@ -17518,7 +17641,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="12">
         <v>43938</v>
       </c>
@@ -17571,7 +17694,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="12">
         <v>43939</v>
       </c>
@@ -17624,7 +17747,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="12">
         <v>43940</v>
       </c>
@@ -17677,7 +17800,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="12">
         <v>43941</v>
       </c>
@@ -17730,7 +17853,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <v>43942</v>
       </c>
@@ -17783,7 +17906,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="12">
         <v>43943</v>
       </c>
@@ -17836,7 +17959,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="12">
         <v>43944</v>
       </c>
@@ -17889,7 +18012,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="12">
         <v>43945</v>
       </c>
@@ -17942,7 +18065,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="12">
         <v>43946</v>
       </c>
@@ -17995,7 +18118,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="12">
         <v>43947</v>
       </c>
@@ -18048,7 +18171,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="30">
         <v>43948</v>
       </c>
@@ -18101,7 +18224,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="30">
         <v>43949</v>
       </c>
@@ -18154,7 +18277,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="30">
         <v>43950</v>
       </c>
@@ -18207,7 +18330,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="30">
         <v>43951</v>
       </c>
@@ -18260,7 +18383,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="30">
         <v>43952</v>
       </c>
@@ -18313,7 +18436,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="30">
         <v>43953</v>
       </c>
@@ -18366,7 +18489,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="30">
         <v>43954</v>
       </c>
@@ -18419,7 +18542,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="30">
         <v>43955</v>
       </c>
@@ -18472,7 +18595,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="30">
         <v>43956</v>
       </c>
@@ -18525,7 +18648,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="30">
         <v>43957</v>
       </c>
@@ -18578,7 +18701,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="30">
         <v>43958</v>
       </c>
@@ -18631,7 +18754,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="30">
         <v>43959</v>
       </c>
@@ -18684,7 +18807,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" s="30">
         <v>43960</v>
       </c>
@@ -18737,7 +18860,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="30">
         <v>43961</v>
       </c>
@@ -18790,7 +18913,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" s="30">
         <v>43962</v>
       </c>
@@ -18843,7 +18966,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="30">
         <v>43963</v>
       </c>
@@ -18896,7 +19019,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" s="30">
         <v>43964</v>
       </c>
@@ -18949,7 +19072,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" s="30">
         <v>43965</v>
       </c>
@@ -19002,7 +19125,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" s="30">
         <v>43966</v>
       </c>
@@ -19055,7 +19178,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" s="30">
         <v>43967</v>
       </c>
@@ -19108,7 +19231,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" s="30">
         <v>43968</v>
       </c>
@@ -19161,7 +19284,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" s="30">
         <v>43969</v>
       </c>
@@ -19214,7 +19337,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" s="30">
         <v>43970</v>
       </c>
@@ -19267,7 +19390,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" s="30">
         <v>43971</v>
       </c>
@@ -19320,7 +19443,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" s="30">
         <v>43972</v>
       </c>
@@ -19373,7 +19496,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" s="30">
         <v>43973</v>
       </c>
@@ -19426,7 +19549,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" s="30">
         <v>43974</v>
       </c>
@@ -19479,7 +19602,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" s="30">
         <v>43975</v>
       </c>
@@ -19532,7 +19655,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" s="30">
         <v>43976</v>
       </c>
@@ -19585,7 +19708,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" s="30">
         <v>43977</v>
       </c>
@@ -19638,7 +19761,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" s="30">
         <v>43978</v>
       </c>
@@ -19691,7 +19814,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" s="30">
         <v>43979</v>
       </c>
@@ -19744,7 +19867,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" s="30">
         <v>43980</v>
       </c>
@@ -19797,7 +19920,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" s="30">
         <v>43981</v>
       </c>
@@ -19850,7 +19973,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" s="30">
         <v>43982</v>
       </c>
@@ -19903,7 +20026,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" s="30">
         <v>43983</v>
       </c>
@@ -19956,7 +20079,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" s="30">
         <v>43984</v>
       </c>
@@ -20009,7 +20132,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" s="30">
         <v>43985</v>
       </c>
@@ -20062,7 +20185,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" s="30">
         <v>43986</v>
       </c>
@@ -20115,7 +20238,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75" s="30">
         <v>43987</v>
       </c>
@@ -20168,7 +20291,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76" s="30">
         <v>43988</v>
       </c>
@@ -20221,7 +20344,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77" s="30">
         <v>43989</v>
       </c>
@@ -20274,7 +20397,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78" s="30">
         <v>43990</v>
       </c>
@@ -20325,6 +20448,59 @@
       </c>
       <c r="Q78" s="13">
         <v>387</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A79" s="30">
+        <v>43991</v>
+      </c>
+      <c r="B79" s="11">
+        <v>19</v>
+      </c>
+      <c r="C79" s="11">
+        <v>18</v>
+      </c>
+      <c r="D79" s="11">
+        <v>18</v>
+      </c>
+      <c r="E79" s="11">
+        <v>17</v>
+      </c>
+      <c r="F79" s="11">
+        <v>24</v>
+      </c>
+      <c r="G79" s="11">
+        <v>9</v>
+      </c>
+      <c r="H79" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I79" s="11">
+        <v>11</v>
+      </c>
+      <c r="J79" s="11">
+        <v>58</v>
+      </c>
+      <c r="K79" s="11">
+        <v>181</v>
+      </c>
+      <c r="L79" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M79" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N79" s="11">
+        <v>13</v>
+      </c>
+      <c r="O79" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P79" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q79" s="13">
+        <v>370</v>
       </c>
     </row>
   </sheetData>
@@ -20357,7 +20533,7 @@
       <value order="0"/>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-08T12:32:35Z</value>
+      <value order="0">2020-06-09T12:29:11Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -20372,13 +20548,13 @@
       <value order="0">Being Drafted</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41607398</value>
+      <value order="0">vA41637421</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">22.2</value>
+      <value order="0">22.4</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">159</value>
+      <value order="0">161</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-10 20:08)
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U445783\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA18464\A28088333\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u419207\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA10434\A28088333\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5988" windowHeight="6036" tabRatio="803" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5990" windowHeight="6030" tabRatio="803" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1732" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1757" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -1636,21 +1636,21 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.44140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="90.44140625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.44140625" style="2"/>
+    <col min="2" max="2" width="29.453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="90.453125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B3" s="18" t="s">
         <v>20</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="20" t="s">
         <v>22</v>
       </c>
@@ -1666,13 +1666,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="22" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="23"/>
     </row>
-    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="24" t="s">
         <v>26</v>
       </c>
@@ -1680,7 +1680,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="24" t="s">
         <v>27</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="24" t="s">
         <v>36</v>
       </c>
@@ -1696,7 +1696,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="20" t="s">
         <v>37</v>
       </c>
@@ -1724,12 +1724,12 @@
       <selection activeCell="K66" sqref="K66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="9.44140625" style="2"/>
+    <col min="1" max="16384" width="9.453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="44" spans="1:1" ht="15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A44" s="43"/>
     </row>
   </sheetData>
@@ -1743,21 +1743,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S160"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="64" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B88" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="R93" sqref="R93"/>
+      <selection pane="bottomRight" activeCell="M101" sqref="M101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" style="2" customWidth="1"/>
-    <col min="2" max="16" width="11.44140625" style="11" customWidth="1"/>
-    <col min="17" max="16384" width="8.5546875" style="2"/>
+    <col min="2" max="16" width="11.453125" style="11" customWidth="1"/>
+    <col min="17" max="16384" width="8.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -1777,7 +1777,7 @@
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -1796,7 +1796,7 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>43897</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>43898</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>43899</v>
       </c>
@@ -1996,7 +1996,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>43900</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>43901</v>
       </c>
@@ -2096,7 +2096,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>43902</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>43903</v>
       </c>
@@ -2196,7 +2196,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>43904</v>
       </c>
@@ -2246,7 +2246,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>43905</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>43906</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>43907</v>
       </c>
@@ -2396,7 +2396,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>43908</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>43909</v>
       </c>
@@ -2496,7 +2496,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>43910</v>
       </c>
@@ -2546,7 +2546,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>43911</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>43912</v>
       </c>
@@ -2646,7 +2646,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>43913</v>
       </c>
@@ -2696,7 +2696,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>43914</v>
       </c>
@@ -2746,7 +2746,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>43915</v>
       </c>
@@ -2796,7 +2796,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>43916</v>
       </c>
@@ -2846,7 +2846,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>43917</v>
       </c>
@@ -2896,7 +2896,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>43918</v>
       </c>
@@ -2946,7 +2946,7 @@
         <v>1264</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>43919</v>
       </c>
@@ -2996,7 +2996,7 @@
         <v>1417</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>43920</v>
       </c>
@@ -3046,7 +3046,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>43921</v>
       </c>
@@ -3096,7 +3096,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>43922</v>
       </c>
@@ -3146,7 +3146,7 @@
         <v>2310</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>43923</v>
       </c>
@@ -3196,7 +3196,7 @@
         <v>2602</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>43924</v>
       </c>
@@ -3246,7 +3246,7 @@
         <v>3001</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>43925</v>
       </c>
@@ -3296,7 +3296,7 @@
         <v>3345</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>43926</v>
       </c>
@@ -3346,7 +3346,7 @@
         <v>3706</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>43927</v>
       </c>
@@ -3396,7 +3396,7 @@
         <v>3961</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>43928</v>
       </c>
@@ -3446,7 +3446,7 @@
         <v>4229</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>43929</v>
       </c>
@@ -3496,7 +3496,7 @@
         <v>4565</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>43930</v>
       </c>
@@ -3546,7 +3546,7 @@
         <v>4957</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>43931</v>
       </c>
@@ -3596,7 +3596,7 @@
         <v>5275</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>43932</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>5590</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>43933</v>
       </c>
@@ -3696,7 +3696,7 @@
         <v>5912</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>43934</v>
       </c>
@@ -3746,7 +3746,7 @@
         <v>6067</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>43935</v>
       </c>
@@ -3796,7 +3796,7 @@
         <v>6358</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>43936</v>
       </c>
@@ -3846,7 +3846,7 @@
         <v>6748</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
         <v>43937</v>
       </c>
@@ -3896,7 +3896,7 @@
         <v>7102</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>43938</v>
       </c>
@@ -3946,7 +3946,7 @@
         <v>7409</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A46" s="5">
         <v>43939</v>
       </c>
@@ -3996,7 +3996,7 @@
         <v>7820</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A47" s="5">
         <v>43940</v>
       </c>
@@ -4046,7 +4046,7 @@
         <v>8187</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A48" s="5">
         <v>43941</v>
       </c>
@@ -4096,7 +4096,7 @@
         <v>8450</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A49" s="5">
         <v>43942</v>
       </c>
@@ -4146,7 +4146,7 @@
         <v>8672</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
         <v>43943</v>
       </c>
@@ -4196,7 +4196,7 @@
         <v>9038</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
         <v>43944</v>
       </c>
@@ -4246,7 +4246,7 @@
         <v>9409</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
         <v>43945</v>
       </c>
@@ -4296,7 +4296,7 @@
         <v>9697</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
         <v>43946</v>
       </c>
@@ -4346,7 +4346,7 @@
         <v>10051</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A54" s="5">
         <v>43947</v>
       </c>
@@ -4397,7 +4397,7 @@
       </c>
       <c r="R54" s="38"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
         <v>43948</v>
       </c>
@@ -4448,7 +4448,7 @@
       </c>
       <c r="R55" s="38"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A56" s="5">
         <v>43949</v>
       </c>
@@ -4499,7 +4499,7 @@
       </c>
       <c r="R56" s="39"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
         <v>43950</v>
       </c>
@@ -4549,7 +4549,7 @@
         <v>11034</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
         <v>43951</v>
       </c>
@@ -4600,7 +4600,7 @@
       </c>
       <c r="R58" s="38"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>43952</v>
       </c>
@@ -4652,7 +4652,7 @@
       <c r="R59" s="38"/>
       <c r="S59" s="38"/>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
         <v>43953</v>
       </c>
@@ -4702,7 +4702,7 @@
         <v>11927</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
         <v>43954</v>
       </c>
@@ -4752,7 +4752,7 @@
         <v>12097</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A62" s="5">
         <v>43955</v>
       </c>
@@ -4802,7 +4802,7 @@
         <v>12266</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A63" s="5">
         <v>43956</v>
       </c>
@@ -4852,7 +4852,7 @@
         <v>12437</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
         <v>43957</v>
       </c>
@@ -4902,7 +4902,7 @@
         <v>12709</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>43958</v>
       </c>
@@ -4952,7 +4952,7 @@
         <v>12924</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
         <v>43959</v>
       </c>
@@ -5002,7 +5002,7 @@
         <v>13149</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
         <v>43960</v>
       </c>
@@ -5052,7 +5052,7 @@
         <v>13305</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A68" s="5">
         <v>43961</v>
       </c>
@@ -5102,7 +5102,7 @@
         <v>13486</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A69" s="5">
         <v>43962</v>
       </c>
@@ -5152,7 +5152,7 @@
         <v>13627</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A70" s="5">
         <v>43963</v>
       </c>
@@ -5202,7 +5202,7 @@
         <v>13763</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A71" s="5">
         <v>43964</v>
       </c>
@@ -5252,7 +5252,7 @@
         <v>13929</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A72" s="5">
         <v>43965</v>
       </c>
@@ -5302,7 +5302,7 @@
         <v>14117</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A73" s="5">
         <v>43966</v>
       </c>
@@ -5352,7 +5352,7 @@
         <v>14260</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A74" s="5">
         <v>43967</v>
       </c>
@@ -5402,7 +5402,7 @@
         <v>14447</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A75" s="5">
         <v>43968</v>
       </c>
@@ -5452,7 +5452,7 @@
         <v>14537</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A76" s="5">
         <v>43969</v>
       </c>
@@ -5502,7 +5502,7 @@
         <v>14594</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A77" s="5">
         <v>43970</v>
       </c>
@@ -5552,7 +5552,7 @@
         <v>14655</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A78" s="5">
         <v>43971</v>
       </c>
@@ -5602,7 +5602,7 @@
         <v>14751</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A79" s="5">
         <v>43972</v>
       </c>
@@ -5652,7 +5652,7 @@
         <v>14856</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A80" s="5">
         <v>43973</v>
       </c>
@@ -5702,7 +5702,7 @@
         <v>14969</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A81" s="5">
         <v>43974</v>
       </c>
@@ -5752,7 +5752,7 @@
         <v>15041</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A82" s="5">
         <v>43975</v>
       </c>
@@ -5802,7 +5802,7 @@
         <v>15101</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A83" s="5">
         <v>43976</v>
       </c>
@@ -5852,7 +5852,7 @@
         <v>15156</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A84" s="5">
         <v>43977</v>
       </c>
@@ -5902,7 +5902,7 @@
         <v>15185</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A85" s="5">
         <v>43978</v>
       </c>
@@ -5952,7 +5952,7 @@
         <v>15240</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A86" s="5">
         <v>43979</v>
       </c>
@@ -6002,7 +6002,7 @@
         <v>15288</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A87" s="5">
         <v>43980</v>
       </c>
@@ -6052,7 +6052,7 @@
         <v>15327</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A88" s="5">
         <v>43981</v>
       </c>
@@ -6102,7 +6102,7 @@
         <v>15382</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A89" s="5">
         <v>43982</v>
       </c>
@@ -6152,7 +6152,7 @@
         <v>15400</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A90" s="5">
         <v>43983</v>
       </c>
@@ -6202,7 +6202,7 @@
         <v>15418</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A91" s="5">
         <v>43984</v>
       </c>
@@ -6252,7 +6252,7 @@
         <v>15471</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A92" s="5">
         <v>43985</v>
       </c>
@@ -6302,7 +6302,7 @@
         <v>15504</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A93" s="5">
         <v>43986</v>
       </c>
@@ -6352,7 +6352,7 @@
         <v>15553</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A94" s="5">
         <v>43987</v>
       </c>
@@ -6402,7 +6402,7 @@
         <v>15582</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A95" s="5">
         <v>43988</v>
       </c>
@@ -6452,7 +6452,7 @@
         <v>15603</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A96" s="5">
         <v>43989</v>
       </c>
@@ -6502,7 +6502,7 @@
         <v>15621</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A97" s="5">
         <v>43990</v>
       </c>
@@ -6552,7 +6552,7 @@
         <v>15639</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A98" s="5">
         <v>43991</v>
       </c>
@@ -6602,23 +6602,57 @@
         <v>15653</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="C99" s="28"/>
-      <c r="D99" s="28"/>
-      <c r="E99" s="28"/>
-      <c r="F99" s="28"/>
-      <c r="G99" s="28"/>
-      <c r="H99" s="28"/>
-      <c r="I99" s="28"/>
-      <c r="J99" s="28"/>
-      <c r="K99" s="28"/>
-      <c r="L99" s="28"/>
-      <c r="M99" s="28"/>
-      <c r="N99" s="28"/>
-      <c r="O99" s="28"/>
-      <c r="P99" s="28"/>
-    </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A99" s="5">
+        <v>43992</v>
+      </c>
+      <c r="B99" s="28">
+        <v>1081</v>
+      </c>
+      <c r="C99" s="28">
+        <v>327</v>
+      </c>
+      <c r="D99" s="28">
+        <v>261</v>
+      </c>
+      <c r="E99" s="28">
+        <v>880</v>
+      </c>
+      <c r="F99" s="28">
+        <v>948</v>
+      </c>
+      <c r="G99" s="28">
+        <v>1287</v>
+      </c>
+      <c r="H99" s="28">
+        <v>3990</v>
+      </c>
+      <c r="I99" s="28">
+        <v>340</v>
+      </c>
+      <c r="J99" s="28">
+        <v>2021</v>
+      </c>
+      <c r="K99" s="28">
+        <v>2778</v>
+      </c>
+      <c r="L99" s="28">
+        <v>8</v>
+      </c>
+      <c r="M99" s="28">
+        <v>54</v>
+      </c>
+      <c r="N99" s="28">
+        <v>1684</v>
+      </c>
+      <c r="O99" s="28">
+        <v>6</v>
+      </c>
+      <c r="P99" s="32">
+        <v>15665</v>
+      </c>
+    </row>
+    <row r="100" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C100" s="28"/>
       <c r="D100" s="28"/>
       <c r="E100" s="28"/>
@@ -6634,7 +6668,7 @@
       <c r="O100" s="28"/>
       <c r="P100" s="28"/>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C101" s="28"/>
       <c r="D101" s="28"/>
       <c r="E101" s="28"/>
@@ -6650,7 +6684,7 @@
       <c r="O101" s="28"/>
       <c r="P101" s="28"/>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C102" s="28"/>
       <c r="D102" s="28"/>
       <c r="E102" s="28"/>
@@ -6666,7 +6700,7 @@
       <c r="O102" s="28"/>
       <c r="P102" s="28"/>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C103" s="28"/>
       <c r="D103" s="28"/>
       <c r="E103" s="28"/>
@@ -6682,7 +6716,7 @@
       <c r="O103" s="28"/>
       <c r="P103" s="28"/>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C104" s="28"/>
       <c r="D104" s="28"/>
       <c r="E104" s="28"/>
@@ -6698,7 +6732,7 @@
       <c r="O104" s="28"/>
       <c r="P104" s="28"/>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C105" s="28"/>
       <c r="D105" s="28"/>
       <c r="E105" s="28"/>
@@ -6714,7 +6748,7 @@
       <c r="O105" s="28"/>
       <c r="P105" s="28"/>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C106" s="28"/>
       <c r="D106" s="28"/>
       <c r="E106" s="28"/>
@@ -6730,7 +6764,7 @@
       <c r="O106" s="28"/>
       <c r="P106" s="28"/>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C107" s="28"/>
       <c r="D107" s="28"/>
       <c r="E107" s="28"/>
@@ -6746,7 +6780,7 @@
       <c r="O107" s="28"/>
       <c r="P107" s="28"/>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C108" s="28"/>
       <c r="D108" s="28"/>
       <c r="E108" s="28"/>
@@ -6762,7 +6796,7 @@
       <c r="O108" s="28"/>
       <c r="P108" s="28"/>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C109" s="28"/>
       <c r="D109" s="28"/>
       <c r="E109" s="28"/>
@@ -6778,7 +6812,7 @@
       <c r="O109" s="28"/>
       <c r="P109" s="28"/>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C110" s="28"/>
       <c r="D110" s="28"/>
       <c r="E110" s="28"/>
@@ -6794,7 +6828,7 @@
       <c r="O110" s="28"/>
       <c r="P110" s="28"/>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C111" s="28"/>
       <c r="D111" s="28"/>
       <c r="E111" s="28"/>
@@ -6810,7 +6844,7 @@
       <c r="O111" s="28"/>
       <c r="P111" s="28"/>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C112" s="28"/>
       <c r="D112" s="28"/>
       <c r="E112" s="28"/>
@@ -6826,7 +6860,7 @@
       <c r="O112" s="28"/>
       <c r="P112" s="28"/>
     </row>
-    <row r="113" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:16" x14ac:dyDescent="0.35">
       <c r="C113" s="28"/>
       <c r="D113" s="28"/>
       <c r="E113" s="28"/>
@@ -6842,7 +6876,7 @@
       <c r="O113" s="28"/>
       <c r="P113" s="28"/>
     </row>
-    <row r="114" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:16" x14ac:dyDescent="0.35">
       <c r="C114" s="28"/>
       <c r="D114" s="28"/>
       <c r="E114" s="28"/>
@@ -6858,7 +6892,7 @@
       <c r="O114" s="28"/>
       <c r="P114" s="28"/>
     </row>
-    <row r="115" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B115" s="28"/>
       <c r="C115" s="28"/>
       <c r="D115" s="28"/>
@@ -6875,7 +6909,7 @@
       <c r="O115" s="28"/>
       <c r="P115" s="28"/>
     </row>
-    <row r="116" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B116" s="28"/>
       <c r="C116" s="28"/>
       <c r="D116" s="28"/>
@@ -6892,7 +6926,7 @@
       <c r="O116" s="28"/>
       <c r="P116" s="28"/>
     </row>
-    <row r="117" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B117" s="28"/>
       <c r="C117" s="28"/>
       <c r="D117" s="28"/>
@@ -6909,7 +6943,7 @@
       <c r="O117" s="28"/>
       <c r="P117" s="28"/>
     </row>
-    <row r="118" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B118" s="28"/>
       <c r="C118" s="28"/>
       <c r="D118" s="28"/>
@@ -6926,7 +6960,7 @@
       <c r="O118" s="28"/>
       <c r="P118" s="28"/>
     </row>
-    <row r="119" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B119" s="28"/>
       <c r="C119" s="28"/>
       <c r="D119" s="28"/>
@@ -6943,7 +6977,7 @@
       <c r="O119" s="28"/>
       <c r="P119" s="28"/>
     </row>
-    <row r="120" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B120" s="28"/>
       <c r="C120" s="28"/>
       <c r="D120" s="28"/>
@@ -6960,7 +6994,7 @@
       <c r="O120" s="28"/>
       <c r="P120" s="28"/>
     </row>
-    <row r="121" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B121" s="28"/>
       <c r="C121" s="28"/>
       <c r="D121" s="28"/>
@@ -6977,7 +7011,7 @@
       <c r="O121" s="28"/>
       <c r="P121" s="28"/>
     </row>
-    <row r="122" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B122" s="28"/>
       <c r="C122" s="28"/>
       <c r="D122" s="28"/>
@@ -6994,7 +7028,7 @@
       <c r="O122" s="28"/>
       <c r="P122" s="28"/>
     </row>
-    <row r="123" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B123" s="28"/>
       <c r="C123" s="28"/>
       <c r="D123" s="28"/>
@@ -7011,7 +7045,7 @@
       <c r="O123" s="28"/>
       <c r="P123" s="28"/>
     </row>
-    <row r="124" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B124" s="28"/>
       <c r="C124" s="28"/>
       <c r="D124" s="28"/>
@@ -7028,7 +7062,7 @@
       <c r="O124" s="28"/>
       <c r="P124" s="28"/>
     </row>
-    <row r="125" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B125" s="28"/>
       <c r="C125" s="28"/>
       <c r="D125" s="28"/>
@@ -7045,7 +7079,7 @@
       <c r="O125" s="28"/>
       <c r="P125" s="28"/>
     </row>
-    <row r="126" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B126" s="28"/>
       <c r="C126" s="28"/>
       <c r="D126" s="28"/>
@@ -7062,7 +7096,7 @@
       <c r="O126" s="28"/>
       <c r="P126" s="28"/>
     </row>
-    <row r="127" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B127" s="28"/>
       <c r="C127" s="28"/>
       <c r="D127" s="28"/>
@@ -7079,7 +7113,7 @@
       <c r="O127" s="28"/>
       <c r="P127" s="28"/>
     </row>
-    <row r="128" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B128" s="28"/>
       <c r="C128" s="28"/>
       <c r="D128" s="28"/>
@@ -7096,7 +7130,7 @@
       <c r="O128" s="28"/>
       <c r="P128" s="28"/>
     </row>
-    <row r="129" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B129" s="28"/>
       <c r="C129" s="28"/>
       <c r="D129" s="28"/>
@@ -7113,7 +7147,7 @@
       <c r="O129" s="28"/>
       <c r="P129" s="28"/>
     </row>
-    <row r="130" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B130" s="28"/>
       <c r="C130" s="28"/>
       <c r="D130" s="28"/>
@@ -7130,7 +7164,7 @@
       <c r="O130" s="28"/>
       <c r="P130" s="28"/>
     </row>
-    <row r="131" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B131" s="28"/>
       <c r="C131" s="28"/>
       <c r="D131" s="28"/>
@@ -7147,7 +7181,7 @@
       <c r="O131" s="28"/>
       <c r="P131" s="28"/>
     </row>
-    <row r="132" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B132" s="28"/>
       <c r="C132" s="28"/>
       <c r="D132" s="28"/>
@@ -7164,7 +7198,7 @@
       <c r="O132" s="28"/>
       <c r="P132" s="28"/>
     </row>
-    <row r="133" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B133" s="28"/>
       <c r="C133" s="28"/>
       <c r="D133" s="28"/>
@@ -7181,7 +7215,7 @@
       <c r="O133" s="28"/>
       <c r="P133" s="28"/>
     </row>
-    <row r="134" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B134" s="28"/>
       <c r="C134" s="28"/>
       <c r="D134" s="28"/>
@@ -7198,7 +7232,7 @@
       <c r="O134" s="28"/>
       <c r="P134" s="28"/>
     </row>
-    <row r="135" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B135" s="28"/>
       <c r="C135" s="28"/>
       <c r="D135" s="28"/>
@@ -7215,7 +7249,7 @@
       <c r="O135" s="28"/>
       <c r="P135" s="28"/>
     </row>
-    <row r="136" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B136" s="28"/>
       <c r="C136" s="28"/>
       <c r="D136" s="28"/>
@@ -7232,7 +7266,7 @@
       <c r="O136" s="28"/>
       <c r="P136" s="28"/>
     </row>
-    <row r="137" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B137" s="28"/>
       <c r="C137" s="28"/>
       <c r="D137" s="28"/>
@@ -7249,7 +7283,7 @@
       <c r="O137" s="28"/>
       <c r="P137" s="28"/>
     </row>
-    <row r="138" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B138" s="28"/>
       <c r="C138" s="28"/>
       <c r="D138" s="28"/>
@@ -7266,7 +7300,7 @@
       <c r="O138" s="28"/>
       <c r="P138" s="28"/>
     </row>
-    <row r="139" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B139" s="28"/>
       <c r="C139" s="28"/>
       <c r="D139" s="28"/>
@@ -7283,7 +7317,7 @@
       <c r="O139" s="28"/>
       <c r="P139" s="28"/>
     </row>
-    <row r="140" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B140" s="28"/>
       <c r="C140" s="28"/>
       <c r="D140" s="28"/>
@@ -7300,7 +7334,7 @@
       <c r="O140" s="28"/>
       <c r="P140" s="28"/>
     </row>
-    <row r="141" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B141" s="28"/>
       <c r="C141" s="28"/>
       <c r="D141" s="28"/>
@@ -7317,7 +7351,7 @@
       <c r="O141" s="28"/>
       <c r="P141" s="28"/>
     </row>
-    <row r="142" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B142" s="28"/>
       <c r="C142" s="28"/>
       <c r="D142" s="28"/>
@@ -7334,7 +7368,7 @@
       <c r="O142" s="28"/>
       <c r="P142" s="28"/>
     </row>
-    <row r="143" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B143" s="28"/>
       <c r="C143" s="28"/>
       <c r="D143" s="28"/>
@@ -7351,7 +7385,7 @@
       <c r="O143" s="28"/>
       <c r="P143" s="28"/>
     </row>
-    <row r="144" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B144" s="28"/>
       <c r="C144" s="28"/>
       <c r="D144" s="28"/>
@@ -7368,7 +7402,7 @@
       <c r="O144" s="28"/>
       <c r="P144" s="28"/>
     </row>
-    <row r="145" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B145" s="28"/>
       <c r="C145" s="28"/>
       <c r="D145" s="28"/>
@@ -7385,7 +7419,7 @@
       <c r="O145" s="28"/>
       <c r="P145" s="28"/>
     </row>
-    <row r="146" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B146" s="28"/>
       <c r="C146" s="28"/>
       <c r="D146" s="28"/>
@@ -7402,7 +7436,7 @@
       <c r="O146" s="28"/>
       <c r="P146" s="28"/>
     </row>
-    <row r="147" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B147" s="28"/>
       <c r="C147" s="28"/>
       <c r="D147" s="28"/>
@@ -7419,7 +7453,7 @@
       <c r="O147" s="28"/>
       <c r="P147" s="28"/>
     </row>
-    <row r="148" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B148" s="28"/>
       <c r="C148" s="28"/>
       <c r="D148" s="28"/>
@@ -7436,7 +7470,7 @@
       <c r="O148" s="28"/>
       <c r="P148" s="28"/>
     </row>
-    <row r="149" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B149" s="28"/>
       <c r="C149" s="28"/>
       <c r="D149" s="28"/>
@@ -7453,7 +7487,7 @@
       <c r="O149" s="28"/>
       <c r="P149" s="28"/>
     </row>
-    <row r="150" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B150" s="28"/>
       <c r="C150" s="28"/>
       <c r="D150" s="28"/>
@@ -7470,7 +7504,7 @@
       <c r="O150" s="28"/>
       <c r="P150" s="28"/>
     </row>
-    <row r="151" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B151" s="28"/>
       <c r="C151" s="28"/>
       <c r="D151" s="28"/>
@@ -7487,7 +7521,7 @@
       <c r="O151" s="28"/>
       <c r="P151" s="28"/>
     </row>
-    <row r="152" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B152" s="28"/>
       <c r="C152" s="28"/>
       <c r="D152" s="28"/>
@@ -7504,7 +7538,7 @@
       <c r="O152" s="28"/>
       <c r="P152" s="28"/>
     </row>
-    <row r="153" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B153" s="28"/>
       <c r="C153" s="28"/>
       <c r="D153" s="28"/>
@@ -7521,7 +7555,7 @@
       <c r="O153" s="28"/>
       <c r="P153" s="28"/>
     </row>
-    <row r="154" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B154" s="28"/>
       <c r="C154" s="28"/>
       <c r="D154" s="28"/>
@@ -7538,7 +7572,7 @@
       <c r="O154" s="28"/>
       <c r="P154" s="28"/>
     </row>
-    <row r="155" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B155" s="28"/>
       <c r="C155" s="28"/>
       <c r="D155" s="28"/>
@@ -7555,7 +7589,7 @@
       <c r="O155" s="28"/>
       <c r="P155" s="28"/>
     </row>
-    <row r="156" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B156" s="28"/>
       <c r="C156" s="28"/>
       <c r="D156" s="28"/>
@@ -7572,7 +7606,7 @@
       <c r="O156" s="28"/>
       <c r="P156" s="28"/>
     </row>
-    <row r="157" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B157" s="28"/>
       <c r="C157" s="28"/>
       <c r="D157" s="28"/>
@@ -7589,7 +7623,7 @@
       <c r="O157" s="28"/>
       <c r="P157" s="28"/>
     </row>
-    <row r="158" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B158" s="28"/>
       <c r="C158" s="28"/>
       <c r="D158" s="28"/>
@@ -7606,7 +7640,7 @@
       <c r="O158" s="28"/>
       <c r="P158" s="28"/>
     </row>
-    <row r="159" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B159" s="28"/>
       <c r="C159" s="28"/>
       <c r="D159" s="28"/>
@@ -7623,7 +7657,7 @@
       <c r="O159" s="28"/>
       <c r="P159" s="28"/>
     </row>
-    <row r="160" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B160" s="28"/>
       <c r="C160" s="28"/>
       <c r="D160" s="28"/>
@@ -7648,21 +7682,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q87"/>
+  <dimension ref="A1:Q88"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A87" sqref="A87"/>
+      <selection pane="bottomLeft" activeCell="M91" sqref="M91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5546875" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5546875" style="2"/>
+    <col min="1" max="1" width="12.453125" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.54296875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -7683,7 +7717,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -7704,7 +7738,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -7757,7 +7791,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="12">
         <v>43908</v>
       </c>
@@ -7810,7 +7844,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
         <v>43909</v>
       </c>
@@ -7863,7 +7897,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="12">
         <v>43910</v>
       </c>
@@ -7916,7 +7950,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
         <v>43911</v>
       </c>
@@ -7969,7 +8003,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="12">
         <v>43912</v>
       </c>
@@ -8022,7 +8056,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="12">
         <v>43913</v>
       </c>
@@ -8075,7 +8109,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="12">
         <v>43914</v>
       </c>
@@ -8128,7 +8162,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
         <v>43915</v>
       </c>
@@ -8181,7 +8215,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="12">
         <v>43916</v>
       </c>
@@ -8234,7 +8268,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <v>43917</v>
       </c>
@@ -8287,7 +8321,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>43918</v>
       </c>
@@ -8340,7 +8374,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="12">
         <v>43919</v>
       </c>
@@ -8393,7 +8427,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="12">
         <v>43920</v>
       </c>
@@ -8446,7 +8480,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="12">
         <v>43921</v>
       </c>
@@ -8499,7 +8533,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="12">
         <v>43922</v>
       </c>
@@ -8552,7 +8586,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="12">
         <v>43923</v>
       </c>
@@ -8605,7 +8639,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="12">
         <v>43924</v>
       </c>
@@ -8658,7 +8692,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="12">
         <v>43925</v>
       </c>
@@ -8711,7 +8745,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="12">
         <v>43926</v>
       </c>
@@ -8764,7 +8798,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="12">
         <v>43927</v>
       </c>
@@ -8817,7 +8851,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" s="12">
         <v>43928</v>
       </c>
@@ -8870,7 +8904,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" s="12">
         <v>43929</v>
       </c>
@@ -8923,7 +8957,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" s="12">
         <v>43930</v>
       </c>
@@ -8976,7 +9010,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" s="12">
         <v>43931</v>
       </c>
@@ -9029,7 +9063,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" s="12">
         <v>43932</v>
       </c>
@@ -9082,7 +9116,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" s="12">
         <v>43933</v>
       </c>
@@ -9135,7 +9169,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" s="12">
         <v>43934</v>
       </c>
@@ -9188,7 +9222,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="12">
         <v>43935</v>
       </c>
@@ -9241,7 +9275,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" s="12">
         <v>43936</v>
       </c>
@@ -9294,7 +9328,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" s="12">
         <v>43937</v>
       </c>
@@ -9347,7 +9381,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" s="12">
         <v>43938</v>
       </c>
@@ -9400,7 +9434,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" s="12">
         <v>43939</v>
       </c>
@@ -9453,7 +9487,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" s="30">
         <v>43940</v>
       </c>
@@ -9506,7 +9540,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" s="30">
         <v>43941</v>
       </c>
@@ -9559,7 +9593,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" s="30">
         <v>43942</v>
       </c>
@@ -9612,7 +9646,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" s="30">
         <v>43943</v>
       </c>
@@ -9665,7 +9699,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" s="30">
         <v>43944</v>
       </c>
@@ -9718,7 +9752,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" s="30">
         <v>43945</v>
       </c>
@@ -9771,7 +9805,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" s="30">
         <v>43946</v>
       </c>
@@ -9824,7 +9858,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" s="30">
         <v>43947</v>
       </c>
@@ -9877,7 +9911,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" s="30">
         <v>43948</v>
       </c>
@@ -9930,7 +9964,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" s="30">
         <v>43949</v>
       </c>
@@ -9983,7 +10017,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" s="30">
         <v>43950</v>
       </c>
@@ -10036,7 +10070,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" s="30">
         <v>43951</v>
       </c>
@@ -10089,7 +10123,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" s="30">
         <v>43952</v>
       </c>
@@ -10142,7 +10176,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" s="30">
         <v>43953</v>
       </c>
@@ -10195,7 +10229,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50" s="30">
         <v>43954</v>
       </c>
@@ -10248,7 +10282,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51" s="30">
         <v>43955</v>
       </c>
@@ -10301,7 +10335,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52" s="30">
         <v>43956</v>
       </c>
@@ -10354,7 +10388,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53" s="30">
         <v>43957</v>
       </c>
@@ -10407,7 +10441,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54" s="30">
         <v>43958</v>
       </c>
@@ -10460,7 +10494,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55" s="30">
         <v>43959</v>
       </c>
@@ -10513,7 +10547,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56" s="30">
         <v>43960</v>
       </c>
@@ -10566,7 +10600,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A57" s="30">
         <v>43961</v>
       </c>
@@ -10619,7 +10653,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A58" s="30">
         <v>43962</v>
       </c>
@@ -10672,7 +10706,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A59" s="30">
         <v>43963</v>
       </c>
@@ -10725,7 +10759,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A60" s="30">
         <v>43964</v>
       </c>
@@ -10778,7 +10812,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A61" s="30">
         <v>43965</v>
       </c>
@@ -10831,7 +10865,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A62" s="30">
         <v>43966</v>
       </c>
@@ -10884,7 +10918,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A63" s="30">
         <v>43967</v>
       </c>
@@ -10937,7 +10971,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A64" s="30">
         <v>43968</v>
       </c>
@@ -10990,7 +11024,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A65" s="30">
         <v>43969</v>
       </c>
@@ -11043,7 +11077,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A66" s="30">
         <v>43970</v>
       </c>
@@ -11096,7 +11130,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A67" s="30">
         <v>43971</v>
       </c>
@@ -11149,7 +11183,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A68" s="30">
         <v>43972</v>
       </c>
@@ -11202,7 +11236,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A69" s="30">
         <v>43973</v>
       </c>
@@ -11255,7 +11289,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A70" s="30">
         <v>43974</v>
       </c>
@@ -11308,7 +11342,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A71" s="30">
         <v>43975</v>
       </c>
@@ -11361,7 +11395,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A72" s="30">
         <v>43976</v>
       </c>
@@ -11414,7 +11448,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A73" s="30">
         <v>43977</v>
       </c>
@@ -11467,7 +11501,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A74" s="30">
         <v>43978</v>
       </c>
@@ -11520,7 +11554,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A75" s="30">
         <v>43979</v>
       </c>
@@ -11573,7 +11607,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A76" s="30">
         <v>43980</v>
       </c>
@@ -11626,7 +11660,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A77" s="30">
         <v>43981</v>
       </c>
@@ -11679,7 +11713,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A78" s="30">
         <v>43982</v>
       </c>
@@ -11732,7 +11766,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A79" s="30">
         <v>43983</v>
       </c>
@@ -11785,7 +11819,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A80" s="30">
         <v>43984</v>
       </c>
@@ -11838,7 +11872,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A81" s="30">
         <v>43985</v>
       </c>
@@ -11891,7 +11925,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A82" s="30">
         <v>43986</v>
       </c>
@@ -11944,7 +11978,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A83" s="30">
         <v>43987</v>
       </c>
@@ -11997,7 +12031,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A84" s="30">
         <v>43988</v>
       </c>
@@ -12050,7 +12084,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A85" s="30">
         <v>43989</v>
       </c>
@@ -12103,7 +12137,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A86" s="30">
         <v>43990</v>
       </c>
@@ -12156,7 +12190,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A87" s="30">
         <v>43991</v>
       </c>
@@ -12207,6 +12241,59 @@
       </c>
       <c r="Q87" s="13">
         <v>21</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A88" s="30">
+        <v>43992</v>
+      </c>
+      <c r="B88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K88" s="11">
+        <v>5</v>
+      </c>
+      <c r="L88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P88" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q88" s="13">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -12217,23 +12304,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q79"/>
+  <dimension ref="A1:Q80"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B67" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A79" sqref="A79"/>
+      <selection pane="bottomRight" activeCell="N83" sqref="N83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5546875" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5546875" style="2"/>
+    <col min="1" max="1" width="15.26953125" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.54296875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -12254,7 +12341,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -12275,7 +12362,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -12328,7 +12415,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="12">
         <v>43916</v>
       </c>
@@ -12381,7 +12468,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
         <v>43917</v>
       </c>
@@ -12434,7 +12521,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="12">
         <v>43918</v>
       </c>
@@ -12487,7 +12574,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
         <v>43919</v>
       </c>
@@ -12540,7 +12627,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="12">
         <v>43920</v>
       </c>
@@ -12593,7 +12680,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="12">
         <v>43921</v>
       </c>
@@ -12646,7 +12733,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="12">
         <v>43922</v>
       </c>
@@ -12699,7 +12786,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
         <v>43923</v>
       </c>
@@ -12752,7 +12839,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="12">
         <v>43924</v>
       </c>
@@ -12805,7 +12892,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <v>43925</v>
       </c>
@@ -12858,7 +12945,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>43926</v>
       </c>
@@ -12911,7 +12998,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="12">
         <v>43927</v>
       </c>
@@ -12964,7 +13051,7 @@
         <v>1262</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="12">
         <v>43928</v>
       </c>
@@ -13017,7 +13104,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="12">
         <v>43929</v>
       </c>
@@ -13070,7 +13157,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="12">
         <v>43930</v>
       </c>
@@ -13123,7 +13210,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="12">
         <v>43931</v>
       </c>
@@ -13176,7 +13263,7 @@
         <v>1461</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="12">
         <v>43932</v>
       </c>
@@ -13229,7 +13316,7 @@
         <v>1467</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="12">
         <v>43933</v>
       </c>
@@ -13282,7 +13369,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="12">
         <v>43934</v>
       </c>
@@ -13335,7 +13422,7 @@
         <v>1482</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="12">
         <v>43935</v>
       </c>
@@ -13388,7 +13475,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" s="12">
         <v>43936</v>
       </c>
@@ -13441,7 +13528,7 @@
         <v>1486</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" s="12">
         <v>43937</v>
       </c>
@@ -13494,7 +13581,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" s="12">
         <v>43938</v>
       </c>
@@ -13547,7 +13634,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" s="12">
         <v>43939</v>
       </c>
@@ -13600,7 +13687,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" s="12">
         <v>43940</v>
       </c>
@@ -13653,7 +13740,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" s="12">
         <v>43941</v>
       </c>
@@ -13706,7 +13793,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" s="12">
         <v>43942</v>
       </c>
@@ -13759,7 +13846,7 @@
         <v>1472</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="12">
         <v>43943</v>
       </c>
@@ -13812,7 +13899,7 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" s="12">
         <v>43944</v>
       </c>
@@ -13865,7 +13952,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" s="12">
         <v>43945</v>
       </c>
@@ -13918,7 +14005,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" s="12">
         <v>43946</v>
       </c>
@@ -13971,7 +14058,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" s="12">
         <v>43947</v>
       </c>
@@ -14024,7 +14111,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" s="30">
         <v>43948</v>
       </c>
@@ -14077,7 +14164,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" s="30">
         <v>43949</v>
       </c>
@@ -14130,7 +14217,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" s="30">
         <v>43950</v>
       </c>
@@ -14183,7 +14270,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" s="30">
         <v>43951</v>
       </c>
@@ -14236,7 +14323,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" s="30">
         <v>43952</v>
       </c>
@@ -14289,7 +14376,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" s="30">
         <v>43953</v>
       </c>
@@ -14342,7 +14429,7 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" s="30">
         <v>43954</v>
       </c>
@@ -14395,7 +14482,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" s="30">
         <v>43955</v>
       </c>
@@ -14448,7 +14535,7 @@
         <v>1279</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" s="30">
         <v>43956</v>
       </c>
@@ -14501,7 +14588,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" s="30">
         <v>43957</v>
       </c>
@@ -14554,7 +14641,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" s="30">
         <v>43958</v>
       </c>
@@ -14607,7 +14694,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" s="30">
         <v>43959</v>
       </c>
@@ -14660,7 +14747,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" s="30">
         <v>43960</v>
       </c>
@@ -14713,7 +14800,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" s="30">
         <v>43961</v>
       </c>
@@ -14766,7 +14853,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50" s="30">
         <v>43962</v>
       </c>
@@ -14819,7 +14906,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51" s="30">
         <v>43963</v>
       </c>
@@ -14872,7 +14959,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52" s="30">
         <v>43964</v>
       </c>
@@ -14925,7 +15012,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53" s="30">
         <v>43965</v>
       </c>
@@ -14978,7 +15065,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54" s="30">
         <v>43966</v>
       </c>
@@ -15031,7 +15118,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55" s="30">
         <v>43967</v>
       </c>
@@ -15084,7 +15171,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56" s="30">
         <v>43968</v>
       </c>
@@ -15137,7 +15224,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A57" s="30">
         <v>43969</v>
       </c>
@@ -15190,7 +15277,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A58" s="30">
         <v>43970</v>
       </c>
@@ -15243,7 +15330,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A59" s="30">
         <v>43971</v>
       </c>
@@ -15296,7 +15383,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A60" s="30">
         <v>43972</v>
       </c>
@@ -15349,7 +15436,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A61" s="30">
         <v>43973</v>
       </c>
@@ -15402,7 +15489,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A62" s="30">
         <v>43974</v>
       </c>
@@ -15455,7 +15542,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A63" s="30">
         <v>43975</v>
       </c>
@@ -15508,7 +15595,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A64" s="30">
         <v>43976</v>
       </c>
@@ -15561,7 +15648,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A65" s="51">
         <v>43977</v>
       </c>
@@ -15614,7 +15701,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A66" s="51">
         <v>43978</v>
       </c>
@@ -15667,7 +15754,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A67" s="51">
         <v>43979</v>
       </c>
@@ -15720,7 +15807,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A68" s="51">
         <v>43980</v>
       </c>
@@ -15773,7 +15860,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A69" s="51">
         <v>43981</v>
       </c>
@@ -15826,7 +15913,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A70" s="51">
         <v>43982</v>
       </c>
@@ -15879,7 +15966,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A71" s="51">
         <v>43983</v>
       </c>
@@ -15932,7 +16019,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A72" s="51">
         <v>43984</v>
       </c>
@@ -15985,7 +16072,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A73" s="51">
         <v>43985</v>
       </c>
@@ -16038,7 +16125,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A74" s="51">
         <v>43986</v>
       </c>
@@ -16091,7 +16178,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A75" s="51">
         <v>43987</v>
       </c>
@@ -16144,7 +16231,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A76" s="51">
         <v>43988</v>
       </c>
@@ -16197,7 +16284,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A77" s="51">
         <v>43989</v>
       </c>
@@ -16250,7 +16337,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A78" s="51">
         <v>43990</v>
       </c>
@@ -16303,7 +16390,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A79" s="51">
         <v>43991</v>
       </c>
@@ -16354,6 +16441,59 @@
       </c>
       <c r="Q79" s="13">
         <v>641</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A80" s="51">
+        <v>43992</v>
+      </c>
+      <c r="B80" s="11">
+        <v>8</v>
+      </c>
+      <c r="C80" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D80" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E80" s="11">
+        <v>53</v>
+      </c>
+      <c r="F80" s="11">
+        <v>9</v>
+      </c>
+      <c r="G80" s="11">
+        <v>60</v>
+      </c>
+      <c r="H80" s="11">
+        <v>279</v>
+      </c>
+      <c r="I80" s="11">
+        <v>9</v>
+      </c>
+      <c r="J80" s="11">
+        <v>55</v>
+      </c>
+      <c r="K80" s="11">
+        <v>142</v>
+      </c>
+      <c r="L80" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M80" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N80" s="11">
+        <v>7</v>
+      </c>
+      <c r="O80" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P80" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q80" s="13">
+        <v>623</v>
       </c>
     </row>
   </sheetData>
@@ -16364,23 +16504,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q79"/>
+  <dimension ref="A1:Q80"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B58" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B66" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A79" sqref="A79"/>
+      <selection pane="bottomRight" activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5546875" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5546875" style="2"/>
+    <col min="1" max="1" width="12.453125" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.54296875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -16401,7 +16541,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -16422,7 +16562,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -16475,7 +16615,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="12">
         <v>43916</v>
       </c>
@@ -16528,7 +16668,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
         <v>43917</v>
       </c>
@@ -16581,7 +16721,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="12">
         <v>43918</v>
       </c>
@@ -16634,7 +16774,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
         <v>43919</v>
       </c>
@@ -16687,7 +16827,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="12">
         <v>43920</v>
       </c>
@@ -16740,7 +16880,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="12">
         <v>43921</v>
       </c>
@@ -16793,7 +16933,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="12">
         <v>43922</v>
       </c>
@@ -16846,7 +16986,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
         <v>43923</v>
       </c>
@@ -16899,7 +17039,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="12">
         <v>43924</v>
       </c>
@@ -16952,7 +17092,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <v>43925</v>
       </c>
@@ -17005,7 +17145,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>43926</v>
       </c>
@@ -17058,7 +17198,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="12">
         <v>43927</v>
       </c>
@@ -17111,7 +17251,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="12">
         <v>43928</v>
       </c>
@@ -17164,7 +17304,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="12">
         <v>43929</v>
       </c>
@@ -17217,7 +17357,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="12">
         <v>43930</v>
       </c>
@@ -17270,7 +17410,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="12">
         <v>43931</v>
       </c>
@@ -17323,7 +17463,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="12">
         <v>43932</v>
       </c>
@@ -17376,7 +17516,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="12">
         <v>43933</v>
       </c>
@@ -17429,7 +17569,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="12">
         <v>43934</v>
       </c>
@@ -17482,7 +17622,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="12">
         <v>43935</v>
       </c>
@@ -17535,7 +17675,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" s="12">
         <v>43936</v>
       </c>
@@ -17588,7 +17728,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" s="12">
         <v>43937</v>
       </c>
@@ -17641,7 +17781,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" s="12">
         <v>43938</v>
       </c>
@@ -17694,7 +17834,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" s="12">
         <v>43939</v>
       </c>
@@ -17747,7 +17887,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" s="12">
         <v>43940</v>
       </c>
@@ -17800,7 +17940,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" s="12">
         <v>43941</v>
       </c>
@@ -17853,7 +17993,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" s="12">
         <v>43942</v>
       </c>
@@ -17906,7 +18046,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="12">
         <v>43943</v>
       </c>
@@ -17959,7 +18099,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" s="12">
         <v>43944</v>
       </c>
@@ -18012,7 +18152,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" s="12">
         <v>43945</v>
       </c>
@@ -18065,7 +18205,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" s="12">
         <v>43946</v>
       </c>
@@ -18118,7 +18258,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" s="12">
         <v>43947</v>
       </c>
@@ -18171,7 +18311,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" s="30">
         <v>43948</v>
       </c>
@@ -18224,7 +18364,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" s="30">
         <v>43949</v>
       </c>
@@ -18277,7 +18417,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" s="30">
         <v>43950</v>
       </c>
@@ -18330,7 +18470,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" s="30">
         <v>43951</v>
       </c>
@@ -18383,7 +18523,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" s="30">
         <v>43952</v>
       </c>
@@ -18436,7 +18576,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" s="30">
         <v>43953</v>
       </c>
@@ -18489,7 +18629,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" s="30">
         <v>43954</v>
       </c>
@@ -18542,7 +18682,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" s="30">
         <v>43955</v>
       </c>
@@ -18595,7 +18735,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" s="30">
         <v>43956</v>
       </c>
@@ -18648,7 +18788,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" s="30">
         <v>43957</v>
       </c>
@@ -18701,7 +18841,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" s="30">
         <v>43958</v>
       </c>
@@ -18754,7 +18894,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" s="30">
         <v>43959</v>
       </c>
@@ -18807,7 +18947,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" s="30">
         <v>43960</v>
       </c>
@@ -18860,7 +19000,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" s="30">
         <v>43961</v>
       </c>
@@ -18913,7 +19053,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50" s="30">
         <v>43962</v>
       </c>
@@ -18966,7 +19106,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51" s="30">
         <v>43963</v>
       </c>
@@ -19019,7 +19159,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52" s="30">
         <v>43964</v>
       </c>
@@ -19072,7 +19212,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53" s="30">
         <v>43965</v>
       </c>
@@ -19125,7 +19265,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54" s="30">
         <v>43966</v>
       </c>
@@ -19178,7 +19318,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55" s="30">
         <v>43967</v>
       </c>
@@ -19231,7 +19371,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56" s="30">
         <v>43968</v>
       </c>
@@ -19284,7 +19424,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A57" s="30">
         <v>43969</v>
       </c>
@@ -19337,7 +19477,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A58" s="30">
         <v>43970</v>
       </c>
@@ -19390,7 +19530,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A59" s="30">
         <v>43971</v>
       </c>
@@ -19443,7 +19583,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A60" s="30">
         <v>43972</v>
       </c>
@@ -19496,7 +19636,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A61" s="30">
         <v>43973</v>
       </c>
@@ -19549,7 +19689,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A62" s="30">
         <v>43974</v>
       </c>
@@ -19602,7 +19742,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A63" s="30">
         <v>43975</v>
       </c>
@@ -19655,7 +19795,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A64" s="30">
         <v>43976</v>
       </c>
@@ -19708,7 +19848,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A65" s="30">
         <v>43977</v>
       </c>
@@ -19761,7 +19901,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A66" s="30">
         <v>43978</v>
       </c>
@@ -19814,7 +19954,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A67" s="30">
         <v>43979</v>
       </c>
@@ -19867,7 +20007,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A68" s="30">
         <v>43980</v>
       </c>
@@ -19920,7 +20060,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A69" s="30">
         <v>43981</v>
       </c>
@@ -19973,7 +20113,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A70" s="30">
         <v>43982</v>
       </c>
@@ -20026,7 +20166,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A71" s="30">
         <v>43983</v>
       </c>
@@ -20079,7 +20219,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A72" s="30">
         <v>43984</v>
       </c>
@@ -20132,7 +20272,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A73" s="30">
         <v>43985</v>
       </c>
@@ -20185,7 +20325,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A74" s="30">
         <v>43986</v>
       </c>
@@ -20238,7 +20378,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A75" s="30">
         <v>43987</v>
       </c>
@@ -20291,7 +20431,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A76" s="30">
         <v>43988</v>
       </c>
@@ -20344,7 +20484,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A77" s="30">
         <v>43989</v>
       </c>
@@ -20397,7 +20537,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A78" s="30">
         <v>43990</v>
       </c>
@@ -20450,7 +20590,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A79" s="30">
         <v>43991</v>
       </c>
@@ -20501,6 +20641,59 @@
       </c>
       <c r="Q79" s="13">
         <v>370</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A80" s="30">
+        <v>43992</v>
+      </c>
+      <c r="B80" s="11">
+        <v>24</v>
+      </c>
+      <c r="C80" s="11">
+        <v>11</v>
+      </c>
+      <c r="D80" s="11">
+        <v>8</v>
+      </c>
+      <c r="E80" s="11">
+        <v>28</v>
+      </c>
+      <c r="F80" s="11">
+        <v>24</v>
+      </c>
+      <c r="G80" s="11">
+        <v>14</v>
+      </c>
+      <c r="H80" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I80" s="11">
+        <v>18</v>
+      </c>
+      <c r="J80" s="11">
+        <v>48</v>
+      </c>
+      <c r="K80" s="11">
+        <v>182</v>
+      </c>
+      <c r="L80" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M80" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N80" s="11">
+        <v>6</v>
+      </c>
+      <c r="O80" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P80" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q80" s="13">
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -20533,7 +20726,7 @@
       <value order="0"/>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-09T12:29:11Z</value>
+      <value order="0">2020-06-10T11:51:41Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -20548,16 +20741,16 @@
       <value order="0">Being Drafted</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41637421</value>
+      <value order="0">vA41664623</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">22.4</value>
+      <value order="0">22.6</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">161</value>
+      <value order="0">163</value>
     </field>
     <field name="Objective-VersionComment">
-      <value order="0"/>
+      <value order="0">testing update</value>
     </field>
     <field name="Objective-FileNumber">
       <value order="0">PUBRES/4199</value>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-10 20:08) (#106)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U445783\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA18464\A28088333\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u419207\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA10434\A28088333\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5988" windowHeight="6036" tabRatio="803" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5990" windowHeight="6030" tabRatio="803" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1732" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1757" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -1636,21 +1636,21 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.44140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="90.44140625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.44140625" style="2"/>
+    <col min="2" max="2" width="29.453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="90.453125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B3" s="18" t="s">
         <v>20</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="20" t="s">
         <v>22</v>
       </c>
@@ -1666,13 +1666,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="22" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="23"/>
     </row>
-    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="24" t="s">
         <v>26</v>
       </c>
@@ -1680,7 +1680,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="24" t="s">
         <v>27</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="24" t="s">
         <v>36</v>
       </c>
@@ -1696,7 +1696,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="20" t="s">
         <v>37</v>
       </c>
@@ -1724,12 +1724,12 @@
       <selection activeCell="K66" sqref="K66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="9.44140625" style="2"/>
+    <col min="1" max="16384" width="9.453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="44" spans="1:1" ht="15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A44" s="43"/>
     </row>
   </sheetData>
@@ -1743,21 +1743,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S160"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="64" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B88" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="R93" sqref="R93"/>
+      <selection pane="bottomRight" activeCell="M101" sqref="M101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" style="2" customWidth="1"/>
-    <col min="2" max="16" width="11.44140625" style="11" customWidth="1"/>
-    <col min="17" max="16384" width="8.5546875" style="2"/>
+    <col min="2" max="16" width="11.453125" style="11" customWidth="1"/>
+    <col min="17" max="16384" width="8.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -1777,7 +1777,7 @@
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -1796,7 +1796,7 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>43897</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>43898</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>43899</v>
       </c>
@@ -1996,7 +1996,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>43900</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>43901</v>
       </c>
@@ -2096,7 +2096,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>43902</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>43903</v>
       </c>
@@ -2196,7 +2196,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>43904</v>
       </c>
@@ -2246,7 +2246,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>43905</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>43906</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>43907</v>
       </c>
@@ -2396,7 +2396,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>43908</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>43909</v>
       </c>
@@ -2496,7 +2496,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>43910</v>
       </c>
@@ -2546,7 +2546,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>43911</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>43912</v>
       </c>
@@ -2646,7 +2646,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>43913</v>
       </c>
@@ -2696,7 +2696,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>43914</v>
       </c>
@@ -2746,7 +2746,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>43915</v>
       </c>
@@ -2796,7 +2796,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>43916</v>
       </c>
@@ -2846,7 +2846,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>43917</v>
       </c>
@@ -2896,7 +2896,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>43918</v>
       </c>
@@ -2946,7 +2946,7 @@
         <v>1264</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>43919</v>
       </c>
@@ -2996,7 +2996,7 @@
         <v>1417</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>43920</v>
       </c>
@@ -3046,7 +3046,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>43921</v>
       </c>
@@ -3096,7 +3096,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>43922</v>
       </c>
@@ -3146,7 +3146,7 @@
         <v>2310</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>43923</v>
       </c>
@@ -3196,7 +3196,7 @@
         <v>2602</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>43924</v>
       </c>
@@ -3246,7 +3246,7 @@
         <v>3001</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>43925</v>
       </c>
@@ -3296,7 +3296,7 @@
         <v>3345</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>43926</v>
       </c>
@@ -3346,7 +3346,7 @@
         <v>3706</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>43927</v>
       </c>
@@ -3396,7 +3396,7 @@
         <v>3961</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>43928</v>
       </c>
@@ -3446,7 +3446,7 @@
         <v>4229</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>43929</v>
       </c>
@@ -3496,7 +3496,7 @@
         <v>4565</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>43930</v>
       </c>
@@ -3546,7 +3546,7 @@
         <v>4957</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>43931</v>
       </c>
@@ -3596,7 +3596,7 @@
         <v>5275</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>43932</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>5590</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>43933</v>
       </c>
@@ -3696,7 +3696,7 @@
         <v>5912</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>43934</v>
       </c>
@@ -3746,7 +3746,7 @@
         <v>6067</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>43935</v>
       </c>
@@ -3796,7 +3796,7 @@
         <v>6358</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>43936</v>
       </c>
@@ -3846,7 +3846,7 @@
         <v>6748</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
         <v>43937</v>
       </c>
@@ -3896,7 +3896,7 @@
         <v>7102</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>43938</v>
       </c>
@@ -3946,7 +3946,7 @@
         <v>7409</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A46" s="5">
         <v>43939</v>
       </c>
@@ -3996,7 +3996,7 @@
         <v>7820</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A47" s="5">
         <v>43940</v>
       </c>
@@ -4046,7 +4046,7 @@
         <v>8187</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A48" s="5">
         <v>43941</v>
       </c>
@@ -4096,7 +4096,7 @@
         <v>8450</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A49" s="5">
         <v>43942</v>
       </c>
@@ -4146,7 +4146,7 @@
         <v>8672</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
         <v>43943</v>
       </c>
@@ -4196,7 +4196,7 @@
         <v>9038</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
         <v>43944</v>
       </c>
@@ -4246,7 +4246,7 @@
         <v>9409</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
         <v>43945</v>
       </c>
@@ -4296,7 +4296,7 @@
         <v>9697</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
         <v>43946</v>
       </c>
@@ -4346,7 +4346,7 @@
         <v>10051</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A54" s="5">
         <v>43947</v>
       </c>
@@ -4397,7 +4397,7 @@
       </c>
       <c r="R54" s="38"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
         <v>43948</v>
       </c>
@@ -4448,7 +4448,7 @@
       </c>
       <c r="R55" s="38"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A56" s="5">
         <v>43949</v>
       </c>
@@ -4499,7 +4499,7 @@
       </c>
       <c r="R56" s="39"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
         <v>43950</v>
       </c>
@@ -4549,7 +4549,7 @@
         <v>11034</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
         <v>43951</v>
       </c>
@@ -4600,7 +4600,7 @@
       </c>
       <c r="R58" s="38"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>43952</v>
       </c>
@@ -4652,7 +4652,7 @@
       <c r="R59" s="38"/>
       <c r="S59" s="38"/>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
         <v>43953</v>
       </c>
@@ -4702,7 +4702,7 @@
         <v>11927</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
         <v>43954</v>
       </c>
@@ -4752,7 +4752,7 @@
         <v>12097</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A62" s="5">
         <v>43955</v>
       </c>
@@ -4802,7 +4802,7 @@
         <v>12266</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A63" s="5">
         <v>43956</v>
       </c>
@@ -4852,7 +4852,7 @@
         <v>12437</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
         <v>43957</v>
       </c>
@@ -4902,7 +4902,7 @@
         <v>12709</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>43958</v>
       </c>
@@ -4952,7 +4952,7 @@
         <v>12924</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
         <v>43959</v>
       </c>
@@ -5002,7 +5002,7 @@
         <v>13149</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
         <v>43960</v>
       </c>
@@ -5052,7 +5052,7 @@
         <v>13305</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A68" s="5">
         <v>43961</v>
       </c>
@@ -5102,7 +5102,7 @@
         <v>13486</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A69" s="5">
         <v>43962</v>
       </c>
@@ -5152,7 +5152,7 @@
         <v>13627</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A70" s="5">
         <v>43963</v>
       </c>
@@ -5202,7 +5202,7 @@
         <v>13763</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A71" s="5">
         <v>43964</v>
       </c>
@@ -5252,7 +5252,7 @@
         <v>13929</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A72" s="5">
         <v>43965</v>
       </c>
@@ -5302,7 +5302,7 @@
         <v>14117</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A73" s="5">
         <v>43966</v>
       </c>
@@ -5352,7 +5352,7 @@
         <v>14260</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A74" s="5">
         <v>43967</v>
       </c>
@@ -5402,7 +5402,7 @@
         <v>14447</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A75" s="5">
         <v>43968</v>
       </c>
@@ -5452,7 +5452,7 @@
         <v>14537</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A76" s="5">
         <v>43969</v>
       </c>
@@ -5502,7 +5502,7 @@
         <v>14594</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A77" s="5">
         <v>43970</v>
       </c>
@@ -5552,7 +5552,7 @@
         <v>14655</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A78" s="5">
         <v>43971</v>
       </c>
@@ -5602,7 +5602,7 @@
         <v>14751</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A79" s="5">
         <v>43972</v>
       </c>
@@ -5652,7 +5652,7 @@
         <v>14856</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A80" s="5">
         <v>43973</v>
       </c>
@@ -5702,7 +5702,7 @@
         <v>14969</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A81" s="5">
         <v>43974</v>
       </c>
@@ -5752,7 +5752,7 @@
         <v>15041</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A82" s="5">
         <v>43975</v>
       </c>
@@ -5802,7 +5802,7 @@
         <v>15101</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A83" s="5">
         <v>43976</v>
       </c>
@@ -5852,7 +5852,7 @@
         <v>15156</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A84" s="5">
         <v>43977</v>
       </c>
@@ -5902,7 +5902,7 @@
         <v>15185</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A85" s="5">
         <v>43978</v>
       </c>
@@ -5952,7 +5952,7 @@
         <v>15240</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A86" s="5">
         <v>43979</v>
       </c>
@@ -6002,7 +6002,7 @@
         <v>15288</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A87" s="5">
         <v>43980</v>
       </c>
@@ -6052,7 +6052,7 @@
         <v>15327</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A88" s="5">
         <v>43981</v>
       </c>
@@ -6102,7 +6102,7 @@
         <v>15382</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A89" s="5">
         <v>43982</v>
       </c>
@@ -6152,7 +6152,7 @@
         <v>15400</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A90" s="5">
         <v>43983</v>
       </c>
@@ -6202,7 +6202,7 @@
         <v>15418</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A91" s="5">
         <v>43984</v>
       </c>
@@ -6252,7 +6252,7 @@
         <v>15471</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A92" s="5">
         <v>43985</v>
       </c>
@@ -6302,7 +6302,7 @@
         <v>15504</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A93" s="5">
         <v>43986</v>
       </c>
@@ -6352,7 +6352,7 @@
         <v>15553</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A94" s="5">
         <v>43987</v>
       </c>
@@ -6402,7 +6402,7 @@
         <v>15582</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A95" s="5">
         <v>43988</v>
       </c>
@@ -6452,7 +6452,7 @@
         <v>15603</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A96" s="5">
         <v>43989</v>
       </c>
@@ -6502,7 +6502,7 @@
         <v>15621</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A97" s="5">
         <v>43990</v>
       </c>
@@ -6552,7 +6552,7 @@
         <v>15639</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A98" s="5">
         <v>43991</v>
       </c>
@@ -6602,23 +6602,57 @@
         <v>15653</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="C99" s="28"/>
-      <c r="D99" s="28"/>
-      <c r="E99" s="28"/>
-      <c r="F99" s="28"/>
-      <c r="G99" s="28"/>
-      <c r="H99" s="28"/>
-      <c r="I99" s="28"/>
-      <c r="J99" s="28"/>
-      <c r="K99" s="28"/>
-      <c r="L99" s="28"/>
-      <c r="M99" s="28"/>
-      <c r="N99" s="28"/>
-      <c r="O99" s="28"/>
-      <c r="P99" s="28"/>
-    </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A99" s="5">
+        <v>43992</v>
+      </c>
+      <c r="B99" s="28">
+        <v>1081</v>
+      </c>
+      <c r="C99" s="28">
+        <v>327</v>
+      </c>
+      <c r="D99" s="28">
+        <v>261</v>
+      </c>
+      <c r="E99" s="28">
+        <v>880</v>
+      </c>
+      <c r="F99" s="28">
+        <v>948</v>
+      </c>
+      <c r="G99" s="28">
+        <v>1287</v>
+      </c>
+      <c r="H99" s="28">
+        <v>3990</v>
+      </c>
+      <c r="I99" s="28">
+        <v>340</v>
+      </c>
+      <c r="J99" s="28">
+        <v>2021</v>
+      </c>
+      <c r="K99" s="28">
+        <v>2778</v>
+      </c>
+      <c r="L99" s="28">
+        <v>8</v>
+      </c>
+      <c r="M99" s="28">
+        <v>54</v>
+      </c>
+      <c r="N99" s="28">
+        <v>1684</v>
+      </c>
+      <c r="O99" s="28">
+        <v>6</v>
+      </c>
+      <c r="P99" s="32">
+        <v>15665</v>
+      </c>
+    </row>
+    <row r="100" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C100" s="28"/>
       <c r="D100" s="28"/>
       <c r="E100" s="28"/>
@@ -6634,7 +6668,7 @@
       <c r="O100" s="28"/>
       <c r="P100" s="28"/>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C101" s="28"/>
       <c r="D101" s="28"/>
       <c r="E101" s="28"/>
@@ -6650,7 +6684,7 @@
       <c r="O101" s="28"/>
       <c r="P101" s="28"/>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C102" s="28"/>
       <c r="D102" s="28"/>
       <c r="E102" s="28"/>
@@ -6666,7 +6700,7 @@
       <c r="O102" s="28"/>
       <c r="P102" s="28"/>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C103" s="28"/>
       <c r="D103" s="28"/>
       <c r="E103" s="28"/>
@@ -6682,7 +6716,7 @@
       <c r="O103" s="28"/>
       <c r="P103" s="28"/>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C104" s="28"/>
       <c r="D104" s="28"/>
       <c r="E104" s="28"/>
@@ -6698,7 +6732,7 @@
       <c r="O104" s="28"/>
       <c r="P104" s="28"/>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C105" s="28"/>
       <c r="D105" s="28"/>
       <c r="E105" s="28"/>
@@ -6714,7 +6748,7 @@
       <c r="O105" s="28"/>
       <c r="P105" s="28"/>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C106" s="28"/>
       <c r="D106" s="28"/>
       <c r="E106" s="28"/>
@@ -6730,7 +6764,7 @@
       <c r="O106" s="28"/>
       <c r="P106" s="28"/>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C107" s="28"/>
       <c r="D107" s="28"/>
       <c r="E107" s="28"/>
@@ -6746,7 +6780,7 @@
       <c r="O107" s="28"/>
       <c r="P107" s="28"/>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C108" s="28"/>
       <c r="D108" s="28"/>
       <c r="E108" s="28"/>
@@ -6762,7 +6796,7 @@
       <c r="O108" s="28"/>
       <c r="P108" s="28"/>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C109" s="28"/>
       <c r="D109" s="28"/>
       <c r="E109" s="28"/>
@@ -6778,7 +6812,7 @@
       <c r="O109" s="28"/>
       <c r="P109" s="28"/>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C110" s="28"/>
       <c r="D110" s="28"/>
       <c r="E110" s="28"/>
@@ -6794,7 +6828,7 @@
       <c r="O110" s="28"/>
       <c r="P110" s="28"/>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C111" s="28"/>
       <c r="D111" s="28"/>
       <c r="E111" s="28"/>
@@ -6810,7 +6844,7 @@
       <c r="O111" s="28"/>
       <c r="P111" s="28"/>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C112" s="28"/>
       <c r="D112" s="28"/>
       <c r="E112" s="28"/>
@@ -6826,7 +6860,7 @@
       <c r="O112" s="28"/>
       <c r="P112" s="28"/>
     </row>
-    <row r="113" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:16" x14ac:dyDescent="0.35">
       <c r="C113" s="28"/>
       <c r="D113" s="28"/>
       <c r="E113" s="28"/>
@@ -6842,7 +6876,7 @@
       <c r="O113" s="28"/>
       <c r="P113" s="28"/>
     </row>
-    <row r="114" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:16" x14ac:dyDescent="0.35">
       <c r="C114" s="28"/>
       <c r="D114" s="28"/>
       <c r="E114" s="28"/>
@@ -6858,7 +6892,7 @@
       <c r="O114" s="28"/>
       <c r="P114" s="28"/>
     </row>
-    <row r="115" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B115" s="28"/>
       <c r="C115" s="28"/>
       <c r="D115" s="28"/>
@@ -6875,7 +6909,7 @@
       <c r="O115" s="28"/>
       <c r="P115" s="28"/>
     </row>
-    <row r="116" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B116" s="28"/>
       <c r="C116" s="28"/>
       <c r="D116" s="28"/>
@@ -6892,7 +6926,7 @@
       <c r="O116" s="28"/>
       <c r="P116" s="28"/>
     </row>
-    <row r="117" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B117" s="28"/>
       <c r="C117" s="28"/>
       <c r="D117" s="28"/>
@@ -6909,7 +6943,7 @@
       <c r="O117" s="28"/>
       <c r="P117" s="28"/>
     </row>
-    <row r="118" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B118" s="28"/>
       <c r="C118" s="28"/>
       <c r="D118" s="28"/>
@@ -6926,7 +6960,7 @@
       <c r="O118" s="28"/>
       <c r="P118" s="28"/>
     </row>
-    <row r="119" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B119" s="28"/>
       <c r="C119" s="28"/>
       <c r="D119" s="28"/>
@@ -6943,7 +6977,7 @@
       <c r="O119" s="28"/>
       <c r="P119" s="28"/>
     </row>
-    <row r="120" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B120" s="28"/>
       <c r="C120" s="28"/>
       <c r="D120" s="28"/>
@@ -6960,7 +6994,7 @@
       <c r="O120" s="28"/>
       <c r="P120" s="28"/>
     </row>
-    <row r="121" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B121" s="28"/>
       <c r="C121" s="28"/>
       <c r="D121" s="28"/>
@@ -6977,7 +7011,7 @@
       <c r="O121" s="28"/>
       <c r="P121" s="28"/>
     </row>
-    <row r="122" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B122" s="28"/>
       <c r="C122" s="28"/>
       <c r="D122" s="28"/>
@@ -6994,7 +7028,7 @@
       <c r="O122" s="28"/>
       <c r="P122" s="28"/>
     </row>
-    <row r="123" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B123" s="28"/>
       <c r="C123" s="28"/>
       <c r="D123" s="28"/>
@@ -7011,7 +7045,7 @@
       <c r="O123" s="28"/>
       <c r="P123" s="28"/>
     </row>
-    <row r="124" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B124" s="28"/>
       <c r="C124" s="28"/>
       <c r="D124" s="28"/>
@@ -7028,7 +7062,7 @@
       <c r="O124" s="28"/>
       <c r="P124" s="28"/>
     </row>
-    <row r="125" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B125" s="28"/>
       <c r="C125" s="28"/>
       <c r="D125" s="28"/>
@@ -7045,7 +7079,7 @@
       <c r="O125" s="28"/>
       <c r="P125" s="28"/>
     </row>
-    <row r="126" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B126" s="28"/>
       <c r="C126" s="28"/>
       <c r="D126" s="28"/>
@@ -7062,7 +7096,7 @@
       <c r="O126" s="28"/>
       <c r="P126" s="28"/>
     </row>
-    <row r="127" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B127" s="28"/>
       <c r="C127" s="28"/>
       <c r="D127" s="28"/>
@@ -7079,7 +7113,7 @@
       <c r="O127" s="28"/>
       <c r="P127" s="28"/>
     </row>
-    <row r="128" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B128" s="28"/>
       <c r="C128" s="28"/>
       <c r="D128" s="28"/>
@@ -7096,7 +7130,7 @@
       <c r="O128" s="28"/>
       <c r="P128" s="28"/>
     </row>
-    <row r="129" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B129" s="28"/>
       <c r="C129" s="28"/>
       <c r="D129" s="28"/>
@@ -7113,7 +7147,7 @@
       <c r="O129" s="28"/>
       <c r="P129" s="28"/>
     </row>
-    <row r="130" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B130" s="28"/>
       <c r="C130" s="28"/>
       <c r="D130" s="28"/>
@@ -7130,7 +7164,7 @@
       <c r="O130" s="28"/>
       <c r="P130" s="28"/>
     </row>
-    <row r="131" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B131" s="28"/>
       <c r="C131" s="28"/>
       <c r="D131" s="28"/>
@@ -7147,7 +7181,7 @@
       <c r="O131" s="28"/>
       <c r="P131" s="28"/>
     </row>
-    <row r="132" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B132" s="28"/>
       <c r="C132" s="28"/>
       <c r="D132" s="28"/>
@@ -7164,7 +7198,7 @@
       <c r="O132" s="28"/>
       <c r="P132" s="28"/>
     </row>
-    <row r="133" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B133" s="28"/>
       <c r="C133" s="28"/>
       <c r="D133" s="28"/>
@@ -7181,7 +7215,7 @@
       <c r="O133" s="28"/>
       <c r="P133" s="28"/>
     </row>
-    <row r="134" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B134" s="28"/>
       <c r="C134" s="28"/>
       <c r="D134" s="28"/>
@@ -7198,7 +7232,7 @@
       <c r="O134" s="28"/>
       <c r="P134" s="28"/>
     </row>
-    <row r="135" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B135" s="28"/>
       <c r="C135" s="28"/>
       <c r="D135" s="28"/>
@@ -7215,7 +7249,7 @@
       <c r="O135" s="28"/>
       <c r="P135" s="28"/>
     </row>
-    <row r="136" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B136" s="28"/>
       <c r="C136" s="28"/>
       <c r="D136" s="28"/>
@@ -7232,7 +7266,7 @@
       <c r="O136" s="28"/>
       <c r="P136" s="28"/>
     </row>
-    <row r="137" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B137" s="28"/>
       <c r="C137" s="28"/>
       <c r="D137" s="28"/>
@@ -7249,7 +7283,7 @@
       <c r="O137" s="28"/>
       <c r="P137" s="28"/>
     </row>
-    <row r="138" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B138" s="28"/>
       <c r="C138" s="28"/>
       <c r="D138" s="28"/>
@@ -7266,7 +7300,7 @@
       <c r="O138" s="28"/>
       <c r="P138" s="28"/>
     </row>
-    <row r="139" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B139" s="28"/>
       <c r="C139" s="28"/>
       <c r="D139" s="28"/>
@@ -7283,7 +7317,7 @@
       <c r="O139" s="28"/>
       <c r="P139" s="28"/>
     </row>
-    <row r="140" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B140" s="28"/>
       <c r="C140" s="28"/>
       <c r="D140" s="28"/>
@@ -7300,7 +7334,7 @@
       <c r="O140" s="28"/>
       <c r="P140" s="28"/>
     </row>
-    <row r="141" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B141" s="28"/>
       <c r="C141" s="28"/>
       <c r="D141" s="28"/>
@@ -7317,7 +7351,7 @@
       <c r="O141" s="28"/>
       <c r="P141" s="28"/>
     </row>
-    <row r="142" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B142" s="28"/>
       <c r="C142" s="28"/>
       <c r="D142" s="28"/>
@@ -7334,7 +7368,7 @@
       <c r="O142" s="28"/>
       <c r="P142" s="28"/>
     </row>
-    <row r="143" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B143" s="28"/>
       <c r="C143" s="28"/>
       <c r="D143" s="28"/>
@@ -7351,7 +7385,7 @@
       <c r="O143" s="28"/>
       <c r="P143" s="28"/>
     </row>
-    <row r="144" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B144" s="28"/>
       <c r="C144" s="28"/>
       <c r="D144" s="28"/>
@@ -7368,7 +7402,7 @@
       <c r="O144" s="28"/>
       <c r="P144" s="28"/>
     </row>
-    <row r="145" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B145" s="28"/>
       <c r="C145" s="28"/>
       <c r="D145" s="28"/>
@@ -7385,7 +7419,7 @@
       <c r="O145" s="28"/>
       <c r="P145" s="28"/>
     </row>
-    <row r="146" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B146" s="28"/>
       <c r="C146" s="28"/>
       <c r="D146" s="28"/>
@@ -7402,7 +7436,7 @@
       <c r="O146" s="28"/>
       <c r="P146" s="28"/>
     </row>
-    <row r="147" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B147" s="28"/>
       <c r="C147" s="28"/>
       <c r="D147" s="28"/>
@@ -7419,7 +7453,7 @@
       <c r="O147" s="28"/>
       <c r="P147" s="28"/>
     </row>
-    <row r="148" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B148" s="28"/>
       <c r="C148" s="28"/>
       <c r="D148" s="28"/>
@@ -7436,7 +7470,7 @@
       <c r="O148" s="28"/>
       <c r="P148" s="28"/>
     </row>
-    <row r="149" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B149" s="28"/>
       <c r="C149" s="28"/>
       <c r="D149" s="28"/>
@@ -7453,7 +7487,7 @@
       <c r="O149" s="28"/>
       <c r="P149" s="28"/>
     </row>
-    <row r="150" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B150" s="28"/>
       <c r="C150" s="28"/>
       <c r="D150" s="28"/>
@@ -7470,7 +7504,7 @@
       <c r="O150" s="28"/>
       <c r="P150" s="28"/>
     </row>
-    <row r="151" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B151" s="28"/>
       <c r="C151" s="28"/>
       <c r="D151" s="28"/>
@@ -7487,7 +7521,7 @@
       <c r="O151" s="28"/>
       <c r="P151" s="28"/>
     </row>
-    <row r="152" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B152" s="28"/>
       <c r="C152" s="28"/>
       <c r="D152" s="28"/>
@@ -7504,7 +7538,7 @@
       <c r="O152" s="28"/>
       <c r="P152" s="28"/>
     </row>
-    <row r="153" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B153" s="28"/>
       <c r="C153" s="28"/>
       <c r="D153" s="28"/>
@@ -7521,7 +7555,7 @@
       <c r="O153" s="28"/>
       <c r="P153" s="28"/>
     </row>
-    <row r="154" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B154" s="28"/>
       <c r="C154" s="28"/>
       <c r="D154" s="28"/>
@@ -7538,7 +7572,7 @@
       <c r="O154" s="28"/>
       <c r="P154" s="28"/>
     </row>
-    <row r="155" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B155" s="28"/>
       <c r="C155" s="28"/>
       <c r="D155" s="28"/>
@@ -7555,7 +7589,7 @@
       <c r="O155" s="28"/>
       <c r="P155" s="28"/>
     </row>
-    <row r="156" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B156" s="28"/>
       <c r="C156" s="28"/>
       <c r="D156" s="28"/>
@@ -7572,7 +7606,7 @@
       <c r="O156" s="28"/>
       <c r="P156" s="28"/>
     </row>
-    <row r="157" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B157" s="28"/>
       <c r="C157" s="28"/>
       <c r="D157" s="28"/>
@@ -7589,7 +7623,7 @@
       <c r="O157" s="28"/>
       <c r="P157" s="28"/>
     </row>
-    <row r="158" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B158" s="28"/>
       <c r="C158" s="28"/>
       <c r="D158" s="28"/>
@@ -7606,7 +7640,7 @@
       <c r="O158" s="28"/>
       <c r="P158" s="28"/>
     </row>
-    <row r="159" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B159" s="28"/>
       <c r="C159" s="28"/>
       <c r="D159" s="28"/>
@@ -7623,7 +7657,7 @@
       <c r="O159" s="28"/>
       <c r="P159" s="28"/>
     </row>
-    <row r="160" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B160" s="28"/>
       <c r="C160" s="28"/>
       <c r="D160" s="28"/>
@@ -7648,21 +7682,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q87"/>
+  <dimension ref="A1:Q88"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A87" sqref="A87"/>
+      <selection pane="bottomLeft" activeCell="M91" sqref="M91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5546875" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5546875" style="2"/>
+    <col min="1" max="1" width="12.453125" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.54296875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -7683,7 +7717,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -7704,7 +7738,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -7757,7 +7791,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="12">
         <v>43908</v>
       </c>
@@ -7810,7 +7844,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
         <v>43909</v>
       </c>
@@ -7863,7 +7897,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="12">
         <v>43910</v>
       </c>
@@ -7916,7 +7950,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
         <v>43911</v>
       </c>
@@ -7969,7 +8003,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="12">
         <v>43912</v>
       </c>
@@ -8022,7 +8056,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="12">
         <v>43913</v>
       </c>
@@ -8075,7 +8109,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="12">
         <v>43914</v>
       </c>
@@ -8128,7 +8162,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
         <v>43915</v>
       </c>
@@ -8181,7 +8215,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="12">
         <v>43916</v>
       </c>
@@ -8234,7 +8268,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <v>43917</v>
       </c>
@@ -8287,7 +8321,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>43918</v>
       </c>
@@ -8340,7 +8374,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="12">
         <v>43919</v>
       </c>
@@ -8393,7 +8427,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="12">
         <v>43920</v>
       </c>
@@ -8446,7 +8480,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="12">
         <v>43921</v>
       </c>
@@ -8499,7 +8533,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="12">
         <v>43922</v>
       </c>
@@ -8552,7 +8586,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="12">
         <v>43923</v>
       </c>
@@ -8605,7 +8639,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="12">
         <v>43924</v>
       </c>
@@ -8658,7 +8692,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="12">
         <v>43925</v>
       </c>
@@ -8711,7 +8745,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="12">
         <v>43926</v>
       </c>
@@ -8764,7 +8798,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="12">
         <v>43927</v>
       </c>
@@ -8817,7 +8851,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" s="12">
         <v>43928</v>
       </c>
@@ -8870,7 +8904,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" s="12">
         <v>43929</v>
       </c>
@@ -8923,7 +8957,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" s="12">
         <v>43930</v>
       </c>
@@ -8976,7 +9010,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" s="12">
         <v>43931</v>
       </c>
@@ -9029,7 +9063,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" s="12">
         <v>43932</v>
       </c>
@@ -9082,7 +9116,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" s="12">
         <v>43933</v>
       </c>
@@ -9135,7 +9169,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" s="12">
         <v>43934</v>
       </c>
@@ -9188,7 +9222,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="12">
         <v>43935</v>
       </c>
@@ -9241,7 +9275,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" s="12">
         <v>43936</v>
       </c>
@@ -9294,7 +9328,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" s="12">
         <v>43937</v>
       </c>
@@ -9347,7 +9381,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" s="12">
         <v>43938</v>
       </c>
@@ -9400,7 +9434,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" s="12">
         <v>43939</v>
       </c>
@@ -9453,7 +9487,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" s="30">
         <v>43940</v>
       </c>
@@ -9506,7 +9540,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" s="30">
         <v>43941</v>
       </c>
@@ -9559,7 +9593,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" s="30">
         <v>43942</v>
       </c>
@@ -9612,7 +9646,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" s="30">
         <v>43943</v>
       </c>
@@ -9665,7 +9699,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" s="30">
         <v>43944</v>
       </c>
@@ -9718,7 +9752,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" s="30">
         <v>43945</v>
       </c>
@@ -9771,7 +9805,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" s="30">
         <v>43946</v>
       </c>
@@ -9824,7 +9858,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" s="30">
         <v>43947</v>
       </c>
@@ -9877,7 +9911,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" s="30">
         <v>43948</v>
       </c>
@@ -9930,7 +9964,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" s="30">
         <v>43949</v>
       </c>
@@ -9983,7 +10017,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" s="30">
         <v>43950</v>
       </c>
@@ -10036,7 +10070,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" s="30">
         <v>43951</v>
       </c>
@@ -10089,7 +10123,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" s="30">
         <v>43952</v>
       </c>
@@ -10142,7 +10176,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" s="30">
         <v>43953</v>
       </c>
@@ -10195,7 +10229,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50" s="30">
         <v>43954</v>
       </c>
@@ -10248,7 +10282,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51" s="30">
         <v>43955</v>
       </c>
@@ -10301,7 +10335,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52" s="30">
         <v>43956</v>
       </c>
@@ -10354,7 +10388,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53" s="30">
         <v>43957</v>
       </c>
@@ -10407,7 +10441,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54" s="30">
         <v>43958</v>
       </c>
@@ -10460,7 +10494,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55" s="30">
         <v>43959</v>
       </c>
@@ -10513,7 +10547,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56" s="30">
         <v>43960</v>
       </c>
@@ -10566,7 +10600,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A57" s="30">
         <v>43961</v>
       </c>
@@ -10619,7 +10653,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A58" s="30">
         <v>43962</v>
       </c>
@@ -10672,7 +10706,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A59" s="30">
         <v>43963</v>
       </c>
@@ -10725,7 +10759,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A60" s="30">
         <v>43964</v>
       </c>
@@ -10778,7 +10812,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A61" s="30">
         <v>43965</v>
       </c>
@@ -10831,7 +10865,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A62" s="30">
         <v>43966</v>
       </c>
@@ -10884,7 +10918,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A63" s="30">
         <v>43967</v>
       </c>
@@ -10937,7 +10971,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A64" s="30">
         <v>43968</v>
       </c>
@@ -10990,7 +11024,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A65" s="30">
         <v>43969</v>
       </c>
@@ -11043,7 +11077,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A66" s="30">
         <v>43970</v>
       </c>
@@ -11096,7 +11130,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A67" s="30">
         <v>43971</v>
       </c>
@@ -11149,7 +11183,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A68" s="30">
         <v>43972</v>
       </c>
@@ -11202,7 +11236,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A69" s="30">
         <v>43973</v>
       </c>
@@ -11255,7 +11289,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A70" s="30">
         <v>43974</v>
       </c>
@@ -11308,7 +11342,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A71" s="30">
         <v>43975</v>
       </c>
@@ -11361,7 +11395,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A72" s="30">
         <v>43976</v>
       </c>
@@ -11414,7 +11448,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A73" s="30">
         <v>43977</v>
       </c>
@@ -11467,7 +11501,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A74" s="30">
         <v>43978</v>
       </c>
@@ -11520,7 +11554,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A75" s="30">
         <v>43979</v>
       </c>
@@ -11573,7 +11607,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A76" s="30">
         <v>43980</v>
       </c>
@@ -11626,7 +11660,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A77" s="30">
         <v>43981</v>
       </c>
@@ -11679,7 +11713,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A78" s="30">
         <v>43982</v>
       </c>
@@ -11732,7 +11766,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A79" s="30">
         <v>43983</v>
       </c>
@@ -11785,7 +11819,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A80" s="30">
         <v>43984</v>
       </c>
@@ -11838,7 +11872,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A81" s="30">
         <v>43985</v>
       </c>
@@ -11891,7 +11925,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A82" s="30">
         <v>43986</v>
       </c>
@@ -11944,7 +11978,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A83" s="30">
         <v>43987</v>
       </c>
@@ -11997,7 +12031,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A84" s="30">
         <v>43988</v>
       </c>
@@ -12050,7 +12084,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A85" s="30">
         <v>43989</v>
       </c>
@@ -12103,7 +12137,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A86" s="30">
         <v>43990</v>
       </c>
@@ -12156,7 +12190,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A87" s="30">
         <v>43991</v>
       </c>
@@ -12207,6 +12241,59 @@
       </c>
       <c r="Q87" s="13">
         <v>21</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A88" s="30">
+        <v>43992</v>
+      </c>
+      <c r="B88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K88" s="11">
+        <v>5</v>
+      </c>
+      <c r="L88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P88" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q88" s="13">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -12217,23 +12304,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q79"/>
+  <dimension ref="A1:Q80"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B67" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A79" sqref="A79"/>
+      <selection pane="bottomRight" activeCell="N83" sqref="N83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5546875" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5546875" style="2"/>
+    <col min="1" max="1" width="15.26953125" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.54296875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -12254,7 +12341,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -12275,7 +12362,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -12328,7 +12415,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="12">
         <v>43916</v>
       </c>
@@ -12381,7 +12468,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
         <v>43917</v>
       </c>
@@ -12434,7 +12521,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="12">
         <v>43918</v>
       </c>
@@ -12487,7 +12574,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
         <v>43919</v>
       </c>
@@ -12540,7 +12627,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="12">
         <v>43920</v>
       </c>
@@ -12593,7 +12680,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="12">
         <v>43921</v>
       </c>
@@ -12646,7 +12733,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="12">
         <v>43922</v>
       </c>
@@ -12699,7 +12786,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
         <v>43923</v>
       </c>
@@ -12752,7 +12839,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="12">
         <v>43924</v>
       </c>
@@ -12805,7 +12892,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <v>43925</v>
       </c>
@@ -12858,7 +12945,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>43926</v>
       </c>
@@ -12911,7 +12998,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="12">
         <v>43927</v>
       </c>
@@ -12964,7 +13051,7 @@
         <v>1262</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="12">
         <v>43928</v>
       </c>
@@ -13017,7 +13104,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="12">
         <v>43929</v>
       </c>
@@ -13070,7 +13157,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="12">
         <v>43930</v>
       </c>
@@ -13123,7 +13210,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="12">
         <v>43931</v>
       </c>
@@ -13176,7 +13263,7 @@
         <v>1461</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="12">
         <v>43932</v>
       </c>
@@ -13229,7 +13316,7 @@
         <v>1467</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="12">
         <v>43933</v>
       </c>
@@ -13282,7 +13369,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="12">
         <v>43934</v>
       </c>
@@ -13335,7 +13422,7 @@
         <v>1482</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="12">
         <v>43935</v>
       </c>
@@ -13388,7 +13475,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" s="12">
         <v>43936</v>
       </c>
@@ -13441,7 +13528,7 @@
         <v>1486</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" s="12">
         <v>43937</v>
       </c>
@@ -13494,7 +13581,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" s="12">
         <v>43938</v>
       </c>
@@ -13547,7 +13634,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" s="12">
         <v>43939</v>
       </c>
@@ -13600,7 +13687,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" s="12">
         <v>43940</v>
       </c>
@@ -13653,7 +13740,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" s="12">
         <v>43941</v>
       </c>
@@ -13706,7 +13793,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" s="12">
         <v>43942</v>
       </c>
@@ -13759,7 +13846,7 @@
         <v>1472</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="12">
         <v>43943</v>
       </c>
@@ -13812,7 +13899,7 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" s="12">
         <v>43944</v>
       </c>
@@ -13865,7 +13952,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" s="12">
         <v>43945</v>
       </c>
@@ -13918,7 +14005,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" s="12">
         <v>43946</v>
       </c>
@@ -13971,7 +14058,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" s="12">
         <v>43947</v>
       </c>
@@ -14024,7 +14111,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" s="30">
         <v>43948</v>
       </c>
@@ -14077,7 +14164,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" s="30">
         <v>43949</v>
       </c>
@@ -14130,7 +14217,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" s="30">
         <v>43950</v>
       </c>
@@ -14183,7 +14270,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" s="30">
         <v>43951</v>
       </c>
@@ -14236,7 +14323,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" s="30">
         <v>43952</v>
       </c>
@@ -14289,7 +14376,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" s="30">
         <v>43953</v>
       </c>
@@ -14342,7 +14429,7 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" s="30">
         <v>43954</v>
       </c>
@@ -14395,7 +14482,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" s="30">
         <v>43955</v>
       </c>
@@ -14448,7 +14535,7 @@
         <v>1279</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" s="30">
         <v>43956</v>
       </c>
@@ -14501,7 +14588,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" s="30">
         <v>43957</v>
       </c>
@@ -14554,7 +14641,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" s="30">
         <v>43958</v>
       </c>
@@ -14607,7 +14694,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" s="30">
         <v>43959</v>
       </c>
@@ -14660,7 +14747,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" s="30">
         <v>43960</v>
       </c>
@@ -14713,7 +14800,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" s="30">
         <v>43961</v>
       </c>
@@ -14766,7 +14853,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50" s="30">
         <v>43962</v>
       </c>
@@ -14819,7 +14906,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51" s="30">
         <v>43963</v>
       </c>
@@ -14872,7 +14959,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52" s="30">
         <v>43964</v>
       </c>
@@ -14925,7 +15012,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53" s="30">
         <v>43965</v>
       </c>
@@ -14978,7 +15065,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54" s="30">
         <v>43966</v>
       </c>
@@ -15031,7 +15118,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55" s="30">
         <v>43967</v>
       </c>
@@ -15084,7 +15171,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56" s="30">
         <v>43968</v>
       </c>
@@ -15137,7 +15224,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A57" s="30">
         <v>43969</v>
       </c>
@@ -15190,7 +15277,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A58" s="30">
         <v>43970</v>
       </c>
@@ -15243,7 +15330,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A59" s="30">
         <v>43971</v>
       </c>
@@ -15296,7 +15383,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A60" s="30">
         <v>43972</v>
       </c>
@@ -15349,7 +15436,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A61" s="30">
         <v>43973</v>
       </c>
@@ -15402,7 +15489,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A62" s="30">
         <v>43974</v>
       </c>
@@ -15455,7 +15542,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A63" s="30">
         <v>43975</v>
       </c>
@@ -15508,7 +15595,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A64" s="30">
         <v>43976</v>
       </c>
@@ -15561,7 +15648,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A65" s="51">
         <v>43977</v>
       </c>
@@ -15614,7 +15701,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A66" s="51">
         <v>43978</v>
       </c>
@@ -15667,7 +15754,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A67" s="51">
         <v>43979</v>
       </c>
@@ -15720,7 +15807,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A68" s="51">
         <v>43980</v>
       </c>
@@ -15773,7 +15860,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A69" s="51">
         <v>43981</v>
       </c>
@@ -15826,7 +15913,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A70" s="51">
         <v>43982</v>
       </c>
@@ -15879,7 +15966,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A71" s="51">
         <v>43983</v>
       </c>
@@ -15932,7 +16019,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A72" s="51">
         <v>43984</v>
       </c>
@@ -15985,7 +16072,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A73" s="51">
         <v>43985</v>
       </c>
@@ -16038,7 +16125,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A74" s="51">
         <v>43986</v>
       </c>
@@ -16091,7 +16178,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A75" s="51">
         <v>43987</v>
       </c>
@@ -16144,7 +16231,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A76" s="51">
         <v>43988</v>
       </c>
@@ -16197,7 +16284,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A77" s="51">
         <v>43989</v>
       </c>
@@ -16250,7 +16337,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A78" s="51">
         <v>43990</v>
       </c>
@@ -16303,7 +16390,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A79" s="51">
         <v>43991</v>
       </c>
@@ -16354,6 +16441,59 @@
       </c>
       <c r="Q79" s="13">
         <v>641</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A80" s="51">
+        <v>43992</v>
+      </c>
+      <c r="B80" s="11">
+        <v>8</v>
+      </c>
+      <c r="C80" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D80" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E80" s="11">
+        <v>53</v>
+      </c>
+      <c r="F80" s="11">
+        <v>9</v>
+      </c>
+      <c r="G80" s="11">
+        <v>60</v>
+      </c>
+      <c r="H80" s="11">
+        <v>279</v>
+      </c>
+      <c r="I80" s="11">
+        <v>9</v>
+      </c>
+      <c r="J80" s="11">
+        <v>55</v>
+      </c>
+      <c r="K80" s="11">
+        <v>142</v>
+      </c>
+      <c r="L80" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M80" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N80" s="11">
+        <v>7</v>
+      </c>
+      <c r="O80" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P80" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q80" s="13">
+        <v>623</v>
       </c>
     </row>
   </sheetData>
@@ -16364,23 +16504,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q79"/>
+  <dimension ref="A1:Q80"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B58" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B66" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A79" sqref="A79"/>
+      <selection pane="bottomRight" activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5546875" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5546875" style="2"/>
+    <col min="1" max="1" width="12.453125" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.54296875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -16401,7 +16541,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -16422,7 +16562,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -16475,7 +16615,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="12">
         <v>43916</v>
       </c>
@@ -16528,7 +16668,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
         <v>43917</v>
       </c>
@@ -16581,7 +16721,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="12">
         <v>43918</v>
       </c>
@@ -16634,7 +16774,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
         <v>43919</v>
       </c>
@@ -16687,7 +16827,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="12">
         <v>43920</v>
       </c>
@@ -16740,7 +16880,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="12">
         <v>43921</v>
       </c>
@@ -16793,7 +16933,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="12">
         <v>43922</v>
       </c>
@@ -16846,7 +16986,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
         <v>43923</v>
       </c>
@@ -16899,7 +17039,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="12">
         <v>43924</v>
       </c>
@@ -16952,7 +17092,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <v>43925</v>
       </c>
@@ -17005,7 +17145,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>43926</v>
       </c>
@@ -17058,7 +17198,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="12">
         <v>43927</v>
       </c>
@@ -17111,7 +17251,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="12">
         <v>43928</v>
       </c>
@@ -17164,7 +17304,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="12">
         <v>43929</v>
       </c>
@@ -17217,7 +17357,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="12">
         <v>43930</v>
       </c>
@@ -17270,7 +17410,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="12">
         <v>43931</v>
       </c>
@@ -17323,7 +17463,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="12">
         <v>43932</v>
       </c>
@@ -17376,7 +17516,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="12">
         <v>43933</v>
       </c>
@@ -17429,7 +17569,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="12">
         <v>43934</v>
       </c>
@@ -17482,7 +17622,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="12">
         <v>43935</v>
       </c>
@@ -17535,7 +17675,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" s="12">
         <v>43936</v>
       </c>
@@ -17588,7 +17728,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" s="12">
         <v>43937</v>
       </c>
@@ -17641,7 +17781,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" s="12">
         <v>43938</v>
       </c>
@@ -17694,7 +17834,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" s="12">
         <v>43939</v>
       </c>
@@ -17747,7 +17887,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" s="12">
         <v>43940</v>
       </c>
@@ -17800,7 +17940,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" s="12">
         <v>43941</v>
       </c>
@@ -17853,7 +17993,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" s="12">
         <v>43942</v>
       </c>
@@ -17906,7 +18046,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="12">
         <v>43943</v>
       </c>
@@ -17959,7 +18099,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" s="12">
         <v>43944</v>
       </c>
@@ -18012,7 +18152,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" s="12">
         <v>43945</v>
       </c>
@@ -18065,7 +18205,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" s="12">
         <v>43946</v>
       </c>
@@ -18118,7 +18258,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" s="12">
         <v>43947</v>
       </c>
@@ -18171,7 +18311,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" s="30">
         <v>43948</v>
       </c>
@@ -18224,7 +18364,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" s="30">
         <v>43949</v>
       </c>
@@ -18277,7 +18417,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" s="30">
         <v>43950</v>
       </c>
@@ -18330,7 +18470,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" s="30">
         <v>43951</v>
       </c>
@@ -18383,7 +18523,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" s="30">
         <v>43952</v>
       </c>
@@ -18436,7 +18576,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" s="30">
         <v>43953</v>
       </c>
@@ -18489,7 +18629,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" s="30">
         <v>43954</v>
       </c>
@@ -18542,7 +18682,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" s="30">
         <v>43955</v>
       </c>
@@ -18595,7 +18735,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" s="30">
         <v>43956</v>
       </c>
@@ -18648,7 +18788,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" s="30">
         <v>43957</v>
       </c>
@@ -18701,7 +18841,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" s="30">
         <v>43958</v>
       </c>
@@ -18754,7 +18894,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" s="30">
         <v>43959</v>
       </c>
@@ -18807,7 +18947,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" s="30">
         <v>43960</v>
       </c>
@@ -18860,7 +19000,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" s="30">
         <v>43961</v>
       </c>
@@ -18913,7 +19053,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50" s="30">
         <v>43962</v>
       </c>
@@ -18966,7 +19106,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51" s="30">
         <v>43963</v>
       </c>
@@ -19019,7 +19159,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52" s="30">
         <v>43964</v>
       </c>
@@ -19072,7 +19212,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53" s="30">
         <v>43965</v>
       </c>
@@ -19125,7 +19265,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54" s="30">
         <v>43966</v>
       </c>
@@ -19178,7 +19318,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55" s="30">
         <v>43967</v>
       </c>
@@ -19231,7 +19371,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56" s="30">
         <v>43968</v>
       </c>
@@ -19284,7 +19424,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A57" s="30">
         <v>43969</v>
       </c>
@@ -19337,7 +19477,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A58" s="30">
         <v>43970</v>
       </c>
@@ -19390,7 +19530,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A59" s="30">
         <v>43971</v>
       </c>
@@ -19443,7 +19583,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A60" s="30">
         <v>43972</v>
       </c>
@@ -19496,7 +19636,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A61" s="30">
         <v>43973</v>
       </c>
@@ -19549,7 +19689,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A62" s="30">
         <v>43974</v>
       </c>
@@ -19602,7 +19742,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A63" s="30">
         <v>43975</v>
       </c>
@@ -19655,7 +19795,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A64" s="30">
         <v>43976</v>
       </c>
@@ -19708,7 +19848,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A65" s="30">
         <v>43977</v>
       </c>
@@ -19761,7 +19901,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A66" s="30">
         <v>43978</v>
       </c>
@@ -19814,7 +19954,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A67" s="30">
         <v>43979</v>
       </c>
@@ -19867,7 +20007,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A68" s="30">
         <v>43980</v>
       </c>
@@ -19920,7 +20060,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A69" s="30">
         <v>43981</v>
       </c>
@@ -19973,7 +20113,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A70" s="30">
         <v>43982</v>
       </c>
@@ -20026,7 +20166,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A71" s="30">
         <v>43983</v>
       </c>
@@ -20079,7 +20219,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A72" s="30">
         <v>43984</v>
       </c>
@@ -20132,7 +20272,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A73" s="30">
         <v>43985</v>
       </c>
@@ -20185,7 +20325,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A74" s="30">
         <v>43986</v>
       </c>
@@ -20238,7 +20378,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A75" s="30">
         <v>43987</v>
       </c>
@@ -20291,7 +20431,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A76" s="30">
         <v>43988</v>
       </c>
@@ -20344,7 +20484,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A77" s="30">
         <v>43989</v>
       </c>
@@ -20397,7 +20537,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A78" s="30">
         <v>43990</v>
       </c>
@@ -20450,7 +20590,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A79" s="30">
         <v>43991</v>
       </c>
@@ -20501,6 +20641,59 @@
       </c>
       <c r="Q79" s="13">
         <v>370</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A80" s="30">
+        <v>43992</v>
+      </c>
+      <c r="B80" s="11">
+        <v>24</v>
+      </c>
+      <c r="C80" s="11">
+        <v>11</v>
+      </c>
+      <c r="D80" s="11">
+        <v>8</v>
+      </c>
+      <c r="E80" s="11">
+        <v>28</v>
+      </c>
+      <c r="F80" s="11">
+        <v>24</v>
+      </c>
+      <c r="G80" s="11">
+        <v>14</v>
+      </c>
+      <c r="H80" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I80" s="11">
+        <v>18</v>
+      </c>
+      <c r="J80" s="11">
+        <v>48</v>
+      </c>
+      <c r="K80" s="11">
+        <v>182</v>
+      </c>
+      <c r="L80" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M80" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N80" s="11">
+        <v>6</v>
+      </c>
+      <c r="O80" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P80" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q80" s="13">
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -20533,7 +20726,7 @@
       <value order="0"/>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-09T12:29:11Z</value>
+      <value order="0">2020-06-10T11:51:41Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -20548,16 +20741,16 @@
       <value order="0">Being Drafted</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41637421</value>
+      <value order="0">vA41664623</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">22.4</value>
+      <value order="0">22.6</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">161</value>
+      <value order="0">163</value>
     </field>
     <field name="Objective-VersionComment">
-      <value order="0"/>
+      <value order="0">testing update</value>
     </field>
     <field name="Objective-FileNumber">
       <value order="0">PUBRES/4199</value>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-11 20:09)
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u419207\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA10434\A28088333\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u207826\Objective\Objects\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5990" windowHeight="6030" tabRatio="803" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5990" windowHeight="6040" tabRatio="803"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1757" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1783" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -1634,7 +1634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1743,11 +1743,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S160"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B88" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B82" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M101" sqref="M101"/>
+      <selection pane="bottomRight" activeCell="P100" sqref="P100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6653,20 +6653,54 @@
       </c>
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="C100" s="28"/>
-      <c r="D100" s="28"/>
-      <c r="E100" s="28"/>
-      <c r="F100" s="28"/>
-      <c r="G100" s="28"/>
-      <c r="H100" s="28"/>
-      <c r="I100" s="28"/>
-      <c r="J100" s="28"/>
-      <c r="K100" s="28"/>
-      <c r="L100" s="28"/>
-      <c r="M100" s="28"/>
-      <c r="N100" s="28"/>
-      <c r="O100" s="28"/>
-      <c r="P100" s="28"/>
+      <c r="A100" s="5">
+        <v>43993</v>
+      </c>
+      <c r="B100" s="28">
+        <v>1082</v>
+      </c>
+      <c r="C100" s="28">
+        <v>327</v>
+      </c>
+      <c r="D100" s="28">
+        <v>261</v>
+      </c>
+      <c r="E100" s="28">
+        <v>882</v>
+      </c>
+      <c r="F100" s="28">
+        <v>948</v>
+      </c>
+      <c r="G100" s="28">
+        <v>1288</v>
+      </c>
+      <c r="H100" s="28">
+        <v>3995</v>
+      </c>
+      <c r="I100" s="28">
+        <v>341</v>
+      </c>
+      <c r="J100" s="28">
+        <v>2022</v>
+      </c>
+      <c r="K100" s="28">
+        <v>2783</v>
+      </c>
+      <c r="L100" s="28">
+        <v>8</v>
+      </c>
+      <c r="M100" s="28">
+        <v>54</v>
+      </c>
+      <c r="N100" s="28">
+        <v>1685</v>
+      </c>
+      <c r="O100" s="28">
+        <v>6</v>
+      </c>
+      <c r="P100" s="32">
+        <v>15682</v>
+      </c>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C101" s="28"/>
@@ -7682,11 +7716,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q88"/>
+  <dimension ref="A1:Q89"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M91" sqref="M91"/>
+      <pane ySplit="3" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O92" sqref="O92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12296,6 +12330,59 @@
         <v>18</v>
       </c>
     </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A89" s="30">
+        <v>43993</v>
+      </c>
+      <c r="B89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J89" s="14">
+        <v>6</v>
+      </c>
+      <c r="K89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="L89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P89" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q89" s="13">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -12304,18 +12391,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q80"/>
+  <dimension ref="A1:Q81"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B67" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B64" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N83" sqref="N83"/>
+      <selection pane="bottomRight" activeCell="G82" sqref="G82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.26953125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="15.36328125" style="11" customWidth="1"/>
     <col min="2" max="17" width="10.54296875" style="11" customWidth="1"/>
     <col min="18" max="16384" width="8.54296875" style="2"/>
   </cols>
@@ -16496,6 +16583,59 @@
         <v>623</v>
       </c>
     </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A81" s="51">
+        <v>43993</v>
+      </c>
+      <c r="B81" s="11">
+        <v>7</v>
+      </c>
+      <c r="C81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E81" s="11">
+        <v>57</v>
+      </c>
+      <c r="F81" s="11">
+        <v>9</v>
+      </c>
+      <c r="G81" s="11">
+        <v>60</v>
+      </c>
+      <c r="H81" s="11">
+        <v>272</v>
+      </c>
+      <c r="I81" s="11">
+        <v>7</v>
+      </c>
+      <c r="J81" s="11">
+        <v>55</v>
+      </c>
+      <c r="K81" s="11">
+        <v>141</v>
+      </c>
+      <c r="L81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P81" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q81" s="11">
+        <v>613</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -16504,13 +16644,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q80"/>
+  <dimension ref="A1:Q81"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B66" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A81" sqref="A81"/>
+      <selection pane="bottomRight" activeCell="J87" sqref="J87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20696,12 +20836,65 @@
         <v>364</v>
       </c>
     </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A81" s="30">
+        <v>43993</v>
+      </c>
+      <c r="B81" s="11">
+        <v>19</v>
+      </c>
+      <c r="C81" s="11">
+        <v>8</v>
+      </c>
+      <c r="D81" s="11">
+        <v>12</v>
+      </c>
+      <c r="E81" s="11">
+        <v>16</v>
+      </c>
+      <c r="F81" s="11">
+        <v>36</v>
+      </c>
+      <c r="G81" s="11">
+        <v>18</v>
+      </c>
+      <c r="H81" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I81" s="11">
+        <v>19</v>
+      </c>
+      <c r="J81" s="11">
+        <v>46</v>
+      </c>
+      <c r="K81" s="11">
+        <v>105</v>
+      </c>
+      <c r="L81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N81" s="11">
+        <v>14</v>
+      </c>
+      <c r="O81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q81" s="36">
+        <v>296</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=customXML/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXML/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA" version="1.0.0">
   <systemFields>
     <field name="Objective-Id">
@@ -20720,13 +20913,13 @@
       <value order="0">false</value>
     </field>
     <field name="Objective-IsPublished">
-      <value order="0">false</value>
+      <value order="0">true</value>
     </field>
     <field name="Objective-DatePublished">
-      <value order="0"/>
+      <value order="0">2020-06-11T12:20:34Z</value>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-10T11:51:41Z</value>
+      <value order="0">2020-06-11T12:20:34Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -20738,19 +20931,19 @@
       <value order="0">Analytical: COVID 19 Analysis: Restricted working papers: Research and analysis: Diseases: 2020-2025</value>
     </field>
     <field name="Objective-State">
-      <value order="0">Being Drafted</value>
+      <value order="0">Published</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41664623</value>
+      <value order="0">vA41693787</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">22.6</value>
+      <value order="0">23.0</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">163</value>
+      <value order="0">168</value>
     </field>
     <field name="Objective-VersionComment">
-      <value order="0">testing update</value>
+      <value order="0"/>
     </field>
     <field name="Objective-FileNumber">
       <value order="0">PUBRES/4199</value>
@@ -20784,7 +20977,7 @@
 </metadata>
 </file>
 
-<file path=customXML/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXML/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5745109E-2DDF-40CB-AC2B-FF9B10C90820}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-12 12:10)
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u419207\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA10434\A28088333\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u207826\Objective\Objects\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5990" windowHeight="6030" tabRatio="803" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5990" windowHeight="6040" tabRatio="803"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1757" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1783" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -1634,7 +1634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1743,11 +1743,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S160"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B88" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B82" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M101" sqref="M101"/>
+      <selection pane="bottomRight" activeCell="P100" sqref="P100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6653,20 +6653,54 @@
       </c>
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="C100" s="28"/>
-      <c r="D100" s="28"/>
-      <c r="E100" s="28"/>
-      <c r="F100" s="28"/>
-      <c r="G100" s="28"/>
-      <c r="H100" s="28"/>
-      <c r="I100" s="28"/>
-      <c r="J100" s="28"/>
-      <c r="K100" s="28"/>
-      <c r="L100" s="28"/>
-      <c r="M100" s="28"/>
-      <c r="N100" s="28"/>
-      <c r="O100" s="28"/>
-      <c r="P100" s="28"/>
+      <c r="A100" s="5">
+        <v>43993</v>
+      </c>
+      <c r="B100" s="28">
+        <v>1082</v>
+      </c>
+      <c r="C100" s="28">
+        <v>327</v>
+      </c>
+      <c r="D100" s="28">
+        <v>261</v>
+      </c>
+      <c r="E100" s="28">
+        <v>882</v>
+      </c>
+      <c r="F100" s="28">
+        <v>948</v>
+      </c>
+      <c r="G100" s="28">
+        <v>1288</v>
+      </c>
+      <c r="H100" s="28">
+        <v>3995</v>
+      </c>
+      <c r="I100" s="28">
+        <v>341</v>
+      </c>
+      <c r="J100" s="28">
+        <v>2022</v>
+      </c>
+      <c r="K100" s="28">
+        <v>2783</v>
+      </c>
+      <c r="L100" s="28">
+        <v>8</v>
+      </c>
+      <c r="M100" s="28">
+        <v>54</v>
+      </c>
+      <c r="N100" s="28">
+        <v>1685</v>
+      </c>
+      <c r="O100" s="28">
+        <v>6</v>
+      </c>
+      <c r="P100" s="32">
+        <v>15682</v>
+      </c>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C101" s="28"/>
@@ -7682,11 +7716,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q88"/>
+  <dimension ref="A1:Q89"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M91" sqref="M91"/>
+      <pane ySplit="3" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O92" sqref="O92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12296,6 +12330,59 @@
         <v>18</v>
       </c>
     </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A89" s="30">
+        <v>43993</v>
+      </c>
+      <c r="B89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J89" s="14">
+        <v>6</v>
+      </c>
+      <c r="K89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="L89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P89" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q89" s="13">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -12304,18 +12391,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q80"/>
+  <dimension ref="A1:Q81"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B67" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B64" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N83" sqref="N83"/>
+      <selection pane="bottomRight" activeCell="G82" sqref="G82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.26953125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="15.36328125" style="11" customWidth="1"/>
     <col min="2" max="17" width="10.54296875" style="11" customWidth="1"/>
     <col min="18" max="16384" width="8.54296875" style="2"/>
   </cols>
@@ -16496,6 +16583,59 @@
         <v>623</v>
       </c>
     </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A81" s="51">
+        <v>43993</v>
+      </c>
+      <c r="B81" s="11">
+        <v>7</v>
+      </c>
+      <c r="C81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E81" s="11">
+        <v>57</v>
+      </c>
+      <c r="F81" s="11">
+        <v>9</v>
+      </c>
+      <c r="G81" s="11">
+        <v>60</v>
+      </c>
+      <c r="H81" s="11">
+        <v>272</v>
+      </c>
+      <c r="I81" s="11">
+        <v>7</v>
+      </c>
+      <c r="J81" s="11">
+        <v>55</v>
+      </c>
+      <c r="K81" s="11">
+        <v>141</v>
+      </c>
+      <c r="L81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P81" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q81" s="11">
+        <v>613</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -16504,13 +16644,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q80"/>
+  <dimension ref="A1:Q81"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B66" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A81" sqref="A81"/>
+      <selection pane="bottomRight" activeCell="J87" sqref="J87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20696,12 +20836,65 @@
         <v>364</v>
       </c>
     </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A81" s="30">
+        <v>43993</v>
+      </c>
+      <c r="B81" s="11">
+        <v>19</v>
+      </c>
+      <c r="C81" s="11">
+        <v>8</v>
+      </c>
+      <c r="D81" s="11">
+        <v>12</v>
+      </c>
+      <c r="E81" s="11">
+        <v>16</v>
+      </c>
+      <c r="F81" s="11">
+        <v>36</v>
+      </c>
+      <c r="G81" s="11">
+        <v>18</v>
+      </c>
+      <c r="H81" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I81" s="11">
+        <v>19</v>
+      </c>
+      <c r="J81" s="11">
+        <v>46</v>
+      </c>
+      <c r="K81" s="11">
+        <v>105</v>
+      </c>
+      <c r="L81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N81" s="11">
+        <v>14</v>
+      </c>
+      <c r="O81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q81" s="36">
+        <v>296</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=customXML/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXML/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA" version="1.0.0">
   <systemFields>
     <field name="Objective-Id">
@@ -20720,13 +20913,13 @@
       <value order="0">false</value>
     </field>
     <field name="Objective-IsPublished">
-      <value order="0">false</value>
+      <value order="0">true</value>
     </field>
     <field name="Objective-DatePublished">
-      <value order="0"/>
+      <value order="0">2020-06-11T12:20:34Z</value>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-10T11:51:41Z</value>
+      <value order="0">2020-06-11T12:20:34Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -20738,19 +20931,19 @@
       <value order="0">Analytical: COVID 19 Analysis: Restricted working papers: Research and analysis: Diseases: 2020-2025</value>
     </field>
     <field name="Objective-State">
-      <value order="0">Being Drafted</value>
+      <value order="0">Published</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41664623</value>
+      <value order="0">vA41693787</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">22.6</value>
+      <value order="0">23.0</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">163</value>
+      <value order="0">168</value>
     </field>
     <field name="Objective-VersionComment">
-      <value order="0">testing update</value>
+      <value order="0"/>
     </field>
     <field name="Objective-FileNumber">
       <value order="0">PUBRES/4199</value>
@@ -20784,7 +20977,7 @@
 </metadata>
 </file>
 
-<file path=customXML/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXML/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5745109E-2DDF-40CB-AC2B-FF9B10C90820}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-12 20:08)
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5990" windowHeight="6030" tabRatio="803" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5990" windowHeight="6050" tabRatio="803" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1757" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1808" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -256,7 +256,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -384,12 +384,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -499,6 +508,8 @@
     <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1245,6 +1256,39 @@
             </a:rPr>
             <a:t>(iv) Due to a revision on the NHS Fife data on the number of confirmed and suspected COVID-19 patients in ICU for 26 May, the total figure for Scotland has been revised from 36 to 35.</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(v) Due to a revision on the NHS Lanarkshire data on the number of confirmed COVID-19 patients in hospital  for 11 June, the total figure for Scotland has been revised from 613  to 610.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
           <a:endParaRPr lang="en-GB" sz="1100">
             <a:effectLst/>
             <a:latin typeface="+mn-lt"/>
@@ -1720,8 +1764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K66" sqref="K66"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="O52" sqref="O52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1744,10 +1788,10 @@
   <dimension ref="A1:S160"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B88" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B82" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M101" sqref="M101"/>
+      <selection pane="bottomRight" activeCell="N102" sqref="N102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6653,36 +6697,104 @@
       </c>
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="C100" s="28"/>
-      <c r="D100" s="28"/>
-      <c r="E100" s="28"/>
-      <c r="F100" s="28"/>
-      <c r="G100" s="28"/>
-      <c r="H100" s="28"/>
-      <c r="I100" s="28"/>
-      <c r="J100" s="28"/>
-      <c r="K100" s="28"/>
-      <c r="L100" s="28"/>
-      <c r="M100" s="28"/>
-      <c r="N100" s="28"/>
-      <c r="O100" s="28"/>
-      <c r="P100" s="28"/>
+      <c r="A100" s="5">
+        <v>43993</v>
+      </c>
+      <c r="B100" s="28">
+        <v>1082</v>
+      </c>
+      <c r="C100" s="28">
+        <v>327</v>
+      </c>
+      <c r="D100" s="28">
+        <v>261</v>
+      </c>
+      <c r="E100" s="28">
+        <v>882</v>
+      </c>
+      <c r="F100" s="28">
+        <v>948</v>
+      </c>
+      <c r="G100" s="28">
+        <v>1288</v>
+      </c>
+      <c r="H100" s="28">
+        <v>3995</v>
+      </c>
+      <c r="I100" s="28">
+        <v>341</v>
+      </c>
+      <c r="J100" s="28">
+        <v>2022</v>
+      </c>
+      <c r="K100" s="28">
+        <v>2783</v>
+      </c>
+      <c r="L100" s="28">
+        <v>8</v>
+      </c>
+      <c r="M100" s="28">
+        <v>54</v>
+      </c>
+      <c r="N100" s="28">
+        <v>1685</v>
+      </c>
+      <c r="O100" s="28">
+        <v>6</v>
+      </c>
+      <c r="P100" s="32">
+        <v>15682</v>
+      </c>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="C101" s="28"/>
-      <c r="D101" s="28"/>
-      <c r="E101" s="28"/>
-      <c r="F101" s="28"/>
-      <c r="G101" s="28"/>
-      <c r="H101" s="28"/>
-      <c r="I101" s="28"/>
-      <c r="J101" s="28"/>
-      <c r="K101" s="28"/>
-      <c r="L101" s="28"/>
-      <c r="M101" s="28"/>
-      <c r="N101" s="28"/>
-      <c r="O101" s="28"/>
-      <c r="P101" s="28"/>
+      <c r="A101" s="5">
+        <v>43994</v>
+      </c>
+      <c r="B101" s="28">
+        <v>1086</v>
+      </c>
+      <c r="C101" s="28">
+        <v>327</v>
+      </c>
+      <c r="D101" s="28">
+        <v>261</v>
+      </c>
+      <c r="E101" s="28">
+        <v>883</v>
+      </c>
+      <c r="F101" s="28">
+        <v>948</v>
+      </c>
+      <c r="G101" s="28">
+        <v>1288</v>
+      </c>
+      <c r="H101" s="28">
+        <v>4000</v>
+      </c>
+      <c r="I101" s="28">
+        <v>341</v>
+      </c>
+      <c r="J101" s="28">
+        <v>2028</v>
+      </c>
+      <c r="K101" s="28">
+        <v>2794</v>
+      </c>
+      <c r="L101" s="28">
+        <v>8</v>
+      </c>
+      <c r="M101" s="28">
+        <v>54</v>
+      </c>
+      <c r="N101" s="28">
+        <v>1685</v>
+      </c>
+      <c r="O101" s="28">
+        <v>6</v>
+      </c>
+      <c r="P101" s="32">
+        <v>15709</v>
+      </c>
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C102" s="28"/>
@@ -7682,11 +7794,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q88"/>
+  <dimension ref="A1:Q90"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M91" sqref="M91"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12296,6 +12408,112 @@
         <v>18</v>
       </c>
     </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A89" s="30">
+        <v>43993</v>
+      </c>
+      <c r="B89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J89" s="14">
+        <v>6</v>
+      </c>
+      <c r="K89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="L89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P89" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q89" s="13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A90" s="30">
+        <v>43994</v>
+      </c>
+      <c r="B90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K90" s="14">
+        <v>8</v>
+      </c>
+      <c r="L90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P90" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q90" s="13">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -12304,18 +12522,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q80"/>
+  <dimension ref="A1:R82"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B67" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B78" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N83" sqref="N83"/>
+      <selection pane="bottomRight" activeCell="K81" sqref="K81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.26953125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="15.453125" style="11" customWidth="1"/>
     <col min="2" max="17" width="10.54296875" style="11" customWidth="1"/>
     <col min="18" max="16384" width="8.54296875" style="2"/>
   </cols>
@@ -15648,7 +15866,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A65" s="51">
         <v>43977</v>
       </c>
@@ -15701,7 +15919,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A66" s="51">
         <v>43978</v>
       </c>
@@ -15754,7 +15972,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A67" s="51">
         <v>43979</v>
       </c>
@@ -15807,7 +16025,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A68" s="51">
         <v>43980</v>
       </c>
@@ -15860,7 +16078,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A69" s="51">
         <v>43981</v>
       </c>
@@ -15913,7 +16131,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A70" s="51">
         <v>43982</v>
       </c>
@@ -15966,7 +16184,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A71" s="51">
         <v>43983</v>
       </c>
@@ -16019,7 +16237,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A72" s="51">
         <v>43984</v>
       </c>
@@ -16072,7 +16290,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A73" s="51">
         <v>43985</v>
       </c>
@@ -16125,7 +16343,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A74" s="51">
         <v>43986</v>
       </c>
@@ -16178,7 +16396,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A75" s="51">
         <v>43987</v>
       </c>
@@ -16231,7 +16449,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A76" s="51">
         <v>43988</v>
       </c>
@@ -16284,7 +16502,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A77" s="51">
         <v>43989</v>
       </c>
@@ -16337,7 +16555,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A78" s="51">
         <v>43990</v>
       </c>
@@ -16390,7 +16608,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A79" s="51">
         <v>43991</v>
       </c>
@@ -16443,7 +16661,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A80" s="51">
         <v>43992</v>
       </c>
@@ -16492,9 +16710,118 @@
       <c r="P80" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="Q80" s="13">
+      <c r="Q80" s="53">
         <v>623</v>
       </c>
+      <c r="R80" s="54"/>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A81" s="51">
+        <v>43993</v>
+      </c>
+      <c r="B81" s="11">
+        <v>7</v>
+      </c>
+      <c r="C81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E81" s="11">
+        <v>57</v>
+      </c>
+      <c r="F81" s="11">
+        <v>9</v>
+      </c>
+      <c r="G81" s="11">
+        <v>60</v>
+      </c>
+      <c r="H81" s="11">
+        <v>272</v>
+      </c>
+      <c r="I81" s="11">
+        <v>7</v>
+      </c>
+      <c r="J81" s="11">
+        <v>52</v>
+      </c>
+      <c r="K81" s="11">
+        <v>141</v>
+      </c>
+      <c r="L81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P81" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q81" s="13">
+        <v>610</v>
+      </c>
+      <c r="R81" s="54"/>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A82" s="51">
+        <v>43994</v>
+      </c>
+      <c r="B82" s="11">
+        <v>6</v>
+      </c>
+      <c r="C82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E82" s="11">
+        <v>57</v>
+      </c>
+      <c r="F82" s="11">
+        <v>7</v>
+      </c>
+      <c r="G82" s="11">
+        <v>58</v>
+      </c>
+      <c r="H82" s="11">
+        <v>260</v>
+      </c>
+      <c r="I82" s="11">
+        <v>7</v>
+      </c>
+      <c r="J82" s="11">
+        <v>51</v>
+      </c>
+      <c r="K82" s="11">
+        <v>138</v>
+      </c>
+      <c r="L82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N82" s="14">
+        <v>5</v>
+      </c>
+      <c r="O82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q82" s="13">
+        <v>590</v>
+      </c>
+      <c r="R82" s="54"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16504,13 +16831,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q80"/>
+  <dimension ref="A1:Q82"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B66" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A81" sqref="A81"/>
+      <selection pane="bottomRight" activeCell="M87" sqref="M87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20696,12 +21023,118 @@
         <v>364</v>
       </c>
     </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A81" s="30">
+        <v>43993</v>
+      </c>
+      <c r="B81" s="11">
+        <v>19</v>
+      </c>
+      <c r="C81" s="11">
+        <v>8</v>
+      </c>
+      <c r="D81" s="11">
+        <v>12</v>
+      </c>
+      <c r="E81" s="11">
+        <v>16</v>
+      </c>
+      <c r="F81" s="11">
+        <v>36</v>
+      </c>
+      <c r="G81" s="11">
+        <v>18</v>
+      </c>
+      <c r="H81" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I81" s="11">
+        <v>19</v>
+      </c>
+      <c r="J81" s="11">
+        <v>46</v>
+      </c>
+      <c r="K81" s="11">
+        <v>105</v>
+      </c>
+      <c r="L81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N81" s="11">
+        <v>14</v>
+      </c>
+      <c r="O81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q81" s="13">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A82" s="30">
+        <v>43994</v>
+      </c>
+      <c r="B82" s="11">
+        <v>17</v>
+      </c>
+      <c r="C82" s="11">
+        <v>18</v>
+      </c>
+      <c r="D82" s="11">
+        <v>14</v>
+      </c>
+      <c r="E82" s="11">
+        <v>22</v>
+      </c>
+      <c r="F82" s="11">
+        <v>33</v>
+      </c>
+      <c r="G82" s="11">
+        <v>13</v>
+      </c>
+      <c r="H82" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I82" s="11">
+        <v>26</v>
+      </c>
+      <c r="J82" s="11">
+        <v>43</v>
+      </c>
+      <c r="K82" s="11">
+        <v>128</v>
+      </c>
+      <c r="L82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N82" s="11">
+        <v>8</v>
+      </c>
+      <c r="O82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q82" s="13">
+        <v>324</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=customXML/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXML/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA" version="1.0.0">
   <systemFields>
     <field name="Objective-Id">
@@ -20720,13 +21153,13 @@
       <value order="0">false</value>
     </field>
     <field name="Objective-IsPublished">
-      <value order="0">false</value>
+      <value order="0">true</value>
     </field>
     <field name="Objective-DatePublished">
-      <value order="0"/>
+      <value order="0">2020-06-12T12:12:01Z</value>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-10T11:51:41Z</value>
+      <value order="0">2020-06-12T12:12:01Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -20738,19 +21171,19 @@
       <value order="0">Analytical: COVID 19 Analysis: Restricted working papers: Research and analysis: Diseases: 2020-2025</value>
     </field>
     <field name="Objective-State">
-      <value order="0">Being Drafted</value>
+      <value order="0">Published</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41664623</value>
+      <value order="0">vA41719189</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">22.6</value>
+      <value order="0">24.0</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">163</value>
+      <value order="0">171</value>
     </field>
     <field name="Objective-VersionComment">
-      <value order="0">testing update</value>
+      <value order="0"/>
     </field>
     <field name="Objective-FileNumber">
       <value order="0">PUBRES/4199</value>
@@ -20784,7 +21217,7 @@
 </metadata>
 </file>
 
-<file path=customXML/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXML/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5745109E-2DDF-40CB-AC2B-FF9B10C90820}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-12 20:08) (#114)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5990" windowHeight="6030" tabRatio="803" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5990" windowHeight="6050" tabRatio="803" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1757" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1808" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -256,7 +256,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -384,12 +384,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -499,6 +508,8 @@
     <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1245,6 +1256,39 @@
             </a:rPr>
             <a:t>(iv) Due to a revision on the NHS Fife data on the number of confirmed and suspected COVID-19 patients in ICU for 26 May, the total figure for Scotland has been revised from 36 to 35.</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(v) Due to a revision on the NHS Lanarkshire data on the number of confirmed COVID-19 patients in hospital  for 11 June, the total figure for Scotland has been revised from 613  to 610.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
           <a:endParaRPr lang="en-GB" sz="1100">
             <a:effectLst/>
             <a:latin typeface="+mn-lt"/>
@@ -1720,8 +1764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K66" sqref="K66"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="O52" sqref="O52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1744,10 +1788,10 @@
   <dimension ref="A1:S160"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B88" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B82" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M101" sqref="M101"/>
+      <selection pane="bottomRight" activeCell="N102" sqref="N102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6653,36 +6697,104 @@
       </c>
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="C100" s="28"/>
-      <c r="D100" s="28"/>
-      <c r="E100" s="28"/>
-      <c r="F100" s="28"/>
-      <c r="G100" s="28"/>
-      <c r="H100" s="28"/>
-      <c r="I100" s="28"/>
-      <c r="J100" s="28"/>
-      <c r="K100" s="28"/>
-      <c r="L100" s="28"/>
-      <c r="M100" s="28"/>
-      <c r="N100" s="28"/>
-      <c r="O100" s="28"/>
-      <c r="P100" s="28"/>
+      <c r="A100" s="5">
+        <v>43993</v>
+      </c>
+      <c r="B100" s="28">
+        <v>1082</v>
+      </c>
+      <c r="C100" s="28">
+        <v>327</v>
+      </c>
+      <c r="D100" s="28">
+        <v>261</v>
+      </c>
+      <c r="E100" s="28">
+        <v>882</v>
+      </c>
+      <c r="F100" s="28">
+        <v>948</v>
+      </c>
+      <c r="G100" s="28">
+        <v>1288</v>
+      </c>
+      <c r="H100" s="28">
+        <v>3995</v>
+      </c>
+      <c r="I100" s="28">
+        <v>341</v>
+      </c>
+      <c r="J100" s="28">
+        <v>2022</v>
+      </c>
+      <c r="K100" s="28">
+        <v>2783</v>
+      </c>
+      <c r="L100" s="28">
+        <v>8</v>
+      </c>
+      <c r="M100" s="28">
+        <v>54</v>
+      </c>
+      <c r="N100" s="28">
+        <v>1685</v>
+      </c>
+      <c r="O100" s="28">
+        <v>6</v>
+      </c>
+      <c r="P100" s="32">
+        <v>15682</v>
+      </c>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="C101" s="28"/>
-      <c r="D101" s="28"/>
-      <c r="E101" s="28"/>
-      <c r="F101" s="28"/>
-      <c r="G101" s="28"/>
-      <c r="H101" s="28"/>
-      <c r="I101" s="28"/>
-      <c r="J101" s="28"/>
-      <c r="K101" s="28"/>
-      <c r="L101" s="28"/>
-      <c r="M101" s="28"/>
-      <c r="N101" s="28"/>
-      <c r="O101" s="28"/>
-      <c r="P101" s="28"/>
+      <c r="A101" s="5">
+        <v>43994</v>
+      </c>
+      <c r="B101" s="28">
+        <v>1086</v>
+      </c>
+      <c r="C101" s="28">
+        <v>327</v>
+      </c>
+      <c r="D101" s="28">
+        <v>261</v>
+      </c>
+      <c r="E101" s="28">
+        <v>883</v>
+      </c>
+      <c r="F101" s="28">
+        <v>948</v>
+      </c>
+      <c r="G101" s="28">
+        <v>1288</v>
+      </c>
+      <c r="H101" s="28">
+        <v>4000</v>
+      </c>
+      <c r="I101" s="28">
+        <v>341</v>
+      </c>
+      <c r="J101" s="28">
+        <v>2028</v>
+      </c>
+      <c r="K101" s="28">
+        <v>2794</v>
+      </c>
+      <c r="L101" s="28">
+        <v>8</v>
+      </c>
+      <c r="M101" s="28">
+        <v>54</v>
+      </c>
+      <c r="N101" s="28">
+        <v>1685</v>
+      </c>
+      <c r="O101" s="28">
+        <v>6</v>
+      </c>
+      <c r="P101" s="32">
+        <v>15709</v>
+      </c>
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C102" s="28"/>
@@ -7682,11 +7794,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q88"/>
+  <dimension ref="A1:Q90"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M91" sqref="M91"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12296,6 +12408,112 @@
         <v>18</v>
       </c>
     </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A89" s="30">
+        <v>43993</v>
+      </c>
+      <c r="B89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J89" s="14">
+        <v>6</v>
+      </c>
+      <c r="K89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="L89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P89" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q89" s="13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A90" s="30">
+        <v>43994</v>
+      </c>
+      <c r="B90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K90" s="14">
+        <v>8</v>
+      </c>
+      <c r="L90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P90" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q90" s="13">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -12304,18 +12522,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q80"/>
+  <dimension ref="A1:R82"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B67" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B78" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N83" sqref="N83"/>
+      <selection pane="bottomRight" activeCell="K81" sqref="K81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.26953125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="15.453125" style="11" customWidth="1"/>
     <col min="2" max="17" width="10.54296875" style="11" customWidth="1"/>
     <col min="18" max="16384" width="8.54296875" style="2"/>
   </cols>
@@ -15648,7 +15866,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A65" s="51">
         <v>43977</v>
       </c>
@@ -15701,7 +15919,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A66" s="51">
         <v>43978</v>
       </c>
@@ -15754,7 +15972,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A67" s="51">
         <v>43979</v>
       </c>
@@ -15807,7 +16025,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A68" s="51">
         <v>43980</v>
       </c>
@@ -15860,7 +16078,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A69" s="51">
         <v>43981</v>
       </c>
@@ -15913,7 +16131,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A70" s="51">
         <v>43982</v>
       </c>
@@ -15966,7 +16184,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A71" s="51">
         <v>43983</v>
       </c>
@@ -16019,7 +16237,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A72" s="51">
         <v>43984</v>
       </c>
@@ -16072,7 +16290,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A73" s="51">
         <v>43985</v>
       </c>
@@ -16125,7 +16343,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A74" s="51">
         <v>43986</v>
       </c>
@@ -16178,7 +16396,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A75" s="51">
         <v>43987</v>
       </c>
@@ -16231,7 +16449,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A76" s="51">
         <v>43988</v>
       </c>
@@ -16284,7 +16502,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A77" s="51">
         <v>43989</v>
       </c>
@@ -16337,7 +16555,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A78" s="51">
         <v>43990</v>
       </c>
@@ -16390,7 +16608,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A79" s="51">
         <v>43991</v>
       </c>
@@ -16443,7 +16661,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A80" s="51">
         <v>43992</v>
       </c>
@@ -16492,9 +16710,118 @@
       <c r="P80" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="Q80" s="13">
+      <c r="Q80" s="53">
         <v>623</v>
       </c>
+      <c r="R80" s="54"/>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A81" s="51">
+        <v>43993</v>
+      </c>
+      <c r="B81" s="11">
+        <v>7</v>
+      </c>
+      <c r="C81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E81" s="11">
+        <v>57</v>
+      </c>
+      <c r="F81" s="11">
+        <v>9</v>
+      </c>
+      <c r="G81" s="11">
+        <v>60</v>
+      </c>
+      <c r="H81" s="11">
+        <v>272</v>
+      </c>
+      <c r="I81" s="11">
+        <v>7</v>
+      </c>
+      <c r="J81" s="11">
+        <v>52</v>
+      </c>
+      <c r="K81" s="11">
+        <v>141</v>
+      </c>
+      <c r="L81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P81" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q81" s="13">
+        <v>610</v>
+      </c>
+      <c r="R81" s="54"/>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A82" s="51">
+        <v>43994</v>
+      </c>
+      <c r="B82" s="11">
+        <v>6</v>
+      </c>
+      <c r="C82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E82" s="11">
+        <v>57</v>
+      </c>
+      <c r="F82" s="11">
+        <v>7</v>
+      </c>
+      <c r="G82" s="11">
+        <v>58</v>
+      </c>
+      <c r="H82" s="11">
+        <v>260</v>
+      </c>
+      <c r="I82" s="11">
+        <v>7</v>
+      </c>
+      <c r="J82" s="11">
+        <v>51</v>
+      </c>
+      <c r="K82" s="11">
+        <v>138</v>
+      </c>
+      <c r="L82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N82" s="14">
+        <v>5</v>
+      </c>
+      <c r="O82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q82" s="13">
+        <v>590</v>
+      </c>
+      <c r="R82" s="54"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16504,13 +16831,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q80"/>
+  <dimension ref="A1:Q82"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B66" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A81" sqref="A81"/>
+      <selection pane="bottomRight" activeCell="M87" sqref="M87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20696,12 +21023,118 @@
         <v>364</v>
       </c>
     </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A81" s="30">
+        <v>43993</v>
+      </c>
+      <c r="B81" s="11">
+        <v>19</v>
+      </c>
+      <c r="C81" s="11">
+        <v>8</v>
+      </c>
+      <c r="D81" s="11">
+        <v>12</v>
+      </c>
+      <c r="E81" s="11">
+        <v>16</v>
+      </c>
+      <c r="F81" s="11">
+        <v>36</v>
+      </c>
+      <c r="G81" s="11">
+        <v>18</v>
+      </c>
+      <c r="H81" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I81" s="11">
+        <v>19</v>
+      </c>
+      <c r="J81" s="11">
+        <v>46</v>
+      </c>
+      <c r="K81" s="11">
+        <v>105</v>
+      </c>
+      <c r="L81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N81" s="11">
+        <v>14</v>
+      </c>
+      <c r="O81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P81" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q81" s="13">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A82" s="30">
+        <v>43994</v>
+      </c>
+      <c r="B82" s="11">
+        <v>17</v>
+      </c>
+      <c r="C82" s="11">
+        <v>18</v>
+      </c>
+      <c r="D82" s="11">
+        <v>14</v>
+      </c>
+      <c r="E82" s="11">
+        <v>22</v>
+      </c>
+      <c r="F82" s="11">
+        <v>33</v>
+      </c>
+      <c r="G82" s="11">
+        <v>13</v>
+      </c>
+      <c r="H82" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I82" s="11">
+        <v>26</v>
+      </c>
+      <c r="J82" s="11">
+        <v>43</v>
+      </c>
+      <c r="K82" s="11">
+        <v>128</v>
+      </c>
+      <c r="L82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N82" s="11">
+        <v>8</v>
+      </c>
+      <c r="O82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P82" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q82" s="13">
+        <v>324</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=customXML/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXML/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA" version="1.0.0">
   <systemFields>
     <field name="Objective-Id">
@@ -20720,13 +21153,13 @@
       <value order="0">false</value>
     </field>
     <field name="Objective-IsPublished">
-      <value order="0">false</value>
+      <value order="0">true</value>
     </field>
     <field name="Objective-DatePublished">
-      <value order="0"/>
+      <value order="0">2020-06-12T12:12:01Z</value>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-10T11:51:41Z</value>
+      <value order="0">2020-06-12T12:12:01Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -20738,19 +21171,19 @@
       <value order="0">Analytical: COVID 19 Analysis: Restricted working papers: Research and analysis: Diseases: 2020-2025</value>
     </field>
     <field name="Objective-State">
-      <value order="0">Being Drafted</value>
+      <value order="0">Published</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41664623</value>
+      <value order="0">vA41719189</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">22.6</value>
+      <value order="0">24.0</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">163</value>
+      <value order="0">171</value>
     </field>
     <field name="Objective-VersionComment">
-      <value order="0">testing update</value>
+      <value order="0"/>
     </field>
     <field name="Objective-FileNumber">
       <value order="0">PUBRES/4199</value>
@@ -20784,7 +21217,7 @@
 </metadata>
 </file>
 
-<file path=customXML/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXML/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5745109E-2DDF-40CB-AC2B-FF9B10C90820}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-14 20:08)
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u207826\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA4095\A28088333\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U445783\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA18464\A28088333\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5985" windowHeight="6045" tabRatio="803"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5988" windowHeight="6048" tabRatio="803" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1833" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1858" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -1927,23 +1927,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="90.42578125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.42578125" style="2"/>
+    <col min="2" max="2" width="29.44140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="90.44140625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" s="18" t="s">
         <v>20</v>
       </c>
@@ -1951,7 +1953,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20" t="s">
         <v>22</v>
       </c>
@@ -1959,13 +1961,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="22" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="23"/>
     </row>
-    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="24" t="s">
         <v>26</v>
       </c>
@@ -1973,7 +1975,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="24" t="s">
         <v>27</v>
       </c>
@@ -1981,7 +1983,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="24" t="s">
         <v>36</v>
       </c>
@@ -1989,7 +1991,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="20" t="s">
         <v>37</v>
       </c>
@@ -2017,12 +2019,12 @@
       <selection activeCell="O52" sqref="O52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.42578125" style="2"/>
+    <col min="1" max="16384" width="9.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" ht="15" x14ac:dyDescent="0.3">
       <c r="A44" s="43"/>
     </row>
   </sheetData>
@@ -2036,21 +2038,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S160"/>
   <sheetViews>
-    <sheetView zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B91" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B85" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L105" sqref="L105"/>
+      <selection pane="bottomRight" activeCell="H93" sqref="H93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" style="2" customWidth="1"/>
-    <col min="2" max="16" width="11.42578125" style="11" customWidth="1"/>
-    <col min="17" max="16384" width="8.5703125" style="2"/>
+    <col min="2" max="16" width="11.44140625" style="11" customWidth="1"/>
+    <col min="17" max="16384" width="8.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -2070,7 +2072,7 @@
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -2089,7 +2091,7 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -2139,7 +2141,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>43897</v>
       </c>
@@ -2189,7 +2191,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>43898</v>
       </c>
@@ -2239,7 +2241,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>43899</v>
       </c>
@@ -2289,7 +2291,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>43900</v>
       </c>
@@ -2339,7 +2341,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>43901</v>
       </c>
@@ -2389,7 +2391,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>43902</v>
       </c>
@@ -2439,7 +2441,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>43903</v>
       </c>
@@ -2489,7 +2491,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>43904</v>
       </c>
@@ -2539,7 +2541,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>43905</v>
       </c>
@@ -2589,7 +2591,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>43906</v>
       </c>
@@ -2639,7 +2641,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>43907</v>
       </c>
@@ -2689,7 +2691,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>43908</v>
       </c>
@@ -2739,7 +2741,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>43909</v>
       </c>
@@ -2789,7 +2791,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>43910</v>
       </c>
@@ -2839,7 +2841,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>43911</v>
       </c>
@@ -2889,7 +2891,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>43912</v>
       </c>
@@ -2939,7 +2941,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>43913</v>
       </c>
@@ -2989,7 +2991,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>43914</v>
       </c>
@@ -3039,7 +3041,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>43915</v>
       </c>
@@ -3089,7 +3091,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>43916</v>
       </c>
@@ -3139,7 +3141,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>43917</v>
       </c>
@@ -3189,7 +3191,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>43918</v>
       </c>
@@ -3239,7 +3241,7 @@
         <v>1264</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>43919</v>
       </c>
@@ -3289,7 +3291,7 @@
         <v>1417</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>43920</v>
       </c>
@@ -3339,7 +3341,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>43921</v>
       </c>
@@ -3389,7 +3391,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>43922</v>
       </c>
@@ -3439,7 +3441,7 @@
         <v>2310</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>43923</v>
       </c>
@@ -3489,7 +3491,7 @@
         <v>2602</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <v>43924</v>
       </c>
@@ -3539,7 +3541,7 @@
         <v>3001</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>43925</v>
       </c>
@@ -3589,7 +3591,7 @@
         <v>3345</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
         <v>43926</v>
       </c>
@@ -3639,7 +3641,7 @@
         <v>3706</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
         <v>43927</v>
       </c>
@@ -3689,7 +3691,7 @@
         <v>3961</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
         <v>43928</v>
       </c>
@@ -3739,7 +3741,7 @@
         <v>4229</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>43929</v>
       </c>
@@ -3789,7 +3791,7 @@
         <v>4565</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
         <v>43930</v>
       </c>
@@ -3839,7 +3841,7 @@
         <v>4957</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
         <v>43931</v>
       </c>
@@ -3889,7 +3891,7 @@
         <v>5275</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>43932</v>
       </c>
@@ -3939,7 +3941,7 @@
         <v>5590</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
         <v>43933</v>
       </c>
@@ -3989,7 +3991,7 @@
         <v>5912</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
         <v>43934</v>
       </c>
@@ -4039,7 +4041,7 @@
         <v>6067</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>43935</v>
       </c>
@@ -4089,7 +4091,7 @@
         <v>6358</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
         <v>43936</v>
       </c>
@@ -4139,7 +4141,7 @@
         <v>6748</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" s="5">
         <v>43937</v>
       </c>
@@ -4189,7 +4191,7 @@
         <v>7102</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
         <v>43938</v>
       </c>
@@ -4239,7 +4241,7 @@
         <v>7409</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" s="5">
         <v>43939</v>
       </c>
@@ -4289,7 +4291,7 @@
         <v>7820</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" s="5">
         <v>43940</v>
       </c>
@@ -4339,7 +4341,7 @@
         <v>8187</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
         <v>43941</v>
       </c>
@@ -4389,7 +4391,7 @@
         <v>8450</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A49" s="5">
         <v>43942</v>
       </c>
@@ -4439,7 +4441,7 @@
         <v>8672</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
         <v>43943</v>
       </c>
@@ -4489,7 +4491,7 @@
         <v>9038</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A51" s="5">
         <v>43944</v>
       </c>
@@ -4539,7 +4541,7 @@
         <v>9409</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A52" s="5">
         <v>43945</v>
       </c>
@@ -4589,7 +4591,7 @@
         <v>9697</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A53" s="5">
         <v>43946</v>
       </c>
@@ -4639,7 +4641,7 @@
         <v>10051</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A54" s="5">
         <v>43947</v>
       </c>
@@ -4690,7 +4692,7 @@
       </c>
       <c r="R54" s="38"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A55" s="5">
         <v>43948</v>
       </c>
@@ -4741,7 +4743,7 @@
       </c>
       <c r="R55" s="38"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A56" s="5">
         <v>43949</v>
       </c>
@@ -4792,7 +4794,7 @@
       </c>
       <c r="R56" s="39"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A57" s="5">
         <v>43950</v>
       </c>
@@ -4842,7 +4844,7 @@
         <v>11034</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A58" s="5">
         <v>43951</v>
       </c>
@@ -4893,7 +4895,7 @@
       </c>
       <c r="R58" s="38"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A59" s="5">
         <v>43952</v>
       </c>
@@ -4945,7 +4947,7 @@
       <c r="R59" s="38"/>
       <c r="S59" s="38"/>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A60" s="5">
         <v>43953</v>
       </c>
@@ -4995,7 +4997,7 @@
         <v>11927</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A61" s="5">
         <v>43954</v>
       </c>
@@ -5045,7 +5047,7 @@
         <v>12097</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A62" s="5">
         <v>43955</v>
       </c>
@@ -5095,7 +5097,7 @@
         <v>12266</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A63" s="5">
         <v>43956</v>
       </c>
@@ -5145,7 +5147,7 @@
         <v>12437</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A64" s="5">
         <v>43957</v>
       </c>
@@ -5195,7 +5197,7 @@
         <v>12709</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65" s="5">
         <v>43958</v>
       </c>
@@ -5245,7 +5247,7 @@
         <v>12924</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66" s="5">
         <v>43959</v>
       </c>
@@ -5295,7 +5297,7 @@
         <v>13149</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A67" s="5">
         <v>43960</v>
       </c>
@@ -5345,7 +5347,7 @@
         <v>13305</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A68" s="5">
         <v>43961</v>
       </c>
@@ -5395,7 +5397,7 @@
         <v>13486</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A69" s="5">
         <v>43962</v>
       </c>
@@ -5445,7 +5447,7 @@
         <v>13627</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A70" s="5">
         <v>43963</v>
       </c>
@@ -5495,7 +5497,7 @@
         <v>13763</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A71" s="5">
         <v>43964</v>
       </c>
@@ -5545,7 +5547,7 @@
         <v>13929</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A72" s="5">
         <v>43965</v>
       </c>
@@ -5595,7 +5597,7 @@
         <v>14117</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A73" s="5">
         <v>43966</v>
       </c>
@@ -5645,7 +5647,7 @@
         <v>14260</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A74" s="5">
         <v>43967</v>
       </c>
@@ -5695,7 +5697,7 @@
         <v>14447</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A75" s="5">
         <v>43968</v>
       </c>
@@ -5745,7 +5747,7 @@
         <v>14537</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A76" s="5">
         <v>43969</v>
       </c>
@@ -5795,7 +5797,7 @@
         <v>14594</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A77" s="5">
         <v>43970</v>
       </c>
@@ -5845,7 +5847,7 @@
         <v>14655</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A78" s="5">
         <v>43971</v>
       </c>
@@ -5895,7 +5897,7 @@
         <v>14751</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A79" s="5">
         <v>43972</v>
       </c>
@@ -5945,7 +5947,7 @@
         <v>14856</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A80" s="5">
         <v>43973</v>
       </c>
@@ -5995,7 +5997,7 @@
         <v>14969</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A81" s="5">
         <v>43974</v>
       </c>
@@ -6045,7 +6047,7 @@
         <v>15041</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A82" s="5">
         <v>43975</v>
       </c>
@@ -6095,7 +6097,7 @@
         <v>15101</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A83" s="5">
         <v>43976</v>
       </c>
@@ -6145,7 +6147,7 @@
         <v>15156</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A84" s="5">
         <v>43977</v>
       </c>
@@ -6195,7 +6197,7 @@
         <v>15185</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A85" s="5">
         <v>43978</v>
       </c>
@@ -6245,7 +6247,7 @@
         <v>15240</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A86" s="5">
         <v>43979</v>
       </c>
@@ -6295,7 +6297,7 @@
         <v>15288</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A87" s="5">
         <v>43980</v>
       </c>
@@ -6345,7 +6347,7 @@
         <v>15327</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A88" s="5">
         <v>43981</v>
       </c>
@@ -6395,7 +6397,7 @@
         <v>15382</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A89" s="5">
         <v>43982</v>
       </c>
@@ -6445,7 +6447,7 @@
         <v>15400</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A90" s="5">
         <v>43983</v>
       </c>
@@ -6495,7 +6497,7 @@
         <v>15418</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A91" s="5">
         <v>43984</v>
       </c>
@@ -6545,7 +6547,7 @@
         <v>15471</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A92" s="5">
         <v>43985</v>
       </c>
@@ -6595,7 +6597,7 @@
         <v>15504</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A93" s="5">
         <v>43986</v>
       </c>
@@ -6645,7 +6647,7 @@
         <v>15553</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A94" s="5">
         <v>43987</v>
       </c>
@@ -6695,7 +6697,7 @@
         <v>15582</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A95" s="5">
         <v>43988</v>
       </c>
@@ -6745,7 +6747,7 @@
         <v>15603</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A96" s="5">
         <v>43989</v>
       </c>
@@ -6795,7 +6797,7 @@
         <v>15621</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A97" s="5">
         <v>43990</v>
       </c>
@@ -6845,7 +6847,7 @@
         <v>15639</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A98" s="5">
         <v>43991</v>
       </c>
@@ -6895,7 +6897,7 @@
         <v>15653</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A99" s="5">
         <v>43992</v>
       </c>
@@ -6945,7 +6947,7 @@
         <v>15665</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A100" s="5">
         <v>43993</v>
       </c>
@@ -6995,7 +6997,7 @@
         <v>15682</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A101" s="5">
         <v>43994</v>
       </c>
@@ -7045,7 +7047,7 @@
         <v>15709</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A102" s="5">
         <v>43995</v>
       </c>
@@ -7095,23 +7097,57 @@
         <v>15730</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C103" s="28"/>
-      <c r="D103" s="28"/>
-      <c r="E103" s="28"/>
-      <c r="F103" s="28"/>
-      <c r="G103" s="28"/>
-      <c r="H103" s="28"/>
-      <c r="I103" s="28"/>
-      <c r="J103" s="28"/>
-      <c r="K103" s="28"/>
-      <c r="L103" s="28"/>
-      <c r="M103" s="28"/>
-      <c r="N103" s="28"/>
-      <c r="O103" s="28"/>
-      <c r="P103" s="28"/>
-    </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A103" s="5">
+        <v>43996</v>
+      </c>
+      <c r="B103" s="28">
+        <v>1088</v>
+      </c>
+      <c r="C103" s="28">
+        <v>327</v>
+      </c>
+      <c r="D103" s="28">
+        <v>261</v>
+      </c>
+      <c r="E103" s="28">
+        <v>885</v>
+      </c>
+      <c r="F103" s="28">
+        <v>952</v>
+      </c>
+      <c r="G103" s="28">
+        <v>1294</v>
+      </c>
+      <c r="H103" s="28">
+        <v>4010</v>
+      </c>
+      <c r="I103" s="28">
+        <v>341</v>
+      </c>
+      <c r="J103" s="28">
+        <v>2035</v>
+      </c>
+      <c r="K103" s="28">
+        <v>2807</v>
+      </c>
+      <c r="L103" s="28">
+        <v>8</v>
+      </c>
+      <c r="M103" s="28">
+        <v>54</v>
+      </c>
+      <c r="N103" s="28">
+        <v>1687</v>
+      </c>
+      <c r="O103" s="28">
+        <v>6</v>
+      </c>
+      <c r="P103" s="32">
+        <v>15755</v>
+      </c>
+    </row>
+    <row r="104" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C104" s="28"/>
       <c r="D104" s="28"/>
       <c r="E104" s="28"/>
@@ -7127,7 +7163,7 @@
       <c r="O104" s="28"/>
       <c r="P104" s="28"/>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C105" s="28"/>
       <c r="D105" s="28"/>
       <c r="E105" s="28"/>
@@ -7143,7 +7179,7 @@
       <c r="O105" s="28"/>
       <c r="P105" s="28"/>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C106" s="28"/>
       <c r="D106" s="28"/>
       <c r="E106" s="28"/>
@@ -7159,7 +7195,7 @@
       <c r="O106" s="28"/>
       <c r="P106" s="28"/>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C107" s="28"/>
       <c r="D107" s="28"/>
       <c r="E107" s="28"/>
@@ -7175,7 +7211,7 @@
       <c r="O107" s="28"/>
       <c r="P107" s="28"/>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C108" s="28"/>
       <c r="D108" s="28"/>
       <c r="E108" s="28"/>
@@ -7191,7 +7227,7 @@
       <c r="O108" s="28"/>
       <c r="P108" s="28"/>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C109" s="28"/>
       <c r="D109" s="28"/>
       <c r="E109" s="28"/>
@@ -7207,7 +7243,7 @@
       <c r="O109" s="28"/>
       <c r="P109" s="28"/>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C110" s="28"/>
       <c r="D110" s="28"/>
       <c r="E110" s="28"/>
@@ -7223,7 +7259,7 @@
       <c r="O110" s="28"/>
       <c r="P110" s="28"/>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C111" s="28"/>
       <c r="D111" s="28"/>
       <c r="E111" s="28"/>
@@ -7239,7 +7275,7 @@
       <c r="O111" s="28"/>
       <c r="P111" s="28"/>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C112" s="28"/>
       <c r="D112" s="28"/>
       <c r="E112" s="28"/>
@@ -7255,7 +7291,7 @@
       <c r="O112" s="28"/>
       <c r="P112" s="28"/>
     </row>
-    <row r="113" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C113" s="28"/>
       <c r="D113" s="28"/>
       <c r="E113" s="28"/>
@@ -7271,7 +7307,7 @@
       <c r="O113" s="28"/>
       <c r="P113" s="28"/>
     </row>
-    <row r="114" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C114" s="28"/>
       <c r="D114" s="28"/>
       <c r="E114" s="28"/>
@@ -7287,7 +7323,7 @@
       <c r="O114" s="28"/>
       <c r="P114" s="28"/>
     </row>
-    <row r="115" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B115" s="28"/>
       <c r="C115" s="28"/>
       <c r="D115" s="28"/>
@@ -7304,7 +7340,7 @@
       <c r="O115" s="28"/>
       <c r="P115" s="28"/>
     </row>
-    <row r="116" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B116" s="28"/>
       <c r="C116" s="28"/>
       <c r="D116" s="28"/>
@@ -7321,7 +7357,7 @@
       <c r="O116" s="28"/>
       <c r="P116" s="28"/>
     </row>
-    <row r="117" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B117" s="28"/>
       <c r="C117" s="28"/>
       <c r="D117" s="28"/>
@@ -7338,7 +7374,7 @@
       <c r="O117" s="28"/>
       <c r="P117" s="28"/>
     </row>
-    <row r="118" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B118" s="28"/>
       <c r="C118" s="28"/>
       <c r="D118" s="28"/>
@@ -7355,7 +7391,7 @@
       <c r="O118" s="28"/>
       <c r="P118" s="28"/>
     </row>
-    <row r="119" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B119" s="28"/>
       <c r="C119" s="28"/>
       <c r="D119" s="28"/>
@@ -7372,7 +7408,7 @@
       <c r="O119" s="28"/>
       <c r="P119" s="28"/>
     </row>
-    <row r="120" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B120" s="28"/>
       <c r="C120" s="28"/>
       <c r="D120" s="28"/>
@@ -7389,7 +7425,7 @@
       <c r="O120" s="28"/>
       <c r="P120" s="28"/>
     </row>
-    <row r="121" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B121" s="28"/>
       <c r="C121" s="28"/>
       <c r="D121" s="28"/>
@@ -7406,7 +7442,7 @@
       <c r="O121" s="28"/>
       <c r="P121" s="28"/>
     </row>
-    <row r="122" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B122" s="28"/>
       <c r="C122" s="28"/>
       <c r="D122" s="28"/>
@@ -7423,7 +7459,7 @@
       <c r="O122" s="28"/>
       <c r="P122" s="28"/>
     </row>
-    <row r="123" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B123" s="28"/>
       <c r="C123" s="28"/>
       <c r="D123" s="28"/>
@@ -7440,7 +7476,7 @@
       <c r="O123" s="28"/>
       <c r="P123" s="28"/>
     </row>
-    <row r="124" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B124" s="28"/>
       <c r="C124" s="28"/>
       <c r="D124" s="28"/>
@@ -7457,7 +7493,7 @@
       <c r="O124" s="28"/>
       <c r="P124" s="28"/>
     </row>
-    <row r="125" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B125" s="28"/>
       <c r="C125" s="28"/>
       <c r="D125" s="28"/>
@@ -7474,7 +7510,7 @@
       <c r="O125" s="28"/>
       <c r="P125" s="28"/>
     </row>
-    <row r="126" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B126" s="28"/>
       <c r="C126" s="28"/>
       <c r="D126" s="28"/>
@@ -7491,7 +7527,7 @@
       <c r="O126" s="28"/>
       <c r="P126" s="28"/>
     </row>
-    <row r="127" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B127" s="28"/>
       <c r="C127" s="28"/>
       <c r="D127" s="28"/>
@@ -7508,7 +7544,7 @@
       <c r="O127" s="28"/>
       <c r="P127" s="28"/>
     </row>
-    <row r="128" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B128" s="28"/>
       <c r="C128" s="28"/>
       <c r="D128" s="28"/>
@@ -7525,7 +7561,7 @@
       <c r="O128" s="28"/>
       <c r="P128" s="28"/>
     </row>
-    <row r="129" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B129" s="28"/>
       <c r="C129" s="28"/>
       <c r="D129" s="28"/>
@@ -7542,7 +7578,7 @@
       <c r="O129" s="28"/>
       <c r="P129" s="28"/>
     </row>
-    <row r="130" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B130" s="28"/>
       <c r="C130" s="28"/>
       <c r="D130" s="28"/>
@@ -7559,7 +7595,7 @@
       <c r="O130" s="28"/>
       <c r="P130" s="28"/>
     </row>
-    <row r="131" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B131" s="28"/>
       <c r="C131" s="28"/>
       <c r="D131" s="28"/>
@@ -7576,7 +7612,7 @@
       <c r="O131" s="28"/>
       <c r="P131" s="28"/>
     </row>
-    <row r="132" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B132" s="28"/>
       <c r="C132" s="28"/>
       <c r="D132" s="28"/>
@@ -7593,7 +7629,7 @@
       <c r="O132" s="28"/>
       <c r="P132" s="28"/>
     </row>
-    <row r="133" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B133" s="28"/>
       <c r="C133" s="28"/>
       <c r="D133" s="28"/>
@@ -7610,7 +7646,7 @@
       <c r="O133" s="28"/>
       <c r="P133" s="28"/>
     </row>
-    <row r="134" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B134" s="28"/>
       <c r="C134" s="28"/>
       <c r="D134" s="28"/>
@@ -7627,7 +7663,7 @@
       <c r="O134" s="28"/>
       <c r="P134" s="28"/>
     </row>
-    <row r="135" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B135" s="28"/>
       <c r="C135" s="28"/>
       <c r="D135" s="28"/>
@@ -7644,7 +7680,7 @@
       <c r="O135" s="28"/>
       <c r="P135" s="28"/>
     </row>
-    <row r="136" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B136" s="28"/>
       <c r="C136" s="28"/>
       <c r="D136" s="28"/>
@@ -7661,7 +7697,7 @@
       <c r="O136" s="28"/>
       <c r="P136" s="28"/>
     </row>
-    <row r="137" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B137" s="28"/>
       <c r="C137" s="28"/>
       <c r="D137" s="28"/>
@@ -7678,7 +7714,7 @@
       <c r="O137" s="28"/>
       <c r="P137" s="28"/>
     </row>
-    <row r="138" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B138" s="28"/>
       <c r="C138" s="28"/>
       <c r="D138" s="28"/>
@@ -7695,7 +7731,7 @@
       <c r="O138" s="28"/>
       <c r="P138" s="28"/>
     </row>
-    <row r="139" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B139" s="28"/>
       <c r="C139" s="28"/>
       <c r="D139" s="28"/>
@@ -7712,7 +7748,7 @@
       <c r="O139" s="28"/>
       <c r="P139" s="28"/>
     </row>
-    <row r="140" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B140" s="28"/>
       <c r="C140" s="28"/>
       <c r="D140" s="28"/>
@@ -7729,7 +7765,7 @@
       <c r="O140" s="28"/>
       <c r="P140" s="28"/>
     </row>
-    <row r="141" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B141" s="28"/>
       <c r="C141" s="28"/>
       <c r="D141" s="28"/>
@@ -7746,7 +7782,7 @@
       <c r="O141" s="28"/>
       <c r="P141" s="28"/>
     </row>
-    <row r="142" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B142" s="28"/>
       <c r="C142" s="28"/>
       <c r="D142" s="28"/>
@@ -7763,7 +7799,7 @@
       <c r="O142" s="28"/>
       <c r="P142" s="28"/>
     </row>
-    <row r="143" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B143" s="28"/>
       <c r="C143" s="28"/>
       <c r="D143" s="28"/>
@@ -7780,7 +7816,7 @@
       <c r="O143" s="28"/>
       <c r="P143" s="28"/>
     </row>
-    <row r="144" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B144" s="28"/>
       <c r="C144" s="28"/>
       <c r="D144" s="28"/>
@@ -7797,7 +7833,7 @@
       <c r="O144" s="28"/>
       <c r="P144" s="28"/>
     </row>
-    <row r="145" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B145" s="28"/>
       <c r="C145" s="28"/>
       <c r="D145" s="28"/>
@@ -7814,7 +7850,7 @@
       <c r="O145" s="28"/>
       <c r="P145" s="28"/>
     </row>
-    <row r="146" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B146" s="28"/>
       <c r="C146" s="28"/>
       <c r="D146" s="28"/>
@@ -7831,7 +7867,7 @@
       <c r="O146" s="28"/>
       <c r="P146" s="28"/>
     </row>
-    <row r="147" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B147" s="28"/>
       <c r="C147" s="28"/>
       <c r="D147" s="28"/>
@@ -7848,7 +7884,7 @@
       <c r="O147" s="28"/>
       <c r="P147" s="28"/>
     </row>
-    <row r="148" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B148" s="28"/>
       <c r="C148" s="28"/>
       <c r="D148" s="28"/>
@@ -7865,7 +7901,7 @@
       <c r="O148" s="28"/>
       <c r="P148" s="28"/>
     </row>
-    <row r="149" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B149" s="28"/>
       <c r="C149" s="28"/>
       <c r="D149" s="28"/>
@@ -7882,7 +7918,7 @@
       <c r="O149" s="28"/>
       <c r="P149" s="28"/>
     </row>
-    <row r="150" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B150" s="28"/>
       <c r="C150" s="28"/>
       <c r="D150" s="28"/>
@@ -7899,7 +7935,7 @@
       <c r="O150" s="28"/>
       <c r="P150" s="28"/>
     </row>
-    <row r="151" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B151" s="28"/>
       <c r="C151" s="28"/>
       <c r="D151" s="28"/>
@@ -7916,7 +7952,7 @@
       <c r="O151" s="28"/>
       <c r="P151" s="28"/>
     </row>
-    <row r="152" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B152" s="28"/>
       <c r="C152" s="28"/>
       <c r="D152" s="28"/>
@@ -7933,7 +7969,7 @@
       <c r="O152" s="28"/>
       <c r="P152" s="28"/>
     </row>
-    <row r="153" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B153" s="28"/>
       <c r="C153" s="28"/>
       <c r="D153" s="28"/>
@@ -7950,7 +7986,7 @@
       <c r="O153" s="28"/>
       <c r="P153" s="28"/>
     </row>
-    <row r="154" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B154" s="28"/>
       <c r="C154" s="28"/>
       <c r="D154" s="28"/>
@@ -7967,7 +8003,7 @@
       <c r="O154" s="28"/>
       <c r="P154" s="28"/>
     </row>
-    <row r="155" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B155" s="28"/>
       <c r="C155" s="28"/>
       <c r="D155" s="28"/>
@@ -7984,7 +8020,7 @@
       <c r="O155" s="28"/>
       <c r="P155" s="28"/>
     </row>
-    <row r="156" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B156" s="28"/>
       <c r="C156" s="28"/>
       <c r="D156" s="28"/>
@@ -8001,7 +8037,7 @@
       <c r="O156" s="28"/>
       <c r="P156" s="28"/>
     </row>
-    <row r="157" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B157" s="28"/>
       <c r="C157" s="28"/>
       <c r="D157" s="28"/>
@@ -8018,7 +8054,7 @@
       <c r="O157" s="28"/>
       <c r="P157" s="28"/>
     </row>
-    <row r="158" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B158" s="28"/>
       <c r="C158" s="28"/>
       <c r="D158" s="28"/>
@@ -8035,7 +8071,7 @@
       <c r="O158" s="28"/>
       <c r="P158" s="28"/>
     </row>
-    <row r="159" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B159" s="28"/>
       <c r="C159" s="28"/>
       <c r="D159" s="28"/>
@@ -8052,7 +8088,7 @@
       <c r="O159" s="28"/>
       <c r="P159" s="28"/>
     </row>
-    <row r="160" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B160" s="28"/>
       <c r="C160" s="28"/>
       <c r="D160" s="28"/>
@@ -8077,21 +8113,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q91"/>
+  <dimension ref="A1:Q92"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L91" sqref="L91"/>
+      <pane ySplit="3" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5703125" style="2"/>
+    <col min="1" max="1" width="12.44140625" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.5546875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -8112,7 +8148,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -8133,7 +8169,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -8186,7 +8222,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>43908</v>
       </c>
@@ -8239,7 +8275,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>43909</v>
       </c>
@@ -8292,7 +8328,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>43910</v>
       </c>
@@ -8345,7 +8381,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>43911</v>
       </c>
@@ -8398,7 +8434,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>43912</v>
       </c>
@@ -8451,7 +8487,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>43913</v>
       </c>
@@ -8504,7 +8540,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>43914</v>
       </c>
@@ -8557,7 +8593,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>43915</v>
       </c>
@@ -8610,7 +8646,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
         <v>43916</v>
       </c>
@@ -8663,7 +8699,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>43917</v>
       </c>
@@ -8716,7 +8752,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>43918</v>
       </c>
@@ -8769,7 +8805,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>43919</v>
       </c>
@@ -8822,7 +8858,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>43920</v>
       </c>
@@ -8875,7 +8911,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>43921</v>
       </c>
@@ -8928,7 +8964,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>43922</v>
       </c>
@@ -8981,7 +9017,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>43923</v>
       </c>
@@ -9034,7 +9070,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>43924</v>
       </c>
@@ -9087,7 +9123,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>43925</v>
       </c>
@@ -9140,7 +9176,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="12">
         <v>43926</v>
       </c>
@@ -9193,7 +9229,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="12">
         <v>43927</v>
       </c>
@@ -9246,7 +9282,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="12">
         <v>43928</v>
       </c>
@@ -9299,7 +9335,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="12">
         <v>43929</v>
       </c>
@@ -9352,7 +9388,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="12">
         <v>43930</v>
       </c>
@@ -9405,7 +9441,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="12">
         <v>43931</v>
       </c>
@@ -9458,7 +9494,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="12">
         <v>43932</v>
       </c>
@@ -9511,7 +9547,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="12">
         <v>43933</v>
       </c>
@@ -9564,7 +9600,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <v>43934</v>
       </c>
@@ -9617,7 +9653,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="12">
         <v>43935</v>
       </c>
@@ -9670,7 +9706,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="12">
         <v>43936</v>
       </c>
@@ -9723,7 +9759,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="12">
         <v>43937</v>
       </c>
@@ -9776,7 +9812,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="12">
         <v>43938</v>
       </c>
@@ -9829,7 +9865,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="12">
         <v>43939</v>
       </c>
@@ -9882,7 +9918,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="30">
         <v>43940</v>
       </c>
@@ -9935,7 +9971,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="30">
         <v>43941</v>
       </c>
@@ -9988,7 +10024,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="30">
         <v>43942</v>
       </c>
@@ -10041,7 +10077,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="30">
         <v>43943</v>
       </c>
@@ -10094,7 +10130,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="30">
         <v>43944</v>
       </c>
@@ -10147,7 +10183,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="30">
         <v>43945</v>
       </c>
@@ -10200,7 +10236,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="30">
         <v>43946</v>
       </c>
@@ -10253,7 +10289,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="30">
         <v>43947</v>
       </c>
@@ -10306,7 +10342,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="30">
         <v>43948</v>
       </c>
@@ -10359,7 +10395,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="30">
         <v>43949</v>
       </c>
@@ -10412,7 +10448,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="30">
         <v>43950</v>
       </c>
@@ -10465,7 +10501,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="30">
         <v>43951</v>
       </c>
@@ -10518,7 +10554,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" s="30">
         <v>43952</v>
       </c>
@@ -10571,7 +10607,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="30">
         <v>43953</v>
       </c>
@@ -10624,7 +10660,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" s="30">
         <v>43954</v>
       </c>
@@ -10677,7 +10713,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="30">
         <v>43955</v>
       </c>
@@ -10730,7 +10766,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" s="30">
         <v>43956</v>
       </c>
@@ -10783,7 +10819,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" s="30">
         <v>43957</v>
       </c>
@@ -10836,7 +10872,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" s="30">
         <v>43958</v>
       </c>
@@ -10889,7 +10925,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" s="30">
         <v>43959</v>
       </c>
@@ -10942,7 +10978,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" s="30">
         <v>43960</v>
       </c>
@@ -10995,7 +11031,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" s="30">
         <v>43961</v>
       </c>
@@ -11048,7 +11084,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" s="30">
         <v>43962</v>
       </c>
@@ -11101,7 +11137,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" s="30">
         <v>43963</v>
       </c>
@@ -11154,7 +11190,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" s="30">
         <v>43964</v>
       </c>
@@ -11207,7 +11243,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" s="30">
         <v>43965</v>
       </c>
@@ -11260,7 +11296,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" s="30">
         <v>43966</v>
       </c>
@@ -11313,7 +11349,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" s="30">
         <v>43967</v>
       </c>
@@ -11366,7 +11402,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" s="30">
         <v>43968</v>
       </c>
@@ -11419,7 +11455,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" s="30">
         <v>43969</v>
       </c>
@@ -11472,7 +11508,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" s="30">
         <v>43970</v>
       </c>
@@ -11525,7 +11561,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" s="30">
         <v>43971</v>
       </c>
@@ -11578,7 +11614,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" s="30">
         <v>43972</v>
       </c>
@@ -11631,7 +11667,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" s="30">
         <v>43973</v>
       </c>
@@ -11684,7 +11720,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" s="30">
         <v>43974</v>
       </c>
@@ -11737,7 +11773,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" s="30">
         <v>43975</v>
       </c>
@@ -11790,7 +11826,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" s="30">
         <v>43976</v>
       </c>
@@ -11843,7 +11879,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" s="30">
         <v>43977</v>
       </c>
@@ -11896,7 +11932,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" s="30">
         <v>43978</v>
       </c>
@@ -11949,7 +11985,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75" s="30">
         <v>43979</v>
       </c>
@@ -12002,7 +12038,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76" s="30">
         <v>43980</v>
       </c>
@@ -12055,7 +12091,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77" s="30">
         <v>43981</v>
       </c>
@@ -12108,7 +12144,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78" s="30">
         <v>43982</v>
       </c>
@@ -12161,7 +12197,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79" s="30">
         <v>43983</v>
       </c>
@@ -12214,7 +12250,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A80" s="30">
         <v>43984</v>
       </c>
@@ -12267,7 +12303,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A81" s="30">
         <v>43985</v>
       </c>
@@ -12320,7 +12356,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A82" s="30">
         <v>43986</v>
       </c>
@@ -12373,7 +12409,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A83" s="30">
         <v>43987</v>
       </c>
@@ -12426,7 +12462,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A84" s="30">
         <v>43988</v>
       </c>
@@ -12479,7 +12515,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A85" s="30">
         <v>43989</v>
       </c>
@@ -12532,7 +12568,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A86" s="30">
         <v>43990</v>
       </c>
@@ -12585,7 +12621,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A87" s="30">
         <v>43991</v>
       </c>
@@ -12638,7 +12674,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A88" s="30">
         <v>43992</v>
       </c>
@@ -12691,7 +12727,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A89" s="30">
         <v>43993</v>
       </c>
@@ -12744,7 +12780,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A90" s="30">
         <v>43994</v>
       </c>
@@ -12797,7 +12833,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A91" s="30">
         <v>43995</v>
       </c>
@@ -12848,6 +12884,59 @@
       </c>
       <c r="Q91" s="13">
         <v>20</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A92" s="30">
+        <v>43996</v>
+      </c>
+      <c r="B92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K92" s="11">
+        <v>5</v>
+      </c>
+      <c r="L92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P92" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q92" s="13">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -12858,23 +12947,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R83"/>
+  <dimension ref="A1:R84"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B64" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="S83" sqref="S83"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5703125" style="2"/>
+    <col min="1" max="1" width="15.44140625" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.5546875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -12895,7 +12984,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -12916,7 +13005,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -12969,7 +13058,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>43916</v>
       </c>
@@ -13022,7 +13111,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>43917</v>
       </c>
@@ -13075,7 +13164,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>43918</v>
       </c>
@@ -13128,7 +13217,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>43919</v>
       </c>
@@ -13181,7 +13270,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>43920</v>
       </c>
@@ -13234,7 +13323,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>43921</v>
       </c>
@@ -13287,7 +13376,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>43922</v>
       </c>
@@ -13340,7 +13429,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>43923</v>
       </c>
@@ -13393,7 +13482,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
         <v>43924</v>
       </c>
@@ -13446,7 +13535,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>43925</v>
       </c>
@@ -13499,7 +13588,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>43926</v>
       </c>
@@ -13552,7 +13641,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>43927</v>
       </c>
@@ -13605,7 +13694,7 @@
         <v>1262</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>43928</v>
       </c>
@@ -13658,7 +13747,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>43929</v>
       </c>
@@ -13711,7 +13800,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>43930</v>
       </c>
@@ -13764,7 +13853,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>43931</v>
       </c>
@@ -13817,7 +13906,7 @@
         <v>1461</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>43932</v>
       </c>
@@ -13870,7 +13959,7 @@
         <v>1467</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>43933</v>
       </c>
@@ -13923,7 +14012,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="12">
         <v>43934</v>
       </c>
@@ -13976,7 +14065,7 @@
         <v>1482</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="12">
         <v>43935</v>
       </c>
@@ -14029,7 +14118,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="12">
         <v>43936</v>
       </c>
@@ -14082,7 +14171,7 @@
         <v>1486</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="12">
         <v>43937</v>
       </c>
@@ -14135,7 +14224,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="12">
         <v>43938</v>
       </c>
@@ -14188,7 +14277,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="12">
         <v>43939</v>
       </c>
@@ -14241,7 +14330,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="12">
         <v>43940</v>
       </c>
@@ -14294,7 +14383,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="12">
         <v>43941</v>
       </c>
@@ -14347,7 +14436,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <v>43942</v>
       </c>
@@ -14400,7 +14489,7 @@
         <v>1472</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="12">
         <v>43943</v>
       </c>
@@ -14453,7 +14542,7 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="12">
         <v>43944</v>
       </c>
@@ -14506,7 +14595,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="12">
         <v>43945</v>
       </c>
@@ -14559,7 +14648,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="12">
         <v>43946</v>
       </c>
@@ -14612,7 +14701,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="12">
         <v>43947</v>
       </c>
@@ -14665,7 +14754,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="30">
         <v>43948</v>
       </c>
@@ -14718,7 +14807,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="30">
         <v>43949</v>
       </c>
@@ -14771,7 +14860,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="30">
         <v>43950</v>
       </c>
@@ -14824,7 +14913,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="30">
         <v>43951</v>
       </c>
@@ -14877,7 +14966,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="30">
         <v>43952</v>
       </c>
@@ -14930,7 +15019,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="30">
         <v>43953</v>
       </c>
@@ -14983,7 +15072,7 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="30">
         <v>43954</v>
       </c>
@@ -15036,7 +15125,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="30">
         <v>43955</v>
       </c>
@@ -15089,7 +15178,7 @@
         <v>1279</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="30">
         <v>43956</v>
       </c>
@@ -15142,7 +15231,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="30">
         <v>43957</v>
       </c>
@@ -15195,7 +15284,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="30">
         <v>43958</v>
       </c>
@@ -15248,7 +15337,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="30">
         <v>43959</v>
       </c>
@@ -15301,7 +15390,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" s="30">
         <v>43960</v>
       </c>
@@ -15354,7 +15443,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="30">
         <v>43961</v>
       </c>
@@ -15407,7 +15496,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" s="30">
         <v>43962</v>
       </c>
@@ -15460,7 +15549,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="30">
         <v>43963</v>
       </c>
@@ -15513,7 +15602,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" s="30">
         <v>43964</v>
       </c>
@@ -15566,7 +15655,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" s="30">
         <v>43965</v>
       </c>
@@ -15619,7 +15708,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" s="30">
         <v>43966</v>
       </c>
@@ -15672,7 +15761,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" s="30">
         <v>43967</v>
       </c>
@@ -15725,7 +15814,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" s="30">
         <v>43968</v>
       </c>
@@ -15778,7 +15867,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" s="30">
         <v>43969</v>
       </c>
@@ -15831,7 +15920,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" s="30">
         <v>43970</v>
       </c>
@@ -15884,7 +15973,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" s="30">
         <v>43971</v>
       </c>
@@ -15937,7 +16026,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" s="30">
         <v>43972</v>
       </c>
@@ -15990,7 +16079,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" s="30">
         <v>43973</v>
       </c>
@@ -16043,7 +16132,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" s="30">
         <v>43974</v>
       </c>
@@ -16096,7 +16185,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" s="30">
         <v>43975</v>
       </c>
@@ -16149,7 +16238,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" s="30">
         <v>43976</v>
       </c>
@@ -16202,7 +16291,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A65" s="51">
         <v>43977</v>
       </c>
@@ -16255,7 +16344,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A66" s="51">
         <v>43978</v>
       </c>
@@ -16308,7 +16397,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A67" s="51">
         <v>43979</v>
       </c>
@@ -16361,7 +16450,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A68" s="51">
         <v>43980</v>
       </c>
@@ -16414,7 +16503,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A69" s="51">
         <v>43981</v>
       </c>
@@ -16467,7 +16556,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A70" s="51">
         <v>43982</v>
       </c>
@@ -16520,7 +16609,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A71" s="51">
         <v>43983</v>
       </c>
@@ -16573,7 +16662,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A72" s="51">
         <v>43984</v>
       </c>
@@ -16626,7 +16715,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A73" s="51">
         <v>43985</v>
       </c>
@@ -16679,7 +16768,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A74" s="51">
         <v>43986</v>
       </c>
@@ -16732,7 +16821,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A75" s="51">
         <v>43987</v>
       </c>
@@ -16785,7 +16874,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A76" s="51">
         <v>43988</v>
       </c>
@@ -16838,7 +16927,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A77" s="51">
         <v>43989</v>
       </c>
@@ -16891,7 +16980,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A78" s="51">
         <v>43990</v>
       </c>
@@ -16944,7 +17033,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A79" s="51">
         <v>43991</v>
       </c>
@@ -16997,7 +17086,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A80" s="51">
         <v>43992</v>
       </c>
@@ -17051,7 +17140,7 @@
       </c>
       <c r="R80" s="54"/>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A81" s="51">
         <v>43993</v>
       </c>
@@ -17105,7 +17194,7 @@
       </c>
       <c r="R81" s="54"/>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A82" s="51">
         <v>43994</v>
       </c>
@@ -17159,7 +17248,7 @@
       </c>
       <c r="R82" s="54"/>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A83" s="51">
         <v>43995</v>
       </c>
@@ -17210,6 +17299,59 @@
       </c>
       <c r="Q83" s="13">
         <v>582</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A84" s="51">
+        <v>43996</v>
+      </c>
+      <c r="B84" s="11">
+        <v>5</v>
+      </c>
+      <c r="C84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E84" s="11">
+        <v>57</v>
+      </c>
+      <c r="F84" s="11">
+        <v>5</v>
+      </c>
+      <c r="G84" s="11">
+        <v>56</v>
+      </c>
+      <c r="H84" s="11">
+        <v>255</v>
+      </c>
+      <c r="I84" s="11">
+        <v>7</v>
+      </c>
+      <c r="J84" s="11">
+        <v>49</v>
+      </c>
+      <c r="K84" s="11">
+        <v>134</v>
+      </c>
+      <c r="L84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N84" s="11">
+        <v>6</v>
+      </c>
+      <c r="O84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q84" s="13">
+        <v>575</v>
       </c>
     </row>
   </sheetData>
@@ -17220,23 +17362,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q83"/>
+  <dimension ref="A1:Q84"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A84" sqref="A84"/>
+      <selection pane="bottomRight" activeCell="O87" sqref="O87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5703125" style="2"/>
+    <col min="1" max="1" width="12.44140625" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.5546875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -17257,7 +17399,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -17278,7 +17420,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -17331,7 +17473,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>43916</v>
       </c>
@@ -17384,7 +17526,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>43917</v>
       </c>
@@ -17437,7 +17579,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>43918</v>
       </c>
@@ -17490,7 +17632,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>43919</v>
       </c>
@@ -17543,7 +17685,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>43920</v>
       </c>
@@ -17596,7 +17738,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>43921</v>
       </c>
@@ -17649,7 +17791,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>43922</v>
       </c>
@@ -17702,7 +17844,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>43923</v>
       </c>
@@ -17755,7 +17897,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
         <v>43924</v>
       </c>
@@ -17808,7 +17950,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>43925</v>
       </c>
@@ -17861,7 +18003,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>43926</v>
       </c>
@@ -17914,7 +18056,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>43927</v>
       </c>
@@ -17967,7 +18109,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>43928</v>
       </c>
@@ -18020,7 +18162,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>43929</v>
       </c>
@@ -18073,7 +18215,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>43930</v>
       </c>
@@ -18126,7 +18268,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>43931</v>
       </c>
@@ -18179,7 +18321,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>43932</v>
       </c>
@@ -18232,7 +18374,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>43933</v>
       </c>
@@ -18285,7 +18427,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="12">
         <v>43934</v>
       </c>
@@ -18338,7 +18480,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="12">
         <v>43935</v>
       </c>
@@ -18391,7 +18533,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="12">
         <v>43936</v>
       </c>
@@ -18444,7 +18586,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="12">
         <v>43937</v>
       </c>
@@ -18497,7 +18639,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="12">
         <v>43938</v>
       </c>
@@ -18550,7 +18692,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="12">
         <v>43939</v>
       </c>
@@ -18603,7 +18745,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="12">
         <v>43940</v>
       </c>
@@ -18656,7 +18798,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="12">
         <v>43941</v>
       </c>
@@ -18709,7 +18851,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <v>43942</v>
       </c>
@@ -18762,7 +18904,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="12">
         <v>43943</v>
       </c>
@@ -18815,7 +18957,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="12">
         <v>43944</v>
       </c>
@@ -18868,7 +19010,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="12">
         <v>43945</v>
       </c>
@@ -18921,7 +19063,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="12">
         <v>43946</v>
       </c>
@@ -18974,7 +19116,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="12">
         <v>43947</v>
       </c>
@@ -19027,7 +19169,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="30">
         <v>43948</v>
       </c>
@@ -19080,7 +19222,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="30">
         <v>43949</v>
       </c>
@@ -19133,7 +19275,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="30">
         <v>43950</v>
       </c>
@@ -19186,7 +19328,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="30">
         <v>43951</v>
       </c>
@@ -19239,7 +19381,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="30">
         <v>43952</v>
       </c>
@@ -19292,7 +19434,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="30">
         <v>43953</v>
       </c>
@@ -19345,7 +19487,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="30">
         <v>43954</v>
       </c>
@@ -19398,7 +19540,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="30">
         <v>43955</v>
       </c>
@@ -19451,7 +19593,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="30">
         <v>43956</v>
       </c>
@@ -19504,7 +19646,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="30">
         <v>43957</v>
       </c>
@@ -19557,7 +19699,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="30">
         <v>43958</v>
       </c>
@@ -19610,7 +19752,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="30">
         <v>43959</v>
       </c>
@@ -19663,7 +19805,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" s="30">
         <v>43960</v>
       </c>
@@ -19716,7 +19858,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="30">
         <v>43961</v>
       </c>
@@ -19769,7 +19911,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" s="30">
         <v>43962</v>
       </c>
@@ -19822,7 +19964,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="30">
         <v>43963</v>
       </c>
@@ -19875,7 +20017,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" s="30">
         <v>43964</v>
       </c>
@@ -19928,7 +20070,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" s="30">
         <v>43965</v>
       </c>
@@ -19981,7 +20123,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" s="30">
         <v>43966</v>
       </c>
@@ -20034,7 +20176,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" s="30">
         <v>43967</v>
       </c>
@@ -20087,7 +20229,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" s="30">
         <v>43968</v>
       </c>
@@ -20140,7 +20282,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" s="30">
         <v>43969</v>
       </c>
@@ -20193,7 +20335,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" s="30">
         <v>43970</v>
       </c>
@@ -20246,7 +20388,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" s="30">
         <v>43971</v>
       </c>
@@ -20299,7 +20441,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" s="30">
         <v>43972</v>
       </c>
@@ -20352,7 +20494,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" s="30">
         <v>43973</v>
       </c>
@@ -20405,7 +20547,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" s="30">
         <v>43974</v>
       </c>
@@ -20458,7 +20600,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" s="30">
         <v>43975</v>
       </c>
@@ -20511,7 +20653,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" s="30">
         <v>43976</v>
       </c>
@@ -20564,7 +20706,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" s="30">
         <v>43977</v>
       </c>
@@ -20617,7 +20759,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" s="30">
         <v>43978</v>
       </c>
@@ -20670,7 +20812,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" s="30">
         <v>43979</v>
       </c>
@@ -20723,7 +20865,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" s="30">
         <v>43980</v>
       </c>
@@ -20776,7 +20918,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" s="30">
         <v>43981</v>
       </c>
@@ -20829,7 +20971,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" s="30">
         <v>43982</v>
       </c>
@@ -20882,7 +21024,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" s="30">
         <v>43983</v>
       </c>
@@ -20935,7 +21077,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" s="30">
         <v>43984</v>
       </c>
@@ -20988,7 +21130,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" s="30">
         <v>43985</v>
       </c>
@@ -21041,7 +21183,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" s="30">
         <v>43986</v>
       </c>
@@ -21094,7 +21236,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75" s="30">
         <v>43987</v>
       </c>
@@ -21147,7 +21289,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76" s="30">
         <v>43988</v>
       </c>
@@ -21200,7 +21342,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77" s="30">
         <v>43989</v>
       </c>
@@ -21253,7 +21395,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78" s="30">
         <v>43990</v>
       </c>
@@ -21306,7 +21448,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79" s="30">
         <v>43991</v>
       </c>
@@ -21359,7 +21501,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A80" s="30">
         <v>43992</v>
       </c>
@@ -21412,7 +21554,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A81" s="30">
         <v>43993</v>
       </c>
@@ -21465,7 +21607,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A82" s="30">
         <v>43994</v>
       </c>
@@ -21518,7 +21660,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A83" s="30">
         <v>43995</v>
       </c>
@@ -21569,6 +21711,59 @@
       </c>
       <c r="Q83" s="13">
         <v>401</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A84" s="30">
+        <v>43996</v>
+      </c>
+      <c r="B84" s="11">
+        <v>25</v>
+      </c>
+      <c r="C84" s="11">
+        <v>9</v>
+      </c>
+      <c r="D84" s="11">
+        <v>11</v>
+      </c>
+      <c r="E84" s="11">
+        <v>25</v>
+      </c>
+      <c r="F84" s="11">
+        <v>32</v>
+      </c>
+      <c r="G84" s="11">
+        <v>14</v>
+      </c>
+      <c r="H84" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I84" s="11">
+        <v>25</v>
+      </c>
+      <c r="J84" s="11">
+        <v>64</v>
+      </c>
+      <c r="K84" s="11">
+        <v>172</v>
+      </c>
+      <c r="L84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N84" s="11">
+        <v>12</v>
+      </c>
+      <c r="O84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q84" s="13">
+        <v>389</v>
       </c>
     </row>
   </sheetData>
@@ -21595,13 +21790,13 @@
       <value order="0">false</value>
     </field>
     <field name="Objective-IsPublished">
-      <value order="0">true</value>
+      <value order="0">false</value>
     </field>
     <field name="Objective-DatePublished">
-      <value order="0">2020-06-13T11:44:27Z</value>
+      <value order="0"/>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-13T11:44:27Z</value>
+      <value order="0">2020-06-14T11:47:42Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -21613,16 +21808,16 @@
       <value order="0">Analytical: COVID 19 Analysis: Restricted working papers: Research and analysis: Diseases: 2020-2025</value>
     </field>
     <field name="Objective-State">
-      <value order="0">Published</value>
+      <value order="0">Being Drafted</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41730562</value>
+      <value order="0">vA41732238</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">25.0</value>
+      <value order="0">25.3</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">175</value>
+      <value order="0">178</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-14 20:08) (#124)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u207826\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA4095\A28088333\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U445783\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA18464\A28088333\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5985" windowHeight="6045" tabRatio="803"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5988" windowHeight="6048" tabRatio="803" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1833" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1858" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -1927,23 +1927,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="90.42578125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.42578125" style="2"/>
+    <col min="2" max="2" width="29.44140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="90.44140625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" s="18" t="s">
         <v>20</v>
       </c>
@@ -1951,7 +1953,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20" t="s">
         <v>22</v>
       </c>
@@ -1959,13 +1961,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="22" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="23"/>
     </row>
-    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="24" t="s">
         <v>26</v>
       </c>
@@ -1973,7 +1975,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="24" t="s">
         <v>27</v>
       </c>
@@ -1981,7 +1983,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="24" t="s">
         <v>36</v>
       </c>
@@ -1989,7 +1991,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="20" t="s">
         <v>37</v>
       </c>
@@ -2017,12 +2019,12 @@
       <selection activeCell="O52" sqref="O52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.42578125" style="2"/>
+    <col min="1" max="16384" width="9.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" ht="15" x14ac:dyDescent="0.3">
       <c r="A44" s="43"/>
     </row>
   </sheetData>
@@ -2036,21 +2038,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S160"/>
   <sheetViews>
-    <sheetView zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B91" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B85" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L105" sqref="L105"/>
+      <selection pane="bottomRight" activeCell="H93" sqref="H93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" style="2" customWidth="1"/>
-    <col min="2" max="16" width="11.42578125" style="11" customWidth="1"/>
-    <col min="17" max="16384" width="8.5703125" style="2"/>
+    <col min="2" max="16" width="11.44140625" style="11" customWidth="1"/>
+    <col min="17" max="16384" width="8.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -2070,7 +2072,7 @@
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -2089,7 +2091,7 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -2139,7 +2141,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>43897</v>
       </c>
@@ -2189,7 +2191,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>43898</v>
       </c>
@@ -2239,7 +2241,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>43899</v>
       </c>
@@ -2289,7 +2291,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>43900</v>
       </c>
@@ -2339,7 +2341,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>43901</v>
       </c>
@@ -2389,7 +2391,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>43902</v>
       </c>
@@ -2439,7 +2441,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>43903</v>
       </c>
@@ -2489,7 +2491,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>43904</v>
       </c>
@@ -2539,7 +2541,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>43905</v>
       </c>
@@ -2589,7 +2591,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>43906</v>
       </c>
@@ -2639,7 +2641,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>43907</v>
       </c>
@@ -2689,7 +2691,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>43908</v>
       </c>
@@ -2739,7 +2741,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>43909</v>
       </c>
@@ -2789,7 +2791,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>43910</v>
       </c>
@@ -2839,7 +2841,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>43911</v>
       </c>
@@ -2889,7 +2891,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>43912</v>
       </c>
@@ -2939,7 +2941,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>43913</v>
       </c>
@@ -2989,7 +2991,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>43914</v>
       </c>
@@ -3039,7 +3041,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>43915</v>
       </c>
@@ -3089,7 +3091,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>43916</v>
       </c>
@@ -3139,7 +3141,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>43917</v>
       </c>
@@ -3189,7 +3191,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>43918</v>
       </c>
@@ -3239,7 +3241,7 @@
         <v>1264</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>43919</v>
       </c>
@@ -3289,7 +3291,7 @@
         <v>1417</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>43920</v>
       </c>
@@ -3339,7 +3341,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>43921</v>
       </c>
@@ -3389,7 +3391,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>43922</v>
       </c>
@@ -3439,7 +3441,7 @@
         <v>2310</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>43923</v>
       </c>
@@ -3489,7 +3491,7 @@
         <v>2602</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <v>43924</v>
       </c>
@@ -3539,7 +3541,7 @@
         <v>3001</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>43925</v>
       </c>
@@ -3589,7 +3591,7 @@
         <v>3345</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
         <v>43926</v>
       </c>
@@ -3639,7 +3641,7 @@
         <v>3706</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
         <v>43927</v>
       </c>
@@ -3689,7 +3691,7 @@
         <v>3961</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
         <v>43928</v>
       </c>
@@ -3739,7 +3741,7 @@
         <v>4229</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>43929</v>
       </c>
@@ -3789,7 +3791,7 @@
         <v>4565</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
         <v>43930</v>
       </c>
@@ -3839,7 +3841,7 @@
         <v>4957</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
         <v>43931</v>
       </c>
@@ -3889,7 +3891,7 @@
         <v>5275</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>43932</v>
       </c>
@@ -3939,7 +3941,7 @@
         <v>5590</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
         <v>43933</v>
       </c>
@@ -3989,7 +3991,7 @@
         <v>5912</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
         <v>43934</v>
       </c>
@@ -4039,7 +4041,7 @@
         <v>6067</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>43935</v>
       </c>
@@ -4089,7 +4091,7 @@
         <v>6358</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
         <v>43936</v>
       </c>
@@ -4139,7 +4141,7 @@
         <v>6748</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" s="5">
         <v>43937</v>
       </c>
@@ -4189,7 +4191,7 @@
         <v>7102</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
         <v>43938</v>
       </c>
@@ -4239,7 +4241,7 @@
         <v>7409</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" s="5">
         <v>43939</v>
       </c>
@@ -4289,7 +4291,7 @@
         <v>7820</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" s="5">
         <v>43940</v>
       </c>
@@ -4339,7 +4341,7 @@
         <v>8187</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
         <v>43941</v>
       </c>
@@ -4389,7 +4391,7 @@
         <v>8450</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A49" s="5">
         <v>43942</v>
       </c>
@@ -4439,7 +4441,7 @@
         <v>8672</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
         <v>43943</v>
       </c>
@@ -4489,7 +4491,7 @@
         <v>9038</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A51" s="5">
         <v>43944</v>
       </c>
@@ -4539,7 +4541,7 @@
         <v>9409</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A52" s="5">
         <v>43945</v>
       </c>
@@ -4589,7 +4591,7 @@
         <v>9697</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A53" s="5">
         <v>43946</v>
       </c>
@@ -4639,7 +4641,7 @@
         <v>10051</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A54" s="5">
         <v>43947</v>
       </c>
@@ -4690,7 +4692,7 @@
       </c>
       <c r="R54" s="38"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A55" s="5">
         <v>43948</v>
       </c>
@@ -4741,7 +4743,7 @@
       </c>
       <c r="R55" s="38"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A56" s="5">
         <v>43949</v>
       </c>
@@ -4792,7 +4794,7 @@
       </c>
       <c r="R56" s="39"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A57" s="5">
         <v>43950</v>
       </c>
@@ -4842,7 +4844,7 @@
         <v>11034</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A58" s="5">
         <v>43951</v>
       </c>
@@ -4893,7 +4895,7 @@
       </c>
       <c r="R58" s="38"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A59" s="5">
         <v>43952</v>
       </c>
@@ -4945,7 +4947,7 @@
       <c r="R59" s="38"/>
       <c r="S59" s="38"/>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A60" s="5">
         <v>43953</v>
       </c>
@@ -4995,7 +4997,7 @@
         <v>11927</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A61" s="5">
         <v>43954</v>
       </c>
@@ -5045,7 +5047,7 @@
         <v>12097</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A62" s="5">
         <v>43955</v>
       </c>
@@ -5095,7 +5097,7 @@
         <v>12266</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A63" s="5">
         <v>43956</v>
       </c>
@@ -5145,7 +5147,7 @@
         <v>12437</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A64" s="5">
         <v>43957</v>
       </c>
@@ -5195,7 +5197,7 @@
         <v>12709</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65" s="5">
         <v>43958</v>
       </c>
@@ -5245,7 +5247,7 @@
         <v>12924</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66" s="5">
         <v>43959</v>
       </c>
@@ -5295,7 +5297,7 @@
         <v>13149</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A67" s="5">
         <v>43960</v>
       </c>
@@ -5345,7 +5347,7 @@
         <v>13305</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A68" s="5">
         <v>43961</v>
       </c>
@@ -5395,7 +5397,7 @@
         <v>13486</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A69" s="5">
         <v>43962</v>
       </c>
@@ -5445,7 +5447,7 @@
         <v>13627</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A70" s="5">
         <v>43963</v>
       </c>
@@ -5495,7 +5497,7 @@
         <v>13763</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A71" s="5">
         <v>43964</v>
       </c>
@@ -5545,7 +5547,7 @@
         <v>13929</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A72" s="5">
         <v>43965</v>
       </c>
@@ -5595,7 +5597,7 @@
         <v>14117</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A73" s="5">
         <v>43966</v>
       </c>
@@ -5645,7 +5647,7 @@
         <v>14260</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A74" s="5">
         <v>43967</v>
       </c>
@@ -5695,7 +5697,7 @@
         <v>14447</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A75" s="5">
         <v>43968</v>
       </c>
@@ -5745,7 +5747,7 @@
         <v>14537</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A76" s="5">
         <v>43969</v>
       </c>
@@ -5795,7 +5797,7 @@
         <v>14594</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A77" s="5">
         <v>43970</v>
       </c>
@@ -5845,7 +5847,7 @@
         <v>14655</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A78" s="5">
         <v>43971</v>
       </c>
@@ -5895,7 +5897,7 @@
         <v>14751</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A79" s="5">
         <v>43972</v>
       </c>
@@ -5945,7 +5947,7 @@
         <v>14856</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A80" s="5">
         <v>43973</v>
       </c>
@@ -5995,7 +5997,7 @@
         <v>14969</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A81" s="5">
         <v>43974</v>
       </c>
@@ -6045,7 +6047,7 @@
         <v>15041</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A82" s="5">
         <v>43975</v>
       </c>
@@ -6095,7 +6097,7 @@
         <v>15101</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A83" s="5">
         <v>43976</v>
       </c>
@@ -6145,7 +6147,7 @@
         <v>15156</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A84" s="5">
         <v>43977</v>
       </c>
@@ -6195,7 +6197,7 @@
         <v>15185</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A85" s="5">
         <v>43978</v>
       </c>
@@ -6245,7 +6247,7 @@
         <v>15240</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A86" s="5">
         <v>43979</v>
       </c>
@@ -6295,7 +6297,7 @@
         <v>15288</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A87" s="5">
         <v>43980</v>
       </c>
@@ -6345,7 +6347,7 @@
         <v>15327</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A88" s="5">
         <v>43981</v>
       </c>
@@ -6395,7 +6397,7 @@
         <v>15382</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A89" s="5">
         <v>43982</v>
       </c>
@@ -6445,7 +6447,7 @@
         <v>15400</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A90" s="5">
         <v>43983</v>
       </c>
@@ -6495,7 +6497,7 @@
         <v>15418</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A91" s="5">
         <v>43984</v>
       </c>
@@ -6545,7 +6547,7 @@
         <v>15471</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A92" s="5">
         <v>43985</v>
       </c>
@@ -6595,7 +6597,7 @@
         <v>15504</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A93" s="5">
         <v>43986</v>
       </c>
@@ -6645,7 +6647,7 @@
         <v>15553</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A94" s="5">
         <v>43987</v>
       </c>
@@ -6695,7 +6697,7 @@
         <v>15582</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A95" s="5">
         <v>43988</v>
       </c>
@@ -6745,7 +6747,7 @@
         <v>15603</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A96" s="5">
         <v>43989</v>
       </c>
@@ -6795,7 +6797,7 @@
         <v>15621</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A97" s="5">
         <v>43990</v>
       </c>
@@ -6845,7 +6847,7 @@
         <v>15639</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A98" s="5">
         <v>43991</v>
       </c>
@@ -6895,7 +6897,7 @@
         <v>15653</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A99" s="5">
         <v>43992</v>
       </c>
@@ -6945,7 +6947,7 @@
         <v>15665</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A100" s="5">
         <v>43993</v>
       </c>
@@ -6995,7 +6997,7 @@
         <v>15682</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A101" s="5">
         <v>43994</v>
       </c>
@@ -7045,7 +7047,7 @@
         <v>15709</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A102" s="5">
         <v>43995</v>
       </c>
@@ -7095,23 +7097,57 @@
         <v>15730</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C103" s="28"/>
-      <c r="D103" s="28"/>
-      <c r="E103" s="28"/>
-      <c r="F103" s="28"/>
-      <c r="G103" s="28"/>
-      <c r="H103" s="28"/>
-      <c r="I103" s="28"/>
-      <c r="J103" s="28"/>
-      <c r="K103" s="28"/>
-      <c r="L103" s="28"/>
-      <c r="M103" s="28"/>
-      <c r="N103" s="28"/>
-      <c r="O103" s="28"/>
-      <c r="P103" s="28"/>
-    </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A103" s="5">
+        <v>43996</v>
+      </c>
+      <c r="B103" s="28">
+        <v>1088</v>
+      </c>
+      <c r="C103" s="28">
+        <v>327</v>
+      </c>
+      <c r="D103" s="28">
+        <v>261</v>
+      </c>
+      <c r="E103" s="28">
+        <v>885</v>
+      </c>
+      <c r="F103" s="28">
+        <v>952</v>
+      </c>
+      <c r="G103" s="28">
+        <v>1294</v>
+      </c>
+      <c r="H103" s="28">
+        <v>4010</v>
+      </c>
+      <c r="I103" s="28">
+        <v>341</v>
+      </c>
+      <c r="J103" s="28">
+        <v>2035</v>
+      </c>
+      <c r="K103" s="28">
+        <v>2807</v>
+      </c>
+      <c r="L103" s="28">
+        <v>8</v>
+      </c>
+      <c r="M103" s="28">
+        <v>54</v>
+      </c>
+      <c r="N103" s="28">
+        <v>1687</v>
+      </c>
+      <c r="O103" s="28">
+        <v>6</v>
+      </c>
+      <c r="P103" s="32">
+        <v>15755</v>
+      </c>
+    </row>
+    <row r="104" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C104" s="28"/>
       <c r="D104" s="28"/>
       <c r="E104" s="28"/>
@@ -7127,7 +7163,7 @@
       <c r="O104" s="28"/>
       <c r="P104" s="28"/>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C105" s="28"/>
       <c r="D105" s="28"/>
       <c r="E105" s="28"/>
@@ -7143,7 +7179,7 @@
       <c r="O105" s="28"/>
       <c r="P105" s="28"/>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C106" s="28"/>
       <c r="D106" s="28"/>
       <c r="E106" s="28"/>
@@ -7159,7 +7195,7 @@
       <c r="O106" s="28"/>
       <c r="P106" s="28"/>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C107" s="28"/>
       <c r="D107" s="28"/>
       <c r="E107" s="28"/>
@@ -7175,7 +7211,7 @@
       <c r="O107" s="28"/>
       <c r="P107" s="28"/>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C108" s="28"/>
       <c r="D108" s="28"/>
       <c r="E108" s="28"/>
@@ -7191,7 +7227,7 @@
       <c r="O108" s="28"/>
       <c r="P108" s="28"/>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C109" s="28"/>
       <c r="D109" s="28"/>
       <c r="E109" s="28"/>
@@ -7207,7 +7243,7 @@
       <c r="O109" s="28"/>
       <c r="P109" s="28"/>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C110" s="28"/>
       <c r="D110" s="28"/>
       <c r="E110" s="28"/>
@@ -7223,7 +7259,7 @@
       <c r="O110" s="28"/>
       <c r="P110" s="28"/>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C111" s="28"/>
       <c r="D111" s="28"/>
       <c r="E111" s="28"/>
@@ -7239,7 +7275,7 @@
       <c r="O111" s="28"/>
       <c r="P111" s="28"/>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C112" s="28"/>
       <c r="D112" s="28"/>
       <c r="E112" s="28"/>
@@ -7255,7 +7291,7 @@
       <c r="O112" s="28"/>
       <c r="P112" s="28"/>
     </row>
-    <row r="113" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C113" s="28"/>
       <c r="D113" s="28"/>
       <c r="E113" s="28"/>
@@ -7271,7 +7307,7 @@
       <c r="O113" s="28"/>
       <c r="P113" s="28"/>
     </row>
-    <row r="114" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C114" s="28"/>
       <c r="D114" s="28"/>
       <c r="E114" s="28"/>
@@ -7287,7 +7323,7 @@
       <c r="O114" s="28"/>
       <c r="P114" s="28"/>
     </row>
-    <row r="115" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B115" s="28"/>
       <c r="C115" s="28"/>
       <c r="D115" s="28"/>
@@ -7304,7 +7340,7 @@
       <c r="O115" s="28"/>
       <c r="P115" s="28"/>
     </row>
-    <row r="116" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B116" s="28"/>
       <c r="C116" s="28"/>
       <c r="D116" s="28"/>
@@ -7321,7 +7357,7 @@
       <c r="O116" s="28"/>
       <c r="P116" s="28"/>
     </row>
-    <row r="117" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B117" s="28"/>
       <c r="C117" s="28"/>
       <c r="D117" s="28"/>
@@ -7338,7 +7374,7 @@
       <c r="O117" s="28"/>
       <c r="P117" s="28"/>
     </row>
-    <row r="118" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B118" s="28"/>
       <c r="C118" s="28"/>
       <c r="D118" s="28"/>
@@ -7355,7 +7391,7 @@
       <c r="O118" s="28"/>
       <c r="P118" s="28"/>
     </row>
-    <row r="119" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B119" s="28"/>
       <c r="C119" s="28"/>
       <c r="D119" s="28"/>
@@ -7372,7 +7408,7 @@
       <c r="O119" s="28"/>
       <c r="P119" s="28"/>
     </row>
-    <row r="120" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B120" s="28"/>
       <c r="C120" s="28"/>
       <c r="D120" s="28"/>
@@ -7389,7 +7425,7 @@
       <c r="O120" s="28"/>
       <c r="P120" s="28"/>
     </row>
-    <row r="121" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B121" s="28"/>
       <c r="C121" s="28"/>
       <c r="D121" s="28"/>
@@ -7406,7 +7442,7 @@
       <c r="O121" s="28"/>
       <c r="P121" s="28"/>
     </row>
-    <row r="122" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B122" s="28"/>
       <c r="C122" s="28"/>
       <c r="D122" s="28"/>
@@ -7423,7 +7459,7 @@
       <c r="O122" s="28"/>
       <c r="P122" s="28"/>
     </row>
-    <row r="123" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B123" s="28"/>
       <c r="C123" s="28"/>
       <c r="D123" s="28"/>
@@ -7440,7 +7476,7 @@
       <c r="O123" s="28"/>
       <c r="P123" s="28"/>
     </row>
-    <row r="124" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B124" s="28"/>
       <c r="C124" s="28"/>
       <c r="D124" s="28"/>
@@ -7457,7 +7493,7 @@
       <c r="O124" s="28"/>
       <c r="P124" s="28"/>
     </row>
-    <row r="125" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B125" s="28"/>
       <c r="C125" s="28"/>
       <c r="D125" s="28"/>
@@ -7474,7 +7510,7 @@
       <c r="O125" s="28"/>
       <c r="P125" s="28"/>
     </row>
-    <row r="126" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B126" s="28"/>
       <c r="C126" s="28"/>
       <c r="D126" s="28"/>
@@ -7491,7 +7527,7 @@
       <c r="O126" s="28"/>
       <c r="P126" s="28"/>
     </row>
-    <row r="127" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B127" s="28"/>
       <c r="C127" s="28"/>
       <c r="D127" s="28"/>
@@ -7508,7 +7544,7 @@
       <c r="O127" s="28"/>
       <c r="P127" s="28"/>
     </row>
-    <row r="128" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B128" s="28"/>
       <c r="C128" s="28"/>
       <c r="D128" s="28"/>
@@ -7525,7 +7561,7 @@
       <c r="O128" s="28"/>
       <c r="P128" s="28"/>
     </row>
-    <row r="129" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B129" s="28"/>
       <c r="C129" s="28"/>
       <c r="D129" s="28"/>
@@ -7542,7 +7578,7 @@
       <c r="O129" s="28"/>
       <c r="P129" s="28"/>
     </row>
-    <row r="130" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B130" s="28"/>
       <c r="C130" s="28"/>
       <c r="D130" s="28"/>
@@ -7559,7 +7595,7 @@
       <c r="O130" s="28"/>
       <c r="P130" s="28"/>
     </row>
-    <row r="131" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B131" s="28"/>
       <c r="C131" s="28"/>
       <c r="D131" s="28"/>
@@ -7576,7 +7612,7 @@
       <c r="O131" s="28"/>
       <c r="P131" s="28"/>
     </row>
-    <row r="132" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B132" s="28"/>
       <c r="C132" s="28"/>
       <c r="D132" s="28"/>
@@ -7593,7 +7629,7 @@
       <c r="O132" s="28"/>
       <c r="P132" s="28"/>
     </row>
-    <row r="133" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B133" s="28"/>
       <c r="C133" s="28"/>
       <c r="D133" s="28"/>
@@ -7610,7 +7646,7 @@
       <c r="O133" s="28"/>
       <c r="P133" s="28"/>
     </row>
-    <row r="134" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B134" s="28"/>
       <c r="C134" s="28"/>
       <c r="D134" s="28"/>
@@ -7627,7 +7663,7 @@
       <c r="O134" s="28"/>
       <c r="P134" s="28"/>
     </row>
-    <row r="135" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B135" s="28"/>
       <c r="C135" s="28"/>
       <c r="D135" s="28"/>
@@ -7644,7 +7680,7 @@
       <c r="O135" s="28"/>
       <c r="P135" s="28"/>
     </row>
-    <row r="136" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B136" s="28"/>
       <c r="C136" s="28"/>
       <c r="D136" s="28"/>
@@ -7661,7 +7697,7 @@
       <c r="O136" s="28"/>
       <c r="P136" s="28"/>
     </row>
-    <row r="137" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B137" s="28"/>
       <c r="C137" s="28"/>
       <c r="D137" s="28"/>
@@ -7678,7 +7714,7 @@
       <c r="O137" s="28"/>
       <c r="P137" s="28"/>
     </row>
-    <row r="138" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B138" s="28"/>
       <c r="C138" s="28"/>
       <c r="D138" s="28"/>
@@ -7695,7 +7731,7 @@
       <c r="O138" s="28"/>
       <c r="P138" s="28"/>
     </row>
-    <row r="139" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B139" s="28"/>
       <c r="C139" s="28"/>
       <c r="D139" s="28"/>
@@ -7712,7 +7748,7 @@
       <c r="O139" s="28"/>
       <c r="P139" s="28"/>
     </row>
-    <row r="140" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B140" s="28"/>
       <c r="C140" s="28"/>
       <c r="D140" s="28"/>
@@ -7729,7 +7765,7 @@
       <c r="O140" s="28"/>
       <c r="P140" s="28"/>
     </row>
-    <row r="141" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B141" s="28"/>
       <c r="C141" s="28"/>
       <c r="D141" s="28"/>
@@ -7746,7 +7782,7 @@
       <c r="O141" s="28"/>
       <c r="P141" s="28"/>
     </row>
-    <row r="142" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B142" s="28"/>
       <c r="C142" s="28"/>
       <c r="D142" s="28"/>
@@ -7763,7 +7799,7 @@
       <c r="O142" s="28"/>
       <c r="P142" s="28"/>
     </row>
-    <row r="143" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B143" s="28"/>
       <c r="C143" s="28"/>
       <c r="D143" s="28"/>
@@ -7780,7 +7816,7 @@
       <c r="O143" s="28"/>
       <c r="P143" s="28"/>
     </row>
-    <row r="144" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B144" s="28"/>
       <c r="C144" s="28"/>
       <c r="D144" s="28"/>
@@ -7797,7 +7833,7 @@
       <c r="O144" s="28"/>
       <c r="P144" s="28"/>
     </row>
-    <row r="145" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B145" s="28"/>
       <c r="C145" s="28"/>
       <c r="D145" s="28"/>
@@ -7814,7 +7850,7 @@
       <c r="O145" s="28"/>
       <c r="P145" s="28"/>
     </row>
-    <row r="146" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B146" s="28"/>
       <c r="C146" s="28"/>
       <c r="D146" s="28"/>
@@ -7831,7 +7867,7 @@
       <c r="O146" s="28"/>
       <c r="P146" s="28"/>
     </row>
-    <row r="147" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B147" s="28"/>
       <c r="C147" s="28"/>
       <c r="D147" s="28"/>
@@ -7848,7 +7884,7 @@
       <c r="O147" s="28"/>
       <c r="P147" s="28"/>
     </row>
-    <row r="148" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B148" s="28"/>
       <c r="C148" s="28"/>
       <c r="D148" s="28"/>
@@ -7865,7 +7901,7 @@
       <c r="O148" s="28"/>
       <c r="P148" s="28"/>
     </row>
-    <row r="149" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B149" s="28"/>
       <c r="C149" s="28"/>
       <c r="D149" s="28"/>
@@ -7882,7 +7918,7 @@
       <c r="O149" s="28"/>
       <c r="P149" s="28"/>
     </row>
-    <row r="150" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B150" s="28"/>
       <c r="C150" s="28"/>
       <c r="D150" s="28"/>
@@ -7899,7 +7935,7 @@
       <c r="O150" s="28"/>
       <c r="P150" s="28"/>
     </row>
-    <row r="151" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B151" s="28"/>
       <c r="C151" s="28"/>
       <c r="D151" s="28"/>
@@ -7916,7 +7952,7 @@
       <c r="O151" s="28"/>
       <c r="P151" s="28"/>
     </row>
-    <row r="152" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B152" s="28"/>
       <c r="C152" s="28"/>
       <c r="D152" s="28"/>
@@ -7933,7 +7969,7 @@
       <c r="O152" s="28"/>
       <c r="P152" s="28"/>
     </row>
-    <row r="153" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B153" s="28"/>
       <c r="C153" s="28"/>
       <c r="D153" s="28"/>
@@ -7950,7 +7986,7 @@
       <c r="O153" s="28"/>
       <c r="P153" s="28"/>
     </row>
-    <row r="154" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B154" s="28"/>
       <c r="C154" s="28"/>
       <c r="D154" s="28"/>
@@ -7967,7 +8003,7 @@
       <c r="O154" s="28"/>
       <c r="P154" s="28"/>
     </row>
-    <row r="155" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B155" s="28"/>
       <c r="C155" s="28"/>
       <c r="D155" s="28"/>
@@ -7984,7 +8020,7 @@
       <c r="O155" s="28"/>
       <c r="P155" s="28"/>
     </row>
-    <row r="156" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B156" s="28"/>
       <c r="C156" s="28"/>
       <c r="D156" s="28"/>
@@ -8001,7 +8037,7 @@
       <c r="O156" s="28"/>
       <c r="P156" s="28"/>
     </row>
-    <row r="157" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B157" s="28"/>
       <c r="C157" s="28"/>
       <c r="D157" s="28"/>
@@ -8018,7 +8054,7 @@
       <c r="O157" s="28"/>
       <c r="P157" s="28"/>
     </row>
-    <row r="158" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B158" s="28"/>
       <c r="C158" s="28"/>
       <c r="D158" s="28"/>
@@ -8035,7 +8071,7 @@
       <c r="O158" s="28"/>
       <c r="P158" s="28"/>
     </row>
-    <row r="159" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B159" s="28"/>
       <c r="C159" s="28"/>
       <c r="D159" s="28"/>
@@ -8052,7 +8088,7 @@
       <c r="O159" s="28"/>
       <c r="P159" s="28"/>
     </row>
-    <row r="160" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B160" s="28"/>
       <c r="C160" s="28"/>
       <c r="D160" s="28"/>
@@ -8077,21 +8113,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q91"/>
+  <dimension ref="A1:Q92"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L91" sqref="L91"/>
+      <pane ySplit="3" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5703125" style="2"/>
+    <col min="1" max="1" width="12.44140625" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.5546875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -8112,7 +8148,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -8133,7 +8169,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -8186,7 +8222,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>43908</v>
       </c>
@@ -8239,7 +8275,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>43909</v>
       </c>
@@ -8292,7 +8328,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>43910</v>
       </c>
@@ -8345,7 +8381,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>43911</v>
       </c>
@@ -8398,7 +8434,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>43912</v>
       </c>
@@ -8451,7 +8487,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>43913</v>
       </c>
@@ -8504,7 +8540,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>43914</v>
       </c>
@@ -8557,7 +8593,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>43915</v>
       </c>
@@ -8610,7 +8646,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
         <v>43916</v>
       </c>
@@ -8663,7 +8699,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>43917</v>
       </c>
@@ -8716,7 +8752,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>43918</v>
       </c>
@@ -8769,7 +8805,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>43919</v>
       </c>
@@ -8822,7 +8858,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>43920</v>
       </c>
@@ -8875,7 +8911,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>43921</v>
       </c>
@@ -8928,7 +8964,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>43922</v>
       </c>
@@ -8981,7 +9017,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>43923</v>
       </c>
@@ -9034,7 +9070,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>43924</v>
       </c>
@@ -9087,7 +9123,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>43925</v>
       </c>
@@ -9140,7 +9176,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="12">
         <v>43926</v>
       </c>
@@ -9193,7 +9229,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="12">
         <v>43927</v>
       </c>
@@ -9246,7 +9282,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="12">
         <v>43928</v>
       </c>
@@ -9299,7 +9335,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="12">
         <v>43929</v>
       </c>
@@ -9352,7 +9388,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="12">
         <v>43930</v>
       </c>
@@ -9405,7 +9441,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="12">
         <v>43931</v>
       </c>
@@ -9458,7 +9494,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="12">
         <v>43932</v>
       </c>
@@ -9511,7 +9547,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="12">
         <v>43933</v>
       </c>
@@ -9564,7 +9600,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <v>43934</v>
       </c>
@@ -9617,7 +9653,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="12">
         <v>43935</v>
       </c>
@@ -9670,7 +9706,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="12">
         <v>43936</v>
       </c>
@@ -9723,7 +9759,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="12">
         <v>43937</v>
       </c>
@@ -9776,7 +9812,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="12">
         <v>43938</v>
       </c>
@@ -9829,7 +9865,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="12">
         <v>43939</v>
       </c>
@@ -9882,7 +9918,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="30">
         <v>43940</v>
       </c>
@@ -9935,7 +9971,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="30">
         <v>43941</v>
       </c>
@@ -9988,7 +10024,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="30">
         <v>43942</v>
       </c>
@@ -10041,7 +10077,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="30">
         <v>43943</v>
       </c>
@@ -10094,7 +10130,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="30">
         <v>43944</v>
       </c>
@@ -10147,7 +10183,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="30">
         <v>43945</v>
       </c>
@@ -10200,7 +10236,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="30">
         <v>43946</v>
       </c>
@@ -10253,7 +10289,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="30">
         <v>43947</v>
       </c>
@@ -10306,7 +10342,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="30">
         <v>43948</v>
       </c>
@@ -10359,7 +10395,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="30">
         <v>43949</v>
       </c>
@@ -10412,7 +10448,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="30">
         <v>43950</v>
       </c>
@@ -10465,7 +10501,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="30">
         <v>43951</v>
       </c>
@@ -10518,7 +10554,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" s="30">
         <v>43952</v>
       </c>
@@ -10571,7 +10607,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="30">
         <v>43953</v>
       </c>
@@ -10624,7 +10660,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" s="30">
         <v>43954</v>
       </c>
@@ -10677,7 +10713,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="30">
         <v>43955</v>
       </c>
@@ -10730,7 +10766,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" s="30">
         <v>43956</v>
       </c>
@@ -10783,7 +10819,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" s="30">
         <v>43957</v>
       </c>
@@ -10836,7 +10872,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" s="30">
         <v>43958</v>
       </c>
@@ -10889,7 +10925,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" s="30">
         <v>43959</v>
       </c>
@@ -10942,7 +10978,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" s="30">
         <v>43960</v>
       </c>
@@ -10995,7 +11031,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" s="30">
         <v>43961</v>
       </c>
@@ -11048,7 +11084,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" s="30">
         <v>43962</v>
       </c>
@@ -11101,7 +11137,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" s="30">
         <v>43963</v>
       </c>
@@ -11154,7 +11190,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" s="30">
         <v>43964</v>
       </c>
@@ -11207,7 +11243,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" s="30">
         <v>43965</v>
       </c>
@@ -11260,7 +11296,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" s="30">
         <v>43966</v>
       </c>
@@ -11313,7 +11349,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" s="30">
         <v>43967</v>
       </c>
@@ -11366,7 +11402,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" s="30">
         <v>43968</v>
       </c>
@@ -11419,7 +11455,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" s="30">
         <v>43969</v>
       </c>
@@ -11472,7 +11508,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" s="30">
         <v>43970</v>
       </c>
@@ -11525,7 +11561,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" s="30">
         <v>43971</v>
       </c>
@@ -11578,7 +11614,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" s="30">
         <v>43972</v>
       </c>
@@ -11631,7 +11667,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" s="30">
         <v>43973</v>
       </c>
@@ -11684,7 +11720,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" s="30">
         <v>43974</v>
       </c>
@@ -11737,7 +11773,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" s="30">
         <v>43975</v>
       </c>
@@ -11790,7 +11826,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" s="30">
         <v>43976</v>
       </c>
@@ -11843,7 +11879,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" s="30">
         <v>43977</v>
       </c>
@@ -11896,7 +11932,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" s="30">
         <v>43978</v>
       </c>
@@ -11949,7 +11985,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75" s="30">
         <v>43979</v>
       </c>
@@ -12002,7 +12038,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76" s="30">
         <v>43980</v>
       </c>
@@ -12055,7 +12091,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77" s="30">
         <v>43981</v>
       </c>
@@ -12108,7 +12144,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78" s="30">
         <v>43982</v>
       </c>
@@ -12161,7 +12197,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79" s="30">
         <v>43983</v>
       </c>
@@ -12214,7 +12250,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A80" s="30">
         <v>43984</v>
       </c>
@@ -12267,7 +12303,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A81" s="30">
         <v>43985</v>
       </c>
@@ -12320,7 +12356,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A82" s="30">
         <v>43986</v>
       </c>
@@ -12373,7 +12409,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A83" s="30">
         <v>43987</v>
       </c>
@@ -12426,7 +12462,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A84" s="30">
         <v>43988</v>
       </c>
@@ -12479,7 +12515,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A85" s="30">
         <v>43989</v>
       </c>
@@ -12532,7 +12568,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A86" s="30">
         <v>43990</v>
       </c>
@@ -12585,7 +12621,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A87" s="30">
         <v>43991</v>
       </c>
@@ -12638,7 +12674,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A88" s="30">
         <v>43992</v>
       </c>
@@ -12691,7 +12727,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A89" s="30">
         <v>43993</v>
       </c>
@@ -12744,7 +12780,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A90" s="30">
         <v>43994</v>
       </c>
@@ -12797,7 +12833,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A91" s="30">
         <v>43995</v>
       </c>
@@ -12848,6 +12884,59 @@
       </c>
       <c r="Q91" s="13">
         <v>20</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A92" s="30">
+        <v>43996</v>
+      </c>
+      <c r="B92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K92" s="11">
+        <v>5</v>
+      </c>
+      <c r="L92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P92" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q92" s="13">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -12858,23 +12947,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R83"/>
+  <dimension ref="A1:R84"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B64" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="S83" sqref="S83"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5703125" style="2"/>
+    <col min="1" max="1" width="15.44140625" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.5546875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -12895,7 +12984,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -12916,7 +13005,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -12969,7 +13058,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>43916</v>
       </c>
@@ -13022,7 +13111,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>43917</v>
       </c>
@@ -13075,7 +13164,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>43918</v>
       </c>
@@ -13128,7 +13217,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>43919</v>
       </c>
@@ -13181,7 +13270,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>43920</v>
       </c>
@@ -13234,7 +13323,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>43921</v>
       </c>
@@ -13287,7 +13376,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>43922</v>
       </c>
@@ -13340,7 +13429,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>43923</v>
       </c>
@@ -13393,7 +13482,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
         <v>43924</v>
       </c>
@@ -13446,7 +13535,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>43925</v>
       </c>
@@ -13499,7 +13588,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>43926</v>
       </c>
@@ -13552,7 +13641,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>43927</v>
       </c>
@@ -13605,7 +13694,7 @@
         <v>1262</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>43928</v>
       </c>
@@ -13658,7 +13747,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>43929</v>
       </c>
@@ -13711,7 +13800,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>43930</v>
       </c>
@@ -13764,7 +13853,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>43931</v>
       </c>
@@ -13817,7 +13906,7 @@
         <v>1461</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>43932</v>
       </c>
@@ -13870,7 +13959,7 @@
         <v>1467</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>43933</v>
       </c>
@@ -13923,7 +14012,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="12">
         <v>43934</v>
       </c>
@@ -13976,7 +14065,7 @@
         <v>1482</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="12">
         <v>43935</v>
       </c>
@@ -14029,7 +14118,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="12">
         <v>43936</v>
       </c>
@@ -14082,7 +14171,7 @@
         <v>1486</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="12">
         <v>43937</v>
       </c>
@@ -14135,7 +14224,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="12">
         <v>43938</v>
       </c>
@@ -14188,7 +14277,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="12">
         <v>43939</v>
       </c>
@@ -14241,7 +14330,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="12">
         <v>43940</v>
       </c>
@@ -14294,7 +14383,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="12">
         <v>43941</v>
       </c>
@@ -14347,7 +14436,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <v>43942</v>
       </c>
@@ -14400,7 +14489,7 @@
         <v>1472</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="12">
         <v>43943</v>
       </c>
@@ -14453,7 +14542,7 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="12">
         <v>43944</v>
       </c>
@@ -14506,7 +14595,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="12">
         <v>43945</v>
       </c>
@@ -14559,7 +14648,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="12">
         <v>43946</v>
       </c>
@@ -14612,7 +14701,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="12">
         <v>43947</v>
       </c>
@@ -14665,7 +14754,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="30">
         <v>43948</v>
       </c>
@@ -14718,7 +14807,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="30">
         <v>43949</v>
       </c>
@@ -14771,7 +14860,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="30">
         <v>43950</v>
       </c>
@@ -14824,7 +14913,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="30">
         <v>43951</v>
       </c>
@@ -14877,7 +14966,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="30">
         <v>43952</v>
       </c>
@@ -14930,7 +15019,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="30">
         <v>43953</v>
       </c>
@@ -14983,7 +15072,7 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="30">
         <v>43954</v>
       </c>
@@ -15036,7 +15125,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="30">
         <v>43955</v>
       </c>
@@ -15089,7 +15178,7 @@
         <v>1279</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="30">
         <v>43956</v>
       </c>
@@ -15142,7 +15231,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="30">
         <v>43957</v>
       </c>
@@ -15195,7 +15284,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="30">
         <v>43958</v>
       </c>
@@ -15248,7 +15337,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="30">
         <v>43959</v>
       </c>
@@ -15301,7 +15390,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" s="30">
         <v>43960</v>
       </c>
@@ -15354,7 +15443,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="30">
         <v>43961</v>
       </c>
@@ -15407,7 +15496,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" s="30">
         <v>43962</v>
       </c>
@@ -15460,7 +15549,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="30">
         <v>43963</v>
       </c>
@@ -15513,7 +15602,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" s="30">
         <v>43964</v>
       </c>
@@ -15566,7 +15655,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" s="30">
         <v>43965</v>
       </c>
@@ -15619,7 +15708,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" s="30">
         <v>43966</v>
       </c>
@@ -15672,7 +15761,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" s="30">
         <v>43967</v>
       </c>
@@ -15725,7 +15814,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" s="30">
         <v>43968</v>
       </c>
@@ -15778,7 +15867,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" s="30">
         <v>43969</v>
       </c>
@@ -15831,7 +15920,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" s="30">
         <v>43970</v>
       </c>
@@ -15884,7 +15973,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" s="30">
         <v>43971</v>
       </c>
@@ -15937,7 +16026,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" s="30">
         <v>43972</v>
       </c>
@@ -15990,7 +16079,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" s="30">
         <v>43973</v>
       </c>
@@ -16043,7 +16132,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" s="30">
         <v>43974</v>
       </c>
@@ -16096,7 +16185,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" s="30">
         <v>43975</v>
       </c>
@@ -16149,7 +16238,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" s="30">
         <v>43976</v>
       </c>
@@ -16202,7 +16291,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A65" s="51">
         <v>43977</v>
       </c>
@@ -16255,7 +16344,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A66" s="51">
         <v>43978</v>
       </c>
@@ -16308,7 +16397,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A67" s="51">
         <v>43979</v>
       </c>
@@ -16361,7 +16450,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A68" s="51">
         <v>43980</v>
       </c>
@@ -16414,7 +16503,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A69" s="51">
         <v>43981</v>
       </c>
@@ -16467,7 +16556,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A70" s="51">
         <v>43982</v>
       </c>
@@ -16520,7 +16609,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A71" s="51">
         <v>43983</v>
       </c>
@@ -16573,7 +16662,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A72" s="51">
         <v>43984</v>
       </c>
@@ -16626,7 +16715,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A73" s="51">
         <v>43985</v>
       </c>
@@ -16679,7 +16768,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A74" s="51">
         <v>43986</v>
       </c>
@@ -16732,7 +16821,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A75" s="51">
         <v>43987</v>
       </c>
@@ -16785,7 +16874,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A76" s="51">
         <v>43988</v>
       </c>
@@ -16838,7 +16927,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A77" s="51">
         <v>43989</v>
       </c>
@@ -16891,7 +16980,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A78" s="51">
         <v>43990</v>
       </c>
@@ -16944,7 +17033,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A79" s="51">
         <v>43991</v>
       </c>
@@ -16997,7 +17086,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A80" s="51">
         <v>43992</v>
       </c>
@@ -17051,7 +17140,7 @@
       </c>
       <c r="R80" s="54"/>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A81" s="51">
         <v>43993</v>
       </c>
@@ -17105,7 +17194,7 @@
       </c>
       <c r="R81" s="54"/>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A82" s="51">
         <v>43994</v>
       </c>
@@ -17159,7 +17248,7 @@
       </c>
       <c r="R82" s="54"/>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A83" s="51">
         <v>43995</v>
       </c>
@@ -17210,6 +17299,59 @@
       </c>
       <c r="Q83" s="13">
         <v>582</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A84" s="51">
+        <v>43996</v>
+      </c>
+      <c r="B84" s="11">
+        <v>5</v>
+      </c>
+      <c r="C84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E84" s="11">
+        <v>57</v>
+      </c>
+      <c r="F84" s="11">
+        <v>5</v>
+      </c>
+      <c r="G84" s="11">
+        <v>56</v>
+      </c>
+      <c r="H84" s="11">
+        <v>255</v>
+      </c>
+      <c r="I84" s="11">
+        <v>7</v>
+      </c>
+      <c r="J84" s="11">
+        <v>49</v>
+      </c>
+      <c r="K84" s="11">
+        <v>134</v>
+      </c>
+      <c r="L84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N84" s="11">
+        <v>6</v>
+      </c>
+      <c r="O84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q84" s="13">
+        <v>575</v>
       </c>
     </row>
   </sheetData>
@@ -17220,23 +17362,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q83"/>
+  <dimension ref="A1:Q84"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A84" sqref="A84"/>
+      <selection pane="bottomRight" activeCell="O87" sqref="O87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5703125" style="2"/>
+    <col min="1" max="1" width="12.44140625" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.5546875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -17257,7 +17399,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -17278,7 +17420,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -17331,7 +17473,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>43916</v>
       </c>
@@ -17384,7 +17526,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>43917</v>
       </c>
@@ -17437,7 +17579,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>43918</v>
       </c>
@@ -17490,7 +17632,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>43919</v>
       </c>
@@ -17543,7 +17685,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>43920</v>
       </c>
@@ -17596,7 +17738,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>43921</v>
       </c>
@@ -17649,7 +17791,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>43922</v>
       </c>
@@ -17702,7 +17844,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>43923</v>
       </c>
@@ -17755,7 +17897,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
         <v>43924</v>
       </c>
@@ -17808,7 +17950,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>43925</v>
       </c>
@@ -17861,7 +18003,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>43926</v>
       </c>
@@ -17914,7 +18056,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>43927</v>
       </c>
@@ -17967,7 +18109,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>43928</v>
       </c>
@@ -18020,7 +18162,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>43929</v>
       </c>
@@ -18073,7 +18215,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>43930</v>
       </c>
@@ -18126,7 +18268,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>43931</v>
       </c>
@@ -18179,7 +18321,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>43932</v>
       </c>
@@ -18232,7 +18374,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>43933</v>
       </c>
@@ -18285,7 +18427,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="12">
         <v>43934</v>
       </c>
@@ -18338,7 +18480,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="12">
         <v>43935</v>
       </c>
@@ -18391,7 +18533,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="12">
         <v>43936</v>
       </c>
@@ -18444,7 +18586,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="12">
         <v>43937</v>
       </c>
@@ -18497,7 +18639,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="12">
         <v>43938</v>
       </c>
@@ -18550,7 +18692,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="12">
         <v>43939</v>
       </c>
@@ -18603,7 +18745,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="12">
         <v>43940</v>
       </c>
@@ -18656,7 +18798,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="12">
         <v>43941</v>
       </c>
@@ -18709,7 +18851,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <v>43942</v>
       </c>
@@ -18762,7 +18904,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="12">
         <v>43943</v>
       </c>
@@ -18815,7 +18957,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="12">
         <v>43944</v>
       </c>
@@ -18868,7 +19010,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="12">
         <v>43945</v>
       </c>
@@ -18921,7 +19063,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="12">
         <v>43946</v>
       </c>
@@ -18974,7 +19116,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="12">
         <v>43947</v>
       </c>
@@ -19027,7 +19169,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="30">
         <v>43948</v>
       </c>
@@ -19080,7 +19222,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="30">
         <v>43949</v>
       </c>
@@ -19133,7 +19275,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="30">
         <v>43950</v>
       </c>
@@ -19186,7 +19328,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="30">
         <v>43951</v>
       </c>
@@ -19239,7 +19381,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="30">
         <v>43952</v>
       </c>
@@ -19292,7 +19434,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="30">
         <v>43953</v>
       </c>
@@ -19345,7 +19487,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="30">
         <v>43954</v>
       </c>
@@ -19398,7 +19540,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="30">
         <v>43955</v>
       </c>
@@ -19451,7 +19593,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="30">
         <v>43956</v>
       </c>
@@ -19504,7 +19646,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="30">
         <v>43957</v>
       </c>
@@ -19557,7 +19699,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="30">
         <v>43958</v>
       </c>
@@ -19610,7 +19752,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="30">
         <v>43959</v>
       </c>
@@ -19663,7 +19805,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" s="30">
         <v>43960</v>
       </c>
@@ -19716,7 +19858,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="30">
         <v>43961</v>
       </c>
@@ -19769,7 +19911,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" s="30">
         <v>43962</v>
       </c>
@@ -19822,7 +19964,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="30">
         <v>43963</v>
       </c>
@@ -19875,7 +20017,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" s="30">
         <v>43964</v>
       </c>
@@ -19928,7 +20070,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" s="30">
         <v>43965</v>
       </c>
@@ -19981,7 +20123,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" s="30">
         <v>43966</v>
       </c>
@@ -20034,7 +20176,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" s="30">
         <v>43967</v>
       </c>
@@ -20087,7 +20229,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" s="30">
         <v>43968</v>
       </c>
@@ -20140,7 +20282,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" s="30">
         <v>43969</v>
       </c>
@@ -20193,7 +20335,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" s="30">
         <v>43970</v>
       </c>
@@ -20246,7 +20388,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" s="30">
         <v>43971</v>
       </c>
@@ -20299,7 +20441,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" s="30">
         <v>43972</v>
       </c>
@@ -20352,7 +20494,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" s="30">
         <v>43973</v>
       </c>
@@ -20405,7 +20547,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" s="30">
         <v>43974</v>
       </c>
@@ -20458,7 +20600,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" s="30">
         <v>43975</v>
       </c>
@@ -20511,7 +20653,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" s="30">
         <v>43976</v>
       </c>
@@ -20564,7 +20706,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" s="30">
         <v>43977</v>
       </c>
@@ -20617,7 +20759,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" s="30">
         <v>43978</v>
       </c>
@@ -20670,7 +20812,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" s="30">
         <v>43979</v>
       </c>
@@ -20723,7 +20865,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" s="30">
         <v>43980</v>
       </c>
@@ -20776,7 +20918,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" s="30">
         <v>43981</v>
       </c>
@@ -20829,7 +20971,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" s="30">
         <v>43982</v>
       </c>
@@ -20882,7 +21024,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" s="30">
         <v>43983</v>
       </c>
@@ -20935,7 +21077,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" s="30">
         <v>43984</v>
       </c>
@@ -20988,7 +21130,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" s="30">
         <v>43985</v>
       </c>
@@ -21041,7 +21183,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" s="30">
         <v>43986</v>
       </c>
@@ -21094,7 +21236,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75" s="30">
         <v>43987</v>
       </c>
@@ -21147,7 +21289,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76" s="30">
         <v>43988</v>
       </c>
@@ -21200,7 +21342,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77" s="30">
         <v>43989</v>
       </c>
@@ -21253,7 +21395,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78" s="30">
         <v>43990</v>
       </c>
@@ -21306,7 +21448,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79" s="30">
         <v>43991</v>
       </c>
@@ -21359,7 +21501,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A80" s="30">
         <v>43992</v>
       </c>
@@ -21412,7 +21554,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A81" s="30">
         <v>43993</v>
       </c>
@@ -21465,7 +21607,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A82" s="30">
         <v>43994</v>
       </c>
@@ -21518,7 +21660,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A83" s="30">
         <v>43995</v>
       </c>
@@ -21569,6 +21711,59 @@
       </c>
       <c r="Q83" s="13">
         <v>401</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A84" s="30">
+        <v>43996</v>
+      </c>
+      <c r="B84" s="11">
+        <v>25</v>
+      </c>
+      <c r="C84" s="11">
+        <v>9</v>
+      </c>
+      <c r="D84" s="11">
+        <v>11</v>
+      </c>
+      <c r="E84" s="11">
+        <v>25</v>
+      </c>
+      <c r="F84" s="11">
+        <v>32</v>
+      </c>
+      <c r="G84" s="11">
+        <v>14</v>
+      </c>
+      <c r="H84" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I84" s="11">
+        <v>25</v>
+      </c>
+      <c r="J84" s="11">
+        <v>64</v>
+      </c>
+      <c r="K84" s="11">
+        <v>172</v>
+      </c>
+      <c r="L84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N84" s="11">
+        <v>12</v>
+      </c>
+      <c r="O84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q84" s="13">
+        <v>389</v>
       </c>
     </row>
   </sheetData>
@@ -21595,13 +21790,13 @@
       <value order="0">false</value>
     </field>
     <field name="Objective-IsPublished">
-      <value order="0">true</value>
+      <value order="0">false</value>
     </field>
     <field name="Objective-DatePublished">
-      <value order="0">2020-06-13T11:44:27Z</value>
+      <value order="0"/>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-13T11:44:27Z</value>
+      <value order="0">2020-06-14T11:47:42Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -21613,16 +21808,16 @@
       <value order="0">Analytical: COVID 19 Analysis: Restricted working papers: Research and analysis: Diseases: 2020-2025</value>
     </field>
     <field name="Objective-State">
-      <value order="0">Published</value>
+      <value order="0">Being Drafted</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41730562</value>
+      <value order="0">vA41732238</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">25.0</value>
+      <value order="0">25.3</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">175</value>
+      <value order="0">178</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-15 20:09)
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U445783\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA18464\A28088333\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u201433\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA1432\A28088333\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5988" windowHeight="6048" tabRatio="803" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5985" windowHeight="6045" tabRatio="803"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1858" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1883" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -659,7 +659,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>1. The data in Table 1 shows the cumulative number of people tested positive for COVID-19 across Scotland to date, broken down by board. </a:t>
+            <a:t>1. The data in Table 1 shows the cumulative number of people tested positive for COVID-19 across Scotland to date, broken down by board.  </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -698,7 +698,25 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>2. Results reported each day refer to the number of positive tests in the Health Protection Scotland ECOSS system reported to HPS by the laboratories in the 24 hours from 08:00 to 08:00. Therefore, the number of positive tests reported each day refers to the number of individuals with a positive result</a:t>
+            <a:t>2. Up</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> until 14 June, r</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>esults reported each day refer to the number of positive tests in the Health Protection Scotland ECOSS system reported to HPS by the laboratories in the 24 hours from 08:00 to 08:00. Therefore, the number of positive tests reported each day refers to the number of individuals with a positive result</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" baseline="0">
@@ -725,7 +743,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>he daily total of people found positive on 2/6/20 contains 40 historic samples from an NHS Fife laboratory.</a:t>
+            <a:t>he daily total of people found positive on 2/6/20 contains 40 historic samples from an NHS Fife laboratory. From 15 June the figures will also include people tested through the UK Government's testing programme including drive through, mobile testing units and home tests. There will be a delay to publishing these but a board table is expected to be available on or before 18 June.</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB">
             <a:effectLst/>
@@ -1662,6 +1680,86 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>771072</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>163284</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5143500" cy="1097643"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12709072" y="19122570"/>
+          <a:ext cx="5143500" cy="1097643"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>As of 15 June, this includes confirmed cases at UK Government Regional Testing Centres (RTCs). </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>A breakdown by NHS Board is not yet available from UK Gov RTCs for 15 June. This table will be updated by 18 June.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1927,25 +2025,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.44140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="90.44140625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.44140625" style="2"/>
+    <col min="2" max="2" width="29.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="90.42578125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>20</v>
       </c>
@@ -1953,7 +2049,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
         <v>22</v>
       </c>
@@ -1961,13 +2057,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="22" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="23"/>
     </row>
-    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="24" t="s">
         <v>26</v>
       </c>
@@ -1975,7 +2071,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="24" t="s">
         <v>27</v>
       </c>
@@ -1983,7 +2079,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="24" t="s">
         <v>36</v>
       </c>
@@ -1991,7 +2087,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
         <v>37</v>
       </c>
@@ -2019,12 +2115,12 @@
       <selection activeCell="O52" sqref="O52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.44140625" style="2"/>
+    <col min="1" max="16384" width="9.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="44" spans="1:1" ht="15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="43"/>
     </row>
   </sheetData>
@@ -2038,21 +2134,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S160"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B85" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B82" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H93" sqref="H93"/>
+      <selection pane="bottomRight" activeCell="R110" sqref="R110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" style="2" customWidth="1"/>
-    <col min="2" max="16" width="11.44140625" style="11" customWidth="1"/>
-    <col min="17" max="16384" width="8.5546875" style="2"/>
+    <col min="2" max="16" width="11.42578125" style="11" customWidth="1"/>
+    <col min="17" max="16384" width="8.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -2072,7 +2168,7 @@
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -2091,7 +2187,7 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -2141,7 +2237,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>43897</v>
       </c>
@@ -2191,7 +2287,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>43898</v>
       </c>
@@ -2241,7 +2337,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>43899</v>
       </c>
@@ -2291,7 +2387,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>43900</v>
       </c>
@@ -2341,7 +2437,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>43901</v>
       </c>
@@ -2391,7 +2487,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>43902</v>
       </c>
@@ -2441,7 +2537,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>43903</v>
       </c>
@@ -2491,7 +2587,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>43904</v>
       </c>
@@ -2541,7 +2637,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>43905</v>
       </c>
@@ -2591,7 +2687,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>43906</v>
       </c>
@@ -2641,7 +2737,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>43907</v>
       </c>
@@ -2691,7 +2787,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>43908</v>
       </c>
@@ -2741,7 +2837,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>43909</v>
       </c>
@@ -2791,7 +2887,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>43910</v>
       </c>
@@ -2841,7 +2937,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>43911</v>
       </c>
@@ -2891,7 +2987,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>43912</v>
       </c>
@@ -2941,7 +3037,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>43913</v>
       </c>
@@ -2991,7 +3087,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>43914</v>
       </c>
@@ -3041,7 +3137,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>43915</v>
       </c>
@@ -3091,7 +3187,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>43916</v>
       </c>
@@ -3141,7 +3237,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>43917</v>
       </c>
@@ -3191,7 +3287,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>43918</v>
       </c>
@@ -3241,7 +3337,7 @@
         <v>1264</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>43919</v>
       </c>
@@ -3291,7 +3387,7 @@
         <v>1417</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>43920</v>
       </c>
@@ -3341,7 +3437,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>43921</v>
       </c>
@@ -3391,7 +3487,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>43922</v>
       </c>
@@ -3441,7 +3537,7 @@
         <v>2310</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>43923</v>
       </c>
@@ -3491,7 +3587,7 @@
         <v>2602</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>43924</v>
       </c>
@@ -3541,7 +3637,7 @@
         <v>3001</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>43925</v>
       </c>
@@ -3591,7 +3687,7 @@
         <v>3345</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>43926</v>
       </c>
@@ -3641,7 +3737,7 @@
         <v>3706</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>43927</v>
       </c>
@@ -3691,7 +3787,7 @@
         <v>3961</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>43928</v>
       </c>
@@ -3741,7 +3837,7 @@
         <v>4229</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>43929</v>
       </c>
@@ -3791,7 +3887,7 @@
         <v>4565</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>43930</v>
       </c>
@@ -3841,7 +3937,7 @@
         <v>4957</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>43931</v>
       </c>
@@ -3891,7 +3987,7 @@
         <v>5275</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>43932</v>
       </c>
@@ -3941,7 +4037,7 @@
         <v>5590</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>43933</v>
       </c>
@@ -3991,7 +4087,7 @@
         <v>5912</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>43934</v>
       </c>
@@ -4041,7 +4137,7 @@
         <v>6067</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>43935</v>
       </c>
@@ -4091,7 +4187,7 @@
         <v>6358</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>43936</v>
       </c>
@@ -4141,7 +4237,7 @@
         <v>6748</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>43937</v>
       </c>
@@ -4191,7 +4287,7 @@
         <v>7102</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>43938</v>
       </c>
@@ -4241,7 +4337,7 @@
         <v>7409</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>43939</v>
       </c>
@@ -4291,7 +4387,7 @@
         <v>7820</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>43940</v>
       </c>
@@ -4341,7 +4437,7 @@
         <v>8187</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>43941</v>
       </c>
@@ -4391,7 +4487,7 @@
         <v>8450</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>43942</v>
       </c>
@@ -4441,7 +4537,7 @@
         <v>8672</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>43943</v>
       </c>
@@ -4491,7 +4587,7 @@
         <v>9038</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>43944</v>
       </c>
@@ -4541,7 +4637,7 @@
         <v>9409</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>43945</v>
       </c>
@@ -4591,7 +4687,7 @@
         <v>9697</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>43946</v>
       </c>
@@ -4641,7 +4737,7 @@
         <v>10051</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>43947</v>
       </c>
@@ -4692,7 +4788,7 @@
       </c>
       <c r="R54" s="38"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>43948</v>
       </c>
@@ -4743,7 +4839,7 @@
       </c>
       <c r="R55" s="38"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>43949</v>
       </c>
@@ -4794,7 +4890,7 @@
       </c>
       <c r="R56" s="39"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>43950</v>
       </c>
@@ -4844,7 +4940,7 @@
         <v>11034</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>43951</v>
       </c>
@@ -4895,7 +4991,7 @@
       </c>
       <c r="R58" s="38"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>43952</v>
       </c>
@@ -4947,7 +5043,7 @@
       <c r="R59" s="38"/>
       <c r="S59" s="38"/>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>43953</v>
       </c>
@@ -4997,7 +5093,7 @@
         <v>11927</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>43954</v>
       </c>
@@ -5047,7 +5143,7 @@
         <v>12097</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>43955</v>
       </c>
@@ -5097,7 +5193,7 @@
         <v>12266</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
         <v>43956</v>
       </c>
@@ -5147,7 +5243,7 @@
         <v>12437</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
         <v>43957</v>
       </c>
@@ -5197,7 +5293,7 @@
         <v>12709</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
         <v>43958</v>
       </c>
@@ -5247,7 +5343,7 @@
         <v>12924</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
         <v>43959</v>
       </c>
@@ -5297,7 +5393,7 @@
         <v>13149</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
         <v>43960</v>
       </c>
@@ -5347,7 +5443,7 @@
         <v>13305</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
         <v>43961</v>
       </c>
@@ -5397,7 +5493,7 @@
         <v>13486</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
         <v>43962</v>
       </c>
@@ -5447,7 +5543,7 @@
         <v>13627</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>43963</v>
       </c>
@@ -5497,7 +5593,7 @@
         <v>13763</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
         <v>43964</v>
       </c>
@@ -5547,7 +5643,7 @@
         <v>13929</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <v>43965</v>
       </c>
@@ -5597,7 +5693,7 @@
         <v>14117</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
         <v>43966</v>
       </c>
@@ -5647,7 +5743,7 @@
         <v>14260</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <v>43967</v>
       </c>
@@ -5697,7 +5793,7 @@
         <v>14447</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
         <v>43968</v>
       </c>
@@ -5747,7 +5843,7 @@
         <v>14537</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
         <v>43969</v>
       </c>
@@ -5797,7 +5893,7 @@
         <v>14594</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" s="5">
         <v>43970</v>
       </c>
@@ -5847,7 +5943,7 @@
         <v>14655</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
         <v>43971</v>
       </c>
@@ -5897,7 +5993,7 @@
         <v>14751</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" s="5">
         <v>43972</v>
       </c>
@@ -5947,7 +6043,7 @@
         <v>14856</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
         <v>43973</v>
       </c>
@@ -5997,7 +6093,7 @@
         <v>14969</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
         <v>43974</v>
       </c>
@@ -6047,7 +6143,7 @@
         <v>15041</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
         <v>43975</v>
       </c>
@@ -6097,7 +6193,7 @@
         <v>15101</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" s="5">
         <v>43976</v>
       </c>
@@ -6147,7 +6243,7 @@
         <v>15156</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" s="5">
         <v>43977</v>
       </c>
@@ -6197,7 +6293,7 @@
         <v>15185</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" s="5">
         <v>43978</v>
       </c>
@@ -6247,7 +6343,7 @@
         <v>15240</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" s="5">
         <v>43979</v>
       </c>
@@ -6297,7 +6393,7 @@
         <v>15288</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" s="5">
         <v>43980</v>
       </c>
@@ -6347,7 +6443,7 @@
         <v>15327</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" s="5">
         <v>43981</v>
       </c>
@@ -6397,7 +6493,7 @@
         <v>15382</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" s="5">
         <v>43982</v>
       </c>
@@ -6447,7 +6543,7 @@
         <v>15400</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" s="5">
         <v>43983</v>
       </c>
@@ -6497,7 +6593,7 @@
         <v>15418</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" s="5">
         <v>43984</v>
       </c>
@@ -6547,7 +6643,7 @@
         <v>15471</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
         <v>43985</v>
       </c>
@@ -6597,7 +6693,7 @@
         <v>15504</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" s="5">
         <v>43986</v>
       </c>
@@ -6647,7 +6743,7 @@
         <v>15553</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
         <v>43987</v>
       </c>
@@ -6697,7 +6793,7 @@
         <v>15582</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" s="5">
         <v>43988</v>
       </c>
@@ -6747,7 +6843,7 @@
         <v>15603</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" s="5">
         <v>43989</v>
       </c>
@@ -6797,7 +6893,7 @@
         <v>15621</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" s="5">
         <v>43990</v>
       </c>
@@ -6847,7 +6943,7 @@
         <v>15639</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" s="5">
         <v>43991</v>
       </c>
@@ -6897,7 +6993,7 @@
         <v>15653</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" s="5">
         <v>43992</v>
       </c>
@@ -6947,7 +7043,7 @@
         <v>15665</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100" s="5">
         <v>43993</v>
       </c>
@@ -6997,7 +7093,7 @@
         <v>15682</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" s="5">
         <v>43994</v>
       </c>
@@ -7047,7 +7143,7 @@
         <v>15709</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" s="5">
         <v>43995</v>
       </c>
@@ -7097,7 +7193,7 @@
         <v>15730</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103" s="5">
         <v>43996</v>
       </c>
@@ -7147,7 +7243,8 @@
         <v>15755</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:16" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="5"/>
       <c r="C104" s="28"/>
       <c r="D104" s="28"/>
       <c r="E104" s="28"/>
@@ -7161,9 +7258,11 @@
       <c r="M104" s="28"/>
       <c r="N104" s="28"/>
       <c r="O104" s="28"/>
-      <c r="P104" s="28"/>
-    </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P104" s="32">
+        <v>18030</v>
+      </c>
+    </row>
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C105" s="28"/>
       <c r="D105" s="28"/>
       <c r="E105" s="28"/>
@@ -7179,7 +7278,7 @@
       <c r="O105" s="28"/>
       <c r="P105" s="28"/>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C106" s="28"/>
       <c r="D106" s="28"/>
       <c r="E106" s="28"/>
@@ -7195,7 +7294,7 @@
       <c r="O106" s="28"/>
       <c r="P106" s="28"/>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C107" s="28"/>
       <c r="D107" s="28"/>
       <c r="E107" s="28"/>
@@ -7211,7 +7310,7 @@
       <c r="O107" s="28"/>
       <c r="P107" s="28"/>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C108" s="28"/>
       <c r="D108" s="28"/>
       <c r="E108" s="28"/>
@@ -7227,7 +7326,7 @@
       <c r="O108" s="28"/>
       <c r="P108" s="28"/>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C109" s="28"/>
       <c r="D109" s="28"/>
       <c r="E109" s="28"/>
@@ -7243,7 +7342,7 @@
       <c r="O109" s="28"/>
       <c r="P109" s="28"/>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C110" s="28"/>
       <c r="D110" s="28"/>
       <c r="E110" s="28"/>
@@ -7259,7 +7358,7 @@
       <c r="O110" s="28"/>
       <c r="P110" s="28"/>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C111" s="28"/>
       <c r="D111" s="28"/>
       <c r="E111" s="28"/>
@@ -7275,7 +7374,7 @@
       <c r="O111" s="28"/>
       <c r="P111" s="28"/>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C112" s="28"/>
       <c r="D112" s="28"/>
       <c r="E112" s="28"/>
@@ -7291,7 +7390,7 @@
       <c r="O112" s="28"/>
       <c r="P112" s="28"/>
     </row>
-    <row r="113" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C113" s="28"/>
       <c r="D113" s="28"/>
       <c r="E113" s="28"/>
@@ -7307,7 +7406,7 @@
       <c r="O113" s="28"/>
       <c r="P113" s="28"/>
     </row>
-    <row r="114" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C114" s="28"/>
       <c r="D114" s="28"/>
       <c r="E114" s="28"/>
@@ -7323,7 +7422,7 @@
       <c r="O114" s="28"/>
       <c r="P114" s="28"/>
     </row>
-    <row r="115" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B115" s="28"/>
       <c r="C115" s="28"/>
       <c r="D115" s="28"/>
@@ -7340,7 +7439,7 @@
       <c r="O115" s="28"/>
       <c r="P115" s="28"/>
     </row>
-    <row r="116" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B116" s="28"/>
       <c r="C116" s="28"/>
       <c r="D116" s="28"/>
@@ -7357,7 +7456,7 @@
       <c r="O116" s="28"/>
       <c r="P116" s="28"/>
     </row>
-    <row r="117" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B117" s="28"/>
       <c r="C117" s="28"/>
       <c r="D117" s="28"/>
@@ -7374,7 +7473,7 @@
       <c r="O117" s="28"/>
       <c r="P117" s="28"/>
     </row>
-    <row r="118" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B118" s="28"/>
       <c r="C118" s="28"/>
       <c r="D118" s="28"/>
@@ -7391,7 +7490,7 @@
       <c r="O118" s="28"/>
       <c r="P118" s="28"/>
     </row>
-    <row r="119" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B119" s="28"/>
       <c r="C119" s="28"/>
       <c r="D119" s="28"/>
@@ -7408,7 +7507,7 @@
       <c r="O119" s="28"/>
       <c r="P119" s="28"/>
     </row>
-    <row r="120" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B120" s="28"/>
       <c r="C120" s="28"/>
       <c r="D120" s="28"/>
@@ -7425,7 +7524,7 @@
       <c r="O120" s="28"/>
       <c r="P120" s="28"/>
     </row>
-    <row r="121" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B121" s="28"/>
       <c r="C121" s="28"/>
       <c r="D121" s="28"/>
@@ -7442,7 +7541,7 @@
       <c r="O121" s="28"/>
       <c r="P121" s="28"/>
     </row>
-    <row r="122" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B122" s="28"/>
       <c r="C122" s="28"/>
       <c r="D122" s="28"/>
@@ -7459,7 +7558,7 @@
       <c r="O122" s="28"/>
       <c r="P122" s="28"/>
     </row>
-    <row r="123" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B123" s="28"/>
       <c r="C123" s="28"/>
       <c r="D123" s="28"/>
@@ -7476,7 +7575,7 @@
       <c r="O123" s="28"/>
       <c r="P123" s="28"/>
     </row>
-    <row r="124" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B124" s="28"/>
       <c r="C124" s="28"/>
       <c r="D124" s="28"/>
@@ -7493,7 +7592,7 @@
       <c r="O124" s="28"/>
       <c r="P124" s="28"/>
     </row>
-    <row r="125" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B125" s="28"/>
       <c r="C125" s="28"/>
       <c r="D125" s="28"/>
@@ -7510,7 +7609,7 @@
       <c r="O125" s="28"/>
       <c r="P125" s="28"/>
     </row>
-    <row r="126" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B126" s="28"/>
       <c r="C126" s="28"/>
       <c r="D126" s="28"/>
@@ -7527,7 +7626,7 @@
       <c r="O126" s="28"/>
       <c r="P126" s="28"/>
     </row>
-    <row r="127" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B127" s="28"/>
       <c r="C127" s="28"/>
       <c r="D127" s="28"/>
@@ -7544,7 +7643,7 @@
       <c r="O127" s="28"/>
       <c r="P127" s="28"/>
     </row>
-    <row r="128" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B128" s="28"/>
       <c r="C128" s="28"/>
       <c r="D128" s="28"/>
@@ -7561,7 +7660,7 @@
       <c r="O128" s="28"/>
       <c r="P128" s="28"/>
     </row>
-    <row r="129" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B129" s="28"/>
       <c r="C129" s="28"/>
       <c r="D129" s="28"/>
@@ -7578,7 +7677,7 @@
       <c r="O129" s="28"/>
       <c r="P129" s="28"/>
     </row>
-    <row r="130" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B130" s="28"/>
       <c r="C130" s="28"/>
       <c r="D130" s="28"/>
@@ -7595,7 +7694,7 @@
       <c r="O130" s="28"/>
       <c r="P130" s="28"/>
     </row>
-    <row r="131" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B131" s="28"/>
       <c r="C131" s="28"/>
       <c r="D131" s="28"/>
@@ -7612,7 +7711,7 @@
       <c r="O131" s="28"/>
       <c r="P131" s="28"/>
     </row>
-    <row r="132" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B132" s="28"/>
       <c r="C132" s="28"/>
       <c r="D132" s="28"/>
@@ -7629,7 +7728,7 @@
       <c r="O132" s="28"/>
       <c r="P132" s="28"/>
     </row>
-    <row r="133" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B133" s="28"/>
       <c r="C133" s="28"/>
       <c r="D133" s="28"/>
@@ -7646,7 +7745,7 @@
       <c r="O133" s="28"/>
       <c r="P133" s="28"/>
     </row>
-    <row r="134" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B134" s="28"/>
       <c r="C134" s="28"/>
       <c r="D134" s="28"/>
@@ -7663,7 +7762,7 @@
       <c r="O134" s="28"/>
       <c r="P134" s="28"/>
     </row>
-    <row r="135" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B135" s="28"/>
       <c r="C135" s="28"/>
       <c r="D135" s="28"/>
@@ -7680,7 +7779,7 @@
       <c r="O135" s="28"/>
       <c r="P135" s="28"/>
     </row>
-    <row r="136" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B136" s="28"/>
       <c r="C136" s="28"/>
       <c r="D136" s="28"/>
@@ -7697,7 +7796,7 @@
       <c r="O136" s="28"/>
       <c r="P136" s="28"/>
     </row>
-    <row r="137" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B137" s="28"/>
       <c r="C137" s="28"/>
       <c r="D137" s="28"/>
@@ -7714,7 +7813,7 @@
       <c r="O137" s="28"/>
       <c r="P137" s="28"/>
     </row>
-    <row r="138" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B138" s="28"/>
       <c r="C138" s="28"/>
       <c r="D138" s="28"/>
@@ -7731,7 +7830,7 @@
       <c r="O138" s="28"/>
       <c r="P138" s="28"/>
     </row>
-    <row r="139" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B139" s="28"/>
       <c r="C139" s="28"/>
       <c r="D139" s="28"/>
@@ -7748,7 +7847,7 @@
       <c r="O139" s="28"/>
       <c r="P139" s="28"/>
     </row>
-    <row r="140" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B140" s="28"/>
       <c r="C140" s="28"/>
       <c r="D140" s="28"/>
@@ -7765,7 +7864,7 @@
       <c r="O140" s="28"/>
       <c r="P140" s="28"/>
     </row>
-    <row r="141" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B141" s="28"/>
       <c r="C141" s="28"/>
       <c r="D141" s="28"/>
@@ -7782,7 +7881,7 @@
       <c r="O141" s="28"/>
       <c r="P141" s="28"/>
     </row>
-    <row r="142" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B142" s="28"/>
       <c r="C142" s="28"/>
       <c r="D142" s="28"/>
@@ -7799,7 +7898,7 @@
       <c r="O142" s="28"/>
       <c r="P142" s="28"/>
     </row>
-    <row r="143" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B143" s="28"/>
       <c r="C143" s="28"/>
       <c r="D143" s="28"/>
@@ -7816,7 +7915,7 @@
       <c r="O143" s="28"/>
       <c r="P143" s="28"/>
     </row>
-    <row r="144" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B144" s="28"/>
       <c r="C144" s="28"/>
       <c r="D144" s="28"/>
@@ -7833,7 +7932,7 @@
       <c r="O144" s="28"/>
       <c r="P144" s="28"/>
     </row>
-    <row r="145" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B145" s="28"/>
       <c r="C145" s="28"/>
       <c r="D145" s="28"/>
@@ -7850,7 +7949,7 @@
       <c r="O145" s="28"/>
       <c r="P145" s="28"/>
     </row>
-    <row r="146" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B146" s="28"/>
       <c r="C146" s="28"/>
       <c r="D146" s="28"/>
@@ -7867,7 +7966,7 @@
       <c r="O146" s="28"/>
       <c r="P146" s="28"/>
     </row>
-    <row r="147" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B147" s="28"/>
       <c r="C147" s="28"/>
       <c r="D147" s="28"/>
@@ -7884,7 +7983,7 @@
       <c r="O147" s="28"/>
       <c r="P147" s="28"/>
     </row>
-    <row r="148" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B148" s="28"/>
       <c r="C148" s="28"/>
       <c r="D148" s="28"/>
@@ -7901,7 +8000,7 @@
       <c r="O148" s="28"/>
       <c r="P148" s="28"/>
     </row>
-    <row r="149" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B149" s="28"/>
       <c r="C149" s="28"/>
       <c r="D149" s="28"/>
@@ -7918,7 +8017,7 @@
       <c r="O149" s="28"/>
       <c r="P149" s="28"/>
     </row>
-    <row r="150" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B150" s="28"/>
       <c r="C150" s="28"/>
       <c r="D150" s="28"/>
@@ -7935,7 +8034,7 @@
       <c r="O150" s="28"/>
       <c r="P150" s="28"/>
     </row>
-    <row r="151" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B151" s="28"/>
       <c r="C151" s="28"/>
       <c r="D151" s="28"/>
@@ -7952,7 +8051,7 @@
       <c r="O151" s="28"/>
       <c r="P151" s="28"/>
     </row>
-    <row r="152" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B152" s="28"/>
       <c r="C152" s="28"/>
       <c r="D152" s="28"/>
@@ -7969,7 +8068,7 @@
       <c r="O152" s="28"/>
       <c r="P152" s="28"/>
     </row>
-    <row r="153" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B153" s="28"/>
       <c r="C153" s="28"/>
       <c r="D153" s="28"/>
@@ -7986,7 +8085,7 @@
       <c r="O153" s="28"/>
       <c r="P153" s="28"/>
     </row>
-    <row r="154" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B154" s="28"/>
       <c r="C154" s="28"/>
       <c r="D154" s="28"/>
@@ -8003,7 +8102,7 @@
       <c r="O154" s="28"/>
       <c r="P154" s="28"/>
     </row>
-    <row r="155" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B155" s="28"/>
       <c r="C155" s="28"/>
       <c r="D155" s="28"/>
@@ -8020,7 +8119,7 @@
       <c r="O155" s="28"/>
       <c r="P155" s="28"/>
     </row>
-    <row r="156" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B156" s="28"/>
       <c r="C156" s="28"/>
       <c r="D156" s="28"/>
@@ -8037,7 +8136,7 @@
       <c r="O156" s="28"/>
       <c r="P156" s="28"/>
     </row>
-    <row r="157" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B157" s="28"/>
       <c r="C157" s="28"/>
       <c r="D157" s="28"/>
@@ -8054,7 +8153,7 @@
       <c r="O157" s="28"/>
       <c r="P157" s="28"/>
     </row>
-    <row r="158" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B158" s="28"/>
       <c r="C158" s="28"/>
       <c r="D158" s="28"/>
@@ -8071,7 +8170,7 @@
       <c r="O158" s="28"/>
       <c r="P158" s="28"/>
     </row>
-    <row r="159" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B159" s="28"/>
       <c r="C159" s="28"/>
       <c r="D159" s="28"/>
@@ -8088,7 +8187,7 @@
       <c r="O159" s="28"/>
       <c r="P159" s="28"/>
     </row>
-    <row r="160" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B160" s="28"/>
       <c r="C160" s="28"/>
       <c r="D160" s="28"/>
@@ -8108,26 +8207,27 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q92"/>
+  <dimension ref="A1:Q93"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="E101" sqref="E101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5546875" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5546875" style="2"/>
+    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -8148,7 +8248,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -8169,7 +8269,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -8222,7 +8322,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>43908</v>
       </c>
@@ -8275,7 +8375,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>43909</v>
       </c>
@@ -8328,7 +8428,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>43910</v>
       </c>
@@ -8381,7 +8481,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>43911</v>
       </c>
@@ -8434,7 +8534,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>43912</v>
       </c>
@@ -8487,7 +8587,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>43913</v>
       </c>
@@ -8540,7 +8640,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>43914</v>
       </c>
@@ -8593,7 +8693,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>43915</v>
       </c>
@@ -8646,7 +8746,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>43916</v>
       </c>
@@ -8699,7 +8799,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>43917</v>
       </c>
@@ -8752,7 +8852,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>43918</v>
       </c>
@@ -8805,7 +8905,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>43919</v>
       </c>
@@ -8858,7 +8958,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>43920</v>
       </c>
@@ -8911,7 +9011,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>43921</v>
       </c>
@@ -8964,7 +9064,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>43922</v>
       </c>
@@ -9017,7 +9117,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>43923</v>
       </c>
@@ -9070,7 +9170,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>43924</v>
       </c>
@@ -9123,7 +9223,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>43925</v>
       </c>
@@ -9176,7 +9276,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>43926</v>
       </c>
@@ -9229,7 +9329,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>43927</v>
       </c>
@@ -9282,7 +9382,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>43928</v>
       </c>
@@ -9335,7 +9435,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>43929</v>
       </c>
@@ -9388,7 +9488,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>43930</v>
       </c>
@@ -9441,7 +9541,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>43931</v>
       </c>
@@ -9494,7 +9594,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <v>43932</v>
       </c>
@@ -9547,7 +9647,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <v>43933</v>
       </c>
@@ -9600,7 +9700,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <v>43934</v>
       </c>
@@ -9653,7 +9753,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <v>43935</v>
       </c>
@@ -9706,7 +9806,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>43936</v>
       </c>
@@ -9759,7 +9859,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <v>43937</v>
       </c>
@@ -9812,7 +9912,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <v>43938</v>
       </c>
@@ -9865,7 +9965,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <v>43939</v>
       </c>
@@ -9918,7 +10018,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="30">
         <v>43940</v>
       </c>
@@ -9971,7 +10071,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="30">
         <v>43941</v>
       </c>
@@ -10024,7 +10124,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="30">
         <v>43942</v>
       </c>
@@ -10077,7 +10177,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="30">
         <v>43943</v>
       </c>
@@ -10130,7 +10230,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="30">
         <v>43944</v>
       </c>
@@ -10183,7 +10283,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="30">
         <v>43945</v>
       </c>
@@ -10236,7 +10336,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="30">
         <v>43946</v>
       </c>
@@ -10289,7 +10389,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="30">
         <v>43947</v>
       </c>
@@ -10342,7 +10442,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="30">
         <v>43948</v>
       </c>
@@ -10395,7 +10495,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="30">
         <v>43949</v>
       </c>
@@ -10448,7 +10548,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="30">
         <v>43950</v>
       </c>
@@ -10501,7 +10601,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="30">
         <v>43951</v>
       </c>
@@ -10554,7 +10654,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="30">
         <v>43952</v>
       </c>
@@ -10607,7 +10707,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="30">
         <v>43953</v>
       </c>
@@ -10660,7 +10760,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="30">
         <v>43954</v>
       </c>
@@ -10713,7 +10813,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="30">
         <v>43955</v>
       </c>
@@ -10766,7 +10866,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="30">
         <v>43956</v>
       </c>
@@ -10819,7 +10919,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="30">
         <v>43957</v>
       </c>
@@ -10872,7 +10972,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="30">
         <v>43958</v>
       </c>
@@ -10925,7 +11025,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="30">
         <v>43959</v>
       </c>
@@ -10978,7 +11078,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="30">
         <v>43960</v>
       </c>
@@ -11031,7 +11131,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="30">
         <v>43961</v>
       </c>
@@ -11084,7 +11184,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="30">
         <v>43962</v>
       </c>
@@ -11137,7 +11237,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="30">
         <v>43963</v>
       </c>
@@ -11190,7 +11290,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="30">
         <v>43964</v>
       </c>
@@ -11243,7 +11343,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" s="30">
         <v>43965</v>
       </c>
@@ -11296,7 +11396,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="30">
         <v>43966</v>
       </c>
@@ -11349,7 +11449,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" s="30">
         <v>43967</v>
       </c>
@@ -11402,7 +11502,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" s="30">
         <v>43968</v>
       </c>
@@ -11455,7 +11555,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" s="30">
         <v>43969</v>
       </c>
@@ -11508,7 +11608,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" s="30">
         <v>43970</v>
       </c>
@@ -11561,7 +11661,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" s="30">
         <v>43971</v>
       </c>
@@ -11614,7 +11714,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" s="30">
         <v>43972</v>
       </c>
@@ -11667,7 +11767,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" s="30">
         <v>43973</v>
       </c>
@@ -11720,7 +11820,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" s="30">
         <v>43974</v>
       </c>
@@ -11773,7 +11873,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" s="30">
         <v>43975</v>
       </c>
@@ -11826,7 +11926,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" s="30">
         <v>43976</v>
       </c>
@@ -11879,7 +11979,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" s="30">
         <v>43977</v>
       </c>
@@ -11932,7 +12032,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" s="30">
         <v>43978</v>
       </c>
@@ -11985,7 +12085,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" s="30">
         <v>43979</v>
       </c>
@@ -12038,7 +12138,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" s="30">
         <v>43980</v>
       </c>
@@ -12091,7 +12191,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" s="30">
         <v>43981</v>
       </c>
@@ -12144,7 +12244,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" s="30">
         <v>43982</v>
       </c>
@@ -12197,7 +12297,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" s="30">
         <v>43983</v>
       </c>
@@ -12250,7 +12350,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" s="30">
         <v>43984</v>
       </c>
@@ -12303,7 +12403,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" s="30">
         <v>43985</v>
       </c>
@@ -12356,7 +12456,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" s="30">
         <v>43986</v>
       </c>
@@ -12409,7 +12509,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" s="30">
         <v>43987</v>
       </c>
@@ -12462,7 +12562,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" s="30">
         <v>43988</v>
       </c>
@@ -12515,7 +12615,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85" s="30">
         <v>43989</v>
       </c>
@@ -12568,7 +12668,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86" s="30">
         <v>43990</v>
       </c>
@@ -12621,7 +12721,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" s="30">
         <v>43991</v>
       </c>
@@ -12674,7 +12774,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88" s="30">
         <v>43992</v>
       </c>
@@ -12727,7 +12827,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89" s="30">
         <v>43993</v>
       </c>
@@ -12780,7 +12880,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90" s="30">
         <v>43994</v>
       </c>
@@ -12833,7 +12933,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91" s="30">
         <v>43995</v>
       </c>
@@ -12886,7 +12986,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92" s="30">
         <v>43996</v>
       </c>
@@ -12937,6 +13037,59 @@
       </c>
       <c r="Q92" s="13">
         <v>15</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A93" s="30">
+        <v>43997</v>
+      </c>
+      <c r="B93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G93" s="11">
+        <v>5</v>
+      </c>
+      <c r="H93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="L93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P93" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q93" s="13">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -12947,23 +13100,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R84"/>
+  <dimension ref="A1:R85"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="P94" sqref="P94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5546875" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5546875" style="2"/>
+    <col min="1" max="1" width="15.42578125" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -12984,7 +13137,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -13005,7 +13158,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -13058,7 +13211,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>43916</v>
       </c>
@@ -13111,7 +13264,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>43917</v>
       </c>
@@ -13164,7 +13317,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>43918</v>
       </c>
@@ -13217,7 +13370,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>43919</v>
       </c>
@@ -13270,7 +13423,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>43920</v>
       </c>
@@ -13323,7 +13476,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>43921</v>
       </c>
@@ -13376,7 +13529,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>43922</v>
       </c>
@@ -13429,7 +13582,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>43923</v>
       </c>
@@ -13482,7 +13635,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>43924</v>
       </c>
@@ -13535,7 +13688,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>43925</v>
       </c>
@@ -13588,7 +13741,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>43926</v>
       </c>
@@ -13641,7 +13794,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>43927</v>
       </c>
@@ -13694,7 +13847,7 @@
         <v>1262</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>43928</v>
       </c>
@@ -13747,7 +13900,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>43929</v>
       </c>
@@ -13800,7 +13953,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>43930</v>
       </c>
@@ -13853,7 +14006,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>43931</v>
       </c>
@@ -13906,7 +14059,7 @@
         <v>1461</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>43932</v>
       </c>
@@ -13959,7 +14112,7 @@
         <v>1467</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>43933</v>
       </c>
@@ -14012,7 +14165,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>43934</v>
       </c>
@@ -14065,7 +14218,7 @@
         <v>1482</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>43935</v>
       </c>
@@ -14118,7 +14271,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>43936</v>
       </c>
@@ -14171,7 +14324,7 @@
         <v>1486</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>43937</v>
       </c>
@@ -14224,7 +14377,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>43938</v>
       </c>
@@ -14277,7 +14430,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>43939</v>
       </c>
@@ -14330,7 +14483,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <v>43940</v>
       </c>
@@ -14383,7 +14536,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <v>43941</v>
       </c>
@@ -14436,7 +14589,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <v>43942</v>
       </c>
@@ -14489,7 +14642,7 @@
         <v>1472</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <v>43943</v>
       </c>
@@ -14542,7 +14695,7 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>43944</v>
       </c>
@@ -14595,7 +14748,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <v>43945</v>
       </c>
@@ -14648,7 +14801,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <v>43946</v>
       </c>
@@ -14701,7 +14854,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <v>43947</v>
       </c>
@@ -14754,7 +14907,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="30">
         <v>43948</v>
       </c>
@@ -14807,7 +14960,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="30">
         <v>43949</v>
       </c>
@@ -14860,7 +15013,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="30">
         <v>43950</v>
       </c>
@@ -14913,7 +15066,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="30">
         <v>43951</v>
       </c>
@@ -14966,7 +15119,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="30">
         <v>43952</v>
       </c>
@@ -15019,7 +15172,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="30">
         <v>43953</v>
       </c>
@@ -15072,7 +15225,7 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="30">
         <v>43954</v>
       </c>
@@ -15125,7 +15278,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="30">
         <v>43955</v>
       </c>
@@ -15178,7 +15331,7 @@
         <v>1279</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="30">
         <v>43956</v>
       </c>
@@ -15231,7 +15384,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="30">
         <v>43957</v>
       </c>
@@ -15284,7 +15437,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="30">
         <v>43958</v>
       </c>
@@ -15337,7 +15490,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="30">
         <v>43959</v>
       </c>
@@ -15390,7 +15543,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="30">
         <v>43960</v>
       </c>
@@ -15443,7 +15596,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="30">
         <v>43961</v>
       </c>
@@ -15496,7 +15649,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="30">
         <v>43962</v>
       </c>
@@ -15549,7 +15702,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="30">
         <v>43963</v>
       </c>
@@ -15602,7 +15755,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="30">
         <v>43964</v>
       </c>
@@ -15655,7 +15808,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="30">
         <v>43965</v>
       </c>
@@ -15708,7 +15861,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="30">
         <v>43966</v>
       </c>
@@ -15761,7 +15914,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="30">
         <v>43967</v>
       </c>
@@ -15814,7 +15967,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="30">
         <v>43968</v>
       </c>
@@ -15867,7 +16020,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="30">
         <v>43969</v>
       </c>
@@ -15920,7 +16073,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="30">
         <v>43970</v>
       </c>
@@ -15973,7 +16126,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="30">
         <v>43971</v>
       </c>
@@ -16026,7 +16179,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="30">
         <v>43972</v>
       </c>
@@ -16079,7 +16232,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" s="30">
         <v>43973</v>
       </c>
@@ -16132,7 +16285,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="30">
         <v>43974</v>
       </c>
@@ -16185,7 +16338,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" s="30">
         <v>43975</v>
       </c>
@@ -16238,7 +16391,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" s="30">
         <v>43976</v>
       </c>
@@ -16291,7 +16444,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" s="51">
         <v>43977</v>
       </c>
@@ -16344,7 +16497,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" s="51">
         <v>43978</v>
       </c>
@@ -16397,7 +16550,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="51">
         <v>43979</v>
       </c>
@@ -16450,7 +16603,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="51">
         <v>43980</v>
       </c>
@@ -16503,7 +16656,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" s="51">
         <v>43981</v>
       </c>
@@ -16556,7 +16709,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" s="51">
         <v>43982</v>
       </c>
@@ -16609,7 +16762,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" s="51">
         <v>43983</v>
       </c>
@@ -16662,7 +16815,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72" s="51">
         <v>43984</v>
       </c>
@@ -16715,7 +16868,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" s="51">
         <v>43985</v>
       </c>
@@ -16768,7 +16921,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" s="51">
         <v>43986</v>
       </c>
@@ -16821,7 +16974,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75" s="51">
         <v>43987</v>
       </c>
@@ -16874,7 +17027,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" s="51">
         <v>43988</v>
       </c>
@@ -16927,7 +17080,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" s="51">
         <v>43989</v>
       </c>
@@ -16980,7 +17133,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" s="51">
         <v>43990</v>
       </c>
@@ -17033,7 +17186,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79" s="51">
         <v>43991</v>
       </c>
@@ -17086,7 +17239,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A80" s="51">
         <v>43992</v>
       </c>
@@ -17140,7 +17293,7 @@
       </c>
       <c r="R80" s="54"/>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" s="51">
         <v>43993</v>
       </c>
@@ -17194,7 +17347,7 @@
       </c>
       <c r="R81" s="54"/>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" s="51">
         <v>43994</v>
       </c>
@@ -17248,7 +17401,7 @@
       </c>
       <c r="R82" s="54"/>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" s="51">
         <v>43995</v>
       </c>
@@ -17301,7 +17454,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" s="51">
         <v>43996</v>
       </c>
@@ -17352,6 +17505,59 @@
       </c>
       <c r="Q84" s="13">
         <v>575</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A85" s="51">
+        <v>43997</v>
+      </c>
+      <c r="B85" s="11">
+        <v>5</v>
+      </c>
+      <c r="C85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E85" s="11">
+        <v>56</v>
+      </c>
+      <c r="F85" s="11">
+        <v>6</v>
+      </c>
+      <c r="G85" s="11">
+        <v>56</v>
+      </c>
+      <c r="H85" s="11">
+        <v>262</v>
+      </c>
+      <c r="I85" s="11">
+        <v>7</v>
+      </c>
+      <c r="J85" s="11">
+        <v>49</v>
+      </c>
+      <c r="K85" s="11">
+        <v>131</v>
+      </c>
+      <c r="L85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N85" s="11">
+        <v>5</v>
+      </c>
+      <c r="O85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q85" s="13">
+        <v>578</v>
       </c>
     </row>
   </sheetData>
@@ -17362,23 +17568,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q84"/>
+  <dimension ref="A1:Q85"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="O87" sqref="O87"/>
+      <selection pane="bottomRight" activeCell="R96" sqref="R96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5546875" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5546875" style="2"/>
+    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -17399,7 +17605,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -17420,7 +17626,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -17473,7 +17679,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>43916</v>
       </c>
@@ -17526,7 +17732,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>43917</v>
       </c>
@@ -17579,7 +17785,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>43918</v>
       </c>
@@ -17632,7 +17838,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>43919</v>
       </c>
@@ -17685,7 +17891,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>43920</v>
       </c>
@@ -17738,7 +17944,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>43921</v>
       </c>
@@ -17791,7 +17997,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>43922</v>
       </c>
@@ -17844,7 +18050,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>43923</v>
       </c>
@@ -17897,7 +18103,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>43924</v>
       </c>
@@ -17950,7 +18156,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>43925</v>
       </c>
@@ -18003,7 +18209,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>43926</v>
       </c>
@@ -18056,7 +18262,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>43927</v>
       </c>
@@ -18109,7 +18315,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>43928</v>
       </c>
@@ -18162,7 +18368,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>43929</v>
       </c>
@@ -18215,7 +18421,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>43930</v>
       </c>
@@ -18268,7 +18474,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>43931</v>
       </c>
@@ -18321,7 +18527,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>43932</v>
       </c>
@@ -18374,7 +18580,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>43933</v>
       </c>
@@ -18427,7 +18633,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>43934</v>
       </c>
@@ -18480,7 +18686,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>43935</v>
       </c>
@@ -18533,7 +18739,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>43936</v>
       </c>
@@ -18586,7 +18792,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>43937</v>
       </c>
@@ -18639,7 +18845,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>43938</v>
       </c>
@@ -18692,7 +18898,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>43939</v>
       </c>
@@ -18745,7 +18951,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <v>43940</v>
       </c>
@@ -18798,7 +19004,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <v>43941</v>
       </c>
@@ -18851,7 +19057,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <v>43942</v>
       </c>
@@ -18904,7 +19110,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <v>43943</v>
       </c>
@@ -18957,7 +19163,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>43944</v>
       </c>
@@ -19010,7 +19216,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <v>43945</v>
       </c>
@@ -19063,7 +19269,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <v>43946</v>
       </c>
@@ -19116,7 +19322,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <v>43947</v>
       </c>
@@ -19169,7 +19375,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="30">
         <v>43948</v>
       </c>
@@ -19222,7 +19428,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="30">
         <v>43949</v>
       </c>
@@ -19275,7 +19481,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="30">
         <v>43950</v>
       </c>
@@ -19328,7 +19534,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="30">
         <v>43951</v>
       </c>
@@ -19381,7 +19587,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="30">
         <v>43952</v>
       </c>
@@ -19434,7 +19640,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="30">
         <v>43953</v>
       </c>
@@ -19487,7 +19693,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="30">
         <v>43954</v>
       </c>
@@ -19540,7 +19746,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="30">
         <v>43955</v>
       </c>
@@ -19593,7 +19799,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="30">
         <v>43956</v>
       </c>
@@ -19646,7 +19852,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="30">
         <v>43957</v>
       </c>
@@ -19699,7 +19905,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="30">
         <v>43958</v>
       </c>
@@ -19752,7 +19958,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="30">
         <v>43959</v>
       </c>
@@ -19805,7 +20011,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="30">
         <v>43960</v>
       </c>
@@ -19858,7 +20064,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="30">
         <v>43961</v>
       </c>
@@ -19911,7 +20117,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="30">
         <v>43962</v>
       </c>
@@ -19964,7 +20170,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="30">
         <v>43963</v>
       </c>
@@ -20017,7 +20223,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="30">
         <v>43964</v>
       </c>
@@ -20070,7 +20276,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="30">
         <v>43965</v>
       </c>
@@ -20123,7 +20329,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="30">
         <v>43966</v>
       </c>
@@ -20176,7 +20382,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="30">
         <v>43967</v>
       </c>
@@ -20229,7 +20435,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="30">
         <v>43968</v>
       </c>
@@ -20282,7 +20488,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="30">
         <v>43969</v>
       </c>
@@ -20335,7 +20541,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="30">
         <v>43970</v>
       </c>
@@ -20388,7 +20594,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="30">
         <v>43971</v>
       </c>
@@ -20441,7 +20647,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="30">
         <v>43972</v>
       </c>
@@ -20494,7 +20700,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" s="30">
         <v>43973</v>
       </c>
@@ -20547,7 +20753,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="30">
         <v>43974</v>
       </c>
@@ -20600,7 +20806,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" s="30">
         <v>43975</v>
       </c>
@@ -20653,7 +20859,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" s="30">
         <v>43976</v>
       </c>
@@ -20706,7 +20912,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" s="30">
         <v>43977</v>
       </c>
@@ -20759,7 +20965,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" s="30">
         <v>43978</v>
       </c>
@@ -20812,7 +21018,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" s="30">
         <v>43979</v>
       </c>
@@ -20865,7 +21071,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" s="30">
         <v>43980</v>
       </c>
@@ -20918,7 +21124,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" s="30">
         <v>43981</v>
       </c>
@@ -20971,7 +21177,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" s="30">
         <v>43982</v>
       </c>
@@ -21024,7 +21230,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" s="30">
         <v>43983</v>
       </c>
@@ -21077,7 +21283,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" s="30">
         <v>43984</v>
       </c>
@@ -21130,7 +21336,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" s="30">
         <v>43985</v>
       </c>
@@ -21183,7 +21389,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" s="30">
         <v>43986</v>
       </c>
@@ -21236,7 +21442,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" s="30">
         <v>43987</v>
       </c>
@@ -21289,7 +21495,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" s="30">
         <v>43988</v>
       </c>
@@ -21342,7 +21548,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" s="30">
         <v>43989</v>
       </c>
@@ -21395,7 +21601,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" s="30">
         <v>43990</v>
       </c>
@@ -21448,7 +21654,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" s="30">
         <v>43991</v>
       </c>
@@ -21501,7 +21707,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" s="30">
         <v>43992</v>
       </c>
@@ -21554,7 +21760,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" s="30">
         <v>43993</v>
       </c>
@@ -21607,7 +21813,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" s="30">
         <v>43994</v>
       </c>
@@ -21660,7 +21866,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" s="30">
         <v>43995</v>
       </c>
@@ -21713,7 +21919,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" s="30">
         <v>43996</v>
       </c>
@@ -21764,6 +21970,59 @@
       </c>
       <c r="Q84" s="13">
         <v>389</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A85" s="30">
+        <v>43997</v>
+      </c>
+      <c r="B85" s="11">
+        <v>11</v>
+      </c>
+      <c r="C85" s="11">
+        <v>22</v>
+      </c>
+      <c r="D85" s="11">
+        <v>8</v>
+      </c>
+      <c r="E85" s="11">
+        <v>19</v>
+      </c>
+      <c r="F85" s="11">
+        <v>38</v>
+      </c>
+      <c r="G85" s="11">
+        <v>11</v>
+      </c>
+      <c r="H85" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I85" s="11">
+        <v>12</v>
+      </c>
+      <c r="J85" s="11">
+        <v>52</v>
+      </c>
+      <c r="K85" s="11">
+        <v>109</v>
+      </c>
+      <c r="L85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N85" s="11">
+        <v>8</v>
+      </c>
+      <c r="O85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q85" s="13">
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -21771,7 +22030,7 @@
 </worksheet>
 </file>
 
-<file path=customXML/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA" version="1.0.0">
   <systemFields>
     <field name="Objective-Id">
@@ -21796,7 +22055,7 @@
       <value order="0"/>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-14T11:47:42Z</value>
+      <value order="0">2020-06-15T12:45:35Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -21808,16 +22067,16 @@
       <value order="0">Analytical: COVID 19 Analysis: Restricted working papers: Research and analysis: Diseases: 2020-2025</value>
     </field>
     <field name="Objective-State">
-      <value order="0">Being Drafted</value>
+      <value order="0">Being Edited</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41732238</value>
+      <value order="0">vA41747896</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">25.3</value>
+      <value order="0">25.8</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">178</value>
+      <value order="0">183</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>
@@ -21854,7 +22113,7 @@
 </metadata>
 </file>
 
-<file path=customXML/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5745109E-2DDF-40CB-AC2B-FF9B10C90820}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-15 20:09) (#131)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U445783\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA18464\A28088333\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u201433\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA1432\A28088333\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5988" windowHeight="6048" tabRatio="803" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5985" windowHeight="6045" tabRatio="803"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1858" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1883" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -659,7 +659,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>1. The data in Table 1 shows the cumulative number of people tested positive for COVID-19 across Scotland to date, broken down by board. </a:t>
+            <a:t>1. The data in Table 1 shows the cumulative number of people tested positive for COVID-19 across Scotland to date, broken down by board.  </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -698,7 +698,25 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>2. Results reported each day refer to the number of positive tests in the Health Protection Scotland ECOSS system reported to HPS by the laboratories in the 24 hours from 08:00 to 08:00. Therefore, the number of positive tests reported each day refers to the number of individuals with a positive result</a:t>
+            <a:t>2. Up</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> until 14 June, r</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>esults reported each day refer to the number of positive tests in the Health Protection Scotland ECOSS system reported to HPS by the laboratories in the 24 hours from 08:00 to 08:00. Therefore, the number of positive tests reported each day refers to the number of individuals with a positive result</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" baseline="0">
@@ -725,7 +743,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>he daily total of people found positive on 2/6/20 contains 40 historic samples from an NHS Fife laboratory.</a:t>
+            <a:t>he daily total of people found positive on 2/6/20 contains 40 historic samples from an NHS Fife laboratory. From 15 June the figures will also include people tested through the UK Government's testing programme including drive through, mobile testing units and home tests. There will be a delay to publishing these but a board table is expected to be available on or before 18 June.</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB">
             <a:effectLst/>
@@ -1662,6 +1680,86 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>771072</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>163284</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5143500" cy="1097643"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12709072" y="19122570"/>
+          <a:ext cx="5143500" cy="1097643"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>As of 15 June, this includes confirmed cases at UK Government Regional Testing Centres (RTCs). </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>A breakdown by NHS Board is not yet available from UK Gov RTCs for 15 June. This table will be updated by 18 June.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1927,25 +2025,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.44140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="90.44140625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.44140625" style="2"/>
+    <col min="2" max="2" width="29.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="90.42578125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>20</v>
       </c>
@@ -1953,7 +2049,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
         <v>22</v>
       </c>
@@ -1961,13 +2057,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="22" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="23"/>
     </row>
-    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="24" t="s">
         <v>26</v>
       </c>
@@ -1975,7 +2071,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="24" t="s">
         <v>27</v>
       </c>
@@ -1983,7 +2079,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="24" t="s">
         <v>36</v>
       </c>
@@ -1991,7 +2087,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
         <v>37</v>
       </c>
@@ -2019,12 +2115,12 @@
       <selection activeCell="O52" sqref="O52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.44140625" style="2"/>
+    <col min="1" max="16384" width="9.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="44" spans="1:1" ht="15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="43"/>
     </row>
   </sheetData>
@@ -2038,21 +2134,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S160"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B85" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B82" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H93" sqref="H93"/>
+      <selection pane="bottomRight" activeCell="R110" sqref="R110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" style="2" customWidth="1"/>
-    <col min="2" max="16" width="11.44140625" style="11" customWidth="1"/>
-    <col min="17" max="16384" width="8.5546875" style="2"/>
+    <col min="2" max="16" width="11.42578125" style="11" customWidth="1"/>
+    <col min="17" max="16384" width="8.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -2072,7 +2168,7 @@
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -2091,7 +2187,7 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -2141,7 +2237,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>43897</v>
       </c>
@@ -2191,7 +2287,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>43898</v>
       </c>
@@ -2241,7 +2337,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>43899</v>
       </c>
@@ -2291,7 +2387,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>43900</v>
       </c>
@@ -2341,7 +2437,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>43901</v>
       </c>
@@ -2391,7 +2487,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>43902</v>
       </c>
@@ -2441,7 +2537,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>43903</v>
       </c>
@@ -2491,7 +2587,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>43904</v>
       </c>
@@ -2541,7 +2637,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>43905</v>
       </c>
@@ -2591,7 +2687,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>43906</v>
       </c>
@@ -2641,7 +2737,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>43907</v>
       </c>
@@ -2691,7 +2787,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>43908</v>
       </c>
@@ -2741,7 +2837,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>43909</v>
       </c>
@@ -2791,7 +2887,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>43910</v>
       </c>
@@ -2841,7 +2937,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>43911</v>
       </c>
@@ -2891,7 +2987,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>43912</v>
       </c>
@@ -2941,7 +3037,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>43913</v>
       </c>
@@ -2991,7 +3087,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>43914</v>
       </c>
@@ -3041,7 +3137,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>43915</v>
       </c>
@@ -3091,7 +3187,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>43916</v>
       </c>
@@ -3141,7 +3237,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>43917</v>
       </c>
@@ -3191,7 +3287,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>43918</v>
       </c>
@@ -3241,7 +3337,7 @@
         <v>1264</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>43919</v>
       </c>
@@ -3291,7 +3387,7 @@
         <v>1417</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>43920</v>
       </c>
@@ -3341,7 +3437,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>43921</v>
       </c>
@@ -3391,7 +3487,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>43922</v>
       </c>
@@ -3441,7 +3537,7 @@
         <v>2310</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>43923</v>
       </c>
@@ -3491,7 +3587,7 @@
         <v>2602</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>43924</v>
       </c>
@@ -3541,7 +3637,7 @@
         <v>3001</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>43925</v>
       </c>
@@ -3591,7 +3687,7 @@
         <v>3345</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>43926</v>
       </c>
@@ -3641,7 +3737,7 @@
         <v>3706</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>43927</v>
       </c>
@@ -3691,7 +3787,7 @@
         <v>3961</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>43928</v>
       </c>
@@ -3741,7 +3837,7 @@
         <v>4229</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>43929</v>
       </c>
@@ -3791,7 +3887,7 @@
         <v>4565</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>43930</v>
       </c>
@@ -3841,7 +3937,7 @@
         <v>4957</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>43931</v>
       </c>
@@ -3891,7 +3987,7 @@
         <v>5275</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>43932</v>
       </c>
@@ -3941,7 +4037,7 @@
         <v>5590</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>43933</v>
       </c>
@@ -3991,7 +4087,7 @@
         <v>5912</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>43934</v>
       </c>
@@ -4041,7 +4137,7 @@
         <v>6067</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>43935</v>
       </c>
@@ -4091,7 +4187,7 @@
         <v>6358</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>43936</v>
       </c>
@@ -4141,7 +4237,7 @@
         <v>6748</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>43937</v>
       </c>
@@ -4191,7 +4287,7 @@
         <v>7102</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>43938</v>
       </c>
@@ -4241,7 +4337,7 @@
         <v>7409</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>43939</v>
       </c>
@@ -4291,7 +4387,7 @@
         <v>7820</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>43940</v>
       </c>
@@ -4341,7 +4437,7 @@
         <v>8187</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>43941</v>
       </c>
@@ -4391,7 +4487,7 @@
         <v>8450</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>43942</v>
       </c>
@@ -4441,7 +4537,7 @@
         <v>8672</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>43943</v>
       </c>
@@ -4491,7 +4587,7 @@
         <v>9038</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>43944</v>
       </c>
@@ -4541,7 +4637,7 @@
         <v>9409</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>43945</v>
       </c>
@@ -4591,7 +4687,7 @@
         <v>9697</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>43946</v>
       </c>
@@ -4641,7 +4737,7 @@
         <v>10051</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>43947</v>
       </c>
@@ -4692,7 +4788,7 @@
       </c>
       <c r="R54" s="38"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>43948</v>
       </c>
@@ -4743,7 +4839,7 @@
       </c>
       <c r="R55" s="38"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>43949</v>
       </c>
@@ -4794,7 +4890,7 @@
       </c>
       <c r="R56" s="39"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>43950</v>
       </c>
@@ -4844,7 +4940,7 @@
         <v>11034</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>43951</v>
       </c>
@@ -4895,7 +4991,7 @@
       </c>
       <c r="R58" s="38"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>43952</v>
       </c>
@@ -4947,7 +5043,7 @@
       <c r="R59" s="38"/>
       <c r="S59" s="38"/>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>43953</v>
       </c>
@@ -4997,7 +5093,7 @@
         <v>11927</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>43954</v>
       </c>
@@ -5047,7 +5143,7 @@
         <v>12097</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>43955</v>
       </c>
@@ -5097,7 +5193,7 @@
         <v>12266</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
         <v>43956</v>
       </c>
@@ -5147,7 +5243,7 @@
         <v>12437</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
         <v>43957</v>
       </c>
@@ -5197,7 +5293,7 @@
         <v>12709</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
         <v>43958</v>
       </c>
@@ -5247,7 +5343,7 @@
         <v>12924</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
         <v>43959</v>
       </c>
@@ -5297,7 +5393,7 @@
         <v>13149</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
         <v>43960</v>
       </c>
@@ -5347,7 +5443,7 @@
         <v>13305</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
         <v>43961</v>
       </c>
@@ -5397,7 +5493,7 @@
         <v>13486</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
         <v>43962</v>
       </c>
@@ -5447,7 +5543,7 @@
         <v>13627</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>43963</v>
       </c>
@@ -5497,7 +5593,7 @@
         <v>13763</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
         <v>43964</v>
       </c>
@@ -5547,7 +5643,7 @@
         <v>13929</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <v>43965</v>
       </c>
@@ -5597,7 +5693,7 @@
         <v>14117</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
         <v>43966</v>
       </c>
@@ -5647,7 +5743,7 @@
         <v>14260</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <v>43967</v>
       </c>
@@ -5697,7 +5793,7 @@
         <v>14447</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
         <v>43968</v>
       </c>
@@ -5747,7 +5843,7 @@
         <v>14537</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
         <v>43969</v>
       </c>
@@ -5797,7 +5893,7 @@
         <v>14594</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" s="5">
         <v>43970</v>
       </c>
@@ -5847,7 +5943,7 @@
         <v>14655</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
         <v>43971</v>
       </c>
@@ -5897,7 +5993,7 @@
         <v>14751</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" s="5">
         <v>43972</v>
       </c>
@@ -5947,7 +6043,7 @@
         <v>14856</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
         <v>43973</v>
       </c>
@@ -5997,7 +6093,7 @@
         <v>14969</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
         <v>43974</v>
       </c>
@@ -6047,7 +6143,7 @@
         <v>15041</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
         <v>43975</v>
       </c>
@@ -6097,7 +6193,7 @@
         <v>15101</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" s="5">
         <v>43976</v>
       </c>
@@ -6147,7 +6243,7 @@
         <v>15156</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" s="5">
         <v>43977</v>
       </c>
@@ -6197,7 +6293,7 @@
         <v>15185</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" s="5">
         <v>43978</v>
       </c>
@@ -6247,7 +6343,7 @@
         <v>15240</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" s="5">
         <v>43979</v>
       </c>
@@ -6297,7 +6393,7 @@
         <v>15288</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" s="5">
         <v>43980</v>
       </c>
@@ -6347,7 +6443,7 @@
         <v>15327</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" s="5">
         <v>43981</v>
       </c>
@@ -6397,7 +6493,7 @@
         <v>15382</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" s="5">
         <v>43982</v>
       </c>
@@ -6447,7 +6543,7 @@
         <v>15400</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" s="5">
         <v>43983</v>
       </c>
@@ -6497,7 +6593,7 @@
         <v>15418</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" s="5">
         <v>43984</v>
       </c>
@@ -6547,7 +6643,7 @@
         <v>15471</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
         <v>43985</v>
       </c>
@@ -6597,7 +6693,7 @@
         <v>15504</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" s="5">
         <v>43986</v>
       </c>
@@ -6647,7 +6743,7 @@
         <v>15553</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
         <v>43987</v>
       </c>
@@ -6697,7 +6793,7 @@
         <v>15582</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" s="5">
         <v>43988</v>
       </c>
@@ -6747,7 +6843,7 @@
         <v>15603</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" s="5">
         <v>43989</v>
       </c>
@@ -6797,7 +6893,7 @@
         <v>15621</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" s="5">
         <v>43990</v>
       </c>
@@ -6847,7 +6943,7 @@
         <v>15639</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" s="5">
         <v>43991</v>
       </c>
@@ -6897,7 +6993,7 @@
         <v>15653</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" s="5">
         <v>43992</v>
       </c>
@@ -6947,7 +7043,7 @@
         <v>15665</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100" s="5">
         <v>43993</v>
       </c>
@@ -6997,7 +7093,7 @@
         <v>15682</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" s="5">
         <v>43994</v>
       </c>
@@ -7047,7 +7143,7 @@
         <v>15709</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" s="5">
         <v>43995</v>
       </c>
@@ -7097,7 +7193,7 @@
         <v>15730</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103" s="5">
         <v>43996</v>
       </c>
@@ -7147,7 +7243,8 @@
         <v>15755</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:16" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="5"/>
       <c r="C104" s="28"/>
       <c r="D104" s="28"/>
       <c r="E104" s="28"/>
@@ -7161,9 +7258,11 @@
       <c r="M104" s="28"/>
       <c r="N104" s="28"/>
       <c r="O104" s="28"/>
-      <c r="P104" s="28"/>
-    </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P104" s="32">
+        <v>18030</v>
+      </c>
+    </row>
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C105" s="28"/>
       <c r="D105" s="28"/>
       <c r="E105" s="28"/>
@@ -7179,7 +7278,7 @@
       <c r="O105" s="28"/>
       <c r="P105" s="28"/>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C106" s="28"/>
       <c r="D106" s="28"/>
       <c r="E106" s="28"/>
@@ -7195,7 +7294,7 @@
       <c r="O106" s="28"/>
       <c r="P106" s="28"/>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C107" s="28"/>
       <c r="D107" s="28"/>
       <c r="E107" s="28"/>
@@ -7211,7 +7310,7 @@
       <c r="O107" s="28"/>
       <c r="P107" s="28"/>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C108" s="28"/>
       <c r="D108" s="28"/>
       <c r="E108" s="28"/>
@@ -7227,7 +7326,7 @@
       <c r="O108" s="28"/>
       <c r="P108" s="28"/>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C109" s="28"/>
       <c r="D109" s="28"/>
       <c r="E109" s="28"/>
@@ -7243,7 +7342,7 @@
       <c r="O109" s="28"/>
       <c r="P109" s="28"/>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C110" s="28"/>
       <c r="D110" s="28"/>
       <c r="E110" s="28"/>
@@ -7259,7 +7358,7 @@
       <c r="O110" s="28"/>
       <c r="P110" s="28"/>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C111" s="28"/>
       <c r="D111" s="28"/>
       <c r="E111" s="28"/>
@@ -7275,7 +7374,7 @@
       <c r="O111" s="28"/>
       <c r="P111" s="28"/>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C112" s="28"/>
       <c r="D112" s="28"/>
       <c r="E112" s="28"/>
@@ -7291,7 +7390,7 @@
       <c r="O112" s="28"/>
       <c r="P112" s="28"/>
     </row>
-    <row r="113" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C113" s="28"/>
       <c r="D113" s="28"/>
       <c r="E113" s="28"/>
@@ -7307,7 +7406,7 @@
       <c r="O113" s="28"/>
       <c r="P113" s="28"/>
     </row>
-    <row r="114" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C114" s="28"/>
       <c r="D114" s="28"/>
       <c r="E114" s="28"/>
@@ -7323,7 +7422,7 @@
       <c r="O114" s="28"/>
       <c r="P114" s="28"/>
     </row>
-    <row r="115" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B115" s="28"/>
       <c r="C115" s="28"/>
       <c r="D115" s="28"/>
@@ -7340,7 +7439,7 @@
       <c r="O115" s="28"/>
       <c r="P115" s="28"/>
     </row>
-    <row r="116" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B116" s="28"/>
       <c r="C116" s="28"/>
       <c r="D116" s="28"/>
@@ -7357,7 +7456,7 @@
       <c r="O116" s="28"/>
       <c r="P116" s="28"/>
     </row>
-    <row r="117" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B117" s="28"/>
       <c r="C117" s="28"/>
       <c r="D117" s="28"/>
@@ -7374,7 +7473,7 @@
       <c r="O117" s="28"/>
       <c r="P117" s="28"/>
     </row>
-    <row r="118" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B118" s="28"/>
       <c r="C118" s="28"/>
       <c r="D118" s="28"/>
@@ -7391,7 +7490,7 @@
       <c r="O118" s="28"/>
       <c r="P118" s="28"/>
     </row>
-    <row r="119" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B119" s="28"/>
       <c r="C119" s="28"/>
       <c r="D119" s="28"/>
@@ -7408,7 +7507,7 @@
       <c r="O119" s="28"/>
       <c r="P119" s="28"/>
     </row>
-    <row r="120" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B120" s="28"/>
       <c r="C120" s="28"/>
       <c r="D120" s="28"/>
@@ -7425,7 +7524,7 @@
       <c r="O120" s="28"/>
       <c r="P120" s="28"/>
     </row>
-    <row r="121" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B121" s="28"/>
       <c r="C121" s="28"/>
       <c r="D121" s="28"/>
@@ -7442,7 +7541,7 @@
       <c r="O121" s="28"/>
       <c r="P121" s="28"/>
     </row>
-    <row r="122" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B122" s="28"/>
       <c r="C122" s="28"/>
       <c r="D122" s="28"/>
@@ -7459,7 +7558,7 @@
       <c r="O122" s="28"/>
       <c r="P122" s="28"/>
     </row>
-    <row r="123" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B123" s="28"/>
       <c r="C123" s="28"/>
       <c r="D123" s="28"/>
@@ -7476,7 +7575,7 @@
       <c r="O123" s="28"/>
       <c r="P123" s="28"/>
     </row>
-    <row r="124" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B124" s="28"/>
       <c r="C124" s="28"/>
       <c r="D124" s="28"/>
@@ -7493,7 +7592,7 @@
       <c r="O124" s="28"/>
       <c r="P124" s="28"/>
     </row>
-    <row r="125" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B125" s="28"/>
       <c r="C125" s="28"/>
       <c r="D125" s="28"/>
@@ -7510,7 +7609,7 @@
       <c r="O125" s="28"/>
       <c r="P125" s="28"/>
     </row>
-    <row r="126" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B126" s="28"/>
       <c r="C126" s="28"/>
       <c r="D126" s="28"/>
@@ -7527,7 +7626,7 @@
       <c r="O126" s="28"/>
       <c r="P126" s="28"/>
     </row>
-    <row r="127" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B127" s="28"/>
       <c r="C127" s="28"/>
       <c r="D127" s="28"/>
@@ -7544,7 +7643,7 @@
       <c r="O127" s="28"/>
       <c r="P127" s="28"/>
     </row>
-    <row r="128" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B128" s="28"/>
       <c r="C128" s="28"/>
       <c r="D128" s="28"/>
@@ -7561,7 +7660,7 @@
       <c r="O128" s="28"/>
       <c r="P128" s="28"/>
     </row>
-    <row r="129" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B129" s="28"/>
       <c r="C129" s="28"/>
       <c r="D129" s="28"/>
@@ -7578,7 +7677,7 @@
       <c r="O129" s="28"/>
       <c r="P129" s="28"/>
     </row>
-    <row r="130" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B130" s="28"/>
       <c r="C130" s="28"/>
       <c r="D130" s="28"/>
@@ -7595,7 +7694,7 @@
       <c r="O130" s="28"/>
       <c r="P130" s="28"/>
     </row>
-    <row r="131" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B131" s="28"/>
       <c r="C131" s="28"/>
       <c r="D131" s="28"/>
@@ -7612,7 +7711,7 @@
       <c r="O131" s="28"/>
       <c r="P131" s="28"/>
     </row>
-    <row r="132" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B132" s="28"/>
       <c r="C132" s="28"/>
       <c r="D132" s="28"/>
@@ -7629,7 +7728,7 @@
       <c r="O132" s="28"/>
       <c r="P132" s="28"/>
     </row>
-    <row r="133" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B133" s="28"/>
       <c r="C133" s="28"/>
       <c r="D133" s="28"/>
@@ -7646,7 +7745,7 @@
       <c r="O133" s="28"/>
       <c r="P133" s="28"/>
     </row>
-    <row r="134" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B134" s="28"/>
       <c r="C134" s="28"/>
       <c r="D134" s="28"/>
@@ -7663,7 +7762,7 @@
       <c r="O134" s="28"/>
       <c r="P134" s="28"/>
     </row>
-    <row r="135" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B135" s="28"/>
       <c r="C135" s="28"/>
       <c r="D135" s="28"/>
@@ -7680,7 +7779,7 @@
       <c r="O135" s="28"/>
       <c r="P135" s="28"/>
     </row>
-    <row r="136" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B136" s="28"/>
       <c r="C136" s="28"/>
       <c r="D136" s="28"/>
@@ -7697,7 +7796,7 @@
       <c r="O136" s="28"/>
       <c r="P136" s="28"/>
     </row>
-    <row r="137" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B137" s="28"/>
       <c r="C137" s="28"/>
       <c r="D137" s="28"/>
@@ -7714,7 +7813,7 @@
       <c r="O137" s="28"/>
       <c r="P137" s="28"/>
     </row>
-    <row r="138" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B138" s="28"/>
       <c r="C138" s="28"/>
       <c r="D138" s="28"/>
@@ -7731,7 +7830,7 @@
       <c r="O138" s="28"/>
       <c r="P138" s="28"/>
     </row>
-    <row r="139" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B139" s="28"/>
       <c r="C139" s="28"/>
       <c r="D139" s="28"/>
@@ -7748,7 +7847,7 @@
       <c r="O139" s="28"/>
       <c r="P139" s="28"/>
     </row>
-    <row r="140" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B140" s="28"/>
       <c r="C140" s="28"/>
       <c r="D140" s="28"/>
@@ -7765,7 +7864,7 @@
       <c r="O140" s="28"/>
       <c r="P140" s="28"/>
     </row>
-    <row r="141" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B141" s="28"/>
       <c r="C141" s="28"/>
       <c r="D141" s="28"/>
@@ -7782,7 +7881,7 @@
       <c r="O141" s="28"/>
       <c r="P141" s="28"/>
     </row>
-    <row r="142" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B142" s="28"/>
       <c r="C142" s="28"/>
       <c r="D142" s="28"/>
@@ -7799,7 +7898,7 @@
       <c r="O142" s="28"/>
       <c r="P142" s="28"/>
     </row>
-    <row r="143" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B143" s="28"/>
       <c r="C143" s="28"/>
       <c r="D143" s="28"/>
@@ -7816,7 +7915,7 @@
       <c r="O143" s="28"/>
       <c r="P143" s="28"/>
     </row>
-    <row r="144" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B144" s="28"/>
       <c r="C144" s="28"/>
       <c r="D144" s="28"/>
@@ -7833,7 +7932,7 @@
       <c r="O144" s="28"/>
       <c r="P144" s="28"/>
     </row>
-    <row r="145" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B145" s="28"/>
       <c r="C145" s="28"/>
       <c r="D145" s="28"/>
@@ -7850,7 +7949,7 @@
       <c r="O145" s="28"/>
       <c r="P145" s="28"/>
     </row>
-    <row r="146" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B146" s="28"/>
       <c r="C146" s="28"/>
       <c r="D146" s="28"/>
@@ -7867,7 +7966,7 @@
       <c r="O146" s="28"/>
       <c r="P146" s="28"/>
     </row>
-    <row r="147" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B147" s="28"/>
       <c r="C147" s="28"/>
       <c r="D147" s="28"/>
@@ -7884,7 +7983,7 @@
       <c r="O147" s="28"/>
       <c r="P147" s="28"/>
     </row>
-    <row r="148" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B148" s="28"/>
       <c r="C148" s="28"/>
       <c r="D148" s="28"/>
@@ -7901,7 +8000,7 @@
       <c r="O148" s="28"/>
       <c r="P148" s="28"/>
     </row>
-    <row r="149" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B149" s="28"/>
       <c r="C149" s="28"/>
       <c r="D149" s="28"/>
@@ -7918,7 +8017,7 @@
       <c r="O149" s="28"/>
       <c r="P149" s="28"/>
     </row>
-    <row r="150" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B150" s="28"/>
       <c r="C150" s="28"/>
       <c r="D150" s="28"/>
@@ -7935,7 +8034,7 @@
       <c r="O150" s="28"/>
       <c r="P150" s="28"/>
     </row>
-    <row r="151" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B151" s="28"/>
       <c r="C151" s="28"/>
       <c r="D151" s="28"/>
@@ -7952,7 +8051,7 @@
       <c r="O151" s="28"/>
       <c r="P151" s="28"/>
     </row>
-    <row r="152" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B152" s="28"/>
       <c r="C152" s="28"/>
       <c r="D152" s="28"/>
@@ -7969,7 +8068,7 @@
       <c r="O152" s="28"/>
       <c r="P152" s="28"/>
     </row>
-    <row r="153" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B153" s="28"/>
       <c r="C153" s="28"/>
       <c r="D153" s="28"/>
@@ -7986,7 +8085,7 @@
       <c r="O153" s="28"/>
       <c r="P153" s="28"/>
     </row>
-    <row r="154" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B154" s="28"/>
       <c r="C154" s="28"/>
       <c r="D154" s="28"/>
@@ -8003,7 +8102,7 @@
       <c r="O154" s="28"/>
       <c r="P154" s="28"/>
     </row>
-    <row r="155" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B155" s="28"/>
       <c r="C155" s="28"/>
       <c r="D155" s="28"/>
@@ -8020,7 +8119,7 @@
       <c r="O155" s="28"/>
       <c r="P155" s="28"/>
     </row>
-    <row r="156" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B156" s="28"/>
       <c r="C156" s="28"/>
       <c r="D156" s="28"/>
@@ -8037,7 +8136,7 @@
       <c r="O156" s="28"/>
       <c r="P156" s="28"/>
     </row>
-    <row r="157" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B157" s="28"/>
       <c r="C157" s="28"/>
       <c r="D157" s="28"/>
@@ -8054,7 +8153,7 @@
       <c r="O157" s="28"/>
       <c r="P157" s="28"/>
     </row>
-    <row r="158" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B158" s="28"/>
       <c r="C158" s="28"/>
       <c r="D158" s="28"/>
@@ -8071,7 +8170,7 @@
       <c r="O158" s="28"/>
       <c r="P158" s="28"/>
     </row>
-    <row r="159" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B159" s="28"/>
       <c r="C159" s="28"/>
       <c r="D159" s="28"/>
@@ -8088,7 +8187,7 @@
       <c r="O159" s="28"/>
       <c r="P159" s="28"/>
     </row>
-    <row r="160" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B160" s="28"/>
       <c r="C160" s="28"/>
       <c r="D160" s="28"/>
@@ -8108,26 +8207,27 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q92"/>
+  <dimension ref="A1:Q93"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="E101" sqref="E101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5546875" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5546875" style="2"/>
+    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -8148,7 +8248,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -8169,7 +8269,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -8222,7 +8322,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>43908</v>
       </c>
@@ -8275,7 +8375,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>43909</v>
       </c>
@@ -8328,7 +8428,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>43910</v>
       </c>
@@ -8381,7 +8481,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>43911</v>
       </c>
@@ -8434,7 +8534,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>43912</v>
       </c>
@@ -8487,7 +8587,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>43913</v>
       </c>
@@ -8540,7 +8640,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>43914</v>
       </c>
@@ -8593,7 +8693,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>43915</v>
       </c>
@@ -8646,7 +8746,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>43916</v>
       </c>
@@ -8699,7 +8799,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>43917</v>
       </c>
@@ -8752,7 +8852,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>43918</v>
       </c>
@@ -8805,7 +8905,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>43919</v>
       </c>
@@ -8858,7 +8958,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>43920</v>
       </c>
@@ -8911,7 +9011,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>43921</v>
       </c>
@@ -8964,7 +9064,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>43922</v>
       </c>
@@ -9017,7 +9117,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>43923</v>
       </c>
@@ -9070,7 +9170,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>43924</v>
       </c>
@@ -9123,7 +9223,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>43925</v>
       </c>
@@ -9176,7 +9276,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>43926</v>
       </c>
@@ -9229,7 +9329,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>43927</v>
       </c>
@@ -9282,7 +9382,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>43928</v>
       </c>
@@ -9335,7 +9435,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>43929</v>
       </c>
@@ -9388,7 +9488,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>43930</v>
       </c>
@@ -9441,7 +9541,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>43931</v>
       </c>
@@ -9494,7 +9594,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <v>43932</v>
       </c>
@@ -9547,7 +9647,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <v>43933</v>
       </c>
@@ -9600,7 +9700,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <v>43934</v>
       </c>
@@ -9653,7 +9753,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <v>43935</v>
       </c>
@@ -9706,7 +9806,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>43936</v>
       </c>
@@ -9759,7 +9859,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <v>43937</v>
       </c>
@@ -9812,7 +9912,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <v>43938</v>
       </c>
@@ -9865,7 +9965,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <v>43939</v>
       </c>
@@ -9918,7 +10018,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="30">
         <v>43940</v>
       </c>
@@ -9971,7 +10071,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="30">
         <v>43941</v>
       </c>
@@ -10024,7 +10124,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="30">
         <v>43942</v>
       </c>
@@ -10077,7 +10177,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="30">
         <v>43943</v>
       </c>
@@ -10130,7 +10230,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="30">
         <v>43944</v>
       </c>
@@ -10183,7 +10283,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="30">
         <v>43945</v>
       </c>
@@ -10236,7 +10336,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="30">
         <v>43946</v>
       </c>
@@ -10289,7 +10389,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="30">
         <v>43947</v>
       </c>
@@ -10342,7 +10442,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="30">
         <v>43948</v>
       </c>
@@ -10395,7 +10495,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="30">
         <v>43949</v>
       </c>
@@ -10448,7 +10548,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="30">
         <v>43950</v>
       </c>
@@ -10501,7 +10601,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="30">
         <v>43951</v>
       </c>
@@ -10554,7 +10654,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="30">
         <v>43952</v>
       </c>
@@ -10607,7 +10707,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="30">
         <v>43953</v>
       </c>
@@ -10660,7 +10760,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="30">
         <v>43954</v>
       </c>
@@ -10713,7 +10813,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="30">
         <v>43955</v>
       </c>
@@ -10766,7 +10866,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="30">
         <v>43956</v>
       </c>
@@ -10819,7 +10919,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="30">
         <v>43957</v>
       </c>
@@ -10872,7 +10972,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="30">
         <v>43958</v>
       </c>
@@ -10925,7 +11025,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="30">
         <v>43959</v>
       </c>
@@ -10978,7 +11078,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="30">
         <v>43960</v>
       </c>
@@ -11031,7 +11131,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="30">
         <v>43961</v>
       </c>
@@ -11084,7 +11184,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="30">
         <v>43962</v>
       </c>
@@ -11137,7 +11237,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="30">
         <v>43963</v>
       </c>
@@ -11190,7 +11290,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="30">
         <v>43964</v>
       </c>
@@ -11243,7 +11343,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" s="30">
         <v>43965</v>
       </c>
@@ -11296,7 +11396,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="30">
         <v>43966</v>
       </c>
@@ -11349,7 +11449,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" s="30">
         <v>43967</v>
       </c>
@@ -11402,7 +11502,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" s="30">
         <v>43968</v>
       </c>
@@ -11455,7 +11555,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" s="30">
         <v>43969</v>
       </c>
@@ -11508,7 +11608,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" s="30">
         <v>43970</v>
       </c>
@@ -11561,7 +11661,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" s="30">
         <v>43971</v>
       </c>
@@ -11614,7 +11714,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" s="30">
         <v>43972</v>
       </c>
@@ -11667,7 +11767,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" s="30">
         <v>43973</v>
       </c>
@@ -11720,7 +11820,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" s="30">
         <v>43974</v>
       </c>
@@ -11773,7 +11873,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" s="30">
         <v>43975</v>
       </c>
@@ -11826,7 +11926,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" s="30">
         <v>43976</v>
       </c>
@@ -11879,7 +11979,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" s="30">
         <v>43977</v>
       </c>
@@ -11932,7 +12032,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" s="30">
         <v>43978</v>
       </c>
@@ -11985,7 +12085,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" s="30">
         <v>43979</v>
       </c>
@@ -12038,7 +12138,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" s="30">
         <v>43980</v>
       </c>
@@ -12091,7 +12191,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" s="30">
         <v>43981</v>
       </c>
@@ -12144,7 +12244,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" s="30">
         <v>43982</v>
       </c>
@@ -12197,7 +12297,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" s="30">
         <v>43983</v>
       </c>
@@ -12250,7 +12350,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" s="30">
         <v>43984</v>
       </c>
@@ -12303,7 +12403,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" s="30">
         <v>43985</v>
       </c>
@@ -12356,7 +12456,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" s="30">
         <v>43986</v>
       </c>
@@ -12409,7 +12509,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" s="30">
         <v>43987</v>
       </c>
@@ -12462,7 +12562,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" s="30">
         <v>43988</v>
       </c>
@@ -12515,7 +12615,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85" s="30">
         <v>43989</v>
       </c>
@@ -12568,7 +12668,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86" s="30">
         <v>43990</v>
       </c>
@@ -12621,7 +12721,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" s="30">
         <v>43991</v>
       </c>
@@ -12674,7 +12774,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88" s="30">
         <v>43992</v>
       </c>
@@ -12727,7 +12827,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89" s="30">
         <v>43993</v>
       </c>
@@ -12780,7 +12880,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90" s="30">
         <v>43994</v>
       </c>
@@ -12833,7 +12933,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91" s="30">
         <v>43995</v>
       </c>
@@ -12886,7 +12986,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92" s="30">
         <v>43996</v>
       </c>
@@ -12937,6 +13037,59 @@
       </c>
       <c r="Q92" s="13">
         <v>15</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A93" s="30">
+        <v>43997</v>
+      </c>
+      <c r="B93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G93" s="11">
+        <v>5</v>
+      </c>
+      <c r="H93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="L93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P93" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q93" s="13">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -12947,23 +13100,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R84"/>
+  <dimension ref="A1:R85"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="P94" sqref="P94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5546875" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5546875" style="2"/>
+    <col min="1" max="1" width="15.42578125" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -12984,7 +13137,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -13005,7 +13158,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -13058,7 +13211,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>43916</v>
       </c>
@@ -13111,7 +13264,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>43917</v>
       </c>
@@ -13164,7 +13317,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>43918</v>
       </c>
@@ -13217,7 +13370,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>43919</v>
       </c>
@@ -13270,7 +13423,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>43920</v>
       </c>
@@ -13323,7 +13476,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>43921</v>
       </c>
@@ -13376,7 +13529,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>43922</v>
       </c>
@@ -13429,7 +13582,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>43923</v>
       </c>
@@ -13482,7 +13635,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>43924</v>
       </c>
@@ -13535,7 +13688,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>43925</v>
       </c>
@@ -13588,7 +13741,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>43926</v>
       </c>
@@ -13641,7 +13794,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>43927</v>
       </c>
@@ -13694,7 +13847,7 @@
         <v>1262</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>43928</v>
       </c>
@@ -13747,7 +13900,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>43929</v>
       </c>
@@ -13800,7 +13953,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>43930</v>
       </c>
@@ -13853,7 +14006,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>43931</v>
       </c>
@@ -13906,7 +14059,7 @@
         <v>1461</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>43932</v>
       </c>
@@ -13959,7 +14112,7 @@
         <v>1467</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>43933</v>
       </c>
@@ -14012,7 +14165,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>43934</v>
       </c>
@@ -14065,7 +14218,7 @@
         <v>1482</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>43935</v>
       </c>
@@ -14118,7 +14271,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>43936</v>
       </c>
@@ -14171,7 +14324,7 @@
         <v>1486</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>43937</v>
       </c>
@@ -14224,7 +14377,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>43938</v>
       </c>
@@ -14277,7 +14430,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>43939</v>
       </c>
@@ -14330,7 +14483,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <v>43940</v>
       </c>
@@ -14383,7 +14536,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <v>43941</v>
       </c>
@@ -14436,7 +14589,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <v>43942</v>
       </c>
@@ -14489,7 +14642,7 @@
         <v>1472</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <v>43943</v>
       </c>
@@ -14542,7 +14695,7 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>43944</v>
       </c>
@@ -14595,7 +14748,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <v>43945</v>
       </c>
@@ -14648,7 +14801,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <v>43946</v>
       </c>
@@ -14701,7 +14854,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <v>43947</v>
       </c>
@@ -14754,7 +14907,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="30">
         <v>43948</v>
       </c>
@@ -14807,7 +14960,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="30">
         <v>43949</v>
       </c>
@@ -14860,7 +15013,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="30">
         <v>43950</v>
       </c>
@@ -14913,7 +15066,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="30">
         <v>43951</v>
       </c>
@@ -14966,7 +15119,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="30">
         <v>43952</v>
       </c>
@@ -15019,7 +15172,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="30">
         <v>43953</v>
       </c>
@@ -15072,7 +15225,7 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="30">
         <v>43954</v>
       </c>
@@ -15125,7 +15278,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="30">
         <v>43955</v>
       </c>
@@ -15178,7 +15331,7 @@
         <v>1279</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="30">
         <v>43956</v>
       </c>
@@ -15231,7 +15384,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="30">
         <v>43957</v>
       </c>
@@ -15284,7 +15437,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="30">
         <v>43958</v>
       </c>
@@ -15337,7 +15490,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="30">
         <v>43959</v>
       </c>
@@ -15390,7 +15543,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="30">
         <v>43960</v>
       </c>
@@ -15443,7 +15596,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="30">
         <v>43961</v>
       </c>
@@ -15496,7 +15649,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="30">
         <v>43962</v>
       </c>
@@ -15549,7 +15702,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="30">
         <v>43963</v>
       </c>
@@ -15602,7 +15755,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="30">
         <v>43964</v>
       </c>
@@ -15655,7 +15808,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="30">
         <v>43965</v>
       </c>
@@ -15708,7 +15861,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="30">
         <v>43966</v>
       </c>
@@ -15761,7 +15914,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="30">
         <v>43967</v>
       </c>
@@ -15814,7 +15967,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="30">
         <v>43968</v>
       </c>
@@ -15867,7 +16020,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="30">
         <v>43969</v>
       </c>
@@ -15920,7 +16073,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="30">
         <v>43970</v>
       </c>
@@ -15973,7 +16126,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="30">
         <v>43971</v>
       </c>
@@ -16026,7 +16179,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="30">
         <v>43972</v>
       </c>
@@ -16079,7 +16232,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" s="30">
         <v>43973</v>
       </c>
@@ -16132,7 +16285,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="30">
         <v>43974</v>
       </c>
@@ -16185,7 +16338,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" s="30">
         <v>43975</v>
       </c>
@@ -16238,7 +16391,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" s="30">
         <v>43976</v>
       </c>
@@ -16291,7 +16444,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" s="51">
         <v>43977</v>
       </c>
@@ -16344,7 +16497,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" s="51">
         <v>43978</v>
       </c>
@@ -16397,7 +16550,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="51">
         <v>43979</v>
       </c>
@@ -16450,7 +16603,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="51">
         <v>43980</v>
       </c>
@@ -16503,7 +16656,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" s="51">
         <v>43981</v>
       </c>
@@ -16556,7 +16709,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" s="51">
         <v>43982</v>
       </c>
@@ -16609,7 +16762,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" s="51">
         <v>43983</v>
       </c>
@@ -16662,7 +16815,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72" s="51">
         <v>43984</v>
       </c>
@@ -16715,7 +16868,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" s="51">
         <v>43985</v>
       </c>
@@ -16768,7 +16921,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" s="51">
         <v>43986</v>
       </c>
@@ -16821,7 +16974,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75" s="51">
         <v>43987</v>
       </c>
@@ -16874,7 +17027,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" s="51">
         <v>43988</v>
       </c>
@@ -16927,7 +17080,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" s="51">
         <v>43989</v>
       </c>
@@ -16980,7 +17133,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" s="51">
         <v>43990</v>
       </c>
@@ -17033,7 +17186,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79" s="51">
         <v>43991</v>
       </c>
@@ -17086,7 +17239,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A80" s="51">
         <v>43992</v>
       </c>
@@ -17140,7 +17293,7 @@
       </c>
       <c r="R80" s="54"/>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" s="51">
         <v>43993</v>
       </c>
@@ -17194,7 +17347,7 @@
       </c>
       <c r="R81" s="54"/>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" s="51">
         <v>43994</v>
       </c>
@@ -17248,7 +17401,7 @@
       </c>
       <c r="R82" s="54"/>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" s="51">
         <v>43995</v>
       </c>
@@ -17301,7 +17454,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" s="51">
         <v>43996</v>
       </c>
@@ -17352,6 +17505,59 @@
       </c>
       <c r="Q84" s="13">
         <v>575</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A85" s="51">
+        <v>43997</v>
+      </c>
+      <c r="B85" s="11">
+        <v>5</v>
+      </c>
+      <c r="C85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E85" s="11">
+        <v>56</v>
+      </c>
+      <c r="F85" s="11">
+        <v>6</v>
+      </c>
+      <c r="G85" s="11">
+        <v>56</v>
+      </c>
+      <c r="H85" s="11">
+        <v>262</v>
+      </c>
+      <c r="I85" s="11">
+        <v>7</v>
+      </c>
+      <c r="J85" s="11">
+        <v>49</v>
+      </c>
+      <c r="K85" s="11">
+        <v>131</v>
+      </c>
+      <c r="L85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N85" s="11">
+        <v>5</v>
+      </c>
+      <c r="O85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q85" s="13">
+        <v>578</v>
       </c>
     </row>
   </sheetData>
@@ -17362,23 +17568,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q84"/>
+  <dimension ref="A1:Q85"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="O87" sqref="O87"/>
+      <selection pane="bottomRight" activeCell="R96" sqref="R96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5546875" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5546875" style="2"/>
+    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -17399,7 +17605,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -17420,7 +17626,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -17473,7 +17679,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>43916</v>
       </c>
@@ -17526,7 +17732,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>43917</v>
       </c>
@@ -17579,7 +17785,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>43918</v>
       </c>
@@ -17632,7 +17838,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>43919</v>
       </c>
@@ -17685,7 +17891,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>43920</v>
       </c>
@@ -17738,7 +17944,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>43921</v>
       </c>
@@ -17791,7 +17997,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>43922</v>
       </c>
@@ -17844,7 +18050,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>43923</v>
       </c>
@@ -17897,7 +18103,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>43924</v>
       </c>
@@ -17950,7 +18156,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>43925</v>
       </c>
@@ -18003,7 +18209,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>43926</v>
       </c>
@@ -18056,7 +18262,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>43927</v>
       </c>
@@ -18109,7 +18315,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>43928</v>
       </c>
@@ -18162,7 +18368,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>43929</v>
       </c>
@@ -18215,7 +18421,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>43930</v>
       </c>
@@ -18268,7 +18474,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>43931</v>
       </c>
@@ -18321,7 +18527,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>43932</v>
       </c>
@@ -18374,7 +18580,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>43933</v>
       </c>
@@ -18427,7 +18633,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>43934</v>
       </c>
@@ -18480,7 +18686,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>43935</v>
       </c>
@@ -18533,7 +18739,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>43936</v>
       </c>
@@ -18586,7 +18792,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>43937</v>
       </c>
@@ -18639,7 +18845,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>43938</v>
       </c>
@@ -18692,7 +18898,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>43939</v>
       </c>
@@ -18745,7 +18951,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <v>43940</v>
       </c>
@@ -18798,7 +19004,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <v>43941</v>
       </c>
@@ -18851,7 +19057,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <v>43942</v>
       </c>
@@ -18904,7 +19110,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <v>43943</v>
       </c>
@@ -18957,7 +19163,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>43944</v>
       </c>
@@ -19010,7 +19216,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <v>43945</v>
       </c>
@@ -19063,7 +19269,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <v>43946</v>
       </c>
@@ -19116,7 +19322,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <v>43947</v>
       </c>
@@ -19169,7 +19375,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="30">
         <v>43948</v>
       </c>
@@ -19222,7 +19428,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="30">
         <v>43949</v>
       </c>
@@ -19275,7 +19481,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="30">
         <v>43950</v>
       </c>
@@ -19328,7 +19534,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="30">
         <v>43951</v>
       </c>
@@ -19381,7 +19587,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="30">
         <v>43952</v>
       </c>
@@ -19434,7 +19640,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="30">
         <v>43953</v>
       </c>
@@ -19487,7 +19693,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="30">
         <v>43954</v>
       </c>
@@ -19540,7 +19746,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="30">
         <v>43955</v>
       </c>
@@ -19593,7 +19799,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="30">
         <v>43956</v>
       </c>
@@ -19646,7 +19852,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="30">
         <v>43957</v>
       </c>
@@ -19699,7 +19905,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="30">
         <v>43958</v>
       </c>
@@ -19752,7 +19958,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="30">
         <v>43959</v>
       </c>
@@ -19805,7 +20011,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="30">
         <v>43960</v>
       </c>
@@ -19858,7 +20064,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="30">
         <v>43961</v>
       </c>
@@ -19911,7 +20117,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="30">
         <v>43962</v>
       </c>
@@ -19964,7 +20170,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="30">
         <v>43963</v>
       </c>
@@ -20017,7 +20223,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="30">
         <v>43964</v>
       </c>
@@ -20070,7 +20276,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="30">
         <v>43965</v>
       </c>
@@ -20123,7 +20329,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="30">
         <v>43966</v>
       </c>
@@ -20176,7 +20382,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="30">
         <v>43967</v>
       </c>
@@ -20229,7 +20435,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="30">
         <v>43968</v>
       </c>
@@ -20282,7 +20488,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="30">
         <v>43969</v>
       </c>
@@ -20335,7 +20541,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="30">
         <v>43970</v>
       </c>
@@ -20388,7 +20594,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="30">
         <v>43971</v>
       </c>
@@ -20441,7 +20647,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="30">
         <v>43972</v>
       </c>
@@ -20494,7 +20700,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" s="30">
         <v>43973</v>
       </c>
@@ -20547,7 +20753,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="30">
         <v>43974</v>
       </c>
@@ -20600,7 +20806,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" s="30">
         <v>43975</v>
       </c>
@@ -20653,7 +20859,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" s="30">
         <v>43976</v>
       </c>
@@ -20706,7 +20912,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" s="30">
         <v>43977</v>
       </c>
@@ -20759,7 +20965,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" s="30">
         <v>43978</v>
       </c>
@@ -20812,7 +21018,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" s="30">
         <v>43979</v>
       </c>
@@ -20865,7 +21071,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" s="30">
         <v>43980</v>
       </c>
@@ -20918,7 +21124,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" s="30">
         <v>43981</v>
       </c>
@@ -20971,7 +21177,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" s="30">
         <v>43982</v>
       </c>
@@ -21024,7 +21230,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" s="30">
         <v>43983</v>
       </c>
@@ -21077,7 +21283,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" s="30">
         <v>43984</v>
       </c>
@@ -21130,7 +21336,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" s="30">
         <v>43985</v>
       </c>
@@ -21183,7 +21389,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" s="30">
         <v>43986</v>
       </c>
@@ -21236,7 +21442,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" s="30">
         <v>43987</v>
       </c>
@@ -21289,7 +21495,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" s="30">
         <v>43988</v>
       </c>
@@ -21342,7 +21548,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" s="30">
         <v>43989</v>
       </c>
@@ -21395,7 +21601,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" s="30">
         <v>43990</v>
       </c>
@@ -21448,7 +21654,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" s="30">
         <v>43991</v>
       </c>
@@ -21501,7 +21707,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" s="30">
         <v>43992</v>
       </c>
@@ -21554,7 +21760,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" s="30">
         <v>43993</v>
       </c>
@@ -21607,7 +21813,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" s="30">
         <v>43994</v>
       </c>
@@ -21660,7 +21866,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" s="30">
         <v>43995</v>
       </c>
@@ -21713,7 +21919,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" s="30">
         <v>43996</v>
       </c>
@@ -21764,6 +21970,59 @@
       </c>
       <c r="Q84" s="13">
         <v>389</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A85" s="30">
+        <v>43997</v>
+      </c>
+      <c r="B85" s="11">
+        <v>11</v>
+      </c>
+      <c r="C85" s="11">
+        <v>22</v>
+      </c>
+      <c r="D85" s="11">
+        <v>8</v>
+      </c>
+      <c r="E85" s="11">
+        <v>19</v>
+      </c>
+      <c r="F85" s="11">
+        <v>38</v>
+      </c>
+      <c r="G85" s="11">
+        <v>11</v>
+      </c>
+      <c r="H85" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I85" s="11">
+        <v>12</v>
+      </c>
+      <c r="J85" s="11">
+        <v>52</v>
+      </c>
+      <c r="K85" s="11">
+        <v>109</v>
+      </c>
+      <c r="L85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N85" s="11">
+        <v>8</v>
+      </c>
+      <c r="O85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P85" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q85" s="13">
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -21771,7 +22030,7 @@
 </worksheet>
 </file>
 
-<file path=customXML/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA" version="1.0.0">
   <systemFields>
     <field name="Objective-Id">
@@ -21796,7 +22055,7 @@
       <value order="0"/>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-14T11:47:42Z</value>
+      <value order="0">2020-06-15T12:45:35Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -21808,16 +22067,16 @@
       <value order="0">Analytical: COVID 19 Analysis: Restricted working papers: Research and analysis: Diseases: 2020-2025</value>
     </field>
     <field name="Objective-State">
-      <value order="0">Being Drafted</value>
+      <value order="0">Being Edited</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41732238</value>
+      <value order="0">vA41747896</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">25.3</value>
+      <value order="0">25.8</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">178</value>
+      <value order="0">183</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>
@@ -21854,7 +22113,7 @@
 </metadata>
 </file>
 
-<file path=customXML/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5745109E-2DDF-40CB-AC2B-FF9B10C90820}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-16 20:09)
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5985" windowHeight="6045" tabRatio="803"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5985" windowHeight="6045" tabRatio="803" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1883" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1908" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -256,7 +256,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -393,12 +393,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -510,6 +519,11 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2025,7 +2039,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2111,7 +2125,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="O52" sqref="O52"/>
     </sheetView>
   </sheetViews>
@@ -2135,10 +2149,10 @@
   <dimension ref="A1:S160"/>
   <sheetViews>
     <sheetView zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B82" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B79" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="R110" sqref="R110"/>
+      <selection pane="bottomRight" activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7194,57 +7208,59 @@
       </c>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A103" s="5">
+      <c r="A103" s="55">
         <v>43996</v>
       </c>
-      <c r="B103" s="28">
+      <c r="B103" s="56">
         <v>1088</v>
       </c>
-      <c r="C103" s="28">
+      <c r="C103" s="56">
         <v>327</v>
       </c>
-      <c r="D103" s="28">
+      <c r="D103" s="56">
         <v>261</v>
       </c>
-      <c r="E103" s="28">
+      <c r="E103" s="56">
         <v>885</v>
       </c>
-      <c r="F103" s="28">
+      <c r="F103" s="56">
         <v>952</v>
       </c>
-      <c r="G103" s="28">
+      <c r="G103" s="56">
         <v>1294</v>
       </c>
-      <c r="H103" s="28">
+      <c r="H103" s="56">
         <v>4010</v>
       </c>
-      <c r="I103" s="28">
+      <c r="I103" s="56">
         <v>341</v>
       </c>
-      <c r="J103" s="28">
+      <c r="J103" s="56">
         <v>2035</v>
       </c>
-      <c r="K103" s="28">
+      <c r="K103" s="56">
         <v>2807</v>
       </c>
-      <c r="L103" s="28">
+      <c r="L103" s="56">
         <v>8</v>
       </c>
-      <c r="M103" s="28">
+      <c r="M103" s="56">
         <v>54</v>
       </c>
-      <c r="N103" s="28">
+      <c r="N103" s="56">
         <v>1687</v>
       </c>
-      <c r="O103" s="28">
+      <c r="O103" s="56">
         <v>6</v>
       </c>
-      <c r="P103" s="32">
+      <c r="P103" s="57">
         <v>15755</v>
       </c>
     </row>
     <row r="104" spans="1:16" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="5"/>
+      <c r="A104" s="5">
+        <v>43997</v>
+      </c>
       <c r="C104" s="28"/>
       <c r="D104" s="28"/>
       <c r="E104" s="28"/>
@@ -7263,6 +7279,9 @@
       </c>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A105" s="5">
+        <v>43998</v>
+      </c>
       <c r="C105" s="28"/>
       <c r="D105" s="28"/>
       <c r="E105" s="28"/>
@@ -7276,7 +7295,9 @@
       <c r="M105" s="28"/>
       <c r="N105" s="28"/>
       <c r="O105" s="28"/>
-      <c r="P105" s="28"/>
+      <c r="P105" s="28">
+        <v>18045</v>
+      </c>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C106" s="28"/>
@@ -8213,11 +8234,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q93"/>
+  <dimension ref="A1:Q94"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E101" sqref="E101"/>
+      <pane ySplit="3" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R101" sqref="R101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13092,6 +13113,59 @@
         <v>18</v>
       </c>
     </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A94" s="30">
+        <v>43998</v>
+      </c>
+      <c r="B94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K94" s="11">
+        <v>6</v>
+      </c>
+      <c r="L94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P94" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q94" s="13">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -13100,13 +13174,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R85"/>
+  <dimension ref="A1:R86"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="P94" sqref="P94"/>
+      <selection pane="bottomRight" activeCell="H107" sqref="H107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17560,6 +17634,59 @@
         <v>578</v>
       </c>
     </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A86" s="51">
+        <v>43998</v>
+      </c>
+      <c r="B86" s="11">
+        <v>5</v>
+      </c>
+      <c r="C86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E86" s="11">
+        <v>56</v>
+      </c>
+      <c r="F86" s="11">
+        <v>7</v>
+      </c>
+      <c r="G86" s="11">
+        <v>58</v>
+      </c>
+      <c r="H86" s="11">
+        <v>255</v>
+      </c>
+      <c r="I86" s="11">
+        <v>7</v>
+      </c>
+      <c r="J86" s="11">
+        <v>44</v>
+      </c>
+      <c r="K86" s="11">
+        <v>131</v>
+      </c>
+      <c r="L86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N86" s="11">
+        <v>4</v>
+      </c>
+      <c r="O86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q86" s="13">
+        <v>567</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -17568,13 +17695,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q85"/>
+  <dimension ref="A1:Q86"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="R96" sqref="R96"/>
+      <selection pane="bottomRight" activeCell="R91" sqref="R91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22025,12 +22152,65 @@
         <v>292</v>
       </c>
     </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A86" s="30">
+        <v>43998</v>
+      </c>
+      <c r="B86" s="11">
+        <v>26</v>
+      </c>
+      <c r="C86" s="11">
+        <v>19</v>
+      </c>
+      <c r="D86" s="11">
+        <v>12</v>
+      </c>
+      <c r="E86" s="11">
+        <v>15</v>
+      </c>
+      <c r="F86" s="11">
+        <v>36</v>
+      </c>
+      <c r="G86" s="11">
+        <v>19</v>
+      </c>
+      <c r="H86" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I86" s="11">
+        <v>41</v>
+      </c>
+      <c r="J86" s="11">
+        <v>42</v>
+      </c>
+      <c r="K86" s="11">
+        <v>193</v>
+      </c>
+      <c r="L86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N86" s="11">
+        <v>16</v>
+      </c>
+      <c r="O86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q86" s="13">
+        <v>419</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXML/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA" version="1.0.0">
   <systemFields>
     <field name="Objective-Id">
@@ -22055,7 +22235,7 @@
       <value order="0"/>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-15T12:45:35Z</value>
+      <value order="0">2020-06-16T12:36:30Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -22067,16 +22247,16 @@
       <value order="0">Analytical: COVID 19 Analysis: Restricted working papers: Research and analysis: Diseases: 2020-2025</value>
     </field>
     <field name="Objective-State">
-      <value order="0">Being Edited</value>
+      <value order="0">Being Drafted</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41747896</value>
+      <value order="0">vA41774359</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">25.8</value>
+      <value order="0">25.10</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">183</value>
+      <value order="0">185</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>
@@ -22113,7 +22293,7 @@
 </metadata>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXML/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5745109E-2DDF-40CB-AC2B-FF9B10C90820}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-17 20:09)
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5985" windowHeight="6045" tabRatio="803" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5985" windowHeight="6045" tabRatio="803"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1908" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1935" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -2039,7 +2039,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2125,7 +2125,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O52" sqref="O52"/>
     </sheetView>
   </sheetViews>
@@ -2149,10 +2149,10 @@
   <dimension ref="A1:S160"/>
   <sheetViews>
     <sheetView zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B79" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B75" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C107" sqref="C107"/>
+      <selection pane="bottomRight" activeCell="P107" sqref="P107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7300,6 +7300,9 @@
       </c>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A106" s="5">
+        <v>43999</v>
+      </c>
       <c r="C106" s="28"/>
       <c r="D106" s="28"/>
       <c r="E106" s="28"/>
@@ -7313,7 +7316,9 @@
       <c r="M106" s="28"/>
       <c r="N106" s="28"/>
       <c r="O106" s="28"/>
-      <c r="P106" s="28"/>
+      <c r="P106" s="28">
+        <v>18066</v>
+      </c>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C107" s="28"/>
@@ -8234,11 +8239,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q94"/>
+  <dimension ref="A1:Q95"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R101" sqref="R101"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A96" sqref="A96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13166,6 +13171,59 @@
         <v>19</v>
       </c>
     </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A95" s="30">
+        <v>43999</v>
+      </c>
+      <c r="B95" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C95" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D95" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E95" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F95" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G95" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H95" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I95" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J95" s="14">
+        <v>6</v>
+      </c>
+      <c r="K95" s="11">
+        <v>6</v>
+      </c>
+      <c r="L95" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M95" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N95" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O95" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P95" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q95" s="13">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -13174,13 +13232,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R86"/>
+  <dimension ref="A1:R87"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B68" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H107" sqref="H107"/>
+      <selection pane="bottomRight" activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17674,8 +17732,8 @@
       <c r="M86" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="N86" s="11">
-        <v>4</v>
+      <c r="N86" s="14" t="s">
+        <v>29</v>
       </c>
       <c r="O86" s="14" t="s">
         <v>29</v>
@@ -17685,6 +17743,59 @@
       </c>
       <c r="Q86" s="13">
         <v>567</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A87" s="51">
+        <v>43999</v>
+      </c>
+      <c r="B87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E87" s="11">
+        <v>56</v>
+      </c>
+      <c r="F87" s="11">
+        <v>6</v>
+      </c>
+      <c r="G87" s="11">
+        <v>55</v>
+      </c>
+      <c r="H87" s="11">
+        <v>256</v>
+      </c>
+      <c r="I87" s="11">
+        <v>5</v>
+      </c>
+      <c r="J87" s="11">
+        <v>38</v>
+      </c>
+      <c r="K87" s="11">
+        <v>131</v>
+      </c>
+      <c r="L87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q87" s="13">
+        <v>553</v>
       </c>
     </row>
   </sheetData>
@@ -17695,13 +17806,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q86"/>
+  <dimension ref="A1:Q87"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B72" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B54" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="R91" sqref="R91"/>
+      <selection pane="bottomRight" activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22203,6 +22314,59 @@
       </c>
       <c r="Q86" s="13">
         <v>419</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A87" s="30">
+        <v>43999</v>
+      </c>
+      <c r="B87" s="11">
+        <v>26</v>
+      </c>
+      <c r="C87" s="11">
+        <v>21</v>
+      </c>
+      <c r="D87" s="11">
+        <v>8</v>
+      </c>
+      <c r="E87" s="11">
+        <v>14</v>
+      </c>
+      <c r="F87" s="11">
+        <v>38</v>
+      </c>
+      <c r="G87" s="11">
+        <v>24</v>
+      </c>
+      <c r="H87" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I87" s="11">
+        <v>20</v>
+      </c>
+      <c r="J87" s="11">
+        <v>56</v>
+      </c>
+      <c r="K87" s="11">
+        <v>193</v>
+      </c>
+      <c r="L87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N87" s="11">
+        <v>11</v>
+      </c>
+      <c r="O87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q87" s="13">
+        <v>412</v>
       </c>
     </row>
   </sheetData>
@@ -22235,7 +22399,7 @@
       <value order="0"/>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-16T12:36:30Z</value>
+      <value order="0">2020-06-17T12:13:29Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -22250,13 +22414,13 @@
       <value order="0">Being Drafted</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41774359</value>
+      <value order="0">vA41801529</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">25.10</value>
+      <value order="0">25.13</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">185</value>
+      <value order="0">188</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-18 20:09)
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5985" windowHeight="6045" tabRatio="803"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5985" windowHeight="6045" tabRatio="803" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1935" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1961" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -554,8 +554,8 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>73</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -565,7 +565,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6962775" cy="14077950"/>
+          <a:ext cx="6962775" cy="14773274"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -757,7 +757,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>he daily total of people found positive on 2/6/20 contains 40 historic samples from an NHS Fife laboratory. From 15 June the figures will also include people tested through the UK Government's testing programme including drive through, mobile testing units and home tests. There will be a delay to publishing these but a board table is expected to be available on or before 18 June.</a:t>
+            <a:t>he daily total of people found positive on 2/6/20 contains 40 historic samples from an NHS Fife laboratory. From 15 June the figures  also include people tested through the UK Government's testing programme including drive through, mobile testing units and home tests. The increase on 15 June is due to the addition of all the UKG data on that day.</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB">
             <a:effectLst/>
@@ -799,7 +799,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>3. Where labs do not provide their overnight data in time for the daily publication, the testing figures will then be added to the return for the subsequent day.   </a:t>
+            <a:t>3. Where labs do not provide their overnight data in time for the daily publication, the figures will then be added to the return for the subsequent day.   </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1698,8 +1698,8 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>771072</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>149226</xdr:colOff>
       <xdr:row>102</xdr:row>
       <xdr:rowOff>163284</xdr:rowOff>
     </xdr:from>
@@ -1711,7 +1711,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12709072" y="19122570"/>
+          <a:off x="12406994" y="20267838"/>
           <a:ext cx="5143500" cy="1097643"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1749,10 +1749,20 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>As of 15 June, this includes confirmed cases at UK Government Regional Testing Centres (RTCs). </a:t>
+            <a:t>As of 15 June, includes people</a:t>
           </a:r>
-        </a:p>
-        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> tested</a:t>
+          </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100">
               <a:solidFill>
@@ -1763,9 +1773,57 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>A breakdown by NHS Board is not yet available from UK Gov RTCs for 15 June. This table will be updated by 18 June.</a:t>
+            <a:t> through the UK Government (UKG) testing programme</a:t>
           </a:r>
-          <a:endParaRPr lang="en-GB" sz="1100"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> (Regional Testing Centres, Mobile Testing Units and home testing kits). Prior to 15 June the figures show people tested through NHS labs only. </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>The increase on 15 June is due to the addition of all the UKG cases to the database. </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>For more information see notes .</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB">
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2039,7 +2097,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2125,7 +2183,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="O52" sqref="O52"/>
     </sheetView>
   </sheetViews>
@@ -2149,10 +2207,10 @@
   <dimension ref="A1:S160"/>
   <sheetViews>
     <sheetView zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B75" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="I83" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="P107" sqref="P107"/>
+      <selection pane="bottomRight" activeCell="N119" sqref="N119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7261,20 +7319,49 @@
       <c r="A104" s="5">
         <v>43997</v>
       </c>
-      <c r="C104" s="28"/>
-      <c r="D104" s="28"/>
-      <c r="E104" s="28"/>
-      <c r="F104" s="28"/>
-      <c r="G104" s="28"/>
-      <c r="H104" s="28"/>
-      <c r="I104" s="28"/>
-      <c r="J104" s="28"/>
-      <c r="K104" s="28"/>
-      <c r="L104" s="28"/>
-      <c r="M104" s="28"/>
-      <c r="N104" s="28"/>
-      <c r="O104" s="28"/>
-      <c r="P104" s="32">
+      <c r="B104" s="28">
+        <v>1243</v>
+      </c>
+      <c r="C104" s="28">
+        <v>345</v>
+      </c>
+      <c r="D104" s="28">
+        <v>274</v>
+      </c>
+      <c r="E104" s="28">
+        <v>926</v>
+      </c>
+      <c r="F104" s="28">
+        <v>1048</v>
+      </c>
+      <c r="G104" s="28">
+        <v>1405</v>
+      </c>
+      <c r="H104" s="28">
+        <v>4805</v>
+      </c>
+      <c r="I104" s="28">
+        <v>373</v>
+      </c>
+      <c r="J104" s="28">
+        <v>2671</v>
+      </c>
+      <c r="K104" s="28">
+        <v>3110</v>
+      </c>
+      <c r="L104" s="28">
+        <v>9</v>
+      </c>
+      <c r="M104" s="28">
+        <v>54</v>
+      </c>
+      <c r="N104" s="28">
+        <v>1760</v>
+      </c>
+      <c r="O104" s="28">
+        <v>7</v>
+      </c>
+      <c r="P104" s="34">
         <v>18030</v>
       </c>
     </row>
@@ -7282,20 +7369,49 @@
       <c r="A105" s="5">
         <v>43998</v>
       </c>
-      <c r="C105" s="28"/>
-      <c r="D105" s="28"/>
-      <c r="E105" s="28"/>
-      <c r="F105" s="28"/>
-      <c r="G105" s="28"/>
-      <c r="H105" s="28"/>
-      <c r="I105" s="28"/>
-      <c r="J105" s="28"/>
-      <c r="K105" s="28"/>
-      <c r="L105" s="28"/>
-      <c r="M105" s="28"/>
-      <c r="N105" s="28"/>
-      <c r="O105" s="28"/>
-      <c r="P105" s="28">
+      <c r="B105" s="28">
+        <v>1243</v>
+      </c>
+      <c r="C105" s="28">
+        <v>345</v>
+      </c>
+      <c r="D105" s="28">
+        <v>274</v>
+      </c>
+      <c r="E105" s="28">
+        <v>926</v>
+      </c>
+      <c r="F105" s="28">
+        <v>1051</v>
+      </c>
+      <c r="G105" s="28">
+        <v>1405</v>
+      </c>
+      <c r="H105" s="28">
+        <v>4808</v>
+      </c>
+      <c r="I105" s="28">
+        <v>373</v>
+      </c>
+      <c r="J105" s="28">
+        <v>2674</v>
+      </c>
+      <c r="K105" s="28">
+        <v>3116</v>
+      </c>
+      <c r="L105" s="28">
+        <v>9</v>
+      </c>
+      <c r="M105" s="28">
+        <v>54</v>
+      </c>
+      <c r="N105" s="28">
+        <v>1760</v>
+      </c>
+      <c r="O105" s="28">
+        <v>7</v>
+      </c>
+      <c r="P105" s="32">
         <v>18045</v>
       </c>
     </row>
@@ -7303,38 +7419,101 @@
       <c r="A106" s="5">
         <v>43999</v>
       </c>
-      <c r="C106" s="28"/>
-      <c r="D106" s="28"/>
-      <c r="E106" s="28"/>
-      <c r="F106" s="28"/>
-      <c r="G106" s="28"/>
-      <c r="H106" s="28"/>
-      <c r="I106" s="28"/>
-      <c r="J106" s="28"/>
-      <c r="K106" s="28"/>
-      <c r="L106" s="28"/>
-      <c r="M106" s="28"/>
-      <c r="N106" s="28"/>
-      <c r="O106" s="28"/>
-      <c r="P106" s="28">
+      <c r="B106" s="28">
+        <v>1245</v>
+      </c>
+      <c r="C106" s="28">
+        <v>345</v>
+      </c>
+      <c r="D106" s="28">
+        <v>274</v>
+      </c>
+      <c r="E106" s="28">
+        <v>928</v>
+      </c>
+      <c r="F106" s="28">
+        <v>1051</v>
+      </c>
+      <c r="G106" s="28">
+        <v>1409</v>
+      </c>
+      <c r="H106" s="28">
+        <v>4810</v>
+      </c>
+      <c r="I106" s="28">
+        <v>373</v>
+      </c>
+      <c r="J106" s="28">
+        <v>2678</v>
+      </c>
+      <c r="K106" s="28">
+        <v>3123</v>
+      </c>
+      <c r="L106" s="28">
+        <v>9</v>
+      </c>
+      <c r="M106" s="28">
+        <v>54</v>
+      </c>
+      <c r="N106" s="28">
+        <v>1760</v>
+      </c>
+      <c r="O106" s="28">
+        <v>7</v>
+      </c>
+      <c r="P106" s="32">
         <v>18066</v>
       </c>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C107" s="28"/>
-      <c r="D107" s="28"/>
-      <c r="E107" s="28"/>
-      <c r="F107" s="28"/>
-      <c r="G107" s="28"/>
-      <c r="H107" s="28"/>
-      <c r="I107" s="28"/>
-      <c r="J107" s="28"/>
-      <c r="K107" s="28"/>
-      <c r="L107" s="28"/>
-      <c r="M107" s="28"/>
-      <c r="N107" s="28"/>
-      <c r="O107" s="28"/>
-      <c r="P107" s="28"/>
+      <c r="A107" s="5">
+        <v>44000</v>
+      </c>
+      <c r="B107" s="28">
+        <v>1245</v>
+      </c>
+      <c r="C107" s="28">
+        <v>345</v>
+      </c>
+      <c r="D107" s="28">
+        <v>274</v>
+      </c>
+      <c r="E107" s="28">
+        <v>928</v>
+      </c>
+      <c r="F107" s="28">
+        <v>1053</v>
+      </c>
+      <c r="G107" s="28">
+        <v>1410</v>
+      </c>
+      <c r="H107" s="28">
+        <v>4813</v>
+      </c>
+      <c r="I107" s="28">
+        <v>373</v>
+      </c>
+      <c r="J107" s="28">
+        <v>2681</v>
+      </c>
+      <c r="K107" s="28">
+        <v>3125</v>
+      </c>
+      <c r="L107" s="28">
+        <v>9</v>
+      </c>
+      <c r="M107" s="28">
+        <v>54</v>
+      </c>
+      <c r="N107" s="28">
+        <v>1760</v>
+      </c>
+      <c r="O107" s="28">
+        <v>7</v>
+      </c>
+      <c r="P107" s="32">
+        <v>18077</v>
+      </c>
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C108" s="28"/>
@@ -8239,11 +8418,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q95"/>
+  <dimension ref="A1:Q96"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A96" sqref="A96"/>
+      <selection pane="bottomLeft" activeCell="A97" sqref="A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13224,6 +13403,59 @@
         <v>24</v>
       </c>
     </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A96" s="30">
+        <v>44000</v>
+      </c>
+      <c r="B96" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C96" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D96" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E96" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F96" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G96" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H96" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I96" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J96" s="11">
+        <v>5</v>
+      </c>
+      <c r="K96" s="11">
+        <v>6</v>
+      </c>
+      <c r="L96" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M96" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N96" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O96" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P96" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q96" s="13">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -13232,13 +13464,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R87"/>
+  <dimension ref="A1:R88"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B56" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B65" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A88" sqref="A88"/>
+      <selection pane="bottomRight" activeCell="A89" sqref="A89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17798,6 +18030,59 @@
         <v>553</v>
       </c>
     </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A88" s="51">
+        <v>44000</v>
+      </c>
+      <c r="B88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E88" s="11">
+        <v>57</v>
+      </c>
+      <c r="F88" s="11">
+        <v>7</v>
+      </c>
+      <c r="G88" s="11">
+        <v>50</v>
+      </c>
+      <c r="H88" s="11">
+        <v>249</v>
+      </c>
+      <c r="I88" s="11">
+        <v>5</v>
+      </c>
+      <c r="J88" s="11">
+        <v>43</v>
+      </c>
+      <c r="K88" s="11">
+        <v>131</v>
+      </c>
+      <c r="L88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q88" s="13">
+        <v>547</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -17806,13 +18091,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q87"/>
+  <dimension ref="A1:Q88"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B54" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B75" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A88" sqref="A88"/>
+      <selection pane="bottomRight" activeCell="A89" sqref="A89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22367,6 +22652,59 @@
       </c>
       <c r="Q87" s="13">
         <v>412</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A88" s="30">
+        <v>44000</v>
+      </c>
+      <c r="B88" s="11">
+        <v>18</v>
+      </c>
+      <c r="C88" s="11">
+        <v>19</v>
+      </c>
+      <c r="D88" s="11">
+        <v>11</v>
+      </c>
+      <c r="E88" s="11">
+        <v>11</v>
+      </c>
+      <c r="F88" s="11">
+        <v>26</v>
+      </c>
+      <c r="G88" s="11">
+        <v>13</v>
+      </c>
+      <c r="H88" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I88" s="11">
+        <v>23</v>
+      </c>
+      <c r="J88" s="11">
+        <v>50</v>
+      </c>
+      <c r="K88" s="11">
+        <v>193</v>
+      </c>
+      <c r="L88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N88" s="11">
+        <v>14</v>
+      </c>
+      <c r="O88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q88" s="13">
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -22399,7 +22737,7 @@
       <value order="0"/>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-17T12:13:29Z</value>
+      <value order="0">2020-06-18T12:46:48Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -22414,13 +22752,13 @@
       <value order="0">Being Drafted</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41801529</value>
+      <value order="0">vA41828407</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">25.13</value>
+      <value order="0">25.17</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">188</value>
+      <value order="0">192</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-20 20:08)
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U446281\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA19028\A28088333\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\scotland.gov.uk\dc2\fs3_home\u205774\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5985" windowHeight="6045" tabRatio="803" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5990" windowHeight="6050" tabRatio="803"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1989" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2016" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -1669,6 +1669,64 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>11. As</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> at 20/06/20, </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Lothian data on confirmed</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> and suspected covid-19 hosptial inpatients is under investigation from 16/06/2020 onwards.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" b="0">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
           <a:endParaRPr lang="en-GB" sz="1100">
             <a:effectLst/>
             <a:latin typeface="+mn-lt"/>
@@ -1824,6 +1882,160 @@
           <a:endParaRPr lang="en-GB">
             <a:effectLst/>
           </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>547688</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>154782</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3845718" cy="333374"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12811126" y="16644938"/>
+          <a:ext cx="3845718" cy="333374"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>* Lothian data</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> from 16/06/2020 onwards under investigation.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3845718" cy="357188"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12644438" y="16680656"/>
+          <a:ext cx="3845718" cy="357188"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>* Lothian data</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> from 16/06/2020 onwards under investigation.</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2097,23 +2309,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="90.42578125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.42578125" style="2"/>
+    <col min="2" max="2" width="29.453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="90.453125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B3" s="18" t="s">
         <v>20</v>
       </c>
@@ -2121,7 +2333,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="20" t="s">
         <v>22</v>
       </c>
@@ -2129,13 +2341,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="22" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="23"/>
     </row>
-    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="24" t="s">
         <v>26</v>
       </c>
@@ -2143,7 +2355,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="24" t="s">
         <v>27</v>
       </c>
@@ -2151,7 +2363,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="24" t="s">
         <v>36</v>
       </c>
@@ -2159,7 +2371,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="20" t="s">
         <v>37</v>
       </c>
@@ -2183,16 +2395,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O52" sqref="O52"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="V71" sqref="V71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="9.42578125" style="2"/>
+    <col min="1" max="16384" width="9.453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A44" s="43"/>
     </row>
   </sheetData>
@@ -2206,21 +2418,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S160"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B85" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="G94" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" style="2" customWidth="1"/>
-    <col min="2" max="16" width="11.42578125" style="11" customWidth="1"/>
-    <col min="17" max="16384" width="8.5703125" style="2"/>
+    <col min="2" max="16" width="11.453125" style="11" customWidth="1"/>
+    <col min="17" max="16384" width="8.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -2240,7 +2452,7 @@
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -2259,7 +2471,7 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -2309,7 +2521,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>43897</v>
       </c>
@@ -2359,7 +2571,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>43898</v>
       </c>
@@ -2409,7 +2621,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>43899</v>
       </c>
@@ -2459,7 +2671,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>43900</v>
       </c>
@@ -2509,7 +2721,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>43901</v>
       </c>
@@ -2559,7 +2771,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>43902</v>
       </c>
@@ -2609,7 +2821,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>43903</v>
       </c>
@@ -2659,7 +2871,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>43904</v>
       </c>
@@ -2709,7 +2921,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>43905</v>
       </c>
@@ -2759,7 +2971,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>43906</v>
       </c>
@@ -2809,7 +3021,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>43907</v>
       </c>
@@ -2859,7 +3071,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>43908</v>
       </c>
@@ -2909,7 +3121,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>43909</v>
       </c>
@@ -2959,7 +3171,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>43910</v>
       </c>
@@ -3009,7 +3221,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>43911</v>
       </c>
@@ -3059,7 +3271,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>43912</v>
       </c>
@@ -3109,7 +3321,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>43913</v>
       </c>
@@ -3159,7 +3371,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>43914</v>
       </c>
@@ -3209,7 +3421,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>43915</v>
       </c>
@@ -3259,7 +3471,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>43916</v>
       </c>
@@ -3309,7 +3521,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>43917</v>
       </c>
@@ -3359,7 +3571,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>43918</v>
       </c>
@@ -3409,7 +3621,7 @@
         <v>1264</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>43919</v>
       </c>
@@ -3459,7 +3671,7 @@
         <v>1417</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>43920</v>
       </c>
@@ -3509,7 +3721,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>43921</v>
       </c>
@@ -3559,7 +3771,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>43922</v>
       </c>
@@ -3609,7 +3821,7 @@
         <v>2310</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>43923</v>
       </c>
@@ -3659,7 +3871,7 @@
         <v>2602</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>43924</v>
       </c>
@@ -3709,7 +3921,7 @@
         <v>3001</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>43925</v>
       </c>
@@ -3759,7 +3971,7 @@
         <v>3345</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>43926</v>
       </c>
@@ -3809,7 +4021,7 @@
         <v>3706</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>43927</v>
       </c>
@@ -3859,7 +4071,7 @@
         <v>3961</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>43928</v>
       </c>
@@ -3909,7 +4121,7 @@
         <v>4229</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>43929</v>
       </c>
@@ -3959,7 +4171,7 @@
         <v>4565</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>43930</v>
       </c>
@@ -4009,7 +4221,7 @@
         <v>4957</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>43931</v>
       </c>
@@ -4059,7 +4271,7 @@
         <v>5275</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>43932</v>
       </c>
@@ -4109,7 +4321,7 @@
         <v>5590</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>43933</v>
       </c>
@@ -4159,7 +4371,7 @@
         <v>5912</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>43934</v>
       </c>
@@ -4209,7 +4421,7 @@
         <v>6067</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>43935</v>
       </c>
@@ -4259,7 +4471,7 @@
         <v>6358</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>43936</v>
       </c>
@@ -4309,7 +4521,7 @@
         <v>6748</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
         <v>43937</v>
       </c>
@@ -4359,7 +4571,7 @@
         <v>7102</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>43938</v>
       </c>
@@ -4409,7 +4621,7 @@
         <v>7409</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A46" s="5">
         <v>43939</v>
       </c>
@@ -4459,7 +4671,7 @@
         <v>7820</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A47" s="5">
         <v>43940</v>
       </c>
@@ -4509,7 +4721,7 @@
         <v>8187</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A48" s="5">
         <v>43941</v>
       </c>
@@ -4559,7 +4771,7 @@
         <v>8450</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A49" s="5">
         <v>43942</v>
       </c>
@@ -4609,7 +4821,7 @@
         <v>8672</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
         <v>43943</v>
       </c>
@@ -4659,7 +4871,7 @@
         <v>9038</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
         <v>43944</v>
       </c>
@@ -4709,7 +4921,7 @@
         <v>9409</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
         <v>43945</v>
       </c>
@@ -4759,7 +4971,7 @@
         <v>9697</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
         <v>43946</v>
       </c>
@@ -4809,7 +5021,7 @@
         <v>10051</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A54" s="5">
         <v>43947</v>
       </c>
@@ -4860,7 +5072,7 @@
       </c>
       <c r="R54" s="38"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
         <v>43948</v>
       </c>
@@ -4911,7 +5123,7 @@
       </c>
       <c r="R55" s="38"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A56" s="5">
         <v>43949</v>
       </c>
@@ -4962,7 +5174,7 @@
       </c>
       <c r="R56" s="39"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
         <v>43950</v>
       </c>
@@ -5012,7 +5224,7 @@
         <v>11034</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
         <v>43951</v>
       </c>
@@ -5063,7 +5275,7 @@
       </c>
       <c r="R58" s="38"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>43952</v>
       </c>
@@ -5115,7 +5327,7 @@
       <c r="R59" s="38"/>
       <c r="S59" s="38"/>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
         <v>43953</v>
       </c>
@@ -5165,7 +5377,7 @@
         <v>11927</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
         <v>43954</v>
       </c>
@@ -5215,7 +5427,7 @@
         <v>12097</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A62" s="5">
         <v>43955</v>
       </c>
@@ -5265,7 +5477,7 @@
         <v>12266</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A63" s="5">
         <v>43956</v>
       </c>
@@ -5315,7 +5527,7 @@
         <v>12437</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
         <v>43957</v>
       </c>
@@ -5365,7 +5577,7 @@
         <v>12709</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>43958</v>
       </c>
@@ -5415,7 +5627,7 @@
         <v>12924</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
         <v>43959</v>
       </c>
@@ -5465,7 +5677,7 @@
         <v>13149</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
         <v>43960</v>
       </c>
@@ -5515,7 +5727,7 @@
         <v>13305</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A68" s="5">
         <v>43961</v>
       </c>
@@ -5565,7 +5777,7 @@
         <v>13486</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A69" s="5">
         <v>43962</v>
       </c>
@@ -5615,7 +5827,7 @@
         <v>13627</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A70" s="5">
         <v>43963</v>
       </c>
@@ -5665,7 +5877,7 @@
         <v>13763</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A71" s="5">
         <v>43964</v>
       </c>
@@ -5715,7 +5927,7 @@
         <v>13929</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A72" s="5">
         <v>43965</v>
       </c>
@@ -5765,7 +5977,7 @@
         <v>14117</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A73" s="5">
         <v>43966</v>
       </c>
@@ -5815,7 +6027,7 @@
         <v>14260</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A74" s="5">
         <v>43967</v>
       </c>
@@ -5865,7 +6077,7 @@
         <v>14447</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A75" s="5">
         <v>43968</v>
       </c>
@@ -5915,7 +6127,7 @@
         <v>14537</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A76" s="5">
         <v>43969</v>
       </c>
@@ -5965,7 +6177,7 @@
         <v>14594</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A77" s="5">
         <v>43970</v>
       </c>
@@ -6015,7 +6227,7 @@
         <v>14655</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A78" s="5">
         <v>43971</v>
       </c>
@@ -6065,7 +6277,7 @@
         <v>14751</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A79" s="5">
         <v>43972</v>
       </c>
@@ -6115,7 +6327,7 @@
         <v>14856</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A80" s="5">
         <v>43973</v>
       </c>
@@ -6165,7 +6377,7 @@
         <v>14969</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A81" s="5">
         <v>43974</v>
       </c>
@@ -6215,7 +6427,7 @@
         <v>15041</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A82" s="5">
         <v>43975</v>
       </c>
@@ -6265,7 +6477,7 @@
         <v>15101</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A83" s="5">
         <v>43976</v>
       </c>
@@ -6315,7 +6527,7 @@
         <v>15156</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A84" s="5">
         <v>43977</v>
       </c>
@@ -6365,7 +6577,7 @@
         <v>15185</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A85" s="5">
         <v>43978</v>
       </c>
@@ -6415,7 +6627,7 @@
         <v>15240</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A86" s="5">
         <v>43979</v>
       </c>
@@ -6465,7 +6677,7 @@
         <v>15288</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A87" s="5">
         <v>43980</v>
       </c>
@@ -6515,7 +6727,7 @@
         <v>15327</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A88" s="5">
         <v>43981</v>
       </c>
@@ -6565,7 +6777,7 @@
         <v>15382</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A89" s="5">
         <v>43982</v>
       </c>
@@ -6615,7 +6827,7 @@
         <v>15400</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A90" s="5">
         <v>43983</v>
       </c>
@@ -6665,7 +6877,7 @@
         <v>15418</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A91" s="5">
         <v>43984</v>
       </c>
@@ -6715,7 +6927,7 @@
         <v>15471</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A92" s="5">
         <v>43985</v>
       </c>
@@ -6765,7 +6977,7 @@
         <v>15504</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A93" s="5">
         <v>43986</v>
       </c>
@@ -6815,7 +7027,7 @@
         <v>15553</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A94" s="5">
         <v>43987</v>
       </c>
@@ -6865,7 +7077,7 @@
         <v>15582</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A95" s="5">
         <v>43988</v>
       </c>
@@ -6915,7 +7127,7 @@
         <v>15603</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A96" s="5">
         <v>43989</v>
       </c>
@@ -6965,7 +7177,7 @@
         <v>15621</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A97" s="5">
         <v>43990</v>
       </c>
@@ -7015,7 +7227,7 @@
         <v>15639</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A98" s="5">
         <v>43991</v>
       </c>
@@ -7065,7 +7277,7 @@
         <v>15653</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A99" s="5">
         <v>43992</v>
       </c>
@@ -7115,7 +7327,7 @@
         <v>15665</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A100" s="5">
         <v>43993</v>
       </c>
@@ -7165,7 +7377,7 @@
         <v>15682</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A101" s="5">
         <v>43994</v>
       </c>
@@ -7215,7 +7427,7 @@
         <v>15709</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A102" s="5">
         <v>43995</v>
       </c>
@@ -7265,7 +7477,7 @@
         <v>15730</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A103" s="55">
         <v>43996</v>
       </c>
@@ -7315,7 +7527,7 @@
         <v>15755</v>
       </c>
     </row>
-    <row r="104" spans="1:16" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" s="5">
         <v>43997</v>
       </c>
@@ -7365,7 +7577,7 @@
         <v>18030</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A105" s="5">
         <v>43998</v>
       </c>
@@ -7415,7 +7627,7 @@
         <v>18045</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A106" s="5">
         <v>43999</v>
       </c>
@@ -7465,7 +7677,7 @@
         <v>18066</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A107" s="5">
         <v>44000</v>
       </c>
@@ -7515,7 +7727,7 @@
         <v>18077</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A108" s="5">
         <v>44001</v>
       </c>
@@ -7565,23 +7777,57 @@
         <v>18104</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C109" s="28"/>
-      <c r="D109" s="28"/>
-      <c r="E109" s="28"/>
-      <c r="F109" s="28"/>
-      <c r="G109" s="28"/>
-      <c r="H109" s="28"/>
-      <c r="I109" s="28"/>
-      <c r="J109" s="28"/>
-      <c r="K109" s="28"/>
-      <c r="L109" s="28"/>
-      <c r="M109" s="28"/>
-      <c r="N109" s="28"/>
-      <c r="O109" s="28"/>
-      <c r="P109" s="28"/>
-    </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A109" s="5">
+        <v>44002</v>
+      </c>
+      <c r="B109" s="28">
+        <v>1249</v>
+      </c>
+      <c r="C109" s="28">
+        <v>345</v>
+      </c>
+      <c r="D109" s="28">
+        <v>284</v>
+      </c>
+      <c r="E109" s="28">
+        <v>928</v>
+      </c>
+      <c r="F109" s="28">
+        <v>1055</v>
+      </c>
+      <c r="G109" s="28">
+        <v>1410</v>
+      </c>
+      <c r="H109" s="28">
+        <v>4819</v>
+      </c>
+      <c r="I109" s="28">
+        <v>373</v>
+      </c>
+      <c r="J109" s="28">
+        <v>2698</v>
+      </c>
+      <c r="K109" s="28">
+        <v>3139</v>
+      </c>
+      <c r="L109" s="28">
+        <v>9</v>
+      </c>
+      <c r="M109" s="28">
+        <v>54</v>
+      </c>
+      <c r="N109" s="28">
+        <v>1760</v>
+      </c>
+      <c r="O109" s="28">
+        <v>7</v>
+      </c>
+      <c r="P109" s="32">
+        <v>18130</v>
+      </c>
+    </row>
+    <row r="110" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B110" s="28"/>
       <c r="C110" s="28"/>
       <c r="D110" s="28"/>
@@ -7598,7 +7844,7 @@
       <c r="O110" s="28"/>
       <c r="P110" s="28"/>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B111" s="28"/>
       <c r="C111" s="28"/>
       <c r="D111" s="28"/>
@@ -7615,7 +7861,7 @@
       <c r="O111" s="28"/>
       <c r="P111" s="28"/>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B112" s="28"/>
       <c r="C112" s="28"/>
       <c r="D112" s="28"/>
@@ -7632,7 +7878,7 @@
       <c r="O112" s="28"/>
       <c r="P112" s="28"/>
     </row>
-    <row r="113" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B113" s="28"/>
       <c r="C113" s="28"/>
       <c r="D113" s="28"/>
@@ -7649,7 +7895,7 @@
       <c r="O113" s="28"/>
       <c r="P113" s="28"/>
     </row>
-    <row r="114" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B114" s="28"/>
       <c r="C114" s="28"/>
       <c r="D114" s="28"/>
@@ -7666,7 +7912,7 @@
       <c r="O114" s="28"/>
       <c r="P114" s="28"/>
     </row>
-    <row r="115" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B115" s="28"/>
       <c r="C115" s="28"/>
       <c r="D115" s="28"/>
@@ -7683,7 +7929,7 @@
       <c r="O115" s="28"/>
       <c r="P115" s="28"/>
     </row>
-    <row r="116" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B116" s="28"/>
       <c r="C116" s="28"/>
       <c r="D116" s="28"/>
@@ -7700,7 +7946,7 @@
       <c r="O116" s="28"/>
       <c r="P116" s="28"/>
     </row>
-    <row r="117" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B117" s="28"/>
       <c r="C117" s="28"/>
       <c r="D117" s="28"/>
@@ -7717,7 +7963,7 @@
       <c r="O117" s="28"/>
       <c r="P117" s="28"/>
     </row>
-    <row r="118" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B118" s="28"/>
       <c r="C118" s="28"/>
       <c r="D118" s="28"/>
@@ -7734,7 +7980,7 @@
       <c r="O118" s="28"/>
       <c r="P118" s="28"/>
     </row>
-    <row r="119" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B119" s="28"/>
       <c r="C119" s="28"/>
       <c r="D119" s="28"/>
@@ -7751,7 +7997,7 @@
       <c r="O119" s="28"/>
       <c r="P119" s="28"/>
     </row>
-    <row r="120" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B120" s="28"/>
       <c r="C120" s="28"/>
       <c r="D120" s="28"/>
@@ -7768,7 +8014,7 @@
       <c r="O120" s="28"/>
       <c r="P120" s="28"/>
     </row>
-    <row r="121" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B121" s="28"/>
       <c r="C121" s="28"/>
       <c r="D121" s="28"/>
@@ -7785,7 +8031,7 @@
       <c r="O121" s="28"/>
       <c r="P121" s="28"/>
     </row>
-    <row r="122" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B122" s="28"/>
       <c r="C122" s="28"/>
       <c r="D122" s="28"/>
@@ -7802,7 +8048,7 @@
       <c r="O122" s="28"/>
       <c r="P122" s="28"/>
     </row>
-    <row r="123" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B123" s="28"/>
       <c r="C123" s="28"/>
       <c r="D123" s="28"/>
@@ -7819,7 +8065,7 @@
       <c r="O123" s="28"/>
       <c r="P123" s="28"/>
     </row>
-    <row r="124" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B124" s="28"/>
       <c r="C124" s="28"/>
       <c r="D124" s="28"/>
@@ -7836,7 +8082,7 @@
       <c r="O124" s="28"/>
       <c r="P124" s="28"/>
     </row>
-    <row r="125" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B125" s="28"/>
       <c r="C125" s="28"/>
       <c r="D125" s="28"/>
@@ -7853,7 +8099,7 @@
       <c r="O125" s="28"/>
       <c r="P125" s="28"/>
     </row>
-    <row r="126" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B126" s="28"/>
       <c r="C126" s="28"/>
       <c r="D126" s="28"/>
@@ -7870,7 +8116,7 @@
       <c r="O126" s="28"/>
       <c r="P126" s="28"/>
     </row>
-    <row r="127" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B127" s="28"/>
       <c r="C127" s="28"/>
       <c r="D127" s="28"/>
@@ -7887,7 +8133,7 @@
       <c r="O127" s="28"/>
       <c r="P127" s="28"/>
     </row>
-    <row r="128" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B128" s="28"/>
       <c r="C128" s="28"/>
       <c r="D128" s="28"/>
@@ -7904,7 +8150,7 @@
       <c r="O128" s="28"/>
       <c r="P128" s="28"/>
     </row>
-    <row r="129" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B129" s="28"/>
       <c r="C129" s="28"/>
       <c r="D129" s="28"/>
@@ -7921,7 +8167,7 @@
       <c r="O129" s="28"/>
       <c r="P129" s="28"/>
     </row>
-    <row r="130" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B130" s="28"/>
       <c r="C130" s="28"/>
       <c r="D130" s="28"/>
@@ -7938,7 +8184,7 @@
       <c r="O130" s="28"/>
       <c r="P130" s="28"/>
     </row>
-    <row r="131" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B131" s="28"/>
       <c r="C131" s="28"/>
       <c r="D131" s="28"/>
@@ -7955,7 +8201,7 @@
       <c r="O131" s="28"/>
       <c r="P131" s="28"/>
     </row>
-    <row r="132" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B132" s="28"/>
       <c r="C132" s="28"/>
       <c r="D132" s="28"/>
@@ -7972,7 +8218,7 @@
       <c r="O132" s="28"/>
       <c r="P132" s="28"/>
     </row>
-    <row r="133" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B133" s="28"/>
       <c r="C133" s="28"/>
       <c r="D133" s="28"/>
@@ -7989,7 +8235,7 @@
       <c r="O133" s="28"/>
       <c r="P133" s="28"/>
     </row>
-    <row r="134" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B134" s="28"/>
       <c r="C134" s="28"/>
       <c r="D134" s="28"/>
@@ -8006,7 +8252,7 @@
       <c r="O134" s="28"/>
       <c r="P134" s="28"/>
     </row>
-    <row r="135" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B135" s="28"/>
       <c r="C135" s="28"/>
       <c r="D135" s="28"/>
@@ -8023,7 +8269,7 @@
       <c r="O135" s="28"/>
       <c r="P135" s="28"/>
     </row>
-    <row r="136" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B136" s="28"/>
       <c r="C136" s="28"/>
       <c r="D136" s="28"/>
@@ -8040,7 +8286,7 @@
       <c r="O136" s="28"/>
       <c r="P136" s="28"/>
     </row>
-    <row r="137" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B137" s="28"/>
       <c r="C137" s="28"/>
       <c r="D137" s="28"/>
@@ -8057,7 +8303,7 @@
       <c r="O137" s="28"/>
       <c r="P137" s="28"/>
     </row>
-    <row r="138" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B138" s="28"/>
       <c r="C138" s="28"/>
       <c r="D138" s="28"/>
@@ -8074,7 +8320,7 @@
       <c r="O138" s="28"/>
       <c r="P138" s="28"/>
     </row>
-    <row r="139" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B139" s="28"/>
       <c r="C139" s="28"/>
       <c r="D139" s="28"/>
@@ -8091,7 +8337,7 @@
       <c r="O139" s="28"/>
       <c r="P139" s="28"/>
     </row>
-    <row r="140" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B140" s="28"/>
       <c r="C140" s="28"/>
       <c r="D140" s="28"/>
@@ -8108,7 +8354,7 @@
       <c r="O140" s="28"/>
       <c r="P140" s="28"/>
     </row>
-    <row r="141" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B141" s="28"/>
       <c r="C141" s="28"/>
       <c r="D141" s="28"/>
@@ -8125,7 +8371,7 @@
       <c r="O141" s="28"/>
       <c r="P141" s="28"/>
     </row>
-    <row r="142" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B142" s="28"/>
       <c r="C142" s="28"/>
       <c r="D142" s="28"/>
@@ -8142,7 +8388,7 @@
       <c r="O142" s="28"/>
       <c r="P142" s="28"/>
     </row>
-    <row r="143" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B143" s="28"/>
       <c r="C143" s="28"/>
       <c r="D143" s="28"/>
@@ -8159,7 +8405,7 @@
       <c r="O143" s="28"/>
       <c r="P143" s="28"/>
     </row>
-    <row r="144" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B144" s="28"/>
       <c r="C144" s="28"/>
       <c r="D144" s="28"/>
@@ -8176,7 +8422,7 @@
       <c r="O144" s="28"/>
       <c r="P144" s="28"/>
     </row>
-    <row r="145" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B145" s="28"/>
       <c r="C145" s="28"/>
       <c r="D145" s="28"/>
@@ -8193,7 +8439,7 @@
       <c r="O145" s="28"/>
       <c r="P145" s="28"/>
     </row>
-    <row r="146" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B146" s="28"/>
       <c r="C146" s="28"/>
       <c r="D146" s="28"/>
@@ -8210,7 +8456,7 @@
       <c r="O146" s="28"/>
       <c r="P146" s="28"/>
     </row>
-    <row r="147" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B147" s="28"/>
       <c r="C147" s="28"/>
       <c r="D147" s="28"/>
@@ -8227,7 +8473,7 @@
       <c r="O147" s="28"/>
       <c r="P147" s="28"/>
     </row>
-    <row r="148" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B148" s="28"/>
       <c r="C148" s="28"/>
       <c r="D148" s="28"/>
@@ -8244,7 +8490,7 @@
       <c r="O148" s="28"/>
       <c r="P148" s="28"/>
     </row>
-    <row r="149" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B149" s="28"/>
       <c r="C149" s="28"/>
       <c r="D149" s="28"/>
@@ -8261,7 +8507,7 @@
       <c r="O149" s="28"/>
       <c r="P149" s="28"/>
     </row>
-    <row r="150" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B150" s="28"/>
       <c r="C150" s="28"/>
       <c r="D150" s="28"/>
@@ -8278,7 +8524,7 @@
       <c r="O150" s="28"/>
       <c r="P150" s="28"/>
     </row>
-    <row r="151" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B151" s="28"/>
       <c r="C151" s="28"/>
       <c r="D151" s="28"/>
@@ -8295,7 +8541,7 @@
       <c r="O151" s="28"/>
       <c r="P151" s="28"/>
     </row>
-    <row r="152" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B152" s="28"/>
       <c r="C152" s="28"/>
       <c r="D152" s="28"/>
@@ -8312,7 +8558,7 @@
       <c r="O152" s="28"/>
       <c r="P152" s="28"/>
     </row>
-    <row r="153" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B153" s="28"/>
       <c r="C153" s="28"/>
       <c r="D153" s="28"/>
@@ -8329,7 +8575,7 @@
       <c r="O153" s="28"/>
       <c r="P153" s="28"/>
     </row>
-    <row r="154" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B154" s="28"/>
       <c r="C154" s="28"/>
       <c r="D154" s="28"/>
@@ -8346,7 +8592,7 @@
       <c r="O154" s="28"/>
       <c r="P154" s="28"/>
     </row>
-    <row r="155" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B155" s="28"/>
       <c r="C155" s="28"/>
       <c r="D155" s="28"/>
@@ -8363,7 +8609,7 @@
       <c r="O155" s="28"/>
       <c r="P155" s="28"/>
     </row>
-    <row r="156" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B156" s="28"/>
       <c r="C156" s="28"/>
       <c r="D156" s="28"/>
@@ -8380,7 +8626,7 @@
       <c r="O156" s="28"/>
       <c r="P156" s="28"/>
     </row>
-    <row r="157" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B157" s="28"/>
       <c r="C157" s="28"/>
       <c r="D157" s="28"/>
@@ -8397,7 +8643,7 @@
       <c r="O157" s="28"/>
       <c r="P157" s="28"/>
     </row>
-    <row r="158" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B158" s="28"/>
       <c r="C158" s="28"/>
       <c r="D158" s="28"/>
@@ -8414,7 +8660,7 @@
       <c r="O158" s="28"/>
       <c r="P158" s="28"/>
     </row>
-    <row r="159" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B159" s="28"/>
       <c r="C159" s="28"/>
       <c r="D159" s="28"/>
@@ -8431,7 +8677,7 @@
       <c r="O159" s="28"/>
       <c r="P159" s="28"/>
     </row>
-    <row r="160" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B160" s="28"/>
       <c r="C160" s="28"/>
       <c r="D160" s="28"/>
@@ -8457,21 +8703,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q97"/>
+  <dimension ref="A1:Q98"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A98" sqref="A98"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S93" sqref="S93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5703125" style="2"/>
+    <col min="1" max="1" width="12.453125" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.54296875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -8492,7 +8738,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -8513,7 +8759,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -8566,7 +8812,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="12">
         <v>43908</v>
       </c>
@@ -8619,7 +8865,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
         <v>43909</v>
       </c>
@@ -8672,7 +8918,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="12">
         <v>43910</v>
       </c>
@@ -8725,7 +8971,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
         <v>43911</v>
       </c>
@@ -8778,7 +9024,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="12">
         <v>43912</v>
       </c>
@@ -8831,7 +9077,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="12">
         <v>43913</v>
       </c>
@@ -8884,7 +9130,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="12">
         <v>43914</v>
       </c>
@@ -8937,7 +9183,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
         <v>43915</v>
       </c>
@@ -8990,7 +9236,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="12">
         <v>43916</v>
       </c>
@@ -9043,7 +9289,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <v>43917</v>
       </c>
@@ -9096,7 +9342,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>43918</v>
       </c>
@@ -9149,7 +9395,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="12">
         <v>43919</v>
       </c>
@@ -9202,7 +9448,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="12">
         <v>43920</v>
       </c>
@@ -9255,7 +9501,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="12">
         <v>43921</v>
       </c>
@@ -9308,7 +9554,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="12">
         <v>43922</v>
       </c>
@@ -9361,7 +9607,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="12">
         <v>43923</v>
       </c>
@@ -9414,7 +9660,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="12">
         <v>43924</v>
       </c>
@@ -9467,7 +9713,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="12">
         <v>43925</v>
       </c>
@@ -9520,7 +9766,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="12">
         <v>43926</v>
       </c>
@@ -9573,7 +9819,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="12">
         <v>43927</v>
       </c>
@@ -9626,7 +9872,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" s="12">
         <v>43928</v>
       </c>
@@ -9679,7 +9925,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" s="12">
         <v>43929</v>
       </c>
@@ -9732,7 +9978,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" s="12">
         <v>43930</v>
       </c>
@@ -9785,7 +10031,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" s="12">
         <v>43931</v>
       </c>
@@ -9838,7 +10084,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" s="12">
         <v>43932</v>
       </c>
@@ -9891,7 +10137,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" s="12">
         <v>43933</v>
       </c>
@@ -9944,7 +10190,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" s="12">
         <v>43934</v>
       </c>
@@ -9997,7 +10243,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="12">
         <v>43935</v>
       </c>
@@ -10050,7 +10296,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" s="12">
         <v>43936</v>
       </c>
@@ -10103,7 +10349,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" s="12">
         <v>43937</v>
       </c>
@@ -10156,7 +10402,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" s="12">
         <v>43938</v>
       </c>
@@ -10209,7 +10455,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" s="12">
         <v>43939</v>
       </c>
@@ -10262,7 +10508,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" s="30">
         <v>43940</v>
       </c>
@@ -10315,7 +10561,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" s="30">
         <v>43941</v>
       </c>
@@ -10368,7 +10614,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" s="30">
         <v>43942</v>
       </c>
@@ -10421,7 +10667,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" s="30">
         <v>43943</v>
       </c>
@@ -10474,7 +10720,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" s="30">
         <v>43944</v>
       </c>
@@ -10527,7 +10773,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" s="30">
         <v>43945</v>
       </c>
@@ -10580,7 +10826,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" s="30">
         <v>43946</v>
       </c>
@@ -10633,7 +10879,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" s="30">
         <v>43947</v>
       </c>
@@ -10686,7 +10932,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" s="30">
         <v>43948</v>
       </c>
@@ -10739,7 +10985,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" s="30">
         <v>43949</v>
       </c>
@@ -10792,7 +11038,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" s="30">
         <v>43950</v>
       </c>
@@ -10845,7 +11091,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" s="30">
         <v>43951</v>
       </c>
@@ -10898,7 +11144,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" s="30">
         <v>43952</v>
       </c>
@@ -10951,7 +11197,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" s="30">
         <v>43953</v>
       </c>
@@ -11004,7 +11250,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50" s="30">
         <v>43954</v>
       </c>
@@ -11057,7 +11303,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51" s="30">
         <v>43955</v>
       </c>
@@ -11110,7 +11356,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52" s="30">
         <v>43956</v>
       </c>
@@ -11163,7 +11409,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53" s="30">
         <v>43957</v>
       </c>
@@ -11216,7 +11462,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54" s="30">
         <v>43958</v>
       </c>
@@ -11269,7 +11515,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55" s="30">
         <v>43959</v>
       </c>
@@ -11322,7 +11568,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56" s="30">
         <v>43960</v>
       </c>
@@ -11375,7 +11621,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A57" s="30">
         <v>43961</v>
       </c>
@@ -11428,7 +11674,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A58" s="30">
         <v>43962</v>
       </c>
@@ -11481,7 +11727,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A59" s="30">
         <v>43963</v>
       </c>
@@ -11534,7 +11780,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A60" s="30">
         <v>43964</v>
       </c>
@@ -11587,7 +11833,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A61" s="30">
         <v>43965</v>
       </c>
@@ -11640,7 +11886,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A62" s="30">
         <v>43966</v>
       </c>
@@ -11693,7 +11939,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A63" s="30">
         <v>43967</v>
       </c>
@@ -11746,7 +11992,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A64" s="30">
         <v>43968</v>
       </c>
@@ -11799,7 +12045,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A65" s="30">
         <v>43969</v>
       </c>
@@ -11852,7 +12098,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A66" s="30">
         <v>43970</v>
       </c>
@@ -11905,7 +12151,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A67" s="30">
         <v>43971</v>
       </c>
@@ -11958,7 +12204,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A68" s="30">
         <v>43972</v>
       </c>
@@ -12011,7 +12257,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A69" s="30">
         <v>43973</v>
       </c>
@@ -12064,7 +12310,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A70" s="30">
         <v>43974</v>
       </c>
@@ -12117,7 +12363,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A71" s="30">
         <v>43975</v>
       </c>
@@ -12170,7 +12416,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A72" s="30">
         <v>43976</v>
       </c>
@@ -12223,7 +12469,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A73" s="30">
         <v>43977</v>
       </c>
@@ -12276,7 +12522,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A74" s="30">
         <v>43978</v>
       </c>
@@ -12329,7 +12575,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A75" s="30">
         <v>43979</v>
       </c>
@@ -12382,7 +12628,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A76" s="30">
         <v>43980</v>
       </c>
@@ -12435,7 +12681,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A77" s="30">
         <v>43981</v>
       </c>
@@ -12488,7 +12734,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A78" s="30">
         <v>43982</v>
       </c>
@@ -12541,7 +12787,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A79" s="30">
         <v>43983</v>
       </c>
@@ -12594,7 +12840,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A80" s="30">
         <v>43984</v>
       </c>
@@ -12647,7 +12893,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A81" s="30">
         <v>43985</v>
       </c>
@@ -12700,7 +12946,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A82" s="30">
         <v>43986</v>
       </c>
@@ -12753,7 +12999,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A83" s="30">
         <v>43987</v>
       </c>
@@ -12806,7 +13052,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A84" s="30">
         <v>43988</v>
       </c>
@@ -12859,7 +13105,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A85" s="30">
         <v>43989</v>
       </c>
@@ -12912,7 +13158,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A86" s="30">
         <v>43990</v>
       </c>
@@ -12965,7 +13211,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A87" s="30">
         <v>43991</v>
       </c>
@@ -13018,7 +13264,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A88" s="30">
         <v>43992</v>
       </c>
@@ -13071,7 +13317,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A89" s="30">
         <v>43993</v>
       </c>
@@ -13124,7 +13370,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A90" s="30">
         <v>43994</v>
       </c>
@@ -13177,7 +13423,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A91" s="30">
         <v>43995</v>
       </c>
@@ -13230,7 +13476,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A92" s="30">
         <v>43996</v>
       </c>
@@ -13283,7 +13529,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A93" s="30">
         <v>43997</v>
       </c>
@@ -13336,7 +13582,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A94" s="30">
         <v>43998</v>
       </c>
@@ -13389,7 +13635,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A95" s="30">
         <v>43999</v>
       </c>
@@ -13442,7 +13688,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A96" s="30">
         <v>44000</v>
       </c>
@@ -13495,7 +13741,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A97" s="30">
         <v>44001</v>
       </c>
@@ -13546,6 +13792,59 @@
       </c>
       <c r="Q97" s="13">
         <v>19</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A98" s="30">
+        <v>44002</v>
+      </c>
+      <c r="B98" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C98" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D98" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E98" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F98" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G98" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H98" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I98" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J98" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K98" s="11">
+        <v>6</v>
+      </c>
+      <c r="L98" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M98" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N98" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O98" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P98" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q98" s="13">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -13556,23 +13855,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R89"/>
+  <dimension ref="A1:R90"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="E83" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="E61" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A90" sqref="A90"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5703125" style="2"/>
+    <col min="1" max="1" width="15.453125" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.54296875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -13593,7 +13892,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -13614,7 +13913,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -13667,7 +13966,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="12">
         <v>43916</v>
       </c>
@@ -13720,7 +14019,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
         <v>43917</v>
       </c>
@@ -13773,7 +14072,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="12">
         <v>43918</v>
       </c>
@@ -13826,7 +14125,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
         <v>43919</v>
       </c>
@@ -13879,7 +14178,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="12">
         <v>43920</v>
       </c>
@@ -13932,7 +14231,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="12">
         <v>43921</v>
       </c>
@@ -13985,7 +14284,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="12">
         <v>43922</v>
       </c>
@@ -14038,7 +14337,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
         <v>43923</v>
       </c>
@@ -14091,7 +14390,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="12">
         <v>43924</v>
       </c>
@@ -14144,7 +14443,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <v>43925</v>
       </c>
@@ -14197,7 +14496,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>43926</v>
       </c>
@@ -14250,7 +14549,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="12">
         <v>43927</v>
       </c>
@@ -14303,7 +14602,7 @@
         <v>1262</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="12">
         <v>43928</v>
       </c>
@@ -14356,7 +14655,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="12">
         <v>43929</v>
       </c>
@@ -14409,7 +14708,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="12">
         <v>43930</v>
       </c>
@@ -14462,7 +14761,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="12">
         <v>43931</v>
       </c>
@@ -14515,7 +14814,7 @@
         <v>1461</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="12">
         <v>43932</v>
       </c>
@@ -14568,7 +14867,7 @@
         <v>1467</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="12">
         <v>43933</v>
       </c>
@@ -14621,7 +14920,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="12">
         <v>43934</v>
       </c>
@@ -14674,7 +14973,7 @@
         <v>1482</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="12">
         <v>43935</v>
       </c>
@@ -14727,7 +15026,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" s="12">
         <v>43936</v>
       </c>
@@ -14780,7 +15079,7 @@
         <v>1486</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" s="12">
         <v>43937</v>
       </c>
@@ -14833,7 +15132,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" s="12">
         <v>43938</v>
       </c>
@@ -14886,7 +15185,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" s="12">
         <v>43939</v>
       </c>
@@ -14939,7 +15238,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" s="12">
         <v>43940</v>
       </c>
@@ -14992,7 +15291,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" s="12">
         <v>43941</v>
       </c>
@@ -15045,7 +15344,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" s="12">
         <v>43942</v>
       </c>
@@ -15098,7 +15397,7 @@
         <v>1472</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="12">
         <v>43943</v>
       </c>
@@ -15151,7 +15450,7 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" s="12">
         <v>43944</v>
       </c>
@@ -15204,7 +15503,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" s="12">
         <v>43945</v>
       </c>
@@ -15257,7 +15556,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" s="12">
         <v>43946</v>
       </c>
@@ -15310,7 +15609,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" s="12">
         <v>43947</v>
       </c>
@@ -15363,7 +15662,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" s="30">
         <v>43948</v>
       </c>
@@ -15416,7 +15715,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" s="30">
         <v>43949</v>
       </c>
@@ -15469,7 +15768,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" s="30">
         <v>43950</v>
       </c>
@@ -15522,7 +15821,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" s="30">
         <v>43951</v>
       </c>
@@ -15575,7 +15874,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" s="30">
         <v>43952</v>
       </c>
@@ -15628,7 +15927,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" s="30">
         <v>43953</v>
       </c>
@@ -15681,7 +15980,7 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" s="30">
         <v>43954</v>
       </c>
@@ -15734,7 +16033,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" s="30">
         <v>43955</v>
       </c>
@@ -15787,7 +16086,7 @@
         <v>1279</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" s="30">
         <v>43956</v>
       </c>
@@ -15840,7 +16139,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" s="30">
         <v>43957</v>
       </c>
@@ -15893,7 +16192,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" s="30">
         <v>43958</v>
       </c>
@@ -15946,7 +16245,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" s="30">
         <v>43959</v>
       </c>
@@ -15999,7 +16298,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" s="30">
         <v>43960</v>
       </c>
@@ -16052,7 +16351,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" s="30">
         <v>43961</v>
       </c>
@@ -16105,7 +16404,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50" s="30">
         <v>43962</v>
       </c>
@@ -16158,7 +16457,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51" s="30">
         <v>43963</v>
       </c>
@@ -16211,7 +16510,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52" s="30">
         <v>43964</v>
       </c>
@@ -16264,7 +16563,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53" s="30">
         <v>43965</v>
       </c>
@@ -16317,7 +16616,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54" s="30">
         <v>43966</v>
       </c>
@@ -16370,7 +16669,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55" s="30">
         <v>43967</v>
       </c>
@@ -16423,7 +16722,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56" s="30">
         <v>43968</v>
       </c>
@@ -16476,7 +16775,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A57" s="30">
         <v>43969</v>
       </c>
@@ -16529,7 +16828,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A58" s="30">
         <v>43970</v>
       </c>
@@ -16582,7 +16881,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A59" s="30">
         <v>43971</v>
       </c>
@@ -16635,7 +16934,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A60" s="30">
         <v>43972</v>
       </c>
@@ -16688,7 +16987,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A61" s="30">
         <v>43973</v>
       </c>
@@ -16741,7 +17040,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A62" s="30">
         <v>43974</v>
       </c>
@@ -16794,7 +17093,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A63" s="30">
         <v>43975</v>
       </c>
@@ -16847,7 +17146,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A64" s="30">
         <v>43976</v>
       </c>
@@ -16900,7 +17199,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A65" s="51">
         <v>43977</v>
       </c>
@@ -16953,7 +17252,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A66" s="51">
         <v>43978</v>
       </c>
@@ -17006,7 +17305,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A67" s="51">
         <v>43979</v>
       </c>
@@ -17059,7 +17358,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A68" s="51">
         <v>43980</v>
       </c>
@@ -17112,7 +17411,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A69" s="51">
         <v>43981</v>
       </c>
@@ -17165,7 +17464,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A70" s="51">
         <v>43982</v>
       </c>
@@ -17218,7 +17517,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A71" s="51">
         <v>43983</v>
       </c>
@@ -17271,7 +17570,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A72" s="51">
         <v>43984</v>
       </c>
@@ -17324,7 +17623,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A73" s="51">
         <v>43985</v>
       </c>
@@ -17377,7 +17676,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A74" s="51">
         <v>43986</v>
       </c>
@@ -17430,7 +17729,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A75" s="51">
         <v>43987</v>
       </c>
@@ -17483,7 +17782,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A76" s="51">
         <v>43988</v>
       </c>
@@ -17536,7 +17835,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A77" s="51">
         <v>43989</v>
       </c>
@@ -17589,7 +17888,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A78" s="51">
         <v>43990</v>
       </c>
@@ -17642,7 +17941,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A79" s="51">
         <v>43991</v>
       </c>
@@ -17695,7 +17994,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A80" s="51">
         <v>43992</v>
       </c>
@@ -17749,7 +18048,7 @@
       </c>
       <c r="R80" s="54"/>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A81" s="51">
         <v>43993</v>
       </c>
@@ -17803,7 +18102,7 @@
       </c>
       <c r="R81" s="54"/>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A82" s="51">
         <v>43994</v>
       </c>
@@ -17857,7 +18156,7 @@
       </c>
       <c r="R82" s="54"/>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A83" s="51">
         <v>43995</v>
       </c>
@@ -17910,7 +18209,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A84" s="51">
         <v>43996</v>
       </c>
@@ -17963,7 +18262,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A85" s="51">
         <v>43997</v>
       </c>
@@ -18016,7 +18315,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A86" s="51">
         <v>43998</v>
       </c>
@@ -18069,7 +18368,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A87" s="51">
         <v>43999</v>
       </c>
@@ -18122,7 +18421,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A88" s="51">
         <v>44000</v>
       </c>
@@ -18175,7 +18474,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A89" s="51">
         <v>44001</v>
       </c>
@@ -18226,33 +18525,87 @@
       </c>
       <c r="Q89" s="13">
         <v>528</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A90" s="51">
+        <v>44002</v>
+      </c>
+      <c r="B90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E90" s="11">
+        <v>52</v>
+      </c>
+      <c r="F90" s="11">
+        <v>5</v>
+      </c>
+      <c r="G90" s="11">
+        <v>46</v>
+      </c>
+      <c r="H90" s="11">
+        <v>234</v>
+      </c>
+      <c r="I90" s="11">
+        <v>7</v>
+      </c>
+      <c r="J90" s="11">
+        <v>39</v>
+      </c>
+      <c r="K90" s="11">
+        <v>131</v>
+      </c>
+      <c r="L90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P90" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q90" s="13">
+        <v>519</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q89"/>
+  <dimension ref="A1:Q90"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B75" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B58" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A90" sqref="A90"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5703125" style="2"/>
+    <col min="1" max="1" width="12.453125" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.54296875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -18273,7 +18626,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -18294,7 +18647,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -18347,7 +18700,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="12">
         <v>43916</v>
       </c>
@@ -18400,7 +18753,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
         <v>43917</v>
       </c>
@@ -18453,7 +18806,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="12">
         <v>43918</v>
       </c>
@@ -18506,7 +18859,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
         <v>43919</v>
       </c>
@@ -18559,7 +18912,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="12">
         <v>43920</v>
       </c>
@@ -18612,7 +18965,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="12">
         <v>43921</v>
       </c>
@@ -18665,7 +19018,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="12">
         <v>43922</v>
       </c>
@@ -18718,7 +19071,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
         <v>43923</v>
       </c>
@@ -18771,7 +19124,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="12">
         <v>43924</v>
       </c>
@@ -18824,7 +19177,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <v>43925</v>
       </c>
@@ -18877,7 +19230,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>43926</v>
       </c>
@@ -18930,7 +19283,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="12">
         <v>43927</v>
       </c>
@@ -18983,7 +19336,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="12">
         <v>43928</v>
       </c>
@@ -19036,7 +19389,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="12">
         <v>43929</v>
       </c>
@@ -19089,7 +19442,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="12">
         <v>43930</v>
       </c>
@@ -19142,7 +19495,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="12">
         <v>43931</v>
       </c>
@@ -19195,7 +19548,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="12">
         <v>43932</v>
       </c>
@@ -19248,7 +19601,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="12">
         <v>43933</v>
       </c>
@@ -19301,7 +19654,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="12">
         <v>43934</v>
       </c>
@@ -19354,7 +19707,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="12">
         <v>43935</v>
       </c>
@@ -19407,7 +19760,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" s="12">
         <v>43936</v>
       </c>
@@ -19460,7 +19813,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" s="12">
         <v>43937</v>
       </c>
@@ -19513,7 +19866,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" s="12">
         <v>43938</v>
       </c>
@@ -19566,7 +19919,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" s="12">
         <v>43939</v>
       </c>
@@ -19619,7 +19972,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" s="12">
         <v>43940</v>
       </c>
@@ -19672,7 +20025,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" s="12">
         <v>43941</v>
       </c>
@@ -19725,7 +20078,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" s="12">
         <v>43942</v>
       </c>
@@ -19778,7 +20131,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="12">
         <v>43943</v>
       </c>
@@ -19831,7 +20184,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" s="12">
         <v>43944</v>
       </c>
@@ -19884,7 +20237,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" s="12">
         <v>43945</v>
       </c>
@@ -19937,7 +20290,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" s="12">
         <v>43946</v>
       </c>
@@ -19990,7 +20343,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" s="12">
         <v>43947</v>
       </c>
@@ -20043,7 +20396,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" s="30">
         <v>43948</v>
       </c>
@@ -20096,7 +20449,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" s="30">
         <v>43949</v>
       </c>
@@ -20149,7 +20502,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" s="30">
         <v>43950</v>
       </c>
@@ -20202,7 +20555,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" s="30">
         <v>43951</v>
       </c>
@@ -20255,7 +20608,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" s="30">
         <v>43952</v>
       </c>
@@ -20308,7 +20661,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" s="30">
         <v>43953</v>
       </c>
@@ -20361,7 +20714,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" s="30">
         <v>43954</v>
       </c>
@@ -20414,7 +20767,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" s="30">
         <v>43955</v>
       </c>
@@ -20467,7 +20820,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" s="30">
         <v>43956</v>
       </c>
@@ -20520,7 +20873,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" s="30">
         <v>43957</v>
       </c>
@@ -20573,7 +20926,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" s="30">
         <v>43958</v>
       </c>
@@ -20626,7 +20979,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" s="30">
         <v>43959</v>
       </c>
@@ -20679,7 +21032,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" s="30">
         <v>43960</v>
       </c>
@@ -20732,7 +21085,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" s="30">
         <v>43961</v>
       </c>
@@ -20785,7 +21138,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50" s="30">
         <v>43962</v>
       </c>
@@ -20838,7 +21191,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51" s="30">
         <v>43963</v>
       </c>
@@ -20891,7 +21244,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52" s="30">
         <v>43964</v>
       </c>
@@ -20944,7 +21297,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53" s="30">
         <v>43965</v>
       </c>
@@ -20997,7 +21350,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54" s="30">
         <v>43966</v>
       </c>
@@ -21050,7 +21403,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55" s="30">
         <v>43967</v>
       </c>
@@ -21103,7 +21456,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56" s="30">
         <v>43968</v>
       </c>
@@ -21156,7 +21509,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A57" s="30">
         <v>43969</v>
       </c>
@@ -21209,7 +21562,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A58" s="30">
         <v>43970</v>
       </c>
@@ -21262,7 +21615,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A59" s="30">
         <v>43971</v>
       </c>
@@ -21315,7 +21668,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A60" s="30">
         <v>43972</v>
       </c>
@@ -21368,7 +21721,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A61" s="30">
         <v>43973</v>
       </c>
@@ -21421,7 +21774,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A62" s="30">
         <v>43974</v>
       </c>
@@ -21474,7 +21827,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A63" s="30">
         <v>43975</v>
       </c>
@@ -21527,7 +21880,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A64" s="30">
         <v>43976</v>
       </c>
@@ -21580,7 +21933,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A65" s="30">
         <v>43977</v>
       </c>
@@ -21633,7 +21986,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A66" s="30">
         <v>43978</v>
       </c>
@@ -21686,7 +22039,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A67" s="30">
         <v>43979</v>
       </c>
@@ -21739,7 +22092,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A68" s="30">
         <v>43980</v>
       </c>
@@ -21792,7 +22145,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A69" s="30">
         <v>43981</v>
       </c>
@@ -21845,7 +22198,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A70" s="30">
         <v>43982</v>
       </c>
@@ -21898,7 +22251,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A71" s="30">
         <v>43983</v>
       </c>
@@ -21951,7 +22304,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A72" s="30">
         <v>43984</v>
       </c>
@@ -22004,7 +22357,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A73" s="30">
         <v>43985</v>
       </c>
@@ -22057,7 +22410,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A74" s="30">
         <v>43986</v>
       </c>
@@ -22110,7 +22463,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A75" s="30">
         <v>43987</v>
       </c>
@@ -22163,7 +22516,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A76" s="30">
         <v>43988</v>
       </c>
@@ -22216,7 +22569,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A77" s="30">
         <v>43989</v>
       </c>
@@ -22269,7 +22622,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A78" s="30">
         <v>43990</v>
       </c>
@@ -22322,7 +22675,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A79" s="30">
         <v>43991</v>
       </c>
@@ -22375,7 +22728,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A80" s="30">
         <v>43992</v>
       </c>
@@ -22428,7 +22781,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A81" s="30">
         <v>43993</v>
       </c>
@@ -22481,7 +22834,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A82" s="30">
         <v>43994</v>
       </c>
@@ -22534,7 +22887,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A83" s="30">
         <v>43995</v>
       </c>
@@ -22587,7 +22940,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A84" s="30">
         <v>43996</v>
       </c>
@@ -22640,7 +22993,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A85" s="30">
         <v>43997</v>
       </c>
@@ -22693,7 +23046,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A86" s="30">
         <v>43998</v>
       </c>
@@ -22746,7 +23099,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A87" s="30">
         <v>43999</v>
       </c>
@@ -22799,7 +23152,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A88" s="30">
         <v>44000</v>
       </c>
@@ -22852,7 +23205,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A89" s="30">
         <v>44001</v>
       </c>
@@ -22905,12 +23258,66 @@
         <v>376</v>
       </c>
     </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A90" s="30">
+        <v>44002</v>
+      </c>
+      <c r="B90" s="11">
+        <v>18</v>
+      </c>
+      <c r="C90" s="11">
+        <v>27</v>
+      </c>
+      <c r="D90" s="11">
+        <v>8</v>
+      </c>
+      <c r="E90" s="11">
+        <v>17</v>
+      </c>
+      <c r="F90" s="11">
+        <v>22</v>
+      </c>
+      <c r="G90" s="11">
+        <v>22</v>
+      </c>
+      <c r="H90" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I90" s="11">
+        <v>17</v>
+      </c>
+      <c r="J90" s="11">
+        <v>47</v>
+      </c>
+      <c r="K90" s="11">
+        <v>193</v>
+      </c>
+      <c r="L90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N90" s="11">
+        <v>13</v>
+      </c>
+      <c r="O90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P90" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q90" s="36">
+        <v>384</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=customXML/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA" version="1.0.0">
   <systemFields>
     <field name="Objective-Id">
@@ -22929,13 +23336,13 @@
       <value order="0">false</value>
     </field>
     <field name="Objective-IsPublished">
-      <value order="0">true</value>
+      <value order="0">false</value>
     </field>
     <field name="Objective-DatePublished">
-      <value order="0">2020-06-19T12:49:38Z</value>
+      <value order="0"/>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-19T12:49:38Z</value>
+      <value order="0">2020-06-20T11:33:16Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -22947,16 +23354,16 @@
       <value order="0">Analytical: COVID 19 Analysis: Restricted working papers: Research and analysis: Diseases: 2020-2025</value>
     </field>
     <field name="Objective-State">
-      <value order="0">Published</value>
+      <value order="0">Being Drafted</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41853927</value>
+      <value order="0">vA41864601</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">26.0</value>
+      <value order="0">27.2</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">196</value>
+      <value order="0">201</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>
@@ -22993,7 +23400,7 @@
 </metadata>
 </file>
 
-<file path=customXML/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5745109E-2DDF-40CB-AC2B-FF9B10C90820}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-22 20:09)
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u201433\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA1432\A28088333\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U445783\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA18464\A28088333\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5985" windowHeight="6045" tabRatio="803"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5988" windowHeight="6048" tabRatio="803" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2044" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2071" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -1617,16 +1617,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> ICU.</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" baseline="0">
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>  The total figures for Scotland have therefor been revised as follows:</a:t>
+            <a:t> ICU.  The total figures for Scotland have therefor been revised as follows:</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB">
             <a:effectLst/>
@@ -2667,25 +2658,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C5:C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="90.42578125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.42578125" style="2"/>
+    <col min="2" max="2" width="29.44140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="90.44140625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" s="18" t="s">
         <v>20</v>
       </c>
@@ -2693,7 +2684,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20" t="s">
         <v>22</v>
       </c>
@@ -2701,13 +2692,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="22" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="23"/>
     </row>
-    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="24" t="s">
         <v>26</v>
       </c>
@@ -2715,7 +2706,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="24" t="s">
         <v>27</v>
       </c>
@@ -2723,7 +2714,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="24" t="s">
         <v>36</v>
       </c>
@@ -2731,7 +2722,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="20" t="s">
         <v>37</v>
       </c>
@@ -2759,12 +2750,12 @@
       <selection activeCell="O81" sqref="O81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.42578125" style="2"/>
+    <col min="1" max="16384" width="9.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" ht="15" x14ac:dyDescent="0.3">
       <c r="A44" s="42"/>
     </row>
   </sheetData>
@@ -2778,21 +2769,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S160"/>
   <sheetViews>
-    <sheetView zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B94" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J108" sqref="J108"/>
+      <selection pane="bottomRight" activeCell="C114" sqref="C114"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" style="2" customWidth="1"/>
-    <col min="2" max="16" width="11.42578125" style="11" customWidth="1"/>
-    <col min="17" max="16384" width="8.5703125" style="2"/>
+    <col min="2" max="16" width="11.44140625" style="11" customWidth="1"/>
+    <col min="17" max="16384" width="8.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -2812,7 +2803,7 @@
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
         <v>30</v>
       </c>
@@ -2831,7 +2822,7 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -2881,7 +2872,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>43897</v>
       </c>
@@ -2931,7 +2922,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>43898</v>
       </c>
@@ -2981,7 +2972,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>43899</v>
       </c>
@@ -3031,7 +3022,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>43900</v>
       </c>
@@ -3081,7 +3072,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>43901</v>
       </c>
@@ -3131,7 +3122,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>43902</v>
       </c>
@@ -3181,7 +3172,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>43903</v>
       </c>
@@ -3231,7 +3222,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>43904</v>
       </c>
@@ -3281,7 +3272,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>43905</v>
       </c>
@@ -3331,7 +3322,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>43906</v>
       </c>
@@ -3381,7 +3372,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>43907</v>
       </c>
@@ -3431,7 +3422,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>43908</v>
       </c>
@@ -3481,7 +3472,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>43909</v>
       </c>
@@ -3531,7 +3522,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>43910</v>
       </c>
@@ -3581,7 +3572,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>43911</v>
       </c>
@@ -3631,7 +3622,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>43912</v>
       </c>
@@ -3681,7 +3672,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>43913</v>
       </c>
@@ -3731,7 +3722,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>43914</v>
       </c>
@@ -3781,7 +3772,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>43915</v>
       </c>
@@ -3831,7 +3822,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>43916</v>
       </c>
@@ -3881,7 +3872,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>43917</v>
       </c>
@@ -3931,7 +3922,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>43918</v>
       </c>
@@ -3981,7 +3972,7 @@
         <v>1264</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>43919</v>
       </c>
@@ -4031,7 +4022,7 @@
         <v>1417</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>43920</v>
       </c>
@@ -4081,7 +4072,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>43921</v>
       </c>
@@ -4131,7 +4122,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>43922</v>
       </c>
@@ -4181,7 +4172,7 @@
         <v>2310</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>43923</v>
       </c>
@@ -4231,7 +4222,7 @@
         <v>2602</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <v>43924</v>
       </c>
@@ -4281,7 +4272,7 @@
         <v>3001</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>43925</v>
       </c>
@@ -4331,7 +4322,7 @@
         <v>3345</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
         <v>43926</v>
       </c>
@@ -4381,7 +4372,7 @@
         <v>3706</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
         <v>43927</v>
       </c>
@@ -4431,7 +4422,7 @@
         <v>3961</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
         <v>43928</v>
       </c>
@@ -4481,7 +4472,7 @@
         <v>4229</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>43929</v>
       </c>
@@ -4531,7 +4522,7 @@
         <v>4565</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
         <v>43930</v>
       </c>
@@ -4581,7 +4572,7 @@
         <v>4957</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
         <v>43931</v>
       </c>
@@ -4631,7 +4622,7 @@
         <v>5275</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>43932</v>
       </c>
@@ -4681,7 +4672,7 @@
         <v>5590</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
         <v>43933</v>
       </c>
@@ -4731,7 +4722,7 @@
         <v>5912</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
         <v>43934</v>
       </c>
@@ -4781,7 +4772,7 @@
         <v>6067</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>43935</v>
       </c>
@@ -4831,7 +4822,7 @@
         <v>6358</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
         <v>43936</v>
       </c>
@@ -4881,7 +4872,7 @@
         <v>6748</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" s="5">
         <v>43937</v>
       </c>
@@ -4931,7 +4922,7 @@
         <v>7102</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
         <v>43938</v>
       </c>
@@ -4981,7 +4972,7 @@
         <v>7409</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" s="5">
         <v>43939</v>
       </c>
@@ -5031,7 +5022,7 @@
         <v>7820</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" s="5">
         <v>43940</v>
       </c>
@@ -5081,7 +5072,7 @@
         <v>8187</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
         <v>43941</v>
       </c>
@@ -5131,7 +5122,7 @@
         <v>8450</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A49" s="5">
         <v>43942</v>
       </c>
@@ -5181,7 +5172,7 @@
         <v>8672</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
         <v>43943</v>
       </c>
@@ -5231,7 +5222,7 @@
         <v>9038</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A51" s="5">
         <v>43944</v>
       </c>
@@ -5281,7 +5272,7 @@
         <v>9409</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A52" s="5">
         <v>43945</v>
       </c>
@@ -5331,7 +5322,7 @@
         <v>9697</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A53" s="5">
         <v>43946</v>
       </c>
@@ -5381,7 +5372,7 @@
         <v>10051</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A54" s="5">
         <v>43947</v>
       </c>
@@ -5432,7 +5423,7 @@
       </c>
       <c r="R54" s="37"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A55" s="5">
         <v>43948</v>
       </c>
@@ -5483,7 +5474,7 @@
       </c>
       <c r="R55" s="37"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A56" s="5">
         <v>43949</v>
       </c>
@@ -5534,7 +5525,7 @@
       </c>
       <c r="R56" s="38"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A57" s="5">
         <v>43950</v>
       </c>
@@ -5584,7 +5575,7 @@
         <v>11034</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A58" s="5">
         <v>43951</v>
       </c>
@@ -5635,7 +5626,7 @@
       </c>
       <c r="R58" s="37"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A59" s="5">
         <v>43952</v>
       </c>
@@ -5687,7 +5678,7 @@
       <c r="R59" s="37"/>
       <c r="S59" s="37"/>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A60" s="5">
         <v>43953</v>
       </c>
@@ -5737,7 +5728,7 @@
         <v>11927</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A61" s="5">
         <v>43954</v>
       </c>
@@ -5787,7 +5778,7 @@
         <v>12097</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A62" s="5">
         <v>43955</v>
       </c>
@@ -5837,7 +5828,7 @@
         <v>12266</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A63" s="5">
         <v>43956</v>
       </c>
@@ -5887,7 +5878,7 @@
         <v>12437</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A64" s="5">
         <v>43957</v>
       </c>
@@ -5937,7 +5928,7 @@
         <v>12709</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65" s="5">
         <v>43958</v>
       </c>
@@ -5987,7 +5978,7 @@
         <v>12924</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66" s="5">
         <v>43959</v>
       </c>
@@ -6037,7 +6028,7 @@
         <v>13149</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A67" s="5">
         <v>43960</v>
       </c>
@@ -6087,7 +6078,7 @@
         <v>13305</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A68" s="5">
         <v>43961</v>
       </c>
@@ -6137,7 +6128,7 @@
         <v>13486</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A69" s="5">
         <v>43962</v>
       </c>
@@ -6187,7 +6178,7 @@
         <v>13627</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A70" s="5">
         <v>43963</v>
       </c>
@@ -6237,7 +6228,7 @@
         <v>13763</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A71" s="5">
         <v>43964</v>
       </c>
@@ -6287,7 +6278,7 @@
         <v>13929</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A72" s="5">
         <v>43965</v>
       </c>
@@ -6337,7 +6328,7 @@
         <v>14117</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A73" s="5">
         <v>43966</v>
       </c>
@@ -6387,7 +6378,7 @@
         <v>14260</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A74" s="5">
         <v>43967</v>
       </c>
@@ -6437,7 +6428,7 @@
         <v>14447</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A75" s="5">
         <v>43968</v>
       </c>
@@ -6487,7 +6478,7 @@
         <v>14537</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A76" s="5">
         <v>43969</v>
       </c>
@@ -6537,7 +6528,7 @@
         <v>14594</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A77" s="5">
         <v>43970</v>
       </c>
@@ -6587,7 +6578,7 @@
         <v>14655</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A78" s="5">
         <v>43971</v>
       </c>
@@ -6637,7 +6628,7 @@
         <v>14751</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A79" s="5">
         <v>43972</v>
       </c>
@@ -6687,7 +6678,7 @@
         <v>14856</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A80" s="5">
         <v>43973</v>
       </c>
@@ -6737,7 +6728,7 @@
         <v>14969</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A81" s="5">
         <v>43974</v>
       </c>
@@ -6787,7 +6778,7 @@
         <v>15041</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A82" s="5">
         <v>43975</v>
       </c>
@@ -6837,7 +6828,7 @@
         <v>15101</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A83" s="5">
         <v>43976</v>
       </c>
@@ -6887,7 +6878,7 @@
         <v>15156</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A84" s="5">
         <v>43977</v>
       </c>
@@ -6937,7 +6928,7 @@
         <v>15185</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A85" s="5">
         <v>43978</v>
       </c>
@@ -6987,7 +6978,7 @@
         <v>15240</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A86" s="5">
         <v>43979</v>
       </c>
@@ -7037,7 +7028,7 @@
         <v>15288</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A87" s="5">
         <v>43980</v>
       </c>
@@ -7087,7 +7078,7 @@
         <v>15327</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A88" s="5">
         <v>43981</v>
       </c>
@@ -7137,7 +7128,7 @@
         <v>15382</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A89" s="5">
         <v>43982</v>
       </c>
@@ -7187,7 +7178,7 @@
         <v>15400</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A90" s="5">
         <v>43983</v>
       </c>
@@ -7237,7 +7228,7 @@
         <v>15418</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A91" s="5">
         <v>43984</v>
       </c>
@@ -7287,7 +7278,7 @@
         <v>15471</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A92" s="5">
         <v>43985</v>
       </c>
@@ -7337,7 +7328,7 @@
         <v>15504</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A93" s="5">
         <v>43986</v>
       </c>
@@ -7387,7 +7378,7 @@
         <v>15553</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A94" s="5">
         <v>43987</v>
       </c>
@@ -7437,7 +7428,7 @@
         <v>15582</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A95" s="5">
         <v>43988</v>
       </c>
@@ -7487,7 +7478,7 @@
         <v>15603</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A96" s="5">
         <v>43989</v>
       </c>
@@ -7537,7 +7528,7 @@
         <v>15621</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A97" s="5">
         <v>43990</v>
       </c>
@@ -7587,7 +7578,7 @@
         <v>15639</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A98" s="5">
         <v>43991</v>
       </c>
@@ -7637,7 +7628,7 @@
         <v>15653</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A99" s="5">
         <v>43992</v>
       </c>
@@ -7687,7 +7678,7 @@
         <v>15665</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A100" s="5">
         <v>43993</v>
       </c>
@@ -7737,7 +7728,7 @@
         <v>15682</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A101" s="5">
         <v>43994</v>
       </c>
@@ -7787,7 +7778,7 @@
         <v>15709</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A102" s="5">
         <v>43995</v>
       </c>
@@ -7837,7 +7828,7 @@
         <v>15730</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A103" s="53">
         <v>43996</v>
       </c>
@@ -7887,7 +7878,7 @@
         <v>15755</v>
       </c>
     </row>
-    <row r="104" spans="1:16" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="5">
         <v>43997</v>
       </c>
@@ -7937,7 +7928,7 @@
         <v>18030</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A105" s="5">
         <v>43998</v>
       </c>
@@ -7987,7 +7978,7 @@
         <v>18045</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A106" s="5">
         <v>43999</v>
       </c>
@@ -8037,7 +8028,7 @@
         <v>18066</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A107" s="5">
         <v>44000</v>
       </c>
@@ -8087,7 +8078,7 @@
         <v>18077</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A108" s="5">
         <v>44001</v>
       </c>
@@ -8137,7 +8128,7 @@
         <v>18104</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A109" s="5">
         <v>44002</v>
       </c>
@@ -8187,7 +8178,7 @@
         <v>18130</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A110" s="5">
         <v>44003</v>
       </c>
@@ -8237,24 +8228,57 @@
         <v>18156</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B111" s="27"/>
-      <c r="C111" s="27"/>
-      <c r="D111" s="27"/>
-      <c r="E111" s="27"/>
-      <c r="F111" s="27"/>
-      <c r="G111" s="27"/>
-      <c r="H111" s="27"/>
-      <c r="I111" s="27"/>
-      <c r="J111" s="27"/>
-      <c r="K111" s="27"/>
-      <c r="L111" s="27"/>
-      <c r="M111" s="27"/>
-      <c r="N111" s="27"/>
-      <c r="O111" s="27"/>
-      <c r="P111" s="27"/>
-    </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A111" s="5">
+        <v>44004</v>
+      </c>
+      <c r="B111" s="27">
+        <v>1250</v>
+      </c>
+      <c r="C111" s="27">
+        <v>346</v>
+      </c>
+      <c r="D111" s="27">
+        <v>285</v>
+      </c>
+      <c r="E111" s="27">
+        <v>928</v>
+      </c>
+      <c r="F111" s="27">
+        <v>1057</v>
+      </c>
+      <c r="G111" s="27">
+        <v>1412</v>
+      </c>
+      <c r="H111" s="27">
+        <v>4830</v>
+      </c>
+      <c r="I111" s="27">
+        <v>373</v>
+      </c>
+      <c r="J111" s="27">
+        <v>2712</v>
+      </c>
+      <c r="K111" s="27">
+        <v>3146</v>
+      </c>
+      <c r="L111" s="27">
+        <v>9</v>
+      </c>
+      <c r="M111" s="27">
+        <v>54</v>
+      </c>
+      <c r="N111" s="27">
+        <v>1761</v>
+      </c>
+      <c r="O111" s="27">
+        <v>7</v>
+      </c>
+      <c r="P111" s="31">
+        <v>18170</v>
+      </c>
+    </row>
+    <row r="112" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B112" s="27"/>
       <c r="C112" s="27"/>
       <c r="D112" s="27"/>
@@ -8271,7 +8295,7 @@
       <c r="O112" s="27"/>
       <c r="P112" s="27"/>
     </row>
-    <row r="113" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B113" s="27"/>
       <c r="C113" s="27"/>
       <c r="D113" s="27"/>
@@ -8288,7 +8312,7 @@
       <c r="O113" s="27"/>
       <c r="P113" s="27"/>
     </row>
-    <row r="114" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B114" s="27"/>
       <c r="C114" s="27"/>
       <c r="D114" s="27"/>
@@ -8305,7 +8329,7 @@
       <c r="O114" s="27"/>
       <c r="P114" s="27"/>
     </row>
-    <row r="115" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B115" s="27"/>
       <c r="C115" s="27"/>
       <c r="D115" s="27"/>
@@ -8322,7 +8346,7 @@
       <c r="O115" s="27"/>
       <c r="P115" s="27"/>
     </row>
-    <row r="116" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B116" s="27"/>
       <c r="C116" s="27"/>
       <c r="D116" s="27"/>
@@ -8339,7 +8363,7 @@
       <c r="O116" s="27"/>
       <c r="P116" s="27"/>
     </row>
-    <row r="117" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B117" s="27"/>
       <c r="C117" s="27"/>
       <c r="D117" s="27"/>
@@ -8356,7 +8380,7 @@
       <c r="O117" s="27"/>
       <c r="P117" s="27"/>
     </row>
-    <row r="118" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B118" s="27"/>
       <c r="C118" s="27"/>
       <c r="D118" s="27"/>
@@ -8373,7 +8397,7 @@
       <c r="O118" s="27"/>
       <c r="P118" s="27"/>
     </row>
-    <row r="119" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B119" s="27"/>
       <c r="C119" s="27"/>
       <c r="D119" s="27"/>
@@ -8390,7 +8414,7 @@
       <c r="O119" s="27"/>
       <c r="P119" s="27"/>
     </row>
-    <row r="120" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B120" s="27"/>
       <c r="C120" s="27"/>
       <c r="D120" s="27"/>
@@ -8407,7 +8431,7 @@
       <c r="O120" s="27"/>
       <c r="P120" s="27"/>
     </row>
-    <row r="121" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B121" s="27"/>
       <c r="C121" s="27"/>
       <c r="D121" s="27"/>
@@ -8424,7 +8448,7 @@
       <c r="O121" s="27"/>
       <c r="P121" s="27"/>
     </row>
-    <row r="122" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B122" s="27"/>
       <c r="C122" s="27"/>
       <c r="D122" s="27"/>
@@ -8441,7 +8465,7 @@
       <c r="O122" s="27"/>
       <c r="P122" s="27"/>
     </row>
-    <row r="123" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B123" s="27"/>
       <c r="C123" s="27"/>
       <c r="D123" s="27"/>
@@ -8458,7 +8482,7 @@
       <c r="O123" s="27"/>
       <c r="P123" s="27"/>
     </row>
-    <row r="124" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B124" s="27"/>
       <c r="C124" s="27"/>
       <c r="D124" s="27"/>
@@ -8475,7 +8499,7 @@
       <c r="O124" s="27"/>
       <c r="P124" s="27"/>
     </row>
-    <row r="125" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B125" s="27"/>
       <c r="C125" s="27"/>
       <c r="D125" s="27"/>
@@ -8492,7 +8516,7 @@
       <c r="O125" s="27"/>
       <c r="P125" s="27"/>
     </row>
-    <row r="126" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B126" s="27"/>
       <c r="C126" s="27"/>
       <c r="D126" s="27"/>
@@ -8509,7 +8533,7 @@
       <c r="O126" s="27"/>
       <c r="P126" s="27"/>
     </row>
-    <row r="127" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B127" s="27"/>
       <c r="C127" s="27"/>
       <c r="D127" s="27"/>
@@ -8526,7 +8550,7 @@
       <c r="O127" s="27"/>
       <c r="P127" s="27"/>
     </row>
-    <row r="128" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B128" s="27"/>
       <c r="C128" s="27"/>
       <c r="D128" s="27"/>
@@ -8543,7 +8567,7 @@
       <c r="O128" s="27"/>
       <c r="P128" s="27"/>
     </row>
-    <row r="129" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B129" s="27"/>
       <c r="C129" s="27"/>
       <c r="D129" s="27"/>
@@ -8560,7 +8584,7 @@
       <c r="O129" s="27"/>
       <c r="P129" s="27"/>
     </row>
-    <row r="130" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B130" s="27"/>
       <c r="C130" s="27"/>
       <c r="D130" s="27"/>
@@ -8577,7 +8601,7 @@
       <c r="O130" s="27"/>
       <c r="P130" s="27"/>
     </row>
-    <row r="131" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B131" s="27"/>
       <c r="C131" s="27"/>
       <c r="D131" s="27"/>
@@ -8594,7 +8618,7 @@
       <c r="O131" s="27"/>
       <c r="P131" s="27"/>
     </row>
-    <row r="132" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B132" s="27"/>
       <c r="C132" s="27"/>
       <c r="D132" s="27"/>
@@ -8611,7 +8635,7 @@
       <c r="O132" s="27"/>
       <c r="P132" s="27"/>
     </row>
-    <row r="133" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B133" s="27"/>
       <c r="C133" s="27"/>
       <c r="D133" s="27"/>
@@ -8628,7 +8652,7 @@
       <c r="O133" s="27"/>
       <c r="P133" s="27"/>
     </row>
-    <row r="134" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B134" s="27"/>
       <c r="C134" s="27"/>
       <c r="D134" s="27"/>
@@ -8645,7 +8669,7 @@
       <c r="O134" s="27"/>
       <c r="P134" s="27"/>
     </row>
-    <row r="135" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B135" s="27"/>
       <c r="C135" s="27"/>
       <c r="D135" s="27"/>
@@ -8662,7 +8686,7 @@
       <c r="O135" s="27"/>
       <c r="P135" s="27"/>
     </row>
-    <row r="136" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B136" s="27"/>
       <c r="C136" s="27"/>
       <c r="D136" s="27"/>
@@ -8679,7 +8703,7 @@
       <c r="O136" s="27"/>
       <c r="P136" s="27"/>
     </row>
-    <row r="137" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B137" s="27"/>
       <c r="C137" s="27"/>
       <c r="D137" s="27"/>
@@ -8696,7 +8720,7 @@
       <c r="O137" s="27"/>
       <c r="P137" s="27"/>
     </row>
-    <row r="138" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B138" s="27"/>
       <c r="C138" s="27"/>
       <c r="D138" s="27"/>
@@ -8713,7 +8737,7 @@
       <c r="O138" s="27"/>
       <c r="P138" s="27"/>
     </row>
-    <row r="139" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B139" s="27"/>
       <c r="C139" s="27"/>
       <c r="D139" s="27"/>
@@ -8730,7 +8754,7 @@
       <c r="O139" s="27"/>
       <c r="P139" s="27"/>
     </row>
-    <row r="140" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B140" s="27"/>
       <c r="C140" s="27"/>
       <c r="D140" s="27"/>
@@ -8747,7 +8771,7 @@
       <c r="O140" s="27"/>
       <c r="P140" s="27"/>
     </row>
-    <row r="141" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B141" s="27"/>
       <c r="C141" s="27"/>
       <c r="D141" s="27"/>
@@ -8764,7 +8788,7 @@
       <c r="O141" s="27"/>
       <c r="P141" s="27"/>
     </row>
-    <row r="142" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B142" s="27"/>
       <c r="C142" s="27"/>
       <c r="D142" s="27"/>
@@ -8781,7 +8805,7 @@
       <c r="O142" s="27"/>
       <c r="P142" s="27"/>
     </row>
-    <row r="143" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B143" s="27"/>
       <c r="C143" s="27"/>
       <c r="D143" s="27"/>
@@ -8798,7 +8822,7 @@
       <c r="O143" s="27"/>
       <c r="P143" s="27"/>
     </row>
-    <row r="144" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B144" s="27"/>
       <c r="C144" s="27"/>
       <c r="D144" s="27"/>
@@ -8815,7 +8839,7 @@
       <c r="O144" s="27"/>
       <c r="P144" s="27"/>
     </row>
-    <row r="145" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B145" s="27"/>
       <c r="C145" s="27"/>
       <c r="D145" s="27"/>
@@ -8832,7 +8856,7 @@
       <c r="O145" s="27"/>
       <c r="P145" s="27"/>
     </row>
-    <row r="146" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B146" s="27"/>
       <c r="C146" s="27"/>
       <c r="D146" s="27"/>
@@ -8849,7 +8873,7 @@
       <c r="O146" s="27"/>
       <c r="P146" s="27"/>
     </row>
-    <row r="147" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B147" s="27"/>
       <c r="C147" s="27"/>
       <c r="D147" s="27"/>
@@ -8866,7 +8890,7 @@
       <c r="O147" s="27"/>
       <c r="P147" s="27"/>
     </row>
-    <row r="148" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B148" s="27"/>
       <c r="C148" s="27"/>
       <c r="D148" s="27"/>
@@ -8883,7 +8907,7 @@
       <c r="O148" s="27"/>
       <c r="P148" s="27"/>
     </row>
-    <row r="149" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B149" s="27"/>
       <c r="C149" s="27"/>
       <c r="D149" s="27"/>
@@ -8900,7 +8924,7 @@
       <c r="O149" s="27"/>
       <c r="P149" s="27"/>
     </row>
-    <row r="150" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B150" s="27"/>
       <c r="C150" s="27"/>
       <c r="D150" s="27"/>
@@ -8917,7 +8941,7 @@
       <c r="O150" s="27"/>
       <c r="P150" s="27"/>
     </row>
-    <row r="151" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B151" s="27"/>
       <c r="C151" s="27"/>
       <c r="D151" s="27"/>
@@ -8934,7 +8958,7 @@
       <c r="O151" s="27"/>
       <c r="P151" s="27"/>
     </row>
-    <row r="152" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B152" s="27"/>
       <c r="C152" s="27"/>
       <c r="D152" s="27"/>
@@ -8951,7 +8975,7 @@
       <c r="O152" s="27"/>
       <c r="P152" s="27"/>
     </row>
-    <row r="153" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B153" s="27"/>
       <c r="C153" s="27"/>
       <c r="D153" s="27"/>
@@ -8968,7 +8992,7 @@
       <c r="O153" s="27"/>
       <c r="P153" s="27"/>
     </row>
-    <row r="154" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B154" s="27"/>
       <c r="C154" s="27"/>
       <c r="D154" s="27"/>
@@ -8985,7 +9009,7 @@
       <c r="O154" s="27"/>
       <c r="P154" s="27"/>
     </row>
-    <row r="155" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B155" s="27"/>
       <c r="C155" s="27"/>
       <c r="D155" s="27"/>
@@ -9002,7 +9026,7 @@
       <c r="O155" s="27"/>
       <c r="P155" s="27"/>
     </row>
-    <row r="156" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B156" s="27"/>
       <c r="C156" s="27"/>
       <c r="D156" s="27"/>
@@ -9019,7 +9043,7 @@
       <c r="O156" s="27"/>
       <c r="P156" s="27"/>
     </row>
-    <row r="157" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B157" s="27"/>
       <c r="C157" s="27"/>
       <c r="D157" s="27"/>
@@ -9036,7 +9060,7 @@
       <c r="O157" s="27"/>
       <c r="P157" s="27"/>
     </row>
-    <row r="158" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B158" s="27"/>
       <c r="C158" s="27"/>
       <c r="D158" s="27"/>
@@ -9053,7 +9077,7 @@
       <c r="O158" s="27"/>
       <c r="P158" s="27"/>
     </row>
-    <row r="159" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B159" s="27"/>
       <c r="C159" s="27"/>
       <c r="D159" s="27"/>
@@ -9070,7 +9094,7 @@
       <c r="O159" s="27"/>
       <c r="P159" s="27"/>
     </row>
-    <row r="160" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B160" s="27"/>
       <c r="C160" s="27"/>
       <c r="D160" s="27"/>
@@ -9096,21 +9120,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q99"/>
+  <dimension ref="A1:Q100"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K95" sqref="K95"/>
+      <selection pane="bottomLeft" activeCell="M106" sqref="M106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5703125" style="2"/>
+    <col min="1" max="1" width="12.44140625" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.5546875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -9131,7 +9155,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
         <v>30</v>
       </c>
@@ -9152,7 +9176,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -9205,7 +9229,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>43908</v>
       </c>
@@ -9258,7 +9282,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>43909</v>
       </c>
@@ -9311,7 +9335,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>43910</v>
       </c>
@@ -9364,7 +9388,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>43911</v>
       </c>
@@ -9417,7 +9441,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>43912</v>
       </c>
@@ -9470,7 +9494,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>43913</v>
       </c>
@@ -9523,7 +9547,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>43914</v>
       </c>
@@ -9576,7 +9600,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>43915</v>
       </c>
@@ -9629,7 +9653,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
         <v>43916</v>
       </c>
@@ -9682,7 +9706,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>43917</v>
       </c>
@@ -9735,7 +9759,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>43918</v>
       </c>
@@ -9788,7 +9812,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>43919</v>
       </c>
@@ -9841,7 +9865,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>43920</v>
       </c>
@@ -9894,7 +9918,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>43921</v>
       </c>
@@ -9947,7 +9971,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>43922</v>
       </c>
@@ -10000,7 +10024,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>43923</v>
       </c>
@@ -10053,7 +10077,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>43924</v>
       </c>
@@ -10106,7 +10130,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>43925</v>
       </c>
@@ -10159,7 +10183,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="12">
         <v>43926</v>
       </c>
@@ -10212,7 +10236,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="12">
         <v>43927</v>
       </c>
@@ -10265,7 +10289,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="12">
         <v>43928</v>
       </c>
@@ -10318,7 +10342,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="12">
         <v>43929</v>
       </c>
@@ -10371,7 +10395,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="12">
         <v>43930</v>
       </c>
@@ -10424,7 +10448,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="12">
         <v>43931</v>
       </c>
@@ -10477,7 +10501,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="12">
         <v>43932</v>
       </c>
@@ -10530,7 +10554,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="12">
         <v>43933</v>
       </c>
@@ -10583,7 +10607,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <v>43934</v>
       </c>
@@ -10636,7 +10660,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="12">
         <v>43935</v>
       </c>
@@ -10689,7 +10713,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="12">
         <v>43936</v>
       </c>
@@ -10742,7 +10766,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="12">
         <v>43937</v>
       </c>
@@ -10795,7 +10819,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="12">
         <v>43938</v>
       </c>
@@ -10848,7 +10872,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="12">
         <v>43939</v>
       </c>
@@ -10901,7 +10925,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="29">
         <v>43940</v>
       </c>
@@ -10954,7 +10978,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="29">
         <v>43941</v>
       </c>
@@ -11007,7 +11031,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="29">
         <v>43942</v>
       </c>
@@ -11060,7 +11084,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="29">
         <v>43943</v>
       </c>
@@ -11113,7 +11137,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="29">
         <v>43944</v>
       </c>
@@ -11166,7 +11190,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="29">
         <v>43945</v>
       </c>
@@ -11219,7 +11243,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="29">
         <v>43946</v>
       </c>
@@ -11272,7 +11296,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="29">
         <v>43947</v>
       </c>
@@ -11325,7 +11349,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="29">
         <v>43948</v>
       </c>
@@ -11378,7 +11402,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="29">
         <v>43949</v>
       </c>
@@ -11431,7 +11455,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="29">
         <v>43950</v>
       </c>
@@ -11484,7 +11508,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="29">
         <v>43951</v>
       </c>
@@ -11537,7 +11561,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" s="29">
         <v>43952</v>
       </c>
@@ -11590,7 +11614,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="29">
         <v>43953</v>
       </c>
@@ -11643,7 +11667,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" s="29">
         <v>43954</v>
       </c>
@@ -11696,7 +11720,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="29">
         <v>43955</v>
       </c>
@@ -11749,7 +11773,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" s="29">
         <v>43956</v>
       </c>
@@ -11802,7 +11826,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" s="29">
         <v>43957</v>
       </c>
@@ -11855,7 +11879,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" s="29">
         <v>43958</v>
       </c>
@@ -11908,7 +11932,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" s="29">
         <v>43959</v>
       </c>
@@ -11961,7 +11985,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" s="29">
         <v>43960</v>
       </c>
@@ -12014,7 +12038,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" s="29">
         <v>43961</v>
       </c>
@@ -12067,7 +12091,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" s="29">
         <v>43962</v>
       </c>
@@ -12120,7 +12144,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" s="29">
         <v>43963</v>
       </c>
@@ -12173,7 +12197,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" s="29">
         <v>43964</v>
       </c>
@@ -12226,7 +12250,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" s="29">
         <v>43965</v>
       </c>
@@ -12279,7 +12303,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" s="29">
         <v>43966</v>
       </c>
@@ -12332,7 +12356,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" s="29">
         <v>43967</v>
       </c>
@@ -12385,7 +12409,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" s="29">
         <v>43968</v>
       </c>
@@ -12438,7 +12462,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" s="29">
         <v>43969</v>
       </c>
@@ -12491,7 +12515,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" s="29">
         <v>43970</v>
       </c>
@@ -12544,7 +12568,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" s="29">
         <v>43971</v>
       </c>
@@ -12597,7 +12621,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" s="29">
         <v>43972</v>
       </c>
@@ -12650,7 +12674,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" s="29">
         <v>43973</v>
       </c>
@@ -12703,7 +12727,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" s="29">
         <v>43974</v>
       </c>
@@ -12756,7 +12780,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" s="29">
         <v>43975</v>
       </c>
@@ -12809,7 +12833,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" s="29">
         <v>43976</v>
       </c>
@@ -12862,7 +12886,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" s="29">
         <v>43977</v>
       </c>
@@ -12915,7 +12939,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" s="29">
         <v>43978</v>
       </c>
@@ -12968,7 +12992,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75" s="29">
         <v>43979</v>
       </c>
@@ -13021,7 +13045,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76" s="29">
         <v>43980</v>
       </c>
@@ -13074,7 +13098,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77" s="29">
         <v>43981</v>
       </c>
@@ -13127,7 +13151,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78" s="29">
         <v>43982</v>
       </c>
@@ -13180,7 +13204,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79" s="29">
         <v>43983</v>
       </c>
@@ -13233,7 +13257,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A80" s="29">
         <v>43984</v>
       </c>
@@ -13286,7 +13310,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A81" s="29">
         <v>43985</v>
       </c>
@@ -13339,7 +13363,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A82" s="29">
         <v>43986</v>
       </c>
@@ -13392,7 +13416,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A83" s="29">
         <v>43987</v>
       </c>
@@ -13445,7 +13469,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A84" s="29">
         <v>43988</v>
       </c>
@@ -13498,7 +13522,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A85" s="29">
         <v>43989</v>
       </c>
@@ -13551,7 +13575,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A86" s="29">
         <v>43990</v>
       </c>
@@ -13604,7 +13628,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A87" s="29">
         <v>43991</v>
       </c>
@@ -13657,7 +13681,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A88" s="29">
         <v>43992</v>
       </c>
@@ -13710,7 +13734,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A89" s="29">
         <v>43993</v>
       </c>
@@ -13763,7 +13787,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A90" s="29">
         <v>43994</v>
       </c>
@@ -13816,7 +13840,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A91" s="29">
         <v>43995</v>
       </c>
@@ -13869,7 +13893,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A92" s="29">
         <v>43996</v>
       </c>
@@ -13922,7 +13946,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A93" s="29">
         <v>43997</v>
       </c>
@@ -13975,7 +13999,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A94" s="29">
         <v>43998</v>
       </c>
@@ -14028,7 +14052,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A95" s="29">
         <v>43999</v>
       </c>
@@ -14081,7 +14105,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A96" s="29">
         <v>44000</v>
       </c>
@@ -14134,7 +14158,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A97" s="29">
         <v>44001</v>
       </c>
@@ -14187,7 +14211,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A98" s="29">
         <v>44002</v>
       </c>
@@ -14240,7 +14264,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A99" s="29">
         <v>44003</v>
       </c>
@@ -14291,6 +14315,59 @@
       </c>
       <c r="Q99" s="13">
         <v>16</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A100" s="29">
+        <v>44004</v>
+      </c>
+      <c r="B100" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C100" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D100" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E100" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F100" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G100" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H100" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I100" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J100" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K100" s="11">
+        <v>6</v>
+      </c>
+      <c r="L100" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M100" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N100" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O100" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P100" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q100" s="13">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -14302,23 +14379,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R91"/>
+  <dimension ref="A1:R92"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B69" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Y94" sqref="Y94"/>
+      <selection pane="bottomRight" activeCell="L86" sqref="L86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5703125" style="2"/>
+    <col min="1" max="1" width="15.44140625" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.5546875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -14339,7 +14416,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
         <v>30</v>
       </c>
@@ -14360,7 +14437,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -14413,7 +14490,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>43916</v>
       </c>
@@ -14466,7 +14543,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>43917</v>
       </c>
@@ -14519,7 +14596,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>43918</v>
       </c>
@@ -14572,7 +14649,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>43919</v>
       </c>
@@ -14625,7 +14702,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>43920</v>
       </c>
@@ -14678,7 +14755,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>43921</v>
       </c>
@@ -14731,7 +14808,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>43922</v>
       </c>
@@ -14784,7 +14861,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>43923</v>
       </c>
@@ -14837,7 +14914,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
         <v>43924</v>
       </c>
@@ -14890,7 +14967,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>43925</v>
       </c>
@@ -14943,7 +15020,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>43926</v>
       </c>
@@ -14996,7 +15073,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>43927</v>
       </c>
@@ -15049,7 +15126,7 @@
         <v>1262</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>43928</v>
       </c>
@@ -15102,7 +15179,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>43929</v>
       </c>
@@ -15155,7 +15232,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>43930</v>
       </c>
@@ -15208,7 +15285,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>43931</v>
       </c>
@@ -15261,7 +15338,7 @@
         <v>1461</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>43932</v>
       </c>
@@ -15314,7 +15391,7 @@
         <v>1467</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>43933</v>
       </c>
@@ -15367,7 +15444,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="12">
         <v>43934</v>
       </c>
@@ -15420,7 +15497,7 @@
         <v>1482</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="12">
         <v>43935</v>
       </c>
@@ -15473,7 +15550,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="12">
         <v>43936</v>
       </c>
@@ -15526,7 +15603,7 @@
         <v>1486</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="12">
         <v>43937</v>
       </c>
@@ -15579,7 +15656,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="12">
         <v>43938</v>
       </c>
@@ -15632,7 +15709,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="12">
         <v>43939</v>
       </c>
@@ -15685,7 +15762,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="12">
         <v>43940</v>
       </c>
@@ -15738,7 +15815,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="12">
         <v>43941</v>
       </c>
@@ -15791,7 +15868,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <v>43942</v>
       </c>
@@ -15844,7 +15921,7 @@
         <v>1472</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="12">
         <v>43943</v>
       </c>
@@ -15897,7 +15974,7 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="12">
         <v>43944</v>
       </c>
@@ -15950,7 +16027,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="12">
         <v>43945</v>
       </c>
@@ -16003,7 +16080,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="12">
         <v>43946</v>
       </c>
@@ -16056,7 +16133,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="12">
         <v>43947</v>
       </c>
@@ -16109,7 +16186,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="29">
         <v>43948</v>
       </c>
@@ -16162,7 +16239,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="29">
         <v>43949</v>
       </c>
@@ -16215,7 +16292,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="29">
         <v>43950</v>
       </c>
@@ -16268,7 +16345,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="29">
         <v>43951</v>
       </c>
@@ -16321,7 +16398,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="29">
         <v>43952</v>
       </c>
@@ -16374,7 +16451,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="29">
         <v>43953</v>
       </c>
@@ -16427,7 +16504,7 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="29">
         <v>43954</v>
       </c>
@@ -16480,7 +16557,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="29">
         <v>43955</v>
       </c>
@@ -16533,7 +16610,7 @@
         <v>1279</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="29">
         <v>43956</v>
       </c>
@@ -16586,7 +16663,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="29">
         <v>43957</v>
       </c>
@@ -16639,7 +16716,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="29">
         <v>43958</v>
       </c>
@@ -16692,7 +16769,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="29">
         <v>43959</v>
       </c>
@@ -16745,7 +16822,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" s="29">
         <v>43960</v>
       </c>
@@ -16798,7 +16875,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="29">
         <v>43961</v>
       </c>
@@ -16851,7 +16928,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" s="29">
         <v>43962</v>
       </c>
@@ -16904,7 +16981,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="29">
         <v>43963</v>
       </c>
@@ -16957,7 +17034,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" s="29">
         <v>43964</v>
       </c>
@@ -17010,7 +17087,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" s="29">
         <v>43965</v>
       </c>
@@ -17063,7 +17140,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" s="29">
         <v>43966</v>
       </c>
@@ -17116,7 +17193,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" s="29">
         <v>43967</v>
       </c>
@@ -17169,7 +17246,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" s="29">
         <v>43968</v>
       </c>
@@ -17222,7 +17299,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" s="29">
         <v>43969</v>
       </c>
@@ -17275,7 +17352,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" s="29">
         <v>43970</v>
       </c>
@@ -17328,7 +17405,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" s="29">
         <v>43971</v>
       </c>
@@ -17381,7 +17458,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" s="29">
         <v>43972</v>
       </c>
@@ -17434,7 +17511,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" s="29">
         <v>43973</v>
       </c>
@@ -17487,7 +17564,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" s="29">
         <v>43974</v>
       </c>
@@ -17540,7 +17617,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" s="29">
         <v>43975</v>
       </c>
@@ -17593,7 +17670,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" s="29">
         <v>43976</v>
       </c>
@@ -17646,7 +17723,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A65" s="49">
         <v>43977</v>
       </c>
@@ -17699,7 +17776,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A66" s="49">
         <v>43978</v>
       </c>
@@ -17752,7 +17829,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A67" s="49">
         <v>43979</v>
       </c>
@@ -17805,7 +17882,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A68" s="49">
         <v>43980</v>
       </c>
@@ -17858,7 +17935,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A69" s="49">
         <v>43981</v>
       </c>
@@ -17911,7 +17988,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A70" s="49">
         <v>43982</v>
       </c>
@@ -17964,7 +18041,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A71" s="49">
         <v>43983</v>
       </c>
@@ -18017,7 +18094,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A72" s="49">
         <v>43984</v>
       </c>
@@ -18070,7 +18147,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A73" s="49">
         <v>43985</v>
       </c>
@@ -18123,7 +18200,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A74" s="49">
         <v>43986</v>
       </c>
@@ -18176,7 +18253,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A75" s="49">
         <v>43987</v>
       </c>
@@ -18229,7 +18306,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A76" s="49">
         <v>43988</v>
       </c>
@@ -18282,7 +18359,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A77" s="49">
         <v>43989</v>
       </c>
@@ -18335,7 +18412,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A78" s="49">
         <v>43990</v>
       </c>
@@ -18388,7 +18465,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A79" s="49">
         <v>43991</v>
       </c>
@@ -18441,7 +18518,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A80" s="49">
         <v>43992</v>
       </c>
@@ -18495,7 +18572,7 @@
       </c>
       <c r="R80" s="52"/>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A81" s="49">
         <v>43993</v>
       </c>
@@ -18549,7 +18626,7 @@
       </c>
       <c r="R81" s="52"/>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A82" s="49">
         <v>43994</v>
       </c>
@@ -18603,7 +18680,7 @@
       </c>
       <c r="R82" s="52"/>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A83" s="49">
         <v>43995</v>
       </c>
@@ -18656,7 +18733,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A84" s="49">
         <v>43996</v>
       </c>
@@ -18709,7 +18786,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A85" s="49">
         <v>43997</v>
       </c>
@@ -18762,7 +18839,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A86" s="49">
         <v>43998</v>
       </c>
@@ -18815,7 +18892,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A87" s="49">
         <v>43999</v>
       </c>
@@ -18868,7 +18945,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A88" s="49">
         <v>44000</v>
       </c>
@@ -18921,7 +18998,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A89" s="49">
         <v>44001</v>
       </c>
@@ -18974,7 +19051,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A90" s="49">
         <v>44002</v>
       </c>
@@ -19027,7 +19104,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A91" s="49">
         <v>44003</v>
       </c>
@@ -19078,6 +19155,59 @@
       </c>
       <c r="Q91" s="13">
         <v>518</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A92" s="49">
+        <v>44004</v>
+      </c>
+      <c r="B92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E92" s="14">
+        <v>53</v>
+      </c>
+      <c r="F92" s="14">
+        <v>5</v>
+      </c>
+      <c r="G92" s="14">
+        <v>42</v>
+      </c>
+      <c r="H92" s="14">
+        <v>236</v>
+      </c>
+      <c r="I92" s="14">
+        <v>7</v>
+      </c>
+      <c r="J92" s="14">
+        <v>39</v>
+      </c>
+      <c r="K92" s="11">
+        <v>127</v>
+      </c>
+      <c r="L92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P92" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q92" s="13">
+        <v>515</v>
       </c>
     </row>
   </sheetData>
@@ -19089,23 +19219,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R91"/>
+  <dimension ref="A1:R92"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B69" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H95" sqref="H95"/>
+      <selection pane="bottomRight" activeCell="Q92" sqref="Q92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5703125" style="2"/>
+    <col min="1" max="1" width="12.44140625" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.5546875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -19126,7 +19256,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
         <v>30</v>
       </c>
@@ -19147,7 +19277,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -19200,7 +19330,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>43916</v>
       </c>
@@ -19253,7 +19383,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>43917</v>
       </c>
@@ -19306,7 +19436,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>43918</v>
       </c>
@@ -19359,7 +19489,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>43919</v>
       </c>
@@ -19412,7 +19542,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>43920</v>
       </c>
@@ -19465,7 +19595,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>43921</v>
       </c>
@@ -19518,7 +19648,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>43922</v>
       </c>
@@ -19571,7 +19701,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>43923</v>
       </c>
@@ -19624,7 +19754,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
         <v>43924</v>
       </c>
@@ -19677,7 +19807,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>43925</v>
       </c>
@@ -19730,7 +19860,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>43926</v>
       </c>
@@ -19783,7 +19913,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>43927</v>
       </c>
@@ -19836,7 +19966,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>43928</v>
       </c>
@@ -19889,7 +20019,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>43929</v>
       </c>
@@ -19942,7 +20072,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>43930</v>
       </c>
@@ -19995,7 +20125,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>43931</v>
       </c>
@@ -20048,7 +20178,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>43932</v>
       </c>
@@ -20101,7 +20231,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>43933</v>
       </c>
@@ -20154,7 +20284,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="12">
         <v>43934</v>
       </c>
@@ -20207,7 +20337,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="12">
         <v>43935</v>
       </c>
@@ -20260,7 +20390,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="12">
         <v>43936</v>
       </c>
@@ -20313,7 +20443,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="12">
         <v>43937</v>
       </c>
@@ -20366,7 +20496,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="12">
         <v>43938</v>
       </c>
@@ -20419,7 +20549,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="12">
         <v>43939</v>
       </c>
@@ -20472,7 +20602,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="12">
         <v>43940</v>
       </c>
@@ -20525,7 +20655,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="12">
         <v>43941</v>
       </c>
@@ -20578,7 +20708,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <v>43942</v>
       </c>
@@ -20631,7 +20761,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="12">
         <v>43943</v>
       </c>
@@ -20684,7 +20814,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="12">
         <v>43944</v>
       </c>
@@ -20737,7 +20867,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="12">
         <v>43945</v>
       </c>
@@ -20790,7 +20920,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="12">
         <v>43946</v>
       </c>
@@ -20843,7 +20973,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="12">
         <v>43947</v>
       </c>
@@ -20896,7 +21026,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="29">
         <v>43948</v>
       </c>
@@ -20949,7 +21079,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="29">
         <v>43949</v>
       </c>
@@ -21002,7 +21132,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="29">
         <v>43950</v>
       </c>
@@ -21055,7 +21185,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="29">
         <v>43951</v>
       </c>
@@ -21108,7 +21238,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="29">
         <v>43952</v>
       </c>
@@ -21161,7 +21291,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="29">
         <v>43953</v>
       </c>
@@ -21214,7 +21344,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="29">
         <v>43954</v>
       </c>
@@ -21267,7 +21397,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="29">
         <v>43955</v>
       </c>
@@ -21320,7 +21450,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="29">
         <v>43956</v>
       </c>
@@ -21373,7 +21503,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="29">
         <v>43957</v>
       </c>
@@ -21426,7 +21556,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="29">
         <v>43958</v>
       </c>
@@ -21479,7 +21609,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="29">
         <v>43959</v>
       </c>
@@ -21532,7 +21662,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" s="29">
         <v>43960</v>
       </c>
@@ -21585,7 +21715,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="29">
         <v>43961</v>
       </c>
@@ -21638,7 +21768,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" s="29">
         <v>43962</v>
       </c>
@@ -21691,7 +21821,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="29">
         <v>43963</v>
       </c>
@@ -21744,7 +21874,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" s="29">
         <v>43964</v>
       </c>
@@ -21797,7 +21927,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" s="29">
         <v>43965</v>
       </c>
@@ -21850,7 +21980,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" s="29">
         <v>43966</v>
       </c>
@@ -21903,7 +22033,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" s="29">
         <v>43967</v>
       </c>
@@ -21956,7 +22086,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" s="29">
         <v>43968</v>
       </c>
@@ -22009,7 +22139,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" s="29">
         <v>43969</v>
       </c>
@@ -22062,7 +22192,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" s="29">
         <v>43970</v>
       </c>
@@ -22115,7 +22245,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" s="29">
         <v>43971</v>
       </c>
@@ -22168,7 +22298,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" s="29">
         <v>43972</v>
       </c>
@@ -22221,7 +22351,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" s="29">
         <v>43973</v>
       </c>
@@ -22274,7 +22404,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" s="29">
         <v>43974</v>
       </c>
@@ -22327,7 +22457,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" s="29">
         <v>43975</v>
       </c>
@@ -22380,7 +22510,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" s="29">
         <v>43976</v>
       </c>
@@ -22433,7 +22563,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" s="29">
         <v>43977</v>
       </c>
@@ -22486,7 +22616,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" s="29">
         <v>43978</v>
       </c>
@@ -22539,7 +22669,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" s="29">
         <v>43979</v>
       </c>
@@ -22592,7 +22722,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" s="29">
         <v>43980</v>
       </c>
@@ -22645,7 +22775,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" s="29">
         <v>43981</v>
       </c>
@@ -22698,7 +22828,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" s="29">
         <v>43982</v>
       </c>
@@ -22751,7 +22881,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" s="29">
         <v>43983</v>
       </c>
@@ -22804,7 +22934,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" s="29">
         <v>43984</v>
       </c>
@@ -22857,7 +22987,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" s="29">
         <v>43985</v>
       </c>
@@ -22910,7 +23040,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" s="29">
         <v>43986</v>
       </c>
@@ -22963,7 +23093,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75" s="29">
         <v>43987</v>
       </c>
@@ -23016,7 +23146,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76" s="29">
         <v>43988</v>
       </c>
@@ -23069,7 +23199,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77" s="29">
         <v>43989</v>
       </c>
@@ -23122,7 +23252,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78" s="29">
         <v>43990</v>
       </c>
@@ -23175,7 +23305,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79" s="29">
         <v>43991</v>
       </c>
@@ -23228,7 +23358,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A80" s="29">
         <v>43992</v>
       </c>
@@ -23281,7 +23411,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A81" s="29">
         <v>43993</v>
       </c>
@@ -23334,7 +23464,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A82" s="29">
         <v>43994</v>
       </c>
@@ -23387,7 +23517,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A83" s="29">
         <v>43995</v>
       </c>
@@ -23440,7 +23570,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A84" s="29">
         <v>43996</v>
       </c>
@@ -23493,7 +23623,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A85" s="29">
         <v>43997</v>
       </c>
@@ -23546,7 +23676,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A86" s="29">
         <v>43998</v>
       </c>
@@ -23599,7 +23729,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A87" s="29">
         <v>43999</v>
       </c>
@@ -23652,7 +23782,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A88" s="29">
         <v>44000</v>
       </c>
@@ -23705,7 +23835,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A89" s="29">
         <v>44001</v>
       </c>
@@ -23758,7 +23888,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A90" s="29">
         <v>44002</v>
       </c>
@@ -23811,7 +23941,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A91" s="29">
         <v>44003</v>
       </c>
@@ -23864,6 +23994,59 @@
         <v>283</v>
       </c>
       <c r="R91" s="52"/>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A92" s="29">
+        <v>44004</v>
+      </c>
+      <c r="B92" s="11">
+        <v>17</v>
+      </c>
+      <c r="C92" s="11">
+        <v>25</v>
+      </c>
+      <c r="D92" s="11">
+        <v>6</v>
+      </c>
+      <c r="E92" s="11">
+        <v>20</v>
+      </c>
+      <c r="F92" s="11">
+        <v>26</v>
+      </c>
+      <c r="G92" s="11">
+        <v>10</v>
+      </c>
+      <c r="H92" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I92" s="11">
+        <v>30</v>
+      </c>
+      <c r="J92" s="11">
+        <v>48</v>
+      </c>
+      <c r="K92" s="11">
+        <v>160</v>
+      </c>
+      <c r="L92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N92" s="11">
+        <v>7</v>
+      </c>
+      <c r="O92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P92" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q92" s="13">
+        <v>352</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23896,7 +24079,7 @@
       <value order="0"/>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-21T11:36:26Z</value>
+      <value order="0">2020-06-22T12:09:14Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -23911,13 +24094,13 @@
       <value order="0">Being Drafted</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41865896</value>
+      <value order="0">vA41884158</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">27.8</value>
+      <value order="0">27.10</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">207</value>
+      <value order="0">209</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-23 20:08)
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2071" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2097" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -2770,10 +2770,10 @@
   <dimension ref="A1:S160"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B94" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B91" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C114" sqref="C114"/>
+      <selection pane="bottomRight" activeCell="K116" sqref="K116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8279,21 +8279,54 @@
       </c>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B112" s="27"/>
-      <c r="C112" s="27"/>
-      <c r="D112" s="27"/>
-      <c r="E112" s="27"/>
-      <c r="F112" s="27"/>
-      <c r="G112" s="27"/>
-      <c r="H112" s="27"/>
-      <c r="I112" s="27"/>
-      <c r="J112" s="27"/>
-      <c r="K112" s="27"/>
-      <c r="L112" s="27"/>
-      <c r="M112" s="27"/>
-      <c r="N112" s="27"/>
-      <c r="O112" s="27"/>
-      <c r="P112" s="27"/>
+      <c r="A112" s="5">
+        <v>44005</v>
+      </c>
+      <c r="B112" s="27">
+        <v>1251</v>
+      </c>
+      <c r="C112" s="27">
+        <v>346</v>
+      </c>
+      <c r="D112" s="27">
+        <v>285</v>
+      </c>
+      <c r="E112" s="27">
+        <v>928</v>
+      </c>
+      <c r="F112" s="27">
+        <v>1058</v>
+      </c>
+      <c r="G112" s="27">
+        <v>1413</v>
+      </c>
+      <c r="H112" s="27">
+        <v>4832</v>
+      </c>
+      <c r="I112" s="27">
+        <v>374</v>
+      </c>
+      <c r="J112" s="27">
+        <v>2715</v>
+      </c>
+      <c r="K112" s="27">
+        <v>3147</v>
+      </c>
+      <c r="L112" s="27">
+        <v>9</v>
+      </c>
+      <c r="M112" s="27">
+        <v>54</v>
+      </c>
+      <c r="N112" s="27">
+        <v>1763</v>
+      </c>
+      <c r="O112" s="27">
+        <v>7</v>
+      </c>
+      <c r="P112" s="31">
+        <v>18182</v>
+      </c>
     </row>
     <row r="113" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B113" s="27"/>
@@ -9120,11 +9153,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q100"/>
+  <dimension ref="A1:Q101"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M106" sqref="M106"/>
+      <selection pane="bottomLeft" activeCell="L100" sqref="L100:P101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14370,6 +14403,59 @@
         <v>15</v>
       </c>
     </row>
+    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A101" s="29">
+        <v>44005</v>
+      </c>
+      <c r="B101" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C101" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D101" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E101" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F101" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G101" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H101" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I101" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J101" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K101" s="11">
+        <v>10</v>
+      </c>
+      <c r="L101" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M101" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N101" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O101" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P101" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q101" s="13">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -14379,13 +14465,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R92"/>
+  <dimension ref="A1:R93"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B69" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B75" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L86" sqref="L86"/>
+      <selection pane="bottomRight" activeCell="S82" sqref="S82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19210,6 +19296,59 @@
         <v>515</v>
       </c>
     </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A93" s="49">
+        <v>44005</v>
+      </c>
+      <c r="B93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E93" s="11">
+        <v>53</v>
+      </c>
+      <c r="F93" s="11">
+        <v>5</v>
+      </c>
+      <c r="G93" s="11">
+        <v>43</v>
+      </c>
+      <c r="H93" s="11">
+        <v>237</v>
+      </c>
+      <c r="I93" s="11">
+        <v>7</v>
+      </c>
+      <c r="J93" s="11">
+        <v>37</v>
+      </c>
+      <c r="K93" s="11">
+        <v>123</v>
+      </c>
+      <c r="L93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N93" s="11">
+        <v>5</v>
+      </c>
+      <c r="O93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P93" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q93" s="11">
+        <v>512</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -19219,13 +19358,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R92"/>
+  <dimension ref="A1:R93"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B69" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Q92" sqref="Q92"/>
+      <selection pane="bottomRight" activeCell="K89" sqref="K89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24046,6 +24185,59 @@
       </c>
       <c r="Q92" s="13">
         <v>352</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A93" s="29">
+        <v>44005</v>
+      </c>
+      <c r="B93" s="11">
+        <v>21</v>
+      </c>
+      <c r="C93" s="11">
+        <v>20</v>
+      </c>
+      <c r="D93" s="11">
+        <v>20</v>
+      </c>
+      <c r="E93" s="11">
+        <v>12</v>
+      </c>
+      <c r="F93" s="11">
+        <v>25</v>
+      </c>
+      <c r="G93" s="11">
+        <v>15</v>
+      </c>
+      <c r="H93" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I93" s="11">
+        <v>18</v>
+      </c>
+      <c r="J93" s="11">
+        <v>56</v>
+      </c>
+      <c r="K93" s="11">
+        <v>155</v>
+      </c>
+      <c r="L93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N93" s="11">
+        <v>11</v>
+      </c>
+      <c r="O93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P93" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q93" s="13">
+        <v>353</v>
       </c>
     </row>
   </sheetData>
@@ -24079,7 +24271,7 @@
       <value order="0"/>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-22T12:09:14Z</value>
+      <value order="0">2020-06-23T11:53:43Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -24094,13 +24286,13 @@
       <value order="0">Being Drafted</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41884158</value>
+      <value order="0">vA41913469</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">27.10</value>
+      <value order="0">27.12</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">209</value>
+      <value order="0">211</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-24 20:08)
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U445783\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA18464\A28088333\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u419207\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA10434\A28088333\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5988" windowHeight="6048" tabRatio="803" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5990" windowHeight="6050" tabRatio="803" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2097" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2123" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -2662,21 +2662,21 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.44140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="90.44140625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.44140625" style="2"/>
+    <col min="2" max="2" width="29.453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="90.453125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B3" s="18" t="s">
         <v>20</v>
       </c>
@@ -2684,7 +2684,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="20" t="s">
         <v>22</v>
       </c>
@@ -2692,13 +2692,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="22" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="23"/>
     </row>
-    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="24" t="s">
         <v>26</v>
       </c>
@@ -2706,7 +2706,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="24" t="s">
         <v>27</v>
       </c>
@@ -2714,7 +2714,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="24" t="s">
         <v>36</v>
       </c>
@@ -2722,7 +2722,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="20" t="s">
         <v>37</v>
       </c>
@@ -2750,12 +2750,12 @@
       <selection activeCell="O81" sqref="O81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="9.44140625" style="2"/>
+    <col min="1" max="16384" width="9.453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="44" spans="1:1" ht="15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A44" s="42"/>
     </row>
   </sheetData>
@@ -2770,20 +2770,20 @@
   <dimension ref="A1:S160"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B91" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B109" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K116" sqref="K116"/>
+      <selection pane="bottomRight" activeCell="A113" sqref="A113"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" style="2" customWidth="1"/>
-    <col min="2" max="16" width="11.44140625" style="11" customWidth="1"/>
-    <col min="17" max="16384" width="8.5546875" style="2"/>
+    <col min="2" max="16" width="11.453125" style="11" customWidth="1"/>
+    <col min="17" max="16384" width="8.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -2803,7 +2803,7 @@
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="26" t="s">
         <v>30</v>
       </c>
@@ -2822,7 +2822,7 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>43897</v>
       </c>
@@ -2922,7 +2922,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>43898</v>
       </c>
@@ -2972,7 +2972,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>43899</v>
       </c>
@@ -3022,7 +3022,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>43900</v>
       </c>
@@ -3072,7 +3072,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>43901</v>
       </c>
@@ -3122,7 +3122,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>43902</v>
       </c>
@@ -3172,7 +3172,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>43903</v>
       </c>
@@ -3222,7 +3222,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>43904</v>
       </c>
@@ -3272,7 +3272,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>43905</v>
       </c>
@@ -3322,7 +3322,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>43906</v>
       </c>
@@ -3372,7 +3372,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>43907</v>
       </c>
@@ -3422,7 +3422,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>43908</v>
       </c>
@@ -3472,7 +3472,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>43909</v>
       </c>
@@ -3522,7 +3522,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>43910</v>
       </c>
@@ -3572,7 +3572,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>43911</v>
       </c>
@@ -3622,7 +3622,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>43912</v>
       </c>
@@ -3672,7 +3672,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>43913</v>
       </c>
@@ -3722,7 +3722,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>43914</v>
       </c>
@@ -3772,7 +3772,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>43915</v>
       </c>
@@ -3822,7 +3822,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>43916</v>
       </c>
@@ -3872,7 +3872,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>43917</v>
       </c>
@@ -3922,7 +3922,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>43918</v>
       </c>
@@ -3972,7 +3972,7 @@
         <v>1264</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>43919</v>
       </c>
@@ -4022,7 +4022,7 @@
         <v>1417</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>43920</v>
       </c>
@@ -4072,7 +4072,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>43921</v>
       </c>
@@ -4122,7 +4122,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>43922</v>
       </c>
@@ -4172,7 +4172,7 @@
         <v>2310</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>43923</v>
       </c>
@@ -4222,7 +4222,7 @@
         <v>2602</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>43924</v>
       </c>
@@ -4272,7 +4272,7 @@
         <v>3001</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>43925</v>
       </c>
@@ -4322,7 +4322,7 @@
         <v>3345</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>43926</v>
       </c>
@@ -4372,7 +4372,7 @@
         <v>3706</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>43927</v>
       </c>
@@ -4422,7 +4422,7 @@
         <v>3961</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>43928</v>
       </c>
@@ -4472,7 +4472,7 @@
         <v>4229</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>43929</v>
       </c>
@@ -4522,7 +4522,7 @@
         <v>4565</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>43930</v>
       </c>
@@ -4572,7 +4572,7 @@
         <v>4957</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>43931</v>
       </c>
@@ -4622,7 +4622,7 @@
         <v>5275</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>43932</v>
       </c>
@@ -4672,7 +4672,7 @@
         <v>5590</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>43933</v>
       </c>
@@ -4722,7 +4722,7 @@
         <v>5912</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>43934</v>
       </c>
@@ -4772,7 +4772,7 @@
         <v>6067</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>43935</v>
       </c>
@@ -4822,7 +4822,7 @@
         <v>6358</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>43936</v>
       </c>
@@ -4872,7 +4872,7 @@
         <v>6748</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
         <v>43937</v>
       </c>
@@ -4922,7 +4922,7 @@
         <v>7102</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>43938</v>
       </c>
@@ -4972,7 +4972,7 @@
         <v>7409</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A46" s="5">
         <v>43939</v>
       </c>
@@ -5022,7 +5022,7 @@
         <v>7820</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A47" s="5">
         <v>43940</v>
       </c>
@@ -5072,7 +5072,7 @@
         <v>8187</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A48" s="5">
         <v>43941</v>
       </c>
@@ -5122,7 +5122,7 @@
         <v>8450</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A49" s="5">
         <v>43942</v>
       </c>
@@ -5172,7 +5172,7 @@
         <v>8672</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
         <v>43943</v>
       </c>
@@ -5222,7 +5222,7 @@
         <v>9038</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
         <v>43944</v>
       </c>
@@ -5272,7 +5272,7 @@
         <v>9409</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
         <v>43945</v>
       </c>
@@ -5322,7 +5322,7 @@
         <v>9697</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
         <v>43946</v>
       </c>
@@ -5372,7 +5372,7 @@
         <v>10051</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A54" s="5">
         <v>43947</v>
       </c>
@@ -5423,7 +5423,7 @@
       </c>
       <c r="R54" s="37"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
         <v>43948</v>
       </c>
@@ -5474,7 +5474,7 @@
       </c>
       <c r="R55" s="37"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A56" s="5">
         <v>43949</v>
       </c>
@@ -5525,7 +5525,7 @@
       </c>
       <c r="R56" s="38"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
         <v>43950</v>
       </c>
@@ -5575,7 +5575,7 @@
         <v>11034</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
         <v>43951</v>
       </c>
@@ -5626,7 +5626,7 @@
       </c>
       <c r="R58" s="37"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>43952</v>
       </c>
@@ -5678,7 +5678,7 @@
       <c r="R59" s="37"/>
       <c r="S59" s="37"/>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
         <v>43953</v>
       </c>
@@ -5728,7 +5728,7 @@
         <v>11927</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
         <v>43954</v>
       </c>
@@ -5778,7 +5778,7 @@
         <v>12097</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A62" s="5">
         <v>43955</v>
       </c>
@@ -5828,7 +5828,7 @@
         <v>12266</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A63" s="5">
         <v>43956</v>
       </c>
@@ -5878,7 +5878,7 @@
         <v>12437</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
         <v>43957</v>
       </c>
@@ -5928,7 +5928,7 @@
         <v>12709</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>43958</v>
       </c>
@@ -5978,7 +5978,7 @@
         <v>12924</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
         <v>43959</v>
       </c>
@@ -6028,7 +6028,7 @@
         <v>13149</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
         <v>43960</v>
       </c>
@@ -6078,7 +6078,7 @@
         <v>13305</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A68" s="5">
         <v>43961</v>
       </c>
@@ -6128,7 +6128,7 @@
         <v>13486</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A69" s="5">
         <v>43962</v>
       </c>
@@ -6178,7 +6178,7 @@
         <v>13627</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A70" s="5">
         <v>43963</v>
       </c>
@@ -6228,7 +6228,7 @@
         <v>13763</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A71" s="5">
         <v>43964</v>
       </c>
@@ -6278,7 +6278,7 @@
         <v>13929</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A72" s="5">
         <v>43965</v>
       </c>
@@ -6328,7 +6328,7 @@
         <v>14117</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A73" s="5">
         <v>43966</v>
       </c>
@@ -6378,7 +6378,7 @@
         <v>14260</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A74" s="5">
         <v>43967</v>
       </c>
@@ -6428,7 +6428,7 @@
         <v>14447</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A75" s="5">
         <v>43968</v>
       </c>
@@ -6478,7 +6478,7 @@
         <v>14537</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A76" s="5">
         <v>43969</v>
       </c>
@@ -6528,7 +6528,7 @@
         <v>14594</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A77" s="5">
         <v>43970</v>
       </c>
@@ -6578,7 +6578,7 @@
         <v>14655</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A78" s="5">
         <v>43971</v>
       </c>
@@ -6628,7 +6628,7 @@
         <v>14751</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A79" s="5">
         <v>43972</v>
       </c>
@@ -6678,7 +6678,7 @@
         <v>14856</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A80" s="5">
         <v>43973</v>
       </c>
@@ -6728,7 +6728,7 @@
         <v>14969</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A81" s="5">
         <v>43974</v>
       </c>
@@ -6778,7 +6778,7 @@
         <v>15041</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A82" s="5">
         <v>43975</v>
       </c>
@@ -6828,7 +6828,7 @@
         <v>15101</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A83" s="5">
         <v>43976</v>
       </c>
@@ -6878,7 +6878,7 @@
         <v>15156</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A84" s="5">
         <v>43977</v>
       </c>
@@ -6928,7 +6928,7 @@
         <v>15185</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A85" s="5">
         <v>43978</v>
       </c>
@@ -6978,7 +6978,7 @@
         <v>15240</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A86" s="5">
         <v>43979</v>
       </c>
@@ -7028,7 +7028,7 @@
         <v>15288</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A87" s="5">
         <v>43980</v>
       </c>
@@ -7078,7 +7078,7 @@
         <v>15327</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A88" s="5">
         <v>43981</v>
       </c>
@@ -7128,7 +7128,7 @@
         <v>15382</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A89" s="5">
         <v>43982</v>
       </c>
@@ -7178,7 +7178,7 @@
         <v>15400</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A90" s="5">
         <v>43983</v>
       </c>
@@ -7228,7 +7228,7 @@
         <v>15418</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A91" s="5">
         <v>43984</v>
       </c>
@@ -7278,7 +7278,7 @@
         <v>15471</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A92" s="5">
         <v>43985</v>
       </c>
@@ -7328,7 +7328,7 @@
         <v>15504</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A93" s="5">
         <v>43986</v>
       </c>
@@ -7378,7 +7378,7 @@
         <v>15553</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A94" s="5">
         <v>43987</v>
       </c>
@@ -7428,7 +7428,7 @@
         <v>15582</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A95" s="5">
         <v>43988</v>
       </c>
@@ -7478,7 +7478,7 @@
         <v>15603</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A96" s="5">
         <v>43989</v>
       </c>
@@ -7528,7 +7528,7 @@
         <v>15621</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A97" s="5">
         <v>43990</v>
       </c>
@@ -7578,7 +7578,7 @@
         <v>15639</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A98" s="5">
         <v>43991</v>
       </c>
@@ -7628,7 +7628,7 @@
         <v>15653</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A99" s="5">
         <v>43992</v>
       </c>
@@ -7678,7 +7678,7 @@
         <v>15665</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A100" s="5">
         <v>43993</v>
       </c>
@@ -7728,7 +7728,7 @@
         <v>15682</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A101" s="5">
         <v>43994</v>
       </c>
@@ -7778,7 +7778,7 @@
         <v>15709</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A102" s="5">
         <v>43995</v>
       </c>
@@ -7828,7 +7828,7 @@
         <v>15730</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A103" s="53">
         <v>43996</v>
       </c>
@@ -7878,7 +7878,7 @@
         <v>15755</v>
       </c>
     </row>
-    <row r="104" spans="1:16" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:16" ht="13.9" customHeight="1" x14ac:dyD